<commit_message>
Update Pertanggal 20 Juli 2022 15:11 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="141">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -430,6 +430,15 @@
   </si>
   <si>
     <t>Setiap Kartu Keluarga Warga Negara bisa saja terdiri dari beberapa Anggota Warga Negara</t>
+  </si>
+  <si>
+    <t>TblBankBranch</t>
+  </si>
+  <si>
+    <t>Cabang Bank</t>
+  </si>
+  <si>
+    <t>Setiap Bank memiliki beberapa cabang</t>
   </si>
 </sst>
 </file>
@@ -1067,8 +1076,287 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1079,296 +1367,17 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1681,20 +1690,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K68"/>
+  <dimension ref="B1:K69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="94" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="94" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="71" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="71" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1705,1067 +1714,1085 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" s="54" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+    <row r="2" spans="2:11" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="17" t="s">
+      <c r="C2" s="105"/>
+      <c r="D2" s="106"/>
+      <c r="E2" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="108"/>
+      <c r="G2" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="106"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="109" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="21"/>
+      <c r="I3" s="110"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="72" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="64" t="s">
+      <c r="E4" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="55" t="s">
+      <c r="G4" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="36" t="s">
+      <c r="H4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="37" t="s">
+      <c r="I4" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="97"/>
-      <c r="C5" s="98" t="s">
+      <c r="B5" s="74"/>
+      <c r="C5" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="E5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="92" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="38" t="s">
+      <c r="I5" s="24" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="97"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="66"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="10" t="s">
+      <c r="B6" s="74"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="99"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="39"/>
+      <c r="I6" s="88"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="97"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="58"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="103"/>
+      <c r="G7" s="94"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="40" t="s">
+      <c r="I7" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="97"/>
-      <c r="C8" s="101" t="s">
+    <row r="8" spans="2:11" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="74"/>
+      <c r="C8" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="68" t="s">
+      <c r="E8" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="59" t="s">
+      <c r="G8" s="39" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="26" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="97"/>
-      <c r="C9" s="98" t="s">
+      <c r="B9" s="74"/>
+      <c r="C9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="69" t="s">
+      <c r="E9" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="56" t="s">
+      <c r="G9" s="92" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="24" t="s">
         <v>72</v>
       </c>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="97"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="10" t="s">
+      <c r="B10" s="74"/>
+      <c r="C10" s="96"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="93"/>
+      <c r="H10" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="39"/>
+      <c r="I10" s="88"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="97"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="58"/>
+      <c r="B11" s="74"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="100"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="94"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="40" t="s">
+      <c r="I11" s="25" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="97"/>
-      <c r="C12" s="98" t="s">
+      <c r="B12" s="74"/>
+      <c r="C12" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="98" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="29" t="s">
+      <c r="F12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="56" t="s">
+      <c r="G12" s="92" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="38" t="s">
+      <c r="I12" s="24" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="97"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="68" t="s">
+      <c r="B13" s="74"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="58"/>
+      <c r="G13" s="94"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="40"/>
+      <c r="I13" s="25"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="97"/>
-      <c r="C14" s="102" t="s">
+      <c r="B14" s="74"/>
+      <c r="C14" s="76" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="72" t="s">
+      <c r="E14" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="47" t="s">
+      <c r="F14" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="60" t="s">
+      <c r="G14" s="40" t="s">
         <v>37</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="38" t="s">
+      <c r="I14" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="103"/>
-      <c r="C15" s="102"/>
-      <c r="D15" s="53"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="60"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="38"/>
+      <c r="I15" s="24"/>
     </row>
     <row r="16" spans="2:11" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="104"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="46"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="79"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="86"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="107" t="s">
+      <c r="C17" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="51" t="s">
+      <c r="D17" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="84"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="81"/>
-      <c r="H17" s="82"/>
-      <c r="I17" s="83"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
     </row>
     <row r="18" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="106"/>
-      <c r="C18" s="101" t="s">
+      <c r="B18" s="80"/>
+      <c r="C18" s="75" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="E18" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="68" t="s">
+      <c r="G18" s="48" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="41" t="s">
+      <c r="I18" s="26" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="106"/>
-      <c r="C19" s="101" t="s">
+      <c r="B19" s="80"/>
+      <c r="C19" s="75" t="s">
+        <v>138</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="E19" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="26" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="80"/>
+      <c r="C20" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D20" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E19" s="85"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="88"/>
-    </row>
-    <row r="20" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="106"/>
-      <c r="C20" s="101" t="s">
+      <c r="E20" s="62"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="64"/>
+      <c r="I20" s="65"/>
+    </row>
+    <row r="21" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="80"/>
+      <c r="C21" s="75" t="s">
         <v>85</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D21" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E20" s="85"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="88"/>
-    </row>
-    <row r="21" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="106"/>
-      <c r="C21" s="102" t="s">
+      <c r="E21" s="62"/>
+      <c r="F21" s="63"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="65"/>
+    </row>
+    <row r="22" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B22" s="80"/>
+      <c r="C22" s="76" t="s">
         <v>86</v>
       </c>
-      <c r="D21" s="53" t="s">
+      <c r="D22" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="E21" s="65" t="s">
+      <c r="E22" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F22" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="G21" s="65" t="s">
+      <c r="G22" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="41" t="s">
+      <c r="I22" s="26" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="106"/>
-      <c r="C22" s="102" t="s">
+    <row r="23" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="80"/>
+      <c r="C23" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="53" t="s">
+      <c r="D23" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="E22" s="85"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="87"/>
-      <c r="I22" s="88"/>
-    </row>
-    <row r="23" spans="2:9" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="106"/>
-      <c r="C23" s="102" t="s">
+      <c r="E23" s="62"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="65"/>
+    </row>
+    <row r="24" spans="2:9" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="80"/>
+      <c r="C24" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="53" t="s">
+      <c r="D24" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="68" t="s">
+      <c r="E24" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F24" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="68" t="s">
+      <c r="G24" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I23" s="41" t="s">
+      <c r="I24" s="26" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="106"/>
-      <c r="C24" s="102" t="s">
+    <row r="25" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B25" s="80"/>
+      <c r="C25" s="76" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="53" t="s">
+      <c r="D25" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="E24" s="85"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="88"/>
-    </row>
-    <row r="25" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="106"/>
-      <c r="C25" s="102" t="s">
+      <c r="E25" s="62"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="64"/>
+      <c r="I25" s="65"/>
+    </row>
+    <row r="26" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="80"/>
+      <c r="C26" s="76" t="s">
         <v>102</v>
       </c>
-      <c r="D25" s="53" t="s">
+      <c r="D26" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="85"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="88"/>
-    </row>
-    <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="106"/>
-      <c r="C26" s="102" t="s">
+      <c r="E26" s="62"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="65"/>
+    </row>
+    <row r="27" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="80"/>
+      <c r="C27" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="D26" s="53" t="s">
+      <c r="D27" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="E26" s="85"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="88"/>
-    </row>
-    <row r="27" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="106"/>
-      <c r="C27" s="102" t="s">
+      <c r="E27" s="62"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="65"/>
+    </row>
+    <row r="28" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="80"/>
+      <c r="C28" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="D27" s="53" t="s">
+      <c r="D28" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E27" s="65" t="s">
+      <c r="E28" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F28" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G27" s="85"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="88"/>
-    </row>
-    <row r="28" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="106"/>
-      <c r="C28" s="102" t="s">
+      <c r="G28" s="62"/>
+      <c r="H28" s="64"/>
+      <c r="I28" s="65"/>
+    </row>
+    <row r="29" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B29" s="80"/>
+      <c r="C29" s="76" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="53" t="s">
+      <c r="D29" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="85"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="87"/>
-      <c r="I28" s="88"/>
-    </row>
-    <row r="29" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="106"/>
-      <c r="C29" s="102" t="s">
+      <c r="E29" s="62"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="65"/>
+    </row>
+    <row r="30" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="80"/>
+      <c r="C30" s="76" t="s">
         <v>106</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D30" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="E29" s="85"/>
-      <c r="F29" s="86"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="88"/>
-    </row>
-    <row r="30" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="106"/>
-      <c r="C30" s="102" t="s">
+      <c r="E30" s="62"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="64"/>
+      <c r="I30" s="65"/>
+    </row>
+    <row r="31" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="80"/>
+      <c r="C31" s="76" t="s">
         <v>115</v>
       </c>
-      <c r="D30" s="53" t="s">
+      <c r="D31" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="E30" s="90"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="90"/>
-      <c r="H30" s="92"/>
-      <c r="I30" s="93"/>
-    </row>
-    <row r="31" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B31" s="106"/>
-      <c r="C31" s="102" t="s">
+      <c r="E31" s="67"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="67"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="70"/>
+    </row>
+    <row r="32" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B32" s="80"/>
+      <c r="C32" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D32" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="65" t="s">
+      <c r="E32" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="F31" s="29" t="s">
+      <c r="F32" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="G31" s="65" t="s">
+      <c r="G32" s="45" t="s">
         <v>120</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I31" s="41" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="106"/>
-      <c r="C32" s="102" t="s">
-        <v>117</v>
-      </c>
-      <c r="D32" s="53" t="s">
-        <v>130</v>
-      </c>
-      <c r="E32" s="65" t="s">
-        <v>123</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="G32" s="65" t="s">
-        <v>123</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="41" t="s">
-        <v>134</v>
+      <c r="I32" s="26" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="106"/>
-      <c r="C33" s="102" t="s">
-        <v>118</v>
-      </c>
-      <c r="D33" s="53" t="s">
-        <v>131</v>
-      </c>
-      <c r="E33" s="65" t="s">
-        <v>124</v>
-      </c>
-      <c r="F33" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="G33" s="65" t="s">
-        <v>124</v>
+      <c r="B33" s="80"/>
+      <c r="C33" s="76" t="s">
+        <v>117</v>
+      </c>
+      <c r="D33" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>123</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="41" t="s">
-        <v>133</v>
+      <c r="I33" s="26" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B34" s="106"/>
-      <c r="C34" s="102" t="s">
-        <v>119</v>
-      </c>
-      <c r="D34" s="53" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="65" t="s">
-        <v>126</v>
-      </c>
-      <c r="F34" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" s="65" t="s">
-        <v>126</v>
+      <c r="B34" s="80"/>
+      <c r="C34" s="76" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="45" t="s">
+        <v>124</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="41" t="s">
+      <c r="I34" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B35" s="80"/>
+      <c r="C35" s="76" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="G35" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I35" s="26" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="35" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="106"/>
-      <c r="C35" s="102"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="38"/>
-    </row>
     <row r="36" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="103"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="89" t="s">
+      <c r="B36" s="80"/>
+      <c r="C36" s="76"/>
+      <c r="D36" s="36"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="24"/>
+    </row>
+    <row r="37" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="77"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="72"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="38"/>
-    </row>
-    <row r="37" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="104"/>
-      <c r="C37" s="105"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="77"/>
-      <c r="I37" s="78"/>
-    </row>
-    <row r="38" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B38" s="97" t="s">
+      <c r="E37" s="49"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="24"/>
+    </row>
+    <row r="38" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="78"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="52"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="55"/>
+    </row>
+    <row r="39" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B39" s="74" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="107" t="s">
+      <c r="C39" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="D38" s="51" t="s">
+      <c r="D39" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="67" t="s">
+      <c r="E39" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="48" t="s">
+      <c r="F39" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="G38" s="61" t="s">
+      <c r="G39" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="H38" s="8" t="s">
+      <c r="H39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I38" s="40" t="s">
+      <c r="I39" s="25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="39" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="97"/>
-      <c r="C39" s="98" t="s">
+    <row r="40" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B40" s="74"/>
+      <c r="C40" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="23" t="s">
+      <c r="D40" s="98" t="s">
         <v>43</v>
       </c>
-      <c r="E39" s="69" t="s">
+      <c r="E40" s="89" t="s">
         <v>45</v>
       </c>
-      <c r="F39" s="27" t="s">
+      <c r="F40" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="G39" s="56" t="s">
+      <c r="G40" s="92" t="s">
         <v>47</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="38" t="s">
+      <c r="I40" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="97"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="70"/>
-      <c r="F40" s="35"/>
-      <c r="G40" s="57"/>
-      <c r="H40" s="10" t="s">
+    <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="74"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="99"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="102"/>
+      <c r="G41" s="93"/>
+      <c r="H41" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="I40" s="39"/>
-    </row>
-    <row r="41" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="97"/>
-      <c r="C41" s="100"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I41" s="40" t="s">
-        <v>49</v>
-      </c>
+      <c r="I41" s="88"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="97"/>
-      <c r="C42" s="101" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="E42" s="67" t="s">
-        <v>24</v>
-      </c>
-      <c r="F42" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="61" t="s">
-        <v>24</v>
-      </c>
+      <c r="B42" s="74"/>
+      <c r="C42" s="97"/>
+      <c r="D42" s="100"/>
+      <c r="E42" s="91"/>
+      <c r="F42" s="103"/>
+      <c r="G42" s="94"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B43" s="74"/>
+      <c r="C43" s="75" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="E43" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="H43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I43" s="25" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="97"/>
-      <c r="C43" s="98" t="s">
+    <row r="44" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B44" s="74"/>
+      <c r="C44" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D44" s="98" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="69" t="s">
+      <c r="E44" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="F43" s="27" t="s">
+      <c r="F44" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="G43" s="56" t="s">
+      <c r="G44" s="92" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H44" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="38" t="s">
+      <c r="I44" s="24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="97"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="70"/>
-      <c r="F44" s="35"/>
-      <c r="G44" s="57"/>
-      <c r="H44" s="10" t="s">
+    <row r="45" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="74"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="99"/>
+      <c r="E45" s="90"/>
+      <c r="F45" s="102"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="I44" s="39"/>
-    </row>
-    <row r="45" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B45" s="97"/>
-      <c r="C45" s="100"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="71"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="58"/>
-      <c r="H45" s="8" t="s">
+      <c r="I45" s="88"/>
+    </row>
+    <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B46" s="74"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="100"/>
+      <c r="E46" s="91"/>
+      <c r="F46" s="103"/>
+      <c r="G46" s="94"/>
+      <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I45" s="40" t="s">
+      <c r="I46" s="25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="46" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="97"/>
-      <c r="C46" s="108"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="30"/>
-      <c r="G46" s="62"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="42"/>
-    </row>
-    <row r="47" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="104"/>
-      <c r="C47" s="105"/>
-      <c r="D47" s="75"/>
+    <row r="47" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="74"/>
+      <c r="C47" s="82"/>
+      <c r="D47" s="19"/>
       <c r="E47" s="50"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="50"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="46"/>
-    </row>
-    <row r="48" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="97" t="s">
+      <c r="F47" s="17"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="27"/>
+    </row>
+    <row r="48" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="78"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="33"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="33"/>
+      <c r="H48" s="85"/>
+      <c r="I48" s="86"/>
+    </row>
+    <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="74" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="107" t="s">
+      <c r="C49" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="51" t="s">
+      <c r="D49" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="E48" s="79"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="81"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="83"/>
-    </row>
-    <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="97"/>
-      <c r="C49" s="107" t="s">
+      <c r="E49" s="56"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="60"/>
+    </row>
+    <row r="50" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="74"/>
+      <c r="C50" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="51" t="s">
+      <c r="D50" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="E49" s="79"/>
-      <c r="F49" s="80"/>
-      <c r="G49" s="81"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="83"/>
-    </row>
-    <row r="50" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="97"/>
-      <c r="C50" s="102" t="s">
+      <c r="E50" s="56"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="60"/>
+    </row>
+    <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="74"/>
+      <c r="C51" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="D50" s="53" t="s">
+      <c r="D51" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="E50" s="72" t="s">
+      <c r="E51" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="F50" s="47" t="s">
+      <c r="F51" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="G50" s="60" t="s">
+      <c r="G51" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="H50" s="6" t="s">
+      <c r="H51" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I50" s="38" t="s">
+      <c r="I51" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="97"/>
-      <c r="C51" s="108"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="73"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="62"/>
-      <c r="H51" s="10" t="s">
+    <row r="52" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="74"/>
+      <c r="C52" s="82"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="50"/>
+      <c r="F52" s="17"/>
+      <c r="G52" s="42"/>
+      <c r="H52" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="I51" s="39"/>
-    </row>
-    <row r="52" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="97"/>
-      <c r="C52" s="107"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="76"/>
-      <c r="F52" s="48"/>
-      <c r="G52" s="61"/>
-      <c r="H52" s="8" t="s">
+      <c r="I52" s="88"/>
+    </row>
+    <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="74"/>
+      <c r="C53" s="81"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="32"/>
+      <c r="G53" s="41"/>
+      <c r="H53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I52" s="40" t="s">
+      <c r="I53" s="25" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="97"/>
-      <c r="C53" s="108"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="73"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="62"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="42"/>
-    </row>
-    <row r="54" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="104"/>
-      <c r="C54" s="105"/>
-      <c r="D54" s="75"/>
+    <row r="54" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="74"/>
+      <c r="C54" s="82"/>
+      <c r="D54" s="19"/>
       <c r="E54" s="50"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="50"/>
-      <c r="H54" s="49"/>
-      <c r="I54" s="46"/>
-    </row>
-    <row r="55" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="97"/>
-      <c r="C55" s="108"/>
-      <c r="D55" s="32"/>
-      <c r="E55" s="73"/>
+      <c r="F54" s="17"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="27"/>
+    </row>
+    <row r="55" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="78"/>
+      <c r="C55" s="79"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="33"/>
       <c r="F55" s="30"/>
-      <c r="G55" s="62"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="42"/>
+      <c r="G55" s="33"/>
+      <c r="H55" s="85"/>
+      <c r="I55" s="86"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="97"/>
-      <c r="C56" s="108"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="73"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="62"/>
+      <c r="B56" s="74"/>
+      <c r="C56" s="82"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="50"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="42"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="42"/>
+      <c r="I56" s="27"/>
     </row>
     <row r="57" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="97"/>
-      <c r="C57" s="108"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="73"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="62"/>
+      <c r="B57" s="74"/>
+      <c r="C57" s="82"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="42"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="42"/>
+      <c r="I57" s="27"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="97"/>
-      <c r="C58" s="108"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="73"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="62"/>
+      <c r="B58" s="74"/>
+      <c r="C58" s="82"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="50"/>
+      <c r="F58" s="17"/>
+      <c r="G58" s="42"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="42"/>
+      <c r="I58" s="27"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="97"/>
-      <c r="C59" s="108"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="73"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="62"/>
+      <c r="B59" s="74"/>
+      <c r="C59" s="82"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="42"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="42"/>
+      <c r="I59" s="27"/>
     </row>
     <row r="60" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="97"/>
-      <c r="C60" s="108"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="73"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="62"/>
+      <c r="B60" s="74"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="50"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="42"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="42"/>
+      <c r="I60" s="27"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="97"/>
-      <c r="C61" s="108"/>
-      <c r="D61" s="32"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="62"/>
+      <c r="B61" s="74"/>
+      <c r="C61" s="82"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="50"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="42"/>
       <c r="H61" s="9"/>
-      <c r="I61" s="42"/>
+      <c r="I61" s="27"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="97"/>
-      <c r="C62" s="108"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="62"/>
+      <c r="B62" s="74"/>
+      <c r="C62" s="82"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="46"/>
+      <c r="F62" s="17"/>
+      <c r="G62" s="42"/>
       <c r="H62" s="9"/>
-      <c r="I62" s="42"/>
+      <c r="I62" s="27"/>
     </row>
     <row r="63" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="97"/>
-      <c r="C63" s="108"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="30"/>
-      <c r="G63" s="62"/>
+      <c r="B63" s="74"/>
+      <c r="C63" s="82"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="42"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="42"/>
+      <c r="I63" s="27"/>
     </row>
     <row r="64" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="97"/>
-      <c r="C64" s="108"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="62"/>
+      <c r="B64" s="74"/>
+      <c r="C64" s="82"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="17"/>
+      <c r="G64" s="42"/>
       <c r="H64" s="9"/>
-      <c r="I64" s="42"/>
+      <c r="I64" s="27"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="97"/>
-      <c r="C65" s="108"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="66"/>
-      <c r="F65" s="30"/>
-      <c r="G65" s="62"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="82"/>
+      <c r="D65" s="19"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="17"/>
+      <c r="G65" s="42"/>
       <c r="H65" s="9"/>
-      <c r="I65" s="42"/>
+      <c r="I65" s="27"/>
     </row>
     <row r="66" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="97"/>
-      <c r="C66" s="108"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="66"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="62"/>
+      <c r="B66" s="74"/>
+      <c r="C66" s="82"/>
+      <c r="D66" s="19"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="17"/>
+      <c r="G66" s="42"/>
       <c r="H66" s="9"/>
-      <c r="I66" s="42"/>
+      <c r="I66" s="27"/>
     </row>
     <row r="67" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="97"/>
-      <c r="C67" s="108"/>
-      <c r="D67" s="32"/>
-      <c r="E67" s="66"/>
-      <c r="F67" s="30"/>
-      <c r="G67" s="62"/>
+      <c r="B67" s="74"/>
+      <c r="C67" s="82"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="17"/>
+      <c r="G67" s="42"/>
       <c r="H67" s="9"/>
-      <c r="I67" s="42"/>
-    </row>
-    <row r="68" spans="2:9" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="109"/>
-      <c r="C68" s="110"/>
-      <c r="D68" s="33"/>
-      <c r="E68" s="74"/>
-      <c r="F68" s="31"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="43"/>
-      <c r="I68" s="44"/>
+      <c r="I67" s="27"/>
+    </row>
+    <row r="68" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="74"/>
+      <c r="C68" s="82"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="17"/>
+      <c r="G68" s="42"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="27"/>
+    </row>
+    <row r="69" spans="2:9" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="83"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="51"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="28"/>
+      <c r="I69" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="E43:E45"/>
-    <mergeCell ref="G43:G45"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="C43:C45"/>
-    <mergeCell ref="D43:D45"/>
-    <mergeCell ref="F43:F45"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -2775,16 +2802,22 @@
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Pertanggal 6 Januari 2023 18:41 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -7,15 +7,17 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Table" sheetId="1" r:id="rId1"/>
-    <sheet name="Schema" sheetId="2" r:id="rId2"/>
+    <sheet name="Function" sheetId="3" r:id="rId1"/>
+    <sheet name="Table" sheetId="1" r:id="rId2"/>
+    <sheet name="Schema" sheetId="2" r:id="rId3"/>
+    <sheet name="Database" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="287">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -439,13 +441,465 @@
   </si>
   <si>
     <t>Setiap Bank memiliki beberapa cabang</t>
+  </si>
+  <si>
+    <t>dbERPReborn</t>
+  </si>
+  <si>
+    <t>dbERPReborn-Data-OLAP</t>
+  </si>
+  <si>
+    <t>dbERPReborn-Data-OLTP</t>
+  </si>
+  <si>
+    <t>dbERPReborn-SysConfig</t>
+  </si>
+  <si>
+    <t>DATABASE</t>
+  </si>
+  <si>
+    <t>SchSysConfig</t>
+  </si>
+  <si>
+    <t>SchSystem</t>
+  </si>
+  <si>
+    <t>SchAccounting</t>
+  </si>
+  <si>
+    <t>SchBudgeting</t>
+  </si>
+  <si>
+    <t>SchCustomerRelation</t>
+  </si>
+  <si>
+    <t>SchDataAcquisition</t>
+  </si>
+  <si>
+    <t>SchFinance</t>
+  </si>
+  <si>
+    <t>SchFixedAsset</t>
+  </si>
+  <si>
+    <t>SchHumanResource</t>
+  </si>
+  <si>
+    <t>SchMaster</t>
+  </si>
+  <si>
+    <t>SchProduction</t>
+  </si>
+  <si>
+    <t>SchProject</t>
+  </si>
+  <si>
+    <t>SchSupplyChain</t>
+  </si>
+  <si>
+    <t>SchTaxation</t>
+  </si>
+  <si>
+    <t>SchData-OLAP</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-Accounting</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-Budgeting</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-CustomerRelation</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-DataAcquisition</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-FixedAsset</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-HumanResource</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-Production</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-Project</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-SupplyChain</t>
+  </si>
+  <si>
+    <t>SchSysAsset</t>
+  </si>
+  <si>
+    <t>SchSysConfig-Import</t>
+  </si>
+  <si>
+    <t>SchSysConfig-Initialize</t>
+  </si>
+  <si>
+    <t>SchSysConfig-Synchronize</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLAP</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchAccounting</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchBudgeting</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchCustomerRelation</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchDataAcquisition</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchFinance</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchFixedAsset</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchHumanResource</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchMaster</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchProduction</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchProject</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchSupplyChain</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper : dbERPReborn-Data-OLTP.SchTaxation</t>
+  </si>
+  <si>
+    <t>Local Schema</t>
+  </si>
+  <si>
+    <t>Foreign Data Wrapper :dbERPReborn-SysConfig.SchSysConfig</t>
+  </si>
+  <si>
+    <t>Skema untuk Inisialisasi Data</t>
+  </si>
+  <si>
+    <t>Skema untuk Import Data</t>
+  </si>
+  <si>
+    <t>Skema untuk Sinkronisasi Data</t>
+  </si>
+  <si>
+    <t>Skema Sistem Internal</t>
+  </si>
+  <si>
+    <t>Skema Konfigurasi Sistem</t>
+  </si>
+  <si>
+    <t>FWD Skema Konfigurasi Sistem</t>
+  </si>
+  <si>
+    <t>Skema untuk Library yang bersifat General</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Akuntansi</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Anggaran</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Hubungan Pelanggan</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Akuisisi Data Eksternal</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Keuangan</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Aset Tetap</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Sumberdaya Manusia</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Master</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Produksi</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Proyek</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Rantai Pasok</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Transaksi Modul Perpajakan</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Akuntansi</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Anggaran</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Hubungan Pelanggan</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Akuisisi Data Eksternal</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Keuangan</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Aset Tetap</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Sumberdaya Manusia</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Master</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Produksi</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Proyek</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Rantai Pasok</t>
+  </si>
+  <si>
+    <t>Skema Data Transaksi Modul Perpajakan</t>
+  </si>
+  <si>
+    <t>FWD Skema Data Analitik dan Resume</t>
+  </si>
+  <si>
+    <t>Database FrontEnd</t>
+  </si>
+  <si>
+    <t>Database BackEnd untuk Data Analitik dan Resume</t>
+  </si>
+  <si>
+    <t>Database BackEnd untuk Data Transaksi</t>
+  </si>
+  <si>
+    <t>Database BackEnd untuk Konfigurasi Sistem</t>
+  </si>
+  <si>
+    <t>FUNCTION</t>
+  </si>
+  <si>
+    <t>Func_General_BigIntArray_Merge</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>LAST UPDATE</t>
+  </si>
+  <si>
+    <t>CREATE DATE</t>
+  </si>
+  <si>
+    <t>VERSIONING</t>
+  </si>
+  <si>
+    <t>1.00.0000</t>
+  </si>
+  <si>
+    <t>Func_General_BigIntArray_RemoveDuplicateElement</t>
+  </si>
+  <si>
+    <t>Func_General_BigIntArray_ReverseElementSequence</t>
+  </si>
+  <si>
+    <t>Menggabungkan Elemen pada suatu Array BigInt dengan Array BigInt lainnya</t>
+  </si>
+  <si>
+    <t>Menghapus duplikasi Elemen pada Array BigInt</t>
+  </si>
+  <si>
+    <t>Membalik urutan Elemen pada Array BigInt</t>
+  </si>
+  <si>
+    <t>Func_General_DataTypeConvert_JSONArrayToBigIntArray</t>
+  </si>
+  <si>
+    <t>Mengkonversi tipe data dari JSON Array ke BigInt Array</t>
+  </si>
+  <si>
+    <t>Func_General_DataTypeConvert_JSONArrayToVarCharArray</t>
+  </si>
+  <si>
+    <t>Mengkonversi tipe data dari JSON Array ke VarChar Array</t>
+  </si>
+  <si>
+    <t>Func_General_Hash_SHA256</t>
+  </si>
+  <si>
+    <t>Mendapatkan SHA256 dari varData</t>
+  </si>
+  <si>
+    <t>Func_General_JSONArray_RemoveElementByIndex</t>
+  </si>
+  <si>
+    <t>Menghapus elemen Array JSON berdasarkan Index</t>
+  </si>
+  <si>
+    <t>Func_General_JSONArray_RemoveElementByIndexArray</t>
+  </si>
+  <si>
+    <t>Menghapus element Array JSON berdasarkan Array Index (Multiple Index)</t>
+  </si>
+  <si>
+    <t>Func_General_NumberSay_English</t>
+  </si>
+  <si>
+    <t>Menampilkan terbilang untuk nominal angka dalam mode bahasa inggris</t>
+  </si>
+  <si>
+    <t>Func_General_NumberSay_Indonesian</t>
+  </si>
+  <si>
+    <t>Menampilkan terbilang untuk nominal angka dalam mode bahasa indonesia</t>
+  </si>
+  <si>
+    <t>Func_General_PeriodByDateTimeTZInterval</t>
+  </si>
+  <si>
+    <t>Mendapatkan Periode berdasarkan Interval Tanggal Awal dan Tanggal Akhir</t>
+  </si>
+  <si>
+    <t>Func_GetDataList_CloudStorageFiles</t>
+  </si>
+  <si>
+    <t>Func_GetDataList_CloudStorageSubDirectories</t>
+  </si>
+  <si>
+    <t>1.00.0002</t>
+  </si>
+  <si>
+    <t>Func_GetDataList_LocalStorageFiles</t>
+  </si>
+  <si>
+    <t>Func_GetDataList_LocalStorageSubDirectories</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data List File Upload Staging Area Detail pada Cloud Storage berdasarkan RPK</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data List File Upload Staging Area pada Cloud Storage</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data List File Upload Staging Area Detail pada Local Storage berdasarkan RPK</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data List File Upload Staging Area pada Local Storage</t>
+  </si>
+  <si>
+    <t>Func_GetData_APIWebTokenByUserSessionID</t>
+  </si>
+  <si>
+    <t>Mendapatkan API Web Token dari User Session ID</t>
+  </si>
+  <si>
+    <t>Func_GetData_ArrayOfSimplifiedEntities</t>
+  </si>
+  <si>
+    <t>Mendapatkan Simplifikasi Array dari Entities</t>
+  </si>
+  <si>
+    <t>Func_GetData_FileUpload_MasterFileRecord</t>
+  </si>
+  <si>
+    <t>1.01.0000</t>
+  </si>
+  <si>
+    <t>Mendapatkan Master File Record dari File Upload</t>
+  </si>
+  <si>
+    <t>Func_GetData_FileUpload_isFileAlreadyExist</t>
+  </si>
+  <si>
+    <t>Mendapatkan Signal apakah suatu file sudah terupload atau belum</t>
+  </si>
+  <si>
+    <t>Mendapatkan User Session ID dari API Web Token</t>
+  </si>
+  <si>
+    <t>Func_GetData_UserSessionIDByAPIWebToken</t>
+  </si>
+  <si>
+    <t>Func_GetFileEntities_StagingArea</t>
+  </si>
+  <si>
+    <t>Mendapatkan File Entities pada Staging Area</t>
+  </si>
+  <si>
+    <t>FuncSys_General_CreateSequence</t>
+  </si>
+  <si>
+    <t>Membangun Object Sequence pada Remote Schema</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAPIWebToken_SysEngine</t>
+  </si>
+  <si>
+    <t>Mendapatkan API Web Token untuk SysEngine</t>
+  </si>
+  <si>
+    <t>Func_GetData_APIWebTokenOfSysEngine</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Obsolete, Replaced with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>SchSysAsset.Func_GetData_APIWebTokenOfSysEngine</t>
+    </r>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllExtensionsName</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama Extension yang terdapat didalam sistem</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllForeignObjectsEntity</t>
+  </si>
+  <si>
+    <t>1.00.0001</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh entitas Foreign yang terdapat didalam sistem</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,19 +947,39 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -554,8 +1028,53 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="1"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="4"/>
+        </stop>
+        <stop position="1">
+          <color theme="1"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="1"/>
+        </stop>
+        <stop position="0.5">
+          <color theme="5"/>
+        </stop>
+        <stop position="1">
+          <color theme="1"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <gradientFill degree="90">
+        <stop position="0">
+          <color theme="1"/>
+        </stop>
+        <stop position="0.5">
+          <color rgb="FF00B050"/>
+        </stop>
+        <stop position="1">
+          <color theme="1"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
-  <borders count="39">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -789,19 +1308,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -955,17 +1461,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1043,11 +1538,87 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1058,327 +1629,446 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="12" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1690,20 +2380,1232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:H109"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.42578125" style="96" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="96" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.140625" style="96" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="146" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="147" customWidth="1"/>
+    <col min="8" max="8" width="16" style="147" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="96"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="139" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="144" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="141" t="s">
+        <v>231</v>
+      </c>
+      <c r="G2" s="142"/>
+      <c r="H2" s="145"/>
+    </row>
+    <row r="3" spans="2:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="113" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="143" t="s">
+        <v>226</v>
+      </c>
+      <c r="E3" s="149"/>
+      <c r="F3" s="150" t="s">
+        <v>228</v>
+      </c>
+      <c r="G3" s="151" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" s="152" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="108" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="153" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="153" t="s">
+        <v>227</v>
+      </c>
+      <c r="E4" s="154" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="155" t="s">
+        <v>232</v>
+      </c>
+      <c r="G4" s="156">
+        <v>44910</v>
+      </c>
+      <c r="H4" s="157">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="103"/>
+      <c r="C5" s="99"/>
+      <c r="D5" s="99" t="s">
+        <v>233</v>
+      </c>
+      <c r="E5" s="120" t="s">
+        <v>236</v>
+      </c>
+      <c r="F5" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G5" s="162">
+        <v>44908</v>
+      </c>
+      <c r="H5" s="163">
+        <v>44908</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="103"/>
+      <c r="C6" s="99"/>
+      <c r="D6" s="99" t="s">
+        <v>234</v>
+      </c>
+      <c r="E6" s="120" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G6" s="162">
+        <v>44908</v>
+      </c>
+      <c r="H6" s="163">
+        <v>44908</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="103"/>
+      <c r="C7" s="99"/>
+      <c r="D7" s="99" t="s">
+        <v>238</v>
+      </c>
+      <c r="E7" s="120" t="s">
+        <v>239</v>
+      </c>
+      <c r="F7" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G7" s="162">
+        <v>44887</v>
+      </c>
+      <c r="H7" s="163">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="103"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99" t="s">
+        <v>240</v>
+      </c>
+      <c r="E8" s="120" t="s">
+        <v>241</v>
+      </c>
+      <c r="F8" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G8" s="162">
+        <v>44887</v>
+      </c>
+      <c r="H8" s="163">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="103"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99" t="s">
+        <v>242</v>
+      </c>
+      <c r="E9" s="120" t="s">
+        <v>243</v>
+      </c>
+      <c r="F9" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G9" s="162">
+        <v>44774</v>
+      </c>
+      <c r="H9" s="163">
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="103"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99" t="s">
+        <v>244</v>
+      </c>
+      <c r="E10" s="120" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="162">
+        <v>44897</v>
+      </c>
+      <c r="H10" s="163">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="103"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99" t="s">
+        <v>246</v>
+      </c>
+      <c r="E11" s="120" t="s">
+        <v>247</v>
+      </c>
+      <c r="F11" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="162">
+        <v>44897</v>
+      </c>
+      <c r="H11" s="163">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="103"/>
+      <c r="C12" s="99"/>
+      <c r="D12" s="99" t="s">
+        <v>248</v>
+      </c>
+      <c r="E12" s="120" t="s">
+        <v>249</v>
+      </c>
+      <c r="F12" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="162">
+        <v>44748</v>
+      </c>
+      <c r="H12" s="163">
+        <v>44748</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="103"/>
+      <c r="C13" s="99"/>
+      <c r="D13" s="99" t="s">
+        <v>250</v>
+      </c>
+      <c r="E13" s="120" t="s">
+        <v>251</v>
+      </c>
+      <c r="F13" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G13" s="162">
+        <v>44735</v>
+      </c>
+      <c r="H13" s="163">
+        <v>44735</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="103"/>
+      <c r="C14" s="99"/>
+      <c r="D14" s="99" t="s">
+        <v>252</v>
+      </c>
+      <c r="E14" s="120" t="s">
+        <v>253</v>
+      </c>
+      <c r="F14" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G14" s="162">
+        <v>44854</v>
+      </c>
+      <c r="H14" s="163">
+        <v>44854</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="103"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99" t="s">
+        <v>254</v>
+      </c>
+      <c r="E15" s="120" t="s">
+        <v>259</v>
+      </c>
+      <c r="F15" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G15" s="162">
+        <v>44770</v>
+      </c>
+      <c r="H15" s="163">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="103"/>
+      <c r="C16" s="99"/>
+      <c r="D16" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="E16" s="120" t="s">
+        <v>260</v>
+      </c>
+      <c r="F16" s="161" t="s">
+        <v>256</v>
+      </c>
+      <c r="G16" s="162">
+        <v>44770</v>
+      </c>
+      <c r="H16" s="163">
+        <v>44427</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="103"/>
+      <c r="C17" s="99"/>
+      <c r="D17" s="99" t="s">
+        <v>257</v>
+      </c>
+      <c r="E17" s="120" t="s">
+        <v>261</v>
+      </c>
+      <c r="F17" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G17" s="162">
+        <v>44770</v>
+      </c>
+      <c r="H17" s="163">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="103"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="E18" s="120" t="s">
+        <v>262</v>
+      </c>
+      <c r="F18" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G18" s="162">
+        <v>44770</v>
+      </c>
+      <c r="H18" s="163">
+        <v>44427</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="103"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="99" t="s">
+        <v>263</v>
+      </c>
+      <c r="E19" s="120" t="s">
+        <v>264</v>
+      </c>
+      <c r="F19" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G19" s="162">
+        <v>44777</v>
+      </c>
+      <c r="H19" s="163">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="103"/>
+      <c r="C20" s="99"/>
+      <c r="D20" s="99" t="s">
+        <v>280</v>
+      </c>
+      <c r="E20" s="120" t="s">
+        <v>279</v>
+      </c>
+      <c r="F20" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G20" s="162">
+        <v>44931</v>
+      </c>
+      <c r="H20" s="163">
+        <v>44931</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="103"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99" t="s">
+        <v>265</v>
+      </c>
+      <c r="E21" s="120" t="s">
+        <v>266</v>
+      </c>
+      <c r="F21" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G21" s="162">
+        <v>44847</v>
+      </c>
+      <c r="H21" s="163">
+        <v>44847</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B22" s="103"/>
+      <c r="C22" s="99"/>
+      <c r="D22" s="99" t="s">
+        <v>267</v>
+      </c>
+      <c r="E22" s="120" t="s">
+        <v>269</v>
+      </c>
+      <c r="F22" s="161" t="s">
+        <v>268</v>
+      </c>
+      <c r="G22" s="162">
+        <v>44792</v>
+      </c>
+      <c r="H22" s="163">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B23" s="103"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="99" t="s">
+        <v>270</v>
+      </c>
+      <c r="E23" s="120" t="s">
+        <v>271</v>
+      </c>
+      <c r="F23" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G23" s="162">
+        <v>44776</v>
+      </c>
+      <c r="H23" s="163">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="103"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99" t="s">
+        <v>273</v>
+      </c>
+      <c r="E24" s="120" t="s">
+        <v>272</v>
+      </c>
+      <c r="F24" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G24" s="162">
+        <v>44777</v>
+      </c>
+      <c r="H24" s="163">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B25" s="103"/>
+      <c r="C25" s="99"/>
+      <c r="D25" s="99" t="s">
+        <v>274</v>
+      </c>
+      <c r="E25" s="120" t="s">
+        <v>275</v>
+      </c>
+      <c r="F25" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G25" s="162">
+        <v>44770</v>
+      </c>
+      <c r="H25" s="163">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B26" s="103"/>
+      <c r="C26" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="98" t="s">
+        <v>276</v>
+      </c>
+      <c r="E26" s="125" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26" s="164" t="s">
+        <v>232</v>
+      </c>
+      <c r="G26" s="165">
+        <v>44167</v>
+      </c>
+      <c r="H26" s="166">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B27" s="103"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="167" t="s">
+        <v>278</v>
+      </c>
+      <c r="E27" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="F27" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="162">
+        <v>44167</v>
+      </c>
+      <c r="H27" s="163">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="103"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="99" t="s">
+        <v>282</v>
+      </c>
+      <c r="E28" s="120" t="s">
+        <v>283</v>
+      </c>
+      <c r="F28" s="161" t="s">
+        <v>232</v>
+      </c>
+      <c r="G28" s="162">
+        <v>43185</v>
+      </c>
+      <c r="H28" s="163">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B29" s="103"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="99" t="s">
+        <v>284</v>
+      </c>
+      <c r="E29" s="120" t="s">
+        <v>286</v>
+      </c>
+      <c r="F29" s="161" t="s">
+        <v>285</v>
+      </c>
+      <c r="G29" s="162">
+        <v>44216</v>
+      </c>
+      <c r="H29" s="163">
+        <v>44216</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B30" s="103"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="99"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="161"/>
+      <c r="G30" s="162"/>
+      <c r="H30" s="163"/>
+    </row>
+    <row r="31" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B31" s="103"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="120"/>
+      <c r="F31" s="161"/>
+      <c r="G31" s="162"/>
+      <c r="H31" s="163"/>
+    </row>
+    <row r="32" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B32" s="103"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="99"/>
+      <c r="E32" s="120"/>
+      <c r="F32" s="161"/>
+      <c r="G32" s="162"/>
+      <c r="H32" s="163"/>
+    </row>
+    <row r="33" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="103"/>
+      <c r="C33" s="99"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="120"/>
+      <c r="F33" s="161"/>
+      <c r="G33" s="162"/>
+      <c r="H33" s="163"/>
+    </row>
+    <row r="34" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B34" s="103"/>
+      <c r="C34" s="99"/>
+      <c r="D34" s="99"/>
+      <c r="E34" s="120"/>
+      <c r="F34" s="161"/>
+      <c r="G34" s="162"/>
+      <c r="H34" s="163"/>
+    </row>
+    <row r="35" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="103"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="120"/>
+      <c r="F35" s="161"/>
+      <c r="G35" s="162"/>
+      <c r="H35" s="163"/>
+    </row>
+    <row r="36" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B36" s="103"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="120"/>
+      <c r="F36" s="161"/>
+      <c r="G36" s="162"/>
+      <c r="H36" s="163"/>
+    </row>
+    <row r="37" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B37" s="103"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="120"/>
+      <c r="F37" s="161"/>
+      <c r="G37" s="162"/>
+      <c r="H37" s="163"/>
+    </row>
+    <row r="38" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="103"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="99"/>
+      <c r="E38" s="120"/>
+      <c r="F38" s="161"/>
+      <c r="G38" s="162"/>
+      <c r="H38" s="163"/>
+    </row>
+    <row r="39" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="103"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="99"/>
+      <c r="E39" s="120"/>
+      <c r="F39" s="161"/>
+      <c r="G39" s="162"/>
+      <c r="H39" s="163"/>
+    </row>
+    <row r="40" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B40" s="103"/>
+      <c r="C40" s="99"/>
+      <c r="D40" s="99"/>
+      <c r="E40" s="120"/>
+      <c r="F40" s="161"/>
+      <c r="G40" s="162"/>
+      <c r="H40" s="163"/>
+    </row>
+    <row r="41" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B41" s="103"/>
+      <c r="C41" s="99"/>
+      <c r="D41" s="99"/>
+      <c r="E41" s="120"/>
+      <c r="F41" s="161"/>
+      <c r="G41" s="162"/>
+      <c r="H41" s="163"/>
+    </row>
+    <row r="42" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="103"/>
+      <c r="C42" s="99"/>
+      <c r="D42" s="99"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="161"/>
+      <c r="G42" s="162"/>
+      <c r="H42" s="163"/>
+    </row>
+    <row r="43" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="103"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="99"/>
+      <c r="E43" s="120"/>
+      <c r="F43" s="161"/>
+      <c r="G43" s="162"/>
+      <c r="H43" s="163"/>
+    </row>
+    <row r="44" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="103"/>
+      <c r="C44" s="99"/>
+      <c r="D44" s="99"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="161"/>
+      <c r="G44" s="162"/>
+      <c r="H44" s="163"/>
+    </row>
+    <row r="45" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B45" s="103"/>
+      <c r="C45" s="99"/>
+      <c r="D45" s="99"/>
+      <c r="E45" s="120"/>
+      <c r="F45" s="161"/>
+      <c r="G45" s="162"/>
+      <c r="H45" s="163"/>
+    </row>
+    <row r="46" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B46" s="103"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="161"/>
+      <c r="G46" s="162"/>
+      <c r="H46" s="163"/>
+    </row>
+    <row r="47" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="103"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="99"/>
+      <c r="E47" s="120"/>
+      <c r="F47" s="161"/>
+      <c r="G47" s="162"/>
+      <c r="H47" s="163"/>
+    </row>
+    <row r="48" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="103"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="161"/>
+      <c r="G48" s="162"/>
+      <c r="H48" s="163"/>
+    </row>
+    <row r="49" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="103"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="120"/>
+      <c r="F49" s="161"/>
+      <c r="G49" s="162"/>
+      <c r="H49" s="163"/>
+    </row>
+    <row r="50" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="103"/>
+      <c r="C50" s="99"/>
+      <c r="D50" s="99"/>
+      <c r="E50" s="120"/>
+      <c r="F50" s="161"/>
+      <c r="G50" s="162"/>
+      <c r="H50" s="163"/>
+    </row>
+    <row r="51" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="103"/>
+      <c r="C51" s="99"/>
+      <c r="D51" s="99"/>
+      <c r="E51" s="120"/>
+      <c r="F51" s="161"/>
+      <c r="G51" s="162"/>
+      <c r="H51" s="163"/>
+    </row>
+    <row r="52" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B52" s="103"/>
+      <c r="C52" s="99"/>
+      <c r="D52" s="99"/>
+      <c r="E52" s="120"/>
+      <c r="F52" s="161"/>
+      <c r="G52" s="162"/>
+      <c r="H52" s="163"/>
+    </row>
+    <row r="53" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B53" s="103"/>
+      <c r="C53" s="99"/>
+      <c r="D53" s="99"/>
+      <c r="E53" s="120"/>
+      <c r="F53" s="161"/>
+      <c r="G53" s="162"/>
+      <c r="H53" s="163"/>
+    </row>
+    <row r="54" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B54" s="103"/>
+      <c r="C54" s="99"/>
+      <c r="D54" s="99"/>
+      <c r="E54" s="120"/>
+      <c r="F54" s="161"/>
+      <c r="G54" s="162"/>
+      <c r="H54" s="163"/>
+    </row>
+    <row r="55" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B55" s="103"/>
+      <c r="C55" s="99"/>
+      <c r="D55" s="99"/>
+      <c r="E55" s="120"/>
+      <c r="F55" s="161"/>
+      <c r="G55" s="162"/>
+      <c r="H55" s="163"/>
+    </row>
+    <row r="56" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B56" s="103"/>
+      <c r="C56" s="99"/>
+      <c r="D56" s="99"/>
+      <c r="E56" s="120"/>
+      <c r="F56" s="161"/>
+      <c r="G56" s="162"/>
+      <c r="H56" s="163"/>
+    </row>
+    <row r="57" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="103"/>
+      <c r="C57" s="99"/>
+      <c r="D57" s="99"/>
+      <c r="E57" s="120"/>
+      <c r="F57" s="161"/>
+      <c r="G57" s="162"/>
+      <c r="H57" s="163"/>
+    </row>
+    <row r="58" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B58" s="103"/>
+      <c r="C58" s="99"/>
+      <c r="D58" s="99"/>
+      <c r="E58" s="120"/>
+      <c r="F58" s="161"/>
+      <c r="G58" s="162"/>
+      <c r="H58" s="163"/>
+    </row>
+    <row r="59" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B59" s="103"/>
+      <c r="C59" s="99"/>
+      <c r="D59" s="99"/>
+      <c r="E59" s="120"/>
+      <c r="F59" s="161"/>
+      <c r="G59" s="162"/>
+      <c r="H59" s="163"/>
+    </row>
+    <row r="60" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B60" s="103"/>
+      <c r="C60" s="99"/>
+      <c r="D60" s="99"/>
+      <c r="E60" s="120"/>
+      <c r="F60" s="161"/>
+      <c r="G60" s="162"/>
+      <c r="H60" s="163"/>
+    </row>
+    <row r="61" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="103"/>
+      <c r="C61" s="99"/>
+      <c r="D61" s="99"/>
+      <c r="E61" s="120"/>
+      <c r="F61" s="161"/>
+      <c r="G61" s="162"/>
+      <c r="H61" s="163"/>
+    </row>
+    <row r="62" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="103"/>
+      <c r="C62" s="99"/>
+      <c r="D62" s="99"/>
+      <c r="E62" s="120"/>
+      <c r="F62" s="161"/>
+      <c r="G62" s="162"/>
+      <c r="H62" s="163"/>
+    </row>
+    <row r="63" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B63" s="103"/>
+      <c r="C63" s="99"/>
+      <c r="D63" s="99"/>
+      <c r="E63" s="120"/>
+      <c r="F63" s="161"/>
+      <c r="G63" s="162"/>
+      <c r="H63" s="163"/>
+    </row>
+    <row r="64" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B64" s="103"/>
+      <c r="C64" s="99"/>
+      <c r="D64" s="99"/>
+      <c r="E64" s="120"/>
+      <c r="F64" s="161"/>
+      <c r="G64" s="162"/>
+      <c r="H64" s="163"/>
+    </row>
+    <row r="65" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B65" s="103"/>
+      <c r="C65" s="99"/>
+      <c r="D65" s="99"/>
+      <c r="E65" s="120"/>
+      <c r="F65" s="161"/>
+      <c r="G65" s="162"/>
+      <c r="H65" s="163"/>
+    </row>
+    <row r="66" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B66" s="103"/>
+      <c r="C66" s="99"/>
+      <c r="D66" s="99"/>
+      <c r="E66" s="120"/>
+      <c r="F66" s="161"/>
+      <c r="G66" s="162"/>
+      <c r="H66" s="163"/>
+    </row>
+    <row r="67" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B67" s="103"/>
+      <c r="C67" s="99"/>
+      <c r="D67" s="99"/>
+      <c r="E67" s="120"/>
+      <c r="F67" s="161"/>
+      <c r="G67" s="162"/>
+      <c r="H67" s="163"/>
+    </row>
+    <row r="68" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B68" s="103"/>
+      <c r="C68" s="99"/>
+      <c r="D68" s="99"/>
+      <c r="E68" s="120"/>
+      <c r="F68" s="161"/>
+      <c r="G68" s="162"/>
+      <c r="H68" s="163"/>
+    </row>
+    <row r="69" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B69" s="103"/>
+      <c r="C69" s="99"/>
+      <c r="D69" s="99"/>
+      <c r="E69" s="120"/>
+      <c r="F69" s="161"/>
+      <c r="G69" s="162"/>
+      <c r="H69" s="163"/>
+    </row>
+    <row r="70" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B70" s="103"/>
+      <c r="C70" s="99"/>
+      <c r="D70" s="99"/>
+      <c r="E70" s="120"/>
+      <c r="F70" s="161"/>
+      <c r="G70" s="162"/>
+      <c r="H70" s="163"/>
+    </row>
+    <row r="71" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B71" s="103"/>
+      <c r="C71" s="99"/>
+      <c r="D71" s="99"/>
+      <c r="E71" s="120"/>
+      <c r="F71" s="161"/>
+      <c r="G71" s="162"/>
+      <c r="H71" s="163"/>
+    </row>
+    <row r="72" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B72" s="103"/>
+      <c r="C72" s="99"/>
+      <c r="D72" s="99"/>
+      <c r="E72" s="120"/>
+      <c r="F72" s="161"/>
+      <c r="G72" s="162"/>
+      <c r="H72" s="163"/>
+    </row>
+    <row r="73" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B73" s="103"/>
+      <c r="C73" s="99"/>
+      <c r="D73" s="99"/>
+      <c r="E73" s="120"/>
+      <c r="F73" s="161"/>
+      <c r="G73" s="162"/>
+      <c r="H73" s="163"/>
+    </row>
+    <row r="74" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B74" s="103"/>
+      <c r="C74" s="99"/>
+      <c r="D74" s="99"/>
+      <c r="E74" s="120"/>
+      <c r="F74" s="161"/>
+      <c r="G74" s="162"/>
+      <c r="H74" s="163"/>
+    </row>
+    <row r="75" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B75" s="103"/>
+      <c r="C75" s="99"/>
+      <c r="D75" s="99"/>
+      <c r="E75" s="120"/>
+      <c r="F75" s="161"/>
+      <c r="G75" s="162"/>
+      <c r="H75" s="163"/>
+    </row>
+    <row r="76" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B76" s="103"/>
+      <c r="C76" s="99"/>
+      <c r="D76" s="99"/>
+      <c r="E76" s="120"/>
+      <c r="F76" s="161"/>
+      <c r="G76" s="162"/>
+      <c r="H76" s="163"/>
+    </row>
+    <row r="77" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B77" s="103"/>
+      <c r="C77" s="99"/>
+      <c r="D77" s="99"/>
+      <c r="E77" s="120"/>
+      <c r="F77" s="161"/>
+      <c r="G77" s="162"/>
+      <c r="H77" s="163"/>
+    </row>
+    <row r="78" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B78" s="103"/>
+      <c r="C78" s="99"/>
+      <c r="D78" s="99"/>
+      <c r="E78" s="120"/>
+      <c r="F78" s="161"/>
+      <c r="G78" s="162"/>
+      <c r="H78" s="163"/>
+    </row>
+    <row r="79" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B79" s="103"/>
+      <c r="C79" s="99"/>
+      <c r="D79" s="99"/>
+      <c r="E79" s="120"/>
+      <c r="F79" s="161"/>
+      <c r="G79" s="162"/>
+      <c r="H79" s="163"/>
+    </row>
+    <row r="80" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B80" s="103"/>
+      <c r="C80" s="99"/>
+      <c r="D80" s="99"/>
+      <c r="E80" s="120"/>
+      <c r="F80" s="161"/>
+      <c r="G80" s="162"/>
+      <c r="H80" s="163"/>
+    </row>
+    <row r="81" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B81" s="103"/>
+      <c r="C81" s="99"/>
+      <c r="D81" s="99"/>
+      <c r="E81" s="120"/>
+      <c r="F81" s="161"/>
+      <c r="G81" s="162"/>
+      <c r="H81" s="163"/>
+    </row>
+    <row r="82" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B82" s="103"/>
+      <c r="C82" s="99"/>
+      <c r="D82" s="99"/>
+      <c r="E82" s="120"/>
+      <c r="F82" s="161"/>
+      <c r="G82" s="162"/>
+      <c r="H82" s="163"/>
+    </row>
+    <row r="83" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B83" s="103"/>
+      <c r="C83" s="99"/>
+      <c r="D83" s="99"/>
+      <c r="E83" s="120"/>
+      <c r="F83" s="161"/>
+      <c r="G83" s="162"/>
+      <c r="H83" s="163"/>
+    </row>
+    <row r="84" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B84" s="103"/>
+      <c r="C84" s="99"/>
+      <c r="D84" s="99"/>
+      <c r="E84" s="120"/>
+      <c r="F84" s="161"/>
+      <c r="G84" s="162"/>
+      <c r="H84" s="163"/>
+    </row>
+    <row r="85" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B85" s="103"/>
+      <c r="C85" s="99"/>
+      <c r="D85" s="99"/>
+      <c r="E85" s="120"/>
+      <c r="F85" s="161"/>
+      <c r="G85" s="162"/>
+      <c r="H85" s="163"/>
+    </row>
+    <row r="86" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B86" s="103"/>
+      <c r="C86" s="99"/>
+      <c r="D86" s="99"/>
+      <c r="E86" s="120"/>
+      <c r="F86" s="161"/>
+      <c r="G86" s="162"/>
+      <c r="H86" s="163"/>
+    </row>
+    <row r="87" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B87" s="103"/>
+      <c r="C87" s="99"/>
+      <c r="D87" s="99"/>
+      <c r="E87" s="120"/>
+      <c r="F87" s="161"/>
+      <c r="G87" s="162"/>
+      <c r="H87" s="163"/>
+    </row>
+    <row r="88" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B88" s="103"/>
+      <c r="C88" s="99"/>
+      <c r="D88" s="99"/>
+      <c r="E88" s="120"/>
+      <c r="F88" s="161"/>
+      <c r="G88" s="162"/>
+      <c r="H88" s="163"/>
+    </row>
+    <row r="89" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B89" s="103"/>
+      <c r="C89" s="99"/>
+      <c r="D89" s="99"/>
+      <c r="E89" s="120"/>
+      <c r="F89" s="161"/>
+      <c r="G89" s="162"/>
+      <c r="H89" s="163"/>
+    </row>
+    <row r="90" spans="2:8" s="97" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="106"/>
+      <c r="C90" s="107"/>
+      <c r="D90" s="107"/>
+      <c r="E90" s="127"/>
+      <c r="F90" s="158"/>
+      <c r="G90" s="159"/>
+      <c r="H90" s="160"/>
+    </row>
+    <row r="91" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F91" s="119"/>
+      <c r="G91" s="148"/>
+      <c r="H91" s="148"/>
+    </row>
+    <row r="92" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F92" s="119"/>
+      <c r="G92" s="148"/>
+      <c r="H92" s="148"/>
+    </row>
+    <row r="93" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F93" s="119"/>
+      <c r="G93" s="148"/>
+      <c r="H93" s="148"/>
+    </row>
+    <row r="94" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F94" s="119"/>
+      <c r="G94" s="148"/>
+      <c r="H94" s="148"/>
+    </row>
+    <row r="95" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F95" s="119"/>
+      <c r="G95" s="148"/>
+      <c r="H95" s="148"/>
+    </row>
+    <row r="96" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F96" s="119"/>
+      <c r="G96" s="148"/>
+      <c r="H96" s="148"/>
+    </row>
+    <row r="97" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F97" s="119"/>
+      <c r="G97" s="148"/>
+      <c r="H97" s="148"/>
+    </row>
+    <row r="98" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F98" s="119"/>
+      <c r="G98" s="148"/>
+      <c r="H98" s="148"/>
+    </row>
+    <row r="99" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F99" s="119"/>
+      <c r="G99" s="148"/>
+      <c r="H99" s="148"/>
+    </row>
+    <row r="100" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F100" s="119"/>
+      <c r="G100" s="148"/>
+      <c r="H100" s="148"/>
+    </row>
+    <row r="101" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F101" s="119"/>
+      <c r="G101" s="148"/>
+      <c r="H101" s="148"/>
+    </row>
+    <row r="102" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F102" s="119"/>
+      <c r="G102" s="148"/>
+      <c r="H102" s="148"/>
+    </row>
+    <row r="103" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F103" s="119"/>
+      <c r="G103" s="148"/>
+      <c r="H103" s="148"/>
+    </row>
+    <row r="104" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F104" s="119"/>
+      <c r="G104" s="148"/>
+      <c r="H104" s="148"/>
+    </row>
+    <row r="105" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F105" s="119"/>
+      <c r="G105" s="148"/>
+      <c r="H105" s="148"/>
+    </row>
+    <row r="106" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F106" s="119"/>
+      <c r="G106" s="148"/>
+      <c r="H106" s="148"/>
+    </row>
+    <row r="107" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F107" s="119"/>
+      <c r="G107" s="148"/>
+      <c r="H107" s="148"/>
+    </row>
+    <row r="108" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F108" s="119"/>
+      <c r="G108" s="148"/>
+      <c r="H108" s="148"/>
+    </row>
+    <row r="109" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F109" s="119"/>
+      <c r="G109" s="148"/>
+      <c r="H109" s="148"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F9" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29" style="71" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="60" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="60" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1714,1085 +3616,1091 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" s="37" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="104" t="s">
+    <row r="2" spans="2:11" s="28" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="110" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="105"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="107" t="s">
+      <c r="C2" s="111"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="136" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="108"/>
-      <c r="G2" s="104" t="s">
+      <c r="F2" s="131"/>
+      <c r="G2" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="105"/>
-      <c r="I2" s="106"/>
-    </row>
-    <row r="3" spans="2:11" s="3" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="H2" s="129"/>
+      <c r="I2" s="131"/>
+    </row>
+    <row r="3" spans="2:11" s="3" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="115" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="114" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="138" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="109" t="s">
+      <c r="H3" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="110"/>
+      <c r="I3" s="132"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="75" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="76" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="38" t="s">
+      <c r="G4" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="74"/>
-      <c r="C5" s="95" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="98" t="s">
+      <c r="D5" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="45" t="s">
+      <c r="E5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="101" t="s">
+      <c r="F5" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="92" t="s">
+      <c r="G5" s="88" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="16" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="74"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="99"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="102"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="87" t="s">
+      <c r="B6" s="61"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="89"/>
+      <c r="H6" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="88"/>
+      <c r="I6" s="78"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B7" s="74"/>
-      <c r="C7" s="97"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="103"/>
-      <c r="G7" s="94"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="90"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="25" t="s">
+      <c r="I7" s="17" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:11" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="74"/>
-      <c r="C8" s="75" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="39" t="s">
+      <c r="G8" s="29" t="s">
         <v>24</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="26" t="s">
+      <c r="I8" s="18" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="74"/>
-      <c r="C9" s="95" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="98" t="s">
+      <c r="D9" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="89" t="s">
+      <c r="E9" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="101" t="s">
+      <c r="F9" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="92" t="s">
+      <c r="G9" s="88" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="16" t="s">
         <v>72</v>
       </c>
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="74"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="90"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="87" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="88"/>
+      <c r="I10" s="78"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="74"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="91"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="94"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="90"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="17" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B12" s="74"/>
-      <c r="C12" s="95" t="s">
+      <c r="B12" s="61"/>
+      <c r="C12" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="92" t="s">
+      <c r="G12" s="88" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="74"/>
-      <c r="C13" s="97"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="48" t="s">
+      <c r="B13" s="61"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="84"/>
+      <c r="E13" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="94"/>
+      <c r="G13" s="90"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="25"/>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="74"/>
-      <c r="C14" s="76" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="30" t="s">
         <v>37</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="24" t="s">
+      <c r="I14" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="77"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="40"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="24"/>
+      <c r="I15" s="16"/>
     </row>
     <row r="16" spans="2:11" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="78"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="85"/>
-      <c r="I16" s="86"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="66"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="68" t="s">
         <v>76</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="E17" s="61"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="60"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="48"/>
+      <c r="I17" s="49"/>
     </row>
     <row r="18" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="80"/>
-      <c r="C18" s="75" t="s">
+      <c r="B18" s="67"/>
+      <c r="C18" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="37" t="s">
         <v>80</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="26" t="s">
+      <c r="I18" s="18" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="80"/>
-      <c r="C19" s="75" t="s">
+      <c r="B19" s="67"/>
+      <c r="C19" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="F19" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="48" t="s">
+      <c r="G19" s="37" t="s">
         <v>80</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="26" t="s">
+      <c r="I19" s="18" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="20" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="80"/>
-      <c r="C20" s="75" t="s">
+      <c r="B20" s="67"/>
+      <c r="C20" s="62" t="s">
         <v>83</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="65"/>
+      <c r="E20" s="51"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="51"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="54"/>
     </row>
     <row r="21" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="80"/>
-      <c r="C21" s="75" t="s">
+      <c r="B21" s="67"/>
+      <c r="C21" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E21" s="62"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="65"/>
+      <c r="E21" s="51"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="51"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="54"/>
     </row>
     <row r="22" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="80"/>
-      <c r="C22" s="76" t="s">
+      <c r="B22" s="67"/>
+      <c r="C22" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="36" t="s">
+      <c r="D22" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="45" t="s">
+      <c r="E22" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="34" t="s">
         <v>90</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="26" t="s">
+      <c r="I22" s="18" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="23" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="80"/>
-      <c r="C23" s="76" t="s">
+      <c r="B23" s="67"/>
+      <c r="C23" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="36" t="s">
+      <c r="D23" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="64"/>
-      <c r="I23" s="65"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="52"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="54"/>
     </row>
     <row r="24" spans="2:9" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="80"/>
-      <c r="C24" s="76" t="s">
+      <c r="B24" s="67"/>
+      <c r="C24" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D24" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="G24" s="48" t="s">
+      <c r="G24" s="37" t="s">
         <v>99</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I24" s="26" t="s">
+      <c r="I24" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B25" s="80"/>
-      <c r="C25" s="76" t="s">
+    <row r="25" spans="2:9" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="67"/>
+      <c r="C25" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="E25" s="62"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="65"/>
+      <c r="E25" s="51"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="51"/>
+      <c r="H25" s="53"/>
+      <c r="I25" s="54"/>
     </row>
     <row r="26" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B26" s="80"/>
-      <c r="C26" s="76" t="s">
+      <c r="B26" s="67"/>
+      <c r="C26" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="62"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="65"/>
-    </row>
-    <row r="27" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="80"/>
-      <c r="C27" s="76" t="s">
+      <c r="E26" s="51"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="51"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+    </row>
+    <row r="27" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="67"/>
+      <c r="C27" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="65"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="54"/>
     </row>
     <row r="28" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="80"/>
-      <c r="C28" s="76" t="s">
+      <c r="B28" s="67"/>
+      <c r="C28" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="D28" s="36" t="s">
+      <c r="D28" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="G28" s="62"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="65"/>
+      <c r="G28" s="51"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B29" s="80"/>
-      <c r="C29" s="76" t="s">
+      <c r="B29" s="67"/>
+      <c r="C29" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="D29" s="36" t="s">
+      <c r="D29" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="65"/>
-    </row>
-    <row r="30" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="80"/>
-      <c r="C30" s="76" t="s">
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="54"/>
+    </row>
+    <row r="30" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="67"/>
+      <c r="C30" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="36" t="s">
+      <c r="D30" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="E30" s="62"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="65"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="54"/>
     </row>
     <row r="31" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="80"/>
-      <c r="C31" s="76" t="s">
+      <c r="B31" s="67"/>
+      <c r="C31" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="D31" s="36" t="s">
+      <c r="D31" s="27" t="s">
         <v>128</v>
       </c>
-      <c r="E31" s="67"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="70"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
     </row>
     <row r="32" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B32" s="80"/>
-      <c r="C32" s="76" t="s">
+      <c r="B32" s="67"/>
+      <c r="C32" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="D32" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="E32" s="45" t="s">
+      <c r="E32" s="34" t="s">
         <v>120</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="G32" s="45" t="s">
+      <c r="G32" s="34" t="s">
         <v>120</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I32" s="26" t="s">
+      <c r="I32" s="18" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="33" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B33" s="80"/>
-      <c r="C33" s="76" t="s">
+      <c r="B33" s="67"/>
+      <c r="C33" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="E33" s="45" t="s">
+      <c r="E33" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="45" t="s">
+      <c r="G33" s="34" t="s">
         <v>123</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I33" s="26" t="s">
+      <c r="I33" s="18" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="34" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B34" s="80"/>
-      <c r="C34" s="76" t="s">
+      <c r="B34" s="67"/>
+      <c r="C34" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D34" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="E34" s="45" t="s">
+      <c r="E34" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="G34" s="45" t="s">
+      <c r="G34" s="34" t="s">
         <v>124</v>
       </c>
       <c r="H34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I34" s="26" t="s">
+      <c r="I34" s="18" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="35" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B35" s="80"/>
-      <c r="C35" s="76" t="s">
+      <c r="B35" s="67"/>
+      <c r="C35" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="36" t="s">
+      <c r="D35" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="E35" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G35" s="45" t="s">
+      <c r="G35" s="34" t="s">
         <v>126</v>
       </c>
       <c r="H35" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="I35" s="26" t="s">
+      <c r="I35" s="18" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="36" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="80"/>
-      <c r="C36" s="76"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="45"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="63"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="34"/>
       <c r="H36" s="6"/>
-      <c r="I36" s="24"/>
+      <c r="I36" s="16"/>
     </row>
     <row r="37" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="77"/>
-      <c r="C37" s="76"/>
-      <c r="D37" s="66" t="s">
+      <c r="B37" s="64"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="55" t="s">
         <v>89</v>
       </c>
-      <c r="E37" s="49"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="40"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="30"/>
       <c r="H37" s="6"/>
-      <c r="I37" s="24"/>
+      <c r="I37" s="16"/>
     </row>
     <row r="38" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="78"/>
-      <c r="C38" s="79"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="33"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="55"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="44"/>
     </row>
     <row r="39" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B39" s="74" t="s">
+      <c r="B39" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="81" t="s">
+      <c r="C39" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="E39" s="47" t="s">
+      <c r="E39" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G39" s="41" t="s">
+      <c r="G39" s="31" t="s">
         <v>24</v>
       </c>
       <c r="H39" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I39" s="25" t="s">
+      <c r="I39" s="17" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B40" s="74"/>
-      <c r="C40" s="95" t="s">
+      <c r="B40" s="61"/>
+      <c r="C40" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="98" t="s">
+      <c r="D40" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="89" t="s">
+      <c r="E40" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="101" t="s">
+      <c r="F40" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="92" t="s">
+      <c r="G40" s="88" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="24" t="s">
+      <c r="I40" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="74"/>
-      <c r="C41" s="96"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="102"/>
-      <c r="G41" s="93"/>
-      <c r="H41" s="87" t="s">
+      <c r="B41" s="61"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="83"/>
+      <c r="E41" s="94"/>
+      <c r="F41" s="86"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="88"/>
+      <c r="I41" s="78"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B42" s="74"/>
-      <c r="C42" s="97"/>
-      <c r="D42" s="100"/>
-      <c r="E42" s="91"/>
-      <c r="F42" s="103"/>
-      <c r="G42" s="94"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="81"/>
+      <c r="D42" s="84"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="87"/>
+      <c r="G42" s="90"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I42" s="25" t="s">
+      <c r="I42" s="17" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="43" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B43" s="74"/>
-      <c r="C43" s="75" t="s">
+      <c r="B43" s="61"/>
+      <c r="C43" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="47" t="s">
+      <c r="E43" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="F43" s="32" t="s">
+      <c r="F43" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G43" s="41" t="s">
+      <c r="G43" s="31" t="s">
         <v>24</v>
       </c>
       <c r="H43" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I43" s="25" t="s">
+      <c r="I43" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="44" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B44" s="74"/>
-      <c r="C44" s="95" t="s">
+      <c r="B44" s="61"/>
+      <c r="C44" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="98" t="s">
+      <c r="D44" s="82" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="89" t="s">
+      <c r="E44" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="101" t="s">
+      <c r="F44" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="92" t="s">
+      <c r="G44" s="88" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I44" s="24" t="s">
+      <c r="I44" s="16" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="45" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="74"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="99"/>
-      <c r="E45" s="90"/>
-      <c r="F45" s="102"/>
-      <c r="G45" s="93"/>
-      <c r="H45" s="87" t="s">
+      <c r="B45" s="61"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="83"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="86"/>
+      <c r="G45" s="89"/>
+      <c r="H45" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="88"/>
+      <c r="I45" s="78"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="74"/>
-      <c r="C46" s="97"/>
-      <c r="D46" s="100"/>
-      <c r="E46" s="91"/>
-      <c r="F46" s="103"/>
-      <c r="G46" s="94"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="84"/>
+      <c r="E46" s="95"/>
+      <c r="F46" s="87"/>
+      <c r="G46" s="90"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I46" s="25" t="s">
+      <c r="I46" s="17" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="47" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="74"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="17"/>
-      <c r="G47" s="42"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="32"/>
       <c r="H47" s="9"/>
-      <c r="I47" s="27"/>
+      <c r="I47" s="19"/>
     </row>
     <row r="48" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="78"/>
-      <c r="C48" s="79"/>
-      <c r="D48" s="52"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="86"/>
+      <c r="B48" s="65"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="92"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="74" t="s">
+      <c r="B49" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="81" t="s">
+      <c r="C49" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="56"/>
-      <c r="F49" s="57"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="59"/>
-      <c r="I49" s="60"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="49"/>
     </row>
     <row r="50" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="74"/>
-      <c r="C50" s="81" t="s">
+      <c r="B50" s="61"/>
+      <c r="C50" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="E50" s="56"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="60"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="49"/>
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B51" s="74"/>
-      <c r="C51" s="76" t="s">
+      <c r="B51" s="61"/>
+      <c r="C51" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="D51" s="36" t="s">
+      <c r="D51" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E51" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="F51" s="31" t="s">
+      <c r="F51" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="G51" s="40" t="s">
+      <c r="G51" s="30" t="s">
         <v>64</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I51" s="24" t="s">
+      <c r="I51" s="16" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="52" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="74"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="50"/>
-      <c r="F52" s="17"/>
-      <c r="G52" s="42"/>
-      <c r="H52" s="87" t="s">
+      <c r="B52" s="61"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="88"/>
+      <c r="I52" s="78"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="74"/>
-      <c r="C53" s="81"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="41"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="68"/>
+      <c r="D53" s="26"/>
+      <c r="E53" s="42"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="31"/>
       <c r="H53" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I53" s="25" t="s">
+      <c r="I53" s="17" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="54" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="74"/>
-      <c r="C54" s="82"/>
-      <c r="D54" s="19"/>
-      <c r="E54" s="50"/>
-      <c r="F54" s="17"/>
-      <c r="G54" s="42"/>
+      <c r="B54" s="61"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="32"/>
       <c r="H54" s="9"/>
-      <c r="I54" s="27"/>
+      <c r="I54" s="19"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="78"/>
-      <c r="C55" s="79"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="30"/>
-      <c r="G55" s="33"/>
-      <c r="H55" s="85"/>
-      <c r="I55" s="86"/>
+      <c r="B55" s="65"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="25"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="91"/>
+      <c r="I55" s="92"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="74"/>
-      <c r="C56" s="82"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="50"/>
-      <c r="F56" s="17"/>
-      <c r="G56" s="42"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="69"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="32"/>
       <c r="H56" s="9"/>
-      <c r="I56" s="27"/>
+      <c r="I56" s="19"/>
     </row>
     <row r="57" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="74"/>
-      <c r="C57" s="82"/>
-      <c r="D57" s="19"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="17"/>
-      <c r="G57" s="42"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="69"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="32"/>
       <c r="H57" s="9"/>
-      <c r="I57" s="27"/>
+      <c r="I57" s="19"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="74"/>
-      <c r="C58" s="82"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="50"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="42"/>
+      <c r="B58" s="61"/>
+      <c r="C58" s="69"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="32"/>
       <c r="H58" s="9"/>
-      <c r="I58" s="27"/>
+      <c r="I58" s="19"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="74"/>
-      <c r="C59" s="82"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="42"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="32"/>
       <c r="H59" s="9"/>
-      <c r="I59" s="27"/>
+      <c r="I59" s="19"/>
     </row>
     <row r="60" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="74"/>
-      <c r="C60" s="82"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="50"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="42"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="69"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="32"/>
       <c r="H60" s="9"/>
-      <c r="I60" s="27"/>
+      <c r="I60" s="19"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="74"/>
-      <c r="C61" s="82"/>
-      <c r="D61" s="19"/>
-      <c r="E61" s="50"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="42"/>
+      <c r="B61" s="61"/>
+      <c r="C61" s="69"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="32"/>
       <c r="H61" s="9"/>
-      <c r="I61" s="27"/>
+      <c r="I61" s="19"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="74"/>
-      <c r="C62" s="82"/>
-      <c r="D62" s="19"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="42"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="69"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="32"/>
       <c r="H62" s="9"/>
-      <c r="I62" s="27"/>
+      <c r="I62" s="19"/>
     </row>
     <row r="63" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="74"/>
-      <c r="C63" s="82"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="42"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="32"/>
       <c r="H63" s="9"/>
-      <c r="I63" s="27"/>
+      <c r="I63" s="19"/>
     </row>
     <row r="64" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="74"/>
-      <c r="C64" s="82"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="17"/>
-      <c r="G64" s="42"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="69"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="35"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="32"/>
       <c r="H64" s="9"/>
-      <c r="I64" s="27"/>
+      <c r="I64" s="19"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="74"/>
-      <c r="C65" s="82"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="17"/>
-      <c r="G65" s="42"/>
+      <c r="B65" s="61"/>
+      <c r="C65" s="69"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="35"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="32"/>
       <c r="H65" s="9"/>
-      <c r="I65" s="27"/>
+      <c r="I65" s="19"/>
     </row>
     <row r="66" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="74"/>
-      <c r="C66" s="82"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="17"/>
-      <c r="G66" s="42"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="35"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="32"/>
       <c r="H66" s="9"/>
-      <c r="I66" s="27"/>
+      <c r="I66" s="19"/>
     </row>
     <row r="67" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="74"/>
-      <c r="C67" s="82"/>
-      <c r="D67" s="19"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="17"/>
-      <c r="G67" s="42"/>
+      <c r="B67" s="61"/>
+      <c r="C67" s="69"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="35"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="32"/>
       <c r="H67" s="9"/>
-      <c r="I67" s="27"/>
+      <c r="I67" s="19"/>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="74"/>
-      <c r="C68" s="82"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="46"/>
-      <c r="F68" s="17"/>
-      <c r="G68" s="42"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="69"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="35"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="32"/>
       <c r="H68" s="9"/>
-      <c r="I68" s="27"/>
+      <c r="I68" s="19"/>
     </row>
     <row r="69" spans="2:9" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="83"/>
-      <c r="C69" s="84"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="51"/>
-      <c r="F69" s="18"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="28"/>
-      <c r="I69" s="29"/>
+      <c r="B69" s="70"/>
+      <c r="C69" s="71"/>
+      <c r="D69" s="15"/>
+      <c r="E69" s="40"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="33"/>
+      <c r="H69" s="20"/>
+      <c r="I69" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -2803,43 +4711,570 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="97" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="97" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="97" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52" style="97" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41" style="97" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="97"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="116" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="117"/>
+      <c r="D2" s="129" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="131" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="113" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="130"/>
+      <c r="E3" s="132"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="103" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="99" t="s">
+        <v>160</v>
+      </c>
+      <c r="D4" s="120" t="s">
+        <v>175</v>
+      </c>
+      <c r="E4" s="121" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="103"/>
+      <c r="C5" s="99" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="120" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" s="121" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="103"/>
+      <c r="C6" s="99" t="s">
+        <v>162</v>
+      </c>
+      <c r="D6" s="120" t="s">
+        <v>177</v>
+      </c>
+      <c r="E6" s="121" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B7" s="103"/>
+      <c r="C7" s="99" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="120" t="s">
+        <v>178</v>
+      </c>
+      <c r="E7" s="121" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B8" s="103"/>
+      <c r="C8" s="99" t="s">
+        <v>164</v>
+      </c>
+      <c r="D8" s="120" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="121" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="103"/>
+      <c r="C9" s="99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="120" t="s">
+        <v>180</v>
+      </c>
+      <c r="E9" s="121" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="103"/>
+      <c r="C10" s="99" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="120" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="121" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="103"/>
+      <c r="C11" s="99" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="120" t="s">
+        <v>182</v>
+      </c>
+      <c r="E11" s="121" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="103"/>
+      <c r="C12" s="99" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="120" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12" s="121" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="103"/>
+      <c r="C13" s="99" t="s">
+        <v>167</v>
+      </c>
+      <c r="D13" s="120" t="s">
+        <v>184</v>
+      </c>
+      <c r="E13" s="121" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="103"/>
+      <c r="C14" s="99" t="s">
+        <v>168</v>
+      </c>
+      <c r="D14" s="120" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="121" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="103"/>
+      <c r="C15" s="99" t="s">
+        <v>169</v>
+      </c>
+      <c r="D15" s="120" t="s">
+        <v>186</v>
+      </c>
+      <c r="E15" s="121" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="103"/>
+      <c r="C16" s="99" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="120" t="s">
+        <v>187</v>
+      </c>
+      <c r="E16" s="121" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="103"/>
+      <c r="C17" s="99" t="s">
+        <v>170</v>
+      </c>
+      <c r="D17" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E17" s="121" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="103"/>
+      <c r="C18" s="99" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="120" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" s="121" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="103"/>
+      <c r="C19" s="99" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E19" s="121" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="103"/>
+      <c r="C20" s="99" t="s">
+        <v>172</v>
+      </c>
+      <c r="D20" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E20" s="121" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="103"/>
+      <c r="C21" s="99" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E21" s="121" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="104"/>
+      <c r="C22" s="100" t="s">
+        <v>147</v>
+      </c>
+      <c r="D22" s="122" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" s="123" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="101" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="122" t="s">
+        <v>188</v>
+      </c>
+      <c r="E23" s="124" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="103" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="99" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E24" s="121" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="103"/>
+      <c r="C25" s="99" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E25" s="121" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="103"/>
+      <c r="C26" s="99" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" s="121" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="103"/>
+      <c r="C27" s="99" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E27" s="121" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="103"/>
+      <c r="C28" s="99" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E28" s="121" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="103"/>
+      <c r="C29" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E29" s="121" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="103"/>
+      <c r="C30" s="99" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E30" s="121" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="103"/>
+      <c r="C31" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E31" s="121" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="103"/>
+      <c r="C32" s="99" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E32" s="121" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="103"/>
+      <c r="C33" s="99" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E33" s="121" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="103"/>
+      <c r="C34" s="99" t="s">
+        <v>158</v>
+      </c>
+      <c r="D34" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="121" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="103"/>
+      <c r="C35" s="99" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E35" s="121" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="103"/>
+      <c r="C36" s="99" t="s">
+        <v>159</v>
+      </c>
+      <c r="D36" s="120" t="s">
+        <v>188</v>
+      </c>
+      <c r="E36" s="121" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="102" t="s">
+        <v>144</v>
+      </c>
+      <c r="C37" s="98" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="125" t="s">
+        <v>188</v>
+      </c>
+      <c r="E37" s="126" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="106"/>
+      <c r="C38" s="107" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38" s="127" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="128" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="1.42578125" style="96" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="96" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="96" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="96"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="118" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="133" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" s="97" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="109" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="134"/>
+    </row>
+    <row r="4" spans="2:3" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="108" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="135" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="103" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="121" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="103" t="s">
+        <v>143</v>
+      </c>
+      <c r="C6" s="121" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="106" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="128" t="s">
+        <v>225</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pertanggal 6 Januari 2023 19:29 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -809,9 +809,6 @@
     <t>Mendapatkan Data List File Upload Staging Area pada Local Storage</t>
   </si>
   <si>
-    <t>Func_GetData_APIWebTokenByUserSessionID</t>
-  </si>
-  <si>
     <t>Mendapatkan API Web Token dari User Session ID</t>
   </si>
   <si>
@@ -860,7 +857,25 @@
     <t>Mendapatkan API Web Token untuk SysEngine</t>
   </si>
   <si>
-    <t>Func_GetData_APIWebTokenOfSysEngine</t>
+    <t>FuncSys_General_GetAllExtensionsName</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama Extension yang terdapat didalam sistem</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllForeignObjectsEntity</t>
+  </si>
+  <si>
+    <t>1.00.0001</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh entitas Foreign yang terdapat didalam sistem</t>
+  </si>
+  <si>
+    <t>Func_GetData_APIWebToken_ByUserSessionID</t>
+  </si>
+  <si>
+    <t>Func_GetData_APIWebToken_SysEngine</t>
   </si>
   <si>
     <r>
@@ -873,23 +888,8 @@
         <rFont val="Arial Narrow"/>
         <family val="2"/>
       </rPr>
-      <t>SchSysAsset.Func_GetData_APIWebTokenOfSysEngine</t>
+      <t>SchSysAsset.Func_GetData_APIWebToken_SysEngine</t>
     </r>
-  </si>
-  <si>
-    <t>FuncSys_General_GetAllExtensionsName</t>
-  </si>
-  <si>
-    <t>Menampilkan seluruh nama Extension yang terdapat didalam sistem</t>
-  </si>
-  <si>
-    <t>FuncSys_General_GetAllForeignObjectsEntity</t>
-  </si>
-  <si>
-    <t>1.00.0001</t>
-  </si>
-  <si>
-    <t>Menampilkan seluruh entitas Foreign yang terdapat didalam sistem</t>
   </si>
 </sst>
 </file>
@@ -897,7 +897,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1848,63 +1848,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1921,15 +1864,6 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1938,12 +1872,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1960,74 +1888,32 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="12" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="12" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2035,40 +1921,154 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2383,1202 +2383,1202 @@
   <dimension ref="B1:H109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="96" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="96" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" style="96" customWidth="1"/>
-    <col min="4" max="4" width="45.140625" style="96" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.140625" style="96" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="146" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="147" customWidth="1"/>
-    <col min="8" max="8" width="16" style="147" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="96"/>
+    <col min="1" max="1" width="1.42578125" style="77" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" style="77" customWidth="1"/>
+    <col min="4" max="4" width="45.140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="66.140625" style="77" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="109" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="110" customWidth="1"/>
+    <col min="8" max="8" width="16" style="110" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="139" t="s">
+      <c r="B2" s="130" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="144" t="s">
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="132" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="141" t="s">
+      <c r="F2" s="134" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="142"/>
-      <c r="H2" s="145"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="136"/>
     </row>
     <row r="3" spans="2:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="91" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="143" t="s">
+      <c r="D3" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="149"/>
-      <c r="F3" s="150" t="s">
+      <c r="E3" s="133"/>
+      <c r="F3" s="112" t="s">
         <v>228</v>
       </c>
-      <c r="G3" s="151" t="s">
+      <c r="G3" s="113" t="s">
         <v>229</v>
       </c>
-      <c r="H3" s="152" t="s">
+      <c r="H3" s="114" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="108" t="s">
+    <row r="4" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="153" t="s">
+      <c r="C4" s="115" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="153" t="s">
+      <c r="D4" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="E4" s="154" t="s">
+      <c r="E4" s="116" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="155" t="s">
+      <c r="F4" s="117" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="156">
+      <c r="G4" s="118">
         <v>44910</v>
       </c>
-      <c r="H4" s="157">
+      <c r="H4" s="119">
         <v>44910</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="103"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99" t="s">
+    <row r="5" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="84"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="120" t="s">
+      <c r="E5" s="96" t="s">
         <v>236</v>
       </c>
-      <c r="F5" s="161" t="s">
+      <c r="F5" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G5" s="162">
+      <c r="G5" s="124">
         <v>44908</v>
       </c>
-      <c r="H5" s="163">
+      <c r="H5" s="125">
         <v>44908</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="103"/>
-      <c r="C6" s="99"/>
-      <c r="D6" s="99" t="s">
+    <row r="6" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="84"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="120" t="s">
+      <c r="E6" s="96" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="161" t="s">
+      <c r="F6" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G6" s="162">
+      <c r="G6" s="124">
         <v>44908</v>
       </c>
-      <c r="H6" s="163">
+      <c r="H6" s="125">
         <v>44908</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="103"/>
-      <c r="C7" s="99"/>
-      <c r="D7" s="99" t="s">
+    <row r="7" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B7" s="84"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80" t="s">
         <v>238</v>
       </c>
-      <c r="E7" s="120" t="s">
+      <c r="E7" s="96" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="161" t="s">
+      <c r="F7" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G7" s="162">
+      <c r="G7" s="124">
         <v>44887</v>
       </c>
-      <c r="H7" s="163">
+      <c r="H7" s="125">
         <v>44887</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="103"/>
-      <c r="C8" s="99"/>
-      <c r="D8" s="99" t="s">
+    <row r="8" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B8" s="84"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="120" t="s">
+      <c r="E8" s="96" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="161" t="s">
+      <c r="F8" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="162">
+      <c r="G8" s="124">
         <v>44887</v>
       </c>
-      <c r="H8" s="163">
+      <c r="H8" s="125">
         <v>44887</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="103"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99" t="s">
+    <row r="9" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B9" s="84"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80" t="s">
         <v>242</v>
       </c>
-      <c r="E9" s="120" t="s">
+      <c r="E9" s="96" t="s">
         <v>243</v>
       </c>
-      <c r="F9" s="161" t="s">
+      <c r="F9" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G9" s="162">
+      <c r="G9" s="124">
         <v>44774</v>
       </c>
-      <c r="H9" s="163">
+      <c r="H9" s="125">
         <v>44774</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="103"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99" t="s">
+    <row r="10" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B10" s="84"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80" t="s">
         <v>244</v>
       </c>
-      <c r="E10" s="120" t="s">
+      <c r="E10" s="96" t="s">
         <v>245</v>
       </c>
-      <c r="F10" s="161" t="s">
+      <c r="F10" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="162">
+      <c r="G10" s="124">
         <v>44897</v>
       </c>
-      <c r="H10" s="163">
+      <c r="H10" s="125">
         <v>44897</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="103"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99" t="s">
+    <row r="11" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B11" s="84"/>
+      <c r="C11" s="80"/>
+      <c r="D11" s="80" t="s">
         <v>246</v>
       </c>
-      <c r="E11" s="120" t="s">
+      <c r="E11" s="96" t="s">
         <v>247</v>
       </c>
-      <c r="F11" s="161" t="s">
+      <c r="F11" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="162">
+      <c r="G11" s="124">
         <v>44897</v>
       </c>
-      <c r="H11" s="163">
+      <c r="H11" s="125">
         <v>44897</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="103"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99" t="s">
+    <row r="12" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B12" s="84"/>
+      <c r="C12" s="80"/>
+      <c r="D12" s="80" t="s">
         <v>248</v>
       </c>
-      <c r="E12" s="120" t="s">
+      <c r="E12" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="F12" s="161" t="s">
+      <c r="F12" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G12" s="162">
+      <c r="G12" s="124">
         <v>44748</v>
       </c>
-      <c r="H12" s="163">
+      <c r="H12" s="125">
         <v>44748</v>
       </c>
     </row>
-    <row r="13" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="103"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99" t="s">
+    <row r="13" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B13" s="84"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80" t="s">
         <v>250</v>
       </c>
-      <c r="E13" s="120" t="s">
+      <c r="E13" s="96" t="s">
         <v>251</v>
       </c>
-      <c r="F13" s="161" t="s">
+      <c r="F13" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G13" s="162">
+      <c r="G13" s="124">
         <v>44735</v>
       </c>
-      <c r="H13" s="163">
+      <c r="H13" s="125">
         <v>44735</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="103"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99" t="s">
+    <row r="14" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B14" s="84"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="120" t="s">
+      <c r="E14" s="96" t="s">
         <v>253</v>
       </c>
-      <c r="F14" s="161" t="s">
+      <c r="F14" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G14" s="162">
+      <c r="G14" s="124">
         <v>44854</v>
       </c>
-      <c r="H14" s="163">
+      <c r="H14" s="125">
         <v>44854</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="103"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99" t="s">
+    <row r="15" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B15" s="84"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80" t="s">
         <v>254</v>
       </c>
-      <c r="E15" s="120" t="s">
+      <c r="E15" s="96" t="s">
         <v>259</v>
       </c>
-      <c r="F15" s="161" t="s">
+      <c r="F15" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G15" s="162">
+      <c r="G15" s="124">
         <v>44770</v>
       </c>
-      <c r="H15" s="163">
+      <c r="H15" s="125">
         <v>44770</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="103"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99" t="s">
+    <row r="16" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B16" s="84"/>
+      <c r="C16" s="80"/>
+      <c r="D16" s="80" t="s">
         <v>255</v>
       </c>
-      <c r="E16" s="120" t="s">
+      <c r="E16" s="96" t="s">
         <v>260</v>
       </c>
-      <c r="F16" s="161" t="s">
+      <c r="F16" s="123" t="s">
         <v>256</v>
       </c>
-      <c r="G16" s="162">
+      <c r="G16" s="124">
         <v>44770</v>
       </c>
-      <c r="H16" s="163">
+      <c r="H16" s="125">
         <v>44427</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="103"/>
-      <c r="C17" s="99"/>
-      <c r="D17" s="99" t="s">
+    <row r="17" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B17" s="84"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="120" t="s">
+      <c r="E17" s="96" t="s">
         <v>261</v>
       </c>
-      <c r="F17" s="161" t="s">
+      <c r="F17" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G17" s="162">
+      <c r="G17" s="124">
         <v>44770</v>
       </c>
-      <c r="H17" s="163">
+      <c r="H17" s="125">
         <v>44770</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="103"/>
-      <c r="C18" s="99"/>
-      <c r="D18" s="99" t="s">
+    <row r="18" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B18" s="84"/>
+      <c r="C18" s="80"/>
+      <c r="D18" s="80" t="s">
         <v>258</v>
       </c>
-      <c r="E18" s="120" t="s">
+      <c r="E18" s="96" t="s">
         <v>262</v>
       </c>
-      <c r="F18" s="161" t="s">
+      <c r="F18" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G18" s="162">
+      <c r="G18" s="124">
         <v>44770</v>
       </c>
-      <c r="H18" s="163">
+      <c r="H18" s="125">
         <v>44427</v>
       </c>
     </row>
-    <row r="19" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="103"/>
-      <c r="C19" s="99"/>
-      <c r="D19" s="99" t="s">
+    <row r="19" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B19" s="84"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="80" t="s">
+        <v>284</v>
+      </c>
+      <c r="E19" s="96" t="s">
         <v>263</v>
       </c>
-      <c r="E19" s="120" t="s">
+      <c r="F19" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="G19" s="124">
+        <v>44777</v>
+      </c>
+      <c r="H19" s="125">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B20" s="84"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="80" t="s">
+        <v>285</v>
+      </c>
+      <c r="E20" s="96" t="s">
+        <v>278</v>
+      </c>
+      <c r="F20" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="G20" s="124">
+        <v>44931</v>
+      </c>
+      <c r="H20" s="125">
+        <v>44931</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B21" s="84"/>
+      <c r="C21" s="80"/>
+      <c r="D21" s="80" t="s">
         <v>264</v>
       </c>
-      <c r="F19" s="161" t="s">
+      <c r="E21" s="96" t="s">
+        <v>265</v>
+      </c>
+      <c r="F21" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G19" s="162">
+      <c r="G21" s="124">
+        <v>44847</v>
+      </c>
+      <c r="H21" s="125">
+        <v>44847</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B22" s="84"/>
+      <c r="C22" s="80"/>
+      <c r="D22" s="80" t="s">
+        <v>266</v>
+      </c>
+      <c r="E22" s="96" t="s">
+        <v>268</v>
+      </c>
+      <c r="F22" s="123" t="s">
+        <v>267</v>
+      </c>
+      <c r="G22" s="124">
+        <v>44792</v>
+      </c>
+      <c r="H22" s="125">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B23" s="84"/>
+      <c r="C23" s="80"/>
+      <c r="D23" s="80" t="s">
+        <v>269</v>
+      </c>
+      <c r="E23" s="96" t="s">
+        <v>270</v>
+      </c>
+      <c r="F23" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="G23" s="124">
+        <v>44776</v>
+      </c>
+      <c r="H23" s="125">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B24" s="84"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80" t="s">
+        <v>272</v>
+      </c>
+      <c r="E24" s="96" t="s">
+        <v>271</v>
+      </c>
+      <c r="F24" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="G24" s="124">
         <v>44777</v>
       </c>
-      <c r="H19" s="163">
+      <c r="H24" s="125">
         <v>44777</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="103"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99" t="s">
+    <row r="25" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B25" s="84"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="80" t="s">
+        <v>273</v>
+      </c>
+      <c r="E25" s="96" t="s">
+        <v>274</v>
+      </c>
+      <c r="F25" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="G25" s="124">
+        <v>44770</v>
+      </c>
+      <c r="H25" s="125">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B26" s="84"/>
+      <c r="C26" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="D26" s="79" t="s">
+        <v>275</v>
+      </c>
+      <c r="E26" s="101" t="s">
+        <v>276</v>
+      </c>
+      <c r="F26" s="126" t="s">
+        <v>232</v>
+      </c>
+      <c r="G26" s="127">
+        <v>44167</v>
+      </c>
+      <c r="H26" s="128">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B27" s="84"/>
+      <c r="C27" s="80"/>
+      <c r="D27" s="129" t="s">
+        <v>277</v>
+      </c>
+      <c r="E27" s="96" t="s">
+        <v>286</v>
+      </c>
+      <c r="F27" s="123" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="124">
+        <v>44167</v>
+      </c>
+      <c r="H27" s="125">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B28" s="84"/>
+      <c r="C28" s="80"/>
+      <c r="D28" s="80" t="s">
+        <v>279</v>
+      </c>
+      <c r="E28" s="96" t="s">
         <v>280</v>
       </c>
-      <c r="E20" s="120" t="s">
-        <v>279</v>
-      </c>
-      <c r="F20" s="161" t="s">
+      <c r="F28" s="123" t="s">
         <v>232</v>
       </c>
-      <c r="G20" s="162">
-        <v>44931</v>
-      </c>
-      <c r="H20" s="163">
-        <v>44931</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B21" s="103"/>
-      <c r="C21" s="99"/>
-      <c r="D21" s="99" t="s">
-        <v>265</v>
-      </c>
-      <c r="E21" s="120" t="s">
-        <v>266</v>
-      </c>
-      <c r="F21" s="161" t="s">
-        <v>232</v>
-      </c>
-      <c r="G21" s="162">
-        <v>44847</v>
-      </c>
-      <c r="H21" s="163">
-        <v>44847</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B22" s="103"/>
-      <c r="C22" s="99"/>
-      <c r="D22" s="99" t="s">
-        <v>267</v>
-      </c>
-      <c r="E22" s="120" t="s">
-        <v>269</v>
-      </c>
-      <c r="F22" s="161" t="s">
-        <v>268</v>
-      </c>
-      <c r="G22" s="162">
-        <v>44792</v>
-      </c>
-      <c r="H22" s="163">
-        <v>44770</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="103"/>
-      <c r="C23" s="99"/>
-      <c r="D23" s="99" t="s">
-        <v>270</v>
-      </c>
-      <c r="E23" s="120" t="s">
-        <v>271</v>
-      </c>
-      <c r="F23" s="161" t="s">
-        <v>232</v>
-      </c>
-      <c r="G23" s="162">
-        <v>44776</v>
-      </c>
-      <c r="H23" s="163">
-        <v>44776</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="103"/>
-      <c r="C24" s="99"/>
-      <c r="D24" s="99" t="s">
-        <v>273</v>
-      </c>
-      <c r="E24" s="120" t="s">
-        <v>272</v>
-      </c>
-      <c r="F24" s="161" t="s">
-        <v>232</v>
-      </c>
-      <c r="G24" s="162">
-        <v>44777</v>
-      </c>
-      <c r="H24" s="163">
-        <v>44777</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="103"/>
-      <c r="C25" s="99"/>
-      <c r="D25" s="99" t="s">
-        <v>274</v>
-      </c>
-      <c r="E25" s="120" t="s">
-        <v>275</v>
-      </c>
-      <c r="F25" s="161" t="s">
-        <v>232</v>
-      </c>
-      <c r="G25" s="162">
-        <v>44770</v>
-      </c>
-      <c r="H25" s="163">
-        <v>44770</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="103"/>
-      <c r="C26" s="98" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="98" t="s">
-        <v>276</v>
-      </c>
-      <c r="E26" s="125" t="s">
-        <v>277</v>
-      </c>
-      <c r="F26" s="164" t="s">
-        <v>232</v>
-      </c>
-      <c r="G26" s="165">
-        <v>44167</v>
-      </c>
-      <c r="H26" s="166">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="103"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="167" t="s">
-        <v>278</v>
-      </c>
-      <c r="E27" s="120" t="s">
+      <c r="G28" s="124">
+        <v>43185</v>
+      </c>
+      <c r="H28" s="125">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B29" s="84"/>
+      <c r="C29" s="80"/>
+      <c r="D29" s="80" t="s">
         <v>281</v>
       </c>
-      <c r="F27" s="161" t="s">
-        <v>232</v>
-      </c>
-      <c r="G27" s="162">
-        <v>44167</v>
-      </c>
-      <c r="H27" s="163">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B28" s="103"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="99" t="s">
+      <c r="E29" s="96" t="s">
+        <v>283</v>
+      </c>
+      <c r="F29" s="123" t="s">
         <v>282</v>
       </c>
-      <c r="E28" s="120" t="s">
-        <v>283</v>
-      </c>
-      <c r="F28" s="161" t="s">
-        <v>232</v>
-      </c>
-      <c r="G28" s="162">
-        <v>43185</v>
-      </c>
-      <c r="H28" s="163">
-        <v>43185</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="103"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99" t="s">
-        <v>284</v>
-      </c>
-      <c r="E29" s="120" t="s">
-        <v>286</v>
-      </c>
-      <c r="F29" s="161" t="s">
-        <v>285</v>
-      </c>
-      <c r="G29" s="162">
+      <c r="G29" s="124">
         <v>44216</v>
       </c>
-      <c r="H29" s="163">
+      <c r="H29" s="125">
         <v>44216</v>
       </c>
     </row>
-    <row r="30" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="103"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="99"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="161"/>
-      <c r="G30" s="162"/>
-      <c r="H30" s="163"/>
-    </row>
-    <row r="31" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B31" s="103"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="99"/>
-      <c r="E31" s="120"/>
-      <c r="F31" s="161"/>
-      <c r="G31" s="162"/>
-      <c r="H31" s="163"/>
-    </row>
-    <row r="32" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="103"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="99"/>
-      <c r="E32" s="120"/>
-      <c r="F32" s="161"/>
-      <c r="G32" s="162"/>
-      <c r="H32" s="163"/>
-    </row>
-    <row r="33" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B33" s="103"/>
-      <c r="C33" s="99"/>
-      <c r="D33" s="99"/>
-      <c r="E33" s="120"/>
-      <c r="F33" s="161"/>
-      <c r="G33" s="162"/>
-      <c r="H33" s="163"/>
-    </row>
-    <row r="34" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B34" s="103"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="120"/>
-      <c r="F34" s="161"/>
-      <c r="G34" s="162"/>
-      <c r="H34" s="163"/>
-    </row>
-    <row r="35" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="103"/>
-      <c r="C35" s="99"/>
-      <c r="D35" s="99"/>
-      <c r="E35" s="120"/>
-      <c r="F35" s="161"/>
-      <c r="G35" s="162"/>
-      <c r="H35" s="163"/>
-    </row>
-    <row r="36" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B36" s="103"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="99"/>
-      <c r="E36" s="120"/>
-      <c r="F36" s="161"/>
-      <c r="G36" s="162"/>
-      <c r="H36" s="163"/>
-    </row>
-    <row r="37" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B37" s="103"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="120"/>
-      <c r="F37" s="161"/>
-      <c r="G37" s="162"/>
-      <c r="H37" s="163"/>
-    </row>
-    <row r="38" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B38" s="103"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="99"/>
-      <c r="E38" s="120"/>
-      <c r="F38" s="161"/>
-      <c r="G38" s="162"/>
-      <c r="H38" s="163"/>
-    </row>
-    <row r="39" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B39" s="103"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="120"/>
-      <c r="F39" s="161"/>
-      <c r="G39" s="162"/>
-      <c r="H39" s="163"/>
-    </row>
-    <row r="40" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B40" s="103"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="120"/>
-      <c r="F40" s="161"/>
-      <c r="G40" s="162"/>
-      <c r="H40" s="163"/>
-    </row>
-    <row r="41" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B41" s="103"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="120"/>
-      <c r="F41" s="161"/>
-      <c r="G41" s="162"/>
-      <c r="H41" s="163"/>
-    </row>
-    <row r="42" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B42" s="103"/>
-      <c r="C42" s="99"/>
-      <c r="D42" s="99"/>
-      <c r="E42" s="120"/>
-      <c r="F42" s="161"/>
-      <c r="G42" s="162"/>
-      <c r="H42" s="163"/>
-    </row>
-    <row r="43" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B43" s="103"/>
-      <c r="C43" s="99"/>
-      <c r="D43" s="99"/>
-      <c r="E43" s="120"/>
-      <c r="F43" s="161"/>
-      <c r="G43" s="162"/>
-      <c r="H43" s="163"/>
-    </row>
-    <row r="44" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B44" s="103"/>
-      <c r="C44" s="99"/>
-      <c r="D44" s="99"/>
-      <c r="E44" s="120"/>
-      <c r="F44" s="161"/>
-      <c r="G44" s="162"/>
-      <c r="H44" s="163"/>
-    </row>
-    <row r="45" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B45" s="103"/>
-      <c r="C45" s="99"/>
-      <c r="D45" s="99"/>
-      <c r="E45" s="120"/>
-      <c r="F45" s="161"/>
-      <c r="G45" s="162"/>
-      <c r="H45" s="163"/>
-    </row>
-    <row r="46" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B46" s="103"/>
-      <c r="C46" s="99"/>
-      <c r="D46" s="99"/>
-      <c r="E46" s="120"/>
-      <c r="F46" s="161"/>
-      <c r="G46" s="162"/>
-      <c r="H46" s="163"/>
-    </row>
-    <row r="47" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="103"/>
-      <c r="C47" s="99"/>
-      <c r="D47" s="99"/>
-      <c r="E47" s="120"/>
-      <c r="F47" s="161"/>
-      <c r="G47" s="162"/>
-      <c r="H47" s="163"/>
-    </row>
-    <row r="48" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B48" s="103"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="120"/>
-      <c r="F48" s="161"/>
-      <c r="G48" s="162"/>
-      <c r="H48" s="163"/>
-    </row>
-    <row r="49" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B49" s="103"/>
-      <c r="C49" s="99"/>
-      <c r="D49" s="99"/>
-      <c r="E49" s="120"/>
-      <c r="F49" s="161"/>
-      <c r="G49" s="162"/>
-      <c r="H49" s="163"/>
-    </row>
-    <row r="50" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B50" s="103"/>
-      <c r="C50" s="99"/>
-      <c r="D50" s="99"/>
-      <c r="E50" s="120"/>
-      <c r="F50" s="161"/>
-      <c r="G50" s="162"/>
-      <c r="H50" s="163"/>
-    </row>
-    <row r="51" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B51" s="103"/>
-      <c r="C51" s="99"/>
-      <c r="D51" s="99"/>
-      <c r="E51" s="120"/>
-      <c r="F51" s="161"/>
-      <c r="G51" s="162"/>
-      <c r="H51" s="163"/>
-    </row>
-    <row r="52" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B52" s="103"/>
-      <c r="C52" s="99"/>
-      <c r="D52" s="99"/>
-      <c r="E52" s="120"/>
-      <c r="F52" s="161"/>
-      <c r="G52" s="162"/>
-      <c r="H52" s="163"/>
-    </row>
-    <row r="53" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B53" s="103"/>
-      <c r="C53" s="99"/>
-      <c r="D53" s="99"/>
-      <c r="E53" s="120"/>
-      <c r="F53" s="161"/>
-      <c r="G53" s="162"/>
-      <c r="H53" s="163"/>
-    </row>
-    <row r="54" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B54" s="103"/>
-      <c r="C54" s="99"/>
-      <c r="D54" s="99"/>
-      <c r="E54" s="120"/>
-      <c r="F54" s="161"/>
-      <c r="G54" s="162"/>
-      <c r="H54" s="163"/>
-    </row>
-    <row r="55" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B55" s="103"/>
-      <c r="C55" s="99"/>
-      <c r="D55" s="99"/>
-      <c r="E55" s="120"/>
-      <c r="F55" s="161"/>
-      <c r="G55" s="162"/>
-      <c r="H55" s="163"/>
-    </row>
-    <row r="56" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B56" s="103"/>
-      <c r="C56" s="99"/>
-      <c r="D56" s="99"/>
-      <c r="E56" s="120"/>
-      <c r="F56" s="161"/>
-      <c r="G56" s="162"/>
-      <c r="H56" s="163"/>
-    </row>
-    <row r="57" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B57" s="103"/>
-      <c r="C57" s="99"/>
-      <c r="D57" s="99"/>
-      <c r="E57" s="120"/>
-      <c r="F57" s="161"/>
-      <c r="G57" s="162"/>
-      <c r="H57" s="163"/>
-    </row>
-    <row r="58" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B58" s="103"/>
-      <c r="C58" s="99"/>
-      <c r="D58" s="99"/>
-      <c r="E58" s="120"/>
-      <c r="F58" s="161"/>
-      <c r="G58" s="162"/>
-      <c r="H58" s="163"/>
-    </row>
-    <row r="59" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B59" s="103"/>
-      <c r="C59" s="99"/>
-      <c r="D59" s="99"/>
-      <c r="E59" s="120"/>
-      <c r="F59" s="161"/>
-      <c r="G59" s="162"/>
-      <c r="H59" s="163"/>
-    </row>
-    <row r="60" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B60" s="103"/>
-      <c r="C60" s="99"/>
-      <c r="D60" s="99"/>
-      <c r="E60" s="120"/>
-      <c r="F60" s="161"/>
-      <c r="G60" s="162"/>
-      <c r="H60" s="163"/>
-    </row>
-    <row r="61" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B61" s="103"/>
-      <c r="C61" s="99"/>
-      <c r="D61" s="99"/>
-      <c r="E61" s="120"/>
-      <c r="F61" s="161"/>
-      <c r="G61" s="162"/>
-      <c r="H61" s="163"/>
-    </row>
-    <row r="62" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B62" s="103"/>
-      <c r="C62" s="99"/>
-      <c r="D62" s="99"/>
-      <c r="E62" s="120"/>
-      <c r="F62" s="161"/>
-      <c r="G62" s="162"/>
-      <c r="H62" s="163"/>
-    </row>
-    <row r="63" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B63" s="103"/>
-      <c r="C63" s="99"/>
-      <c r="D63" s="99"/>
-      <c r="E63" s="120"/>
-      <c r="F63" s="161"/>
-      <c r="G63" s="162"/>
-      <c r="H63" s="163"/>
-    </row>
-    <row r="64" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="103"/>
-      <c r="C64" s="99"/>
-      <c r="D64" s="99"/>
-      <c r="E64" s="120"/>
-      <c r="F64" s="161"/>
-      <c r="G64" s="162"/>
-      <c r="H64" s="163"/>
-    </row>
-    <row r="65" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="103"/>
-      <c r="C65" s="99"/>
-      <c r="D65" s="99"/>
-      <c r="E65" s="120"/>
-      <c r="F65" s="161"/>
-      <c r="G65" s="162"/>
-      <c r="H65" s="163"/>
-    </row>
-    <row r="66" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="103"/>
-      <c r="C66" s="99"/>
-      <c r="D66" s="99"/>
-      <c r="E66" s="120"/>
-      <c r="F66" s="161"/>
-      <c r="G66" s="162"/>
-      <c r="H66" s="163"/>
-    </row>
-    <row r="67" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="103"/>
-      <c r="C67" s="99"/>
-      <c r="D67" s="99"/>
-      <c r="E67" s="120"/>
-      <c r="F67" s="161"/>
-      <c r="G67" s="162"/>
-      <c r="H67" s="163"/>
-    </row>
-    <row r="68" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="103"/>
-      <c r="C68" s="99"/>
-      <c r="D68" s="99"/>
-      <c r="E68" s="120"/>
-      <c r="F68" s="161"/>
-      <c r="G68" s="162"/>
-      <c r="H68" s="163"/>
-    </row>
-    <row r="69" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B69" s="103"/>
-      <c r="C69" s="99"/>
-      <c r="D69" s="99"/>
-      <c r="E69" s="120"/>
-      <c r="F69" s="161"/>
-      <c r="G69" s="162"/>
-      <c r="H69" s="163"/>
-    </row>
-    <row r="70" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B70" s="103"/>
-      <c r="C70" s="99"/>
-      <c r="D70" s="99"/>
-      <c r="E70" s="120"/>
-      <c r="F70" s="161"/>
-      <c r="G70" s="162"/>
-      <c r="H70" s="163"/>
-    </row>
-    <row r="71" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="103"/>
-      <c r="C71" s="99"/>
-      <c r="D71" s="99"/>
-      <c r="E71" s="120"/>
-      <c r="F71" s="161"/>
-      <c r="G71" s="162"/>
-      <c r="H71" s="163"/>
-    </row>
-    <row r="72" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B72" s="103"/>
-      <c r="C72" s="99"/>
-      <c r="D72" s="99"/>
-      <c r="E72" s="120"/>
-      <c r="F72" s="161"/>
-      <c r="G72" s="162"/>
-      <c r="H72" s="163"/>
-    </row>
-    <row r="73" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B73" s="103"/>
-      <c r="C73" s="99"/>
-      <c r="D73" s="99"/>
-      <c r="E73" s="120"/>
-      <c r="F73" s="161"/>
-      <c r="G73" s="162"/>
-      <c r="H73" s="163"/>
-    </row>
-    <row r="74" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B74" s="103"/>
-      <c r="C74" s="99"/>
-      <c r="D74" s="99"/>
-      <c r="E74" s="120"/>
-      <c r="F74" s="161"/>
-      <c r="G74" s="162"/>
-      <c r="H74" s="163"/>
-    </row>
-    <row r="75" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B75" s="103"/>
-      <c r="C75" s="99"/>
-      <c r="D75" s="99"/>
-      <c r="E75" s="120"/>
-      <c r="F75" s="161"/>
-      <c r="G75" s="162"/>
-      <c r="H75" s="163"/>
-    </row>
-    <row r="76" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B76" s="103"/>
-      <c r="C76" s="99"/>
-      <c r="D76" s="99"/>
-      <c r="E76" s="120"/>
-      <c r="F76" s="161"/>
-      <c r="G76" s="162"/>
-      <c r="H76" s="163"/>
-    </row>
-    <row r="77" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B77" s="103"/>
-      <c r="C77" s="99"/>
-      <c r="D77" s="99"/>
-      <c r="E77" s="120"/>
-      <c r="F77" s="161"/>
-      <c r="G77" s="162"/>
-      <c r="H77" s="163"/>
-    </row>
-    <row r="78" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B78" s="103"/>
-      <c r="C78" s="99"/>
-      <c r="D78" s="99"/>
-      <c r="E78" s="120"/>
-      <c r="F78" s="161"/>
-      <c r="G78" s="162"/>
-      <c r="H78" s="163"/>
-    </row>
-    <row r="79" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B79" s="103"/>
-      <c r="C79" s="99"/>
-      <c r="D79" s="99"/>
-      <c r="E79" s="120"/>
-      <c r="F79" s="161"/>
-      <c r="G79" s="162"/>
-      <c r="H79" s="163"/>
-    </row>
-    <row r="80" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="103"/>
-      <c r="C80" s="99"/>
-      <c r="D80" s="99"/>
-      <c r="E80" s="120"/>
-      <c r="F80" s="161"/>
-      <c r="G80" s="162"/>
-      <c r="H80" s="163"/>
-    </row>
-    <row r="81" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="103"/>
-      <c r="C81" s="99"/>
-      <c r="D81" s="99"/>
-      <c r="E81" s="120"/>
-      <c r="F81" s="161"/>
-      <c r="G81" s="162"/>
-      <c r="H81" s="163"/>
-    </row>
-    <row r="82" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B82" s="103"/>
-      <c r="C82" s="99"/>
-      <c r="D82" s="99"/>
-      <c r="E82" s="120"/>
-      <c r="F82" s="161"/>
-      <c r="G82" s="162"/>
-      <c r="H82" s="163"/>
-    </row>
-    <row r="83" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B83" s="103"/>
-      <c r="C83" s="99"/>
-      <c r="D83" s="99"/>
-      <c r="E83" s="120"/>
-      <c r="F83" s="161"/>
-      <c r="G83" s="162"/>
-      <c r="H83" s="163"/>
-    </row>
-    <row r="84" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B84" s="103"/>
-      <c r="C84" s="99"/>
-      <c r="D84" s="99"/>
-      <c r="E84" s="120"/>
-      <c r="F84" s="161"/>
-      <c r="G84" s="162"/>
-      <c r="H84" s="163"/>
-    </row>
-    <row r="85" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B85" s="103"/>
-      <c r="C85" s="99"/>
-      <c r="D85" s="99"/>
-      <c r="E85" s="120"/>
-      <c r="F85" s="161"/>
-      <c r="G85" s="162"/>
-      <c r="H85" s="163"/>
-    </row>
-    <row r="86" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B86" s="103"/>
-      <c r="C86" s="99"/>
-      <c r="D86" s="99"/>
-      <c r="E86" s="120"/>
-      <c r="F86" s="161"/>
-      <c r="G86" s="162"/>
-      <c r="H86" s="163"/>
-    </row>
-    <row r="87" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B87" s="103"/>
-      <c r="C87" s="99"/>
-      <c r="D87" s="99"/>
-      <c r="E87" s="120"/>
-      <c r="F87" s="161"/>
-      <c r="G87" s="162"/>
-      <c r="H87" s="163"/>
-    </row>
-    <row r="88" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B88" s="103"/>
-      <c r="C88" s="99"/>
-      <c r="D88" s="99"/>
-      <c r="E88" s="120"/>
-      <c r="F88" s="161"/>
-      <c r="G88" s="162"/>
-      <c r="H88" s="163"/>
-    </row>
-    <row r="89" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B89" s="103"/>
-      <c r="C89" s="99"/>
-      <c r="D89" s="99"/>
-      <c r="E89" s="120"/>
-      <c r="F89" s="161"/>
-      <c r="G89" s="162"/>
-      <c r="H89" s="163"/>
-    </row>
-    <row r="90" spans="2:8" s="97" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="106"/>
-      <c r="C90" s="107"/>
-      <c r="D90" s="107"/>
-      <c r="E90" s="127"/>
-      <c r="F90" s="158"/>
-      <c r="G90" s="159"/>
-      <c r="H90" s="160"/>
-    </row>
-    <row r="91" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F91" s="119"/>
-      <c r="G91" s="148"/>
-      <c r="H91" s="148"/>
-    </row>
-    <row r="92" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F92" s="119"/>
-      <c r="G92" s="148"/>
-      <c r="H92" s="148"/>
-    </row>
-    <row r="93" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F93" s="119"/>
-      <c r="G93" s="148"/>
-      <c r="H93" s="148"/>
-    </row>
-    <row r="94" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F94" s="119"/>
-      <c r="G94" s="148"/>
-      <c r="H94" s="148"/>
-    </row>
-    <row r="95" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F95" s="119"/>
-      <c r="G95" s="148"/>
-      <c r="H95" s="148"/>
-    </row>
-    <row r="96" spans="2:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F96" s="119"/>
-      <c r="G96" s="148"/>
-      <c r="H96" s="148"/>
-    </row>
-    <row r="97" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F97" s="119"/>
-      <c r="G97" s="148"/>
-      <c r="H97" s="148"/>
-    </row>
-    <row r="98" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F98" s="119"/>
-      <c r="G98" s="148"/>
-      <c r="H98" s="148"/>
-    </row>
-    <row r="99" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F99" s="119"/>
-      <c r="G99" s="148"/>
-      <c r="H99" s="148"/>
-    </row>
-    <row r="100" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F100" s="119"/>
-      <c r="G100" s="148"/>
-      <c r="H100" s="148"/>
-    </row>
-    <row r="101" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F101" s="119"/>
-      <c r="G101" s="148"/>
-      <c r="H101" s="148"/>
-    </row>
-    <row r="102" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F102" s="119"/>
-      <c r="G102" s="148"/>
-      <c r="H102" s="148"/>
-    </row>
-    <row r="103" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F103" s="119"/>
-      <c r="G103" s="148"/>
-      <c r="H103" s="148"/>
-    </row>
-    <row r="104" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F104" s="119"/>
-      <c r="G104" s="148"/>
-      <c r="H104" s="148"/>
-    </row>
-    <row r="105" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F105" s="119"/>
-      <c r="G105" s="148"/>
-      <c r="H105" s="148"/>
-    </row>
-    <row r="106" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F106" s="119"/>
-      <c r="G106" s="148"/>
-      <c r="H106" s="148"/>
-    </row>
-    <row r="107" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F107" s="119"/>
-      <c r="G107" s="148"/>
-      <c r="H107" s="148"/>
-    </row>
-    <row r="108" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F108" s="119"/>
-      <c r="G108" s="148"/>
-      <c r="H108" s="148"/>
-    </row>
-    <row r="109" spans="6:8" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F109" s="119"/>
-      <c r="G109" s="148"/>
-      <c r="H109" s="148"/>
+    <row r="30" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B30" s="84"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="80"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="123"/>
+      <c r="G30" s="124"/>
+      <c r="H30" s="125"/>
+    </row>
+    <row r="31" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B31" s="84"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="124"/>
+      <c r="H31" s="125"/>
+    </row>
+    <row r="32" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B32" s="84"/>
+      <c r="C32" s="80"/>
+      <c r="D32" s="80"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="123"/>
+      <c r="G32" s="124"/>
+      <c r="H32" s="125"/>
+    </row>
+    <row r="33" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B33" s="84"/>
+      <c r="C33" s="80"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="96"/>
+      <c r="F33" s="123"/>
+      <c r="G33" s="124"/>
+      <c r="H33" s="125"/>
+    </row>
+    <row r="34" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B34" s="84"/>
+      <c r="C34" s="80"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="96"/>
+      <c r="F34" s="123"/>
+      <c r="G34" s="124"/>
+      <c r="H34" s="125"/>
+    </row>
+    <row r="35" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="84"/>
+      <c r="C35" s="80"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="124"/>
+      <c r="H35" s="125"/>
+    </row>
+    <row r="36" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B36" s="84"/>
+      <c r="C36" s="80"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="124"/>
+      <c r="H36" s="125"/>
+    </row>
+    <row r="37" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B37" s="84"/>
+      <c r="C37" s="80"/>
+      <c r="D37" s="80"/>
+      <c r="E37" s="96"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="124"/>
+      <c r="H37" s="125"/>
+    </row>
+    <row r="38" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B38" s="84"/>
+      <c r="C38" s="80"/>
+      <c r="D38" s="80"/>
+      <c r="E38" s="96"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="124"/>
+      <c r="H38" s="125"/>
+    </row>
+    <row r="39" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B39" s="84"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="96"/>
+      <c r="F39" s="123"/>
+      <c r="G39" s="124"/>
+      <c r="H39" s="125"/>
+    </row>
+    <row r="40" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B40" s="84"/>
+      <c r="C40" s="80"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="123"/>
+      <c r="G40" s="124"/>
+      <c r="H40" s="125"/>
+    </row>
+    <row r="41" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B41" s="84"/>
+      <c r="C41" s="80"/>
+      <c r="D41" s="80"/>
+      <c r="E41" s="96"/>
+      <c r="F41" s="123"/>
+      <c r="G41" s="124"/>
+      <c r="H41" s="125"/>
+    </row>
+    <row r="42" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B42" s="84"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="96"/>
+      <c r="F42" s="123"/>
+      <c r="G42" s="124"/>
+      <c r="H42" s="125"/>
+    </row>
+    <row r="43" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B43" s="84"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="96"/>
+      <c r="F43" s="123"/>
+      <c r="G43" s="124"/>
+      <c r="H43" s="125"/>
+    </row>
+    <row r="44" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B44" s="84"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="96"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="124"/>
+      <c r="H44" s="125"/>
+    </row>
+    <row r="45" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B45" s="84"/>
+      <c r="C45" s="80"/>
+      <c r="D45" s="80"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="123"/>
+      <c r="G45" s="124"/>
+      <c r="H45" s="125"/>
+    </row>
+    <row r="46" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B46" s="84"/>
+      <c r="C46" s="80"/>
+      <c r="D46" s="80"/>
+      <c r="E46" s="96"/>
+      <c r="F46" s="123"/>
+      <c r="G46" s="124"/>
+      <c r="H46" s="125"/>
+    </row>
+    <row r="47" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B47" s="84"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="80"/>
+      <c r="E47" s="96"/>
+      <c r="F47" s="123"/>
+      <c r="G47" s="124"/>
+      <c r="H47" s="125"/>
+    </row>
+    <row r="48" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B48" s="84"/>
+      <c r="C48" s="80"/>
+      <c r="D48" s="80"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="123"/>
+      <c r="G48" s="124"/>
+      <c r="H48" s="125"/>
+    </row>
+    <row r="49" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B49" s="84"/>
+      <c r="C49" s="80"/>
+      <c r="D49" s="80"/>
+      <c r="E49" s="96"/>
+      <c r="F49" s="123"/>
+      <c r="G49" s="124"/>
+      <c r="H49" s="125"/>
+    </row>
+    <row r="50" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B50" s="84"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="80"/>
+      <c r="E50" s="96"/>
+      <c r="F50" s="123"/>
+      <c r="G50" s="124"/>
+      <c r="H50" s="125"/>
+    </row>
+    <row r="51" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B51" s="84"/>
+      <c r="C51" s="80"/>
+      <c r="D51" s="80"/>
+      <c r="E51" s="96"/>
+      <c r="F51" s="123"/>
+      <c r="G51" s="124"/>
+      <c r="H51" s="125"/>
+    </row>
+    <row r="52" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B52" s="84"/>
+      <c r="C52" s="80"/>
+      <c r="D52" s="80"/>
+      <c r="E52" s="96"/>
+      <c r="F52" s="123"/>
+      <c r="G52" s="124"/>
+      <c r="H52" s="125"/>
+    </row>
+    <row r="53" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B53" s="84"/>
+      <c r="C53" s="80"/>
+      <c r="D53" s="80"/>
+      <c r="E53" s="96"/>
+      <c r="F53" s="123"/>
+      <c r="G53" s="124"/>
+      <c r="H53" s="125"/>
+    </row>
+    <row r="54" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B54" s="84"/>
+      <c r="C54" s="80"/>
+      <c r="D54" s="80"/>
+      <c r="E54" s="96"/>
+      <c r="F54" s="123"/>
+      <c r="G54" s="124"/>
+      <c r="H54" s="125"/>
+    </row>
+    <row r="55" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B55" s="84"/>
+      <c r="C55" s="80"/>
+      <c r="D55" s="80"/>
+      <c r="E55" s="96"/>
+      <c r="F55" s="123"/>
+      <c r="G55" s="124"/>
+      <c r="H55" s="125"/>
+    </row>
+    <row r="56" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B56" s="84"/>
+      <c r="C56" s="80"/>
+      <c r="D56" s="80"/>
+      <c r="E56" s="96"/>
+      <c r="F56" s="123"/>
+      <c r="G56" s="124"/>
+      <c r="H56" s="125"/>
+    </row>
+    <row r="57" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B57" s="84"/>
+      <c r="C57" s="80"/>
+      <c r="D57" s="80"/>
+      <c r="E57" s="96"/>
+      <c r="F57" s="123"/>
+      <c r="G57" s="124"/>
+      <c r="H57" s="125"/>
+    </row>
+    <row r="58" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B58" s="84"/>
+      <c r="C58" s="80"/>
+      <c r="D58" s="80"/>
+      <c r="E58" s="96"/>
+      <c r="F58" s="123"/>
+      <c r="G58" s="124"/>
+      <c r="H58" s="125"/>
+    </row>
+    <row r="59" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B59" s="84"/>
+      <c r="C59" s="80"/>
+      <c r="D59" s="80"/>
+      <c r="E59" s="96"/>
+      <c r="F59" s="123"/>
+      <c r="G59" s="124"/>
+      <c r="H59" s="125"/>
+    </row>
+    <row r="60" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B60" s="84"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="96"/>
+      <c r="F60" s="123"/>
+      <c r="G60" s="124"/>
+      <c r="H60" s="125"/>
+    </row>
+    <row r="61" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B61" s="84"/>
+      <c r="C61" s="80"/>
+      <c r="D61" s="80"/>
+      <c r="E61" s="96"/>
+      <c r="F61" s="123"/>
+      <c r="G61" s="124"/>
+      <c r="H61" s="125"/>
+    </row>
+    <row r="62" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B62" s="84"/>
+      <c r="C62" s="80"/>
+      <c r="D62" s="80"/>
+      <c r="E62" s="96"/>
+      <c r="F62" s="123"/>
+      <c r="G62" s="124"/>
+      <c r="H62" s="125"/>
+    </row>
+    <row r="63" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B63" s="84"/>
+      <c r="C63" s="80"/>
+      <c r="D63" s="80"/>
+      <c r="E63" s="96"/>
+      <c r="F63" s="123"/>
+      <c r="G63" s="124"/>
+      <c r="H63" s="125"/>
+    </row>
+    <row r="64" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B64" s="84"/>
+      <c r="C64" s="80"/>
+      <c r="D64" s="80"/>
+      <c r="E64" s="96"/>
+      <c r="F64" s="123"/>
+      <c r="G64" s="124"/>
+      <c r="H64" s="125"/>
+    </row>
+    <row r="65" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B65" s="84"/>
+      <c r="C65" s="80"/>
+      <c r="D65" s="80"/>
+      <c r="E65" s="96"/>
+      <c r="F65" s="123"/>
+      <c r="G65" s="124"/>
+      <c r="H65" s="125"/>
+    </row>
+    <row r="66" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B66" s="84"/>
+      <c r="C66" s="80"/>
+      <c r="D66" s="80"/>
+      <c r="E66" s="96"/>
+      <c r="F66" s="123"/>
+      <c r="G66" s="124"/>
+      <c r="H66" s="125"/>
+    </row>
+    <row r="67" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B67" s="84"/>
+      <c r="C67" s="80"/>
+      <c r="D67" s="80"/>
+      <c r="E67" s="96"/>
+      <c r="F67" s="123"/>
+      <c r="G67" s="124"/>
+      <c r="H67" s="125"/>
+    </row>
+    <row r="68" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B68" s="84"/>
+      <c r="C68" s="80"/>
+      <c r="D68" s="80"/>
+      <c r="E68" s="96"/>
+      <c r="F68" s="123"/>
+      <c r="G68" s="124"/>
+      <c r="H68" s="125"/>
+    </row>
+    <row r="69" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B69" s="84"/>
+      <c r="C69" s="80"/>
+      <c r="D69" s="80"/>
+      <c r="E69" s="96"/>
+      <c r="F69" s="123"/>
+      <c r="G69" s="124"/>
+      <c r="H69" s="125"/>
+    </row>
+    <row r="70" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B70" s="84"/>
+      <c r="C70" s="80"/>
+      <c r="D70" s="80"/>
+      <c r="E70" s="96"/>
+      <c r="F70" s="123"/>
+      <c r="G70" s="124"/>
+      <c r="H70" s="125"/>
+    </row>
+    <row r="71" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B71" s="84"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="80"/>
+      <c r="E71" s="96"/>
+      <c r="F71" s="123"/>
+      <c r="G71" s="124"/>
+      <c r="H71" s="125"/>
+    </row>
+    <row r="72" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B72" s="84"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="80"/>
+      <c r="E72" s="96"/>
+      <c r="F72" s="123"/>
+      <c r="G72" s="124"/>
+      <c r="H72" s="125"/>
+    </row>
+    <row r="73" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B73" s="84"/>
+      <c r="C73" s="80"/>
+      <c r="D73" s="80"/>
+      <c r="E73" s="96"/>
+      <c r="F73" s="123"/>
+      <c r="G73" s="124"/>
+      <c r="H73" s="125"/>
+    </row>
+    <row r="74" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B74" s="84"/>
+      <c r="C74" s="80"/>
+      <c r="D74" s="80"/>
+      <c r="E74" s="96"/>
+      <c r="F74" s="123"/>
+      <c r="G74" s="124"/>
+      <c r="H74" s="125"/>
+    </row>
+    <row r="75" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B75" s="84"/>
+      <c r="C75" s="80"/>
+      <c r="D75" s="80"/>
+      <c r="E75" s="96"/>
+      <c r="F75" s="123"/>
+      <c r="G75" s="124"/>
+      <c r="H75" s="125"/>
+    </row>
+    <row r="76" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B76" s="84"/>
+      <c r="C76" s="80"/>
+      <c r="D76" s="80"/>
+      <c r="E76" s="96"/>
+      <c r="F76" s="123"/>
+      <c r="G76" s="124"/>
+      <c r="H76" s="125"/>
+    </row>
+    <row r="77" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B77" s="84"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="96"/>
+      <c r="F77" s="123"/>
+      <c r="G77" s="124"/>
+      <c r="H77" s="125"/>
+    </row>
+    <row r="78" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B78" s="84"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="80"/>
+      <c r="E78" s="96"/>
+      <c r="F78" s="123"/>
+      <c r="G78" s="124"/>
+      <c r="H78" s="125"/>
+    </row>
+    <row r="79" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B79" s="84"/>
+      <c r="C79" s="80"/>
+      <c r="D79" s="80"/>
+      <c r="E79" s="96"/>
+      <c r="F79" s="123"/>
+      <c r="G79" s="124"/>
+      <c r="H79" s="125"/>
+    </row>
+    <row r="80" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B80" s="84"/>
+      <c r="C80" s="80"/>
+      <c r="D80" s="80"/>
+      <c r="E80" s="96"/>
+      <c r="F80" s="123"/>
+      <c r="G80" s="124"/>
+      <c r="H80" s="125"/>
+    </row>
+    <row r="81" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B81" s="84"/>
+      <c r="C81" s="80"/>
+      <c r="D81" s="80"/>
+      <c r="E81" s="96"/>
+      <c r="F81" s="123"/>
+      <c r="G81" s="124"/>
+      <c r="H81" s="125"/>
+    </row>
+    <row r="82" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B82" s="84"/>
+      <c r="C82" s="80"/>
+      <c r="D82" s="80"/>
+      <c r="E82" s="96"/>
+      <c r="F82" s="123"/>
+      <c r="G82" s="124"/>
+      <c r="H82" s="125"/>
+    </row>
+    <row r="83" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B83" s="84"/>
+      <c r="C83" s="80"/>
+      <c r="D83" s="80"/>
+      <c r="E83" s="96"/>
+      <c r="F83" s="123"/>
+      <c r="G83" s="124"/>
+      <c r="H83" s="125"/>
+    </row>
+    <row r="84" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B84" s="84"/>
+      <c r="C84" s="80"/>
+      <c r="D84" s="80"/>
+      <c r="E84" s="96"/>
+      <c r="F84" s="123"/>
+      <c r="G84" s="124"/>
+      <c r="H84" s="125"/>
+    </row>
+    <row r="85" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B85" s="84"/>
+      <c r="C85" s="80"/>
+      <c r="D85" s="80"/>
+      <c r="E85" s="96"/>
+      <c r="F85" s="123"/>
+      <c r="G85" s="124"/>
+      <c r="H85" s="125"/>
+    </row>
+    <row r="86" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B86" s="84"/>
+      <c r="C86" s="80"/>
+      <c r="D86" s="80"/>
+      <c r="E86" s="96"/>
+      <c r="F86" s="123"/>
+      <c r="G86" s="124"/>
+      <c r="H86" s="125"/>
+    </row>
+    <row r="87" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B87" s="84"/>
+      <c r="C87" s="80"/>
+      <c r="D87" s="80"/>
+      <c r="E87" s="96"/>
+      <c r="F87" s="123"/>
+      <c r="G87" s="124"/>
+      <c r="H87" s="125"/>
+    </row>
+    <row r="88" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B88" s="84"/>
+      <c r="C88" s="80"/>
+      <c r="D88" s="80"/>
+      <c r="E88" s="96"/>
+      <c r="F88" s="123"/>
+      <c r="G88" s="124"/>
+      <c r="H88" s="125"/>
+    </row>
+    <row r="89" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B89" s="84"/>
+      <c r="C89" s="80"/>
+      <c r="D89" s="80"/>
+      <c r="E89" s="96"/>
+      <c r="F89" s="123"/>
+      <c r="G89" s="124"/>
+      <c r="H89" s="125"/>
+    </row>
+    <row r="90" spans="2:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="87"/>
+      <c r="C90" s="88"/>
+      <c r="D90" s="88"/>
+      <c r="E90" s="103"/>
+      <c r="F90" s="120"/>
+      <c r="G90" s="121"/>
+      <c r="H90" s="122"/>
+    </row>
+    <row r="91" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F91" s="95"/>
+      <c r="G91" s="111"/>
+      <c r="H91" s="111"/>
+    </row>
+    <row r="92" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F92" s="95"/>
+      <c r="G92" s="111"/>
+      <c r="H92" s="111"/>
+    </row>
+    <row r="93" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F93" s="95"/>
+      <c r="G93" s="111"/>
+      <c r="H93" s="111"/>
+    </row>
+    <row r="94" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F94" s="95"/>
+      <c r="G94" s="111"/>
+      <c r="H94" s="111"/>
+    </row>
+    <row r="95" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F95" s="95"/>
+      <c r="G95" s="111"/>
+      <c r="H95" s="111"/>
+    </row>
+    <row r="96" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F96" s="95"/>
+      <c r="G96" s="111"/>
+      <c r="H96" s="111"/>
+    </row>
+    <row r="97" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F97" s="95"/>
+      <c r="G97" s="111"/>
+      <c r="H97" s="111"/>
+    </row>
+    <row r="98" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F98" s="95"/>
+      <c r="G98" s="111"/>
+      <c r="H98" s="111"/>
+    </row>
+    <row r="99" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F99" s="95"/>
+      <c r="G99" s="111"/>
+      <c r="H99" s="111"/>
+    </row>
+    <row r="100" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F100" s="95"/>
+      <c r="G100" s="111"/>
+      <c r="H100" s="111"/>
+    </row>
+    <row r="101" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F101" s="95"/>
+      <c r="G101" s="111"/>
+      <c r="H101" s="111"/>
+    </row>
+    <row r="102" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F102" s="95"/>
+      <c r="G102" s="111"/>
+      <c r="H102" s="111"/>
+    </row>
+    <row r="103" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F103" s="95"/>
+      <c r="G103" s="111"/>
+      <c r="H103" s="111"/>
+    </row>
+    <row r="104" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F104" s="95"/>
+      <c r="G104" s="111"/>
+      <c r="H104" s="111"/>
+    </row>
+    <row r="105" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F105" s="95"/>
+      <c r="G105" s="111"/>
+      <c r="H105" s="111"/>
+    </row>
+    <row r="106" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F106" s="95"/>
+      <c r="G106" s="111"/>
+      <c r="H106" s="111"/>
+    </row>
+    <row r="107" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F107" s="95"/>
+      <c r="G107" s="111"/>
+      <c r="H107" s="111"/>
+    </row>
+    <row r="108" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F108" s="95"/>
+      <c r="G108" s="111"/>
+      <c r="H108" s="111"/>
+    </row>
+    <row r="109" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F109" s="95"/>
+      <c r="G109" s="111"/>
+      <c r="H109" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3617,44 +3617,44 @@
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="159" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="136" t="s">
+      <c r="C2" s="160"/>
+      <c r="D2" s="161"/>
+      <c r="E2" s="156" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="131"/>
-      <c r="G2" s="136" t="s">
+      <c r="F2" s="158"/>
+      <c r="G2" s="156" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="129"/>
-      <c r="I2" s="131"/>
+      <c r="H2" s="157"/>
+      <c r="I2" s="158"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="137" t="s">
+      <c r="E3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="138" t="s">
+      <c r="F3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="137" t="s">
+      <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="130" t="s">
+      <c r="H3" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="132"/>
+      <c r="I3" s="163"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -3684,19 +3684,19 @@
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="61"/>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="150" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="85" t="s">
+      <c r="F5" s="153" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="88" t="s">
+      <c r="G5" s="144" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -3708,23 +3708,23 @@
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="83"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="151"/>
       <c r="E6" s="35"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="77" t="s">
+      <c r="F6" s="154"/>
+      <c r="G6" s="145"/>
+      <c r="H6" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="78"/>
+      <c r="I6" s="140"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="84"/>
+      <c r="C7" s="149"/>
+      <c r="D7" s="152"/>
       <c r="E7" s="36"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="90"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="146"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -3758,19 +3758,19 @@
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="150" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="93" t="s">
+      <c r="E9" s="141" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="85" t="s">
+      <c r="F9" s="153" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="88" t="s">
+      <c r="G9" s="144" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -3783,24 +3783,24 @@
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="77" t="s">
+      <c r="C10" s="148"/>
+      <c r="D10" s="151"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="145"/>
+      <c r="H10" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="78"/>
+      <c r="I10" s="140"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="90"/>
+      <c r="C11" s="149"/>
+      <c r="D11" s="152"/>
+      <c r="E11" s="143"/>
+      <c r="F11" s="155"/>
+      <c r="G11" s="146"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3810,10 +3810,10 @@
     </row>
     <row r="12" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="61"/>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="147" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="82" t="s">
+      <c r="D12" s="150" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="37" t="s">
@@ -3822,7 +3822,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="88" t="s">
+      <c r="G12" s="144" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -3834,15 +3834,15 @@
     </row>
     <row r="13" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="61"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="84"/>
+      <c r="C13" s="149"/>
+      <c r="D13" s="152"/>
       <c r="E13" s="37" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="90"/>
+      <c r="G13" s="146"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -3887,10 +3887,10 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="92"/>
-    </row>
-    <row r="17" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="H16" s="137"/>
+      <c r="I16" s="138"/>
+    </row>
+    <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
         <v>75</v>
       </c>
@@ -4302,19 +4302,19 @@
     </row>
     <row r="40" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="61"/>
-      <c r="C40" s="79" t="s">
+      <c r="C40" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="82" t="s">
+      <c r="D40" s="150" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="93" t="s">
+      <c r="E40" s="141" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="85" t="s">
+      <c r="F40" s="153" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="88" t="s">
+      <c r="G40" s="144" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -4326,23 +4326,23 @@
     </row>
     <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="61"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="83"/>
-      <c r="E41" s="94"/>
-      <c r="F41" s="86"/>
-      <c r="G41" s="89"/>
-      <c r="H41" s="77" t="s">
+      <c r="C41" s="148"/>
+      <c r="D41" s="151"/>
+      <c r="E41" s="142"/>
+      <c r="F41" s="154"/>
+      <c r="G41" s="145"/>
+      <c r="H41" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="78"/>
+      <c r="I41" s="140"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="84"/>
-      <c r="E42" s="95"/>
-      <c r="F42" s="87"/>
-      <c r="G42" s="90"/>
+      <c r="C42" s="149"/>
+      <c r="D42" s="152"/>
+      <c r="E42" s="143"/>
+      <c r="F42" s="155"/>
+      <c r="G42" s="146"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -4376,19 +4376,19 @@
     </row>
     <row r="44" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="61"/>
-      <c r="C44" s="79" t="s">
+      <c r="C44" s="147" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="82" t="s">
+      <c r="D44" s="150" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="93" t="s">
+      <c r="E44" s="141" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="85" t="s">
+      <c r="F44" s="153" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="88" t="s">
+      <c r="G44" s="144" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -4400,23 +4400,23 @@
     </row>
     <row r="45" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="61"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="86"/>
-      <c r="G45" s="89"/>
-      <c r="H45" s="77" t="s">
+      <c r="C45" s="148"/>
+      <c r="D45" s="151"/>
+      <c r="E45" s="142"/>
+      <c r="F45" s="154"/>
+      <c r="G45" s="145"/>
+      <c r="H45" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="78"/>
+      <c r="I45" s="140"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
-      <c r="C46" s="81"/>
-      <c r="D46" s="84"/>
-      <c r="E46" s="95"/>
-      <c r="F46" s="87"/>
-      <c r="G46" s="90"/>
+      <c r="C46" s="149"/>
+      <c r="D46" s="152"/>
+      <c r="E46" s="143"/>
+      <c r="F46" s="155"/>
+      <c r="G46" s="146"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -4441,8 +4441,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="91"/>
-      <c r="I48" s="92"/>
+      <c r="H48" s="137"/>
+      <c r="I48" s="138"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -4505,10 +4505,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="77" t="s">
+      <c r="H52" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="78"/>
+      <c r="I52" s="140"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -4541,8 +4541,8 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="91"/>
-      <c r="I55" s="92"/>
+      <c r="H55" s="137"/>
+      <c r="I55" s="138"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="61"/>
@@ -4686,21 +4686,15 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -4711,15 +4705,21 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4738,462 +4738,462 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="97" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="97" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="97" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52" style="97" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="41" style="97" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="97"/>
+    <col min="1" max="1" width="2.85546875" style="78" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="78" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52" style="78" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41" style="78" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="78"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="164" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="129" t="s">
+      <c r="C2" s="165"/>
+      <c r="D2" s="157" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="131" t="s">
+      <c r="E2" s="158" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="91" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="130"/>
-      <c r="E3" s="132"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="163"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="103" t="s">
+      <c r="B4" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="80" t="s">
         <v>160</v>
       </c>
-      <c r="D4" s="120" t="s">
+      <c r="D4" s="96" t="s">
         <v>175</v>
       </c>
-      <c r="E4" s="121" t="s">
+      <c r="E4" s="97" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="103"/>
-      <c r="C5" s="99" t="s">
+      <c r="B5" s="84"/>
+      <c r="C5" s="80" t="s">
         <v>161</v>
       </c>
-      <c r="D5" s="120" t="s">
+      <c r="D5" s="96" t="s">
         <v>176</v>
       </c>
-      <c r="E5" s="121" t="s">
+      <c r="E5" s="97" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="103"/>
-      <c r="C6" s="99" t="s">
+      <c r="B6" s="84"/>
+      <c r="C6" s="80" t="s">
         <v>162</v>
       </c>
-      <c r="D6" s="120" t="s">
+      <c r="D6" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="E6" s="121" t="s">
+      <c r="E6" s="97" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="103"/>
-      <c r="C7" s="99" t="s">
+      <c r="B7" s="84"/>
+      <c r="C7" s="80" t="s">
         <v>163</v>
       </c>
-      <c r="D7" s="120" t="s">
+      <c r="D7" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="E7" s="121" t="s">
+      <c r="E7" s="97" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="103"/>
-      <c r="C8" s="99" t="s">
+      <c r="B8" s="84"/>
+      <c r="C8" s="80" t="s">
         <v>164</v>
       </c>
-      <c r="D8" s="120" t="s">
+      <c r="D8" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="E8" s="121" t="s">
+      <c r="E8" s="97" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="103"/>
-      <c r="C9" s="99" t="s">
+      <c r="B9" s="84"/>
+      <c r="C9" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="120" t="s">
+      <c r="D9" s="96" t="s">
         <v>180</v>
       </c>
-      <c r="E9" s="121" t="s">
+      <c r="E9" s="97" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="103"/>
-      <c r="C10" s="99" t="s">
+      <c r="B10" s="84"/>
+      <c r="C10" s="80" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="120" t="s">
+      <c r="D10" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="E10" s="121" t="s">
+      <c r="E10" s="97" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="103"/>
-      <c r="C11" s="99" t="s">
+      <c r="B11" s="84"/>
+      <c r="C11" s="80" t="s">
         <v>166</v>
       </c>
-      <c r="D11" s="120" t="s">
+      <c r="D11" s="96" t="s">
         <v>182</v>
       </c>
-      <c r="E11" s="121" t="s">
+      <c r="E11" s="97" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="103"/>
-      <c r="C12" s="99" t="s">
+      <c r="B12" s="84"/>
+      <c r="C12" s="80" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="120" t="s">
+      <c r="D12" s="96" t="s">
         <v>183</v>
       </c>
-      <c r="E12" s="121" t="s">
+      <c r="E12" s="97" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="103"/>
-      <c r="C13" s="99" t="s">
+      <c r="B13" s="84"/>
+      <c r="C13" s="80" t="s">
         <v>167</v>
       </c>
-      <c r="D13" s="120" t="s">
+      <c r="D13" s="96" t="s">
         <v>184</v>
       </c>
-      <c r="E13" s="121" t="s">
+      <c r="E13" s="97" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="103"/>
-      <c r="C14" s="99" t="s">
+      <c r="B14" s="84"/>
+      <c r="C14" s="80" t="s">
         <v>168</v>
       </c>
-      <c r="D14" s="120" t="s">
+      <c r="D14" s="96" t="s">
         <v>185</v>
       </c>
-      <c r="E14" s="121" t="s">
+      <c r="E14" s="97" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="103"/>
-      <c r="C15" s="99" t="s">
+      <c r="B15" s="84"/>
+      <c r="C15" s="80" t="s">
         <v>169</v>
       </c>
-      <c r="D15" s="120" t="s">
+      <c r="D15" s="96" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="121" t="s">
+      <c r="E15" s="97" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="103"/>
-      <c r="C16" s="99" t="s">
+      <c r="B16" s="84"/>
+      <c r="C16" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="120" t="s">
+      <c r="D16" s="96" t="s">
         <v>187</v>
       </c>
-      <c r="E16" s="121" t="s">
+      <c r="E16" s="97" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="103"/>
-      <c r="C17" s="99" t="s">
+      <c r="B17" s="84"/>
+      <c r="C17" s="80" t="s">
         <v>170</v>
       </c>
-      <c r="D17" s="120" t="s">
+      <c r="D17" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E17" s="121" t="s">
+      <c r="E17" s="97" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="103"/>
-      <c r="C18" s="99" t="s">
+      <c r="B18" s="84"/>
+      <c r="C18" s="80" t="s">
         <v>146</v>
       </c>
-      <c r="D18" s="120" t="s">
+      <c r="D18" s="96" t="s">
         <v>189</v>
       </c>
-      <c r="E18" s="121" t="s">
+      <c r="E18" s="97" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="103"/>
-      <c r="C19" s="99" t="s">
+      <c r="B19" s="84"/>
+      <c r="C19" s="80" t="s">
         <v>171</v>
       </c>
-      <c r="D19" s="120" t="s">
+      <c r="D19" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E19" s="121" t="s">
+      <c r="E19" s="97" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="103"/>
-      <c r="C20" s="99" t="s">
+      <c r="B20" s="84"/>
+      <c r="C20" s="80" t="s">
         <v>172</v>
       </c>
-      <c r="D20" s="120" t="s">
+      <c r="D20" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E20" s="121" t="s">
+      <c r="E20" s="97" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="103"/>
-      <c r="C21" s="99" t="s">
+      <c r="B21" s="84"/>
+      <c r="C21" s="80" t="s">
         <v>173</v>
       </c>
-      <c r="D21" s="120" t="s">
+      <c r="D21" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E21" s="121" t="s">
+      <c r="E21" s="97" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="104"/>
-      <c r="C22" s="100" t="s">
+      <c r="B22" s="85"/>
+      <c r="C22" s="81" t="s">
         <v>147</v>
       </c>
-      <c r="D22" s="122" t="s">
+      <c r="D22" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="E22" s="123" t="s">
+      <c r="E22" s="99" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="105" t="s">
+      <c r="B23" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="C23" s="101" t="s">
+      <c r="C23" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="122" t="s">
+      <c r="D23" s="98" t="s">
         <v>188</v>
       </c>
-      <c r="E23" s="124" t="s">
+      <c r="E23" s="100" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="84" t="s">
         <v>143</v>
       </c>
-      <c r="C24" s="99" t="s">
+      <c r="C24" s="80" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="120" t="s">
+      <c r="D24" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E24" s="121" t="s">
+      <c r="E24" s="97" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="103"/>
-      <c r="C25" s="99" t="s">
+      <c r="B25" s="84"/>
+      <c r="C25" s="80" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="120" t="s">
+      <c r="D25" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E25" s="121" t="s">
+      <c r="E25" s="97" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B26" s="103"/>
-      <c r="C26" s="99" t="s">
+      <c r="B26" s="84"/>
+      <c r="C26" s="80" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="120" t="s">
+      <c r="D26" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E26" s="121" t="s">
+      <c r="E26" s="97" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="103"/>
-      <c r="C27" s="99" t="s">
+      <c r="B27" s="84"/>
+      <c r="C27" s="80" t="s">
         <v>151</v>
       </c>
-      <c r="D27" s="120" t="s">
+      <c r="D27" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E27" s="121" t="s">
+      <c r="E27" s="97" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B28" s="103"/>
-      <c r="C28" s="99" t="s">
+      <c r="B28" s="84"/>
+      <c r="C28" s="80" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="120" t="s">
+      <c r="D28" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E28" s="121" t="s">
+      <c r="E28" s="97" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B29" s="103"/>
-      <c r="C29" s="99" t="s">
+      <c r="B29" s="84"/>
+      <c r="C29" s="80" t="s">
         <v>153</v>
       </c>
-      <c r="D29" s="120" t="s">
+      <c r="D29" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E29" s="121" t="s">
+      <c r="E29" s="97" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B30" s="103"/>
-      <c r="C30" s="99" t="s">
+      <c r="B30" s="84"/>
+      <c r="C30" s="80" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="120" t="s">
+      <c r="D30" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E30" s="121" t="s">
+      <c r="E30" s="97" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B31" s="103"/>
-      <c r="C31" s="99" t="s">
+      <c r="B31" s="84"/>
+      <c r="C31" s="80" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="120" t="s">
+      <c r="D31" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E31" s="121" t="s">
+      <c r="E31" s="97" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B32" s="103"/>
-      <c r="C32" s="99" t="s">
+      <c r="B32" s="84"/>
+      <c r="C32" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="D32" s="120" t="s">
+      <c r="D32" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E32" s="121" t="s">
+      <c r="E32" s="97" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B33" s="103"/>
-      <c r="C33" s="99" t="s">
+      <c r="B33" s="84"/>
+      <c r="C33" s="80" t="s">
         <v>157</v>
       </c>
-      <c r="D33" s="120" t="s">
+      <c r="D33" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E33" s="121" t="s">
+      <c r="E33" s="97" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B34" s="103"/>
-      <c r="C34" s="99" t="s">
+      <c r="B34" s="84"/>
+      <c r="C34" s="80" t="s">
         <v>158</v>
       </c>
-      <c r="D34" s="120" t="s">
+      <c r="D34" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E34" s="121" t="s">
+      <c r="E34" s="97" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B35" s="103"/>
-      <c r="C35" s="99" t="s">
+      <c r="B35" s="84"/>
+      <c r="C35" s="80" t="s">
         <v>147</v>
       </c>
-      <c r="D35" s="120" t="s">
+      <c r="D35" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E35" s="121" t="s">
+      <c r="E35" s="97" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B36" s="103"/>
-      <c r="C36" s="99" t="s">
+      <c r="B36" s="84"/>
+      <c r="C36" s="80" t="s">
         <v>159</v>
       </c>
-      <c r="D36" s="120" t="s">
+      <c r="D36" s="96" t="s">
         <v>188</v>
       </c>
-      <c r="E36" s="121" t="s">
+      <c r="E36" s="97" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B37" s="102" t="s">
+      <c r="B37" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="C37" s="98" t="s">
+      <c r="C37" s="79" t="s">
         <v>146</v>
       </c>
-      <c r="D37" s="125" t="s">
+      <c r="D37" s="101" t="s">
         <v>188</v>
       </c>
-      <c r="E37" s="126" t="s">
+      <c r="E37" s="102" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="106"/>
-      <c r="C38" s="107" t="s">
+      <c r="B38" s="87"/>
+      <c r="C38" s="88" t="s">
         <v>147</v>
       </c>
-      <c r="D38" s="127" t="s">
+      <c r="D38" s="103" t="s">
         <v>188</v>
       </c>
-      <c r="E38" s="128" t="s">
+      <c r="E38" s="104" t="s">
         <v>193</v>
       </c>
     </row>
@@ -5218,56 +5218,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.42578125" style="96" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="96" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="96" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="96"/>
+    <col min="1" max="1" width="1.42578125" style="77" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="77" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="77" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="133" t="s">
+      <c r="C2" s="166" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="97" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="109" t="s">
+    <row r="3" spans="2:3" s="78" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="134"/>
-    </row>
-    <row r="4" spans="2:3" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="108" t="s">
+      <c r="C3" s="167"/>
+    </row>
+    <row r="4" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B4" s="89" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="105" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="103" t="s">
+    <row r="5" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B5" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="C5" s="121" t="s">
+      <c r="C5" s="97" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="97" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="103" t="s">
+    <row r="6" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B6" s="84" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="97" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="87" t="s">
         <v>144</v>
       </c>
-      <c r="C7" s="128" t="s">
+      <c r="C7" s="104" t="s">
         <v>225</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Pertanggal 23 Januari 2023 17:58 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="340">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -834,9 +834,6 @@
   </si>
   <si>
     <t>Mendapatkan User Session ID dari API Web Token</t>
-  </si>
-  <si>
-    <t>Func_GetData_UserSessionIDByAPIWebToken</t>
   </si>
   <si>
     <t>Func_GetFileEntities_StagingArea</t>
@@ -890,6 +887,176 @@
       </rPr>
       <t>SchSysAsset.Func_GetData_APIWebToken_SysEngine</t>
     </r>
+  </si>
+  <si>
+    <t>FuncSys_General_GetTableRecordsLastModified</t>
+  </si>
+  <si>
+    <t>menampilkan informasi perubahan terakhir pada records yang terdapat didalam table</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_VarChar</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_TimestampTZ</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_SmallInt</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_Int</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_Numeric</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_Boolean</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_BigInt</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal BOOLEAN yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal BIGINT yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal INT yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal NUMERIC yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal SMALLINT yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal TIMESTAMPTZ yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal VARCHAR yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>Func_GetData_UserSessionID_ByAPIWebToken</t>
+  </si>
+  <si>
+    <t>Func_GetData_APIWebToken_IsExist</t>
+  </si>
+  <si>
+    <t>Mengecek Apakah API Web Token ada atau tidak</t>
+  </si>
+  <si>
+    <t>Func_General_JSONArray_ExtractToElements</t>
+  </si>
+  <si>
+    <t>Mengkestraksi element pada Array JSON</t>
+  </si>
+  <si>
+    <t>Func_GetStringLiteralConvertion_JSON</t>
+  </si>
+  <si>
+    <t>Menghasilkan String Literal JSON yang diperlukan dalam men-generate String Query (Seperti : varSQL) dari varData.
+Bila varData adalah NULL adalah maka akan menghasilkan string NULL tanpa "Under Closing Single Quote", dan bila selainnya maka akan dimunculkan string varData dalam kondisi "Under Closing Single Quote"</t>
+  </si>
+  <si>
+    <t>TblAppObject_WorkFlow</t>
+  </si>
+  <si>
+    <t>WorkFlow</t>
+  </si>
+  <si>
+    <t>TblAppObject_WorkFlowEdge</t>
+  </si>
+  <si>
+    <t>TblAppObject_WorkFlowNode</t>
+  </si>
+  <si>
+    <t>Edge pada Graph WorkFlow</t>
+  </si>
+  <si>
+    <t>Node pada Graph WorkFlow</t>
+  </si>
+  <si>
+    <t>TblAppObject_WorkFlowVersion</t>
+  </si>
+  <si>
+    <t>Versi WorkFlow</t>
+  </si>
+  <si>
+    <t>WorkFlow_RefID</t>
+  </si>
+  <si>
+    <t>SchSysConfig.TblAppObject_WorkFlow</t>
+  </si>
+  <si>
+    <t>WorkFlowVersion_RefID</t>
+  </si>
+  <si>
+    <t>SchSysConfig.TblAppObject_WorkFlowVersion</t>
+  </si>
+  <si>
+    <t>Func_General_GetWorkFlowPathSegment</t>
+  </si>
+  <si>
+    <t>Func_General_SetWorkFlowGraphExportToPath</t>
+  </si>
+  <si>
+    <t>Mengkespor Work Flow Graph menjadi Work Flow Path berdasarkan Work Flow Version (varWorkFlowVersion_RefID) pada Table SchSysConfig.TblAppObject_WorkFlowPath</t>
+  </si>
+  <si>
+    <t>Func_General_GetWorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Path Approval dari Workflow berdasarkan ID WorkFlowVersion (varWorkFlowVersion_RefID)</t>
+  </si>
+  <si>
+    <t>Mendapatkan Worklow Path Segment dari Workflow Graph berdasarkan ID WorkFlowVersion (varWorkFlowVersion_RefID) dan ID Start Work Flow Node (varStartWorkFlowNode_RefID)</t>
+  </si>
+  <si>
+    <t>Func_General_GetWorkFlowApproverEntities</t>
+  </si>
+  <si>
+    <t>Mendapatkan Approver Entity dari Workflow berdasarkan Array ID WorkerCareerInternal (varArrayID)</t>
+  </si>
+  <si>
+    <t>Func_General_SetWorkFlowGraph</t>
+  </si>
+  <si>
+    <t>Mengeset WorkFlow Graph</t>
+  </si>
+  <si>
+    <t>Func_TblAppObject_WorkFlow_SET</t>
+  </si>
+  <si>
+    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblAppObject_WorkFlow</t>
+  </si>
+  <si>
+    <t>Func_General_GetWorkFlowGraphToClosedGraph</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   (Membuang Path yang berbentuk ranting)</t>
+  </si>
+  <si>
+    <t>Mendapatkan Workflow Closed Graph dari Workflow Graph (dengan membuang Path yang berbentuk ranting)</t>
+  </si>
+  <si>
+    <t>Func_General_SetWorkFlowGraphWithoutLoopPath</t>
+  </si>
+  <si>
+    <t>Menghapus Edge yang menyebabkan Loop pada ID WorkFlowVersion (varWorkFlowVersion_RefID)</t>
+  </si>
+  <si>
+    <t>Sudah bener</t>
+  </si>
+  <si>
+    <t>doble cross</t>
   </si>
 </sst>
 </file>
@@ -1618,7 +1785,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="168">
+  <cellXfs count="188">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1916,45 +2083,111 @@
     <xf numFmtId="164" fontId="8" fillId="12" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1976,18 +2209,78 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1996,66 +2289,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2380,10 +2613,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H109"/>
+  <dimension ref="A1:J121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2399,23 +2635,23 @@
     <col min="9" max="16384" width="9.140625" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="130" t="s">
+    <row r="1" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="150" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="131"/>
-      <c r="D2" s="131"/>
-      <c r="E2" s="132" t="s">
+      <c r="C2" s="151"/>
+      <c r="D2" s="151"/>
+      <c r="E2" s="152" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="134" t="s">
+      <c r="F2" s="154" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="135"/>
-      <c r="H2" s="136"/>
-    </row>
-    <row r="3" spans="2:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G2" s="155"/>
+      <c r="H2" s="156"/>
+    </row>
+    <row r="3" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="91" t="s">
         <v>145</v>
       </c>
@@ -2425,7 +2661,7 @@
       <c r="D3" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="133"/>
+      <c r="E3" s="153"/>
       <c r="F3" s="112" t="s">
         <v>228</v>
       </c>
@@ -2436,1149 +2672,1633 @@
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B4" s="89" t="s">
+    <row r="4" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="115" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="115" t="s">
+      <c r="D4" s="116" t="s">
         <v>227</v>
       </c>
-      <c r="E4" s="116" t="s">
+      <c r="E4" s="117" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="117" t="s">
+      <c r="F4" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="118">
+      <c r="G4" s="119">
         <v>44910</v>
       </c>
-      <c r="H4" s="119">
+      <c r="H4" s="120">
         <v>44910</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B5" s="84"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80" t="s">
+    <row r="5" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="96" t="s">
+      <c r="E5" s="123" t="s">
         <v>236</v>
       </c>
-      <c r="F5" s="123" t="s">
+      <c r="F5" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G5" s="124">
+      <c r="G5" s="125">
         <v>44908</v>
       </c>
-      <c r="H5" s="125">
+      <c r="H5" s="126">
         <v>44908</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="84"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80" t="s">
+    <row r="6" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="122"/>
+      <c r="D6" s="122" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="96" t="s">
+      <c r="E6" s="123" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="123" t="s">
+      <c r="F6" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G6" s="124">
+      <c r="G6" s="125">
         <v>44908</v>
       </c>
-      <c r="H6" s="125">
+      <c r="H6" s="126">
         <v>44908</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B7" s="84"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80" t="s">
+    <row r="7" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="122"/>
+      <c r="D7" s="122" t="s">
         <v>238</v>
       </c>
-      <c r="E7" s="96" t="s">
+      <c r="E7" s="123" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="123" t="s">
+      <c r="F7" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G7" s="124">
+      <c r="G7" s="125">
         <v>44887</v>
       </c>
-      <c r="H7" s="125">
+      <c r="H7" s="126">
         <v>44887</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B8" s="84"/>
-      <c r="C8" s="80"/>
-      <c r="D8" s="80" t="s">
+    <row r="8" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="96" t="s">
+      <c r="E8" s="123" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="123" t="s">
+      <c r="F8" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="124">
+      <c r="G8" s="125">
         <v>44887</v>
       </c>
-      <c r="H8" s="125">
+      <c r="H8" s="126">
         <v>44887</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B9" s="84"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80" t="s">
+    <row r="9" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122" t="s">
         <v>242</v>
       </c>
-      <c r="E9" s="96" t="s">
+      <c r="E9" s="123" t="s">
         <v>243</v>
       </c>
-      <c r="F9" s="123" t="s">
+      <c r="F9" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G9" s="124">
+      <c r="G9" s="125">
         <v>44774</v>
       </c>
-      <c r="H9" s="125">
+      <c r="H9" s="126">
         <v>44774</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="84"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80" t="s">
+    <row r="10" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122" t="s">
+        <v>305</v>
+      </c>
+      <c r="E10" s="123" t="s">
+        <v>306</v>
+      </c>
+      <c r="F10" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G10" s="125">
+        <v>44897</v>
+      </c>
+      <c r="H10" s="126">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122" t="s">
         <v>244</v>
       </c>
-      <c r="E10" s="96" t="s">
+      <c r="E11" s="123" t="s">
         <v>245</v>
       </c>
-      <c r="F10" s="123" t="s">
+      <c r="F11" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="124">
+      <c r="G11" s="125">
         <v>44897</v>
       </c>
-      <c r="H10" s="125">
+      <c r="H11" s="126">
         <v>44897</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B11" s="84"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80" t="s">
+    <row r="12" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122" t="s">
         <v>246</v>
       </c>
-      <c r="E11" s="96" t="s">
+      <c r="E12" s="123" t="s">
         <v>247</v>
       </c>
-      <c r="F11" s="123" t="s">
+      <c r="F12" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="124">
+      <c r="G12" s="125">
         <v>44897</v>
       </c>
-      <c r="H11" s="125">
+      <c r="H12" s="126">
         <v>44897</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="84"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80" t="s">
+    <row r="13" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122" t="s">
         <v>248</v>
       </c>
-      <c r="E12" s="96" t="s">
+      <c r="E13" s="123" t="s">
         <v>249</v>
       </c>
-      <c r="F12" s="123" t="s">
+      <c r="F13" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G12" s="124">
+      <c r="G13" s="125">
         <v>44748</v>
       </c>
-      <c r="H12" s="125">
+      <c r="H13" s="126">
         <v>44748</v>
       </c>
     </row>
-    <row r="13" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="84"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80" t="s">
+    <row r="14" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122" t="s">
         <v>250</v>
       </c>
-      <c r="E13" s="96" t="s">
+      <c r="E14" s="123" t="s">
         <v>251</v>
       </c>
-      <c r="F13" s="123" t="s">
+      <c r="F14" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G13" s="124">
+      <c r="G14" s="125">
         <v>44735</v>
       </c>
-      <c r="H13" s="125">
+      <c r="H14" s="126">
         <v>44735</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B14" s="84"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80" t="s">
+    <row r="15" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122" t="s">
         <v>252</v>
       </c>
-      <c r="E14" s="96" t="s">
+      <c r="E15" s="123" t="s">
         <v>253</v>
       </c>
-      <c r="F14" s="123" t="s">
+      <c r="F15" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G14" s="124">
+      <c r="G15" s="125">
         <v>44854</v>
       </c>
-      <c r="H14" s="125">
+      <c r="H15" s="126">
         <v>44854</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="84"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80" t="s">
+    <row r="16" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122" t="s">
         <v>254</v>
       </c>
-      <c r="E15" s="96" t="s">
+      <c r="E16" s="123" t="s">
         <v>259</v>
       </c>
-      <c r="F15" s="123" t="s">
+      <c r="F16" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G15" s="124">
+      <c r="G16" s="125">
         <v>44770</v>
       </c>
-      <c r="H15" s="125">
+      <c r="H16" s="126">
         <v>44770</v>
       </c>
     </row>
-    <row r="16" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B16" s="84"/>
-      <c r="C16" s="80"/>
-      <c r="D16" s="80" t="s">
+    <row r="17" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122" t="s">
         <v>255</v>
       </c>
-      <c r="E16" s="96" t="s">
+      <c r="E17" s="123" t="s">
         <v>260</v>
       </c>
-      <c r="F16" s="123" t="s">
+      <c r="F17" s="124" t="s">
         <v>256</v>
       </c>
-      <c r="G16" s="124">
+      <c r="G17" s="125">
         <v>44770</v>
       </c>
-      <c r="H16" s="125">
+      <c r="H17" s="126">
         <v>44427</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B17" s="84"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80" t="s">
+    <row r="18" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122" t="s">
         <v>257</v>
       </c>
-      <c r="E17" s="96" t="s">
+      <c r="E18" s="123" t="s">
         <v>261</v>
       </c>
-      <c r="F17" s="123" t="s">
+      <c r="F18" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G17" s="124">
+      <c r="G18" s="125">
         <v>44770</v>
       </c>
-      <c r="H17" s="125">
+      <c r="H18" s="126">
         <v>44770</v>
       </c>
     </row>
-    <row r="18" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B18" s="84"/>
-      <c r="C18" s="80"/>
-      <c r="D18" s="80" t="s">
+    <row r="19" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122" t="s">
         <v>258</v>
       </c>
-      <c r="E18" s="96" t="s">
+      <c r="E19" s="123" t="s">
         <v>262</v>
       </c>
-      <c r="F18" s="123" t="s">
+      <c r="F19" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G18" s="124">
+      <c r="G19" s="125">
         <v>44770</v>
       </c>
-      <c r="H18" s="125">
+      <c r="H19" s="126">
         <v>44427</v>
       </c>
     </row>
-    <row r="19" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B19" s="84"/>
-      <c r="C19" s="80"/>
-      <c r="D19" s="80" t="s">
+    <row r="20" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="121"/>
+      <c r="C20" s="122"/>
+      <c r="D20" s="122" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="123" t="s">
+        <v>263</v>
+      </c>
+      <c r="F20" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G20" s="125">
+        <v>44777</v>
+      </c>
+      <c r="H20" s="126">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="121"/>
+      <c r="C21" s="122"/>
+      <c r="D21" s="122" t="s">
+        <v>303</v>
+      </c>
+      <c r="E21" s="123" t="s">
+        <v>304</v>
+      </c>
+      <c r="F21" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G21" s="125">
+        <v>44935</v>
+      </c>
+      <c r="H21" s="126">
+        <v>44935</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="121"/>
+      <c r="C22" s="122"/>
+      <c r="D22" s="122" t="s">
         <v>284</v>
       </c>
-      <c r="E19" s="96" t="s">
-        <v>263</v>
-      </c>
-      <c r="F19" s="123" t="s">
+      <c r="E22" s="123" t="s">
+        <v>277</v>
+      </c>
+      <c r="F22" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G19" s="124">
+      <c r="G22" s="125">
+        <v>44931</v>
+      </c>
+      <c r="H22" s="126">
+        <v>44931</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="121"/>
+      <c r="C23" s="122"/>
+      <c r="D23" s="122" t="s">
+        <v>264</v>
+      </c>
+      <c r="E23" s="123" t="s">
+        <v>265</v>
+      </c>
+      <c r="F23" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G23" s="125">
+        <v>44847</v>
+      </c>
+      <c r="H23" s="126">
+        <v>44847</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="121"/>
+      <c r="C24" s="122"/>
+      <c r="D24" s="122" t="s">
+        <v>266</v>
+      </c>
+      <c r="E24" s="123" t="s">
+        <v>268</v>
+      </c>
+      <c r="F24" s="124" t="s">
+        <v>267</v>
+      </c>
+      <c r="G24" s="125">
+        <v>44792</v>
+      </c>
+      <c r="H24" s="126">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="121"/>
+      <c r="C25" s="122"/>
+      <c r="D25" s="122" t="s">
+        <v>269</v>
+      </c>
+      <c r="E25" s="123" t="s">
+        <v>270</v>
+      </c>
+      <c r="F25" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G25" s="125">
+        <v>44776</v>
+      </c>
+      <c r="H25" s="126">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="121"/>
+      <c r="C26" s="122"/>
+      <c r="D26" s="122" t="s">
+        <v>302</v>
+      </c>
+      <c r="E26" s="123" t="s">
+        <v>271</v>
+      </c>
+      <c r="F26" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G26" s="125">
         <v>44777</v>
       </c>
-      <c r="H19" s="125">
+      <c r="H26" s="126">
         <v>44777</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B20" s="84"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80" t="s">
+    <row r="27" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="121"/>
+      <c r="C27" s="122"/>
+      <c r="D27" s="122" t="s">
+        <v>272</v>
+      </c>
+      <c r="E27" s="123" t="s">
+        <v>273</v>
+      </c>
+      <c r="F27" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G27" s="125">
+        <v>44770</v>
+      </c>
+      <c r="H27" s="126">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="121"/>
+      <c r="C28" s="122"/>
+      <c r="D28" s="122" t="s">
+        <v>294</v>
+      </c>
+      <c r="E28" s="127" t="s">
+        <v>296</v>
+      </c>
+      <c r="F28" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G28" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H28" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="121"/>
+      <c r="C29" s="122"/>
+      <c r="D29" s="122" t="s">
+        <v>293</v>
+      </c>
+      <c r="E29" s="127" t="s">
+        <v>295</v>
+      </c>
+      <c r="F29" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G29" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H29" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="121"/>
+      <c r="C30" s="122"/>
+      <c r="D30" s="122" t="s">
+        <v>291</v>
+      </c>
+      <c r="E30" s="127" t="s">
+        <v>297</v>
+      </c>
+      <c r="F30" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G30" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H30" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="121"/>
+      <c r="C31" s="122"/>
+      <c r="D31" s="122" t="s">
+        <v>307</v>
+      </c>
+      <c r="E31" s="127" t="s">
+        <v>308</v>
+      </c>
+      <c r="F31" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G31" s="125">
+        <v>44949</v>
+      </c>
+      <c r="H31" s="126">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="121"/>
+      <c r="C32" s="122"/>
+      <c r="D32" s="122" t="s">
+        <v>292</v>
+      </c>
+      <c r="E32" s="127" t="s">
+        <v>298</v>
+      </c>
+      <c r="F32" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G32" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H32" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="121"/>
+      <c r="C33" s="122"/>
+      <c r="D33" s="122" t="s">
+        <v>290</v>
+      </c>
+      <c r="E33" s="127" t="s">
+        <v>299</v>
+      </c>
+      <c r="F33" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G33" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H33" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="121"/>
+      <c r="C34" s="122"/>
+      <c r="D34" s="122" t="s">
+        <v>289</v>
+      </c>
+      <c r="E34" s="127" t="s">
+        <v>300</v>
+      </c>
+      <c r="F34" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G34" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H34" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="121"/>
+      <c r="C35" s="122"/>
+      <c r="D35" s="122" t="s">
+        <v>288</v>
+      </c>
+      <c r="E35" s="127" t="s">
+        <v>301</v>
+      </c>
+      <c r="F35" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G35" s="125">
+        <v>44937</v>
+      </c>
+      <c r="H35" s="126">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="121"/>
+      <c r="C36" s="128" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="128" t="s">
+        <v>274</v>
+      </c>
+      <c r="E36" s="129" t="s">
+        <v>275</v>
+      </c>
+      <c r="F36" s="130" t="s">
+        <v>232</v>
+      </c>
+      <c r="G36" s="131">
+        <v>44167</v>
+      </c>
+      <c r="H36" s="132">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="121"/>
+      <c r="C37" s="122"/>
+      <c r="D37" s="133" t="s">
+        <v>276</v>
+      </c>
+      <c r="E37" s="123" t="s">
         <v>285</v>
       </c>
-      <c r="E20" s="96" t="s">
+      <c r="F37" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G37" s="125">
+        <v>44167</v>
+      </c>
+      <c r="H37" s="126">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="121"/>
+      <c r="C38" s="122"/>
+      <c r="D38" s="122" t="s">
         <v>278</v>
       </c>
-      <c r="F20" s="123" t="s">
+      <c r="E38" s="123" t="s">
+        <v>279</v>
+      </c>
+      <c r="F38" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G20" s="124">
-        <v>44931</v>
-      </c>
-      <c r="H20" s="125">
-        <v>44931</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B21" s="84"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80" t="s">
-        <v>264</v>
-      </c>
-      <c r="E21" s="96" t="s">
-        <v>265</v>
-      </c>
-      <c r="F21" s="123" t="s">
+      <c r="G38" s="125">
+        <v>43185</v>
+      </c>
+      <c r="H38" s="126">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="121"/>
+      <c r="C39" s="122"/>
+      <c r="D39" s="122" t="s">
+        <v>280</v>
+      </c>
+      <c r="E39" s="123" t="s">
+        <v>282</v>
+      </c>
+      <c r="F39" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G39" s="125">
+        <v>44216</v>
+      </c>
+      <c r="H39" s="126">
+        <v>44216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="121"/>
+      <c r="C40" s="122"/>
+      <c r="D40" s="122"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="124"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="126"/>
+    </row>
+    <row r="41" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="121"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122" t="s">
+        <v>286</v>
+      </c>
+      <c r="E41" s="123" t="s">
+        <v>287</v>
+      </c>
+      <c r="F41" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G21" s="124">
-        <v>44847</v>
-      </c>
-      <c r="H21" s="125">
-        <v>44847</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B22" s="84"/>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80" t="s">
-        <v>266</v>
-      </c>
-      <c r="E22" s="96" t="s">
-        <v>268</v>
-      </c>
-      <c r="F22" s="123" t="s">
-        <v>267</v>
-      </c>
-      <c r="G22" s="124">
-        <v>44792</v>
-      </c>
-      <c r="H22" s="125">
-        <v>44770</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B23" s="84"/>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80" t="s">
-        <v>269</v>
-      </c>
-      <c r="E23" s="96" t="s">
-        <v>270</v>
-      </c>
-      <c r="F23" s="123" t="s">
+      <c r="G41" s="125">
+        <v>44949</v>
+      </c>
+      <c r="H41" s="126">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="121"/>
+      <c r="C42" s="122"/>
+      <c r="D42" s="122"/>
+      <c r="E42" s="123"/>
+      <c r="F42" s="124"/>
+      <c r="G42" s="125"/>
+      <c r="H42" s="126"/>
+    </row>
+    <row r="43" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="121"/>
+      <c r="C43" s="122"/>
+      <c r="D43" s="122"/>
+      <c r="E43" s="123"/>
+      <c r="F43" s="124"/>
+      <c r="G43" s="125"/>
+      <c r="H43" s="126"/>
+    </row>
+    <row r="44" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="121"/>
+      <c r="C44" s="122"/>
+      <c r="D44" s="122"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="124"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="126"/>
+    </row>
+    <row r="45" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="121"/>
+      <c r="C45" s="122"/>
+      <c r="D45" s="122"/>
+      <c r="E45" s="127"/>
+      <c r="F45" s="124"/>
+      <c r="G45" s="125"/>
+      <c r="H45" s="126"/>
+    </row>
+    <row r="46" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="121"/>
+      <c r="C46" s="122"/>
+      <c r="D46" s="122"/>
+      <c r="E46" s="123"/>
+      <c r="F46" s="124"/>
+      <c r="G46" s="125"/>
+      <c r="H46" s="126"/>
+    </row>
+    <row r="47" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="121"/>
+      <c r="C47" s="122" t="s">
+        <v>338</v>
+      </c>
+      <c r="D47" s="122" t="s">
+        <v>327</v>
+      </c>
+      <c r="E47" s="127" t="s">
+        <v>328</v>
+      </c>
+      <c r="F47" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G23" s="124">
-        <v>44776</v>
-      </c>
-      <c r="H23" s="125">
-        <v>44776</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B24" s="84"/>
-      <c r="C24" s="80"/>
-      <c r="D24" s="80" t="s">
-        <v>272</v>
-      </c>
-      <c r="E24" s="96" t="s">
-        <v>271</v>
-      </c>
-      <c r="F24" s="123" t="s">
+      <c r="G47" s="125">
+        <v>44902</v>
+      </c>
+      <c r="H47" s="126">
+        <v>44902</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="121"/>
+      <c r="C48" s="122"/>
+      <c r="D48" s="122" t="s">
+        <v>333</v>
+      </c>
+      <c r="E48" s="127" t="s">
+        <v>335</v>
+      </c>
+      <c r="F48" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G24" s="124">
-        <v>44777</v>
-      </c>
-      <c r="H24" s="125">
-        <v>44777</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B25" s="84"/>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80" t="s">
-        <v>273</v>
-      </c>
-      <c r="E25" s="96" t="s">
-        <v>274</v>
-      </c>
-      <c r="F25" s="123" t="s">
+      <c r="G48" s="125">
+        <v>44897</v>
+      </c>
+      <c r="H48" s="126">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="121"/>
+      <c r="C49" s="122"/>
+      <c r="D49" s="122" t="s">
+        <v>321</v>
+      </c>
+      <c r="E49" s="127" t="s">
+        <v>326</v>
+      </c>
+      <c r="F49" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G49" s="125">
+        <v>44900</v>
+      </c>
+      <c r="H49" s="126">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="121"/>
+      <c r="C50" s="122"/>
+      <c r="D50" s="122" t="s">
+        <v>329</v>
+      </c>
+      <c r="E50" s="123" t="s">
+        <v>330</v>
+      </c>
+      <c r="F50" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G50" s="125">
+        <v>44896</v>
+      </c>
+      <c r="H50" s="126">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="121"/>
+      <c r="C51" s="122"/>
+      <c r="D51" s="122" t="s">
+        <v>322</v>
+      </c>
+      <c r="E51" s="127" t="s">
+        <v>323</v>
+      </c>
+      <c r="F51" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G51" s="125">
+        <v>44945</v>
+      </c>
+      <c r="H51" s="126">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="121"/>
+      <c r="C52" s="122"/>
+      <c r="D52" s="122" t="s">
+        <v>336</v>
+      </c>
+      <c r="E52" s="127" t="s">
+        <v>337</v>
+      </c>
+      <c r="F52" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G52" s="125">
+        <v>44910</v>
+      </c>
+      <c r="H52" s="126">
+        <v>44910</v>
+      </c>
+      <c r="J52" s="78" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A53" s="1"/>
+      <c r="B53" s="121"/>
+      <c r="C53" s="122"/>
+      <c r="D53" s="122" t="s">
+        <v>331</v>
+      </c>
+      <c r="E53" s="123" t="s">
+        <v>332</v>
+      </c>
+      <c r="F53" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G25" s="124">
-        <v>44770</v>
-      </c>
-      <c r="H25" s="125">
-        <v>44770</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B26" s="84"/>
-      <c r="C26" s="79" t="s">
-        <v>146</v>
-      </c>
-      <c r="D26" s="79" t="s">
-        <v>275</v>
-      </c>
-      <c r="E26" s="101" t="s">
-        <v>276</v>
-      </c>
-      <c r="F26" s="126" t="s">
+      <c r="G53" s="125">
+        <v>44893</v>
+      </c>
+      <c r="H53" s="126">
+        <v>44893</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A54" s="1"/>
+      <c r="B54" s="121"/>
+      <c r="C54" s="122"/>
+      <c r="D54" s="122"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="124"/>
+      <c r="G54" s="125"/>
+      <c r="H54" s="126"/>
+    </row>
+    <row r="55" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="121"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="124"/>
+      <c r="G55" s="125"/>
+      <c r="H55" s="126"/>
+    </row>
+    <row r="56" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="121"/>
+      <c r="C56" s="122"/>
+      <c r="D56" s="122"/>
+      <c r="E56" s="123"/>
+      <c r="F56" s="124"/>
+      <c r="G56" s="125"/>
+      <c r="H56" s="126"/>
+    </row>
+    <row r="57" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="1"/>
+      <c r="B57" s="121"/>
+      <c r="C57" s="122"/>
+      <c r="D57" s="122"/>
+      <c r="E57" s="123"/>
+      <c r="F57" s="124"/>
+      <c r="G57" s="125"/>
+      <c r="H57" s="126"/>
+    </row>
+    <row r="58" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="121"/>
+      <c r="C58" s="122" t="s">
+        <v>339</v>
+      </c>
+      <c r="D58" s="122" t="s">
+        <v>324</v>
+      </c>
+      <c r="E58" s="127" t="s">
+        <v>325</v>
+      </c>
+      <c r="F58" s="124" t="s">
         <v>232</v>
       </c>
-      <c r="G26" s="127">
-        <v>44167</v>
-      </c>
-      <c r="H26" s="128">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B27" s="84"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="129" t="s">
-        <v>277</v>
-      </c>
-      <c r="E27" s="96" t="s">
-        <v>286</v>
-      </c>
-      <c r="F27" s="123" t="s">
-        <v>232</v>
-      </c>
-      <c r="G27" s="124">
-        <v>44167</v>
-      </c>
-      <c r="H27" s="125">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B28" s="84"/>
-      <c r="C28" s="80"/>
-      <c r="D28" s="80" t="s">
-        <v>279</v>
-      </c>
-      <c r="E28" s="96" t="s">
-        <v>280</v>
-      </c>
-      <c r="F28" s="123" t="s">
-        <v>232</v>
-      </c>
-      <c r="G28" s="124">
-        <v>43185</v>
-      </c>
-      <c r="H28" s="125">
-        <v>43185</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B29" s="84"/>
-      <c r="C29" s="80"/>
-      <c r="D29" s="80" t="s">
-        <v>281</v>
-      </c>
-      <c r="E29" s="96" t="s">
-        <v>283</v>
-      </c>
-      <c r="F29" s="123" t="s">
-        <v>282</v>
-      </c>
-      <c r="G29" s="124">
-        <v>44216</v>
-      </c>
-      <c r="H29" s="125">
-        <v>44216</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B30" s="84"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="80"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="124"/>
-      <c r="H30" s="125"/>
-    </row>
-    <row r="31" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B31" s="84"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="123"/>
-      <c r="G31" s="124"/>
-      <c r="H31" s="125"/>
-    </row>
-    <row r="32" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B32" s="84"/>
-      <c r="C32" s="80"/>
-      <c r="D32" s="80"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="123"/>
-      <c r="G32" s="124"/>
-      <c r="H32" s="125"/>
-    </row>
-    <row r="33" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B33" s="84"/>
-      <c r="C33" s="80"/>
-      <c r="D33" s="80"/>
-      <c r="E33" s="96"/>
-      <c r="F33" s="123"/>
-      <c r="G33" s="124"/>
-      <c r="H33" s="125"/>
-    </row>
-    <row r="34" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B34" s="84"/>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="96"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="125"/>
-    </row>
-    <row r="35" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B35" s="84"/>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="96"/>
-      <c r="F35" s="123"/>
-      <c r="G35" s="124"/>
-      <c r="H35" s="125"/>
-    </row>
-    <row r="36" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B36" s="84"/>
-      <c r="C36" s="80"/>
-      <c r="D36" s="80"/>
-      <c r="E36" s="96"/>
-      <c r="F36" s="123"/>
-      <c r="G36" s="124"/>
-      <c r="H36" s="125"/>
-    </row>
-    <row r="37" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B37" s="84"/>
-      <c r="C37" s="80"/>
-      <c r="D37" s="80"/>
-      <c r="E37" s="96"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="124"/>
-      <c r="H37" s="125"/>
-    </row>
-    <row r="38" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B38" s="84"/>
-      <c r="C38" s="80"/>
-      <c r="D38" s="80"/>
-      <c r="E38" s="96"/>
-      <c r="F38" s="123"/>
-      <c r="G38" s="124"/>
-      <c r="H38" s="125"/>
-    </row>
-    <row r="39" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B39" s="84"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="96"/>
-      <c r="F39" s="123"/>
-      <c r="G39" s="124"/>
-      <c r="H39" s="125"/>
-    </row>
-    <row r="40" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B40" s="84"/>
-      <c r="C40" s="80"/>
-      <c r="D40" s="80"/>
-      <c r="E40" s="96"/>
-      <c r="F40" s="123"/>
-      <c r="G40" s="124"/>
-      <c r="H40" s="125"/>
-    </row>
-    <row r="41" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B41" s="84"/>
-      <c r="C41" s="80"/>
-      <c r="D41" s="80"/>
-      <c r="E41" s="96"/>
-      <c r="F41" s="123"/>
-      <c r="G41" s="124"/>
-      <c r="H41" s="125"/>
-    </row>
-    <row r="42" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B42" s="84"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="96"/>
-      <c r="F42" s="123"/>
-      <c r="G42" s="124"/>
-      <c r="H42" s="125"/>
-    </row>
-    <row r="43" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B43" s="84"/>
-      <c r="C43" s="80"/>
-      <c r="D43" s="80"/>
-      <c r="E43" s="96"/>
-      <c r="F43" s="123"/>
-      <c r="G43" s="124"/>
-      <c r="H43" s="125"/>
-    </row>
-    <row r="44" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B44" s="84"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="96"/>
-      <c r="F44" s="123"/>
-      <c r="G44" s="124"/>
-      <c r="H44" s="125"/>
-    </row>
-    <row r="45" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B45" s="84"/>
-      <c r="C45" s="80"/>
-      <c r="D45" s="80"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="123"/>
-      <c r="G45" s="124"/>
-      <c r="H45" s="125"/>
-    </row>
-    <row r="46" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B46" s="84"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="123"/>
-      <c r="G46" s="124"/>
-      <c r="H46" s="125"/>
-    </row>
-    <row r="47" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="84"/>
-      <c r="C47" s="80"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="96"/>
-      <c r="F47" s="123"/>
-      <c r="G47" s="124"/>
-      <c r="H47" s="125"/>
-    </row>
-    <row r="48" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B48" s="84"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="96"/>
-      <c r="F48" s="123"/>
-      <c r="G48" s="124"/>
-      <c r="H48" s="125"/>
-    </row>
-    <row r="49" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B49" s="84"/>
-      <c r="C49" s="80"/>
-      <c r="D49" s="80"/>
-      <c r="E49" s="96"/>
-      <c r="F49" s="123"/>
-      <c r="G49" s="124"/>
-      <c r="H49" s="125"/>
-    </row>
-    <row r="50" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B50" s="84"/>
-      <c r="C50" s="80"/>
-      <c r="D50" s="80"/>
-      <c r="E50" s="96"/>
-      <c r="F50" s="123"/>
-      <c r="G50" s="124"/>
-      <c r="H50" s="125"/>
-    </row>
-    <row r="51" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B51" s="84"/>
-      <c r="C51" s="80"/>
-      <c r="D51" s="80"/>
-      <c r="E51" s="96"/>
-      <c r="F51" s="123"/>
-      <c r="G51" s="124"/>
-      <c r="H51" s="125"/>
-    </row>
-    <row r="52" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B52" s="84"/>
-      <c r="C52" s="80"/>
-      <c r="D52" s="80"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="123"/>
-      <c r="G52" s="124"/>
-      <c r="H52" s="125"/>
-    </row>
-    <row r="53" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B53" s="84"/>
-      <c r="C53" s="80"/>
-      <c r="D53" s="80"/>
-      <c r="E53" s="96"/>
-      <c r="F53" s="123"/>
-      <c r="G53" s="124"/>
-      <c r="H53" s="125"/>
-    </row>
-    <row r="54" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B54" s="84"/>
-      <c r="C54" s="80"/>
-      <c r="D54" s="80"/>
-      <c r="E54" s="96"/>
-      <c r="F54" s="123"/>
-      <c r="G54" s="124"/>
-      <c r="H54" s="125"/>
-    </row>
-    <row r="55" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B55" s="84"/>
-      <c r="C55" s="80"/>
-      <c r="D55" s="80"/>
-      <c r="E55" s="96"/>
-      <c r="F55" s="123"/>
-      <c r="G55" s="124"/>
-      <c r="H55" s="125"/>
-    </row>
-    <row r="56" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B56" s="84"/>
-      <c r="C56" s="80"/>
-      <c r="D56" s="80"/>
-      <c r="E56" s="96"/>
-      <c r="F56" s="123"/>
-      <c r="G56" s="124"/>
-      <c r="H56" s="125"/>
-    </row>
-    <row r="57" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B57" s="84"/>
-      <c r="C57" s="80"/>
-      <c r="D57" s="80"/>
-      <c r="E57" s="96"/>
-      <c r="F57" s="123"/>
-      <c r="G57" s="124"/>
-      <c r="H57" s="125"/>
-    </row>
-    <row r="58" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B58" s="84"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="80"/>
-      <c r="E58" s="96"/>
-      <c r="F58" s="123"/>
-      <c r="G58" s="124"/>
-      <c r="H58" s="125"/>
-    </row>
-    <row r="59" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B59" s="84"/>
-      <c r="C59" s="80"/>
-      <c r="D59" s="80"/>
-      <c r="E59" s="96"/>
-      <c r="F59" s="123"/>
-      <c r="G59" s="124"/>
-      <c r="H59" s="125"/>
-    </row>
-    <row r="60" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B60" s="84"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="80"/>
-      <c r="E60" s="96"/>
-      <c r="F60" s="123"/>
-      <c r="G60" s="124"/>
-      <c r="H60" s="125"/>
-    </row>
-    <row r="61" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B61" s="84"/>
-      <c r="C61" s="80"/>
-      <c r="D61" s="80"/>
-      <c r="E61" s="96"/>
-      <c r="F61" s="123"/>
-      <c r="G61" s="124"/>
-      <c r="H61" s="125"/>
-    </row>
-    <row r="62" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B62" s="84"/>
-      <c r="C62" s="80"/>
-      <c r="D62" s="80"/>
-      <c r="E62" s="96"/>
-      <c r="F62" s="123"/>
-      <c r="G62" s="124"/>
-      <c r="H62" s="125"/>
-    </row>
-    <row r="63" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B63" s="84"/>
-      <c r="C63" s="80"/>
-      <c r="D63" s="80"/>
-      <c r="E63" s="96"/>
-      <c r="F63" s="123"/>
-      <c r="G63" s="124"/>
-      <c r="H63" s="125"/>
-    </row>
-    <row r="64" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B64" s="84"/>
-      <c r="C64" s="80"/>
-      <c r="D64" s="80"/>
-      <c r="E64" s="96"/>
-      <c r="F64" s="123"/>
-      <c r="G64" s="124"/>
-      <c r="H64" s="125"/>
-    </row>
-    <row r="65" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B65" s="84"/>
-      <c r="C65" s="80"/>
-      <c r="D65" s="80"/>
-      <c r="E65" s="96"/>
-      <c r="F65" s="123"/>
-      <c r="G65" s="124"/>
-      <c r="H65" s="125"/>
-    </row>
-    <row r="66" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B66" s="84"/>
-      <c r="C66" s="80"/>
-      <c r="D66" s="80"/>
-      <c r="E66" s="96"/>
-      <c r="F66" s="123"/>
-      <c r="G66" s="124"/>
-      <c r="H66" s="125"/>
-    </row>
-    <row r="67" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B67" s="84"/>
-      <c r="C67" s="80"/>
-      <c r="D67" s="80"/>
-      <c r="E67" s="96"/>
-      <c r="F67" s="123"/>
-      <c r="G67" s="124"/>
-      <c r="H67" s="125"/>
-    </row>
-    <row r="68" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B68" s="84"/>
-      <c r="C68" s="80"/>
-      <c r="D68" s="80"/>
-      <c r="E68" s="96"/>
-      <c r="F68" s="123"/>
-      <c r="G68" s="124"/>
-      <c r="H68" s="125"/>
-    </row>
-    <row r="69" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B69" s="84"/>
-      <c r="C69" s="80"/>
-      <c r="D69" s="80"/>
-      <c r="E69" s="96"/>
-      <c r="F69" s="123"/>
-      <c r="G69" s="124"/>
-      <c r="H69" s="125"/>
-    </row>
-    <row r="70" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B70" s="84"/>
-      <c r="C70" s="80"/>
-      <c r="D70" s="80"/>
-      <c r="E70" s="96"/>
-      <c r="F70" s="123"/>
-      <c r="G70" s="124"/>
-      <c r="H70" s="125"/>
-    </row>
-    <row r="71" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B71" s="84"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="80"/>
-      <c r="E71" s="96"/>
-      <c r="F71" s="123"/>
-      <c r="G71" s="124"/>
-      <c r="H71" s="125"/>
-    </row>
-    <row r="72" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B72" s="84"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="80"/>
-      <c r="E72" s="96"/>
-      <c r="F72" s="123"/>
-      <c r="G72" s="124"/>
-      <c r="H72" s="125"/>
-    </row>
-    <row r="73" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B73" s="84"/>
-      <c r="C73" s="80"/>
-      <c r="D73" s="80"/>
-      <c r="E73" s="96"/>
-      <c r="F73" s="123"/>
-      <c r="G73" s="124"/>
-      <c r="H73" s="125"/>
-    </row>
-    <row r="74" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B74" s="84"/>
-      <c r="C74" s="80"/>
-      <c r="D74" s="80"/>
-      <c r="E74" s="96"/>
-      <c r="F74" s="123"/>
-      <c r="G74" s="124"/>
-      <c r="H74" s="125"/>
-    </row>
-    <row r="75" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B75" s="84"/>
-      <c r="C75" s="80"/>
-      <c r="D75" s="80"/>
-      <c r="E75" s="96"/>
-      <c r="F75" s="123"/>
-      <c r="G75" s="124"/>
-      <c r="H75" s="125"/>
-    </row>
-    <row r="76" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B76" s="84"/>
-      <c r="C76" s="80"/>
-      <c r="D76" s="80"/>
-      <c r="E76" s="96"/>
-      <c r="F76" s="123"/>
-      <c r="G76" s="124"/>
-      <c r="H76" s="125"/>
-    </row>
-    <row r="77" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B77" s="84"/>
-      <c r="C77" s="80"/>
-      <c r="D77" s="80"/>
-      <c r="E77" s="96"/>
-      <c r="F77" s="123"/>
-      <c r="G77" s="124"/>
-      <c r="H77" s="125"/>
-    </row>
-    <row r="78" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B78" s="84"/>
-      <c r="C78" s="80"/>
-      <c r="D78" s="80"/>
-      <c r="E78" s="96"/>
-      <c r="F78" s="123"/>
-      <c r="G78" s="124"/>
-      <c r="H78" s="125"/>
-    </row>
-    <row r="79" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B79" s="84"/>
-      <c r="C79" s="80"/>
-      <c r="D79" s="80"/>
-      <c r="E79" s="96"/>
-      <c r="F79" s="123"/>
-      <c r="G79" s="124"/>
-      <c r="H79" s="125"/>
-    </row>
-    <row r="80" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="84"/>
-      <c r="C80" s="80"/>
-      <c r="D80" s="80"/>
-      <c r="E80" s="96"/>
-      <c r="F80" s="123"/>
-      <c r="G80" s="124"/>
-      <c r="H80" s="125"/>
-    </row>
-    <row r="81" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B81" s="84"/>
-      <c r="C81" s="80"/>
-      <c r="D81" s="80"/>
-      <c r="E81" s="96"/>
-      <c r="F81" s="123"/>
-      <c r="G81" s="124"/>
-      <c r="H81" s="125"/>
-    </row>
-    <row r="82" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B82" s="84"/>
-      <c r="C82" s="80"/>
-      <c r="D82" s="80"/>
-      <c r="E82" s="96"/>
-      <c r="F82" s="123"/>
-      <c r="G82" s="124"/>
-      <c r="H82" s="125"/>
-    </row>
-    <row r="83" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B83" s="84"/>
-      <c r="C83" s="80"/>
-      <c r="D83" s="80"/>
-      <c r="E83" s="96"/>
-      <c r="F83" s="123"/>
-      <c r="G83" s="124"/>
-      <c r="H83" s="125"/>
-    </row>
-    <row r="84" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B84" s="84"/>
-      <c r="C84" s="80"/>
-      <c r="D84" s="80"/>
-      <c r="E84" s="96"/>
-      <c r="F84" s="123"/>
-      <c r="G84" s="124"/>
-      <c r="H84" s="125"/>
-    </row>
-    <row r="85" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B85" s="84"/>
-      <c r="C85" s="80"/>
-      <c r="D85" s="80"/>
-      <c r="E85" s="96"/>
-      <c r="F85" s="123"/>
-      <c r="G85" s="124"/>
-      <c r="H85" s="125"/>
-    </row>
-    <row r="86" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B86" s="84"/>
-      <c r="C86" s="80"/>
-      <c r="D86" s="80"/>
-      <c r="E86" s="96"/>
-      <c r="F86" s="123"/>
-      <c r="G86" s="124"/>
-      <c r="H86" s="125"/>
-    </row>
-    <row r="87" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B87" s="84"/>
-      <c r="C87" s="80"/>
-      <c r="D87" s="80"/>
-      <c r="E87" s="96"/>
-      <c r="F87" s="123"/>
-      <c r="G87" s="124"/>
-      <c r="H87" s="125"/>
-    </row>
-    <row r="88" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B88" s="84"/>
-      <c r="C88" s="80"/>
-      <c r="D88" s="80"/>
-      <c r="E88" s="96"/>
-      <c r="F88" s="123"/>
-      <c r="G88" s="124"/>
-      <c r="H88" s="125"/>
-    </row>
-    <row r="89" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B89" s="84"/>
-      <c r="C89" s="80"/>
-      <c r="D89" s="80"/>
-      <c r="E89" s="96"/>
-      <c r="F89" s="123"/>
-      <c r="G89" s="124"/>
-      <c r="H89" s="125"/>
-    </row>
-    <row r="90" spans="2:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="87"/>
-      <c r="C90" s="88"/>
-      <c r="D90" s="88"/>
-      <c r="E90" s="103"/>
-      <c r="F90" s="120"/>
-      <c r="G90" s="121"/>
-      <c r="H90" s="122"/>
-    </row>
-    <row r="91" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F91" s="95"/>
-      <c r="G91" s="111"/>
-      <c r="H91" s="111"/>
-    </row>
-    <row r="92" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F92" s="95"/>
-      <c r="G92" s="111"/>
-      <c r="H92" s="111"/>
-    </row>
-    <row r="93" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F93" s="95"/>
-      <c r="G93" s="111"/>
-      <c r="H93" s="111"/>
-    </row>
-    <row r="94" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F94" s="95"/>
-      <c r="G94" s="111"/>
-      <c r="H94" s="111"/>
-    </row>
-    <row r="95" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F95" s="95"/>
-      <c r="G95" s="111"/>
-      <c r="H95" s="111"/>
-    </row>
-    <row r="96" spans="2:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F96" s="95"/>
-      <c r="G96" s="111"/>
-      <c r="H96" s="111"/>
-    </row>
-    <row r="97" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F97" s="95"/>
-      <c r="G97" s="111"/>
-      <c r="H97" s="111"/>
-    </row>
-    <row r="98" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F98" s="95"/>
-      <c r="G98" s="111"/>
-      <c r="H98" s="111"/>
-    </row>
-    <row r="99" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F99" s="95"/>
-      <c r="G99" s="111"/>
-      <c r="H99" s="111"/>
-    </row>
-    <row r="100" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F100" s="95"/>
-      <c r="G100" s="111"/>
-      <c r="H100" s="111"/>
-    </row>
-    <row r="101" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F101" s="95"/>
-      <c r="G101" s="111"/>
-      <c r="H101" s="111"/>
-    </row>
-    <row r="102" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F102" s="95"/>
-      <c r="G102" s="111"/>
-      <c r="H102" s="111"/>
-    </row>
-    <row r="103" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F103" s="95"/>
-      <c r="G103" s="111"/>
-      <c r="H103" s="111"/>
-    </row>
-    <row r="104" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F104" s="95"/>
-      <c r="G104" s="111"/>
-      <c r="H104" s="111"/>
-    </row>
-    <row r="105" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F105" s="95"/>
-      <c r="G105" s="111"/>
-      <c r="H105" s="111"/>
-    </row>
-    <row r="106" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F106" s="95"/>
-      <c r="G106" s="111"/>
-      <c r="H106" s="111"/>
-    </row>
-    <row r="107" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F107" s="95"/>
-      <c r="G107" s="111"/>
-      <c r="H107" s="111"/>
-    </row>
-    <row r="108" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F108" s="95"/>
-      <c r="G108" s="111"/>
-      <c r="H108" s="111"/>
-    </row>
-    <row r="109" spans="6:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F109" s="95"/>
-      <c r="G109" s="111"/>
-      <c r="H109" s="111"/>
+      <c r="G58" s="125">
+        <v>44900</v>
+      </c>
+      <c r="H58" s="126">
+        <v>44900</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="121"/>
+      <c r="C59" s="122"/>
+      <c r="D59" s="122"/>
+      <c r="E59" s="123"/>
+      <c r="F59" s="124"/>
+      <c r="G59" s="125"/>
+      <c r="H59" s="126"/>
+    </row>
+    <row r="60" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="121"/>
+      <c r="C60" s="122"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="123"/>
+      <c r="F60" s="124"/>
+      <c r="G60" s="125"/>
+      <c r="H60" s="126"/>
+    </row>
+    <row r="61" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="121"/>
+      <c r="C61" s="122"/>
+      <c r="D61" s="122"/>
+      <c r="E61" s="123"/>
+      <c r="F61" s="124"/>
+      <c r="G61" s="125"/>
+      <c r="H61" s="126"/>
+    </row>
+    <row r="62" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="121"/>
+      <c r="C62" s="122"/>
+      <c r="D62" s="122"/>
+      <c r="E62" s="123"/>
+      <c r="F62" s="124"/>
+      <c r="G62" s="125"/>
+      <c r="H62" s="126"/>
+    </row>
+    <row r="63" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="121"/>
+      <c r="C63" s="122"/>
+      <c r="D63" s="122"/>
+      <c r="E63" s="123"/>
+      <c r="F63" s="124"/>
+      <c r="G63" s="125"/>
+      <c r="H63" s="126"/>
+    </row>
+    <row r="64" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="121"/>
+      <c r="C64" s="122"/>
+      <c r="D64" s="122"/>
+      <c r="E64" s="123"/>
+      <c r="F64" s="124"/>
+      <c r="G64" s="125"/>
+      <c r="H64" s="126"/>
+    </row>
+    <row r="65" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="121"/>
+      <c r="C65" s="122"/>
+      <c r="D65" s="122"/>
+      <c r="E65" s="123"/>
+      <c r="F65" s="124"/>
+      <c r="G65" s="125"/>
+      <c r="H65" s="126"/>
+    </row>
+    <row r="66" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="B66" s="121"/>
+      <c r="C66" s="122"/>
+      <c r="D66" s="122"/>
+      <c r="E66" s="123"/>
+      <c r="F66" s="124"/>
+      <c r="G66" s="125"/>
+      <c r="H66" s="126"/>
+    </row>
+    <row r="67" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="B67" s="121"/>
+      <c r="C67" s="122"/>
+      <c r="D67" s="122"/>
+      <c r="E67" s="123"/>
+      <c r="F67" s="124"/>
+      <c r="G67" s="125"/>
+      <c r="H67" s="126"/>
+    </row>
+    <row r="68" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="121"/>
+      <c r="C68" s="122"/>
+      <c r="D68" s="122"/>
+      <c r="E68" s="123"/>
+      <c r="F68" s="124"/>
+      <c r="G68" s="125"/>
+      <c r="H68" s="126"/>
+    </row>
+    <row r="69" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="121"/>
+      <c r="C69" s="122"/>
+      <c r="D69" s="122"/>
+      <c r="E69" s="123"/>
+      <c r="F69" s="124"/>
+      <c r="G69" s="125"/>
+      <c r="H69" s="126"/>
+    </row>
+    <row r="70" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="B70" s="121"/>
+      <c r="C70" s="122"/>
+      <c r="D70" s="122"/>
+      <c r="E70" s="123"/>
+      <c r="F70" s="124"/>
+      <c r="G70" s="125"/>
+      <c r="H70" s="126"/>
+    </row>
+    <row r="71" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="1"/>
+      <c r="B71" s="121"/>
+      <c r="C71" s="122"/>
+      <c r="D71" s="122"/>
+      <c r="E71" s="123"/>
+      <c r="F71" s="124"/>
+      <c r="G71" s="125"/>
+      <c r="H71" s="126"/>
+    </row>
+    <row r="72" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="1"/>
+      <c r="B72" s="121"/>
+      <c r="C72" s="122"/>
+      <c r="D72" s="122"/>
+      <c r="E72" s="123"/>
+      <c r="F72" s="124"/>
+      <c r="G72" s="125"/>
+      <c r="H72" s="126"/>
+    </row>
+    <row r="73" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="1"/>
+      <c r="B73" s="121"/>
+      <c r="C73" s="122"/>
+      <c r="D73" s="122"/>
+      <c r="E73" s="123"/>
+      <c r="F73" s="124"/>
+      <c r="G73" s="125"/>
+      <c r="H73" s="126"/>
+    </row>
+    <row r="74" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="121"/>
+      <c r="C74" s="122"/>
+      <c r="D74" s="122"/>
+      <c r="E74" s="123"/>
+      <c r="F74" s="124"/>
+      <c r="G74" s="125"/>
+      <c r="H74" s="126"/>
+    </row>
+    <row r="75" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="121"/>
+      <c r="C75" s="122"/>
+      <c r="D75" s="122"/>
+      <c r="E75" s="123"/>
+      <c r="F75" s="124"/>
+      <c r="G75" s="125"/>
+      <c r="H75" s="126"/>
+    </row>
+    <row r="76" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="121"/>
+      <c r="C76" s="122"/>
+      <c r="D76" s="122"/>
+      <c r="E76" s="123"/>
+      <c r="F76" s="124"/>
+      <c r="G76" s="125"/>
+      <c r="H76" s="126"/>
+    </row>
+    <row r="77" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="1"/>
+      <c r="B77" s="121"/>
+      <c r="C77" s="122"/>
+      <c r="D77" s="122"/>
+      <c r="E77" s="123"/>
+      <c r="F77" s="124"/>
+      <c r="G77" s="125"/>
+      <c r="H77" s="126"/>
+    </row>
+    <row r="78" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="121"/>
+      <c r="C78" s="122"/>
+      <c r="D78" s="122"/>
+      <c r="E78" s="123"/>
+      <c r="F78" s="124"/>
+      <c r="G78" s="125"/>
+      <c r="H78" s="126"/>
+    </row>
+    <row r="79" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="121"/>
+      <c r="C79" s="122"/>
+      <c r="D79" s="122"/>
+      <c r="E79" s="123"/>
+      <c r="F79" s="124"/>
+      <c r="G79" s="125"/>
+      <c r="H79" s="126"/>
+    </row>
+    <row r="80" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="121"/>
+      <c r="C80" s="122"/>
+      <c r="D80" s="122"/>
+      <c r="E80" s="123"/>
+      <c r="F80" s="124"/>
+      <c r="G80" s="125"/>
+      <c r="H80" s="126"/>
+    </row>
+    <row r="81" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="121"/>
+      <c r="C81" s="122"/>
+      <c r="D81" s="122"/>
+      <c r="E81" s="123"/>
+      <c r="F81" s="124"/>
+      <c r="G81" s="125"/>
+      <c r="H81" s="126"/>
+    </row>
+    <row r="82" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+      <c r="B82" s="121"/>
+      <c r="C82" s="122"/>
+      <c r="D82" s="122"/>
+      <c r="E82" s="123"/>
+      <c r="F82" s="124"/>
+      <c r="G82" s="125"/>
+      <c r="H82" s="126"/>
+    </row>
+    <row r="83" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A83" s="1"/>
+      <c r="B83" s="121"/>
+      <c r="C83" s="122"/>
+      <c r="D83" s="122"/>
+      <c r="E83" s="123"/>
+      <c r="F83" s="124"/>
+      <c r="G83" s="125"/>
+      <c r="H83" s="126"/>
+    </row>
+    <row r="84" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A84" s="1"/>
+      <c r="B84" s="121"/>
+      <c r="C84" s="122"/>
+      <c r="D84" s="122"/>
+      <c r="E84" s="123"/>
+      <c r="F84" s="124"/>
+      <c r="G84" s="125"/>
+      <c r="H84" s="126"/>
+    </row>
+    <row r="85" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A85" s="1"/>
+      <c r="B85" s="121"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
+      <c r="E85" s="123"/>
+      <c r="F85" s="124"/>
+      <c r="G85" s="125"/>
+      <c r="H85" s="126"/>
+    </row>
+    <row r="86" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A86" s="1"/>
+      <c r="B86" s="121"/>
+      <c r="C86" s="122"/>
+      <c r="D86" s="122"/>
+      <c r="E86" s="123"/>
+      <c r="F86" s="124"/>
+      <c r="G86" s="125"/>
+      <c r="H86" s="126"/>
+    </row>
+    <row r="87" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A87" s="1"/>
+      <c r="B87" s="121"/>
+      <c r="C87" s="122"/>
+      <c r="D87" s="122"/>
+      <c r="E87" s="123"/>
+      <c r="F87" s="124"/>
+      <c r="G87" s="125"/>
+      <c r="H87" s="126"/>
+    </row>
+    <row r="88" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A88" s="1"/>
+      <c r="B88" s="121"/>
+      <c r="C88" s="122"/>
+      <c r="D88" s="122"/>
+      <c r="E88" s="123"/>
+      <c r="F88" s="124"/>
+      <c r="G88" s="125"/>
+      <c r="H88" s="126"/>
+    </row>
+    <row r="89" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A89" s="1"/>
+      <c r="B89" s="121"/>
+      <c r="C89" s="122"/>
+      <c r="D89" s="122"/>
+      <c r="E89" s="123"/>
+      <c r="F89" s="124"/>
+      <c r="G89" s="125"/>
+      <c r="H89" s="126"/>
+    </row>
+    <row r="90" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="121"/>
+      <c r="C90" s="122"/>
+      <c r="D90" s="122"/>
+      <c r="E90" s="123"/>
+      <c r="F90" s="124"/>
+      <c r="G90" s="125"/>
+      <c r="H90" s="126"/>
+    </row>
+    <row r="91" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
+      <c r="B91" s="121"/>
+      <c r="C91" s="122"/>
+      <c r="D91" s="122"/>
+      <c r="E91" s="123"/>
+      <c r="F91" s="124"/>
+      <c r="G91" s="125"/>
+      <c r="H91" s="126"/>
+    </row>
+    <row r="92" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A92" s="1"/>
+      <c r="B92" s="121"/>
+      <c r="C92" s="122"/>
+      <c r="D92" s="122"/>
+      <c r="E92" s="123"/>
+      <c r="F92" s="124"/>
+      <c r="G92" s="125"/>
+      <c r="H92" s="126"/>
+    </row>
+    <row r="93" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A93" s="1"/>
+      <c r="B93" s="121"/>
+      <c r="C93" s="122"/>
+      <c r="D93" s="122"/>
+      <c r="E93" s="123"/>
+      <c r="F93" s="124"/>
+      <c r="G93" s="125"/>
+      <c r="H93" s="126"/>
+    </row>
+    <row r="94" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="121"/>
+      <c r="C94" s="122"/>
+      <c r="D94" s="122"/>
+      <c r="E94" s="123"/>
+      <c r="F94" s="124"/>
+      <c r="G94" s="125"/>
+      <c r="H94" s="126"/>
+    </row>
+    <row r="95" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
+      <c r="B95" s="121"/>
+      <c r="C95" s="122"/>
+      <c r="D95" s="122"/>
+      <c r="E95" s="123"/>
+      <c r="F95" s="124"/>
+      <c r="G95" s="125"/>
+      <c r="H95" s="126"/>
+    </row>
+    <row r="96" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="1"/>
+      <c r="B96" s="121"/>
+      <c r="C96" s="122"/>
+      <c r="D96" s="122"/>
+      <c r="E96" s="123"/>
+      <c r="F96" s="124"/>
+      <c r="G96" s="125"/>
+      <c r="H96" s="126"/>
+    </row>
+    <row r="97" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A97" s="1"/>
+      <c r="B97" s="121"/>
+      <c r="C97" s="122"/>
+      <c r="D97" s="122"/>
+      <c r="E97" s="123"/>
+      <c r="F97" s="124"/>
+      <c r="G97" s="125"/>
+      <c r="H97" s="126"/>
+    </row>
+    <row r="98" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A98" s="1"/>
+      <c r="B98" s="121"/>
+      <c r="C98" s="122"/>
+      <c r="D98" s="122"/>
+      <c r="E98" s="123"/>
+      <c r="F98" s="124"/>
+      <c r="G98" s="125"/>
+      <c r="H98" s="126"/>
+    </row>
+    <row r="99" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A99" s="1"/>
+      <c r="B99" s="121"/>
+      <c r="C99" s="122"/>
+      <c r="D99" s="122"/>
+      <c r="E99" s="123"/>
+      <c r="F99" s="124"/>
+      <c r="G99" s="125"/>
+      <c r="H99" s="126"/>
+    </row>
+    <row r="100" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+      <c r="B100" s="121"/>
+      <c r="C100" s="122"/>
+      <c r="D100" s="122"/>
+      <c r="E100" s="123"/>
+      <c r="F100" s="124"/>
+      <c r="G100" s="125"/>
+      <c r="H100" s="126"/>
+    </row>
+    <row r="101" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+      <c r="B101" s="121"/>
+      <c r="C101" s="122"/>
+      <c r="D101" s="122"/>
+      <c r="E101" s="123"/>
+      <c r="F101" s="124"/>
+      <c r="G101" s="125"/>
+      <c r="H101" s="126"/>
+    </row>
+    <row r="102" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="134"/>
+      <c r="C102" s="135"/>
+      <c r="D102" s="135"/>
+      <c r="E102" s="136"/>
+      <c r="F102" s="137"/>
+      <c r="G102" s="138"/>
+      <c r="H102" s="139"/>
+    </row>
+    <row r="103" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="140"/>
+      <c r="G103" s="141"/>
+      <c r="H103" s="141"/>
+    </row>
+    <row r="104" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+      <c r="D104" s="1"/>
+      <c r="E104" s="1"/>
+      <c r="F104" s="140"/>
+      <c r="G104" s="141"/>
+      <c r="H104" s="141"/>
+    </row>
+    <row r="105" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+      <c r="D105" s="1"/>
+      <c r="E105" s="1"/>
+      <c r="F105" s="140"/>
+      <c r="G105" s="141"/>
+      <c r="H105" s="141"/>
+    </row>
+    <row r="106" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="140"/>
+      <c r="G106" s="141"/>
+      <c r="H106" s="141"/>
+    </row>
+    <row r="107" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+      <c r="C107" s="1"/>
+      <c r="D107" s="1"/>
+      <c r="E107" s="1"/>
+      <c r="F107" s="140"/>
+      <c r="G107" s="141"/>
+      <c r="H107" s="141"/>
+    </row>
+    <row r="108" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A108" s="1"/>
+      <c r="B108" s="1"/>
+      <c r="C108" s="1"/>
+      <c r="D108" s="1"/>
+      <c r="E108" s="1"/>
+      <c r="F108" s="140"/>
+      <c r="G108" s="141"/>
+      <c r="H108" s="141"/>
+    </row>
+    <row r="109" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+      <c r="C109" s="1"/>
+      <c r="D109" s="1"/>
+      <c r="E109" s="1"/>
+      <c r="F109" s="140"/>
+      <c r="G109" s="141"/>
+      <c r="H109" s="141"/>
+    </row>
+    <row r="110" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A110" s="1"/>
+      <c r="B110" s="1"/>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="140"/>
+      <c r="G110" s="141"/>
+      <c r="H110" s="141"/>
+    </row>
+    <row r="111" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A111" s="1"/>
+      <c r="B111" s="1"/>
+      <c r="C111" s="1"/>
+      <c r="D111" s="1"/>
+      <c r="E111" s="1"/>
+      <c r="F111" s="140"/>
+      <c r="G111" s="141"/>
+      <c r="H111" s="141"/>
+    </row>
+    <row r="112" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A112" s="1"/>
+      <c r="B112" s="1"/>
+      <c r="C112" s="1"/>
+      <c r="D112" s="1"/>
+      <c r="E112" s="1"/>
+      <c r="F112" s="140"/>
+      <c r="G112" s="141"/>
+      <c r="H112" s="141"/>
+    </row>
+    <row r="113" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A113" s="1"/>
+      <c r="B113" s="1"/>
+      <c r="C113" s="1"/>
+      <c r="D113" s="1"/>
+      <c r="E113" s="1"/>
+      <c r="F113" s="140"/>
+      <c r="G113" s="141"/>
+      <c r="H113" s="141"/>
+    </row>
+    <row r="114" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
+      <c r="D114" s="1"/>
+      <c r="E114" s="1"/>
+      <c r="F114" s="140"/>
+      <c r="G114" s="141"/>
+      <c r="H114" s="141"/>
+    </row>
+    <row r="115" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A115" s="1"/>
+      <c r="B115" s="1"/>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="140"/>
+      <c r="G115" s="141"/>
+      <c r="H115" s="141"/>
+    </row>
+    <row r="116" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+      <c r="B116" s="1"/>
+      <c r="C116" s="1"/>
+      <c r="D116" s="1"/>
+      <c r="E116" s="1"/>
+      <c r="F116" s="140"/>
+      <c r="G116" s="141"/>
+      <c r="H116" s="141"/>
+    </row>
+    <row r="117" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A117" s="1"/>
+      <c r="B117" s="1"/>
+      <c r="C117" s="1"/>
+      <c r="D117" s="1"/>
+      <c r="E117" s="1"/>
+      <c r="F117" s="140"/>
+      <c r="G117" s="141"/>
+      <c r="H117" s="141"/>
+    </row>
+    <row r="118" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A118" s="1"/>
+      <c r="B118" s="1"/>
+      <c r="C118" s="1"/>
+      <c r="D118" s="1"/>
+      <c r="E118" s="1"/>
+      <c r="F118" s="140"/>
+      <c r="G118" s="141"/>
+      <c r="H118" s="141"/>
+    </row>
+    <row r="119" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F119" s="95"/>
+      <c r="G119" s="111"/>
+      <c r="H119" s="111"/>
+    </row>
+    <row r="120" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F120" s="95"/>
+      <c r="G120" s="111"/>
+      <c r="H120" s="111"/>
+    </row>
+    <row r="121" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F121" s="95"/>
+      <c r="G121" s="111"/>
+      <c r="H121" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3592,13 +4312,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K69"/>
+  <dimension ref="B1:K75"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3617,20 +4337,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="162" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="160"/>
-      <c r="D2" s="161"/>
-      <c r="E2" s="156" t="s">
+      <c r="C2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="158"/>
-      <c r="G2" s="156" t="s">
+      <c r="F2" s="161"/>
+      <c r="G2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="157"/>
-      <c r="I2" s="158"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="161"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -3651,10 +4371,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="162" t="s">
+      <c r="H3" s="165" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="163"/>
+      <c r="I3" s="166"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -3684,19 +4404,19 @@
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="61"/>
-      <c r="C5" s="147" t="s">
+      <c r="C5" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="150" t="s">
+      <c r="D5" s="170" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="153" t="s">
+      <c r="F5" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="144" t="s">
+      <c r="G5" s="176" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -3708,23 +4428,23 @@
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61"/>
-      <c r="C6" s="148"/>
-      <c r="D6" s="151"/>
+      <c r="C6" s="168"/>
+      <c r="D6" s="171"/>
       <c r="E6" s="35"/>
-      <c r="F6" s="154"/>
-      <c r="G6" s="145"/>
-      <c r="H6" s="139" t="s">
+      <c r="F6" s="174"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="140"/>
+      <c r="I6" s="158"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
-      <c r="C7" s="149"/>
-      <c r="D7" s="152"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="172"/>
       <c r="E7" s="36"/>
-      <c r="F7" s="155"/>
-      <c r="G7" s="146"/>
+      <c r="F7" s="175"/>
+      <c r="G7" s="178"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -3758,19 +4478,19 @@
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
-      <c r="C9" s="147" t="s">
+      <c r="C9" s="167" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="150" t="s">
+      <c r="D9" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="141" t="s">
+      <c r="E9" s="181" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="153" t="s">
+      <c r="F9" s="173" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="144" t="s">
+      <c r="G9" s="176" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -3783,24 +4503,24 @@
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
-      <c r="C10" s="148"/>
-      <c r="D10" s="151"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="154"/>
-      <c r="G10" s="145"/>
-      <c r="H10" s="139" t="s">
+      <c r="C10" s="168"/>
+      <c r="D10" s="171"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="174"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="140"/>
+      <c r="I10" s="158"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
-      <c r="C11" s="149"/>
-      <c r="D11" s="152"/>
-      <c r="E11" s="143"/>
-      <c r="F11" s="155"/>
-      <c r="G11" s="146"/>
+      <c r="C11" s="169"/>
+      <c r="D11" s="172"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="175"/>
+      <c r="G11" s="178"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -3810,10 +4530,10 @@
     </row>
     <row r="12" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="61"/>
-      <c r="C12" s="147" t="s">
+      <c r="C12" s="167" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="150" t="s">
+      <c r="D12" s="170" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="37" t="s">
@@ -3822,7 +4542,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="144" t="s">
+      <c r="G12" s="176" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -3834,15 +4554,15 @@
     </row>
     <row r="13" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="61"/>
-      <c r="C13" s="149"/>
-      <c r="D13" s="152"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="172"/>
       <c r="E13" s="37" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="146"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -3887,8 +4607,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="137"/>
-      <c r="I16" s="138"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="180"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -4302,19 +5022,19 @@
     </row>
     <row r="40" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="61"/>
-      <c r="C40" s="147" t="s">
+      <c r="C40" s="167" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="150" t="s">
+      <c r="D40" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="141" t="s">
+      <c r="E40" s="181" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="153" t="s">
+      <c r="F40" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="144" t="s">
+      <c r="G40" s="176" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -4326,23 +5046,23 @@
     </row>
     <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="61"/>
-      <c r="C41" s="148"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="142"/>
-      <c r="F41" s="154"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="139" t="s">
+      <c r="C41" s="168"/>
+      <c r="D41" s="171"/>
+      <c r="E41" s="182"/>
+      <c r="F41" s="174"/>
+      <c r="G41" s="177"/>
+      <c r="H41" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="140"/>
+      <c r="I41" s="158"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
-      <c r="C42" s="149"/>
-      <c r="D42" s="152"/>
-      <c r="E42" s="143"/>
-      <c r="F42" s="155"/>
-      <c r="G42" s="146"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="172"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="175"/>
+      <c r="G42" s="178"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -4376,19 +5096,19 @@
     </row>
     <row r="44" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="61"/>
-      <c r="C44" s="147" t="s">
+      <c r="C44" s="167" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="150" t="s">
+      <c r="D44" s="170" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="141" t="s">
+      <c r="E44" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="153" t="s">
+      <c r="F44" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="144" t="s">
+      <c r="G44" s="176" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -4400,23 +5120,23 @@
     </row>
     <row r="45" spans="2:9" s="5" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="61"/>
-      <c r="C45" s="148"/>
-      <c r="D45" s="151"/>
-      <c r="E45" s="142"/>
-      <c r="F45" s="154"/>
-      <c r="G45" s="145"/>
-      <c r="H45" s="139" t="s">
+      <c r="C45" s="168"/>
+      <c r="D45" s="171"/>
+      <c r="E45" s="182"/>
+      <c r="F45" s="174"/>
+      <c r="G45" s="177"/>
+      <c r="H45" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="140"/>
+      <c r="I45" s="158"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
-      <c r="C46" s="149"/>
-      <c r="D46" s="152"/>
-      <c r="E46" s="143"/>
-      <c r="F46" s="155"/>
-      <c r="G46" s="146"/>
+      <c r="C46" s="169"/>
+      <c r="D46" s="172"/>
+      <c r="E46" s="183"/>
+      <c r="F46" s="175"/>
+      <c r="G46" s="178"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -4441,8 +5161,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="137"/>
-      <c r="I48" s="138"/>
+      <c r="H48" s="179"/>
+      <c r="I48" s="180"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -4505,10 +5225,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="139" t="s">
+      <c r="H52" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="140"/>
+      <c r="I52" s="158"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -4541,74 +5261,100 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="137"/>
-      <c r="I55" s="138"/>
+      <c r="H55" s="179"/>
+      <c r="I55" s="180"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="61"/>
-      <c r="C56" s="69"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="19"/>
-    </row>
-    <row r="57" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="61"/>
-      <c r="C57" s="69"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="19"/>
-    </row>
-    <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="61"/>
-      <c r="C58" s="69"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="39"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="19"/>
+      <c r="B56" s="61" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="145" t="s">
+        <v>309</v>
+      </c>
+      <c r="D56" s="147" t="s">
+        <v>310</v>
+      </c>
+      <c r="E56" s="45"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="48"/>
+      <c r="I56" s="49"/>
+    </row>
+    <row r="57" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B57" s="64"/>
+      <c r="C57" s="145" t="s">
+        <v>311</v>
+      </c>
+      <c r="D57" s="147" t="s">
+        <v>313</v>
+      </c>
+      <c r="E57" s="42" t="s">
+        <v>319</v>
+      </c>
+      <c r="F57" s="149" t="s">
+        <v>320</v>
+      </c>
+      <c r="G57" s="143"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="64"/>
+      <c r="C58" s="145" t="s">
+        <v>312</v>
+      </c>
+      <c r="D58" s="147" t="s">
+        <v>314</v>
+      </c>
+      <c r="E58" s="42"/>
+      <c r="F58" s="149"/>
+      <c r="G58" s="143"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="17"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="61"/>
-      <c r="C59" s="69"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="39"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="19"/>
+      <c r="B59" s="64"/>
+      <c r="C59" s="145" t="s">
+        <v>315</v>
+      </c>
+      <c r="D59" s="147" t="s">
+        <v>316</v>
+      </c>
+      <c r="E59" s="42" t="s">
+        <v>317</v>
+      </c>
+      <c r="F59" s="149" t="s">
+        <v>318</v>
+      </c>
+      <c r="G59" s="143"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="17"/>
     </row>
     <row r="60" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="61"/>
-      <c r="C60" s="69"/>
-      <c r="D60" s="14"/>
+      <c r="B60" s="64"/>
+      <c r="C60" s="144"/>
+      <c r="D60" s="146"/>
       <c r="E60" s="39"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="32"/>
+      <c r="F60" s="148"/>
+      <c r="G60" s="142"/>
       <c r="H60" s="9"/>
       <c r="I60" s="19"/>
     </row>
-    <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="61"/>
-      <c r="C61" s="69"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="39"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="19"/>
+    <row r="61" spans="2:9" s="5" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="65"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="25"/>
+      <c r="F61" s="22"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="179"/>
+      <c r="I61" s="180"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
       <c r="C62" s="69"/>
       <c r="D62" s="14"/>
-      <c r="E62" s="35"/>
+      <c r="E62" s="39"/>
       <c r="F62" s="12"/>
       <c r="G62" s="32"/>
       <c r="H62" s="9"/>
@@ -4618,7 +5364,7 @@
       <c r="B63" s="61"/>
       <c r="C63" s="69"/>
       <c r="D63" s="14"/>
-      <c r="E63" s="35"/>
+      <c r="E63" s="39"/>
       <c r="F63" s="12"/>
       <c r="G63" s="32"/>
       <c r="H63" s="9"/>
@@ -4628,7 +5374,7 @@
       <c r="B64" s="61"/>
       <c r="C64" s="69"/>
       <c r="D64" s="14"/>
-      <c r="E64" s="35"/>
+      <c r="E64" s="39"/>
       <c r="F64" s="12"/>
       <c r="G64" s="32"/>
       <c r="H64" s="9"/>
@@ -4638,7 +5384,7 @@
       <c r="B65" s="61"/>
       <c r="C65" s="69"/>
       <c r="D65" s="14"/>
-      <c r="E65" s="35"/>
+      <c r="E65" s="39"/>
       <c r="F65" s="12"/>
       <c r="G65" s="32"/>
       <c r="H65" s="9"/>
@@ -4648,7 +5394,7 @@
       <c r="B66" s="61"/>
       <c r="C66" s="69"/>
       <c r="D66" s="14"/>
-      <c r="E66" s="35"/>
+      <c r="E66" s="39"/>
       <c r="F66" s="12"/>
       <c r="G66" s="32"/>
       <c r="H66" s="9"/>
@@ -4658,7 +5404,7 @@
       <c r="B67" s="61"/>
       <c r="C67" s="69"/>
       <c r="D67" s="14"/>
-      <c r="E67" s="35"/>
+      <c r="E67" s="39"/>
       <c r="F67" s="12"/>
       <c r="G67" s="32"/>
       <c r="H67" s="9"/>
@@ -4674,27 +5420,94 @@
       <c r="H68" s="9"/>
       <c r="I68" s="19"/>
     </row>
-    <row r="69" spans="2:9" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="70"/>
-      <c r="C69" s="71"/>
-      <c r="D69" s="15"/>
-      <c r="E69" s="40"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="33"/>
-      <c r="H69" s="20"/>
-      <c r="I69" s="21"/>
+    <row r="69" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="61"/>
+      <c r="C69" s="69"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="9"/>
+      <c r="I69" s="19"/>
+    </row>
+    <row r="70" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="61"/>
+      <c r="C70" s="69"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="19"/>
+    </row>
+    <row r="71" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="61"/>
+      <c r="C71" s="69"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="35"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="19"/>
+    </row>
+    <row r="72" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="61"/>
+      <c r="C72" s="69"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="9"/>
+      <c r="I72" s="19"/>
+    </row>
+    <row r="73" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="61"/>
+      <c r="C73" s="69"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="9"/>
+      <c r="I73" s="19"/>
+    </row>
+    <row r="74" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="61"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="35"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="32"/>
+      <c r="H74" s="9"/>
+      <c r="I74" s="19"/>
+    </row>
+    <row r="75" spans="2:9" s="5" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="70"/>
+      <c r="C75" s="71"/>
+      <c r="D75" s="15"/>
+      <c r="E75" s="40"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="33"/>
+      <c r="H75" s="20"/>
+      <c r="I75" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+  <mergeCells count="35">
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -4705,21 +5518,15 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4748,14 +5555,14 @@
   <sheetData>
     <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="184" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="165"/>
-      <c r="D2" s="157" t="s">
+      <c r="C2" s="185"/>
+      <c r="D2" s="160" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="158" t="s">
+      <c r="E2" s="161" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4766,8 +5573,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="162"/>
-      <c r="E3" s="163"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="166"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">
@@ -5229,7 +6036,7 @@
       <c r="B2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="166" t="s">
+      <c r="C2" s="186" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5237,7 +6044,7 @@
       <c r="B3" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="167"/>
+      <c r="C3" s="187"/>
     </row>
     <row r="4" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="89" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 24 Januari 2023 18:33 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="342">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1056,7 +1056,13 @@
     <t>Sudah bener</t>
   </si>
   <si>
-    <t>doble cross</t>
+    <t xml:space="preserve">   Workflow berdasarkan ID WorkFlowVersion (varWorkFlowVersion_RefID)</t>
+  </si>
+  <si>
+    <t>mendapatkan Path Approval versi COMPACT dari  Workflow berdasarkan ID WorkFlowVersion (varWorkFlowVersion_RefID)</t>
+  </si>
+  <si>
+    <t>Func_General_GetWorkFlowPath_COMPACT</t>
   </si>
 </sst>
 </file>
@@ -2209,12 +2215,63 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2238,57 +2295,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2613,13 +2619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J121"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3525,39 +3531,39 @@
       <c r="B49" s="121"/>
       <c r="C49" s="122"/>
       <c r="D49" s="122" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="E49" s="127" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F49" s="124" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G49" s="125">
-        <v>44900</v>
+        <v>44950</v>
       </c>
       <c r="H49" s="126">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44950</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="121"/>
       <c r="C50" s="122"/>
       <c r="D50" s="122" t="s">
-        <v>329</v>
-      </c>
-      <c r="E50" s="123" t="s">
-        <v>330</v>
+        <v>341</v>
+      </c>
+      <c r="E50" s="127" t="s">
+        <v>340</v>
       </c>
       <c r="F50" s="124" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G50" s="125">
-        <v>44896</v>
+        <v>44950</v>
       </c>
       <c r="H50" s="126">
-        <v>44896</v>
+        <v>44950</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3565,83 +3571,103 @@
       <c r="B51" s="121"/>
       <c r="C51" s="122"/>
       <c r="D51" s="122" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E51" s="127" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F51" s="124" t="s">
         <v>281</v>
       </c>
       <c r="G51" s="125">
-        <v>44945</v>
+        <v>44900</v>
       </c>
       <c r="H51" s="126">
         <v>44949</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="121"/>
       <c r="C52" s="122"/>
       <c r="D52" s="122" t="s">
-        <v>336</v>
-      </c>
-      <c r="E52" s="127" t="s">
-        <v>337</v>
+        <v>329</v>
+      </c>
+      <c r="E52" s="123" t="s">
+        <v>330</v>
       </c>
       <c r="F52" s="124" t="s">
         <v>281</v>
       </c>
       <c r="G52" s="125">
-        <v>44910</v>
+        <v>44896</v>
       </c>
       <c r="H52" s="126">
-        <v>44910</v>
-      </c>
-      <c r="J52" s="78" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="121"/>
       <c r="C53" s="122"/>
       <c r="D53" s="122" t="s">
-        <v>331</v>
-      </c>
-      <c r="E53" s="123" t="s">
-        <v>332</v>
+        <v>322</v>
+      </c>
+      <c r="E53" s="127" t="s">
+        <v>323</v>
       </c>
       <c r="F53" s="124" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G53" s="125">
-        <v>44893</v>
+        <v>44945</v>
       </c>
       <c r="H53" s="126">
-        <v>44893</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="121"/>
       <c r="C54" s="122"/>
-      <c r="D54" s="122"/>
-      <c r="E54" s="123"/>
-      <c r="F54" s="124"/>
-      <c r="G54" s="125"/>
-      <c r="H54" s="126"/>
+      <c r="D54" s="122" t="s">
+        <v>336</v>
+      </c>
+      <c r="E54" s="127" t="s">
+        <v>337</v>
+      </c>
+      <c r="F54" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G54" s="125">
+        <v>44910</v>
+      </c>
+      <c r="H54" s="126">
+        <v>44910</v>
+      </c>
+      <c r="J54" s="78" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="55" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="121"/>
       <c r="C55" s="122"/>
-      <c r="D55" s="122"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="124"/>
-      <c r="G55" s="125"/>
-      <c r="H55" s="126"/>
+      <c r="D55" s="122" t="s">
+        <v>331</v>
+      </c>
+      <c r="E55" s="123" t="s">
+        <v>332</v>
+      </c>
+      <c r="F55" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G55" s="125">
+        <v>44893</v>
+      </c>
+      <c r="H55" s="126">
+        <v>44893</v>
+      </c>
     </row>
     <row r="56" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
@@ -3663,27 +3689,15 @@
       <c r="G57" s="125"/>
       <c r="H57" s="126"/>
     </row>
-    <row r="58" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="121"/>
-      <c r="C58" s="122" t="s">
-        <v>339</v>
-      </c>
-      <c r="D58" s="122" t="s">
-        <v>324</v>
-      </c>
-      <c r="E58" s="127" t="s">
-        <v>325</v>
-      </c>
-      <c r="F58" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G58" s="125">
-        <v>44900</v>
-      </c>
-      <c r="H58" s="126">
-        <v>44900</v>
-      </c>
+      <c r="C58" s="122"/>
+      <c r="D58" s="122"/>
+      <c r="E58" s="123"/>
+      <c r="F58" s="124"/>
+      <c r="G58" s="125"/>
+      <c r="H58" s="126"/>
     </row>
     <row r="59" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
@@ -3714,6 +3728,9 @@
       <c r="F61" s="124"/>
       <c r="G61" s="125"/>
       <c r="H61" s="126"/>
+      <c r="J61" s="78" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="62" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
@@ -4105,25 +4122,25 @@
       <c r="G100" s="125"/>
       <c r="H100" s="126"/>
     </row>
-    <row r="101" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
-      <c r="B101" s="121"/>
-      <c r="C101" s="122"/>
-      <c r="D101" s="122"/>
-      <c r="E101" s="123"/>
-      <c r="F101" s="124"/>
-      <c r="G101" s="125"/>
-      <c r="H101" s="126"/>
-    </row>
-    <row r="102" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="134"/>
+      <c r="C101" s="135"/>
+      <c r="D101" s="135"/>
+      <c r="E101" s="136"/>
+      <c r="F101" s="137"/>
+      <c r="G101" s="138"/>
+      <c r="H101" s="139"/>
+    </row>
+    <row r="102" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
-      <c r="B102" s="134"/>
-      <c r="C102" s="135"/>
-      <c r="D102" s="135"/>
-      <c r="E102" s="136"/>
-      <c r="F102" s="137"/>
-      <c r="G102" s="138"/>
-      <c r="H102" s="139"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="140"/>
+      <c r="G102" s="141"/>
+      <c r="H102" s="141"/>
     </row>
     <row r="103" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
@@ -4276,14 +4293,9 @@
       <c r="H117" s="141"/>
     </row>
     <row r="118" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="140"/>
-      <c r="G118" s="141"/>
-      <c r="H118" s="141"/>
+      <c r="F118" s="95"/>
+      <c r="G118" s="111"/>
+      <c r="H118" s="111"/>
     </row>
     <row r="119" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F119" s="95"/>
@@ -4294,11 +4306,6 @@
       <c r="F120" s="95"/>
       <c r="G120" s="111"/>
       <c r="H120" s="111"/>
-    </row>
-    <row r="121" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F121" s="95"/>
-      <c r="G121" s="111"/>
-      <c r="H121" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4337,20 +4344,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="179" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="159" t="s">
+      <c r="C2" s="180"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="176" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="161"/>
-      <c r="G2" s="159" t="s">
+      <c r="F2" s="178"/>
+      <c r="G2" s="176" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="160"/>
-      <c r="I2" s="161"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="178"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -4371,10 +4378,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="165" t="s">
+      <c r="H3" s="182" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="166"/>
+      <c r="I3" s="183"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -4416,7 +4423,7 @@
       <c r="F5" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="176" t="s">
+      <c r="G5" s="164" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -4432,11 +4439,11 @@
       <c r="D6" s="171"/>
       <c r="E6" s="35"/>
       <c r="F6" s="174"/>
-      <c r="G6" s="177"/>
-      <c r="H6" s="157" t="s">
+      <c r="G6" s="165"/>
+      <c r="H6" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="158"/>
+      <c r="I6" s="160"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
@@ -4444,7 +4451,7 @@
       <c r="D7" s="172"/>
       <c r="E7" s="36"/>
       <c r="F7" s="175"/>
-      <c r="G7" s="178"/>
+      <c r="G7" s="166"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -4484,13 +4491,13 @@
       <c r="D9" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="181" t="s">
+      <c r="E9" s="161" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="173" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="176" t="s">
+      <c r="G9" s="164" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -4505,22 +4512,22 @@
       <c r="B10" s="61"/>
       <c r="C10" s="168"/>
       <c r="D10" s="171"/>
-      <c r="E10" s="182"/>
+      <c r="E10" s="162"/>
       <c r="F10" s="174"/>
-      <c r="G10" s="177"/>
-      <c r="H10" s="157" t="s">
+      <c r="G10" s="165"/>
+      <c r="H10" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="158"/>
+      <c r="I10" s="160"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
       <c r="C11" s="169"/>
       <c r="D11" s="172"/>
-      <c r="E11" s="183"/>
+      <c r="E11" s="163"/>
       <c r="F11" s="175"/>
-      <c r="G11" s="178"/>
+      <c r="G11" s="166"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4542,7 +4549,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="176" t="s">
+      <c r="G12" s="164" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -4562,7 +4569,7 @@
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="178"/>
+      <c r="G13" s="166"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -4607,8 +4614,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="179"/>
-      <c r="I16" s="180"/>
+      <c r="H16" s="157"/>
+      <c r="I16" s="158"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -5028,13 +5035,13 @@
       <c r="D40" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="181" t="s">
+      <c r="E40" s="161" t="s">
         <v>45</v>
       </c>
       <c r="F40" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="176" t="s">
+      <c r="G40" s="164" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -5048,21 +5055,21 @@
       <c r="B41" s="61"/>
       <c r="C41" s="168"/>
       <c r="D41" s="171"/>
-      <c r="E41" s="182"/>
+      <c r="E41" s="162"/>
       <c r="F41" s="174"/>
-      <c r="G41" s="177"/>
-      <c r="H41" s="157" t="s">
+      <c r="G41" s="165"/>
+      <c r="H41" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="158"/>
+      <c r="I41" s="160"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
       <c r="C42" s="169"/>
       <c r="D42" s="172"/>
-      <c r="E42" s="183"/>
+      <c r="E42" s="163"/>
       <c r="F42" s="175"/>
-      <c r="G42" s="178"/>
+      <c r="G42" s="166"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -5102,13 +5109,13 @@
       <c r="D44" s="170" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="181" t="s">
+      <c r="E44" s="161" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="176" t="s">
+      <c r="G44" s="164" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -5122,21 +5129,21 @@
       <c r="B45" s="61"/>
       <c r="C45" s="168"/>
       <c r="D45" s="171"/>
-      <c r="E45" s="182"/>
+      <c r="E45" s="162"/>
       <c r="F45" s="174"/>
-      <c r="G45" s="177"/>
-      <c r="H45" s="157" t="s">
+      <c r="G45" s="165"/>
+      <c r="H45" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="158"/>
+      <c r="I45" s="160"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
       <c r="C46" s="169"/>
       <c r="D46" s="172"/>
-      <c r="E46" s="183"/>
+      <c r="E46" s="163"/>
       <c r="F46" s="175"/>
-      <c r="G46" s="178"/>
+      <c r="G46" s="166"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -5161,8 +5168,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="179"/>
-      <c r="I48" s="180"/>
+      <c r="H48" s="157"/>
+      <c r="I48" s="158"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -5225,10 +5232,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="157" t="s">
+      <c r="H52" s="159" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="158"/>
+      <c r="I52" s="160"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -5261,8 +5268,8 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="179"/>
-      <c r="I55" s="180"/>
+      <c r="H55" s="157"/>
+      <c r="I55" s="158"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="61" t="s">
@@ -5347,8 +5354,8 @@
       <c r="E61" s="25"/>
       <c r="F61" s="22"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="179"/>
-      <c r="I61" s="180"/>
+      <c r="H61" s="157"/>
+      <c r="I61" s="158"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -5492,22 +5499,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -5518,15 +5518,22 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H55:I55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5559,10 +5566,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="185"/>
-      <c r="D2" s="160" t="s">
+      <c r="D2" s="177" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="161" t="s">
+      <c r="E2" s="178" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5573,8 +5580,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="165"/>
-      <c r="E3" s="166"/>
+      <c r="D3" s="182"/>
+      <c r="E3" s="183"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 25 Januari 2023 11:01 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -1008,9 +1008,6 @@
     <t>Func_General_SetWorkFlowGraphExportToPath</t>
   </si>
   <si>
-    <t>Mengkespor Work Flow Graph menjadi Work Flow Path berdasarkan Work Flow Version (varWorkFlowVersion_RefID) pada Table SchSysConfig.TblAppObject_WorkFlowPath</t>
-  </si>
-  <si>
     <t>Func_General_GetWorkFlowPath</t>
   </si>
   <si>
@@ -1063,6 +1060,9 @@
   </si>
   <si>
     <t>Func_General_GetWorkFlowPath_COMPACT</t>
+  </si>
+  <si>
+    <t>Mengekspor Work Flow Graph menjadi Work Flow Path berdasarkan Work Flow Version (varWorkFlowVersion_RefID) pada Table SchSysConfig.TblAppObject_WorkFlowPath</t>
   </si>
 </sst>
 </file>
@@ -2625,7 +2625,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E51" sqref="E51"/>
+      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3488,13 +3488,13 @@
       <c r="A47" s="1"/>
       <c r="B47" s="121"/>
       <c r="C47" s="122" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D47" s="122" t="s">
+        <v>326</v>
+      </c>
+      <c r="E47" s="127" t="s">
         <v>327</v>
-      </c>
-      <c r="E47" s="127" t="s">
-        <v>328</v>
       </c>
       <c r="F47" s="124" t="s">
         <v>232</v>
@@ -3511,10 +3511,10 @@
       <c r="B48" s="121"/>
       <c r="C48" s="122"/>
       <c r="D48" s="122" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E48" s="127" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F48" s="124" t="s">
         <v>232</v>
@@ -3531,10 +3531,10 @@
       <c r="B49" s="121"/>
       <c r="C49" s="122"/>
       <c r="D49" s="122" t="s">
+        <v>323</v>
+      </c>
+      <c r="E49" s="127" t="s">
         <v>324</v>
-      </c>
-      <c r="E49" s="127" t="s">
-        <v>325</v>
       </c>
       <c r="F49" s="124" t="s">
         <v>232</v>
@@ -3551,10 +3551,10 @@
       <c r="B50" s="121"/>
       <c r="C50" s="122"/>
       <c r="D50" s="122" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E50" s="127" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F50" s="124" t="s">
         <v>232</v>
@@ -3574,7 +3574,7 @@
         <v>321</v>
       </c>
       <c r="E51" s="127" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F51" s="124" t="s">
         <v>281</v>
@@ -3591,10 +3591,10 @@
       <c r="B52" s="121"/>
       <c r="C52" s="122"/>
       <c r="D52" s="122" t="s">
+        <v>328</v>
+      </c>
+      <c r="E52" s="123" t="s">
         <v>329</v>
-      </c>
-      <c r="E52" s="123" t="s">
-        <v>330</v>
       </c>
       <c r="F52" s="124" t="s">
         <v>281</v>
@@ -3614,7 +3614,7 @@
         <v>322</v>
       </c>
       <c r="E53" s="127" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="F53" s="124" t="s">
         <v>281</v>
@@ -3631,10 +3631,10 @@
       <c r="B54" s="121"/>
       <c r="C54" s="122"/>
       <c r="D54" s="122" t="s">
+        <v>335</v>
+      </c>
+      <c r="E54" s="127" t="s">
         <v>336</v>
-      </c>
-      <c r="E54" s="127" t="s">
-        <v>337</v>
       </c>
       <c r="F54" s="124" t="s">
         <v>281</v>
@@ -3646,7 +3646,7 @@
         <v>44910</v>
       </c>
       <c r="J54" s="78" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="55" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -3654,10 +3654,10 @@
       <c r="B55" s="121"/>
       <c r="C55" s="122"/>
       <c r="D55" s="122" t="s">
+        <v>330</v>
+      </c>
+      <c r="E55" s="123" t="s">
         <v>331</v>
-      </c>
-      <c r="E55" s="123" t="s">
-        <v>332</v>
       </c>
       <c r="F55" s="124" t="s">
         <v>232</v>
@@ -3729,7 +3729,7 @@
       <c r="G61" s="125"/>
       <c r="H61" s="126"/>
       <c r="J61" s="78" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="62" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Pertanggal 26 Januari 2023 09:43 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="346">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1063,6 +1063,18 @@
   </si>
   <si>
     <t>Mengekspor Work Flow Graph menjadi Work Flow Path berdasarkan Work Flow Version (varWorkFlowVersion_RefID) pada Table SchSysConfig.TblAppObject_WorkFlowPath</t>
+  </si>
+  <si>
+    <t>Func_GetDataList_AppObject_WorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data List Work Flow Path berdasarkan ID Branch (varBranch_RefID) dan ID Work Flow Version (varWorkFlowVersion_RefID)</t>
+  </si>
+  <si>
+    <t>Func_GetDataPickList_AppObject_WorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Pick List Work Flow Path berdasarkan ID Branch (varBranch_RefID) dan ID Work Flow Version (varWorkFlowVersion_RefID)</t>
   </si>
 </sst>
 </file>
@@ -2215,18 +2227,78 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2235,66 +2307,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2622,10 +2634,10 @@
   <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E54" sqref="E54"/>
+      <selection pane="bottomRight" activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3540,10 +3552,10 @@
         <v>232</v>
       </c>
       <c r="G49" s="125">
-        <v>44950</v>
+        <v>44951</v>
       </c>
       <c r="H49" s="126">
-        <v>44950</v>
+        <v>44951</v>
       </c>
     </row>
     <row r="50" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3560,10 +3572,10 @@
         <v>232</v>
       </c>
       <c r="G50" s="125">
-        <v>44950</v>
+        <v>44951</v>
       </c>
       <c r="H50" s="126">
-        <v>44950</v>
+        <v>44951</v>
       </c>
     </row>
     <row r="51" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3649,45 +3661,65 @@
         <v>333</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="121"/>
       <c r="C55" s="122"/>
       <c r="D55" s="122" t="s">
-        <v>330</v>
-      </c>
-      <c r="E55" s="123" t="s">
-        <v>331</v>
+        <v>342</v>
+      </c>
+      <c r="E55" s="127" t="s">
+        <v>343</v>
       </c>
       <c r="F55" s="124" t="s">
         <v>232</v>
       </c>
       <c r="G55" s="125">
-        <v>44893</v>
+        <v>44951</v>
       </c>
       <c r="H55" s="126">
-        <v>44893</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="121"/>
       <c r="C56" s="122"/>
-      <c r="D56" s="122"/>
-      <c r="E56" s="123"/>
-      <c r="F56" s="124"/>
-      <c r="G56" s="125"/>
-      <c r="H56" s="126"/>
+      <c r="D56" s="122" t="s">
+        <v>344</v>
+      </c>
+      <c r="E56" s="127" t="s">
+        <v>345</v>
+      </c>
+      <c r="F56" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G56" s="125">
+        <v>44952</v>
+      </c>
+      <c r="H56" s="126">
+        <v>44952</v>
+      </c>
     </row>
     <row r="57" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="121"/>
       <c r="C57" s="122"/>
-      <c r="D57" s="122"/>
-      <c r="E57" s="123"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="125"/>
-      <c r="H57" s="126"/>
+      <c r="D57" s="122" t="s">
+        <v>330</v>
+      </c>
+      <c r="E57" s="123" t="s">
+        <v>331</v>
+      </c>
+      <c r="F57" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G57" s="125">
+        <v>44893</v>
+      </c>
+      <c r="H57" s="126">
+        <v>44893</v>
+      </c>
     </row>
     <row r="58" spans="1:10" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
@@ -4344,20 +4376,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="179" t="s">
+      <c r="B2" s="162" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="180"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="176" t="s">
+      <c r="C2" s="163"/>
+      <c r="D2" s="164"/>
+      <c r="E2" s="159" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="178"/>
-      <c r="G2" s="176" t="s">
+      <c r="F2" s="161"/>
+      <c r="G2" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="177"/>
-      <c r="I2" s="178"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="161"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -4378,10 +4410,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="182" t="s">
+      <c r="H3" s="165" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="183"/>
+      <c r="I3" s="166"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -4423,7 +4455,7 @@
       <c r="F5" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="164" t="s">
+      <c r="G5" s="176" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -4439,11 +4471,11 @@
       <c r="D6" s="171"/>
       <c r="E6" s="35"/>
       <c r="F6" s="174"/>
-      <c r="G6" s="165"/>
-      <c r="H6" s="159" t="s">
+      <c r="G6" s="177"/>
+      <c r="H6" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="160"/>
+      <c r="I6" s="158"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
@@ -4451,7 +4483,7 @@
       <c r="D7" s="172"/>
       <c r="E7" s="36"/>
       <c r="F7" s="175"/>
-      <c r="G7" s="166"/>
+      <c r="G7" s="178"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -4491,13 +4523,13 @@
       <c r="D9" s="170" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="161" t="s">
+      <c r="E9" s="181" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="173" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="164" t="s">
+      <c r="G9" s="176" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -4512,22 +4544,22 @@
       <c r="B10" s="61"/>
       <c r="C10" s="168"/>
       <c r="D10" s="171"/>
-      <c r="E10" s="162"/>
+      <c r="E10" s="182"/>
       <c r="F10" s="174"/>
-      <c r="G10" s="165"/>
-      <c r="H10" s="159" t="s">
+      <c r="G10" s="177"/>
+      <c r="H10" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="160"/>
+      <c r="I10" s="158"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
       <c r="C11" s="169"/>
       <c r="D11" s="172"/>
-      <c r="E11" s="163"/>
+      <c r="E11" s="183"/>
       <c r="F11" s="175"/>
-      <c r="G11" s="166"/>
+      <c r="G11" s="178"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -4549,7 +4581,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="164" t="s">
+      <c r="G12" s="176" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -4569,7 +4601,7 @@
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="166"/>
+      <c r="G13" s="178"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -4614,8 +4646,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="157"/>
-      <c r="I16" s="158"/>
+      <c r="H16" s="179"/>
+      <c r="I16" s="180"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -5035,13 +5067,13 @@
       <c r="D40" s="170" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="161" t="s">
+      <c r="E40" s="181" t="s">
         <v>45</v>
       </c>
       <c r="F40" s="173" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="164" t="s">
+      <c r="G40" s="176" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -5055,21 +5087,21 @@
       <c r="B41" s="61"/>
       <c r="C41" s="168"/>
       <c r="D41" s="171"/>
-      <c r="E41" s="162"/>
+      <c r="E41" s="182"/>
       <c r="F41" s="174"/>
-      <c r="G41" s="165"/>
-      <c r="H41" s="159" t="s">
+      <c r="G41" s="177"/>
+      <c r="H41" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="160"/>
+      <c r="I41" s="158"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
       <c r="C42" s="169"/>
       <c r="D42" s="172"/>
-      <c r="E42" s="163"/>
+      <c r="E42" s="183"/>
       <c r="F42" s="175"/>
-      <c r="G42" s="166"/>
+      <c r="G42" s="178"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -5109,13 +5141,13 @@
       <c r="D44" s="170" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="161" t="s">
+      <c r="E44" s="181" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="173" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="164" t="s">
+      <c r="G44" s="176" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -5129,21 +5161,21 @@
       <c r="B45" s="61"/>
       <c r="C45" s="168"/>
       <c r="D45" s="171"/>
-      <c r="E45" s="162"/>
+      <c r="E45" s="182"/>
       <c r="F45" s="174"/>
-      <c r="G45" s="165"/>
-      <c r="H45" s="159" t="s">
+      <c r="G45" s="177"/>
+      <c r="H45" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="160"/>
+      <c r="I45" s="158"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
       <c r="C46" s="169"/>
       <c r="D46" s="172"/>
-      <c r="E46" s="163"/>
+      <c r="E46" s="183"/>
       <c r="F46" s="175"/>
-      <c r="G46" s="166"/>
+      <c r="G46" s="178"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -5168,8 +5200,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="157"/>
-      <c r="I48" s="158"/>
+      <c r="H48" s="179"/>
+      <c r="I48" s="180"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -5232,10 +5264,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="159" t="s">
+      <c r="H52" s="157" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="160"/>
+      <c r="I52" s="158"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -5268,8 +5300,8 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="157"/>
-      <c r="I55" s="158"/>
+      <c r="H55" s="179"/>
+      <c r="I55" s="180"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="61" t="s">
@@ -5354,8 +5386,8 @@
       <c r="E61" s="25"/>
       <c r="F61" s="22"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="157"/>
-      <c r="I61" s="158"/>
+      <c r="H61" s="179"/>
+      <c r="I61" s="180"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -5499,15 +5531,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -5518,22 +5557,15 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5566,10 +5598,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="185"/>
-      <c r="D2" s="177" t="s">
+      <c r="D2" s="160" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="178" t="s">
+      <c r="E2" s="161" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5580,8 +5612,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="182"/>
-      <c r="E3" s="183"/>
+      <c r="D3" s="165"/>
+      <c r="E3" s="166"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 1 Februari 2023 10:12 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="415">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1240,6 +1240,48 @@
   </si>
   <si>
     <t>Mengupdate satu atau beberapa field yang didefiniskan pada Array Data (varData) pada Record Table yang diidentifikasi melalui Record ID (varID)</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllIndexName</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllLDAPUserToPerson</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama Index yang terdapat didalam sistem berdasarkan Nama Skema (varSchemaName) dan Nama Tabel (varTableName)</t>
+  </si>
+  <si>
+    <t>Menampilkan pemetaan RPK, ID, dan Name dari LDAP User ke Person</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllPartitionTablesName</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama Table Berpartisi yang terdapat didalam sistem berdasarkan Nama Skema (varSchemaName) dan Nama Tabel (varTableName)</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllSchemasName</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama Schema yang terdapat didalam sistem</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllTablesName</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama Table yang terdapat didalam sistem berdasarkan Nama Skema (varSchemaName)</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetAllUsersName</t>
+  </si>
+  <si>
+    <t>Menampilkan seluruh nama User yang terdapat didalam sistem</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetBranchGroupFilter</t>
+  </si>
+  <si>
+    <t>Menampilkan ID Institution Branch satu Group yang difilter berdasarkan ID Institution Branch (varBranchID)</t>
   </si>
 </sst>
 </file>
@@ -2832,13 +2874,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H124"/>
+  <dimension ref="A1:H136"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E70" sqref="E70"/>
+      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3617,294 +3659,262 @@
         <v>44216</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="121"/>
       <c r="C40" s="122"/>
-      <c r="D40" s="122"/>
-      <c r="E40" s="123"/>
-      <c r="F40" s="124"/>
-      <c r="G40" s="125"/>
-      <c r="H40" s="126"/>
+      <c r="D40" s="122" t="s">
+        <v>401</v>
+      </c>
+      <c r="E40" s="127" t="s">
+        <v>403</v>
+      </c>
+      <c r="F40" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G40" s="125">
+        <v>43720</v>
+      </c>
+      <c r="H40" s="126">
+        <v>43720</v>
+      </c>
     </row>
     <row r="41" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="121"/>
       <c r="C41" s="122"/>
       <c r="D41" s="122" t="s">
-        <v>286</v>
-      </c>
-      <c r="E41" s="123" t="s">
-        <v>287</v>
+        <v>402</v>
+      </c>
+      <c r="E41" s="127" t="s">
+        <v>404</v>
       </c>
       <c r="F41" s="124" t="s">
         <v>232</v>
       </c>
       <c r="G41" s="125">
-        <v>44949</v>
+        <v>43785</v>
       </c>
       <c r="H41" s="126">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="121"/>
       <c r="C42" s="122"/>
-      <c r="D42" s="122"/>
-      <c r="E42" s="123"/>
-      <c r="F42" s="124"/>
-      <c r="G42" s="125"/>
-      <c r="H42" s="126"/>
+      <c r="D42" s="122" t="s">
+        <v>405</v>
+      </c>
+      <c r="E42" s="127" t="s">
+        <v>406</v>
+      </c>
+      <c r="F42" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G42" s="125">
+        <v>43208</v>
+      </c>
+      <c r="H42" s="126">
+        <v>43208</v>
+      </c>
     </row>
     <row r="43" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="121"/>
       <c r="C43" s="122"/>
-      <c r="D43" s="122"/>
-      <c r="E43" s="123"/>
-      <c r="F43" s="124"/>
-      <c r="G43" s="125"/>
-      <c r="H43" s="126"/>
-    </row>
-    <row r="44" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D43" s="122" t="s">
+        <v>407</v>
+      </c>
+      <c r="E43" s="127" t="s">
+        <v>408</v>
+      </c>
+      <c r="F43" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G43" s="125">
+        <v>43181</v>
+      </c>
+      <c r="H43" s="126">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="121"/>
       <c r="C44" s="122"/>
-      <c r="D44" s="122"/>
-      <c r="E44" s="123"/>
-      <c r="F44" s="124"/>
-      <c r="G44" s="125"/>
-      <c r="H44" s="126"/>
+      <c r="D44" s="122" t="s">
+        <v>409</v>
+      </c>
+      <c r="E44" s="127" t="s">
+        <v>410</v>
+      </c>
+      <c r="F44" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G44" s="125">
+        <v>44958</v>
+      </c>
+      <c r="H44" s="126">
+        <v>43181</v>
+      </c>
     </row>
     <row r="45" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="121"/>
       <c r="C45" s="122"/>
-      <c r="D45" s="122"/>
-      <c r="E45" s="127"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="125"/>
-      <c r="H45" s="126"/>
-    </row>
-    <row r="46" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D45" s="122" t="s">
+        <v>411</v>
+      </c>
+      <c r="E45" s="127" t="s">
+        <v>412</v>
+      </c>
+      <c r="F45" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G45" s="125">
+        <v>44958</v>
+      </c>
+      <c r="H45" s="126">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="121"/>
       <c r="C46" s="122"/>
-      <c r="D46" s="122"/>
-      <c r="E46" s="123"/>
-      <c r="F46" s="124"/>
-      <c r="G46" s="125"/>
-      <c r="H46" s="126"/>
-    </row>
-    <row r="47" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D46" s="122" t="s">
+        <v>413</v>
+      </c>
+      <c r="E46" s="127" t="s">
+        <v>414</v>
+      </c>
+      <c r="F46" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G46" s="125">
+        <v>44958</v>
+      </c>
+      <c r="H46" s="126">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="121"/>
-      <c r="C47" s="122" t="s">
-        <v>336</v>
-      </c>
-      <c r="D47" s="122" t="s">
-        <v>326</v>
-      </c>
-      <c r="E47" s="127" t="s">
-        <v>327</v>
-      </c>
-      <c r="F47" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G47" s="125">
-        <v>44902</v>
-      </c>
-      <c r="H47" s="126">
-        <v>44902</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C47" s="122"/>
+      <c r="D47" s="122"/>
+      <c r="E47" s="127"/>
+      <c r="F47" s="124"/>
+      <c r="G47" s="125"/>
+      <c r="H47" s="126"/>
+    </row>
+    <row r="48" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="121"/>
       <c r="C48" s="122"/>
-      <c r="D48" s="122" t="s">
-        <v>332</v>
-      </c>
-      <c r="E48" s="127" t="s">
-        <v>333</v>
-      </c>
-      <c r="F48" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G48" s="125">
-        <v>44897</v>
-      </c>
-      <c r="H48" s="126">
-        <v>44897</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D48" s="122"/>
+      <c r="E48" s="127"/>
+      <c r="F48" s="124"/>
+      <c r="G48" s="125"/>
+      <c r="H48" s="126"/>
+    </row>
+    <row r="49" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="121"/>
       <c r="C49" s="122"/>
-      <c r="D49" s="122" t="s">
-        <v>323</v>
-      </c>
-      <c r="E49" s="127" t="s">
-        <v>324</v>
-      </c>
-      <c r="F49" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G49" s="125">
-        <v>44951</v>
-      </c>
-      <c r="H49" s="126">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D49" s="122"/>
+      <c r="E49" s="127"/>
+      <c r="F49" s="124"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="126"/>
+    </row>
+    <row r="50" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="121"/>
       <c r="C50" s="122"/>
-      <c r="D50" s="122" t="s">
-        <v>338</v>
-      </c>
-      <c r="E50" s="127" t="s">
-        <v>337</v>
-      </c>
-      <c r="F50" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G50" s="125">
-        <v>44951</v>
-      </c>
-      <c r="H50" s="126">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D50" s="122"/>
+      <c r="E50" s="127"/>
+      <c r="F50" s="124"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="126"/>
+    </row>
+    <row r="51" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="121"/>
       <c r="C51" s="122"/>
-      <c r="D51" s="122" t="s">
-        <v>321</v>
-      </c>
-      <c r="E51" s="127" t="s">
-        <v>325</v>
-      </c>
-      <c r="F51" s="124" t="s">
-        <v>281</v>
-      </c>
-      <c r="G51" s="125">
-        <v>44900</v>
-      </c>
-      <c r="H51" s="126">
-        <v>44949</v>
-      </c>
+      <c r="D51" s="122"/>
+      <c r="E51" s="127"/>
+      <c r="F51" s="124"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="126"/>
     </row>
     <row r="52" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="121"/>
       <c r="C52" s="122"/>
-      <c r="D52" s="122" t="s">
-        <v>328</v>
-      </c>
-      <c r="E52" s="123" t="s">
-        <v>329</v>
-      </c>
-      <c r="F52" s="124" t="s">
-        <v>281</v>
-      </c>
-      <c r="G52" s="125">
-        <v>44896</v>
-      </c>
-      <c r="H52" s="126">
-        <v>44896</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D52" s="122"/>
+      <c r="E52" s="123"/>
+      <c r="F52" s="124"/>
+      <c r="G52" s="125"/>
+      <c r="H52" s="126"/>
+    </row>
+    <row r="53" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="121"/>
       <c r="C53" s="122"/>
       <c r="D53" s="122" t="s">
-        <v>322</v>
-      </c>
-      <c r="E53" s="127" t="s">
-        <v>339</v>
+        <v>286</v>
+      </c>
+      <c r="E53" s="123" t="s">
+        <v>287</v>
       </c>
       <c r="F53" s="124" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G53" s="125">
-        <v>44945</v>
+        <v>44949</v>
       </c>
       <c r="H53" s="126">
         <v>44949</v>
       </c>
     </row>
-    <row r="54" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
       <c r="B54" s="121"/>
       <c r="C54" s="122"/>
-      <c r="D54" s="122" t="s">
-        <v>334</v>
-      </c>
-      <c r="E54" s="127" t="s">
-        <v>335</v>
-      </c>
-      <c r="F54" s="124" t="s">
-        <v>281</v>
-      </c>
-      <c r="G54" s="125">
-        <v>44910</v>
-      </c>
-      <c r="H54" s="126">
-        <v>44910</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D54" s="122"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="124"/>
+      <c r="G54" s="125"/>
+      <c r="H54" s="126"/>
+    </row>
+    <row r="55" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="121"/>
       <c r="C55" s="122"/>
-      <c r="D55" s="122" t="s">
-        <v>340</v>
-      </c>
-      <c r="E55" s="127" t="s">
-        <v>341</v>
-      </c>
-      <c r="F55" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G55" s="125">
-        <v>44951</v>
-      </c>
-      <c r="H55" s="126">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D55" s="122"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="124"/>
+      <c r="G55" s="125"/>
+      <c r="H55" s="126"/>
+    </row>
+    <row r="56" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="121"/>
       <c r="C56" s="122"/>
-      <c r="D56" s="122" t="s">
-        <v>342</v>
-      </c>
-      <c r="E56" s="127" t="s">
-        <v>343</v>
-      </c>
-      <c r="F56" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G56" s="125">
-        <v>44952</v>
-      </c>
-      <c r="H56" s="126">
-        <v>44952</v>
-      </c>
+      <c r="D56" s="122"/>
+      <c r="E56" s="123"/>
+      <c r="F56" s="124"/>
+      <c r="G56" s="125"/>
+      <c r="H56" s="126"/>
     </row>
     <row r="57" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
       <c r="B57" s="121"/>
       <c r="C57" s="122"/>
       <c r="D57" s="122"/>
-      <c r="E57" s="123"/>
+      <c r="E57" s="127"/>
       <c r="F57" s="124"/>
       <c r="G57" s="125"/>
       <c r="H57" s="126"/>
@@ -3919,54 +3929,66 @@
       <c r="G58" s="125"/>
       <c r="H58" s="126"/>
     </row>
-    <row r="59" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="121"/>
-      <c r="C59" s="122"/>
-      <c r="D59" s="122"/>
-      <c r="E59" s="123"/>
-      <c r="F59" s="124"/>
-      <c r="G59" s="125"/>
-      <c r="H59" s="126"/>
-    </row>
-    <row r="60" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="C59" s="122" t="s">
+        <v>336</v>
+      </c>
+      <c r="D59" s="122" t="s">
+        <v>326</v>
+      </c>
+      <c r="E59" s="127" t="s">
+        <v>327</v>
+      </c>
+      <c r="F59" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G59" s="125">
+        <v>44902</v>
+      </c>
+      <c r="H59" s="126">
+        <v>44902</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="121"/>
       <c r="C60" s="122"/>
       <c r="D60" s="122" t="s">
-        <v>394</v>
+        <v>332</v>
       </c>
       <c r="E60" s="127" t="s">
-        <v>395</v>
+        <v>333</v>
       </c>
       <c r="F60" s="124" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G60" s="125">
-        <v>44957</v>
+        <v>44897</v>
       </c>
       <c r="H60" s="126">
-        <v>42982</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="121"/>
       <c r="C61" s="122"/>
       <c r="D61" s="122" t="s">
-        <v>393</v>
+        <v>323</v>
       </c>
       <c r="E61" s="127" t="s">
-        <v>396</v>
+        <v>324</v>
       </c>
       <c r="F61" s="124" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G61" s="125">
-        <v>44281</v>
+        <v>44951</v>
       </c>
       <c r="H61" s="126">
-        <v>44557</v>
+        <v>44951</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3974,19 +3996,19 @@
       <c r="B62" s="121"/>
       <c r="C62" s="122"/>
       <c r="D62" s="122" t="s">
-        <v>397</v>
+        <v>338</v>
       </c>
       <c r="E62" s="127" t="s">
-        <v>398</v>
+        <v>337</v>
       </c>
       <c r="F62" s="124" t="s">
         <v>232</v>
       </c>
       <c r="G62" s="125">
-        <v>43257</v>
+        <v>44951</v>
       </c>
       <c r="H62" s="126">
-        <v>43257</v>
+        <v>44951</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -3994,16 +4016,16 @@
       <c r="B63" s="121"/>
       <c r="C63" s="122"/>
       <c r="D63" s="122" t="s">
-        <v>286</v>
+        <v>321</v>
       </c>
       <c r="E63" s="127" t="s">
-        <v>399</v>
+        <v>325</v>
       </c>
       <c r="F63" s="124" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G63" s="125">
-        <v>44949</v>
+        <v>44900</v>
       </c>
       <c r="H63" s="126">
         <v>44949</v>
@@ -4013,70 +4035,100 @@
       <c r="A64" s="1"/>
       <c r="B64" s="121"/>
       <c r="C64" s="122"/>
-      <c r="D64" s="122"/>
-      <c r="E64" s="127"/>
-      <c r="F64" s="124"/>
-      <c r="G64" s="125"/>
-      <c r="H64" s="126"/>
+      <c r="D64" s="122" t="s">
+        <v>328</v>
+      </c>
+      <c r="E64" s="123" t="s">
+        <v>329</v>
+      </c>
+      <c r="F64" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G64" s="125">
+        <v>44896</v>
+      </c>
+      <c r="H64" s="126">
+        <v>44896</v>
+      </c>
     </row>
     <row r="65" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="121"/>
       <c r="C65" s="122"/>
       <c r="D65" s="122" t="s">
-        <v>392</v>
+        <v>322</v>
       </c>
       <c r="E65" s="127" t="s">
-        <v>400</v>
+        <v>339</v>
       </c>
       <c r="F65" s="124" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G65" s="125">
-        <v>44957</v>
+        <v>44945</v>
       </c>
       <c r="H65" s="126">
-        <v>44957</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
       <c r="B66" s="121"/>
       <c r="C66" s="122"/>
-      <c r="D66" s="122"/>
-      <c r="E66" s="127"/>
-      <c r="F66" s="124"/>
-      <c r="G66" s="125"/>
-      <c r="H66" s="126"/>
-    </row>
-    <row r="67" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D66" s="122" t="s">
+        <v>334</v>
+      </c>
+      <c r="E66" s="127" t="s">
+        <v>335</v>
+      </c>
+      <c r="F66" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G66" s="125">
+        <v>44910</v>
+      </c>
+      <c r="H66" s="126">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="121"/>
       <c r="C67" s="122"/>
-      <c r="D67" s="122"/>
-      <c r="E67" s="123"/>
-      <c r="F67" s="124"/>
-      <c r="G67" s="125"/>
-      <c r="H67" s="126"/>
-    </row>
-    <row r="68" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D67" s="122" t="s">
+        <v>340</v>
+      </c>
+      <c r="E67" s="127" t="s">
+        <v>341</v>
+      </c>
+      <c r="F67" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G67" s="125">
+        <v>44951</v>
+      </c>
+      <c r="H67" s="126">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="121"/>
       <c r="C68" s="122"/>
       <c r="D68" s="122" t="s">
-        <v>330</v>
-      </c>
-      <c r="E68" s="123" t="s">
-        <v>331</v>
+        <v>342</v>
+      </c>
+      <c r="E68" s="127" t="s">
+        <v>343</v>
       </c>
       <c r="F68" s="124" t="s">
         <v>232</v>
       </c>
       <c r="G68" s="125">
-        <v>44893</v>
+        <v>44952</v>
       </c>
       <c r="H68" s="126">
-        <v>44893</v>
+        <v>44952</v>
       </c>
     </row>
     <row r="69" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4109,72 +4161,122 @@
       <c r="G71" s="125"/>
       <c r="H71" s="126"/>
     </row>
-    <row r="72" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="121"/>
       <c r="C72" s="122"/>
-      <c r="D72" s="122"/>
-      <c r="E72" s="123"/>
-      <c r="F72" s="124"/>
-      <c r="G72" s="125"/>
-      <c r="H72" s="126"/>
-    </row>
-    <row r="73" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D72" s="122" t="s">
+        <v>394</v>
+      </c>
+      <c r="E72" s="127" t="s">
+        <v>395</v>
+      </c>
+      <c r="F72" s="124" t="s">
+        <v>267</v>
+      </c>
+      <c r="G72" s="125">
+        <v>44957</v>
+      </c>
+      <c r="H72" s="126">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="121"/>
       <c r="C73" s="122"/>
-      <c r="D73" s="122"/>
-      <c r="E73" s="123"/>
-      <c r="F73" s="124"/>
-      <c r="G73" s="125"/>
-      <c r="H73" s="126"/>
-    </row>
-    <row r="74" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D73" s="122" t="s">
+        <v>393</v>
+      </c>
+      <c r="E73" s="127" t="s">
+        <v>396</v>
+      </c>
+      <c r="F73" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="G73" s="125">
+        <v>44281</v>
+      </c>
+      <c r="H73" s="126">
+        <v>44557</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="121"/>
       <c r="C74" s="122"/>
-      <c r="D74" s="122"/>
-      <c r="E74" s="123"/>
-      <c r="F74" s="124"/>
-      <c r="G74" s="125"/>
-      <c r="H74" s="126"/>
-    </row>
-    <row r="75" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D74" s="122" t="s">
+        <v>397</v>
+      </c>
+      <c r="E74" s="127" t="s">
+        <v>398</v>
+      </c>
+      <c r="F74" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G74" s="125">
+        <v>43257</v>
+      </c>
+      <c r="H74" s="126">
+        <v>43257</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="121"/>
       <c r="C75" s="122"/>
-      <c r="D75" s="122"/>
-      <c r="E75" s="123"/>
-      <c r="F75" s="124"/>
-      <c r="G75" s="125"/>
-      <c r="H75" s="126"/>
+      <c r="D75" s="122" t="s">
+        <v>286</v>
+      </c>
+      <c r="E75" s="127" t="s">
+        <v>399</v>
+      </c>
+      <c r="F75" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G75" s="125">
+        <v>44949</v>
+      </c>
+      <c r="H75" s="126">
+        <v>44949</v>
+      </c>
     </row>
     <row r="76" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="121"/>
       <c r="C76" s="122"/>
       <c r="D76" s="122"/>
-      <c r="E76" s="123"/>
+      <c r="E76" s="127"/>
       <c r="F76" s="124"/>
       <c r="G76" s="125"/>
       <c r="H76" s="126"/>
     </row>
-    <row r="77" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="121"/>
       <c r="C77" s="122"/>
-      <c r="D77" s="122"/>
-      <c r="E77" s="123"/>
-      <c r="F77" s="124"/>
-      <c r="G77" s="125"/>
-      <c r="H77" s="126"/>
+      <c r="D77" s="122" t="s">
+        <v>392</v>
+      </c>
+      <c r="E77" s="127" t="s">
+        <v>400</v>
+      </c>
+      <c r="F77" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G77" s="125">
+        <v>44957</v>
+      </c>
+      <c r="H77" s="126">
+        <v>44957</v>
+      </c>
     </row>
     <row r="78" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="121"/>
       <c r="C78" s="122"/>
       <c r="D78" s="122"/>
-      <c r="E78" s="123"/>
+      <c r="E78" s="127"/>
       <c r="F78" s="124"/>
       <c r="G78" s="125"/>
       <c r="H78" s="126"/>
@@ -4193,11 +4295,21 @@
       <c r="A80" s="1"/>
       <c r="B80" s="121"/>
       <c r="C80" s="122"/>
-      <c r="D80" s="122"/>
-      <c r="E80" s="123"/>
-      <c r="F80" s="124"/>
-      <c r="G80" s="125"/>
-      <c r="H80" s="126"/>
+      <c r="D80" s="122" t="s">
+        <v>330</v>
+      </c>
+      <c r="E80" s="123" t="s">
+        <v>331</v>
+      </c>
+      <c r="F80" s="124" t="s">
+        <v>232</v>
+      </c>
+      <c r="G80" s="125">
+        <v>44893</v>
+      </c>
+      <c r="H80" s="126">
+        <v>44893</v>
+      </c>
     </row>
     <row r="81" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
@@ -4439,135 +4551,135 @@
       <c r="G104" s="125"/>
       <c r="H104" s="126"/>
     </row>
-    <row r="105" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
-      <c r="B105" s="134"/>
-      <c r="C105" s="135"/>
-      <c r="D105" s="135"/>
-      <c r="E105" s="136"/>
-      <c r="F105" s="137"/>
-      <c r="G105" s="138"/>
-      <c r="H105" s="139"/>
+      <c r="B105" s="121"/>
+      <c r="C105" s="122"/>
+      <c r="D105" s="122"/>
+      <c r="E105" s="123"/>
+      <c r="F105" s="124"/>
+      <c r="G105" s="125"/>
+      <c r="H105" s="126"/>
     </row>
     <row r="106" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
-      <c r="E106" s="1"/>
-      <c r="F106" s="140"/>
-      <c r="G106" s="141"/>
-      <c r="H106" s="141"/>
+      <c r="B106" s="121"/>
+      <c r="C106" s="122"/>
+      <c r="D106" s="122"/>
+      <c r="E106" s="123"/>
+      <c r="F106" s="124"/>
+      <c r="G106" s="125"/>
+      <c r="H106" s="126"/>
     </row>
     <row r="107" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
-      <c r="E107" s="1"/>
-      <c r="F107" s="140"/>
-      <c r="G107" s="141"/>
-      <c r="H107" s="141"/>
+      <c r="B107" s="121"/>
+      <c r="C107" s="122"/>
+      <c r="D107" s="122"/>
+      <c r="E107" s="123"/>
+      <c r="F107" s="124"/>
+      <c r="G107" s="125"/>
+      <c r="H107" s="126"/>
     </row>
     <row r="108" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="140"/>
-      <c r="G108" s="141"/>
-      <c r="H108" s="141"/>
+      <c r="B108" s="121"/>
+      <c r="C108" s="122"/>
+      <c r="D108" s="122"/>
+      <c r="E108" s="123"/>
+      <c r="F108" s="124"/>
+      <c r="G108" s="125"/>
+      <c r="H108" s="126"/>
     </row>
     <row r="109" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
-      <c r="D109" s="1"/>
-      <c r="E109" s="1"/>
-      <c r="F109" s="140"/>
-      <c r="G109" s="141"/>
-      <c r="H109" s="141"/>
+      <c r="B109" s="121"/>
+      <c r="C109" s="122"/>
+      <c r="D109" s="122"/>
+      <c r="E109" s="123"/>
+      <c r="F109" s="124"/>
+      <c r="G109" s="125"/>
+      <c r="H109" s="126"/>
     </row>
     <row r="110" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
-      <c r="B110" s="1"/>
-      <c r="C110" s="1"/>
-      <c r="D110" s="1"/>
-      <c r="E110" s="1"/>
-      <c r="F110" s="140"/>
-      <c r="G110" s="141"/>
-      <c r="H110" s="141"/>
+      <c r="B110" s="121"/>
+      <c r="C110" s="122"/>
+      <c r="D110" s="122"/>
+      <c r="E110" s="123"/>
+      <c r="F110" s="124"/>
+      <c r="G110" s="125"/>
+      <c r="H110" s="126"/>
     </row>
     <row r="111" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
-      <c r="B111" s="1"/>
-      <c r="C111" s="1"/>
-      <c r="D111" s="1"/>
-      <c r="E111" s="1"/>
-      <c r="F111" s="140"/>
-      <c r="G111" s="141"/>
-      <c r="H111" s="141"/>
+      <c r="B111" s="121"/>
+      <c r="C111" s="122"/>
+      <c r="D111" s="122"/>
+      <c r="E111" s="123"/>
+      <c r="F111" s="124"/>
+      <c r="G111" s="125"/>
+      <c r="H111" s="126"/>
     </row>
     <row r="112" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
-      <c r="B112" s="1"/>
-      <c r="C112" s="1"/>
-      <c r="D112" s="1"/>
-      <c r="E112" s="1"/>
-      <c r="F112" s="140"/>
-      <c r="G112" s="141"/>
-      <c r="H112" s="141"/>
+      <c r="B112" s="121"/>
+      <c r="C112" s="122"/>
+      <c r="D112" s="122"/>
+      <c r="E112" s="123"/>
+      <c r="F112" s="124"/>
+      <c r="G112" s="125"/>
+      <c r="H112" s="126"/>
     </row>
     <row r="113" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-      <c r="C113" s="1"/>
-      <c r="D113" s="1"/>
-      <c r="E113" s="1"/>
-      <c r="F113" s="140"/>
-      <c r="G113" s="141"/>
-      <c r="H113" s="141"/>
+      <c r="B113" s="121"/>
+      <c r="C113" s="122"/>
+      <c r="D113" s="122"/>
+      <c r="E113" s="123"/>
+      <c r="F113" s="124"/>
+      <c r="G113" s="125"/>
+      <c r="H113" s="126"/>
     </row>
     <row r="114" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
-      <c r="B114" s="1"/>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="140"/>
-      <c r="G114" s="141"/>
-      <c r="H114" s="141"/>
+      <c r="B114" s="121"/>
+      <c r="C114" s="122"/>
+      <c r="D114" s="122"/>
+      <c r="E114" s="123"/>
+      <c r="F114" s="124"/>
+      <c r="G114" s="125"/>
+      <c r="H114" s="126"/>
     </row>
     <row r="115" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
-      <c r="B115" s="1"/>
-      <c r="C115" s="1"/>
-      <c r="D115" s="1"/>
-      <c r="E115" s="1"/>
-      <c r="F115" s="140"/>
-      <c r="G115" s="141"/>
-      <c r="H115" s="141"/>
+      <c r="B115" s="121"/>
+      <c r="C115" s="122"/>
+      <c r="D115" s="122"/>
+      <c r="E115" s="123"/>
+      <c r="F115" s="124"/>
+      <c r="G115" s="125"/>
+      <c r="H115" s="126"/>
     </row>
     <row r="116" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
-      <c r="B116" s="1"/>
-      <c r="C116" s="1"/>
-      <c r="D116" s="1"/>
-      <c r="E116" s="1"/>
-      <c r="F116" s="140"/>
-      <c r="G116" s="141"/>
-      <c r="H116" s="141"/>
-    </row>
-    <row r="117" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B116" s="121"/>
+      <c r="C116" s="122"/>
+      <c r="D116" s="122"/>
+      <c r="E116" s="123"/>
+      <c r="F116" s="124"/>
+      <c r="G116" s="125"/>
+      <c r="H116" s="126"/>
+    </row>
+    <row r="117" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A117" s="1"/>
-      <c r="B117" s="1"/>
-      <c r="C117" s="1"/>
-      <c r="D117" s="1"/>
-      <c r="E117" s="1"/>
-      <c r="F117" s="140"/>
-      <c r="G117" s="141"/>
-      <c r="H117" s="141"/>
+      <c r="B117" s="134"/>
+      <c r="C117" s="135"/>
+      <c r="D117" s="135"/>
+      <c r="E117" s="136"/>
+      <c r="F117" s="137"/>
+      <c r="G117" s="138"/>
+      <c r="H117" s="139"/>
     </row>
     <row r="118" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
@@ -4610,19 +4722,139 @@
       <c r="H121" s="141"/>
     </row>
     <row r="122" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F122" s="95"/>
-      <c r="G122" s="111"/>
-      <c r="H122" s="111"/>
+      <c r="A122" s="1"/>
+      <c r="B122" s="1"/>
+      <c r="C122" s="1"/>
+      <c r="D122" s="1"/>
+      <c r="E122" s="1"/>
+      <c r="F122" s="140"/>
+      <c r="G122" s="141"/>
+      <c r="H122" s="141"/>
     </row>
     <row r="123" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F123" s="95"/>
-      <c r="G123" s="111"/>
-      <c r="H123" s="111"/>
+      <c r="A123" s="1"/>
+      <c r="B123" s="1"/>
+      <c r="C123" s="1"/>
+      <c r="D123" s="1"/>
+      <c r="E123" s="1"/>
+      <c r="F123" s="140"/>
+      <c r="G123" s="141"/>
+      <c r="H123" s="141"/>
     </row>
     <row r="124" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F124" s="95"/>
-      <c r="G124" s="111"/>
-      <c r="H124" s="111"/>
+      <c r="A124" s="1"/>
+      <c r="B124" s="1"/>
+      <c r="C124" s="1"/>
+      <c r="D124" s="1"/>
+      <c r="E124" s="1"/>
+      <c r="F124" s="140"/>
+      <c r="G124" s="141"/>
+      <c r="H124" s="141"/>
+    </row>
+    <row r="125" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A125" s="1"/>
+      <c r="B125" s="1"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+      <c r="E125" s="1"/>
+      <c r="F125" s="140"/>
+      <c r="G125" s="141"/>
+      <c r="H125" s="141"/>
+    </row>
+    <row r="126" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A126" s="1"/>
+      <c r="B126" s="1"/>
+      <c r="C126" s="1"/>
+      <c r="D126" s="1"/>
+      <c r="E126" s="1"/>
+      <c r="F126" s="140"/>
+      <c r="G126" s="141"/>
+      <c r="H126" s="141"/>
+    </row>
+    <row r="127" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A127" s="1"/>
+      <c r="B127" s="1"/>
+      <c r="C127" s="1"/>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1"/>
+      <c r="F127" s="140"/>
+      <c r="G127" s="141"/>
+      <c r="H127" s="141"/>
+    </row>
+    <row r="128" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A128" s="1"/>
+      <c r="B128" s="1"/>
+      <c r="C128" s="1"/>
+      <c r="D128" s="1"/>
+      <c r="E128" s="1"/>
+      <c r="F128" s="140"/>
+      <c r="G128" s="141"/>
+      <c r="H128" s="141"/>
+    </row>
+    <row r="129" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A129" s="1"/>
+      <c r="B129" s="1"/>
+      <c r="C129" s="1"/>
+      <c r="D129" s="1"/>
+      <c r="E129" s="1"/>
+      <c r="F129" s="140"/>
+      <c r="G129" s="141"/>
+      <c r="H129" s="141"/>
+    </row>
+    <row r="130" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A130" s="1"/>
+      <c r="B130" s="1"/>
+      <c r="C130" s="1"/>
+      <c r="D130" s="1"/>
+      <c r="E130" s="1"/>
+      <c r="F130" s="140"/>
+      <c r="G130" s="141"/>
+      <c r="H130" s="141"/>
+    </row>
+    <row r="131" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A131" s="1"/>
+      <c r="B131" s="1"/>
+      <c r="C131" s="1"/>
+      <c r="D131" s="1"/>
+      <c r="E131" s="1"/>
+      <c r="F131" s="140"/>
+      <c r="G131" s="141"/>
+      <c r="H131" s="141"/>
+    </row>
+    <row r="132" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A132" s="1"/>
+      <c r="B132" s="1"/>
+      <c r="C132" s="1"/>
+      <c r="D132" s="1"/>
+      <c r="E132" s="1"/>
+      <c r="F132" s="140"/>
+      <c r="G132" s="141"/>
+      <c r="H132" s="141"/>
+    </row>
+    <row r="133" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A133" s="1"/>
+      <c r="B133" s="1"/>
+      <c r="C133" s="1"/>
+      <c r="D133" s="1"/>
+      <c r="E133" s="1"/>
+      <c r="F133" s="140"/>
+      <c r="G133" s="141"/>
+      <c r="H133" s="141"/>
+    </row>
+    <row r="134" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F134" s="95"/>
+      <c r="G134" s="111"/>
+      <c r="H134" s="111"/>
+    </row>
+    <row r="135" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F135" s="95"/>
+      <c r="G135" s="111"/>
+      <c r="H135" s="111"/>
+    </row>
+    <row r="136" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F136" s="95"/>
+      <c r="G136" s="111"/>
+      <c r="H136" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4631,6 +4863,7 @@
     <mergeCell ref="F2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Update Pertanggal 01 Februari 2023 16:08 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -2010,7 +2010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="213">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2314,18 +2314,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2351,9 +2339,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2362,9 +2347,6 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2470,12 +2452,63 @@
     <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2500,57 +2533,6 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2562,6 +2544,63 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2874,13 +2913,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H136"/>
+  <dimension ref="A1:H137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2898,19 +2937,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="162" t="s">
+      <c r="B2" s="156" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="163"/>
-      <c r="E2" s="164" t="s">
+      <c r="C2" s="157"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="158" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="166" t="s">
+      <c r="F2" s="160" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="167"/>
-      <c r="H2" s="168"/>
+      <c r="G2" s="161"/>
+      <c r="H2" s="162"/>
     </row>
     <row r="3" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="91" t="s">
@@ -2922,7 +2961,7 @@
       <c r="D3" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="165"/>
+      <c r="E3" s="159"/>
       <c r="F3" s="112" t="s">
         <v>228</v>
       </c>
@@ -2941,1755 +2980,1755 @@
       <c r="C4" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="116" t="s">
+      <c r="D4" s="201" t="s">
         <v>227</v>
       </c>
-      <c r="E4" s="117" t="s">
+      <c r="E4" s="202" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="118" t="s">
+      <c r="F4" s="203" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="119">
+      <c r="G4" s="204">
         <v>44910</v>
       </c>
-      <c r="H4" s="120">
+      <c r="H4" s="205">
         <v>44910</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="121"/>
-      <c r="C5" s="122"/>
-      <c r="D5" s="122" t="s">
+      <c r="B5" s="117"/>
+      <c r="C5" s="118"/>
+      <c r="D5" s="194" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="123" t="s">
+      <c r="E5" s="195" t="s">
         <v>236</v>
       </c>
-      <c r="F5" s="124" t="s">
+      <c r="F5" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G5" s="125">
+      <c r="G5" s="197">
         <v>44908</v>
       </c>
-      <c r="H5" s="126">
+      <c r="H5" s="198">
         <v>44908</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="121"/>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122" t="s">
+      <c r="B6" s="117"/>
+      <c r="C6" s="118"/>
+      <c r="D6" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="123" t="s">
+      <c r="E6" s="195" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="124" t="s">
+      <c r="F6" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G6" s="125">
+      <c r="G6" s="197">
         <v>44908</v>
       </c>
-      <c r="H6" s="126">
+      <c r="H6" s="198">
         <v>44908</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="121"/>
-      <c r="C7" s="122"/>
-      <c r="D7" s="122" t="s">
+      <c r="B7" s="117"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="194" t="s">
         <v>238</v>
       </c>
-      <c r="E7" s="123" t="s">
+      <c r="E7" s="195" t="s">
         <v>239</v>
       </c>
-      <c r="F7" s="124" t="s">
+      <c r="F7" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G7" s="125">
+      <c r="G7" s="197">
         <v>44887</v>
       </c>
-      <c r="H7" s="126">
+      <c r="H7" s="198">
         <v>44887</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="121"/>
-      <c r="C8" s="122"/>
-      <c r="D8" s="122" t="s">
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="194" t="s">
         <v>240</v>
       </c>
-      <c r="E8" s="123" t="s">
+      <c r="E8" s="195" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="124" t="s">
+      <c r="F8" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="125">
+      <c r="G8" s="197">
         <v>44887</v>
       </c>
-      <c r="H8" s="126">
+      <c r="H8" s="198">
         <v>44887</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="121"/>
-      <c r="C9" s="122"/>
-      <c r="D9" s="122" t="s">
+      <c r="B9" s="117"/>
+      <c r="C9" s="118"/>
+      <c r="D9" s="194" t="s">
         <v>242</v>
       </c>
-      <c r="E9" s="123" t="s">
+      <c r="E9" s="195" t="s">
         <v>243</v>
       </c>
-      <c r="F9" s="124" t="s">
+      <c r="F9" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G9" s="125">
+      <c r="G9" s="197">
         <v>44774</v>
       </c>
-      <c r="H9" s="126">
+      <c r="H9" s="198">
         <v>44774</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="121"/>
-      <c r="C10" s="122"/>
-      <c r="D10" s="122" t="s">
+      <c r="B10" s="117"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="194" t="s">
         <v>305</v>
       </c>
-      <c r="E10" s="123" t="s">
+      <c r="E10" s="195" t="s">
         <v>306</v>
       </c>
-      <c r="F10" s="124" t="s">
+      <c r="F10" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="125">
+      <c r="G10" s="197">
         <v>44897</v>
       </c>
-      <c r="H10" s="126">
+      <c r="H10" s="198">
         <v>44897</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="121"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122" t="s">
+      <c r="B11" s="117"/>
+      <c r="C11" s="118"/>
+      <c r="D11" s="194" t="s">
         <v>244</v>
       </c>
-      <c r="E11" s="123" t="s">
+      <c r="E11" s="195" t="s">
         <v>245</v>
       </c>
-      <c r="F11" s="124" t="s">
+      <c r="F11" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="125">
+      <c r="G11" s="197">
         <v>44897</v>
       </c>
-      <c r="H11" s="126">
+      <c r="H11" s="198">
         <v>44897</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="122" t="s">
+      <c r="B12" s="117"/>
+      <c r="C12" s="118"/>
+      <c r="D12" s="194" t="s">
         <v>246</v>
       </c>
-      <c r="E12" s="123" t="s">
+      <c r="E12" s="195" t="s">
         <v>247</v>
       </c>
-      <c r="F12" s="124" t="s">
+      <c r="F12" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G12" s="125">
+      <c r="G12" s="197">
         <v>44897</v>
       </c>
-      <c r="H12" s="126">
+      <c r="H12" s="198">
         <v>44897</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="121"/>
-      <c r="C13" s="122"/>
-      <c r="D13" s="122" t="s">
+      <c r="B13" s="117"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="194" t="s">
         <v>248</v>
       </c>
-      <c r="E13" s="123" t="s">
+      <c r="E13" s="195" t="s">
         <v>249</v>
       </c>
-      <c r="F13" s="124" t="s">
+      <c r="F13" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G13" s="125">
+      <c r="G13" s="197">
         <v>44748</v>
       </c>
-      <c r="H13" s="126">
+      <c r="H13" s="198">
         <v>44748</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="121"/>
-      <c r="C14" s="122"/>
-      <c r="D14" s="122" t="s">
+      <c r="B14" s="117"/>
+      <c r="C14" s="118"/>
+      <c r="D14" s="194" t="s">
         <v>250</v>
       </c>
-      <c r="E14" s="123" t="s">
+      <c r="E14" s="195" t="s">
         <v>251</v>
       </c>
-      <c r="F14" s="124" t="s">
+      <c r="F14" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G14" s="125">
+      <c r="G14" s="197">
         <v>44735</v>
       </c>
-      <c r="H14" s="126">
+      <c r="H14" s="198">
         <v>44735</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122" t="s">
+      <c r="B15" s="117"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="194" t="s">
         <v>252</v>
       </c>
-      <c r="E15" s="123" t="s">
+      <c r="E15" s="195" t="s">
         <v>253</v>
       </c>
-      <c r="F15" s="124" t="s">
+      <c r="F15" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G15" s="125">
+      <c r="G15" s="197">
         <v>44854</v>
       </c>
-      <c r="H15" s="126">
+      <c r="H15" s="198">
         <v>44854</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="121"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122" t="s">
+      <c r="B16" s="117"/>
+      <c r="C16" s="118"/>
+      <c r="D16" s="194" t="s">
         <v>254</v>
       </c>
-      <c r="E16" s="123" t="s">
+      <c r="E16" s="195" t="s">
         <v>259</v>
       </c>
-      <c r="F16" s="124" t="s">
+      <c r="F16" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G16" s="125">
+      <c r="G16" s="197">
         <v>44770</v>
       </c>
-      <c r="H16" s="126">
+      <c r="H16" s="198">
         <v>44770</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="121"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122" t="s">
+      <c r="B17" s="117"/>
+      <c r="C17" s="118"/>
+      <c r="D17" s="194" t="s">
         <v>255</v>
       </c>
-      <c r="E17" s="123" t="s">
+      <c r="E17" s="195" t="s">
         <v>260</v>
       </c>
-      <c r="F17" s="124" t="s">
+      <c r="F17" s="196" t="s">
         <v>256</v>
       </c>
-      <c r="G17" s="125">
+      <c r="G17" s="197">
         <v>44770</v>
       </c>
-      <c r="H17" s="126">
+      <c r="H17" s="198">
         <v>44427</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="121"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122" t="s">
+      <c r="B18" s="117"/>
+      <c r="C18" s="118"/>
+      <c r="D18" s="194" t="s">
         <v>257</v>
       </c>
-      <c r="E18" s="123" t="s">
+      <c r="E18" s="195" t="s">
         <v>261</v>
       </c>
-      <c r="F18" s="124" t="s">
+      <c r="F18" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G18" s="125">
+      <c r="G18" s="197">
         <v>44770</v>
       </c>
-      <c r="H18" s="126">
+      <c r="H18" s="198">
         <v>44770</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122" t="s">
+      <c r="B19" s="117"/>
+      <c r="C19" s="118"/>
+      <c r="D19" s="194" t="s">
         <v>258</v>
       </c>
-      <c r="E19" s="123" t="s">
+      <c r="E19" s="195" t="s">
         <v>262</v>
       </c>
-      <c r="F19" s="124" t="s">
+      <c r="F19" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G19" s="125">
+      <c r="G19" s="197">
         <v>44770</v>
       </c>
-      <c r="H19" s="126">
+      <c r="H19" s="198">
         <v>44427</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
-      <c r="B20" s="121"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="122" t="s">
+      <c r="B20" s="117"/>
+      <c r="C20" s="118"/>
+      <c r="D20" s="194" t="s">
         <v>283</v>
       </c>
-      <c r="E20" s="123" t="s">
+      <c r="E20" s="195" t="s">
         <v>263</v>
       </c>
-      <c r="F20" s="124" t="s">
+      <c r="F20" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G20" s="125">
+      <c r="G20" s="197">
         <v>44777</v>
       </c>
-      <c r="H20" s="126">
+      <c r="H20" s="198">
         <v>44777</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
-      <c r="B21" s="121"/>
-      <c r="C21" s="122"/>
-      <c r="D21" s="122" t="s">
+      <c r="B21" s="117"/>
+      <c r="C21" s="118"/>
+      <c r="D21" s="194" t="s">
         <v>303</v>
       </c>
-      <c r="E21" s="123" t="s">
+      <c r="E21" s="195" t="s">
         <v>304</v>
       </c>
-      <c r="F21" s="124" t="s">
+      <c r="F21" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G21" s="125">
+      <c r="G21" s="197">
         <v>44935</v>
       </c>
-      <c r="H21" s="126">
+      <c r="H21" s="198">
         <v>44935</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
-      <c r="B22" s="121"/>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122" t="s">
+      <c r="B22" s="117"/>
+      <c r="C22" s="118"/>
+      <c r="D22" s="194" t="s">
         <v>284</v>
       </c>
-      <c r="E22" s="123" t="s">
+      <c r="E22" s="195" t="s">
         <v>277</v>
       </c>
-      <c r="F22" s="124" t="s">
+      <c r="F22" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G22" s="125">
+      <c r="G22" s="197">
         <v>44931</v>
       </c>
-      <c r="H22" s="126">
+      <c r="H22" s="198">
         <v>44931</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
-      <c r="B23" s="121"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122" t="s">
+      <c r="B23" s="117"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="194" t="s">
         <v>264</v>
       </c>
-      <c r="E23" s="123" t="s">
+      <c r="E23" s="195" t="s">
         <v>265</v>
       </c>
-      <c r="F23" s="124" t="s">
+      <c r="F23" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G23" s="125">
+      <c r="G23" s="197">
         <v>44847</v>
       </c>
-      <c r="H23" s="126">
+      <c r="H23" s="198">
         <v>44847</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
-      <c r="B24" s="121"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122" t="s">
+      <c r="B24" s="117"/>
+      <c r="C24" s="118"/>
+      <c r="D24" s="194" t="s">
         <v>266</v>
       </c>
-      <c r="E24" s="123" t="s">
+      <c r="E24" s="195" t="s">
         <v>268</v>
       </c>
-      <c r="F24" s="124" t="s">
+      <c r="F24" s="196" t="s">
         <v>267</v>
       </c>
-      <c r="G24" s="125">
+      <c r="G24" s="197">
         <v>44792</v>
       </c>
-      <c r="H24" s="126">
+      <c r="H24" s="198">
         <v>44770</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
-      <c r="B25" s="121"/>
-      <c r="C25" s="122"/>
-      <c r="D25" s="122" t="s">
+      <c r="B25" s="117"/>
+      <c r="C25" s="118"/>
+      <c r="D25" s="194" t="s">
         <v>269</v>
       </c>
-      <c r="E25" s="123" t="s">
+      <c r="E25" s="195" t="s">
         <v>270</v>
       </c>
-      <c r="F25" s="124" t="s">
+      <c r="F25" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G25" s="125">
+      <c r="G25" s="197">
         <v>44776</v>
       </c>
-      <c r="H25" s="126">
+      <c r="H25" s="198">
         <v>44776</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
-      <c r="B26" s="121"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="122" t="s">
+      <c r="B26" s="117"/>
+      <c r="C26" s="118"/>
+      <c r="D26" s="194" t="s">
         <v>302</v>
       </c>
-      <c r="E26" s="123" t="s">
+      <c r="E26" s="195" t="s">
         <v>271</v>
       </c>
-      <c r="F26" s="124" t="s">
+      <c r="F26" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G26" s="125">
+      <c r="G26" s="197">
         <v>44777</v>
       </c>
-      <c r="H26" s="126">
+      <c r="H26" s="198">
         <v>44777</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
-      <c r="B27" s="121"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122" t="s">
+      <c r="B27" s="117"/>
+      <c r="C27" s="118"/>
+      <c r="D27" s="194" t="s">
         <v>272</v>
       </c>
-      <c r="E27" s="123" t="s">
+      <c r="E27" s="195" t="s">
         <v>273</v>
       </c>
-      <c r="F27" s="124" t="s">
+      <c r="F27" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G27" s="125">
+      <c r="G27" s="197">
         <v>44770</v>
       </c>
-      <c r="H27" s="126">
+      <c r="H27" s="198">
         <v>44770</v>
       </c>
     </row>
     <row r="28" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
-      <c r="B28" s="121"/>
-      <c r="C28" s="122"/>
-      <c r="D28" s="122" t="s">
+      <c r="B28" s="117"/>
+      <c r="C28" s="118"/>
+      <c r="D28" s="194" t="s">
         <v>294</v>
       </c>
-      <c r="E28" s="127" t="s">
+      <c r="E28" s="200" t="s">
         <v>296</v>
       </c>
-      <c r="F28" s="124" t="s">
+      <c r="F28" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G28" s="125">
+      <c r="G28" s="197">
         <v>44937</v>
       </c>
-      <c r="H28" s="126">
+      <c r="H28" s="198">
         <v>44937</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
-      <c r="B29" s="121"/>
-      <c r="C29" s="122"/>
-      <c r="D29" s="122" t="s">
+      <c r="B29" s="117"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="194" t="s">
         <v>293</v>
       </c>
-      <c r="E29" s="127" t="s">
+      <c r="E29" s="200" t="s">
         <v>295</v>
       </c>
-      <c r="F29" s="124" t="s">
+      <c r="F29" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G29" s="125">
+      <c r="G29" s="197">
         <v>44937</v>
       </c>
-      <c r="H29" s="126">
+      <c r="H29" s="198">
         <v>44937</v>
       </c>
     </row>
     <row r="30" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
-      <c r="B30" s="121"/>
-      <c r="C30" s="122"/>
-      <c r="D30" s="122" t="s">
+      <c r="B30" s="117"/>
+      <c r="C30" s="118"/>
+      <c r="D30" s="194" t="s">
         <v>291</v>
       </c>
-      <c r="E30" s="127" t="s">
+      <c r="E30" s="200" t="s">
         <v>297</v>
       </c>
-      <c r="F30" s="124" t="s">
+      <c r="F30" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G30" s="125">
+      <c r="G30" s="197">
         <v>44937</v>
       </c>
-      <c r="H30" s="126">
+      <c r="H30" s="198">
         <v>44937</v>
       </c>
     </row>
     <row r="31" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
-      <c r="B31" s="121"/>
-      <c r="C31" s="122"/>
-      <c r="D31" s="122" t="s">
+      <c r="B31" s="117"/>
+      <c r="C31" s="118"/>
+      <c r="D31" s="194" t="s">
         <v>307</v>
       </c>
-      <c r="E31" s="127" t="s">
+      <c r="E31" s="200" t="s">
         <v>308</v>
       </c>
-      <c r="F31" s="124" t="s">
+      <c r="F31" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G31" s="125">
+      <c r="G31" s="197">
         <v>44949</v>
       </c>
-      <c r="H31" s="126">
+      <c r="H31" s="198">
         <v>44949</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="121"/>
-      <c r="C32" s="122"/>
-      <c r="D32" s="122" t="s">
+      <c r="B32" s="117"/>
+      <c r="C32" s="118"/>
+      <c r="D32" s="194" t="s">
         <v>292</v>
       </c>
-      <c r="E32" s="127" t="s">
+      <c r="E32" s="200" t="s">
         <v>298</v>
       </c>
-      <c r="F32" s="124" t="s">
+      <c r="F32" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G32" s="125">
+      <c r="G32" s="197">
         <v>44937</v>
       </c>
-      <c r="H32" s="126">
+      <c r="H32" s="198">
         <v>44937</v>
       </c>
     </row>
     <row r="33" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="121"/>
-      <c r="C33" s="122"/>
-      <c r="D33" s="122" t="s">
+      <c r="B33" s="117"/>
+      <c r="C33" s="118"/>
+      <c r="D33" s="194" t="s">
         <v>290</v>
       </c>
-      <c r="E33" s="127" t="s">
+      <c r="E33" s="200" t="s">
         <v>299</v>
       </c>
-      <c r="F33" s="124" t="s">
+      <c r="F33" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G33" s="125">
+      <c r="G33" s="197">
         <v>44937</v>
       </c>
-      <c r="H33" s="126">
+      <c r="H33" s="198">
         <v>44937</v>
       </c>
     </row>
     <row r="34" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="121"/>
-      <c r="C34" s="122"/>
-      <c r="D34" s="122" t="s">
+      <c r="B34" s="117"/>
+      <c r="C34" s="118"/>
+      <c r="D34" s="194" t="s">
         <v>289</v>
       </c>
-      <c r="E34" s="127" t="s">
+      <c r="E34" s="200" t="s">
         <v>300</v>
       </c>
-      <c r="F34" s="124" t="s">
+      <c r="F34" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G34" s="125">
+      <c r="G34" s="197">
         <v>44937</v>
       </c>
-      <c r="H34" s="126">
+      <c r="H34" s="198">
         <v>44937</v>
       </c>
     </row>
     <row r="35" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="121"/>
-      <c r="C35" s="122"/>
-      <c r="D35" s="122" t="s">
+      <c r="B35" s="117"/>
+      <c r="C35" s="118"/>
+      <c r="D35" s="124" t="s">
         <v>288</v>
       </c>
-      <c r="E35" s="127" t="s">
+      <c r="E35" s="206" t="s">
         <v>301</v>
       </c>
-      <c r="F35" s="124" t="s">
+      <c r="F35" s="125" t="s">
         <v>232</v>
       </c>
-      <c r="G35" s="125">
+      <c r="G35" s="126">
         <v>44937</v>
       </c>
-      <c r="H35" s="126">
+      <c r="H35" s="127">
         <v>44937</v>
       </c>
     </row>
     <row r="36" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="121"/>
-      <c r="C36" s="128" t="s">
-        <v>146</v>
-      </c>
-      <c r="D36" s="128" t="s">
-        <v>274</v>
-      </c>
-      <c r="E36" s="129" t="s">
-        <v>275</v>
-      </c>
-      <c r="F36" s="130" t="s">
-        <v>232</v>
-      </c>
-      <c r="G36" s="131">
-        <v>44167</v>
-      </c>
-      <c r="H36" s="132">
-        <v>44167</v>
-      </c>
+      <c r="B36" s="117"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="212"/>
     </row>
     <row r="37" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="121"/>
-      <c r="C37" s="122"/>
-      <c r="D37" s="133" t="s">
-        <v>276</v>
-      </c>
-      <c r="E37" s="123" t="s">
-        <v>285</v>
-      </c>
-      <c r="F37" s="124" t="s">
+      <c r="B37" s="117"/>
+      <c r="C37" s="118" t="s">
+        <v>146</v>
+      </c>
+      <c r="D37" s="207" t="s">
+        <v>274</v>
+      </c>
+      <c r="E37" s="208" t="s">
+        <v>275</v>
+      </c>
+      <c r="F37" s="209" t="s">
         <v>232</v>
       </c>
-      <c r="G37" s="125">
+      <c r="G37" s="210">
         <v>44167</v>
       </c>
-      <c r="H37" s="126">
+      <c r="H37" s="211">
         <v>44167</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="121"/>
-      <c r="C38" s="122"/>
-      <c r="D38" s="122" t="s">
-        <v>278</v>
-      </c>
-      <c r="E38" s="123" t="s">
-        <v>279</v>
-      </c>
-      <c r="F38" s="124" t="s">
+      <c r="B38" s="117"/>
+      <c r="C38" s="118"/>
+      <c r="D38" s="199" t="s">
+        <v>276</v>
+      </c>
+      <c r="E38" s="195" t="s">
+        <v>285</v>
+      </c>
+      <c r="F38" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G38" s="125">
-        <v>43185</v>
-      </c>
-      <c r="H38" s="126">
-        <v>43185</v>
+      <c r="G38" s="197">
+        <v>44167</v>
+      </c>
+      <c r="H38" s="198">
+        <v>44167</v>
       </c>
     </row>
     <row r="39" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
-      <c r="B39" s="121"/>
-      <c r="C39" s="122"/>
-      <c r="D39" s="122" t="s">
+      <c r="B39" s="117"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="194" t="s">
+        <v>278</v>
+      </c>
+      <c r="E39" s="195" t="s">
+        <v>279</v>
+      </c>
+      <c r="F39" s="196" t="s">
+        <v>232</v>
+      </c>
+      <c r="G39" s="197">
+        <v>43185</v>
+      </c>
+      <c r="H39" s="198">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="117"/>
+      <c r="C40" s="118"/>
+      <c r="D40" s="194" t="s">
         <v>280</v>
       </c>
-      <c r="E39" s="123" t="s">
+      <c r="E40" s="195" t="s">
         <v>282</v>
       </c>
-      <c r="F39" s="124" t="s">
+      <c r="F40" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="G39" s="125">
+      <c r="G40" s="197">
         <v>44216</v>
       </c>
-      <c r="H39" s="126">
+      <c r="H40" s="198">
         <v>44216</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="121"/>
-      <c r="C40" s="122"/>
-      <c r="D40" s="122" t="s">
+    <row r="41" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="117"/>
+      <c r="C41" s="118"/>
+      <c r="D41" s="194" t="s">
         <v>401</v>
       </c>
-      <c r="E40" s="127" t="s">
+      <c r="E41" s="200" t="s">
         <v>403</v>
       </c>
-      <c r="F40" s="124" t="s">
+      <c r="F41" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G40" s="125">
+      <c r="G41" s="197">
         <v>43720</v>
       </c>
-      <c r="H40" s="126">
+      <c r="H41" s="198">
         <v>43720</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="121"/>
-      <c r="C41" s="122"/>
-      <c r="D41" s="122" t="s">
+    <row r="42" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A42" s="1"/>
+      <c r="B42" s="117"/>
+      <c r="C42" s="118"/>
+      <c r="D42" s="194" t="s">
         <v>402</v>
       </c>
-      <c r="E41" s="127" t="s">
+      <c r="E42" s="200" t="s">
         <v>404</v>
       </c>
-      <c r="F41" s="124" t="s">
+      <c r="F42" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G41" s="125">
+      <c r="G42" s="197">
         <v>43785</v>
       </c>
-      <c r="H41" s="126">
+      <c r="H42" s="198">
         <v>43785</v>
       </c>
     </row>
-    <row r="42" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-      <c r="B42" s="121"/>
-      <c r="C42" s="122"/>
-      <c r="D42" s="122" t="s">
+    <row r="43" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="117"/>
+      <c r="C43" s="118"/>
+      <c r="D43" s="194" t="s">
         <v>405</v>
       </c>
-      <c r="E42" s="127" t="s">
+      <c r="E43" s="200" t="s">
         <v>406</v>
       </c>
-      <c r="F42" s="124" t="s">
+      <c r="F43" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G42" s="125">
+      <c r="G43" s="197">
         <v>43208</v>
       </c>
-      <c r="H42" s="126">
+      <c r="H43" s="198">
         <v>43208</v>
       </c>
     </row>
-    <row r="43" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-      <c r="B43" s="121"/>
-      <c r="C43" s="122"/>
-      <c r="D43" s="122" t="s">
+    <row r="44" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="117"/>
+      <c r="C44" s="118"/>
+      <c r="D44" s="194" t="s">
         <v>407</v>
       </c>
-      <c r="E43" s="127" t="s">
+      <c r="E44" s="200" t="s">
         <v>408</v>
       </c>
-      <c r="F43" s="124" t="s">
+      <c r="F44" s="196" t="s">
         <v>232</v>
       </c>
-      <c r="G43" s="125">
+      <c r="G44" s="197">
         <v>43181</v>
       </c>
-      <c r="H43" s="126">
+      <c r="H44" s="198">
         <v>43181</v>
       </c>
     </row>
-    <row r="44" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-      <c r="B44" s="121"/>
-      <c r="C44" s="122"/>
-      <c r="D44" s="122" t="s">
+    <row r="45" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="117"/>
+      <c r="C45" s="118"/>
+      <c r="D45" s="194" t="s">
         <v>409</v>
       </c>
-      <c r="E44" s="127" t="s">
+      <c r="E45" s="200" t="s">
         <v>410</v>
       </c>
-      <c r="F44" s="124" t="s">
+      <c r="F45" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="G44" s="125">
+      <c r="G45" s="197">
         <v>44958</v>
       </c>
-      <c r="H44" s="126">
+      <c r="H45" s="198">
         <v>43181</v>
       </c>
     </row>
-    <row r="45" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="121"/>
-      <c r="C45" s="122"/>
-      <c r="D45" s="122" t="s">
+    <row r="46" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="117"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="194" t="s">
         <v>411</v>
       </c>
-      <c r="E45" s="127" t="s">
+      <c r="E46" s="200" t="s">
         <v>412</v>
       </c>
-      <c r="F45" s="124" t="s">
+      <c r="F46" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="G45" s="125">
+      <c r="G46" s="197">
         <v>44958</v>
       </c>
-      <c r="H45" s="126">
+      <c r="H46" s="198">
         <v>43181</v>
       </c>
     </row>
-    <row r="46" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-      <c r="B46" s="121"/>
-      <c r="C46" s="122"/>
-      <c r="D46" s="122" t="s">
+    <row r="47" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="117"/>
+      <c r="C47" s="118"/>
+      <c r="D47" s="194" t="s">
         <v>413</v>
       </c>
-      <c r="E46" s="127" t="s">
+      <c r="E47" s="200" t="s">
         <v>414</v>
       </c>
-      <c r="F46" s="124" t="s">
+      <c r="F47" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="G46" s="125">
+      <c r="G47" s="197">
         <v>44958</v>
       </c>
-      <c r="H46" s="126">
+      <c r="H47" s="198">
         <v>43922</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-      <c r="B47" s="121"/>
-      <c r="C47" s="122"/>
-      <c r="D47" s="122"/>
-      <c r="E47" s="127"/>
-      <c r="F47" s="124"/>
-      <c r="G47" s="125"/>
-      <c r="H47" s="126"/>
     </row>
     <row r="48" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
-      <c r="B48" s="121"/>
-      <c r="C48" s="122"/>
-      <c r="D48" s="122"/>
-      <c r="E48" s="127"/>
-      <c r="F48" s="124"/>
-      <c r="G48" s="125"/>
-      <c r="H48" s="126"/>
+      <c r="B48" s="117"/>
+      <c r="C48" s="118"/>
+      <c r="D48" s="118"/>
+      <c r="E48" s="123"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="121"/>
+      <c r="H48" s="122"/>
     </row>
     <row r="49" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
-      <c r="B49" s="121"/>
-      <c r="C49" s="122"/>
-      <c r="D49" s="122"/>
-      <c r="E49" s="127"/>
-      <c r="F49" s="124"/>
-      <c r="G49" s="125"/>
-      <c r="H49" s="126"/>
+      <c r="B49" s="117"/>
+      <c r="C49" s="118"/>
+      <c r="D49" s="118"/>
+      <c r="E49" s="123"/>
+      <c r="F49" s="120"/>
+      <c r="G49" s="121"/>
+      <c r="H49" s="122"/>
     </row>
     <row r="50" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
-      <c r="B50" s="121"/>
-      <c r="C50" s="122"/>
-      <c r="D50" s="122"/>
-      <c r="E50" s="127"/>
-      <c r="F50" s="124"/>
-      <c r="G50" s="125"/>
-      <c r="H50" s="126"/>
+      <c r="B50" s="117"/>
+      <c r="C50" s="118"/>
+      <c r="D50" s="118"/>
+      <c r="E50" s="123"/>
+      <c r="F50" s="120"/>
+      <c r="G50" s="121"/>
+      <c r="H50" s="122"/>
     </row>
     <row r="51" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
-      <c r="B51" s="121"/>
-      <c r="C51" s="122"/>
-      <c r="D51" s="122"/>
-      <c r="E51" s="127"/>
-      <c r="F51" s="124"/>
-      <c r="G51" s="125"/>
-      <c r="H51" s="126"/>
+      <c r="B51" s="117"/>
+      <c r="C51" s="118"/>
+      <c r="D51" s="118"/>
+      <c r="E51" s="123"/>
+      <c r="F51" s="120"/>
+      <c r="G51" s="121"/>
+      <c r="H51" s="122"/>
     </row>
     <row r="52" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
-      <c r="B52" s="121"/>
-      <c r="C52" s="122"/>
-      <c r="D52" s="122"/>
+      <c r="B52" s="117"/>
+      <c r="C52" s="118"/>
+      <c r="D52" s="118"/>
       <c r="E52" s="123"/>
-      <c r="F52" s="124"/>
-      <c r="G52" s="125"/>
-      <c r="H52" s="126"/>
+      <c r="F52" s="120"/>
+      <c r="G52" s="121"/>
+      <c r="H52" s="122"/>
     </row>
     <row r="53" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
-      <c r="B53" s="121"/>
-      <c r="C53" s="122"/>
-      <c r="D53" s="122" t="s">
-        <v>286</v>
-      </c>
-      <c r="E53" s="123" t="s">
-        <v>287</v>
-      </c>
-      <c r="F53" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G53" s="125">
-        <v>44949</v>
-      </c>
-      <c r="H53" s="126">
-        <v>44949</v>
-      </c>
+      <c r="B53" s="117"/>
+      <c r="C53" s="118"/>
+      <c r="D53" s="118"/>
+      <c r="E53" s="119"/>
+      <c r="F53" s="120"/>
+      <c r="G53" s="121"/>
+      <c r="H53" s="122"/>
     </row>
     <row r="54" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
-      <c r="B54" s="121"/>
-      <c r="C54" s="122"/>
-      <c r="D54" s="122"/>
-      <c r="E54" s="123"/>
-      <c r="F54" s="124"/>
-      <c r="G54" s="125"/>
-      <c r="H54" s="126"/>
+      <c r="B54" s="117"/>
+      <c r="C54" s="118"/>
+      <c r="D54" s="118" t="s">
+        <v>286</v>
+      </c>
+      <c r="E54" s="119" t="s">
+        <v>287</v>
+      </c>
+      <c r="F54" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G54" s="121">
+        <v>44949</v>
+      </c>
+      <c r="H54" s="122">
+        <v>44949</v>
+      </c>
     </row>
     <row r="55" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
-      <c r="B55" s="121"/>
-      <c r="C55" s="122"/>
-      <c r="D55" s="122"/>
-      <c r="E55" s="123"/>
-      <c r="F55" s="124"/>
-      <c r="G55" s="125"/>
-      <c r="H55" s="126"/>
+      <c r="B55" s="117"/>
+      <c r="C55" s="118"/>
+      <c r="D55" s="118"/>
+      <c r="E55" s="119"/>
+      <c r="F55" s="120"/>
+      <c r="G55" s="121"/>
+      <c r="H55" s="122"/>
     </row>
     <row r="56" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
-      <c r="B56" s="121"/>
-      <c r="C56" s="122"/>
-      <c r="D56" s="122"/>
-      <c r="E56" s="123"/>
-      <c r="F56" s="124"/>
-      <c r="G56" s="125"/>
-      <c r="H56" s="126"/>
+      <c r="B56" s="117"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="119"/>
+      <c r="F56" s="120"/>
+      <c r="G56" s="121"/>
+      <c r="H56" s="122"/>
     </row>
     <row r="57" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
-      <c r="B57" s="121"/>
-      <c r="C57" s="122"/>
-      <c r="D57" s="122"/>
-      <c r="E57" s="127"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="125"/>
-      <c r="H57" s="126"/>
+      <c r="B57" s="117"/>
+      <c r="C57" s="118"/>
+      <c r="D57" s="118"/>
+      <c r="E57" s="119"/>
+      <c r="F57" s="120"/>
+      <c r="G57" s="121"/>
+      <c r="H57" s="122"/>
     </row>
     <row r="58" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
-      <c r="B58" s="121"/>
-      <c r="C58" s="122"/>
-      <c r="D58" s="122"/>
+      <c r="B58" s="117"/>
+      <c r="C58" s="118"/>
+      <c r="D58" s="118"/>
       <c r="E58" s="123"/>
-      <c r="F58" s="124"/>
-      <c r="G58" s="125"/>
-      <c r="H58" s="126"/>
-    </row>
-    <row r="59" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F58" s="120"/>
+      <c r="G58" s="121"/>
+      <c r="H58" s="122"/>
+    </row>
+    <row r="59" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
-      <c r="B59" s="121"/>
-      <c r="C59" s="122" t="s">
-        <v>336</v>
-      </c>
-      <c r="D59" s="122" t="s">
-        <v>326</v>
-      </c>
-      <c r="E59" s="127" t="s">
-        <v>327</v>
-      </c>
-      <c r="F59" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G59" s="125">
-        <v>44902</v>
-      </c>
-      <c r="H59" s="126">
-        <v>44902</v>
-      </c>
+      <c r="B59" s="117"/>
+      <c r="C59" s="118"/>
+      <c r="D59" s="118"/>
+      <c r="E59" s="119"/>
+      <c r="F59" s="120"/>
+      <c r="G59" s="121"/>
+      <c r="H59" s="122"/>
     </row>
     <row r="60" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
-      <c r="B60" s="121"/>
-      <c r="C60" s="122"/>
-      <c r="D60" s="122" t="s">
-        <v>332</v>
-      </c>
-      <c r="E60" s="127" t="s">
-        <v>333</v>
-      </c>
-      <c r="F60" s="124" t="s">
+      <c r="B60" s="117"/>
+      <c r="C60" s="118" t="s">
+        <v>336</v>
+      </c>
+      <c r="D60" s="118" t="s">
+        <v>326</v>
+      </c>
+      <c r="E60" s="123" t="s">
+        <v>327</v>
+      </c>
+      <c r="F60" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="G60" s="125">
-        <v>44897</v>
-      </c>
-      <c r="H60" s="126">
-        <v>44897</v>
+      <c r="G60" s="121">
+        <v>44902</v>
+      </c>
+      <c r="H60" s="122">
+        <v>44902</v>
       </c>
     </row>
     <row r="61" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
-      <c r="B61" s="121"/>
-      <c r="C61" s="122"/>
-      <c r="D61" s="122" t="s">
-        <v>323</v>
-      </c>
-      <c r="E61" s="127" t="s">
-        <v>324</v>
-      </c>
-      <c r="F61" s="124" t="s">
+      <c r="B61" s="117"/>
+      <c r="C61" s="118"/>
+      <c r="D61" s="118" t="s">
+        <v>332</v>
+      </c>
+      <c r="E61" s="123" t="s">
+        <v>333</v>
+      </c>
+      <c r="F61" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="G61" s="125">
-        <v>44951</v>
-      </c>
-      <c r="H61" s="126">
-        <v>44951</v>
+      <c r="G61" s="121">
+        <v>44897</v>
+      </c>
+      <c r="H61" s="122">
+        <v>44897</v>
       </c>
     </row>
     <row r="62" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
-      <c r="B62" s="121"/>
-      <c r="C62" s="122"/>
-      <c r="D62" s="122" t="s">
-        <v>338</v>
-      </c>
-      <c r="E62" s="127" t="s">
-        <v>337</v>
-      </c>
-      <c r="F62" s="124" t="s">
+      <c r="B62" s="117"/>
+      <c r="C62" s="118"/>
+      <c r="D62" s="118" t="s">
+        <v>323</v>
+      </c>
+      <c r="E62" s="123" t="s">
+        <v>324</v>
+      </c>
+      <c r="F62" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="G62" s="125">
+      <c r="G62" s="121">
         <v>44951</v>
       </c>
-      <c r="H62" s="126">
+      <c r="H62" s="122">
         <v>44951</v>
       </c>
     </row>
     <row r="63" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
-      <c r="B63" s="121"/>
-      <c r="C63" s="122"/>
-      <c r="D63" s="122" t="s">
+      <c r="B63" s="117"/>
+      <c r="C63" s="118"/>
+      <c r="D63" s="118" t="s">
+        <v>338</v>
+      </c>
+      <c r="E63" s="123" t="s">
+        <v>337</v>
+      </c>
+      <c r="F63" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G63" s="121">
+        <v>44951</v>
+      </c>
+      <c r="H63" s="122">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="117"/>
+      <c r="C64" s="118"/>
+      <c r="D64" s="118" t="s">
         <v>321</v>
       </c>
-      <c r="E63" s="127" t="s">
+      <c r="E64" s="123" t="s">
         <v>325</v>
       </c>
-      <c r="F63" s="124" t="s">
+      <c r="F64" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="G63" s="125">
+      <c r="G64" s="121">
         <v>44900</v>
       </c>
-      <c r="H63" s="126">
+      <c r="H64" s="122">
         <v>44949</v>
       </c>
     </row>
-    <row r="64" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-      <c r="B64" s="121"/>
-      <c r="C64" s="122"/>
-      <c r="D64" s="122" t="s">
+    <row r="65" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A65" s="1"/>
+      <c r="B65" s="117"/>
+      <c r="C65" s="118"/>
+      <c r="D65" s="118" t="s">
         <v>328</v>
       </c>
-      <c r="E64" s="123" t="s">
+      <c r="E65" s="119" t="s">
         <v>329</v>
       </c>
-      <c r="F64" s="124" t="s">
+      <c r="F65" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="G64" s="125">
+      <c r="G65" s="121">
         <v>44896</v>
       </c>
-      <c r="H64" s="126">
+      <c r="H65" s="122">
         <v>44896</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
-      <c r="B65" s="121"/>
-      <c r="C65" s="122"/>
-      <c r="D65" s="122" t="s">
-        <v>322</v>
-      </c>
-      <c r="E65" s="127" t="s">
-        <v>339</v>
-      </c>
-      <c r="F65" s="124" t="s">
-        <v>281</v>
-      </c>
-      <c r="G65" s="125">
-        <v>44945</v>
-      </c>
-      <c r="H65" s="126">
-        <v>44949</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A66" s="1"/>
-      <c r="B66" s="121"/>
-      <c r="C66" s="122"/>
-      <c r="D66" s="122" t="s">
-        <v>334</v>
-      </c>
-      <c r="E66" s="127" t="s">
-        <v>335</v>
-      </c>
-      <c r="F66" s="124" t="s">
+      <c r="B66" s="117"/>
+      <c r="C66" s="118"/>
+      <c r="D66" s="118" t="s">
+        <v>322</v>
+      </c>
+      <c r="E66" s="123" t="s">
+        <v>339</v>
+      </c>
+      <c r="F66" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="G66" s="125">
-        <v>44910</v>
-      </c>
-      <c r="H66" s="126">
-        <v>44910</v>
+      <c r="G66" s="121">
+        <v>44945</v>
+      </c>
+      <c r="H66" s="122">
+        <v>44949</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
-      <c r="B67" s="121"/>
-      <c r="C67" s="122"/>
-      <c r="D67" s="122" t="s">
-        <v>340</v>
-      </c>
-      <c r="E67" s="127" t="s">
-        <v>341</v>
-      </c>
-      <c r="F67" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G67" s="125">
-        <v>44951</v>
-      </c>
-      <c r="H67" s="126">
-        <v>44951</v>
+      <c r="B67" s="117"/>
+      <c r="C67" s="118"/>
+      <c r="D67" s="118" t="s">
+        <v>334</v>
+      </c>
+      <c r="E67" s="123" t="s">
+        <v>335</v>
+      </c>
+      <c r="F67" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="G67" s="121">
+        <v>44910</v>
+      </c>
+      <c r="H67" s="122">
+        <v>44910</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
-      <c r="B68" s="121"/>
-      <c r="C68" s="122"/>
-      <c r="D68" s="122" t="s">
+      <c r="B68" s="117"/>
+      <c r="C68" s="118"/>
+      <c r="D68" s="118" t="s">
+        <v>340</v>
+      </c>
+      <c r="E68" s="123" t="s">
+        <v>341</v>
+      </c>
+      <c r="F68" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G68" s="121">
+        <v>44951</v>
+      </c>
+      <c r="H68" s="122">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="117"/>
+      <c r="C69" s="118"/>
+      <c r="D69" s="118" t="s">
         <v>342</v>
       </c>
-      <c r="E68" s="127" t="s">
+      <c r="E69" s="123" t="s">
         <v>343</v>
       </c>
-      <c r="F68" s="124" t="s">
+      <c r="F69" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="G68" s="125">
+      <c r="G69" s="121">
         <v>44952</v>
       </c>
-      <c r="H68" s="126">
+      <c r="H69" s="122">
         <v>44952</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
-      <c r="B69" s="121"/>
-      <c r="C69" s="122"/>
-      <c r="D69" s="122"/>
-      <c r="E69" s="123"/>
-      <c r="F69" s="124"/>
-      <c r="G69" s="125"/>
-      <c r="H69" s="126"/>
     </row>
     <row r="70" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="B70" s="121"/>
-      <c r="C70" s="122"/>
-      <c r="D70" s="122"/>
-      <c r="E70" s="123"/>
-      <c r="F70" s="124"/>
-      <c r="G70" s="125"/>
-      <c r="H70" s="126"/>
+      <c r="B70" s="117"/>
+      <c r="C70" s="118"/>
+      <c r="D70" s="118"/>
+      <c r="E70" s="119"/>
+      <c r="F70" s="120"/>
+      <c r="G70" s="121"/>
+      <c r="H70" s="122"/>
     </row>
     <row r="71" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
-      <c r="B71" s="121"/>
-      <c r="C71" s="122"/>
-      <c r="D71" s="122"/>
-      <c r="E71" s="123"/>
-      <c r="F71" s="124"/>
-      <c r="G71" s="125"/>
-      <c r="H71" s="126"/>
-    </row>
-    <row r="72" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B71" s="117"/>
+      <c r="C71" s="118"/>
+      <c r="D71" s="118"/>
+      <c r="E71" s="119"/>
+      <c r="F71" s="120"/>
+      <c r="G71" s="121"/>
+      <c r="H71" s="122"/>
+    </row>
+    <row r="72" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-      <c r="B72" s="121"/>
-      <c r="C72" s="122"/>
-      <c r="D72" s="122" t="s">
-        <v>394</v>
-      </c>
-      <c r="E72" s="127" t="s">
-        <v>395</v>
-      </c>
-      <c r="F72" s="124" t="s">
-        <v>267</v>
-      </c>
-      <c r="G72" s="125">
-        <v>44957</v>
-      </c>
-      <c r="H72" s="126">
-        <v>42982</v>
-      </c>
+      <c r="B72" s="117"/>
+      <c r="C72" s="118"/>
+      <c r="D72" s="118"/>
+      <c r="E72" s="119"/>
+      <c r="F72" s="120"/>
+      <c r="G72" s="121"/>
+      <c r="H72" s="122"/>
     </row>
     <row r="73" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
-      <c r="B73" s="121"/>
-      <c r="C73" s="122"/>
-      <c r="D73" s="122" t="s">
+      <c r="B73" s="117"/>
+      <c r="C73" s="118"/>
+      <c r="D73" s="118" t="s">
+        <v>394</v>
+      </c>
+      <c r="E73" s="123" t="s">
+        <v>395</v>
+      </c>
+      <c r="F73" s="120" t="s">
+        <v>267</v>
+      </c>
+      <c r="G73" s="121">
+        <v>44957</v>
+      </c>
+      <c r="H73" s="122">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A74" s="1"/>
+      <c r="B74" s="117"/>
+      <c r="C74" s="118"/>
+      <c r="D74" s="118" t="s">
         <v>393</v>
       </c>
-      <c r="E73" s="127" t="s">
+      <c r="E74" s="123" t="s">
         <v>396</v>
       </c>
-      <c r="F73" s="124" t="s">
+      <c r="F74" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="G73" s="125">
+      <c r="G74" s="121">
         <v>44281</v>
       </c>
-      <c r="H73" s="126">
+      <c r="H74" s="122">
         <v>44557</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="B74" s="121"/>
-      <c r="C74" s="122"/>
-      <c r="D74" s="122" t="s">
-        <v>397</v>
-      </c>
-      <c r="E74" s="127" t="s">
-        <v>398</v>
-      </c>
-      <c r="F74" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G74" s="125">
-        <v>43257</v>
-      </c>
-      <c r="H74" s="126">
-        <v>43257</v>
       </c>
     </row>
     <row r="75" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
-      <c r="B75" s="121"/>
-      <c r="C75" s="122"/>
-      <c r="D75" s="122" t="s">
+      <c r="B75" s="117"/>
+      <c r="C75" s="118"/>
+      <c r="D75" s="118" t="s">
+        <v>397</v>
+      </c>
+      <c r="E75" s="123" t="s">
+        <v>398</v>
+      </c>
+      <c r="F75" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G75" s="121">
+        <v>43257</v>
+      </c>
+      <c r="H75" s="122">
+        <v>43257</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1"/>
+      <c r="B76" s="117"/>
+      <c r="C76" s="118"/>
+      <c r="D76" s="118" t="s">
         <v>286</v>
       </c>
-      <c r="E75" s="127" t="s">
+      <c r="E76" s="123" t="s">
         <v>399</v>
       </c>
-      <c r="F75" s="124" t="s">
+      <c r="F76" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="G75" s="125">
+      <c r="G76" s="121">
         <v>44949</v>
       </c>
-      <c r="H75" s="126">
+      <c r="H76" s="122">
         <v>44949</v>
       </c>
     </row>
-    <row r="76" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-      <c r="B76" s="121"/>
-      <c r="C76" s="122"/>
-      <c r="D76" s="122"/>
-      <c r="E76" s="127"/>
-      <c r="F76" s="124"/>
-      <c r="G76" s="125"/>
-      <c r="H76" s="126"/>
-    </row>
-    <row r="77" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
-      <c r="B77" s="121"/>
-      <c r="C77" s="122"/>
-      <c r="D77" s="122" t="s">
+      <c r="B77" s="117"/>
+      <c r="C77" s="118"/>
+      <c r="D77" s="118"/>
+      <c r="E77" s="123"/>
+      <c r="F77" s="120"/>
+      <c r="G77" s="121"/>
+      <c r="H77" s="122"/>
+    </row>
+    <row r="78" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1"/>
+      <c r="B78" s="117"/>
+      <c r="C78" s="118"/>
+      <c r="D78" s="118" t="s">
         <v>392</v>
       </c>
-      <c r="E77" s="127" t="s">
+      <c r="E78" s="123" t="s">
         <v>400</v>
       </c>
-      <c r="F77" s="124" t="s">
+      <c r="F78" s="120" t="s">
         <v>232</v>
       </c>
-      <c r="G77" s="125">
+      <c r="G78" s="121">
         <v>44957</v>
       </c>
-      <c r="H77" s="126">
+      <c r="H78" s="122">
         <v>44957</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="1"/>
-      <c r="B78" s="121"/>
-      <c r="C78" s="122"/>
-      <c r="D78" s="122"/>
-      <c r="E78" s="127"/>
-      <c r="F78" s="124"/>
-      <c r="G78" s="125"/>
-      <c r="H78" s="126"/>
     </row>
     <row r="79" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
-      <c r="B79" s="121"/>
-      <c r="C79" s="122"/>
-      <c r="D79" s="122"/>
+      <c r="B79" s="117"/>
+      <c r="C79" s="118"/>
+      <c r="D79" s="118"/>
       <c r="E79" s="123"/>
-      <c r="F79" s="124"/>
-      <c r="G79" s="125"/>
-      <c r="H79" s="126"/>
+      <c r="F79" s="120"/>
+      <c r="G79" s="121"/>
+      <c r="H79" s="122"/>
     </row>
     <row r="80" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
-      <c r="B80" s="121"/>
-      <c r="C80" s="122"/>
-      <c r="D80" s="122" t="s">
-        <v>330</v>
-      </c>
-      <c r="E80" s="123" t="s">
-        <v>331</v>
-      </c>
-      <c r="F80" s="124" t="s">
-        <v>232</v>
-      </c>
-      <c r="G80" s="125">
-        <v>44893</v>
-      </c>
-      <c r="H80" s="126">
-        <v>44893</v>
-      </c>
+      <c r="B80" s="117"/>
+      <c r="C80" s="118"/>
+      <c r="D80" s="118"/>
+      <c r="E80" s="119"/>
+      <c r="F80" s="120"/>
+      <c r="G80" s="121"/>
+      <c r="H80" s="122"/>
     </row>
     <row r="81" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
-      <c r="B81" s="121"/>
-      <c r="C81" s="122"/>
-      <c r="D81" s="122"/>
-      <c r="E81" s="123"/>
-      <c r="F81" s="124"/>
-      <c r="G81" s="125"/>
-      <c r="H81" s="126"/>
+      <c r="B81" s="117"/>
+      <c r="C81" s="118"/>
+      <c r="D81" s="118" t="s">
+        <v>330</v>
+      </c>
+      <c r="E81" s="119" t="s">
+        <v>331</v>
+      </c>
+      <c r="F81" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G81" s="121">
+        <v>44893</v>
+      </c>
+      <c r="H81" s="122">
+        <v>44893</v>
+      </c>
     </row>
     <row r="82" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
-      <c r="B82" s="121"/>
-      <c r="C82" s="122"/>
-      <c r="D82" s="122"/>
-      <c r="E82" s="123"/>
-      <c r="F82" s="124"/>
-      <c r="G82" s="125"/>
-      <c r="H82" s="126"/>
+      <c r="B82" s="117"/>
+      <c r="C82" s="118"/>
+      <c r="D82" s="118"/>
+      <c r="E82" s="119"/>
+      <c r="F82" s="120"/>
+      <c r="G82" s="121"/>
+      <c r="H82" s="122"/>
     </row>
     <row r="83" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
-      <c r="B83" s="121"/>
-      <c r="C83" s="122"/>
-      <c r="D83" s="122"/>
-      <c r="E83" s="123"/>
-      <c r="F83" s="124"/>
-      <c r="G83" s="125"/>
-      <c r="H83" s="126"/>
+      <c r="B83" s="117"/>
+      <c r="C83" s="118"/>
+      <c r="D83" s="118"/>
+      <c r="E83" s="119"/>
+      <c r="F83" s="120"/>
+      <c r="G83" s="121"/>
+      <c r="H83" s="122"/>
     </row>
     <row r="84" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
-      <c r="B84" s="121"/>
-      <c r="C84" s="122"/>
-      <c r="D84" s="122"/>
-      <c r="E84" s="123"/>
-      <c r="F84" s="124"/>
-      <c r="G84" s="125"/>
-      <c r="H84" s="126"/>
+      <c r="B84" s="117"/>
+      <c r="C84" s="118"/>
+      <c r="D84" s="118"/>
+      <c r="E84" s="119"/>
+      <c r="F84" s="120"/>
+      <c r="G84" s="121"/>
+      <c r="H84" s="122"/>
     </row>
     <row r="85" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
-      <c r="B85" s="121"/>
-      <c r="C85" s="122"/>
-      <c r="D85" s="122"/>
-      <c r="E85" s="123"/>
-      <c r="F85" s="124"/>
-      <c r="G85" s="125"/>
-      <c r="H85" s="126"/>
+      <c r="B85" s="117"/>
+      <c r="C85" s="118"/>
+      <c r="D85" s="118"/>
+      <c r="E85" s="119"/>
+      <c r="F85" s="120"/>
+      <c r="G85" s="121"/>
+      <c r="H85" s="122"/>
     </row>
     <row r="86" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
-      <c r="B86" s="121"/>
-      <c r="C86" s="122"/>
-      <c r="D86" s="122"/>
-      <c r="E86" s="123"/>
-      <c r="F86" s="124"/>
-      <c r="G86" s="125"/>
-      <c r="H86" s="126"/>
+      <c r="B86" s="117"/>
+      <c r="C86" s="118"/>
+      <c r="D86" s="118"/>
+      <c r="E86" s="119"/>
+      <c r="F86" s="120"/>
+      <c r="G86" s="121"/>
+      <c r="H86" s="122"/>
     </row>
     <row r="87" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
-      <c r="B87" s="121"/>
-      <c r="C87" s="122"/>
-      <c r="D87" s="122"/>
-      <c r="E87" s="123"/>
-      <c r="F87" s="124"/>
-      <c r="G87" s="125"/>
-      <c r="H87" s="126"/>
+      <c r="B87" s="117"/>
+      <c r="C87" s="118"/>
+      <c r="D87" s="118"/>
+      <c r="E87" s="119"/>
+      <c r="F87" s="120"/>
+      <c r="G87" s="121"/>
+      <c r="H87" s="122"/>
     </row>
     <row r="88" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
-      <c r="B88" s="121"/>
-      <c r="C88" s="122"/>
-      <c r="D88" s="122"/>
-      <c r="E88" s="123"/>
-      <c r="F88" s="124"/>
-      <c r="G88" s="125"/>
-      <c r="H88" s="126"/>
+      <c r="B88" s="117"/>
+      <c r="C88" s="118"/>
+      <c r="D88" s="118"/>
+      <c r="E88" s="119"/>
+      <c r="F88" s="120"/>
+      <c r="G88" s="121"/>
+      <c r="H88" s="122"/>
     </row>
     <row r="89" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
-      <c r="B89" s="121"/>
-      <c r="C89" s="122"/>
-      <c r="D89" s="122"/>
-      <c r="E89" s="123"/>
-      <c r="F89" s="124"/>
-      <c r="G89" s="125"/>
-      <c r="H89" s="126"/>
+      <c r="B89" s="117"/>
+      <c r="C89" s="118"/>
+      <c r="D89" s="118"/>
+      <c r="E89" s="119"/>
+      <c r="F89" s="120"/>
+      <c r="G89" s="121"/>
+      <c r="H89" s="122"/>
     </row>
     <row r="90" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
-      <c r="B90" s="121"/>
-      <c r="C90" s="122"/>
-      <c r="D90" s="122"/>
-      <c r="E90" s="123"/>
-      <c r="F90" s="124"/>
-      <c r="G90" s="125"/>
-      <c r="H90" s="126"/>
+      <c r="B90" s="117"/>
+      <c r="C90" s="118"/>
+      <c r="D90" s="118"/>
+      <c r="E90" s="119"/>
+      <c r="F90" s="120"/>
+      <c r="G90" s="121"/>
+      <c r="H90" s="122"/>
     </row>
     <row r="91" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
-      <c r="B91" s="121"/>
-      <c r="C91" s="122"/>
-      <c r="D91" s="122"/>
-      <c r="E91" s="123"/>
-      <c r="F91" s="124"/>
-      <c r="G91" s="125"/>
-      <c r="H91" s="126"/>
+      <c r="B91" s="117"/>
+      <c r="C91" s="118"/>
+      <c r="D91" s="118"/>
+      <c r="E91" s="119"/>
+      <c r="F91" s="120"/>
+      <c r="G91" s="121"/>
+      <c r="H91" s="122"/>
     </row>
     <row r="92" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
-      <c r="B92" s="121"/>
-      <c r="C92" s="122"/>
-      <c r="D92" s="122"/>
-      <c r="E92" s="123"/>
-      <c r="F92" s="124"/>
-      <c r="G92" s="125"/>
-      <c r="H92" s="126"/>
+      <c r="B92" s="117"/>
+      <c r="C92" s="118"/>
+      <c r="D92" s="118"/>
+      <c r="E92" s="119"/>
+      <c r="F92" s="120"/>
+      <c r="G92" s="121"/>
+      <c r="H92" s="122"/>
     </row>
     <row r="93" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
-      <c r="B93" s="121"/>
-      <c r="C93" s="122"/>
-      <c r="D93" s="122"/>
-      <c r="E93" s="123"/>
-      <c r="F93" s="124"/>
-      <c r="G93" s="125"/>
-      <c r="H93" s="126"/>
+      <c r="B93" s="117"/>
+      <c r="C93" s="118"/>
+      <c r="D93" s="118"/>
+      <c r="E93" s="119"/>
+      <c r="F93" s="120"/>
+      <c r="G93" s="121"/>
+      <c r="H93" s="122"/>
     </row>
     <row r="94" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
-      <c r="B94" s="121"/>
-      <c r="C94" s="122"/>
-      <c r="D94" s="122"/>
-      <c r="E94" s="123"/>
-      <c r="F94" s="124"/>
-      <c r="G94" s="125"/>
-      <c r="H94" s="126"/>
+      <c r="B94" s="117"/>
+      <c r="C94" s="118"/>
+      <c r="D94" s="118"/>
+      <c r="E94" s="119"/>
+      <c r="F94" s="120"/>
+      <c r="G94" s="121"/>
+      <c r="H94" s="122"/>
     </row>
     <row r="95" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
-      <c r="B95" s="121"/>
-      <c r="C95" s="122"/>
-      <c r="D95" s="122"/>
-      <c r="E95" s="123"/>
-      <c r="F95" s="124"/>
-      <c r="G95" s="125"/>
-      <c r="H95" s="126"/>
+      <c r="B95" s="117"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="118"/>
+      <c r="E95" s="119"/>
+      <c r="F95" s="120"/>
+      <c r="G95" s="121"/>
+      <c r="H95" s="122"/>
     </row>
     <row r="96" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
-      <c r="B96" s="121"/>
-      <c r="C96" s="122"/>
-      <c r="D96" s="122"/>
-      <c r="E96" s="123"/>
-      <c r="F96" s="124"/>
-      <c r="G96" s="125"/>
-      <c r="H96" s="126"/>
+      <c r="B96" s="117"/>
+      <c r="C96" s="118"/>
+      <c r="D96" s="118"/>
+      <c r="E96" s="119"/>
+      <c r="F96" s="120"/>
+      <c r="G96" s="121"/>
+      <c r="H96" s="122"/>
     </row>
     <row r="97" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
-      <c r="B97" s="121"/>
-      <c r="C97" s="122"/>
-      <c r="D97" s="122"/>
-      <c r="E97" s="123"/>
-      <c r="F97" s="124"/>
-      <c r="G97" s="125"/>
-      <c r="H97" s="126"/>
+      <c r="B97" s="117"/>
+      <c r="C97" s="118"/>
+      <c r="D97" s="118"/>
+      <c r="E97" s="119"/>
+      <c r="F97" s="120"/>
+      <c r="G97" s="121"/>
+      <c r="H97" s="122"/>
     </row>
     <row r="98" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
-      <c r="B98" s="121"/>
-      <c r="C98" s="122"/>
-      <c r="D98" s="122"/>
-      <c r="E98" s="123"/>
-      <c r="F98" s="124"/>
-      <c r="G98" s="125"/>
-      <c r="H98" s="126"/>
+      <c r="B98" s="117"/>
+      <c r="C98" s="118"/>
+      <c r="D98" s="118"/>
+      <c r="E98" s="119"/>
+      <c r="F98" s="120"/>
+      <c r="G98" s="121"/>
+      <c r="H98" s="122"/>
     </row>
     <row r="99" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
-      <c r="B99" s="121"/>
-      <c r="C99" s="122"/>
-      <c r="D99" s="122"/>
-      <c r="E99" s="123"/>
-      <c r="F99" s="124"/>
-      <c r="G99" s="125"/>
-      <c r="H99" s="126"/>
+      <c r="B99" s="117"/>
+      <c r="C99" s="118"/>
+      <c r="D99" s="118"/>
+      <c r="E99" s="119"/>
+      <c r="F99" s="120"/>
+      <c r="G99" s="121"/>
+      <c r="H99" s="122"/>
     </row>
     <row r="100" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
-      <c r="B100" s="121"/>
-      <c r="C100" s="122"/>
-      <c r="D100" s="122"/>
-      <c r="E100" s="123"/>
-      <c r="F100" s="124"/>
-      <c r="G100" s="125"/>
-      <c r="H100" s="126"/>
+      <c r="B100" s="117"/>
+      <c r="C100" s="118"/>
+      <c r="D100" s="118"/>
+      <c r="E100" s="119"/>
+      <c r="F100" s="120"/>
+      <c r="G100" s="121"/>
+      <c r="H100" s="122"/>
     </row>
     <row r="101" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
-      <c r="B101" s="121"/>
-      <c r="C101" s="122"/>
-      <c r="D101" s="122"/>
-      <c r="E101" s="123"/>
-      <c r="F101" s="124"/>
-      <c r="G101" s="125"/>
-      <c r="H101" s="126"/>
+      <c r="B101" s="117"/>
+      <c r="C101" s="118"/>
+      <c r="D101" s="118"/>
+      <c r="E101" s="119"/>
+      <c r="F101" s="120"/>
+      <c r="G101" s="121"/>
+      <c r="H101" s="122"/>
     </row>
     <row r="102" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
-      <c r="B102" s="121"/>
-      <c r="C102" s="122"/>
-      <c r="D102" s="122"/>
-      <c r="E102" s="123"/>
-      <c r="F102" s="124"/>
-      <c r="G102" s="125"/>
-      <c r="H102" s="126"/>
+      <c r="B102" s="117"/>
+      <c r="C102" s="118"/>
+      <c r="D102" s="118"/>
+      <c r="E102" s="119"/>
+      <c r="F102" s="120"/>
+      <c r="G102" s="121"/>
+      <c r="H102" s="122"/>
     </row>
     <row r="103" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
-      <c r="B103" s="121"/>
-      <c r="C103" s="122"/>
-      <c r="D103" s="122"/>
-      <c r="E103" s="123"/>
-      <c r="F103" s="124"/>
-      <c r="G103" s="125"/>
-      <c r="H103" s="126"/>
+      <c r="B103" s="117"/>
+      <c r="C103" s="118"/>
+      <c r="D103" s="118"/>
+      <c r="E103" s="119"/>
+      <c r="F103" s="120"/>
+      <c r="G103" s="121"/>
+      <c r="H103" s="122"/>
     </row>
     <row r="104" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
-      <c r="B104" s="121"/>
-      <c r="C104" s="122"/>
-      <c r="D104" s="122"/>
-      <c r="E104" s="123"/>
-      <c r="F104" s="124"/>
-      <c r="G104" s="125"/>
-      <c r="H104" s="126"/>
+      <c r="B104" s="117"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="118"/>
+      <c r="E104" s="119"/>
+      <c r="F104" s="120"/>
+      <c r="G104" s="121"/>
+      <c r="H104" s="122"/>
     </row>
     <row r="105" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
-      <c r="B105" s="121"/>
-      <c r="C105" s="122"/>
-      <c r="D105" s="122"/>
-      <c r="E105" s="123"/>
-      <c r="F105" s="124"/>
-      <c r="G105" s="125"/>
-      <c r="H105" s="126"/>
+      <c r="B105" s="117"/>
+      <c r="C105" s="118"/>
+      <c r="D105" s="118"/>
+      <c r="E105" s="119"/>
+      <c r="F105" s="120"/>
+      <c r="G105" s="121"/>
+      <c r="H105" s="122"/>
     </row>
     <row r="106" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A106" s="1"/>
-      <c r="B106" s="121"/>
-      <c r="C106" s="122"/>
-      <c r="D106" s="122"/>
-      <c r="E106" s="123"/>
-      <c r="F106" s="124"/>
-      <c r="G106" s="125"/>
-      <c r="H106" s="126"/>
+      <c r="B106" s="117"/>
+      <c r="C106" s="118"/>
+      <c r="D106" s="118"/>
+      <c r="E106" s="119"/>
+      <c r="F106" s="120"/>
+      <c r="G106" s="121"/>
+      <c r="H106" s="122"/>
     </row>
     <row r="107" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A107" s="1"/>
-      <c r="B107" s="121"/>
-      <c r="C107" s="122"/>
-      <c r="D107" s="122"/>
-      <c r="E107" s="123"/>
-      <c r="F107" s="124"/>
-      <c r="G107" s="125"/>
-      <c r="H107" s="126"/>
+      <c r="B107" s="117"/>
+      <c r="C107" s="118"/>
+      <c r="D107" s="118"/>
+      <c r="E107" s="119"/>
+      <c r="F107" s="120"/>
+      <c r="G107" s="121"/>
+      <c r="H107" s="122"/>
     </row>
     <row r="108" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A108" s="1"/>
-      <c r="B108" s="121"/>
-      <c r="C108" s="122"/>
-      <c r="D108" s="122"/>
-      <c r="E108" s="123"/>
-      <c r="F108" s="124"/>
-      <c r="G108" s="125"/>
-      <c r="H108" s="126"/>
+      <c r="B108" s="117"/>
+      <c r="C108" s="118"/>
+      <c r="D108" s="118"/>
+      <c r="E108" s="119"/>
+      <c r="F108" s="120"/>
+      <c r="G108" s="121"/>
+      <c r="H108" s="122"/>
     </row>
     <row r="109" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A109" s="1"/>
-      <c r="B109" s="121"/>
-      <c r="C109" s="122"/>
-      <c r="D109" s="122"/>
-      <c r="E109" s="123"/>
-      <c r="F109" s="124"/>
-      <c r="G109" s="125"/>
-      <c r="H109" s="126"/>
+      <c r="B109" s="117"/>
+      <c r="C109" s="118"/>
+      <c r="D109" s="118"/>
+      <c r="E109" s="119"/>
+      <c r="F109" s="120"/>
+      <c r="G109" s="121"/>
+      <c r="H109" s="122"/>
     </row>
     <row r="110" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
-      <c r="B110" s="121"/>
-      <c r="C110" s="122"/>
-      <c r="D110" s="122"/>
-      <c r="E110" s="123"/>
-      <c r="F110" s="124"/>
-      <c r="G110" s="125"/>
-      <c r="H110" s="126"/>
+      <c r="B110" s="117"/>
+      <c r="C110" s="118"/>
+      <c r="D110" s="118"/>
+      <c r="E110" s="119"/>
+      <c r="F110" s="120"/>
+      <c r="G110" s="121"/>
+      <c r="H110" s="122"/>
     </row>
     <row r="111" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A111" s="1"/>
-      <c r="B111" s="121"/>
-      <c r="C111" s="122"/>
-      <c r="D111" s="122"/>
-      <c r="E111" s="123"/>
-      <c r="F111" s="124"/>
-      <c r="G111" s="125"/>
-      <c r="H111" s="126"/>
+      <c r="B111" s="117"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="118"/>
+      <c r="E111" s="119"/>
+      <c r="F111" s="120"/>
+      <c r="G111" s="121"/>
+      <c r="H111" s="122"/>
     </row>
     <row r="112" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A112" s="1"/>
-      <c r="B112" s="121"/>
-      <c r="C112" s="122"/>
-      <c r="D112" s="122"/>
-      <c r="E112" s="123"/>
-      <c r="F112" s="124"/>
-      <c r="G112" s="125"/>
-      <c r="H112" s="126"/>
+      <c r="B112" s="117"/>
+      <c r="C112" s="118"/>
+      <c r="D112" s="118"/>
+      <c r="E112" s="119"/>
+      <c r="F112" s="120"/>
+      <c r="G112" s="121"/>
+      <c r="H112" s="122"/>
     </row>
     <row r="113" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A113" s="1"/>
-      <c r="B113" s="121"/>
-      <c r="C113" s="122"/>
-      <c r="D113" s="122"/>
-      <c r="E113" s="123"/>
-      <c r="F113" s="124"/>
-      <c r="G113" s="125"/>
-      <c r="H113" s="126"/>
+      <c r="B113" s="117"/>
+      <c r="C113" s="118"/>
+      <c r="D113" s="118"/>
+      <c r="E113" s="119"/>
+      <c r="F113" s="120"/>
+      <c r="G113" s="121"/>
+      <c r="H113" s="122"/>
     </row>
     <row r="114" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A114" s="1"/>
-      <c r="B114" s="121"/>
-      <c r="C114" s="122"/>
-      <c r="D114" s="122"/>
-      <c r="E114" s="123"/>
-      <c r="F114" s="124"/>
-      <c r="G114" s="125"/>
-      <c r="H114" s="126"/>
+      <c r="B114" s="117"/>
+      <c r="C114" s="118"/>
+      <c r="D114" s="118"/>
+      <c r="E114" s="119"/>
+      <c r="F114" s="120"/>
+      <c r="G114" s="121"/>
+      <c r="H114" s="122"/>
     </row>
     <row r="115" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A115" s="1"/>
-      <c r="B115" s="121"/>
-      <c r="C115" s="122"/>
-      <c r="D115" s="122"/>
-      <c r="E115" s="123"/>
-      <c r="F115" s="124"/>
-      <c r="G115" s="125"/>
-      <c r="H115" s="126"/>
+      <c r="B115" s="117"/>
+      <c r="C115" s="118"/>
+      <c r="D115" s="118"/>
+      <c r="E115" s="119"/>
+      <c r="F115" s="120"/>
+      <c r="G115" s="121"/>
+      <c r="H115" s="122"/>
     </row>
     <row r="116" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A116" s="1"/>
-      <c r="B116" s="121"/>
-      <c r="C116" s="122"/>
-      <c r="D116" s="122"/>
-      <c r="E116" s="123"/>
-      <c r="F116" s="124"/>
-      <c r="G116" s="125"/>
-      <c r="H116" s="126"/>
-    </row>
-    <row r="117" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="117"/>
+      <c r="C116" s="118"/>
+      <c r="D116" s="118"/>
+      <c r="E116" s="119"/>
+      <c r="F116" s="120"/>
+      <c r="G116" s="121"/>
+      <c r="H116" s="122"/>
+    </row>
+    <row r="117" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
-      <c r="B117" s="134"/>
-      <c r="C117" s="135"/>
-      <c r="D117" s="135"/>
-      <c r="E117" s="136"/>
-      <c r="F117" s="137"/>
-      <c r="G117" s="138"/>
-      <c r="H117" s="139"/>
-    </row>
-    <row r="118" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B117" s="117"/>
+      <c r="C117" s="118"/>
+      <c r="D117" s="118"/>
+      <c r="E117" s="119"/>
+      <c r="F117" s="120"/>
+      <c r="G117" s="121"/>
+      <c r="H117" s="122"/>
+    </row>
+    <row r="118" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A118" s="1"/>
-      <c r="B118" s="1"/>
-      <c r="C118" s="1"/>
-      <c r="D118" s="1"/>
-      <c r="E118" s="1"/>
-      <c r="F118" s="140"/>
-      <c r="G118" s="141"/>
-      <c r="H118" s="141"/>
+      <c r="B118" s="128"/>
+      <c r="C118" s="129"/>
+      <c r="D118" s="129"/>
+      <c r="E118" s="130"/>
+      <c r="F118" s="131"/>
+      <c r="G118" s="132"/>
+      <c r="H118" s="133"/>
     </row>
     <row r="119" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
@@ -4697,9 +4736,9 @@
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
-      <c r="F119" s="140"/>
-      <c r="G119" s="141"/>
-      <c r="H119" s="141"/>
+      <c r="F119" s="134"/>
+      <c r="G119" s="135"/>
+      <c r="H119" s="135"/>
     </row>
     <row r="120" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
@@ -4707,9 +4746,9 @@
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
-      <c r="F120" s="140"/>
-      <c r="G120" s="141"/>
-      <c r="H120" s="141"/>
+      <c r="F120" s="134"/>
+      <c r="G120" s="135"/>
+      <c r="H120" s="135"/>
     </row>
     <row r="121" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
@@ -4717,9 +4756,9 @@
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
-      <c r="F121" s="140"/>
-      <c r="G121" s="141"/>
-      <c r="H121" s="141"/>
+      <c r="F121" s="134"/>
+      <c r="G121" s="135"/>
+      <c r="H121" s="135"/>
     </row>
     <row r="122" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
@@ -4727,9 +4766,9 @@
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
-      <c r="F122" s="140"/>
-      <c r="G122" s="141"/>
-      <c r="H122" s="141"/>
+      <c r="F122" s="134"/>
+      <c r="G122" s="135"/>
+      <c r="H122" s="135"/>
     </row>
     <row r="123" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
@@ -4737,9 +4776,9 @@
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
-      <c r="F123" s="140"/>
-      <c r="G123" s="141"/>
-      <c r="H123" s="141"/>
+      <c r="F123" s="134"/>
+      <c r="G123" s="135"/>
+      <c r="H123" s="135"/>
     </row>
     <row r="124" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
@@ -4747,9 +4786,9 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="140"/>
-      <c r="G124" s="141"/>
-      <c r="H124" s="141"/>
+      <c r="F124" s="134"/>
+      <c r="G124" s="135"/>
+      <c r="H124" s="135"/>
     </row>
     <row r="125" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
@@ -4757,9 +4796,9 @@
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="140"/>
-      <c r="G125" s="141"/>
-      <c r="H125" s="141"/>
+      <c r="F125" s="134"/>
+      <c r="G125" s="135"/>
+      <c r="H125" s="135"/>
     </row>
     <row r="126" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
@@ -4767,9 +4806,9 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="140"/>
-      <c r="G126" s="141"/>
-      <c r="H126" s="141"/>
+      <c r="F126" s="134"/>
+      <c r="G126" s="135"/>
+      <c r="H126" s="135"/>
     </row>
     <row r="127" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
@@ -4777,9 +4816,9 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="140"/>
-      <c r="G127" s="141"/>
-      <c r="H127" s="141"/>
+      <c r="F127" s="134"/>
+      <c r="G127" s="135"/>
+      <c r="H127" s="135"/>
     </row>
     <row r="128" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
@@ -4787,9 +4826,9 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="140"/>
-      <c r="G128" s="141"/>
-      <c r="H128" s="141"/>
+      <c r="F128" s="134"/>
+      <c r="G128" s="135"/>
+      <c r="H128" s="135"/>
     </row>
     <row r="129" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
@@ -4797,9 +4836,9 @@
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="140"/>
-      <c r="G129" s="141"/>
-      <c r="H129" s="141"/>
+      <c r="F129" s="134"/>
+      <c r="G129" s="135"/>
+      <c r="H129" s="135"/>
     </row>
     <row r="130" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
@@ -4807,9 +4846,9 @@
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
-      <c r="F130" s="140"/>
-      <c r="G130" s="141"/>
-      <c r="H130" s="141"/>
+      <c r="F130" s="134"/>
+      <c r="G130" s="135"/>
+      <c r="H130" s="135"/>
     </row>
     <row r="131" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
@@ -4817,9 +4856,9 @@
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="140"/>
-      <c r="G131" s="141"/>
-      <c r="H131" s="141"/>
+      <c r="F131" s="134"/>
+      <c r="G131" s="135"/>
+      <c r="H131" s="135"/>
     </row>
     <row r="132" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
@@ -4827,9 +4866,9 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="140"/>
-      <c r="G132" s="141"/>
-      <c r="H132" s="141"/>
+      <c r="F132" s="134"/>
+      <c r="G132" s="135"/>
+      <c r="H132" s="135"/>
     </row>
     <row r="133" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
@@ -4837,14 +4876,19 @@
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="140"/>
-      <c r="G133" s="141"/>
-      <c r="H133" s="141"/>
+      <c r="F133" s="134"/>
+      <c r="G133" s="135"/>
+      <c r="H133" s="135"/>
     </row>
     <row r="134" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F134" s="95"/>
-      <c r="G134" s="111"/>
-      <c r="H134" s="111"/>
+      <c r="A134" s="1"/>
+      <c r="B134" s="1"/>
+      <c r="C134" s="1"/>
+      <c r="D134" s="1"/>
+      <c r="E134" s="1"/>
+      <c r="F134" s="134"/>
+      <c r="G134" s="135"/>
+      <c r="H134" s="135"/>
     </row>
     <row r="135" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="F135" s="95"/>
@@ -4855,6 +4899,11 @@
       <c r="F136" s="95"/>
       <c r="G136" s="111"/>
       <c r="H136" s="111"/>
+    </row>
+    <row r="137" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F137" s="95"/>
+      <c r="G137" s="111"/>
+      <c r="H137" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4872,10 +4921,10 @@
   <dimension ref="B1:K97"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="F46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C79" sqref="C79"/>
+      <selection pane="bottomRight" activeCell="H55" sqref="H55:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -4894,20 +4943,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="185" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="171" t="s">
+      <c r="C2" s="186"/>
+      <c r="D2" s="187"/>
+      <c r="E2" s="182" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="173"/>
-      <c r="G2" s="171" t="s">
+      <c r="F2" s="184"/>
+      <c r="G2" s="182" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="172"/>
-      <c r="I2" s="173"/>
+      <c r="H2" s="183"/>
+      <c r="I2" s="184"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -4928,10 +4977,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="177" t="s">
+      <c r="H3" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="178"/>
+      <c r="I3" s="189"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -4961,19 +5010,19 @@
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="61"/>
-      <c r="C5" s="179" t="s">
+      <c r="C5" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="182" t="s">
+      <c r="D5" s="176" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="185" t="s">
+      <c r="F5" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="188" t="s">
+      <c r="G5" s="170" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -4985,23 +5034,23 @@
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61"/>
-      <c r="C6" s="180"/>
-      <c r="D6" s="183"/>
+      <c r="C6" s="174"/>
+      <c r="D6" s="177"/>
       <c r="E6" s="35"/>
-      <c r="F6" s="186"/>
-      <c r="G6" s="189"/>
-      <c r="H6" s="169" t="s">
+      <c r="F6" s="180"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="170"/>
+      <c r="I6" s="166"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
-      <c r="C7" s="181"/>
-      <c r="D7" s="184"/>
+      <c r="C7" s="175"/>
+      <c r="D7" s="178"/>
       <c r="E7" s="36"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="190"/>
+      <c r="F7" s="181"/>
+      <c r="G7" s="172"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -5035,19 +5084,19 @@
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
-      <c r="C9" s="179" t="s">
+      <c r="C9" s="173" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="182" t="s">
+      <c r="D9" s="176" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="193" t="s">
+      <c r="E9" s="167" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="185" t="s">
+      <c r="F9" s="179" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="188" t="s">
+      <c r="G9" s="170" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -5060,24 +5109,24 @@
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
-      <c r="C10" s="180"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="194"/>
-      <c r="F10" s="186"/>
-      <c r="G10" s="189"/>
-      <c r="H10" s="169" t="s">
+      <c r="C10" s="174"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="168"/>
+      <c r="F10" s="180"/>
+      <c r="G10" s="171"/>
+      <c r="H10" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="170"/>
+      <c r="I10" s="166"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
-      <c r="C11" s="181"/>
-      <c r="D11" s="184"/>
-      <c r="E11" s="195"/>
-      <c r="F11" s="187"/>
-      <c r="G11" s="190"/>
+      <c r="C11" s="175"/>
+      <c r="D11" s="178"/>
+      <c r="E11" s="169"/>
+      <c r="F11" s="181"/>
+      <c r="G11" s="172"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5087,10 +5136,10 @@
     </row>
     <row r="12" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="61"/>
-      <c r="C12" s="179" t="s">
+      <c r="C12" s="173" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="182" t="s">
+      <c r="D12" s="176" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="37" t="s">
@@ -5099,7 +5148,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="188" t="s">
+      <c r="G12" s="170" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -5111,15 +5160,15 @@
     </row>
     <row r="13" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="61"/>
-      <c r="C13" s="181"/>
-      <c r="D13" s="184"/>
+      <c r="C13" s="175"/>
+      <c r="D13" s="178"/>
       <c r="E13" s="37" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="190"/>
+      <c r="G13" s="172"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -5164,8 +5213,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="191"/>
-      <c r="I16" s="192"/>
+      <c r="H16" s="163"/>
+      <c r="I16" s="164"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -5579,19 +5628,19 @@
     </row>
     <row r="40" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="61"/>
-      <c r="C40" s="179" t="s">
+      <c r="C40" s="173" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="182" t="s">
+      <c r="D40" s="176" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="193" t="s">
+      <c r="E40" s="167" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="185" t="s">
+      <c r="F40" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="188" t="s">
+      <c r="G40" s="170" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -5603,23 +5652,23 @@
     </row>
     <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="61"/>
-      <c r="C41" s="180"/>
-      <c r="D41" s="183"/>
-      <c r="E41" s="194"/>
-      <c r="F41" s="186"/>
-      <c r="G41" s="189"/>
-      <c r="H41" s="169" t="s">
+      <c r="C41" s="174"/>
+      <c r="D41" s="177"/>
+      <c r="E41" s="168"/>
+      <c r="F41" s="180"/>
+      <c r="G41" s="171"/>
+      <c r="H41" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="170"/>
+      <c r="I41" s="166"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
-      <c r="C42" s="181"/>
-      <c r="D42" s="184"/>
-      <c r="E42" s="195"/>
-      <c r="F42" s="187"/>
-      <c r="G42" s="190"/>
+      <c r="C42" s="175"/>
+      <c r="D42" s="178"/>
+      <c r="E42" s="169"/>
+      <c r="F42" s="181"/>
+      <c r="G42" s="172"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -5653,19 +5702,19 @@
     </row>
     <row r="44" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="61"/>
-      <c r="C44" s="179" t="s">
+      <c r="C44" s="173" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="182" t="s">
+      <c r="D44" s="176" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="193" t="s">
+      <c r="E44" s="167" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="185" t="s">
+      <c r="F44" s="179" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="188" t="s">
+      <c r="G44" s="170" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -5677,23 +5726,23 @@
     </row>
     <row r="45" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="61"/>
-      <c r="C45" s="180"/>
-      <c r="D45" s="183"/>
-      <c r="E45" s="194"/>
-      <c r="F45" s="186"/>
-      <c r="G45" s="189"/>
-      <c r="H45" s="169" t="s">
+      <c r="C45" s="174"/>
+      <c r="D45" s="177"/>
+      <c r="E45" s="168"/>
+      <c r="F45" s="180"/>
+      <c r="G45" s="171"/>
+      <c r="H45" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="170"/>
+      <c r="I45" s="166"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
-      <c r="C46" s="181"/>
-      <c r="D46" s="184"/>
-      <c r="E46" s="195"/>
-      <c r="F46" s="187"/>
-      <c r="G46" s="190"/>
+      <c r="C46" s="175"/>
+      <c r="D46" s="178"/>
+      <c r="E46" s="169"/>
+      <c r="F46" s="181"/>
+      <c r="G46" s="172"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -5718,8 +5767,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="191"/>
-      <c r="I48" s="192"/>
+      <c r="H48" s="163"/>
+      <c r="I48" s="164"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -5782,10 +5831,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="169" t="s">
+      <c r="H52" s="165" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="170"/>
+      <c r="I52" s="166"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -5818,35 +5867,35 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="191"/>
-      <c r="I55" s="192"/>
+      <c r="H55" s="163"/>
+      <c r="I55" s="164"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="C56" s="155" t="s">
+      <c r="C56" s="149" t="s">
         <v>374</v>
       </c>
-      <c r="D56" s="156" t="s">
+      <c r="D56" s="150" t="s">
         <v>379</v>
       </c>
       <c r="E56" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="F56" s="157" t="s">
+      <c r="F56" s="151" t="s">
         <v>382</v>
       </c>
-      <c r="G56" s="154"/>
+      <c r="G56" s="148"/>
       <c r="H56" s="8"/>
       <c r="I56" s="17"/>
     </row>
     <row r="57" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="61"/>
-      <c r="C57" s="155" t="s">
+      <c r="C57" s="149" t="s">
         <v>375</v>
       </c>
-      <c r="D57" s="151" t="s">
+      <c r="D57" s="145" t="s">
         <v>377</v>
       </c>
       <c r="E57" s="45"/>
@@ -5857,28 +5906,28 @@
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="64"/>
-      <c r="C58" s="155" t="s">
+      <c r="C58" s="149" t="s">
         <v>376</v>
       </c>
-      <c r="D58" s="156" t="s">
+      <c r="D58" s="150" t="s">
         <v>378</v>
       </c>
       <c r="E58" s="42" t="s">
         <v>381</v>
       </c>
-      <c r="F58" s="157" t="s">
+      <c r="F58" s="151" t="s">
         <v>383</v>
       </c>
-      <c r="G58" s="154"/>
+      <c r="G58" s="148"/>
       <c r="H58" s="8"/>
       <c r="I58" s="17"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
-      <c r="C59" s="145" t="s">
+      <c r="C59" s="139" t="s">
         <v>309</v>
       </c>
-      <c r="D59" s="147" t="s">
+      <c r="D59" s="141" t="s">
         <v>310</v>
       </c>
       <c r="E59" s="45"/>
@@ -5889,28 +5938,28 @@
     </row>
     <row r="60" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="64"/>
-      <c r="C60" s="145" t="s">
+      <c r="C60" s="139" t="s">
         <v>311</v>
       </c>
-      <c r="D60" s="147" t="s">
+      <c r="D60" s="141" t="s">
         <v>313</v>
       </c>
       <c r="E60" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="F60" s="149" t="s">
+      <c r="F60" s="143" t="s">
         <v>320</v>
       </c>
-      <c r="G60" s="143"/>
+      <c r="G60" s="137"/>
       <c r="H60" s="8"/>
       <c r="I60" s="17"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="64"/>
-      <c r="C61" s="145" t="s">
+      <c r="C61" s="139" t="s">
         <v>312</v>
       </c>
-      <c r="D61" s="147" t="s">
+      <c r="D61" s="141" t="s">
         <v>314</v>
       </c>
       <c r="E61" s="45"/>
@@ -5921,124 +5970,124 @@
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="64"/>
-      <c r="C62" s="150" t="s">
+      <c r="C62" s="144" t="s">
         <v>344</v>
       </c>
-      <c r="D62" s="151" t="s">
+      <c r="D62" s="145" t="s">
         <v>346</v>
       </c>
       <c r="E62" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="F62" s="152" t="s">
+      <c r="F62" s="146" t="s">
         <v>320</v>
       </c>
-      <c r="G62" s="153"/>
+      <c r="G62" s="147"/>
       <c r="H62" s="8"/>
       <c r="I62" s="17"/>
     </row>
     <row r="63" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B63" s="64"/>
-      <c r="C63" s="150" t="s">
+      <c r="C63" s="144" t="s">
         <v>345</v>
       </c>
-      <c r="D63" s="151" t="s">
+      <c r="D63" s="145" t="s">
         <v>347</v>
       </c>
       <c r="E63" s="42" t="s">
         <v>348</v>
       </c>
-      <c r="F63" s="152" t="s">
+      <c r="F63" s="146" t="s">
         <v>349</v>
       </c>
-      <c r="G63" s="153"/>
+      <c r="G63" s="147"/>
       <c r="H63" s="8"/>
       <c r="I63" s="17"/>
     </row>
     <row r="64" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="64"/>
-      <c r="C64" s="145" t="s">
+      <c r="C64" s="139" t="s">
         <v>315</v>
       </c>
-      <c r="D64" s="147" t="s">
+      <c r="D64" s="141" t="s">
         <v>316</v>
       </c>
       <c r="E64" s="42" t="s">
         <v>317</v>
       </c>
-      <c r="F64" s="149" t="s">
+      <c r="F64" s="143" t="s">
         <v>318</v>
       </c>
-      <c r="G64" s="143"/>
+      <c r="G64" s="137"/>
       <c r="H64" s="8"/>
       <c r="I64" s="17"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64"/>
-      <c r="C65" s="150" t="s">
+      <c r="C65" s="144" t="s">
         <v>351</v>
       </c>
-      <c r="D65" s="151"/>
+      <c r="D65" s="145"/>
       <c r="E65" s="42"/>
-      <c r="F65" s="152"/>
-      <c r="G65" s="153"/>
+      <c r="F65" s="146"/>
+      <c r="G65" s="147"/>
       <c r="H65" s="8"/>
       <c r="I65" s="17"/>
     </row>
     <row r="66" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="64"/>
-      <c r="C66" s="150" t="s">
+      <c r="C66" s="144" t="s">
         <v>352</v>
       </c>
-      <c r="D66" s="151"/>
+      <c r="D66" s="145"/>
       <c r="E66" s="42"/>
-      <c r="F66" s="152"/>
-      <c r="G66" s="153"/>
+      <c r="F66" s="146"/>
+      <c r="G66" s="147"/>
       <c r="H66" s="8"/>
       <c r="I66" s="17"/>
     </row>
     <row r="67" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="64"/>
-      <c r="C67" s="150" t="s">
+      <c r="C67" s="144" t="s">
         <v>350</v>
       </c>
-      <c r="D67" s="151" t="s">
+      <c r="D67" s="145" t="s">
         <v>353</v>
       </c>
       <c r="E67" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="F67" s="152" t="s">
+      <c r="F67" s="146" t="s">
         <v>355</v>
       </c>
-      <c r="G67" s="153"/>
+      <c r="G67" s="147"/>
       <c r="H67" s="8"/>
       <c r="I67" s="17"/>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B68" s="64"/>
-      <c r="C68" s="150" t="s">
+      <c r="C68" s="144" t="s">
         <v>356</v>
       </c>
-      <c r="D68" s="151" t="s">
+      <c r="D68" s="145" t="s">
         <v>357</v>
       </c>
       <c r="E68" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="F68" s="152" t="s">
+      <c r="F68" s="146" t="s">
         <v>355</v>
       </c>
-      <c r="G68" s="153"/>
+      <c r="G68" s="147"/>
       <c r="H68" s="8"/>
       <c r="I68" s="17"/>
     </row>
     <row r="69" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B69" s="64"/>
-      <c r="C69" s="150" t="s">
+      <c r="C69" s="144" t="s">
         <v>358</v>
       </c>
-      <c r="D69" s="151" t="s">
+      <c r="D69" s="145" t="s">
         <v>359</v>
       </c>
       <c r="E69" s="45"/>
@@ -6049,28 +6098,28 @@
     </row>
     <row r="70" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B70" s="64"/>
-      <c r="C70" s="150" t="s">
+      <c r="C70" s="144" t="s">
         <v>360</v>
       </c>
-      <c r="D70" s="151" t="s">
+      <c r="D70" s="145" t="s">
         <v>362</v>
       </c>
       <c r="E70" s="42" t="s">
         <v>364</v>
       </c>
-      <c r="F70" s="152" t="s">
+      <c r="F70" s="146" t="s">
         <v>365</v>
       </c>
-      <c r="G70" s="153"/>
+      <c r="G70" s="147"/>
       <c r="H70" s="8"/>
       <c r="I70" s="17"/>
     </row>
     <row r="71" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B71" s="64"/>
-      <c r="C71" s="150" t="s">
+      <c r="C71" s="144" t="s">
         <v>361</v>
       </c>
-      <c r="D71" s="151" t="s">
+      <c r="D71" s="145" t="s">
         <v>363</v>
       </c>
       <c r="E71" s="45"/>
@@ -6081,10 +6130,10 @@
     </row>
     <row r="72" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="64"/>
-      <c r="C72" s="150" t="s">
+      <c r="C72" s="144" t="s">
         <v>366</v>
       </c>
-      <c r="D72" s="151" t="s">
+      <c r="D72" s="145" t="s">
         <v>369</v>
       </c>
       <c r="E72" s="45"/>
@@ -6095,28 +6144,28 @@
     </row>
     <row r="73" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="64"/>
-      <c r="C73" s="150" t="s">
+      <c r="C73" s="144" t="s">
         <v>367</v>
       </c>
-      <c r="D73" s="151" t="s">
+      <c r="D73" s="145" t="s">
         <v>370</v>
       </c>
       <c r="E73" s="42" t="s">
         <v>372</v>
       </c>
-      <c r="F73" s="152" t="s">
+      <c r="F73" s="146" t="s">
         <v>373</v>
       </c>
-      <c r="G73" s="153"/>
+      <c r="G73" s="147"/>
       <c r="H73" s="8"/>
       <c r="I73" s="17"/>
     </row>
     <row r="74" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="64"/>
-      <c r="C74" s="150" t="s">
+      <c r="C74" s="144" t="s">
         <v>368</v>
       </c>
-      <c r="D74" s="151" t="s">
+      <c r="D74" s="145" t="s">
         <v>371</v>
       </c>
       <c r="E74" s="45"/>
@@ -6127,10 +6176,10 @@
     </row>
     <row r="75" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="64"/>
-      <c r="C75" s="158" t="s">
+      <c r="C75" s="152" t="s">
         <v>384</v>
       </c>
-      <c r="D75" s="159" t="s">
+      <c r="D75" s="153" t="s">
         <v>385</v>
       </c>
       <c r="E75" s="45"/>
@@ -6141,87 +6190,87 @@
     </row>
     <row r="76" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B76" s="64"/>
-      <c r="C76" s="158" t="s">
+      <c r="C76" s="152" t="s">
         <v>386</v>
       </c>
-      <c r="D76" s="159" t="s">
+      <c r="D76" s="153" t="s">
         <v>391</v>
       </c>
       <c r="E76" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F76" s="160" t="s">
+      <c r="F76" s="154" t="s">
         <v>91</v>
       </c>
-      <c r="G76" s="161"/>
+      <c r="G76" s="155"/>
       <c r="H76" s="8"/>
       <c r="I76" s="17"/>
     </row>
     <row r="77" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B77" s="64"/>
-      <c r="C77" s="158" t="s">
+      <c r="C77" s="152" t="s">
         <v>387</v>
       </c>
-      <c r="D77" s="159" t="s">
+      <c r="D77" s="153" t="s">
         <v>390</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>388</v>
       </c>
-      <c r="F77" s="160" t="s">
+      <c r="F77" s="154" t="s">
         <v>389</v>
       </c>
-      <c r="G77" s="161"/>
+      <c r="G77" s="155"/>
       <c r="H77" s="8"/>
       <c r="I77" s="17"/>
     </row>
     <row r="78" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="64"/>
-      <c r="C78" s="158"/>
-      <c r="D78" s="159"/>
+      <c r="C78" s="152"/>
+      <c r="D78" s="153"/>
       <c r="E78" s="42"/>
-      <c r="F78" s="160"/>
-      <c r="G78" s="161"/>
+      <c r="F78" s="154"/>
+      <c r="G78" s="155"/>
       <c r="H78" s="8"/>
       <c r="I78" s="17"/>
     </row>
     <row r="79" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="64"/>
-      <c r="C79" s="158"/>
-      <c r="D79" s="159"/>
+      <c r="C79" s="152"/>
+      <c r="D79" s="153"/>
       <c r="E79" s="42"/>
-      <c r="F79" s="160"/>
-      <c r="G79" s="161"/>
+      <c r="F79" s="154"/>
+      <c r="G79" s="155"/>
       <c r="H79" s="8"/>
       <c r="I79" s="17"/>
     </row>
     <row r="80" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="64"/>
-      <c r="C80" s="158"/>
-      <c r="D80" s="159"/>
+      <c r="C80" s="152"/>
+      <c r="D80" s="153"/>
       <c r="E80" s="42"/>
-      <c r="F80" s="160"/>
-      <c r="G80" s="161"/>
+      <c r="F80" s="154"/>
+      <c r="G80" s="155"/>
       <c r="H80" s="8"/>
       <c r="I80" s="17"/>
     </row>
     <row r="81" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="64"/>
-      <c r="C81" s="158"/>
-      <c r="D81" s="159"/>
+      <c r="C81" s="152"/>
+      <c r="D81" s="153"/>
       <c r="E81" s="42"/>
-      <c r="F81" s="160"/>
-      <c r="G81" s="161"/>
+      <c r="F81" s="154"/>
+      <c r="G81" s="155"/>
       <c r="H81" s="8"/>
       <c r="I81" s="17"/>
     </row>
     <row r="82" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="64"/>
-      <c r="C82" s="144"/>
-      <c r="D82" s="146"/>
+      <c r="C82" s="138"/>
+      <c r="D82" s="140"/>
       <c r="E82" s="39"/>
-      <c r="F82" s="148"/>
-      <c r="G82" s="142"/>
+      <c r="F82" s="142"/>
+      <c r="G82" s="136"/>
       <c r="H82" s="9"/>
       <c r="I82" s="19"/>
     </row>
@@ -6232,8 +6281,8 @@
       <c r="E83" s="25"/>
       <c r="F83" s="22"/>
       <c r="G83" s="25"/>
-      <c r="H83" s="191"/>
-      <c r="I83" s="192"/>
+      <c r="H83" s="163"/>
+      <c r="I83" s="164"/>
     </row>
     <row r="84" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="61"/>
@@ -6377,22 +6426,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -6403,15 +6445,22 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H55:I55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6422,7 +6471,7 @@
   <dimension ref="B1:E38"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
@@ -6440,14 +6489,14 @@
   <sheetData>
     <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="190" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="172" t="s">
+      <c r="C2" s="191"/>
+      <c r="D2" s="183" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="173" t="s">
+      <c r="E2" s="184" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6458,8 +6507,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="177"/>
-      <c r="E3" s="178"/>
+      <c r="D3" s="188"/>
+      <c r="E3" s="189"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">
@@ -6921,7 +6970,7 @@
       <c r="B2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="198" t="s">
+      <c r="C2" s="192" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6929,7 +6978,7 @@
       <c r="B3" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="199"/>
+      <c r="C3" s="193"/>
     </row>
     <row r="4" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="89" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 03 Februari 2023 18:06 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="425">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1282,6 +1282,36 @@
   </si>
   <si>
     <t>Menampilkan ID Institution Branch satu Group yang difilter berdasarkan ID Institution Branch (varBranchID)</t>
+  </si>
+  <si>
+    <t>Func_General_DataCheck_IsNumeric</t>
+  </si>
+  <si>
+    <t>Mengecek apakah Data Input (varData) termasuk dalam kategori data numerik atau tidak</t>
+  </si>
+  <si>
+    <t>Func_General_DataTypeConvert_RecordToVarCharArray</t>
+  </si>
+  <si>
+    <t>Func_General_DataTypeConvert_VarCharArrayToRecord</t>
+  </si>
+  <si>
+    <t>Func_General_DataTypeConvert_VarCharArrayToValues</t>
+  </si>
+  <si>
+    <t>Mengkonversi tipe data dari Record ke VarChar Array</t>
+  </si>
+  <si>
+    <t>Mengkonversi tipe data dari Array VarChar ke Record</t>
+  </si>
+  <si>
+    <t>Mengkonversi tipe data dari Array VarChar ke Values</t>
+  </si>
+  <si>
+    <t>Func_SQLTools_QuerySpeedUp</t>
+  </si>
+  <si>
+    <t>Mempercepat waktu proses Query Rumit Berlapis (melibatkan banyak open table dalam proses join) menjadi Query Sedehana (berbasis Values) yang lebih efisien dalam penggunaan memory</t>
   </si>
 </sst>
 </file>
@@ -2010,7 +2040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="213">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2335,18 +2365,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2431,6 +2449,60 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2544,63 +2616,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2913,13 +2928,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H137"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I40" sqref="I40"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2937,19 +2952,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="156" t="s">
+      <c r="B2" s="170" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="157"/>
-      <c r="D2" s="157"/>
-      <c r="E2" s="158" t="s">
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="172" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="160" t="s">
+      <c r="F2" s="174" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="161"/>
-      <c r="H2" s="162"/>
+      <c r="G2" s="175"/>
+      <c r="H2" s="176"/>
     </row>
     <row r="3" spans="1:8" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="91" t="s">
@@ -2961,7 +2976,7 @@
       <c r="D3" s="108" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="159"/>
+      <c r="E3" s="173"/>
       <c r="F3" s="112" t="s">
         <v>228</v>
       </c>
@@ -2980,19 +2995,19 @@
       <c r="C4" s="116" t="s">
         <v>170</v>
       </c>
-      <c r="D4" s="201" t="s">
+      <c r="D4" s="159" t="s">
         <v>227</v>
       </c>
-      <c r="E4" s="202" t="s">
+      <c r="E4" s="160" t="s">
         <v>235</v>
       </c>
-      <c r="F4" s="203" t="s">
+      <c r="F4" s="161" t="s">
         <v>232</v>
       </c>
-      <c r="G4" s="204">
+      <c r="G4" s="162">
         <v>44910</v>
       </c>
-      <c r="H4" s="205">
+      <c r="H4" s="163">
         <v>44910</v>
       </c>
     </row>
@@ -3000,19 +3015,19 @@
       <c r="A5" s="1"/>
       <c r="B5" s="117"/>
       <c r="C5" s="118"/>
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="152" t="s">
         <v>233</v>
       </c>
-      <c r="E5" s="195" t="s">
+      <c r="E5" s="153" t="s">
         <v>236</v>
       </c>
-      <c r="F5" s="196" t="s">
+      <c r="F5" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G5" s="197">
+      <c r="G5" s="155">
         <v>44908</v>
       </c>
-      <c r="H5" s="198">
+      <c r="H5" s="156">
         <v>44908</v>
       </c>
     </row>
@@ -3020,19 +3035,19 @@
       <c r="A6" s="1"/>
       <c r="B6" s="117"/>
       <c r="C6" s="118"/>
-      <c r="D6" s="194" t="s">
+      <c r="D6" s="152" t="s">
         <v>234</v>
       </c>
-      <c r="E6" s="195" t="s">
+      <c r="E6" s="153" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="196" t="s">
+      <c r="F6" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G6" s="197">
+      <c r="G6" s="155">
         <v>44908</v>
       </c>
-      <c r="H6" s="198">
+      <c r="H6" s="156">
         <v>44908</v>
       </c>
     </row>
@@ -3040,39 +3055,39 @@
       <c r="A7" s="1"/>
       <c r="B7" s="117"/>
       <c r="C7" s="118"/>
-      <c r="D7" s="194" t="s">
-        <v>238</v>
-      </c>
-      <c r="E7" s="195" t="s">
-        <v>239</v>
-      </c>
-      <c r="F7" s="196" t="s">
+      <c r="D7" s="152" t="s">
+        <v>415</v>
+      </c>
+      <c r="E7" s="158" t="s">
+        <v>416</v>
+      </c>
+      <c r="F7" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G7" s="197">
-        <v>44887</v>
-      </c>
-      <c r="H7" s="198">
-        <v>44887</v>
+      <c r="G7" s="155">
+        <v>44960</v>
+      </c>
+      <c r="H7" s="156">
+        <v>44960</v>
       </c>
     </row>
     <row r="8" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="117"/>
       <c r="C8" s="118"/>
-      <c r="D8" s="194" t="s">
-        <v>240</v>
-      </c>
-      <c r="E8" s="195" t="s">
-        <v>241</v>
-      </c>
-      <c r="F8" s="196" t="s">
+      <c r="D8" s="152" t="s">
+        <v>238</v>
+      </c>
+      <c r="E8" s="153" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G8" s="197">
+      <c r="G8" s="155">
         <v>44887</v>
       </c>
-      <c r="H8" s="198">
+      <c r="H8" s="156">
         <v>44887</v>
       </c>
     </row>
@@ -3080,479 +3095,479 @@
       <c r="A9" s="1"/>
       <c r="B9" s="117"/>
       <c r="C9" s="118"/>
-      <c r="D9" s="194" t="s">
-        <v>242</v>
-      </c>
-      <c r="E9" s="195" t="s">
-        <v>243</v>
-      </c>
-      <c r="F9" s="196" t="s">
+      <c r="D9" s="152" t="s">
+        <v>240</v>
+      </c>
+      <c r="E9" s="153" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G9" s="197">
-        <v>44774</v>
-      </c>
-      <c r="H9" s="198">
-        <v>44774</v>
+      <c r="G9" s="155">
+        <v>44887</v>
+      </c>
+      <c r="H9" s="156">
+        <v>44887</v>
       </c>
     </row>
     <row r="10" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="117"/>
       <c r="C10" s="118"/>
-      <c r="D10" s="194" t="s">
-        <v>305</v>
-      </c>
-      <c r="E10" s="195" t="s">
-        <v>306</v>
-      </c>
-      <c r="F10" s="196" t="s">
+      <c r="D10" s="152" t="s">
+        <v>417</v>
+      </c>
+      <c r="E10" s="158" t="s">
+        <v>420</v>
+      </c>
+      <c r="F10" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G10" s="197">
-        <v>44897</v>
-      </c>
-      <c r="H10" s="198">
-        <v>44897</v>
+      <c r="G10" s="155">
+        <v>44959</v>
+      </c>
+      <c r="H10" s="156">
+        <v>44959</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="117"/>
       <c r="C11" s="118"/>
-      <c r="D11" s="194" t="s">
-        <v>244</v>
-      </c>
-      <c r="E11" s="195" t="s">
-        <v>245</v>
-      </c>
-      <c r="F11" s="196" t="s">
+      <c r="D11" s="152" t="s">
+        <v>418</v>
+      </c>
+      <c r="E11" s="153" t="s">
+        <v>421</v>
+      </c>
+      <c r="F11" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G11" s="197">
-        <v>44897</v>
-      </c>
-      <c r="H11" s="198">
-        <v>44897</v>
+      <c r="G11" s="155">
+        <v>44960</v>
+      </c>
+      <c r="H11" s="156">
+        <v>44960</v>
       </c>
     </row>
     <row r="12" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="117"/>
       <c r="C12" s="118"/>
-      <c r="D12" s="194" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" s="195" t="s">
-        <v>247</v>
-      </c>
-      <c r="F12" s="196" t="s">
+      <c r="D12" s="152" t="s">
+        <v>419</v>
+      </c>
+      <c r="E12" s="153" t="s">
+        <v>422</v>
+      </c>
+      <c r="F12" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G12" s="197">
-        <v>44897</v>
-      </c>
-      <c r="H12" s="198">
-        <v>44897</v>
+      <c r="G12" s="155">
+        <v>44960</v>
+      </c>
+      <c r="H12" s="156">
+        <v>44960</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="117"/>
       <c r="C13" s="118"/>
-      <c r="D13" s="194" t="s">
-        <v>248</v>
-      </c>
-      <c r="E13" s="195" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" s="196" t="s">
+      <c r="D13" s="152" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="153" t="s">
+        <v>243</v>
+      </c>
+      <c r="F13" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G13" s="197">
-        <v>44748</v>
-      </c>
-      <c r="H13" s="198">
-        <v>44748</v>
+      <c r="G13" s="155">
+        <v>44774</v>
+      </c>
+      <c r="H13" s="156">
+        <v>44774</v>
       </c>
     </row>
     <row r="14" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="117"/>
       <c r="C14" s="118"/>
-      <c r="D14" s="194" t="s">
-        <v>250</v>
-      </c>
-      <c r="E14" s="195" t="s">
-        <v>251</v>
-      </c>
-      <c r="F14" s="196" t="s">
+      <c r="D14" s="152" t="s">
+        <v>305</v>
+      </c>
+      <c r="E14" s="153" t="s">
+        <v>306</v>
+      </c>
+      <c r="F14" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G14" s="197">
-        <v>44735</v>
-      </c>
-      <c r="H14" s="198">
-        <v>44735</v>
+      <c r="G14" s="155">
+        <v>44897</v>
+      </c>
+      <c r="H14" s="156">
+        <v>44897</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="117"/>
       <c r="C15" s="118"/>
-      <c r="D15" s="194" t="s">
-        <v>252</v>
-      </c>
-      <c r="E15" s="195" t="s">
-        <v>253</v>
-      </c>
-      <c r="F15" s="196" t="s">
+      <c r="D15" s="152" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" s="153" t="s">
+        <v>245</v>
+      </c>
+      <c r="F15" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G15" s="197">
-        <v>44854</v>
-      </c>
-      <c r="H15" s="198">
-        <v>44854</v>
+      <c r="G15" s="155">
+        <v>44897</v>
+      </c>
+      <c r="H15" s="156">
+        <v>44897</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="117"/>
       <c r="C16" s="118"/>
-      <c r="D16" s="194" t="s">
-        <v>254</v>
-      </c>
-      <c r="E16" s="195" t="s">
-        <v>259</v>
-      </c>
-      <c r="F16" s="196" t="s">
+      <c r="D16" s="152" t="s">
+        <v>246</v>
+      </c>
+      <c r="E16" s="153" t="s">
+        <v>247</v>
+      </c>
+      <c r="F16" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G16" s="197">
-        <v>44770</v>
-      </c>
-      <c r="H16" s="198">
-        <v>44770</v>
+      <c r="G16" s="155">
+        <v>44897</v>
+      </c>
+      <c r="H16" s="156">
+        <v>44897</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="117"/>
       <c r="C17" s="118"/>
-      <c r="D17" s="194" t="s">
-        <v>255</v>
-      </c>
-      <c r="E17" s="195" t="s">
-        <v>260</v>
-      </c>
-      <c r="F17" s="196" t="s">
-        <v>256</v>
-      </c>
-      <c r="G17" s="197">
-        <v>44770</v>
-      </c>
-      <c r="H17" s="198">
-        <v>44427</v>
+      <c r="D17" s="152" t="s">
+        <v>248</v>
+      </c>
+      <c r="E17" s="153" t="s">
+        <v>249</v>
+      </c>
+      <c r="F17" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G17" s="155">
+        <v>44748</v>
+      </c>
+      <c r="H17" s="156">
+        <v>44748</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="117"/>
       <c r="C18" s="118"/>
-      <c r="D18" s="194" t="s">
-        <v>257</v>
-      </c>
-      <c r="E18" s="195" t="s">
-        <v>261</v>
-      </c>
-      <c r="F18" s="196" t="s">
+      <c r="D18" s="152" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" s="153" t="s">
+        <v>251</v>
+      </c>
+      <c r="F18" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G18" s="197">
-        <v>44770</v>
-      </c>
-      <c r="H18" s="198">
-        <v>44770</v>
+      <c r="G18" s="155">
+        <v>44735</v>
+      </c>
+      <c r="H18" s="156">
+        <v>44735</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="117"/>
       <c r="C19" s="118"/>
-      <c r="D19" s="194" t="s">
-        <v>258</v>
-      </c>
-      <c r="E19" s="195" t="s">
-        <v>262</v>
-      </c>
-      <c r="F19" s="196" t="s">
+      <c r="D19" s="152" t="s">
+        <v>252</v>
+      </c>
+      <c r="E19" s="153" t="s">
+        <v>253</v>
+      </c>
+      <c r="F19" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G19" s="197">
-        <v>44770</v>
-      </c>
-      <c r="H19" s="198">
-        <v>44427</v>
+      <c r="G19" s="155">
+        <v>44854</v>
+      </c>
+      <c r="H19" s="156">
+        <v>44854</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="117"/>
       <c r="C20" s="118"/>
-      <c r="D20" s="194" t="s">
-        <v>283</v>
-      </c>
-      <c r="E20" s="195" t="s">
-        <v>263</v>
-      </c>
-      <c r="F20" s="196" t="s">
+      <c r="D20" s="152" t="s">
+        <v>254</v>
+      </c>
+      <c r="E20" s="153" t="s">
+        <v>259</v>
+      </c>
+      <c r="F20" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G20" s="197">
-        <v>44777</v>
-      </c>
-      <c r="H20" s="198">
-        <v>44777</v>
+      <c r="G20" s="155">
+        <v>44770</v>
+      </c>
+      <c r="H20" s="156">
+        <v>44770</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="117"/>
       <c r="C21" s="118"/>
-      <c r="D21" s="194" t="s">
-        <v>303</v>
-      </c>
-      <c r="E21" s="195" t="s">
-        <v>304</v>
-      </c>
-      <c r="F21" s="196" t="s">
-        <v>232</v>
-      </c>
-      <c r="G21" s="197">
-        <v>44935</v>
-      </c>
-      <c r="H21" s="198">
-        <v>44935</v>
+      <c r="D21" s="152" t="s">
+        <v>255</v>
+      </c>
+      <c r="E21" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="F21" s="154" t="s">
+        <v>256</v>
+      </c>
+      <c r="G21" s="155">
+        <v>44770</v>
+      </c>
+      <c r="H21" s="156">
+        <v>44427</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="117"/>
       <c r="C22" s="118"/>
-      <c r="D22" s="194" t="s">
-        <v>284</v>
-      </c>
-      <c r="E22" s="195" t="s">
-        <v>277</v>
-      </c>
-      <c r="F22" s="196" t="s">
+      <c r="D22" s="152" t="s">
+        <v>257</v>
+      </c>
+      <c r="E22" s="153" t="s">
+        <v>261</v>
+      </c>
+      <c r="F22" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G22" s="197">
-        <v>44931</v>
-      </c>
-      <c r="H22" s="198">
-        <v>44931</v>
+      <c r="G22" s="155">
+        <v>44770</v>
+      </c>
+      <c r="H22" s="156">
+        <v>44770</v>
       </c>
     </row>
     <row r="23" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="117"/>
       <c r="C23" s="118"/>
-      <c r="D23" s="194" t="s">
-        <v>264</v>
-      </c>
-      <c r="E23" s="195" t="s">
-        <v>265</v>
-      </c>
-      <c r="F23" s="196" t="s">
+      <c r="D23" s="152" t="s">
+        <v>258</v>
+      </c>
+      <c r="E23" s="153" t="s">
+        <v>262</v>
+      </c>
+      <c r="F23" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G23" s="197">
-        <v>44847</v>
-      </c>
-      <c r="H23" s="198">
-        <v>44847</v>
+      <c r="G23" s="155">
+        <v>44770</v>
+      </c>
+      <c r="H23" s="156">
+        <v>44427</v>
       </c>
     </row>
     <row r="24" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="117"/>
       <c r="C24" s="118"/>
-      <c r="D24" s="194" t="s">
-        <v>266</v>
-      </c>
-      <c r="E24" s="195" t="s">
-        <v>268</v>
-      </c>
-      <c r="F24" s="196" t="s">
-        <v>267</v>
-      </c>
-      <c r="G24" s="197">
-        <v>44792</v>
-      </c>
-      <c r="H24" s="198">
-        <v>44770</v>
+      <c r="D24" s="152" t="s">
+        <v>283</v>
+      </c>
+      <c r="E24" s="153" t="s">
+        <v>263</v>
+      </c>
+      <c r="F24" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G24" s="155">
+        <v>44777</v>
+      </c>
+      <c r="H24" s="156">
+        <v>44777</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="117"/>
       <c r="C25" s="118"/>
-      <c r="D25" s="194" t="s">
-        <v>269</v>
-      </c>
-      <c r="E25" s="195" t="s">
-        <v>270</v>
-      </c>
-      <c r="F25" s="196" t="s">
+      <c r="D25" s="152" t="s">
+        <v>303</v>
+      </c>
+      <c r="E25" s="153" t="s">
+        <v>304</v>
+      </c>
+      <c r="F25" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G25" s="197">
-        <v>44776</v>
-      </c>
-      <c r="H25" s="198">
-        <v>44776</v>
+      <c r="G25" s="155">
+        <v>44935</v>
+      </c>
+      <c r="H25" s="156">
+        <v>44935</v>
       </c>
     </row>
     <row r="26" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="117"/>
       <c r="C26" s="118"/>
-      <c r="D26" s="194" t="s">
-        <v>302</v>
-      </c>
-      <c r="E26" s="195" t="s">
-        <v>271</v>
-      </c>
-      <c r="F26" s="196" t="s">
+      <c r="D26" s="152" t="s">
+        <v>284</v>
+      </c>
+      <c r="E26" s="153" t="s">
+        <v>277</v>
+      </c>
+      <c r="F26" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G26" s="197">
-        <v>44777</v>
-      </c>
-      <c r="H26" s="198">
-        <v>44777</v>
+      <c r="G26" s="155">
+        <v>44931</v>
+      </c>
+      <c r="H26" s="156">
+        <v>44931</v>
       </c>
     </row>
     <row r="27" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="117"/>
       <c r="C27" s="118"/>
-      <c r="D27" s="194" t="s">
-        <v>272</v>
-      </c>
-      <c r="E27" s="195" t="s">
-        <v>273</v>
-      </c>
-      <c r="F27" s="196" t="s">
+      <c r="D27" s="152" t="s">
+        <v>264</v>
+      </c>
+      <c r="E27" s="153" t="s">
+        <v>265</v>
+      </c>
+      <c r="F27" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G27" s="197">
-        <v>44770</v>
-      </c>
-      <c r="H27" s="198">
-        <v>44770</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="G27" s="155">
+        <v>44847</v>
+      </c>
+      <c r="H27" s="156">
+        <v>44847</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="117"/>
       <c r="C28" s="118"/>
-      <c r="D28" s="194" t="s">
-        <v>294</v>
-      </c>
-      <c r="E28" s="200" t="s">
-        <v>296</v>
-      </c>
-      <c r="F28" s="196" t="s">
-        <v>232</v>
-      </c>
-      <c r="G28" s="197">
-        <v>44937</v>
-      </c>
-      <c r="H28" s="198">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="D28" s="152" t="s">
+        <v>266</v>
+      </c>
+      <c r="E28" s="153" t="s">
+        <v>268</v>
+      </c>
+      <c r="F28" s="154" t="s">
+        <v>267</v>
+      </c>
+      <c r="G28" s="155">
+        <v>44792</v>
+      </c>
+      <c r="H28" s="156">
+        <v>44770</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="117"/>
       <c r="C29" s="118"/>
-      <c r="D29" s="194" t="s">
-        <v>293</v>
-      </c>
-      <c r="E29" s="200" t="s">
-        <v>295</v>
-      </c>
-      <c r="F29" s="196" t="s">
+      <c r="D29" s="152" t="s">
+        <v>269</v>
+      </c>
+      <c r="E29" s="153" t="s">
+        <v>270</v>
+      </c>
+      <c r="F29" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G29" s="197">
-        <v>44937</v>
-      </c>
-      <c r="H29" s="198">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="G29" s="155">
+        <v>44776</v>
+      </c>
+      <c r="H29" s="156">
+        <v>44776</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="117"/>
       <c r="C30" s="118"/>
-      <c r="D30" s="194" t="s">
-        <v>291</v>
-      </c>
-      <c r="E30" s="200" t="s">
-        <v>297</v>
-      </c>
-      <c r="F30" s="196" t="s">
+      <c r="D30" s="152" t="s">
+        <v>302</v>
+      </c>
+      <c r="E30" s="153" t="s">
+        <v>271</v>
+      </c>
+      <c r="F30" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G30" s="197">
-        <v>44937</v>
-      </c>
-      <c r="H30" s="198">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="G30" s="155">
+        <v>44777</v>
+      </c>
+      <c r="H30" s="156">
+        <v>44777</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="117"/>
       <c r="C31" s="118"/>
-      <c r="D31" s="194" t="s">
-        <v>307</v>
-      </c>
-      <c r="E31" s="200" t="s">
-        <v>308</v>
-      </c>
-      <c r="F31" s="196" t="s">
+      <c r="D31" s="152" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" s="153" t="s">
+        <v>273</v>
+      </c>
+      <c r="F31" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G31" s="197">
-        <v>44949</v>
-      </c>
-      <c r="H31" s="198">
-        <v>44949</v>
+      <c r="G31" s="155">
+        <v>44770</v>
+      </c>
+      <c r="H31" s="156">
+        <v>44770</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="117"/>
       <c r="C32" s="118"/>
-      <c r="D32" s="194" t="s">
-        <v>292</v>
-      </c>
-      <c r="E32" s="200" t="s">
-        <v>298</v>
-      </c>
-      <c r="F32" s="196" t="s">
+      <c r="D32" s="152" t="s">
+        <v>294</v>
+      </c>
+      <c r="E32" s="158" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G32" s="197">
+      <c r="G32" s="155">
         <v>44937</v>
       </c>
-      <c r="H32" s="198">
+      <c r="H32" s="156">
         <v>44937</v>
       </c>
     </row>
@@ -3560,19 +3575,19 @@
       <c r="A33" s="1"/>
       <c r="B33" s="117"/>
       <c r="C33" s="118"/>
-      <c r="D33" s="194" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" s="200" t="s">
-        <v>299</v>
-      </c>
-      <c r="F33" s="196" t="s">
+      <c r="D33" s="152" t="s">
+        <v>293</v>
+      </c>
+      <c r="E33" s="158" t="s">
+        <v>295</v>
+      </c>
+      <c r="F33" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G33" s="197">
+      <c r="G33" s="155">
         <v>44937</v>
       </c>
-      <c r="H33" s="198">
+      <c r="H33" s="156">
         <v>44937</v>
       </c>
     </row>
@@ -3580,19 +3595,19 @@
       <c r="A34" s="1"/>
       <c r="B34" s="117"/>
       <c r="C34" s="118"/>
-      <c r="D34" s="194" t="s">
-        <v>289</v>
-      </c>
-      <c r="E34" s="200" t="s">
-        <v>300</v>
-      </c>
-      <c r="F34" s="196" t="s">
+      <c r="D34" s="152" t="s">
+        <v>291</v>
+      </c>
+      <c r="E34" s="158" t="s">
+        <v>297</v>
+      </c>
+      <c r="F34" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G34" s="197">
+      <c r="G34" s="155">
         <v>44937</v>
       </c>
-      <c r="H34" s="198">
+      <c r="H34" s="156">
         <v>44937</v>
       </c>
     </row>
@@ -3600,310 +3615,360 @@
       <c r="A35" s="1"/>
       <c r="B35" s="117"/>
       <c r="C35" s="118"/>
-      <c r="D35" s="124" t="s">
-        <v>288</v>
-      </c>
-      <c r="E35" s="206" t="s">
-        <v>301</v>
-      </c>
-      <c r="F35" s="125" t="s">
+      <c r="D35" s="152" t="s">
+        <v>307</v>
+      </c>
+      <c r="E35" s="158" t="s">
+        <v>308</v>
+      </c>
+      <c r="F35" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G35" s="126">
-        <v>44937</v>
-      </c>
-      <c r="H35" s="127">
-        <v>44937</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G35" s="155">
+        <v>44949</v>
+      </c>
+      <c r="H35" s="156">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="117"/>
-      <c r="C36" s="66"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
-      <c r="F36" s="66"/>
-      <c r="G36" s="66"/>
-      <c r="H36" s="212"/>
-    </row>
-    <row r="37" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C36" s="118"/>
+      <c r="D36" s="152" t="s">
+        <v>292</v>
+      </c>
+      <c r="E36" s="158" t="s">
+        <v>298</v>
+      </c>
+      <c r="F36" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G36" s="155">
+        <v>44937</v>
+      </c>
+      <c r="H36" s="156">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="117"/>
-      <c r="C37" s="118" t="s">
-        <v>146</v>
-      </c>
-      <c r="D37" s="207" t="s">
-        <v>274</v>
-      </c>
-      <c r="E37" s="208" t="s">
-        <v>275</v>
-      </c>
-      <c r="F37" s="209" t="s">
+      <c r="C37" s="118"/>
+      <c r="D37" s="152" t="s">
+        <v>290</v>
+      </c>
+      <c r="E37" s="158" t="s">
+        <v>299</v>
+      </c>
+      <c r="F37" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G37" s="210">
-        <v>44167</v>
-      </c>
-      <c r="H37" s="211">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G37" s="155">
+        <v>44937</v>
+      </c>
+      <c r="H37" s="156">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="117"/>
       <c r="C38" s="118"/>
-      <c r="D38" s="199" t="s">
-        <v>276</v>
-      </c>
-      <c r="E38" s="195" t="s">
-        <v>285</v>
-      </c>
-      <c r="F38" s="196" t="s">
+      <c r="D38" s="152" t="s">
+        <v>289</v>
+      </c>
+      <c r="E38" s="158" t="s">
+        <v>300</v>
+      </c>
+      <c r="F38" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G38" s="197">
-        <v>44167</v>
-      </c>
-      <c r="H38" s="198">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G38" s="155">
+        <v>44937</v>
+      </c>
+      <c r="H38" s="156">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="B39" s="117"/>
       <c r="C39" s="118"/>
-      <c r="D39" s="194" t="s">
-        <v>278</v>
-      </c>
-      <c r="E39" s="195" t="s">
-        <v>279</v>
-      </c>
-      <c r="F39" s="196" t="s">
+      <c r="D39" s="152" t="s">
+        <v>288</v>
+      </c>
+      <c r="E39" s="158" t="s">
+        <v>301</v>
+      </c>
+      <c r="F39" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G39" s="197">
-        <v>43185</v>
-      </c>
-      <c r="H39" s="198">
-        <v>43185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G39" s="155">
+        <v>44937</v>
+      </c>
+      <c r="H39" s="156">
+        <v>44937</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="B40" s="117"/>
       <c r="C40" s="118"/>
-      <c r="D40" s="194" t="s">
-        <v>280</v>
-      </c>
-      <c r="E40" s="195" t="s">
-        <v>282</v>
-      </c>
-      <c r="F40" s="196" t="s">
-        <v>281</v>
-      </c>
-      <c r="G40" s="197">
-        <v>44216</v>
-      </c>
-      <c r="H40" s="198">
-        <v>44216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D40" s="118" t="s">
+        <v>423</v>
+      </c>
+      <c r="E40" s="123" t="s">
+        <v>424</v>
+      </c>
+      <c r="F40" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G40" s="121">
+        <v>44959</v>
+      </c>
+      <c r="H40" s="122">
+        <v>44959</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="B41" s="117"/>
-      <c r="C41" s="118"/>
-      <c r="D41" s="194" t="s">
-        <v>401</v>
-      </c>
-      <c r="E41" s="200" t="s">
-        <v>403</v>
-      </c>
-      <c r="F41" s="196" t="s">
-        <v>232</v>
-      </c>
-      <c r="G41" s="197">
-        <v>43720</v>
-      </c>
-      <c r="H41" s="198">
-        <v>43720</v>
-      </c>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="169"/>
     </row>
     <row r="42" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1"/>
       <c r="B42" s="117"/>
-      <c r="C42" s="118"/>
-      <c r="D42" s="194" t="s">
-        <v>402</v>
-      </c>
-      <c r="E42" s="200" t="s">
-        <v>404</v>
-      </c>
-      <c r="F42" s="196" t="s">
+      <c r="C42" s="118" t="s">
+        <v>146</v>
+      </c>
+      <c r="D42" s="164" t="s">
+        <v>274</v>
+      </c>
+      <c r="E42" s="165" t="s">
+        <v>275</v>
+      </c>
+      <c r="F42" s="166" t="s">
         <v>232</v>
       </c>
-      <c r="G42" s="197">
-        <v>43785</v>
-      </c>
-      <c r="H42" s="198">
-        <v>43785</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G42" s="167">
+        <v>44167</v>
+      </c>
+      <c r="H42" s="168">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="117"/>
       <c r="C43" s="118"/>
-      <c r="D43" s="194" t="s">
-        <v>405</v>
-      </c>
-      <c r="E43" s="200" t="s">
-        <v>406</v>
-      </c>
-      <c r="F43" s="196" t="s">
+      <c r="D43" s="157" t="s">
+        <v>276</v>
+      </c>
+      <c r="E43" s="153" t="s">
+        <v>285</v>
+      </c>
+      <c r="F43" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G43" s="197">
-        <v>43208</v>
-      </c>
-      <c r="H43" s="198">
-        <v>43208</v>
+      <c r="G43" s="155">
+        <v>44167</v>
+      </c>
+      <c r="H43" s="156">
+        <v>44167</v>
       </c>
     </row>
     <row r="44" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1"/>
       <c r="B44" s="117"/>
       <c r="C44" s="118"/>
-      <c r="D44" s="194" t="s">
-        <v>407</v>
-      </c>
-      <c r="E44" s="200" t="s">
-        <v>408</v>
-      </c>
-      <c r="F44" s="196" t="s">
+      <c r="D44" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="E44" s="153" t="s">
+        <v>279</v>
+      </c>
+      <c r="F44" s="154" t="s">
         <v>232</v>
       </c>
-      <c r="G44" s="197">
-        <v>43181</v>
-      </c>
-      <c r="H44" s="198">
-        <v>43181</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="G44" s="155">
+        <v>43185</v>
+      </c>
+      <c r="H44" s="156">
+        <v>43185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1"/>
       <c r="B45" s="117"/>
       <c r="C45" s="118"/>
-      <c r="D45" s="194" t="s">
-        <v>409</v>
-      </c>
-      <c r="E45" s="200" t="s">
-        <v>410</v>
-      </c>
-      <c r="F45" s="196" t="s">
+      <c r="D45" s="152" t="s">
+        <v>280</v>
+      </c>
+      <c r="E45" s="153" t="s">
+        <v>282</v>
+      </c>
+      <c r="F45" s="154" t="s">
         <v>281</v>
       </c>
-      <c r="G45" s="197">
-        <v>44958</v>
-      </c>
-      <c r="H45" s="198">
-        <v>43181</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="G45" s="155">
+        <v>44216</v>
+      </c>
+      <c r="H45" s="156">
+        <v>44216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="117"/>
       <c r="C46" s="118"/>
-      <c r="D46" s="194" t="s">
-        <v>411</v>
-      </c>
-      <c r="E46" s="200" t="s">
-        <v>412</v>
-      </c>
-      <c r="F46" s="196" t="s">
-        <v>281</v>
-      </c>
-      <c r="G46" s="197">
-        <v>44958</v>
-      </c>
-      <c r="H46" s="198">
-        <v>43181</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D46" s="152" t="s">
+        <v>401</v>
+      </c>
+      <c r="E46" s="158" t="s">
+        <v>403</v>
+      </c>
+      <c r="F46" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G46" s="155">
+        <v>43720</v>
+      </c>
+      <c r="H46" s="156">
+        <v>43720</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="117"/>
       <c r="C47" s="118"/>
-      <c r="D47" s="194" t="s">
-        <v>413</v>
-      </c>
-      <c r="E47" s="200" t="s">
-        <v>414</v>
-      </c>
-      <c r="F47" s="196" t="s">
-        <v>281</v>
-      </c>
-      <c r="G47" s="197">
-        <v>44958</v>
-      </c>
-      <c r="H47" s="198">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D47" s="152" t="s">
+        <v>402</v>
+      </c>
+      <c r="E47" s="158" t="s">
+        <v>404</v>
+      </c>
+      <c r="F47" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G47" s="155">
+        <v>43785</v>
+      </c>
+      <c r="H47" s="156">
+        <v>43785</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="117"/>
       <c r="C48" s="118"/>
-      <c r="D48" s="118"/>
-      <c r="E48" s="123"/>
-      <c r="F48" s="120"/>
-      <c r="G48" s="121"/>
-      <c r="H48" s="122"/>
+      <c r="D48" s="152" t="s">
+        <v>405</v>
+      </c>
+      <c r="E48" s="158" t="s">
+        <v>406</v>
+      </c>
+      <c r="F48" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G48" s="155">
+        <v>43208</v>
+      </c>
+      <c r="H48" s="156">
+        <v>43208</v>
+      </c>
     </row>
     <row r="49" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1"/>
       <c r="B49" s="117"/>
       <c r="C49" s="118"/>
-      <c r="D49" s="118"/>
-      <c r="E49" s="123"/>
-      <c r="F49" s="120"/>
-      <c r="G49" s="121"/>
-      <c r="H49" s="122"/>
-    </row>
-    <row r="50" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D49" s="152" t="s">
+        <v>407</v>
+      </c>
+      <c r="E49" s="158" t="s">
+        <v>408</v>
+      </c>
+      <c r="F49" s="154" t="s">
+        <v>232</v>
+      </c>
+      <c r="G49" s="155">
+        <v>43181</v>
+      </c>
+      <c r="H49" s="156">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A50" s="1"/>
       <c r="B50" s="117"/>
       <c r="C50" s="118"/>
-      <c r="D50" s="118"/>
-      <c r="E50" s="123"/>
-      <c r="F50" s="120"/>
-      <c r="G50" s="121"/>
-      <c r="H50" s="122"/>
+      <c r="D50" s="152" t="s">
+        <v>409</v>
+      </c>
+      <c r="E50" s="158" t="s">
+        <v>410</v>
+      </c>
+      <c r="F50" s="154" t="s">
+        <v>281</v>
+      </c>
+      <c r="G50" s="155">
+        <v>44958</v>
+      </c>
+      <c r="H50" s="156">
+        <v>43181</v>
+      </c>
     </row>
     <row r="51" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1"/>
       <c r="B51" s="117"/>
       <c r="C51" s="118"/>
-      <c r="D51" s="118"/>
-      <c r="E51" s="123"/>
-      <c r="F51" s="120"/>
-      <c r="G51" s="121"/>
-      <c r="H51" s="122"/>
-    </row>
-    <row r="52" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D51" s="152" t="s">
+        <v>411</v>
+      </c>
+      <c r="E51" s="158" t="s">
+        <v>412</v>
+      </c>
+      <c r="F51" s="154" t="s">
+        <v>281</v>
+      </c>
+      <c r="G51" s="155">
+        <v>44958</v>
+      </c>
+      <c r="H51" s="156">
+        <v>43181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" s="1"/>
       <c r="B52" s="117"/>
       <c r="C52" s="118"/>
-      <c r="D52" s="118"/>
-      <c r="E52" s="123"/>
-      <c r="F52" s="120"/>
-      <c r="G52" s="121"/>
-      <c r="H52" s="122"/>
+      <c r="D52" s="152" t="s">
+        <v>413</v>
+      </c>
+      <c r="E52" s="158" t="s">
+        <v>414</v>
+      </c>
+      <c r="F52" s="154" t="s">
+        <v>281</v>
+      </c>
+      <c r="G52" s="155">
+        <v>44958</v>
+      </c>
+      <c r="H52" s="156">
+        <v>43922</v>
+      </c>
     </row>
     <row r="53" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="117"/>
       <c r="C53" s="118"/>
       <c r="D53" s="118"/>
-      <c r="E53" s="119"/>
+      <c r="E53" s="123"/>
       <c r="F53" s="120"/>
       <c r="G53" s="121"/>
       <c r="H53" s="122"/>
@@ -3912,28 +3977,18 @@
       <c r="A54" s="1"/>
       <c r="B54" s="117"/>
       <c r="C54" s="118"/>
-      <c r="D54" s="118" t="s">
-        <v>286</v>
-      </c>
-      <c r="E54" s="119" t="s">
-        <v>287</v>
-      </c>
-      <c r="F54" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G54" s="121">
-        <v>44949</v>
-      </c>
-      <c r="H54" s="122">
-        <v>44949</v>
-      </c>
+      <c r="D54" s="118"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="120"/>
+      <c r="G54" s="121"/>
+      <c r="H54" s="122"/>
     </row>
     <row r="55" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="117"/>
       <c r="C55" s="118"/>
       <c r="D55" s="118"/>
-      <c r="E55" s="119"/>
+      <c r="E55" s="123"/>
       <c r="F55" s="120"/>
       <c r="G55" s="121"/>
       <c r="H55" s="122"/>
@@ -3943,7 +3998,7 @@
       <c r="B56" s="117"/>
       <c r="C56" s="118"/>
       <c r="D56" s="118"/>
-      <c r="E56" s="119"/>
+      <c r="E56" s="123"/>
       <c r="F56" s="120"/>
       <c r="G56" s="121"/>
       <c r="H56" s="122"/>
@@ -3953,7 +4008,7 @@
       <c r="B57" s="117"/>
       <c r="C57" s="118"/>
       <c r="D57" s="118"/>
-      <c r="E57" s="119"/>
+      <c r="E57" s="123"/>
       <c r="F57" s="120"/>
       <c r="G57" s="121"/>
       <c r="H57" s="122"/>
@@ -3963,7 +4018,7 @@
       <c r="B58" s="117"/>
       <c r="C58" s="118"/>
       <c r="D58" s="118"/>
-      <c r="E58" s="123"/>
+      <c r="E58" s="119"/>
       <c r="F58" s="120"/>
       <c r="G58" s="121"/>
       <c r="H58" s="122"/>
@@ -3972,132 +4027,92 @@
       <c r="A59" s="1"/>
       <c r="B59" s="117"/>
       <c r="C59" s="118"/>
-      <c r="D59" s="118"/>
-      <c r="E59" s="119"/>
-      <c r="F59" s="120"/>
-      <c r="G59" s="121"/>
-      <c r="H59" s="122"/>
-    </row>
-    <row r="60" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D59" s="118" t="s">
+        <v>286</v>
+      </c>
+      <c r="E59" s="119" t="s">
+        <v>287</v>
+      </c>
+      <c r="F59" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G59" s="121">
+        <v>44949</v>
+      </c>
+      <c r="H59" s="122">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
       <c r="B60" s="117"/>
-      <c r="C60" s="118" t="s">
-        <v>336</v>
-      </c>
-      <c r="D60" s="118" t="s">
-        <v>326</v>
-      </c>
-      <c r="E60" s="123" t="s">
-        <v>327</v>
-      </c>
-      <c r="F60" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G60" s="121">
-        <v>44902</v>
-      </c>
-      <c r="H60" s="122">
-        <v>44902</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C60" s="118"/>
+      <c r="D60" s="118"/>
+      <c r="E60" s="119"/>
+      <c r="F60" s="120"/>
+      <c r="G60" s="121"/>
+      <c r="H60" s="122"/>
+    </row>
+    <row r="61" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="B61" s="117"/>
       <c r="C61" s="118"/>
-      <c r="D61" s="118" t="s">
-        <v>332</v>
-      </c>
-      <c r="E61" s="123" t="s">
-        <v>333</v>
-      </c>
-      <c r="F61" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G61" s="121">
-        <v>44897</v>
-      </c>
-      <c r="H61" s="122">
-        <v>44897</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D61" s="118"/>
+      <c r="E61" s="119"/>
+      <c r="F61" s="120"/>
+      <c r="G61" s="121"/>
+      <c r="H61" s="122"/>
+    </row>
+    <row r="62" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="B62" s="117"/>
       <c r="C62" s="118"/>
-      <c r="D62" s="118" t="s">
-        <v>323</v>
-      </c>
-      <c r="E62" s="123" t="s">
-        <v>324</v>
-      </c>
-      <c r="F62" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G62" s="121">
-        <v>44951</v>
-      </c>
-      <c r="H62" s="122">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D62" s="118"/>
+      <c r="E62" s="119"/>
+      <c r="F62" s="120"/>
+      <c r="G62" s="121"/>
+      <c r="H62" s="122"/>
+    </row>
+    <row r="63" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
       <c r="B63" s="117"/>
       <c r="C63" s="118"/>
-      <c r="D63" s="118" t="s">
-        <v>338</v>
-      </c>
-      <c r="E63" s="123" t="s">
-        <v>337</v>
-      </c>
-      <c r="F63" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G63" s="121">
-        <v>44951</v>
-      </c>
-      <c r="H63" s="122">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D63" s="118"/>
+      <c r="E63" s="123"/>
+      <c r="F63" s="120"/>
+      <c r="G63" s="121"/>
+      <c r="H63" s="122"/>
+    </row>
+    <row r="64" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="B64" s="117"/>
       <c r="C64" s="118"/>
-      <c r="D64" s="118" t="s">
-        <v>321</v>
-      </c>
-      <c r="E64" s="123" t="s">
-        <v>325</v>
-      </c>
-      <c r="F64" s="120" t="s">
-        <v>281</v>
-      </c>
-      <c r="G64" s="121">
-        <v>44900</v>
-      </c>
-      <c r="H64" s="122">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D64" s="118"/>
+      <c r="E64" s="119"/>
+      <c r="F64" s="120"/>
+      <c r="G64" s="121"/>
+      <c r="H64" s="122"/>
+    </row>
+    <row r="65" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="B65" s="117"/>
-      <c r="C65" s="118"/>
+      <c r="C65" s="118" t="s">
+        <v>336</v>
+      </c>
       <c r="D65" s="118" t="s">
-        <v>328</v>
-      </c>
-      <c r="E65" s="119" t="s">
-        <v>329</v>
+        <v>326</v>
+      </c>
+      <c r="E65" s="123" t="s">
+        <v>327</v>
       </c>
       <c r="F65" s="120" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G65" s="121">
-        <v>44896</v>
+        <v>44902</v>
       </c>
       <c r="H65" s="122">
-        <v>44896</v>
+        <v>44902</v>
       </c>
     </row>
     <row r="66" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4105,19 +4120,19 @@
       <c r="B66" s="117"/>
       <c r="C66" s="118"/>
       <c r="D66" s="118" t="s">
-        <v>322</v>
+        <v>332</v>
       </c>
       <c r="E66" s="123" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="F66" s="120" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G66" s="121">
-        <v>44945</v>
+        <v>44897</v>
       </c>
       <c r="H66" s="122">
-        <v>44949</v>
+        <v>44897</v>
       </c>
     </row>
     <row r="67" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4125,19 +4140,19 @@
       <c r="B67" s="117"/>
       <c r="C67" s="118"/>
       <c r="D67" s="118" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="E67" s="123" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="F67" s="120" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G67" s="121">
-        <v>44910</v>
+        <v>44951</v>
       </c>
       <c r="H67" s="122">
-        <v>44910</v>
+        <v>44951</v>
       </c>
     </row>
     <row r="68" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -4145,10 +4160,10 @@
       <c r="B68" s="117"/>
       <c r="C68" s="118"/>
       <c r="D68" s="118" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="E68" s="123" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F68" s="120" t="s">
         <v>232</v>
@@ -4165,199 +4180,229 @@
       <c r="B69" s="117"/>
       <c r="C69" s="118"/>
       <c r="D69" s="118" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="E69" s="123" t="s">
-        <v>343</v>
+        <v>325</v>
       </c>
       <c r="F69" s="120" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G69" s="121">
-        <v>44952</v>
+        <v>44900</v>
       </c>
       <c r="H69" s="122">
-        <v>44952</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="70" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="117"/>
       <c r="C70" s="118"/>
-      <c r="D70" s="118"/>
-      <c r="E70" s="119"/>
-      <c r="F70" s="120"/>
-      <c r="G70" s="121"/>
-      <c r="H70" s="122"/>
-    </row>
-    <row r="71" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D70" s="118" t="s">
+        <v>328</v>
+      </c>
+      <c r="E70" s="119" t="s">
+        <v>329</v>
+      </c>
+      <c r="F70" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="G70" s="121">
+        <v>44896</v>
+      </c>
+      <c r="H70" s="122">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="117"/>
       <c r="C71" s="118"/>
-      <c r="D71" s="118"/>
-      <c r="E71" s="119"/>
-      <c r="F71" s="120"/>
-      <c r="G71" s="121"/>
-      <c r="H71" s="122"/>
-    </row>
-    <row r="72" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D71" s="118" t="s">
+        <v>322</v>
+      </c>
+      <c r="E71" s="123" t="s">
+        <v>339</v>
+      </c>
+      <c r="F71" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="G71" s="121">
+        <v>44945</v>
+      </c>
+      <c r="H71" s="122">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="117"/>
       <c r="C72" s="118"/>
-      <c r="D72" s="118"/>
-      <c r="E72" s="119"/>
-      <c r="F72" s="120"/>
-      <c r="G72" s="121"/>
-      <c r="H72" s="122"/>
-    </row>
-    <row r="73" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D72" s="118" t="s">
+        <v>334</v>
+      </c>
+      <c r="E72" s="123" t="s">
+        <v>335</v>
+      </c>
+      <c r="F72" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="G72" s="121">
+        <v>44910</v>
+      </c>
+      <c r="H72" s="122">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="117"/>
       <c r="C73" s="118"/>
       <c r="D73" s="118" t="s">
-        <v>394</v>
+        <v>340</v>
       </c>
       <c r="E73" s="123" t="s">
-        <v>395</v>
+        <v>341</v>
       </c>
       <c r="F73" s="120" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G73" s="121">
-        <v>44957</v>
+        <v>44951</v>
       </c>
       <c r="H73" s="122">
-        <v>42982</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="117"/>
       <c r="C74" s="118"/>
       <c r="D74" s="118" t="s">
-        <v>393</v>
+        <v>342</v>
       </c>
       <c r="E74" s="123" t="s">
-        <v>396</v>
+        <v>343</v>
       </c>
       <c r="F74" s="120" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G74" s="121">
-        <v>44281</v>
+        <v>44952</v>
       </c>
       <c r="H74" s="122">
-        <v>44557</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>44952</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="117"/>
       <c r="C75" s="118"/>
-      <c r="D75" s="118" t="s">
-        <v>397</v>
-      </c>
-      <c r="E75" s="123" t="s">
-        <v>398</v>
-      </c>
-      <c r="F75" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G75" s="121">
-        <v>43257</v>
-      </c>
-      <c r="H75" s="122">
-        <v>43257</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D75" s="118"/>
+      <c r="E75" s="119"/>
+      <c r="F75" s="120"/>
+      <c r="G75" s="121"/>
+      <c r="H75" s="122"/>
+    </row>
+    <row r="76" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="117"/>
       <c r="C76" s="118"/>
-      <c r="D76" s="118" t="s">
-        <v>286</v>
-      </c>
-      <c r="E76" s="123" t="s">
-        <v>399</v>
-      </c>
-      <c r="F76" s="120" t="s">
-        <v>232</v>
-      </c>
-      <c r="G76" s="121">
-        <v>44949</v>
-      </c>
-      <c r="H76" s="122">
-        <v>44949</v>
-      </c>
+      <c r="D76" s="118"/>
+      <c r="E76" s="119"/>
+      <c r="F76" s="120"/>
+      <c r="G76" s="121"/>
+      <c r="H76" s="122"/>
     </row>
     <row r="77" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="117"/>
       <c r="C77" s="118"/>
       <c r="D77" s="118"/>
-      <c r="E77" s="123"/>
+      <c r="E77" s="119"/>
       <c r="F77" s="120"/>
       <c r="G77" s="121"/>
       <c r="H77" s="122"/>
     </row>
-    <row r="78" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="117"/>
       <c r="C78" s="118"/>
       <c r="D78" s="118" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="E78" s="123" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="F78" s="120" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G78" s="121">
         <v>44957</v>
       </c>
       <c r="H78" s="122">
-        <v>44957</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="117"/>
       <c r="C79" s="118"/>
-      <c r="D79" s="118"/>
-      <c r="E79" s="123"/>
-      <c r="F79" s="120"/>
-      <c r="G79" s="121"/>
-      <c r="H79" s="122"/>
-    </row>
-    <row r="80" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D79" s="118" t="s">
+        <v>393</v>
+      </c>
+      <c r="E79" s="123" t="s">
+        <v>396</v>
+      </c>
+      <c r="F79" s="120" t="s">
+        <v>281</v>
+      </c>
+      <c r="G79" s="121">
+        <v>44281</v>
+      </c>
+      <c r="H79" s="122">
+        <v>44557</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="117"/>
       <c r="C80" s="118"/>
-      <c r="D80" s="118"/>
-      <c r="E80" s="119"/>
-      <c r="F80" s="120"/>
-      <c r="G80" s="121"/>
-      <c r="H80" s="122"/>
-    </row>
-    <row r="81" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D80" s="118" t="s">
+        <v>397</v>
+      </c>
+      <c r="E80" s="123" t="s">
+        <v>398</v>
+      </c>
+      <c r="F80" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G80" s="121">
+        <v>43257</v>
+      </c>
+      <c r="H80" s="122">
+        <v>43257</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="117"/>
       <c r="C81" s="118"/>
       <c r="D81" s="118" t="s">
-        <v>330</v>
-      </c>
-      <c r="E81" s="119" t="s">
-        <v>331</v>
+        <v>286</v>
+      </c>
+      <c r="E81" s="123" t="s">
+        <v>399</v>
       </c>
       <c r="F81" s="120" t="s">
         <v>232</v>
       </c>
       <c r="G81" s="121">
-        <v>44893</v>
+        <v>44949</v>
       </c>
       <c r="H81" s="122">
-        <v>44893</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="82" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -4365,27 +4410,37 @@
       <c r="B82" s="117"/>
       <c r="C82" s="118"/>
       <c r="D82" s="118"/>
-      <c r="E82" s="119"/>
+      <c r="E82" s="123"/>
       <c r="F82" s="120"/>
       <c r="G82" s="121"/>
       <c r="H82" s="122"/>
     </row>
-    <row r="83" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="117"/>
       <c r="C83" s="118"/>
-      <c r="D83" s="118"/>
-      <c r="E83" s="119"/>
-      <c r="F83" s="120"/>
-      <c r="G83" s="121"/>
-      <c r="H83" s="122"/>
+      <c r="D83" s="118" t="s">
+        <v>392</v>
+      </c>
+      <c r="E83" s="123" t="s">
+        <v>400</v>
+      </c>
+      <c r="F83" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G83" s="121">
+        <v>44957</v>
+      </c>
+      <c r="H83" s="122">
+        <v>44957</v>
+      </c>
     </row>
     <row r="84" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="117"/>
       <c r="C84" s="118"/>
       <c r="D84" s="118"/>
-      <c r="E84" s="119"/>
+      <c r="E84" s="123"/>
       <c r="F84" s="120"/>
       <c r="G84" s="121"/>
       <c r="H84" s="122"/>
@@ -4404,11 +4459,21 @@
       <c r="A86" s="1"/>
       <c r="B86" s="117"/>
       <c r="C86" s="118"/>
-      <c r="D86" s="118"/>
-      <c r="E86" s="119"/>
-      <c r="F86" s="120"/>
-      <c r="G86" s="121"/>
-      <c r="H86" s="122"/>
+      <c r="D86" s="118" t="s">
+        <v>330</v>
+      </c>
+      <c r="E86" s="119" t="s">
+        <v>331</v>
+      </c>
+      <c r="F86" s="120" t="s">
+        <v>232</v>
+      </c>
+      <c r="G86" s="121">
+        <v>44893</v>
+      </c>
+      <c r="H86" s="122">
+        <v>44893</v>
+      </c>
     </row>
     <row r="87" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
@@ -4720,65 +4785,65 @@
       <c r="G117" s="121"/>
       <c r="H117" s="122"/>
     </row>
-    <row r="118" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
-      <c r="B118" s="128"/>
-      <c r="C118" s="129"/>
-      <c r="D118" s="129"/>
-      <c r="E118" s="130"/>
-      <c r="F118" s="131"/>
-      <c r="G118" s="132"/>
-      <c r="H118" s="133"/>
+      <c r="B118" s="117"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
+      <c r="E118" s="119"/>
+      <c r="F118" s="120"/>
+      <c r="G118" s="121"/>
+      <c r="H118" s="122"/>
     </row>
     <row r="119" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
-      <c r="B119" s="1"/>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-      <c r="F119" s="134"/>
-      <c r="G119" s="135"/>
-      <c r="H119" s="135"/>
+      <c r="B119" s="117"/>
+      <c r="C119" s="118"/>
+      <c r="D119" s="118"/>
+      <c r="E119" s="119"/>
+      <c r="F119" s="120"/>
+      <c r="G119" s="121"/>
+      <c r="H119" s="122"/>
     </row>
     <row r="120" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
-      <c r="B120" s="1"/>
-      <c r="C120" s="1"/>
-      <c r="D120" s="1"/>
-      <c r="E120" s="1"/>
-      <c r="F120" s="134"/>
-      <c r="G120" s="135"/>
-      <c r="H120" s="135"/>
+      <c r="B120" s="117"/>
+      <c r="C120" s="118"/>
+      <c r="D120" s="118"/>
+      <c r="E120" s="119"/>
+      <c r="F120" s="120"/>
+      <c r="G120" s="121"/>
+      <c r="H120" s="122"/>
     </row>
     <row r="121" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
-      <c r="B121" s="1"/>
-      <c r="C121" s="1"/>
-      <c r="D121" s="1"/>
-      <c r="E121" s="1"/>
-      <c r="F121" s="134"/>
-      <c r="G121" s="135"/>
-      <c r="H121" s="135"/>
+      <c r="B121" s="117"/>
+      <c r="C121" s="118"/>
+      <c r="D121" s="118"/>
+      <c r="E121" s="119"/>
+      <c r="F121" s="120"/>
+      <c r="G121" s="121"/>
+      <c r="H121" s="122"/>
     </row>
     <row r="122" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
-      <c r="B122" s="1"/>
-      <c r="C122" s="1"/>
-      <c r="D122" s="1"/>
-      <c r="E122" s="1"/>
-      <c r="F122" s="134"/>
-      <c r="G122" s="135"/>
-      <c r="H122" s="135"/>
-    </row>
-    <row r="123" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B122" s="117"/>
+      <c r="C122" s="118"/>
+      <c r="D122" s="118"/>
+      <c r="E122" s="119"/>
+      <c r="F122" s="120"/>
+      <c r="G122" s="121"/>
+      <c r="H122" s="122"/>
+    </row>
+    <row r="123" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A123" s="1"/>
-      <c r="B123" s="1"/>
-      <c r="C123" s="1"/>
-      <c r="D123" s="1"/>
-      <c r="E123" s="1"/>
-      <c r="F123" s="134"/>
-      <c r="G123" s="135"/>
-      <c r="H123" s="135"/>
+      <c r="B123" s="124"/>
+      <c r="C123" s="125"/>
+      <c r="D123" s="125"/>
+      <c r="E123" s="126"/>
+      <c r="F123" s="127"/>
+      <c r="G123" s="128"/>
+      <c r="H123" s="129"/>
     </row>
     <row r="124" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
@@ -4786,9 +4851,9 @@
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
-      <c r="F124" s="134"/>
-      <c r="G124" s="135"/>
-      <c r="H124" s="135"/>
+      <c r="F124" s="130"/>
+      <c r="G124" s="131"/>
+      <c r="H124" s="131"/>
     </row>
     <row r="125" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
@@ -4796,9 +4861,9 @@
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
-      <c r="F125" s="134"/>
-      <c r="G125" s="135"/>
-      <c r="H125" s="135"/>
+      <c r="F125" s="130"/>
+      <c r="G125" s="131"/>
+      <c r="H125" s="131"/>
     </row>
     <row r="126" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
@@ -4806,9 +4871,9 @@
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
-      <c r="F126" s="134"/>
-      <c r="G126" s="135"/>
-      <c r="H126" s="135"/>
+      <c r="F126" s="130"/>
+      <c r="G126" s="131"/>
+      <c r="H126" s="131"/>
     </row>
     <row r="127" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
@@ -4816,9 +4881,9 @@
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
-      <c r="F127" s="134"/>
-      <c r="G127" s="135"/>
-      <c r="H127" s="135"/>
+      <c r="F127" s="130"/>
+      <c r="G127" s="131"/>
+      <c r="H127" s="131"/>
     </row>
     <row r="128" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
@@ -4826,9 +4891,9 @@
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
-      <c r="F128" s="134"/>
-      <c r="G128" s="135"/>
-      <c r="H128" s="135"/>
+      <c r="F128" s="130"/>
+      <c r="G128" s="131"/>
+      <c r="H128" s="131"/>
     </row>
     <row r="129" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A129" s="1"/>
@@ -4836,9 +4901,9 @@
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
-      <c r="F129" s="134"/>
-      <c r="G129" s="135"/>
-      <c r="H129" s="135"/>
+      <c r="F129" s="130"/>
+      <c r="G129" s="131"/>
+      <c r="H129" s="131"/>
     </row>
     <row r="130" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="1"/>
@@ -4846,9 +4911,9 @@
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
-      <c r="F130" s="134"/>
-      <c r="G130" s="135"/>
-      <c r="H130" s="135"/>
+      <c r="F130" s="130"/>
+      <c r="G130" s="131"/>
+      <c r="H130" s="131"/>
     </row>
     <row r="131" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="1"/>
@@ -4856,9 +4921,9 @@
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
-      <c r="F131" s="134"/>
-      <c r="G131" s="135"/>
-      <c r="H131" s="135"/>
+      <c r="F131" s="130"/>
+      <c r="G131" s="131"/>
+      <c r="H131" s="131"/>
     </row>
     <row r="132" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="1"/>
@@ -4866,9 +4931,9 @@
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
-      <c r="F132" s="134"/>
-      <c r="G132" s="135"/>
-      <c r="H132" s="135"/>
+      <c r="F132" s="130"/>
+      <c r="G132" s="131"/>
+      <c r="H132" s="131"/>
     </row>
     <row r="133" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="1"/>
@@ -4876,9 +4941,9 @@
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
-      <c r="F133" s="134"/>
-      <c r="G133" s="135"/>
-      <c r="H133" s="135"/>
+      <c r="F133" s="130"/>
+      <c r="G133" s="131"/>
+      <c r="H133" s="131"/>
     </row>
     <row r="134" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="1"/>
@@ -4886,24 +4951,74 @@
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
-      <c r="F134" s="134"/>
-      <c r="G134" s="135"/>
-      <c r="H134" s="135"/>
+      <c r="F134" s="130"/>
+      <c r="G134" s="131"/>
+      <c r="H134" s="131"/>
     </row>
     <row r="135" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F135" s="95"/>
-      <c r="G135" s="111"/>
-      <c r="H135" s="111"/>
+      <c r="A135" s="1"/>
+      <c r="B135" s="1"/>
+      <c r="C135" s="1"/>
+      <c r="D135" s="1"/>
+      <c r="E135" s="1"/>
+      <c r="F135" s="130"/>
+      <c r="G135" s="131"/>
+      <c r="H135" s="131"/>
     </row>
     <row r="136" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F136" s="95"/>
-      <c r="G136" s="111"/>
-      <c r="H136" s="111"/>
+      <c r="A136" s="1"/>
+      <c r="B136" s="1"/>
+      <c r="C136" s="1"/>
+      <c r="D136" s="1"/>
+      <c r="E136" s="1"/>
+      <c r="F136" s="130"/>
+      <c r="G136" s="131"/>
+      <c r="H136" s="131"/>
     </row>
     <row r="137" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="F137" s="95"/>
-      <c r="G137" s="111"/>
-      <c r="H137" s="111"/>
+      <c r="A137" s="1"/>
+      <c r="B137" s="1"/>
+      <c r="C137" s="1"/>
+      <c r="D137" s="1"/>
+      <c r="E137" s="1"/>
+      <c r="F137" s="130"/>
+      <c r="G137" s="131"/>
+      <c r="H137" s="131"/>
+    </row>
+    <row r="138" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+      <c r="C138" s="1"/>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
+      <c r="F138" s="130"/>
+      <c r="G138" s="131"/>
+      <c r="H138" s="131"/>
+    </row>
+    <row r="139" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A139" s="1"/>
+      <c r="B139" s="1"/>
+      <c r="C139" s="1"/>
+      <c r="D139" s="1"/>
+      <c r="E139" s="1"/>
+      <c r="F139" s="130"/>
+      <c r="G139" s="131"/>
+      <c r="H139" s="131"/>
+    </row>
+    <row r="140" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F140" s="95"/>
+      <c r="G140" s="111"/>
+      <c r="H140" s="111"/>
+    </row>
+    <row r="141" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F141" s="95"/>
+      <c r="G141" s="111"/>
+      <c r="H141" s="111"/>
+    </row>
+    <row r="142" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F142" s="95"/>
+      <c r="G142" s="111"/>
+      <c r="H142" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4943,20 +5058,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="185" t="s">
+      <c r="B2" s="199" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="186"/>
-      <c r="D2" s="187"/>
-      <c r="E2" s="182" t="s">
+      <c r="C2" s="200"/>
+      <c r="D2" s="201"/>
+      <c r="E2" s="196" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="184"/>
-      <c r="G2" s="182" t="s">
+      <c r="F2" s="198"/>
+      <c r="G2" s="196" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="183"/>
-      <c r="I2" s="184"/>
+      <c r="H2" s="197"/>
+      <c r="I2" s="198"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -4977,10 +5092,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="188" t="s">
+      <c r="H3" s="202" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="189"/>
+      <c r="I3" s="203"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -5010,19 +5125,19 @@
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="61"/>
-      <c r="C5" s="173" t="s">
+      <c r="C5" s="187" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="176" t="s">
+      <c r="D5" s="190" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="179" t="s">
+      <c r="F5" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="170" t="s">
+      <c r="G5" s="184" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -5034,23 +5149,23 @@
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61"/>
-      <c r="C6" s="174"/>
-      <c r="D6" s="177"/>
+      <c r="C6" s="188"/>
+      <c r="D6" s="191"/>
       <c r="E6" s="35"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="171"/>
-      <c r="H6" s="165" t="s">
+      <c r="F6" s="194"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="166"/>
+      <c r="I6" s="180"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
-      <c r="C7" s="175"/>
-      <c r="D7" s="178"/>
+      <c r="C7" s="189"/>
+      <c r="D7" s="192"/>
       <c r="E7" s="36"/>
-      <c r="F7" s="181"/>
-      <c r="G7" s="172"/>
+      <c r="F7" s="195"/>
+      <c r="G7" s="186"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -5084,19 +5199,19 @@
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="176" t="s">
+      <c r="D9" s="190" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="167" t="s">
+      <c r="E9" s="181" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="179" t="s">
+      <c r="F9" s="193" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="170" t="s">
+      <c r="G9" s="184" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -5109,24 +5224,24 @@
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
-      <c r="C10" s="174"/>
-      <c r="D10" s="177"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="171"/>
-      <c r="H10" s="165" t="s">
+      <c r="C10" s="188"/>
+      <c r="D10" s="191"/>
+      <c r="E10" s="182"/>
+      <c r="F10" s="194"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="166"/>
+      <c r="I10" s="180"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
-      <c r="C11" s="175"/>
-      <c r="D11" s="178"/>
-      <c r="E11" s="169"/>
-      <c r="F11" s="181"/>
-      <c r="G11" s="172"/>
+      <c r="C11" s="189"/>
+      <c r="D11" s="192"/>
+      <c r="E11" s="183"/>
+      <c r="F11" s="195"/>
+      <c r="G11" s="186"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -5136,10 +5251,10 @@
     </row>
     <row r="12" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B12" s="61"/>
-      <c r="C12" s="173" t="s">
+      <c r="C12" s="187" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="176" t="s">
+      <c r="D12" s="190" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="37" t="s">
@@ -5148,7 +5263,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="170" t="s">
+      <c r="G12" s="184" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -5160,15 +5275,15 @@
     </row>
     <row r="13" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B13" s="61"/>
-      <c r="C13" s="175"/>
-      <c r="D13" s="178"/>
+      <c r="C13" s="189"/>
+      <c r="D13" s="192"/>
       <c r="E13" s="37" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="172"/>
+      <c r="G13" s="186"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -5213,8 +5328,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="164"/>
+      <c r="H16" s="177"/>
+      <c r="I16" s="178"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -5628,19 +5743,19 @@
     </row>
     <row r="40" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B40" s="61"/>
-      <c r="C40" s="173" t="s">
+      <c r="C40" s="187" t="s">
         <v>42</v>
       </c>
-      <c r="D40" s="176" t="s">
+      <c r="D40" s="190" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="167" t="s">
+      <c r="E40" s="181" t="s">
         <v>45</v>
       </c>
-      <c r="F40" s="179" t="s">
+      <c r="F40" s="193" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="170" t="s">
+      <c r="G40" s="184" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -5652,23 +5767,23 @@
     </row>
     <row r="41" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="61"/>
-      <c r="C41" s="174"/>
-      <c r="D41" s="177"/>
-      <c r="E41" s="168"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="171"/>
-      <c r="H41" s="165" t="s">
+      <c r="C41" s="188"/>
+      <c r="D41" s="191"/>
+      <c r="E41" s="182"/>
+      <c r="F41" s="194"/>
+      <c r="G41" s="185"/>
+      <c r="H41" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="166"/>
+      <c r="I41" s="180"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
-      <c r="C42" s="175"/>
-      <c r="D42" s="178"/>
-      <c r="E42" s="169"/>
-      <c r="F42" s="181"/>
-      <c r="G42" s="172"/>
+      <c r="C42" s="189"/>
+      <c r="D42" s="192"/>
+      <c r="E42" s="183"/>
+      <c r="F42" s="195"/>
+      <c r="G42" s="186"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -5702,19 +5817,19 @@
     </row>
     <row r="44" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B44" s="61"/>
-      <c r="C44" s="173" t="s">
+      <c r="C44" s="187" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="176" t="s">
+      <c r="D44" s="190" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="167" t="s">
+      <c r="E44" s="181" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="179" t="s">
+      <c r="F44" s="193" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="170" t="s">
+      <c r="G44" s="184" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -5726,23 +5841,23 @@
     </row>
     <row r="45" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="61"/>
-      <c r="C45" s="174"/>
-      <c r="D45" s="177"/>
-      <c r="E45" s="168"/>
-      <c r="F45" s="180"/>
-      <c r="G45" s="171"/>
-      <c r="H45" s="165" t="s">
+      <c r="C45" s="188"/>
+      <c r="D45" s="191"/>
+      <c r="E45" s="182"/>
+      <c r="F45" s="194"/>
+      <c r="G45" s="185"/>
+      <c r="H45" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="166"/>
+      <c r="I45" s="180"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
-      <c r="C46" s="175"/>
-      <c r="D46" s="178"/>
-      <c r="E46" s="169"/>
-      <c r="F46" s="181"/>
-      <c r="G46" s="172"/>
+      <c r="C46" s="189"/>
+      <c r="D46" s="192"/>
+      <c r="E46" s="183"/>
+      <c r="F46" s="195"/>
+      <c r="G46" s="186"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -5767,8 +5882,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="163"/>
-      <c r="I48" s="164"/>
+      <c r="H48" s="177"/>
+      <c r="I48" s="178"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -5831,10 +5946,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="165" t="s">
+      <c r="H52" s="179" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="166"/>
+      <c r="I52" s="180"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -5867,35 +5982,35 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="163"/>
-      <c r="I55" s="164"/>
+      <c r="H55" s="177"/>
+      <c r="I55" s="178"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="64" t="s">
         <v>146</v>
       </c>
-      <c r="C56" s="149" t="s">
+      <c r="C56" s="145" t="s">
         <v>374</v>
       </c>
-      <c r="D56" s="150" t="s">
+      <c r="D56" s="146" t="s">
         <v>379</v>
       </c>
       <c r="E56" s="42" t="s">
         <v>380</v>
       </c>
-      <c r="F56" s="151" t="s">
+      <c r="F56" s="147" t="s">
         <v>382</v>
       </c>
-      <c r="G56" s="148"/>
+      <c r="G56" s="144"/>
       <c r="H56" s="8"/>
       <c r="I56" s="17"/>
     </row>
     <row r="57" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="61"/>
-      <c r="C57" s="149" t="s">
+      <c r="C57" s="145" t="s">
         <v>375</v>
       </c>
-      <c r="D57" s="145" t="s">
+      <c r="D57" s="141" t="s">
         <v>377</v>
       </c>
       <c r="E57" s="45"/>
@@ -5906,28 +6021,28 @@
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="64"/>
-      <c r="C58" s="149" t="s">
+      <c r="C58" s="145" t="s">
         <v>376</v>
       </c>
-      <c r="D58" s="150" t="s">
+      <c r="D58" s="146" t="s">
         <v>378</v>
       </c>
       <c r="E58" s="42" t="s">
         <v>381</v>
       </c>
-      <c r="F58" s="151" t="s">
+      <c r="F58" s="147" t="s">
         <v>383</v>
       </c>
-      <c r="G58" s="148"/>
+      <c r="G58" s="144"/>
       <c r="H58" s="8"/>
       <c r="I58" s="17"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
-      <c r="C59" s="139" t="s">
+      <c r="C59" s="135" t="s">
         <v>309</v>
       </c>
-      <c r="D59" s="141" t="s">
+      <c r="D59" s="137" t="s">
         <v>310</v>
       </c>
       <c r="E59" s="45"/>
@@ -5938,28 +6053,28 @@
     </row>
     <row r="60" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="64"/>
-      <c r="C60" s="139" t="s">
+      <c r="C60" s="135" t="s">
         <v>311</v>
       </c>
-      <c r="D60" s="141" t="s">
+      <c r="D60" s="137" t="s">
         <v>313</v>
       </c>
       <c r="E60" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="F60" s="143" t="s">
+      <c r="F60" s="139" t="s">
         <v>320</v>
       </c>
-      <c r="G60" s="137"/>
+      <c r="G60" s="133"/>
       <c r="H60" s="8"/>
       <c r="I60" s="17"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="64"/>
-      <c r="C61" s="139" t="s">
+      <c r="C61" s="135" t="s">
         <v>312</v>
       </c>
-      <c r="D61" s="141" t="s">
+      <c r="D61" s="137" t="s">
         <v>314</v>
       </c>
       <c r="E61" s="45"/>
@@ -5970,124 +6085,124 @@
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="64"/>
-      <c r="C62" s="144" t="s">
+      <c r="C62" s="140" t="s">
         <v>344</v>
       </c>
-      <c r="D62" s="145" t="s">
+      <c r="D62" s="141" t="s">
         <v>346</v>
       </c>
       <c r="E62" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="F62" s="146" t="s">
+      <c r="F62" s="142" t="s">
         <v>320</v>
       </c>
-      <c r="G62" s="147"/>
+      <c r="G62" s="143"/>
       <c r="H62" s="8"/>
       <c r="I62" s="17"/>
     </row>
     <row r="63" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B63" s="64"/>
-      <c r="C63" s="144" t="s">
+      <c r="C63" s="140" t="s">
         <v>345</v>
       </c>
-      <c r="D63" s="145" t="s">
+      <c r="D63" s="141" t="s">
         <v>347</v>
       </c>
       <c r="E63" s="42" t="s">
         <v>348</v>
       </c>
-      <c r="F63" s="146" t="s">
+      <c r="F63" s="142" t="s">
         <v>349</v>
       </c>
-      <c r="G63" s="147"/>
+      <c r="G63" s="143"/>
       <c r="H63" s="8"/>
       <c r="I63" s="17"/>
     </row>
     <row r="64" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="64"/>
-      <c r="C64" s="139" t="s">
+      <c r="C64" s="135" t="s">
         <v>315</v>
       </c>
-      <c r="D64" s="141" t="s">
+      <c r="D64" s="137" t="s">
         <v>316</v>
       </c>
       <c r="E64" s="42" t="s">
         <v>317</v>
       </c>
-      <c r="F64" s="143" t="s">
+      <c r="F64" s="139" t="s">
         <v>318</v>
       </c>
-      <c r="G64" s="137"/>
+      <c r="G64" s="133"/>
       <c r="H64" s="8"/>
       <c r="I64" s="17"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64"/>
-      <c r="C65" s="144" t="s">
+      <c r="C65" s="140" t="s">
         <v>351</v>
       </c>
-      <c r="D65" s="145"/>
+      <c r="D65" s="141"/>
       <c r="E65" s="42"/>
-      <c r="F65" s="146"/>
-      <c r="G65" s="147"/>
+      <c r="F65" s="142"/>
+      <c r="G65" s="143"/>
       <c r="H65" s="8"/>
       <c r="I65" s="17"/>
     </row>
     <row r="66" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="64"/>
-      <c r="C66" s="144" t="s">
+      <c r="C66" s="140" t="s">
         <v>352</v>
       </c>
-      <c r="D66" s="145"/>
+      <c r="D66" s="141"/>
       <c r="E66" s="42"/>
-      <c r="F66" s="146"/>
-      <c r="G66" s="147"/>
+      <c r="F66" s="142"/>
+      <c r="G66" s="143"/>
       <c r="H66" s="8"/>
       <c r="I66" s="17"/>
     </row>
     <row r="67" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="64"/>
-      <c r="C67" s="144" t="s">
+      <c r="C67" s="140" t="s">
         <v>350</v>
       </c>
-      <c r="D67" s="145" t="s">
+      <c r="D67" s="141" t="s">
         <v>353</v>
       </c>
       <c r="E67" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="F67" s="146" t="s">
+      <c r="F67" s="142" t="s">
         <v>355</v>
       </c>
-      <c r="G67" s="147"/>
+      <c r="G67" s="143"/>
       <c r="H67" s="8"/>
       <c r="I67" s="17"/>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B68" s="64"/>
-      <c r="C68" s="144" t="s">
+      <c r="C68" s="140" t="s">
         <v>356</v>
       </c>
-      <c r="D68" s="145" t="s">
+      <c r="D68" s="141" t="s">
         <v>357</v>
       </c>
       <c r="E68" s="42" t="s">
         <v>354</v>
       </c>
-      <c r="F68" s="146" t="s">
+      <c r="F68" s="142" t="s">
         <v>355</v>
       </c>
-      <c r="G68" s="147"/>
+      <c r="G68" s="143"/>
       <c r="H68" s="8"/>
       <c r="I68" s="17"/>
     </row>
     <row r="69" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B69" s="64"/>
-      <c r="C69" s="144" t="s">
+      <c r="C69" s="140" t="s">
         <v>358</v>
       </c>
-      <c r="D69" s="145" t="s">
+      <c r="D69" s="141" t="s">
         <v>359</v>
       </c>
       <c r="E69" s="45"/>
@@ -6098,28 +6213,28 @@
     </row>
     <row r="70" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B70" s="64"/>
-      <c r="C70" s="144" t="s">
+      <c r="C70" s="140" t="s">
         <v>360</v>
       </c>
-      <c r="D70" s="145" t="s">
+      <c r="D70" s="141" t="s">
         <v>362</v>
       </c>
       <c r="E70" s="42" t="s">
         <v>364</v>
       </c>
-      <c r="F70" s="146" t="s">
+      <c r="F70" s="142" t="s">
         <v>365</v>
       </c>
-      <c r="G70" s="147"/>
+      <c r="G70" s="143"/>
       <c r="H70" s="8"/>
       <c r="I70" s="17"/>
     </row>
     <row r="71" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B71" s="64"/>
-      <c r="C71" s="144" t="s">
+      <c r="C71" s="140" t="s">
         <v>361</v>
       </c>
-      <c r="D71" s="145" t="s">
+      <c r="D71" s="141" t="s">
         <v>363</v>
       </c>
       <c r="E71" s="45"/>
@@ -6130,10 +6245,10 @@
     </row>
     <row r="72" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="64"/>
-      <c r="C72" s="144" t="s">
+      <c r="C72" s="140" t="s">
         <v>366</v>
       </c>
-      <c r="D72" s="145" t="s">
+      <c r="D72" s="141" t="s">
         <v>369</v>
       </c>
       <c r="E72" s="45"/>
@@ -6144,28 +6259,28 @@
     </row>
     <row r="73" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="64"/>
-      <c r="C73" s="144" t="s">
+      <c r="C73" s="140" t="s">
         <v>367</v>
       </c>
-      <c r="D73" s="145" t="s">
+      <c r="D73" s="141" t="s">
         <v>370</v>
       </c>
       <c r="E73" s="42" t="s">
         <v>372</v>
       </c>
-      <c r="F73" s="146" t="s">
+      <c r="F73" s="142" t="s">
         <v>373</v>
       </c>
-      <c r="G73" s="147"/>
+      <c r="G73" s="143"/>
       <c r="H73" s="8"/>
       <c r="I73" s="17"/>
     </row>
     <row r="74" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="64"/>
-      <c r="C74" s="144" t="s">
+      <c r="C74" s="140" t="s">
         <v>368</v>
       </c>
-      <c r="D74" s="145" t="s">
+      <c r="D74" s="141" t="s">
         <v>371</v>
       </c>
       <c r="E74" s="45"/>
@@ -6176,10 +6291,10 @@
     </row>
     <row r="75" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="64"/>
-      <c r="C75" s="152" t="s">
+      <c r="C75" s="148" t="s">
         <v>384</v>
       </c>
-      <c r="D75" s="153" t="s">
+      <c r="D75" s="149" t="s">
         <v>385</v>
       </c>
       <c r="E75" s="45"/>
@@ -6190,87 +6305,87 @@
     </row>
     <row r="76" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B76" s="64"/>
-      <c r="C76" s="152" t="s">
+      <c r="C76" s="148" t="s">
         <v>386</v>
       </c>
-      <c r="D76" s="153" t="s">
+      <c r="D76" s="149" t="s">
         <v>391</v>
       </c>
       <c r="E76" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="F76" s="154" t="s">
+      <c r="F76" s="150" t="s">
         <v>91</v>
       </c>
-      <c r="G76" s="155"/>
+      <c r="G76" s="151"/>
       <c r="H76" s="8"/>
       <c r="I76" s="17"/>
     </row>
     <row r="77" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B77" s="64"/>
-      <c r="C77" s="152" t="s">
+      <c r="C77" s="148" t="s">
         <v>387</v>
       </c>
-      <c r="D77" s="153" t="s">
+      <c r="D77" s="149" t="s">
         <v>390</v>
       </c>
       <c r="E77" s="42" t="s">
         <v>388</v>
       </c>
-      <c r="F77" s="154" t="s">
+      <c r="F77" s="150" t="s">
         <v>389</v>
       </c>
-      <c r="G77" s="155"/>
+      <c r="G77" s="151"/>
       <c r="H77" s="8"/>
       <c r="I77" s="17"/>
     </row>
     <row r="78" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="64"/>
-      <c r="C78" s="152"/>
-      <c r="D78" s="153"/>
+      <c r="C78" s="148"/>
+      <c r="D78" s="149"/>
       <c r="E78" s="42"/>
-      <c r="F78" s="154"/>
-      <c r="G78" s="155"/>
+      <c r="F78" s="150"/>
+      <c r="G78" s="151"/>
       <c r="H78" s="8"/>
       <c r="I78" s="17"/>
     </row>
     <row r="79" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="64"/>
-      <c r="C79" s="152"/>
-      <c r="D79" s="153"/>
+      <c r="C79" s="148"/>
+      <c r="D79" s="149"/>
       <c r="E79" s="42"/>
-      <c r="F79" s="154"/>
-      <c r="G79" s="155"/>
+      <c r="F79" s="150"/>
+      <c r="G79" s="151"/>
       <c r="H79" s="8"/>
       <c r="I79" s="17"/>
     </row>
     <row r="80" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="64"/>
-      <c r="C80" s="152"/>
-      <c r="D80" s="153"/>
+      <c r="C80" s="148"/>
+      <c r="D80" s="149"/>
       <c r="E80" s="42"/>
-      <c r="F80" s="154"/>
-      <c r="G80" s="155"/>
+      <c r="F80" s="150"/>
+      <c r="G80" s="151"/>
       <c r="H80" s="8"/>
       <c r="I80" s="17"/>
     </row>
     <row r="81" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="64"/>
-      <c r="C81" s="152"/>
-      <c r="D81" s="153"/>
+      <c r="C81" s="148"/>
+      <c r="D81" s="149"/>
       <c r="E81" s="42"/>
-      <c r="F81" s="154"/>
-      <c r="G81" s="155"/>
+      <c r="F81" s="150"/>
+      <c r="G81" s="151"/>
       <c r="H81" s="8"/>
       <c r="I81" s="17"/>
     </row>
     <row r="82" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="64"/>
-      <c r="C82" s="138"/>
-      <c r="D82" s="140"/>
+      <c r="C82" s="134"/>
+      <c r="D82" s="136"/>
       <c r="E82" s="39"/>
-      <c r="F82" s="142"/>
-      <c r="G82" s="136"/>
+      <c r="F82" s="138"/>
+      <c r="G82" s="132"/>
       <c r="H82" s="9"/>
       <c r="I82" s="19"/>
     </row>
@@ -6281,8 +6396,8 @@
       <c r="E83" s="25"/>
       <c r="F83" s="22"/>
       <c r="G83" s="25"/>
-      <c r="H83" s="163"/>
-      <c r="I83" s="164"/>
+      <c r="H83" s="177"/>
+      <c r="I83" s="178"/>
     </row>
     <row r="84" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="61"/>
@@ -6489,14 +6604,14 @@
   <sheetData>
     <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="190" t="s">
+      <c r="B2" s="204" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="191"/>
-      <c r="D2" s="183" t="s">
+      <c r="C2" s="205"/>
+      <c r="D2" s="197" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="184" t="s">
+      <c r="E2" s="198" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6507,8 +6622,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="188"/>
-      <c r="E3" s="189"/>
+      <c r="D3" s="202"/>
+      <c r="E3" s="203"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">
@@ -6970,7 +7085,7 @@
       <c r="B2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="192" t="s">
+      <c r="C2" s="206" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6978,7 +7093,7 @@
       <c r="B3" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="193"/>
+      <c r="C3" s="207"/>
     </row>
     <row r="4" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="89" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 08 Februari 2023 16:16 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="922" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="634">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -1985,6 +1985,30 @@
   </si>
   <si>
     <t>Mendapatkan Data Entities untuk Edge Work Flow berdasarkan ID (varID).
+Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
+Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
+  </si>
+  <si>
+    <t>Func_GetDataEntities_AppObject_WorkFlow</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Entities untuk Work Flow berdasarkan ID (varID).
+Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
+Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
+  </si>
+  <si>
+    <t>Func_GetDataEntities_AppObject_WorkFlowVersion</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Entities untuk Versi Work Flow berdasarkan ID (varID).
+Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
+Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
+  </si>
+  <si>
+    <t>Func_GetDataEntities_AppObject_WorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Entities untuk Jalur Work Flow berdasarkan ID (varID).
 Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
 Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
   </si>
@@ -3667,13 +3691,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H364"/>
+  <dimension ref="A1:H367"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E238" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E242" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E240" sqref="E240"/>
+      <selection pane="bottomRight" activeCell="E243" sqref="E243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7215,10 +7239,10 @@
       <c r="B240" s="111"/>
       <c r="C240" s="112"/>
       <c r="D240" s="148" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
       <c r="E240" s="214" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="F240" s="149" t="s">
         <v>232</v>
@@ -7235,39 +7259,39 @@
       <c r="B241" s="111"/>
       <c r="C241" s="112"/>
       <c r="D241" s="148" t="s">
-        <v>576</v>
+        <v>626</v>
       </c>
       <c r="E241" s="214" t="s">
-        <v>577</v>
+        <v>627</v>
       </c>
       <c r="F241" s="149" t="s">
         <v>232</v>
       </c>
       <c r="G241" s="150">
-        <v>44964</v>
+        <v>44965</v>
       </c>
       <c r="H241" s="151">
-        <v>44964</v>
+        <v>44965</v>
       </c>
     </row>
     <row r="242" spans="1:8" s="78" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A242" s="1"/>
       <c r="B242" s="111"/>
       <c r="C242" s="112"/>
-      <c r="D242" s="143" t="s">
-        <v>593</v>
-      </c>
-      <c r="E242" s="215" t="s">
-        <v>594</v>
-      </c>
-      <c r="F242" s="144" t="s">
-        <v>281</v>
-      </c>
-      <c r="G242" s="145">
-        <v>44964</v>
-      </c>
-      <c r="H242" s="146">
-        <v>44901</v>
+      <c r="D242" s="148" t="s">
+        <v>632</v>
+      </c>
+      <c r="E242" s="214" t="s">
+        <v>633</v>
+      </c>
+      <c r="F242" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G242" s="150">
+        <v>44965</v>
+      </c>
+      <c r="H242" s="151">
+        <v>44965</v>
       </c>
     </row>
     <row r="243" spans="1:8" s="78" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
@@ -7275,279 +7299,299 @@
       <c r="B243" s="111"/>
       <c r="C243" s="112"/>
       <c r="D243" s="148" t="s">
-        <v>622</v>
+        <v>576</v>
       </c>
       <c r="E243" s="214" t="s">
-        <v>624</v>
+        <v>577</v>
       </c>
       <c r="F243" s="149" t="s">
         <v>232</v>
       </c>
       <c r="G243" s="150">
-        <v>44965</v>
+        <v>44964</v>
       </c>
       <c r="H243" s="151">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="244" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" s="78" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A244" s="1"/>
       <c r="B244" s="111"/>
       <c r="C244" s="112"/>
-      <c r="D244" s="112" t="s">
-        <v>623</v>
-      </c>
-      <c r="E244" s="216" t="s">
-        <v>625</v>
-      </c>
-      <c r="F244" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G244" s="114">
-        <v>44965</v>
-      </c>
-      <c r="H244" s="115">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="245" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D244" s="143" t="s">
+        <v>593</v>
+      </c>
+      <c r="E244" s="215" t="s">
+        <v>594</v>
+      </c>
+      <c r="F244" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="G244" s="145">
+        <v>44964</v>
+      </c>
+      <c r="H244" s="146">
+        <v>44901</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" s="78" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A245" s="1"/>
       <c r="B245" s="111"/>
       <c r="C245" s="112"/>
-      <c r="D245" s="163"/>
-      <c r="E245" s="213"/>
-      <c r="F245" s="163"/>
-      <c r="G245" s="163"/>
-      <c r="H245" s="164"/>
-    </row>
-    <row r="246" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D245" s="148" t="s">
+        <v>630</v>
+      </c>
+      <c r="E245" s="214" t="s">
+        <v>631</v>
+      </c>
+      <c r="F245" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G245" s="150">
+        <v>44965</v>
+      </c>
+      <c r="H245" s="151">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" s="78" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A246" s="1"/>
       <c r="B246" s="111"/>
       <c r="C246" s="112"/>
-      <c r="D246" s="112" t="s">
-        <v>339</v>
-      </c>
-      <c r="E246" s="216" t="s">
-        <v>340</v>
-      </c>
-      <c r="F246" s="113" t="s">
+      <c r="D246" s="148" t="s">
+        <v>622</v>
+      </c>
+      <c r="E246" s="214" t="s">
+        <v>624</v>
+      </c>
+      <c r="F246" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G246" s="114">
-        <v>44951</v>
-      </c>
-      <c r="H246" s="115">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="247" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G246" s="150">
+        <v>44965</v>
+      </c>
+      <c r="H246" s="151">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A247" s="1"/>
       <c r="B247" s="111"/>
       <c r="C247" s="112"/>
-      <c r="D247" s="163"/>
-      <c r="E247" s="213"/>
-      <c r="F247" s="163"/>
-      <c r="G247" s="163"/>
-      <c r="H247" s="164"/>
-    </row>
-    <row r="248" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D247" s="112" t="s">
+        <v>623</v>
+      </c>
+      <c r="E247" s="216" t="s">
+        <v>625</v>
+      </c>
+      <c r="F247" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G247" s="114">
+        <v>44965</v>
+      </c>
+      <c r="H247" s="115">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1"/>
       <c r="B248" s="111"/>
       <c r="C248" s="112"/>
-      <c r="D248" s="112" t="s">
-        <v>341</v>
-      </c>
-      <c r="E248" s="216" t="s">
-        <v>342</v>
-      </c>
-      <c r="F248" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G248" s="114">
-        <v>44952</v>
-      </c>
-      <c r="H248" s="115">
-        <v>44952</v>
-      </c>
-    </row>
-    <row r="249" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D248" s="163"/>
+      <c r="E248" s="213"/>
+      <c r="F248" s="163"/>
+      <c r="G248" s="163"/>
+      <c r="H248" s="164"/>
+    </row>
+    <row r="249" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="B249" s="111"/>
       <c r="C249" s="112"/>
-      <c r="D249" s="112"/>
-      <c r="E249" s="212"/>
-      <c r="F249" s="113"/>
-      <c r="G249" s="114"/>
-      <c r="H249" s="115"/>
-    </row>
-    <row r="250" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D249" s="112" t="s">
+        <v>339</v>
+      </c>
+      <c r="E249" s="216" t="s">
+        <v>340</v>
+      </c>
+      <c r="F249" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G249" s="114">
+        <v>44951</v>
+      </c>
+      <c r="H249" s="115">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="1"/>
       <c r="B250" s="111"/>
       <c r="C250" s="112"/>
-      <c r="D250" s="112"/>
-      <c r="E250" s="212"/>
-      <c r="F250" s="113"/>
-      <c r="G250" s="114"/>
-      <c r="H250" s="115"/>
-    </row>
-    <row r="251" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D250" s="163"/>
+      <c r="E250" s="213"/>
+      <c r="F250" s="163"/>
+      <c r="G250" s="163"/>
+      <c r="H250" s="164"/>
+    </row>
+    <row r="251" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A251" s="1"/>
       <c r="B251" s="111"/>
       <c r="C251" s="112"/>
-      <c r="D251" s="112"/>
-      <c r="E251" s="212"/>
-      <c r="F251" s="113"/>
-      <c r="G251" s="114"/>
-      <c r="H251" s="115"/>
-    </row>
-    <row r="252" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D251" s="112" t="s">
+        <v>341</v>
+      </c>
+      <c r="E251" s="216" t="s">
+        <v>342</v>
+      </c>
+      <c r="F251" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G251" s="114">
+        <v>44952</v>
+      </c>
+      <c r="H251" s="115">
+        <v>44952</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="B252" s="111"/>
       <c r="C252" s="112"/>
-      <c r="D252" s="112" t="s">
-        <v>393</v>
-      </c>
-      <c r="E252" s="216" t="s">
-        <v>394</v>
-      </c>
-      <c r="F252" s="113" t="s">
-        <v>267</v>
-      </c>
-      <c r="G252" s="114">
-        <v>44957</v>
-      </c>
-      <c r="H252" s="115">
-        <v>42982</v>
-      </c>
-    </row>
-    <row r="253" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D252" s="112"/>
+      <c r="E252" s="212"/>
+      <c r="F252" s="113"/>
+      <c r="G252" s="114"/>
+      <c r="H252" s="115"/>
+    </row>
+    <row r="253" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="B253" s="111"/>
       <c r="C253" s="112"/>
-      <c r="D253" s="112" t="s">
-        <v>392</v>
-      </c>
-      <c r="E253" s="216" t="s">
-        <v>395</v>
-      </c>
-      <c r="F253" s="113" t="s">
-        <v>281</v>
-      </c>
-      <c r="G253" s="114">
-        <v>44281</v>
-      </c>
-      <c r="H253" s="115">
-        <v>44557</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D253" s="112"/>
+      <c r="E253" s="212"/>
+      <c r="F253" s="113"/>
+      <c r="G253" s="114"/>
+      <c r="H253" s="115"/>
+    </row>
+    <row r="254" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="B254" s="111"/>
       <c r="C254" s="112"/>
-      <c r="D254" s="112" t="s">
-        <v>396</v>
-      </c>
-      <c r="E254" s="216" t="s">
-        <v>397</v>
-      </c>
-      <c r="F254" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G254" s="114">
-        <v>43257</v>
-      </c>
-      <c r="H254" s="115">
-        <v>43257</v>
-      </c>
+      <c r="D254" s="112"/>
+      <c r="E254" s="212"/>
+      <c r="F254" s="113"/>
+      <c r="G254" s="114"/>
+      <c r="H254" s="115"/>
     </row>
     <row r="255" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="B255" s="111"/>
       <c r="C255" s="112"/>
       <c r="D255" s="112" t="s">
-        <v>285</v>
+        <v>393</v>
       </c>
       <c r="E255" s="216" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F255" s="113" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G255" s="114">
-        <v>44949</v>
+        <v>44957</v>
       </c>
       <c r="H255" s="115">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="B256" s="111"/>
       <c r="C256" s="112"/>
-      <c r="D256" s="112"/>
-      <c r="E256" s="216"/>
-      <c r="F256" s="113"/>
-      <c r="G256" s="114"/>
-      <c r="H256" s="115"/>
+      <c r="D256" s="112" t="s">
+        <v>392</v>
+      </c>
+      <c r="E256" s="216" t="s">
+        <v>395</v>
+      </c>
+      <c r="F256" s="113" t="s">
+        <v>281</v>
+      </c>
+      <c r="G256" s="114">
+        <v>44281</v>
+      </c>
+      <c r="H256" s="115">
+        <v>44557</v>
+      </c>
     </row>
     <row r="257" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A257" s="1"/>
       <c r="B257" s="111"/>
       <c r="C257" s="112"/>
       <c r="D257" s="112" t="s">
-        <v>391</v>
+        <v>396</v>
       </c>
       <c r="E257" s="216" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="F257" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G257" s="114">
-        <v>44957</v>
+        <v>43257</v>
       </c>
       <c r="H257" s="115">
-        <v>44957</v>
-      </c>
-    </row>
-    <row r="258" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>43257</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="B258" s="111"/>
       <c r="C258" s="112"/>
-      <c r="D258" s="112"/>
-      <c r="E258" s="216"/>
-      <c r="F258" s="113"/>
-      <c r="G258" s="114"/>
-      <c r="H258" s="115"/>
+      <c r="D258" s="112" t="s">
+        <v>285</v>
+      </c>
+      <c r="E258" s="216" t="s">
+        <v>398</v>
+      </c>
+      <c r="F258" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G258" s="114">
+        <v>44949</v>
+      </c>
+      <c r="H258" s="115">
+        <v>44949</v>
+      </c>
     </row>
     <row r="259" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="B259" s="111"/>
       <c r="C259" s="112"/>
       <c r="D259" s="112"/>
-      <c r="E259" s="212"/>
+      <c r="E259" s="216"/>
       <c r="F259" s="113"/>
       <c r="G259" s="114"/>
       <c r="H259" s="115"/>
     </row>
-    <row r="260" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A260" s="1"/>
       <c r="B260" s="111"/>
       <c r="C260" s="112"/>
       <c r="D260" s="112" t="s">
-        <v>329</v>
-      </c>
-      <c r="E260" s="212" t="s">
-        <v>330</v>
+        <v>391</v>
+      </c>
+      <c r="E260" s="216" t="s">
+        <v>399</v>
       </c>
       <c r="F260" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G260" s="114">
-        <v>44893</v>
+        <v>44957</v>
       </c>
       <c r="H260" s="115">
-        <v>44893</v>
+        <v>44957</v>
       </c>
     </row>
     <row r="261" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -7555,104 +7599,112 @@
       <c r="B261" s="111"/>
       <c r="C261" s="112"/>
       <c r="D261" s="112"/>
-      <c r="E261" s="212"/>
+      <c r="E261" s="216"/>
       <c r="F261" s="113"/>
       <c r="G261" s="114"/>
       <c r="H261" s="115"/>
     </row>
-    <row r="262" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A262" s="154"/>
-      <c r="B262" s="173" t="s">
-        <v>143</v>
-      </c>
-      <c r="C262" s="152"/>
-      <c r="D262" s="152"/>
-      <c r="E262" s="211"/>
-      <c r="F262" s="152"/>
-      <c r="G262" s="152"/>
-      <c r="H262" s="153"/>
-    </row>
-    <row r="263" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A263" s="154"/>
-      <c r="B263" s="173"/>
-      <c r="C263" s="174" t="s">
-        <v>160</v>
-      </c>
-      <c r="D263" s="152"/>
-      <c r="E263" s="211"/>
-      <c r="F263" s="152"/>
-      <c r="G263" s="152"/>
-      <c r="H263" s="153"/>
+    <row r="262" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A262" s="1"/>
+      <c r="B262" s="111"/>
+      <c r="C262" s="112"/>
+      <c r="D262" s="112"/>
+      <c r="E262" s="212"/>
+      <c r="F262" s="113"/>
+      <c r="G262" s="114"/>
+      <c r="H262" s="115"/>
+    </row>
+    <row r="263" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A263" s="1"/>
+      <c r="B263" s="111"/>
+      <c r="C263" s="112"/>
+      <c r="D263" s="112" t="s">
+        <v>329</v>
+      </c>
+      <c r="E263" s="212" t="s">
+        <v>330</v>
+      </c>
+      <c r="F263" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G263" s="114">
+        <v>44893</v>
+      </c>
+      <c r="H263" s="115">
+        <v>44893</v>
+      </c>
     </row>
     <row r="264" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="B264" s="111"/>
-      <c r="C264" s="174"/>
+      <c r="C264" s="112"/>
       <c r="D264" s="112"/>
       <c r="E264" s="212"/>
       <c r="F264" s="113"/>
       <c r="G264" s="114"/>
       <c r="H264" s="115"/>
     </row>
-    <row r="265" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A265" s="1"/>
-      <c r="B265" s="111"/>
-      <c r="C265" s="112"/>
-      <c r="D265" s="112"/>
-      <c r="E265" s="212"/>
-      <c r="F265" s="113"/>
-      <c r="G265" s="114"/>
-      <c r="H265" s="115"/>
-    </row>
-    <row r="266" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A265" s="154"/>
+      <c r="B265" s="173" t="s">
+        <v>143</v>
+      </c>
+      <c r="C265" s="152"/>
+      <c r="D265" s="152"/>
+      <c r="E265" s="211"/>
+      <c r="F265" s="152"/>
+      <c r="G265" s="152"/>
+      <c r="H265" s="153"/>
+    </row>
+    <row r="266" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A266" s="154"/>
-      <c r="B266" s="173" t="s">
-        <v>142</v>
-      </c>
-      <c r="C266" s="152"/>
+      <c r="B266" s="173"/>
+      <c r="C266" s="174" t="s">
+        <v>160</v>
+      </c>
       <c r="D266" s="152"/>
       <c r="E266" s="211"/>
       <c r="F266" s="152"/>
       <c r="G266" s="152"/>
       <c r="H266" s="153"/>
     </row>
-    <row r="267" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A267" s="154"/>
-      <c r="B267" s="173"/>
-      <c r="C267" s="174" t="s">
-        <v>148</v>
-      </c>
-      <c r="D267" s="152"/>
-      <c r="E267" s="211"/>
-      <c r="F267" s="152"/>
-      <c r="G267" s="152"/>
-      <c r="H267" s="153"/>
+    <row r="267" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A267" s="1"/>
+      <c r="B267" s="111"/>
+      <c r="C267" s="174"/>
+      <c r="D267" s="112"/>
+      <c r="E267" s="212"/>
+      <c r="F267" s="113"/>
+      <c r="G267" s="114"/>
+      <c r="H267" s="115"/>
     </row>
     <row r="268" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="B268" s="111"/>
-      <c r="C268" s="174"/>
+      <c r="C268" s="112"/>
       <c r="D268" s="112"/>
       <c r="E268" s="212"/>
       <c r="F268" s="113"/>
       <c r="G268" s="114"/>
       <c r="H268" s="115"/>
     </row>
-    <row r="269" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A269" s="1"/>
-      <c r="B269" s="111"/>
-      <c r="C269" s="112"/>
-      <c r="D269" s="112"/>
-      <c r="E269" s="212"/>
-      <c r="F269" s="113"/>
-      <c r="G269" s="114"/>
-      <c r="H269" s="115"/>
-    </row>
-    <row r="270" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A270" s="1"/>
-      <c r="B270" s="111"/>
+    <row r="269" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A269" s="154"/>
+      <c r="B269" s="173" t="s">
+        <v>142</v>
+      </c>
+      <c r="C269" s="152"/>
+      <c r="D269" s="152"/>
+      <c r="E269" s="211"/>
+      <c r="F269" s="152"/>
+      <c r="G269" s="152"/>
+      <c r="H269" s="153"/>
+    </row>
+    <row r="270" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A270" s="154"/>
+      <c r="B270" s="173"/>
       <c r="C270" s="174" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D270" s="152"/>
       <c r="E270" s="211"/>
@@ -7684,7 +7736,7 @@
       <c r="A273" s="1"/>
       <c r="B273" s="111"/>
       <c r="C273" s="174" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D273" s="152"/>
       <c r="E273" s="211"/>
@@ -7716,7 +7768,7 @@
       <c r="A276" s="1"/>
       <c r="B276" s="111"/>
       <c r="C276" s="174" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D276" s="152"/>
       <c r="E276" s="211"/>
@@ -7748,7 +7800,7 @@
       <c r="A279" s="1"/>
       <c r="B279" s="111"/>
       <c r="C279" s="174" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D279" s="152"/>
       <c r="E279" s="211"/>
@@ -7780,7 +7832,7 @@
       <c r="A282" s="1"/>
       <c r="B282" s="111"/>
       <c r="C282" s="174" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D282" s="152"/>
       <c r="E282" s="211"/>
@@ -7812,7 +7864,7 @@
       <c r="A285" s="1"/>
       <c r="B285" s="111"/>
       <c r="C285" s="174" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D285" s="152"/>
       <c r="E285" s="211"/>
@@ -7844,7 +7896,7 @@
       <c r="A288" s="1"/>
       <c r="B288" s="111"/>
       <c r="C288" s="174" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D288" s="152"/>
       <c r="E288" s="211"/>
@@ -7876,7 +7928,7 @@
       <c r="A291" s="1"/>
       <c r="B291" s="111"/>
       <c r="C291" s="174" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D291" s="152"/>
       <c r="E291" s="211"/>
@@ -7908,7 +7960,7 @@
       <c r="A294" s="1"/>
       <c r="B294" s="111"/>
       <c r="C294" s="174" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D294" s="152"/>
       <c r="E294" s="211"/>
@@ -7940,7 +7992,7 @@
       <c r="A297" s="1"/>
       <c r="B297" s="111"/>
       <c r="C297" s="174" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D297" s="152"/>
       <c r="E297" s="211"/>
@@ -7952,80 +8004,52 @@
       <c r="A298" s="1"/>
       <c r="B298" s="111"/>
       <c r="C298" s="174"/>
-      <c r="D298" s="148" t="s">
-        <v>471</v>
-      </c>
-      <c r="E298" s="219" t="s">
-        <v>472</v>
-      </c>
-      <c r="F298" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G298" s="150">
-        <v>44663</v>
-      </c>
-      <c r="H298" s="151">
-        <v>44663</v>
-      </c>
+      <c r="D298" s="112"/>
+      <c r="E298" s="212"/>
+      <c r="F298" s="113"/>
+      <c r="G298" s="114"/>
+      <c r="H298" s="115"/>
     </row>
     <row r="299" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="B299" s="111"/>
       <c r="C299" s="112"/>
-      <c r="D299" s="143" t="s">
-        <v>473</v>
-      </c>
-      <c r="E299" s="217" t="s">
-        <v>474</v>
-      </c>
-      <c r="F299" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="G299" s="145">
-        <v>44663</v>
-      </c>
-      <c r="H299" s="146">
-        <v>44663</v>
-      </c>
+      <c r="D299" s="112"/>
+      <c r="E299" s="212"/>
+      <c r="F299" s="113"/>
+      <c r="G299" s="114"/>
+      <c r="H299" s="115"/>
     </row>
     <row r="300" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="B300" s="111"/>
-      <c r="C300" s="112"/>
-      <c r="D300" s="143" t="s">
-        <v>476</v>
-      </c>
-      <c r="E300" s="217" t="s">
-        <v>475</v>
-      </c>
-      <c r="F300" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="G300" s="145">
-        <v>44630</v>
-      </c>
-      <c r="H300" s="146">
-        <v>44630</v>
-      </c>
+      <c r="C300" s="174" t="s">
+        <v>158</v>
+      </c>
+      <c r="D300" s="152"/>
+      <c r="E300" s="211"/>
+      <c r="F300" s="152"/>
+      <c r="G300" s="152"/>
+      <c r="H300" s="153"/>
     </row>
     <row r="301" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="B301" s="111"/>
-      <c r="C301" s="112"/>
-      <c r="D301" s="143" t="s">
-        <v>477</v>
-      </c>
-      <c r="E301" s="217" t="s">
-        <v>478</v>
-      </c>
-      <c r="F301" s="144" t="s">
+      <c r="C301" s="174"/>
+      <c r="D301" s="148" t="s">
+        <v>471</v>
+      </c>
+      <c r="E301" s="219" t="s">
+        <v>472</v>
+      </c>
+      <c r="F301" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G301" s="145">
-        <v>44630</v>
-      </c>
-      <c r="H301" s="146">
-        <v>44630</v>
+      <c r="G301" s="150">
+        <v>44663</v>
+      </c>
+      <c r="H301" s="151">
+        <v>44663</v>
       </c>
     </row>
     <row r="302" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8033,19 +8057,19 @@
       <c r="B302" s="111"/>
       <c r="C302" s="112"/>
       <c r="D302" s="143" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="E302" s="217" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="F302" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G302" s="145">
-        <v>44698</v>
+        <v>44663</v>
       </c>
       <c r="H302" s="146">
-        <v>44630</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="303" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8053,16 +8077,16 @@
       <c r="B303" s="111"/>
       <c r="C303" s="112"/>
       <c r="D303" s="143" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E303" s="217" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="F303" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G303" s="145">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H303" s="146">
         <v>44630</v>
@@ -8073,19 +8097,19 @@
       <c r="B304" s="111"/>
       <c r="C304" s="112"/>
       <c r="D304" s="143" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="E304" s="217" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="F304" s="144" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G304" s="145">
-        <v>44669</v>
+        <v>44630</v>
       </c>
       <c r="H304" s="146">
-        <v>44824</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="305" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8093,19 +8117,19 @@
       <c r="B305" s="111"/>
       <c r="C305" s="112"/>
       <c r="D305" s="143" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="E305" s="217" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="F305" s="144" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G305" s="145">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H305" s="146">
-        <v>44824</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="306" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8113,19 +8137,19 @@
       <c r="B306" s="111"/>
       <c r="C306" s="112"/>
       <c r="D306" s="143" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="E306" s="217" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="F306" s="144" t="s">
-        <v>464</v>
+        <v>281</v>
       </c>
       <c r="G306" s="145">
-        <v>44733</v>
+        <v>44698</v>
       </c>
       <c r="H306" s="146">
-        <v>44622</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="307" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8133,19 +8157,19 @@
       <c r="B307" s="111"/>
       <c r="C307" s="112"/>
       <c r="D307" s="143" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="E307" s="217" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="F307" s="144" t="s">
-        <v>464</v>
+        <v>256</v>
       </c>
       <c r="G307" s="145">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H307" s="146">
-        <v>44621</v>
+        <v>44824</v>
       </c>
     </row>
     <row r="308" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8153,19 +8177,19 @@
       <c r="B308" s="111"/>
       <c r="C308" s="112"/>
       <c r="D308" s="143" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="E308" s="217" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="F308" s="144" t="s">
-        <v>464</v>
+        <v>256</v>
       </c>
       <c r="G308" s="145">
-        <v>44671</v>
+        <v>44669</v>
       </c>
       <c r="H308" s="146">
-        <v>44732</v>
+        <v>44824</v>
       </c>
     </row>
     <row r="309" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8173,19 +8197,19 @@
       <c r="B309" s="111"/>
       <c r="C309" s="112"/>
       <c r="D309" s="143" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="E309" s="217" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
       <c r="F309" s="144" t="s">
         <v>464</v>
       </c>
       <c r="G309" s="145">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H309" s="146">
-        <v>44732</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="310" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8193,16 +8217,16 @@
       <c r="B310" s="111"/>
       <c r="C310" s="112"/>
       <c r="D310" s="143" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
       <c r="E310" s="217" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="F310" s="144" t="s">
-        <v>497</v>
+        <v>464</v>
       </c>
       <c r="G310" s="145">
-        <v>44698</v>
+        <v>44733</v>
       </c>
       <c r="H310" s="146">
         <v>44621</v>
@@ -8213,19 +8237,19 @@
       <c r="B311" s="111"/>
       <c r="C311" s="112"/>
       <c r="D311" s="143" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="E311" s="217" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="F311" s="144" t="s">
-        <v>497</v>
+        <v>464</v>
       </c>
       <c r="G311" s="145">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H311" s="146">
-        <v>44621</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="312" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8233,19 +8257,19 @@
       <c r="B312" s="111"/>
       <c r="C312" s="112"/>
       <c r="D312" s="143" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="E312" s="217" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="F312" s="144" t="s">
-        <v>267</v>
+        <v>464</v>
       </c>
       <c r="G312" s="145">
-        <v>44644</v>
+        <v>44671</v>
       </c>
       <c r="H312" s="146">
-        <v>44622</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="313" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8253,16 +8277,16 @@
       <c r="B313" s="111"/>
       <c r="C313" s="112"/>
       <c r="D313" s="143" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="E313" s="217" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="F313" s="144" t="s">
-        <v>267</v>
+        <v>497</v>
       </c>
       <c r="G313" s="145">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H313" s="146">
         <v>44621</v>
@@ -8273,13 +8297,13 @@
       <c r="B314" s="111"/>
       <c r="C314" s="112"/>
       <c r="D314" s="143" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="E314" s="217" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
       <c r="F314" s="144" t="s">
-        <v>464</v>
+        <v>497</v>
       </c>
       <c r="G314" s="145">
         <v>44698</v>
@@ -8293,19 +8317,19 @@
       <c r="B315" s="111"/>
       <c r="C315" s="112"/>
       <c r="D315" s="143" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
       <c r="E315" s="217" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="F315" s="144" t="s">
-        <v>464</v>
+        <v>267</v>
       </c>
       <c r="G315" s="145">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H315" s="146">
-        <v>44621</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="316" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8313,19 +8337,19 @@
       <c r="B316" s="111"/>
       <c r="C316" s="112"/>
       <c r="D316" s="143" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="E316" s="217" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="F316" s="144" t="s">
         <v>267</v>
       </c>
       <c r="G316" s="145">
-        <v>44846</v>
+        <v>44644</v>
       </c>
       <c r="H316" s="146">
-        <v>44627</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="317" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8333,19 +8357,19 @@
       <c r="B317" s="111"/>
       <c r="C317" s="112"/>
       <c r="D317" s="143" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="E317" s="217" t="s">
-        <v>511</v>
+        <v>504</v>
       </c>
       <c r="F317" s="144" t="s">
-        <v>267</v>
+        <v>464</v>
       </c>
       <c r="G317" s="145">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H317" s="146">
-        <v>44627</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="318" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8353,19 +8377,19 @@
       <c r="B318" s="111"/>
       <c r="C318" s="112"/>
       <c r="D318" s="143" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
       <c r="E318" s="217" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="F318" s="144" t="s">
-        <v>232</v>
+        <v>464</v>
       </c>
       <c r="G318" s="145">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H318" s="146">
-        <v>44628</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="319" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8373,19 +8397,19 @@
       <c r="B319" s="111"/>
       <c r="C319" s="112"/>
       <c r="D319" s="143" t="s">
-        <v>514</v>
+        <v>508</v>
       </c>
       <c r="E319" s="217" t="s">
-        <v>515</v>
+        <v>509</v>
       </c>
       <c r="F319" s="144" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G319" s="145">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H319" s="146">
-        <v>44628</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="320" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8393,19 +8417,19 @@
       <c r="B320" s="111"/>
       <c r="C320" s="112"/>
       <c r="D320" s="143" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="E320" s="217" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="F320" s="144" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G320" s="145">
-        <v>44698</v>
+        <v>44846</v>
       </c>
       <c r="H320" s="146">
-        <v>44628</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="321" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8413,16 +8437,16 @@
       <c r="B321" s="111"/>
       <c r="C321" s="112"/>
       <c r="D321" s="143" t="s">
-        <v>518</v>
+        <v>512</v>
       </c>
       <c r="E321" s="217" t="s">
-        <v>519</v>
+        <v>513</v>
       </c>
       <c r="F321" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G321" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H321" s="146">
         <v>44628</v>
@@ -8433,10 +8457,10 @@
       <c r="B322" s="111"/>
       <c r="C322" s="112"/>
       <c r="D322" s="143" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="E322" s="217" t="s">
-        <v>522</v>
+        <v>515</v>
       </c>
       <c r="F322" s="144" t="s">
         <v>232</v>
@@ -8453,16 +8477,16 @@
       <c r="B323" s="111"/>
       <c r="C323" s="112"/>
       <c r="D323" s="143" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="E323" s="217" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="F323" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G323" s="145">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H323" s="146">
         <v>44628</v>
@@ -8473,10 +8497,10 @@
       <c r="B324" s="111"/>
       <c r="C324" s="112"/>
       <c r="D324" s="143" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E324" s="217" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="F324" s="144" t="s">
         <v>281</v>
@@ -8493,16 +8517,16 @@
       <c r="B325" s="111"/>
       <c r="C325" s="112"/>
       <c r="D325" s="143" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="E325" s="217" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="F325" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G325" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H325" s="146">
         <v>44628</v>
@@ -8513,19 +8537,19 @@
       <c r="B326" s="111"/>
       <c r="C326" s="112"/>
       <c r="D326" s="143" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="E326" s="217" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="F326" s="144" t="s">
         <v>232</v>
       </c>
       <c r="G326" s="145">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="H326" s="146">
-        <v>44617</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="327" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8533,19 +8557,19 @@
       <c r="B327" s="111"/>
       <c r="C327" s="112"/>
       <c r="D327" s="143" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
       <c r="E327" s="217" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="F327" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G327" s="145">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H327" s="146">
-        <v>44617</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="328" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8553,19 +8577,19 @@
       <c r="B328" s="111"/>
       <c r="C328" s="112"/>
       <c r="D328" s="143" t="s">
-        <v>532</v>
+        <v>526</v>
       </c>
       <c r="E328" s="217" t="s">
-        <v>533</v>
+        <v>527</v>
       </c>
       <c r="F328" s="144" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G328" s="145">
-        <v>44740</v>
+        <v>44698</v>
       </c>
       <c r="H328" s="146">
-        <v>44662</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="329" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8573,202 +8597,202 @@
       <c r="B329" s="111"/>
       <c r="C329" s="112"/>
       <c r="D329" s="143" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="E329" s="217" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="F329" s="144" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G329" s="145">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H329" s="146">
-        <v>44662</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="330" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A330" s="1"/>
       <c r="B330" s="111"/>
       <c r="C330" s="112"/>
-      <c r="D330" s="112"/>
-      <c r="E330" s="212"/>
-      <c r="F330" s="113"/>
-      <c r="G330" s="114"/>
-      <c r="H330" s="115"/>
+      <c r="D330" s="143" t="s">
+        <v>531</v>
+      </c>
+      <c r="E330" s="217" t="s">
+        <v>530</v>
+      </c>
+      <c r="F330" s="144" t="s">
+        <v>232</v>
+      </c>
+      <c r="G330" s="145">
+        <v>44617</v>
+      </c>
+      <c r="H330" s="146">
+        <v>44617</v>
+      </c>
     </row>
     <row r="331" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A331" s="1"/>
       <c r="B331" s="111"/>
-      <c r="C331" s="174" t="s">
-        <v>147</v>
-      </c>
-      <c r="D331" s="152"/>
-      <c r="E331" s="211"/>
-      <c r="F331" s="152"/>
-      <c r="G331" s="152"/>
-      <c r="H331" s="153"/>
+      <c r="C331" s="112"/>
+      <c r="D331" s="143" t="s">
+        <v>532</v>
+      </c>
+      <c r="E331" s="217" t="s">
+        <v>533</v>
+      </c>
+      <c r="F331" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G331" s="145">
+        <v>44740</v>
+      </c>
+      <c r="H331" s="146">
+        <v>44662</v>
+      </c>
     </row>
     <row r="332" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A332" s="1"/>
       <c r="B332" s="111"/>
-      <c r="C332" s="174"/>
-      <c r="D332" s="148" t="s">
-        <v>274</v>
-      </c>
-      <c r="E332" s="219" t="s">
-        <v>449</v>
-      </c>
-      <c r="F332" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G332" s="150">
-        <v>44167</v>
-      </c>
-      <c r="H332" s="151">
-        <v>44167</v>
+      <c r="C332" s="112"/>
+      <c r="D332" s="143" t="s">
+        <v>535</v>
+      </c>
+      <c r="E332" s="217" t="s">
+        <v>534</v>
+      </c>
+      <c r="F332" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G332" s="145">
+        <v>44740</v>
+      </c>
+      <c r="H332" s="146">
+        <v>44662</v>
       </c>
     </row>
     <row r="333" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A333" s="1"/>
       <c r="B333" s="111"/>
       <c r="C333" s="112"/>
-      <c r="D333" s="143" t="s">
-        <v>450</v>
-      </c>
-      <c r="E333" s="217" t="s">
-        <v>451</v>
-      </c>
-      <c r="F333" s="144" t="s">
-        <v>256</v>
-      </c>
-      <c r="G333" s="145">
-        <v>44575</v>
-      </c>
-      <c r="H333" s="146">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="334" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D333" s="112"/>
+      <c r="E333" s="212"/>
+      <c r="F333" s="113"/>
+      <c r="G333" s="114"/>
+      <c r="H333" s="115"/>
+    </row>
+    <row r="334" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A334" s="1"/>
       <c r="B334" s="111"/>
-      <c r="C334" s="112"/>
-      <c r="D334" s="143" t="s">
-        <v>453</v>
-      </c>
-      <c r="E334" s="215" t="s">
-        <v>452</v>
-      </c>
-      <c r="F334" s="144" t="s">
-        <v>281</v>
-      </c>
-      <c r="G334" s="145">
-        <v>44404</v>
-      </c>
-      <c r="H334" s="146">
-        <v>44404</v>
-      </c>
+      <c r="C334" s="174" t="s">
+        <v>147</v>
+      </c>
+      <c r="D334" s="152"/>
+      <c r="E334" s="211"/>
+      <c r="F334" s="152"/>
+      <c r="G334" s="152"/>
+      <c r="H334" s="153"/>
     </row>
     <row r="335" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A335" s="1"/>
       <c r="B335" s="111"/>
-      <c r="C335" s="112"/>
-      <c r="D335" s="112"/>
-      <c r="E335" s="212"/>
-      <c r="F335" s="113"/>
-      <c r="G335" s="114"/>
-      <c r="H335" s="115"/>
+      <c r="C335" s="174"/>
+      <c r="D335" s="148" t="s">
+        <v>274</v>
+      </c>
+      <c r="E335" s="219" t="s">
+        <v>449</v>
+      </c>
+      <c r="F335" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G335" s="150">
+        <v>44167</v>
+      </c>
+      <c r="H335" s="151">
+        <v>44167</v>
+      </c>
     </row>
     <row r="336" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A336" s="1"/>
       <c r="B336" s="111"/>
-      <c r="C336" s="174" t="s">
-        <v>159</v>
-      </c>
-      <c r="D336" s="152"/>
-      <c r="E336" s="211"/>
-      <c r="F336" s="152"/>
-      <c r="G336" s="152"/>
-      <c r="H336" s="153"/>
-    </row>
-    <row r="337" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C336" s="112"/>
+      <c r="D336" s="143" t="s">
+        <v>450</v>
+      </c>
+      <c r="E336" s="217" t="s">
+        <v>451</v>
+      </c>
+      <c r="F336" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G336" s="145">
+        <v>44575</v>
+      </c>
+      <c r="H336" s="146">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="337" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A337" s="1"/>
       <c r="B337" s="111"/>
-      <c r="C337" s="174"/>
-      <c r="D337" s="148" t="s">
-        <v>455</v>
-      </c>
-      <c r="E337" s="219" t="s">
-        <v>454</v>
-      </c>
-      <c r="F337" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G337" s="150">
-        <v>44635</v>
-      </c>
-      <c r="H337" s="151">
-        <v>44635</v>
+      <c r="C337" s="112"/>
+      <c r="D337" s="143" t="s">
+        <v>453</v>
+      </c>
+      <c r="E337" s="215" t="s">
+        <v>452</v>
+      </c>
+      <c r="F337" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="G337" s="145">
+        <v>44404</v>
+      </c>
+      <c r="H337" s="146">
+        <v>44404</v>
       </c>
     </row>
     <row r="338" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A338" s="1"/>
       <c r="B338" s="111"/>
       <c r="C338" s="112"/>
-      <c r="D338" s="143" t="s">
-        <v>457</v>
-      </c>
-      <c r="E338" s="217" t="s">
-        <v>456</v>
-      </c>
-      <c r="F338" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="G338" s="145">
-        <v>44635</v>
-      </c>
-      <c r="H338" s="146">
-        <v>44635</v>
-      </c>
+      <c r="D338" s="112"/>
+      <c r="E338" s="212"/>
+      <c r="F338" s="113"/>
+      <c r="G338" s="114"/>
+      <c r="H338" s="115"/>
     </row>
     <row r="339" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A339" s="1"/>
       <c r="B339" s="111"/>
-      <c r="C339" s="112"/>
-      <c r="D339" s="143" t="s">
-        <v>458</v>
-      </c>
-      <c r="E339" s="217" t="s">
-        <v>460</v>
-      </c>
-      <c r="F339" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="G339" s="145">
-        <v>44635</v>
-      </c>
-      <c r="H339" s="146">
-        <v>44635</v>
-      </c>
+      <c r="C339" s="174" t="s">
+        <v>159</v>
+      </c>
+      <c r="D339" s="152"/>
+      <c r="E339" s="211"/>
+      <c r="F339" s="152"/>
+      <c r="G339" s="152"/>
+      <c r="H339" s="153"/>
     </row>
     <row r="340" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A340" s="1"/>
       <c r="B340" s="111"/>
-      <c r="C340" s="112"/>
-      <c r="D340" s="143" t="s">
-        <v>459</v>
-      </c>
-      <c r="E340" s="217" t="s">
-        <v>461</v>
-      </c>
-      <c r="F340" s="144" t="s">
+      <c r="C340" s="174"/>
+      <c r="D340" s="148" t="s">
+        <v>455</v>
+      </c>
+      <c r="E340" s="219" t="s">
+        <v>454</v>
+      </c>
+      <c r="F340" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G340" s="145">
+      <c r="G340" s="150">
         <v>44635</v>
       </c>
-      <c r="H340" s="146">
+      <c r="H340" s="151">
         <v>44635</v>
       </c>
     </row>
@@ -8777,19 +8801,19 @@
       <c r="B341" s="111"/>
       <c r="C341" s="112"/>
       <c r="D341" s="143" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E341" s="217" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="F341" s="144" t="s">
-        <v>464</v>
+        <v>232</v>
       </c>
       <c r="G341" s="145">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H341" s="146">
-        <v>44644</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="342" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8797,19 +8821,19 @@
       <c r="B342" s="111"/>
       <c r="C342" s="112"/>
       <c r="D342" s="143" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="E342" s="217" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="F342" s="144" t="s">
-        <v>464</v>
+        <v>232</v>
       </c>
       <c r="G342" s="145">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H342" s="146">
-        <v>44644</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="343" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8817,19 +8841,19 @@
       <c r="B343" s="111"/>
       <c r="C343" s="112"/>
       <c r="D343" s="143" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="E343" s="217" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="F343" s="144" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G343" s="145">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H343" s="146">
-        <v>44636</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="344" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8837,60 +8861,90 @@
       <c r="B344" s="111"/>
       <c r="C344" s="112"/>
       <c r="D344" s="143" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="E344" s="217" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="F344" s="144" t="s">
-        <v>267</v>
+        <v>464</v>
       </c>
       <c r="G344" s="145">
+        <v>44701</v>
+      </c>
+      <c r="H344" s="146">
         <v>44644</v>
       </c>
-      <c r="H344" s="146">
-        <v>44636</v>
-      </c>
-    </row>
-    <row r="345" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="345" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A345" s="1"/>
-      <c r="B345" s="116"/>
-      <c r="C345" s="117"/>
-      <c r="D345" s="117"/>
-      <c r="E345" s="220"/>
-      <c r="F345" s="118"/>
-      <c r="G345" s="119"/>
-      <c r="H345" s="120"/>
+      <c r="B345" s="111"/>
+      <c r="C345" s="112"/>
+      <c r="D345" s="143" t="s">
+        <v>463</v>
+      </c>
+      <c r="E345" s="217" t="s">
+        <v>466</v>
+      </c>
+      <c r="F345" s="144" t="s">
+        <v>464</v>
+      </c>
+      <c r="G345" s="145">
+        <v>44701</v>
+      </c>
+      <c r="H345" s="146">
+        <v>44644</v>
+      </c>
     </row>
     <row r="346" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
-      <c r="B346" s="1"/>
-      <c r="C346" s="1"/>
-      <c r="D346" s="1"/>
-      <c r="E346" s="221"/>
-      <c r="F346" s="121"/>
-      <c r="G346" s="122"/>
-      <c r="H346" s="122"/>
+      <c r="B346" s="111"/>
+      <c r="C346" s="112"/>
+      <c r="D346" s="143" t="s">
+        <v>467</v>
+      </c>
+      <c r="E346" s="217" t="s">
+        <v>468</v>
+      </c>
+      <c r="F346" s="144" t="s">
+        <v>267</v>
+      </c>
+      <c r="G346" s="145">
+        <v>44644</v>
+      </c>
+      <c r="H346" s="146">
+        <v>44636</v>
+      </c>
     </row>
     <row r="347" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A347" s="1"/>
-      <c r="B347" s="1"/>
-      <c r="C347" s="1"/>
-      <c r="D347" s="1"/>
-      <c r="E347" s="221"/>
-      <c r="F347" s="121"/>
-      <c r="G347" s="122"/>
-      <c r="H347" s="122"/>
-    </row>
-    <row r="348" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B347" s="111"/>
+      <c r="C347" s="112"/>
+      <c r="D347" s="143" t="s">
+        <v>469</v>
+      </c>
+      <c r="E347" s="217" t="s">
+        <v>470</v>
+      </c>
+      <c r="F347" s="144" t="s">
+        <v>267</v>
+      </c>
+      <c r="G347" s="145">
+        <v>44644</v>
+      </c>
+      <c r="H347" s="146">
+        <v>44636</v>
+      </c>
+    </row>
+    <row r="348" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A348" s="1"/>
-      <c r="B348" s="1"/>
-      <c r="C348" s="1"/>
-      <c r="D348" s="1"/>
-      <c r="E348" s="221"/>
-      <c r="F348" s="121"/>
-      <c r="G348" s="122"/>
-      <c r="H348" s="122"/>
+      <c r="B348" s="116"/>
+      <c r="C348" s="117"/>
+      <c r="D348" s="117"/>
+      <c r="E348" s="220"/>
+      <c r="F348" s="118"/>
+      <c r="G348" s="119"/>
+      <c r="H348" s="120"/>
     </row>
     <row r="349" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A349" s="1"/>
@@ -9022,38 +9076,68 @@
       <c r="G361" s="122"/>
       <c r="H361" s="122"/>
     </row>
-    <row r="362" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E362" s="210"/>
-      <c r="F362" s="95"/>
-      <c r="G362" s="110"/>
-      <c r="H362" s="110"/>
-    </row>
-    <row r="363" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E363" s="210"/>
-      <c r="F363" s="95"/>
-      <c r="G363" s="110"/>
-      <c r="H363" s="110"/>
-    </row>
-    <row r="364" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E364" s="210"/>
-      <c r="F364" s="95"/>
-      <c r="G364" s="110"/>
-      <c r="H364" s="110"/>
+    <row r="362" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A362" s="1"/>
+      <c r="B362" s="1"/>
+      <c r="C362" s="1"/>
+      <c r="D362" s="1"/>
+      <c r="E362" s="221"/>
+      <c r="F362" s="121"/>
+      <c r="G362" s="122"/>
+      <c r="H362" s="122"/>
+    </row>
+    <row r="363" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A363" s="1"/>
+      <c r="B363" s="1"/>
+      <c r="C363" s="1"/>
+      <c r="D363" s="1"/>
+      <c r="E363" s="221"/>
+      <c r="F363" s="121"/>
+      <c r="G363" s="122"/>
+      <c r="H363" s="122"/>
+    </row>
+    <row r="364" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A364" s="1"/>
+      <c r="B364" s="1"/>
+      <c r="C364" s="1"/>
+      <c r="D364" s="1"/>
+      <c r="E364" s="221"/>
+      <c r="F364" s="121"/>
+      <c r="G364" s="122"/>
+      <c r="H364" s="122"/>
+    </row>
+    <row r="365" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E365" s="210"/>
+      <c r="F365" s="95"/>
+      <c r="G365" s="110"/>
+      <c r="H365" s="110"/>
+    </row>
+    <row r="366" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E366" s="210"/>
+      <c r="F366" s="95"/>
+      <c r="G366" s="110"/>
+      <c r="H366" s="110"/>
+    </row>
+    <row r="367" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E367" s="210"/>
+      <c r="F367" s="95"/>
+      <c r="G367" s="110"/>
+      <c r="H367" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C291:C292"/>
     <mergeCell ref="C294:C295"/>
     <mergeCell ref="C297:C298"/>
-    <mergeCell ref="C331:C332"/>
-    <mergeCell ref="C336:C337"/>
-    <mergeCell ref="C276:C277"/>
+    <mergeCell ref="C300:C301"/>
+    <mergeCell ref="C334:C335"/>
+    <mergeCell ref="C339:C340"/>
     <mergeCell ref="C279:C280"/>
     <mergeCell ref="C282:C283"/>
     <mergeCell ref="C285:C286"/>
     <mergeCell ref="C288:C289"/>
-    <mergeCell ref="C270:C271"/>
+    <mergeCell ref="C291:C292"/>
     <mergeCell ref="C273:C274"/>
+    <mergeCell ref="C276:C277"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C14:C15"/>
@@ -9070,11 +9154,11 @@
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B266:B267"/>
-    <mergeCell ref="C267:C268"/>
+    <mergeCell ref="B269:B270"/>
+    <mergeCell ref="C270:C271"/>
     <mergeCell ref="C151:C152"/>
-    <mergeCell ref="B262:B263"/>
-    <mergeCell ref="C263:C264"/>
+    <mergeCell ref="B265:B266"/>
+    <mergeCell ref="C266:C267"/>
     <mergeCell ref="C207:C208"/>
     <mergeCell ref="E2:E3"/>
   </mergeCells>

</xml_diff>

<commit_message>
Update Pertanggal 13 Februari 2023 17:59 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="658">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -2077,6 +2077,18 @@
     <t>Mendapatkan Data Entities untuk Pemasok berdasarkan ID (varID).
 Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
 Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
+  </si>
+  <si>
+    <t>Func_General_GetBusinessDocumentCurrentAndNextWorkFlowStage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mendapatkan Tahapan saat ini dan Tahapan selanjutnya pada Work Flow Dokumen Bisnis sesuai ID Dokumen Bisnis (varBusinessDocument_RefID) </t>
+  </si>
+  <si>
+    <t>Mendapatkan Jalur Work Flow berdasarkan ID Jenis Doumen Bisnis (varBusinessDocumentType_RefID) dan ID Entitas Submitter (varSubmitterEntity_RefID</t>
+  </si>
+  <si>
+    <t>Func_General_GetBusinessDocumentTypeWorkFlowPath</t>
   </si>
 </sst>
 </file>
@@ -3323,35 +3335,41 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3359,6 +3377,51 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3382,57 +3445,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3757,13 +3769,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H384"/>
+  <dimension ref="A1:H386"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E112" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E247" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E113" sqref="E113"/>
+      <selection pane="bottomRight" activeCell="E251" sqref="E251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3781,19 +3793,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="182" t="s">
+      <c r="B2" s="189" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="183"/>
-      <c r="D2" s="183"/>
-      <c r="E2" s="189" t="s">
+      <c r="C2" s="190"/>
+      <c r="D2" s="190"/>
+      <c r="E2" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="184" t="s">
+      <c r="F2" s="181" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="185"/>
-      <c r="H2" s="186"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="183"/>
     </row>
     <row r="3" spans="1:8" s="156" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="157" t="s">
@@ -3805,7 +3817,7 @@
       <c r="D3" s="159" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="190"/>
+      <c r="E3" s="188"/>
       <c r="F3" s="160" t="s">
         <v>228</v>
       </c>
@@ -3818,7 +3830,7 @@
     </row>
     <row r="4" spans="1:8" s="155" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="154"/>
-      <c r="B4" s="187" t="s">
+      <c r="B4" s="184" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="152"/>
@@ -3830,8 +3842,8 @@
     </row>
     <row r="5" spans="1:8" s="155" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="154"/>
-      <c r="B5" s="188"/>
-      <c r="C5" s="181" t="s">
+      <c r="B5" s="185"/>
+      <c r="C5" s="186" t="s">
         <v>160</v>
       </c>
       <c r="D5" s="152"/>
@@ -3843,7 +3855,7 @@
     <row r="6" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="111"/>
-      <c r="C6" s="181"/>
+      <c r="C6" s="186"/>
       <c r="D6" s="112"/>
       <c r="E6" s="171"/>
       <c r="F6" s="113"/>
@@ -3863,7 +3875,7 @@
     <row r="8" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="111"/>
-      <c r="C8" s="181" t="s">
+      <c r="C8" s="186" t="s">
         <v>161</v>
       </c>
       <c r="D8" s="152"/>
@@ -3875,7 +3887,7 @@
     <row r="9" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="111"/>
-      <c r="C9" s="181"/>
+      <c r="C9" s="186"/>
       <c r="D9" s="112"/>
       <c r="E9" s="171"/>
       <c r="F9" s="113"/>
@@ -3895,7 +3907,7 @@
     <row r="11" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="111"/>
-      <c r="C11" s="181" t="s">
+      <c r="C11" s="186" t="s">
         <v>162</v>
       </c>
       <c r="D11" s="152"/>
@@ -3907,7 +3919,7 @@
     <row r="12" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="111"/>
-      <c r="C12" s="181"/>
+      <c r="C12" s="186"/>
       <c r="D12" s="112"/>
       <c r="E12" s="171"/>
       <c r="F12" s="113"/>
@@ -3927,7 +3939,7 @@
     <row r="14" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="111"/>
-      <c r="C14" s="181" t="s">
+      <c r="C14" s="186" t="s">
         <v>163</v>
       </c>
       <c r="D14" s="152"/>
@@ -3939,7 +3951,7 @@
     <row r="15" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="111"/>
-      <c r="C15" s="181"/>
+      <c r="C15" s="186"/>
       <c r="D15" s="112"/>
       <c r="E15" s="171"/>
       <c r="F15" s="113"/>
@@ -3959,7 +3971,7 @@
     <row r="17" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="111"/>
-      <c r="C17" s="181" t="s">
+      <c r="C17" s="186" t="s">
         <v>164</v>
       </c>
       <c r="D17" s="152"/>
@@ -3971,7 +3983,7 @@
     <row r="18" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="111"/>
-      <c r="C18" s="181"/>
+      <c r="C18" s="186"/>
       <c r="D18" s="112"/>
       <c r="E18" s="171"/>
       <c r="F18" s="113"/>
@@ -3991,7 +4003,7 @@
     <row r="20" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="111"/>
-      <c r="C20" s="181" t="s">
+      <c r="C20" s="186" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="152"/>
@@ -4003,7 +4015,7 @@
     <row r="21" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="111"/>
-      <c r="C21" s="181"/>
+      <c r="C21" s="186"/>
       <c r="D21" s="112"/>
       <c r="E21" s="171"/>
       <c r="F21" s="113"/>
@@ -4083,7 +4095,7 @@
     <row r="27" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="111"/>
-      <c r="C27" s="181" t="s">
+      <c r="C27" s="186" t="s">
         <v>165</v>
       </c>
       <c r="D27" s="152"/>
@@ -4095,7 +4107,7 @@
     <row r="28" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="111"/>
-      <c r="C28" s="181"/>
+      <c r="C28" s="186"/>
       <c r="D28" s="112"/>
       <c r="E28" s="171"/>
       <c r="F28" s="113"/>
@@ -4115,7 +4127,7 @@
     <row r="30" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="111"/>
-      <c r="C30" s="181" t="s">
+      <c r="C30" s="186" t="s">
         <v>166</v>
       </c>
       <c r="D30" s="152"/>
@@ -4127,7 +4139,7 @@
     <row r="31" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="111"/>
-      <c r="C31" s="181"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="112"/>
       <c r="E31" s="171"/>
       <c r="F31" s="113"/>
@@ -4337,7 +4349,7 @@
     <row r="47" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="111"/>
-      <c r="C47" s="181" t="s">
+      <c r="C47" s="186" t="s">
         <v>75</v>
       </c>
       <c r="D47" s="152"/>
@@ -4349,7 +4361,7 @@
     <row r="48" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="111"/>
-      <c r="C48" s="181"/>
+      <c r="C48" s="186"/>
       <c r="D48" s="112" t="s">
         <v>566</v>
       </c>
@@ -5019,7 +5031,7 @@
     <row r="98" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="111"/>
-      <c r="C98" s="181" t="s">
+      <c r="C98" s="186" t="s">
         <v>167</v>
       </c>
       <c r="D98" s="152"/>
@@ -5031,7 +5043,7 @@
     <row r="99" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="111"/>
-      <c r="C99" s="181"/>
+      <c r="C99" s="186"/>
       <c r="D99" s="112"/>
       <c r="E99" s="171"/>
       <c r="F99" s="113"/>
@@ -5051,7 +5063,7 @@
     <row r="101" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="111"/>
-      <c r="C101" s="181" t="s">
+      <c r="C101" s="186" t="s">
         <v>168</v>
       </c>
       <c r="D101" s="152"/>
@@ -5063,7 +5075,7 @@
     <row r="102" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="111"/>
-      <c r="C102" s="181"/>
+      <c r="C102" s="186"/>
       <c r="D102" s="112"/>
       <c r="E102" s="171"/>
       <c r="F102" s="113"/>
@@ -5083,7 +5095,7 @@
     <row r="104" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="111"/>
-      <c r="C104" s="181" t="s">
+      <c r="C104" s="186" t="s">
         <v>169</v>
       </c>
       <c r="D104" s="152"/>
@@ -5095,7 +5107,7 @@
     <row r="105" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="111"/>
-      <c r="C105" s="181"/>
+      <c r="C105" s="186"/>
       <c r="D105" s="148" t="s">
         <v>535</v>
       </c>
@@ -5575,7 +5587,7 @@
     <row r="137" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="111"/>
-      <c r="C137" s="181" t="s">
+      <c r="C137" s="186" t="s">
         <v>57</v>
       </c>
       <c r="D137" s="152"/>
@@ -5587,7 +5599,7 @@
     <row r="138" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="111"/>
-      <c r="C138" s="181"/>
+      <c r="C138" s="186"/>
       <c r="D138" s="148" t="s">
         <v>423</v>
       </c>
@@ -5887,7 +5899,7 @@
     <row r="156" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="111"/>
-      <c r="C156" s="181" t="s">
+      <c r="C156" s="186" t="s">
         <v>170</v>
       </c>
       <c r="D156" s="152"/>
@@ -5899,7 +5911,7 @@
     <row r="157" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="111"/>
-      <c r="C157" s="181"/>
+      <c r="C157" s="186"/>
       <c r="D157" s="148" t="s">
         <v>651</v>
       </c>
@@ -7039,7 +7051,7 @@
     <row r="224" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="B224" s="111"/>
-      <c r="C224" s="181" t="s">
+      <c r="C224" s="186" t="s">
         <v>146</v>
       </c>
       <c r="D224" s="152"/>
@@ -7051,7 +7063,7 @@
     <row r="225" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" s="111"/>
-      <c r="C225" s="181"/>
+      <c r="C225" s="186"/>
       <c r="D225" s="148" t="s">
         <v>274</v>
       </c>
@@ -7405,19 +7417,19 @@
         <v>335</v>
       </c>
       <c r="D248" s="112" t="s">
-        <v>325</v>
+        <v>654</v>
       </c>
       <c r="E248" s="175" t="s">
-        <v>326</v>
+        <v>655</v>
       </c>
       <c r="F248" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G248" s="114">
-        <v>44902</v>
+        <v>44970</v>
       </c>
       <c r="H248" s="115">
-        <v>44902</v>
+        <v>44970</v>
       </c>
     </row>
     <row r="249" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7425,19 +7437,19 @@
       <c r="B249" s="111"/>
       <c r="C249" s="112"/>
       <c r="D249" s="112" t="s">
-        <v>331</v>
+        <v>657</v>
       </c>
       <c r="E249" s="175" t="s">
-        <v>332</v>
+        <v>656</v>
       </c>
       <c r="F249" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G249" s="114">
-        <v>44897</v>
+        <v>44952</v>
       </c>
       <c r="H249" s="115">
-        <v>44897</v>
+        <v>44952</v>
       </c>
     </row>
     <row r="250" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7445,19 +7457,19 @@
       <c r="B250" s="111"/>
       <c r="C250" s="112"/>
       <c r="D250" s="112" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="E250" s="175" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="F250" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G250" s="114">
-        <v>44951</v>
+        <v>44902</v>
       </c>
       <c r="H250" s="115">
-        <v>44951</v>
+        <v>44902</v>
       </c>
     </row>
     <row r="251" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7465,160 +7477,160 @@
       <c r="B251" s="111"/>
       <c r="C251" s="112"/>
       <c r="D251" s="112" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E251" s="175" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F251" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G251" s="114">
-        <v>44951</v>
+        <v>44897</v>
       </c>
       <c r="H251" s="115">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="252" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+        <v>44897</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A252" s="1"/>
       <c r="B252" s="111"/>
       <c r="C252" s="112"/>
       <c r="D252" s="112" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="E252" s="175" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F252" s="113" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G252" s="114">
-        <v>44900</v>
+        <v>44951</v>
       </c>
       <c r="H252" s="115">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="253" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A253" s="1"/>
       <c r="B253" s="111"/>
       <c r="C253" s="112"/>
       <c r="D253" s="112" t="s">
-        <v>327</v>
-      </c>
-      <c r="E253" s="171" t="s">
-        <v>328</v>
+        <v>337</v>
+      </c>
+      <c r="E253" s="175" t="s">
+        <v>336</v>
       </c>
       <c r="F253" s="113" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G253" s="114">
-        <v>44896</v>
+        <v>44951</v>
       </c>
       <c r="H253" s="115">
-        <v>44896</v>
-      </c>
-    </row>
-    <row r="254" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="B254" s="111"/>
       <c r="C254" s="112"/>
       <c r="D254" s="112" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E254" s="175" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
       <c r="F254" s="113" t="s">
         <v>281</v>
       </c>
       <c r="G254" s="114">
-        <v>44945</v>
+        <v>44900</v>
       </c>
       <c r="H254" s="115">
         <v>44949</v>
       </c>
     </row>
-    <row r="255" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="B255" s="111"/>
       <c r="C255" s="112"/>
       <c r="D255" s="112" t="s">
-        <v>333</v>
-      </c>
-      <c r="E255" s="175" t="s">
-        <v>334</v>
+        <v>327</v>
+      </c>
+      <c r="E255" s="171" t="s">
+        <v>328</v>
       </c>
       <c r="F255" s="113" t="s">
         <v>281</v>
       </c>
       <c r="G255" s="114">
-        <v>44910</v>
+        <v>44896</v>
       </c>
       <c r="H255" s="115">
-        <v>44910</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>44896</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="B256" s="111"/>
       <c r="C256" s="112"/>
-      <c r="D256" s="163"/>
-      <c r="E256" s="172"/>
-      <c r="F256" s="163"/>
-      <c r="G256" s="163"/>
-      <c r="H256" s="164"/>
-    </row>
-    <row r="257" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="D256" s="112" t="s">
+        <v>321</v>
+      </c>
+      <c r="E256" s="175" t="s">
+        <v>338</v>
+      </c>
+      <c r="F256" s="113" t="s">
+        <v>281</v>
+      </c>
+      <c r="G256" s="114">
+        <v>44945</v>
+      </c>
+      <c r="H256" s="115">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A257" s="1"/>
       <c r="B257" s="111"/>
       <c r="C257" s="112"/>
-      <c r="D257" s="148" t="s">
-        <v>626</v>
-      </c>
-      <c r="E257" s="173" t="s">
-        <v>627</v>
-      </c>
-      <c r="F257" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G257" s="150">
-        <v>44965</v>
-      </c>
-      <c r="H257" s="151">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="258" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="D257" s="112" t="s">
+        <v>333</v>
+      </c>
+      <c r="E257" s="175" t="s">
+        <v>334</v>
+      </c>
+      <c r="F257" s="113" t="s">
+        <v>281</v>
+      </c>
+      <c r="G257" s="114">
+        <v>44910</v>
+      </c>
+      <c r="H257" s="115">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="B258" s="111"/>
       <c r="C258" s="112"/>
-      <c r="D258" s="148" t="s">
-        <v>624</v>
-      </c>
-      <c r="E258" s="173" t="s">
-        <v>625</v>
-      </c>
-      <c r="F258" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G258" s="150">
-        <v>44965</v>
-      </c>
-      <c r="H258" s="151">
-        <v>44965</v>
-      </c>
+      <c r="D258" s="163"/>
+      <c r="E258" s="172"/>
+      <c r="F258" s="163"/>
+      <c r="G258" s="163"/>
+      <c r="H258" s="164"/>
     </row>
     <row r="259" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="B259" s="111"/>
       <c r="C259" s="112"/>
       <c r="D259" s="148" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="E259" s="173" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="F259" s="149" t="s">
         <v>232</v>
@@ -7635,39 +7647,39 @@
       <c r="B260" s="111"/>
       <c r="C260" s="112"/>
       <c r="D260" s="148" t="s">
-        <v>574</v>
+        <v>624</v>
       </c>
       <c r="E260" s="173" t="s">
-        <v>575</v>
+        <v>625</v>
       </c>
       <c r="F260" s="149" t="s">
         <v>232</v>
       </c>
       <c r="G260" s="150">
-        <v>44964</v>
+        <v>44965</v>
       </c>
       <c r="H260" s="151">
-        <v>44964</v>
+        <v>44965</v>
       </c>
     </row>
     <row r="261" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A261" s="1"/>
       <c r="B261" s="111"/>
       <c r="C261" s="112"/>
-      <c r="D261" s="143" t="s">
-        <v>591</v>
-      </c>
-      <c r="E261" s="174" t="s">
-        <v>592</v>
-      </c>
-      <c r="F261" s="144" t="s">
-        <v>281</v>
-      </c>
-      <c r="G261" s="145">
-        <v>44964</v>
-      </c>
-      <c r="H261" s="146">
-        <v>44901</v>
+      <c r="D261" s="148" t="s">
+        <v>630</v>
+      </c>
+      <c r="E261" s="173" t="s">
+        <v>631</v>
+      </c>
+      <c r="F261" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G261" s="150">
+        <v>44965</v>
+      </c>
+      <c r="H261" s="151">
+        <v>44965</v>
       </c>
     </row>
     <row r="262" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
@@ -7675,89 +7687,99 @@
       <c r="B262" s="111"/>
       <c r="C262" s="112"/>
       <c r="D262" s="148" t="s">
-        <v>628</v>
+        <v>574</v>
       </c>
       <c r="E262" s="173" t="s">
-        <v>629</v>
+        <v>575</v>
       </c>
       <c r="F262" s="149" t="s">
         <v>232</v>
       </c>
       <c r="G262" s="150">
-        <v>44965</v>
+        <v>44964</v>
       </c>
       <c r="H262" s="151">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="263" spans="1:8" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+        <v>44964</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A263" s="1"/>
       <c r="B263" s="111"/>
       <c r="C263" s="112"/>
-      <c r="D263" s="148" t="s">
-        <v>620</v>
-      </c>
-      <c r="E263" s="173" t="s">
-        <v>622</v>
-      </c>
-      <c r="F263" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G263" s="150">
-        <v>44965</v>
-      </c>
-      <c r="H263" s="151">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="264" spans="1:8" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="D263" s="143" t="s">
+        <v>591</v>
+      </c>
+      <c r="E263" s="174" t="s">
+        <v>592</v>
+      </c>
+      <c r="F263" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="G263" s="145">
+        <v>44964</v>
+      </c>
+      <c r="H263" s="146">
+        <v>44901</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="B264" s="111"/>
       <c r="C264" s="112"/>
-      <c r="D264" s="112" t="s">
-        <v>621</v>
-      </c>
-      <c r="E264" s="175" t="s">
-        <v>623</v>
-      </c>
-      <c r="F264" s="113" t="s">
+      <c r="D264" s="148" t="s">
+        <v>628</v>
+      </c>
+      <c r="E264" s="173" t="s">
+        <v>629</v>
+      </c>
+      <c r="F264" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G264" s="114">
+      <c r="G264" s="150">
         <v>44965</v>
       </c>
-      <c r="H264" s="115">
+      <c r="H264" s="151">
         <v>44965</v>
       </c>
     </row>
-    <row r="265" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A265" s="1"/>
       <c r="B265" s="111"/>
       <c r="C265" s="112"/>
-      <c r="D265" s="163"/>
-      <c r="E265" s="172"/>
-      <c r="F265" s="163"/>
-      <c r="G265" s="163"/>
-      <c r="H265" s="164"/>
-    </row>
-    <row r="266" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D265" s="148" t="s">
+        <v>620</v>
+      </c>
+      <c r="E265" s="173" t="s">
+        <v>622</v>
+      </c>
+      <c r="F265" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G265" s="150">
+        <v>44965</v>
+      </c>
+      <c r="H265" s="151">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A266" s="1"/>
       <c r="B266" s="111"/>
       <c r="C266" s="112"/>
       <c r="D266" s="112" t="s">
-        <v>339</v>
+        <v>621</v>
       </c>
       <c r="E266" s="175" t="s">
-        <v>340</v>
+        <v>623</v>
       </c>
       <c r="F266" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G266" s="114">
-        <v>44951</v>
+        <v>44965</v>
       </c>
       <c r="H266" s="115">
-        <v>44951</v>
+        <v>44965</v>
       </c>
     </row>
     <row r="267" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7775,40 +7797,50 @@
       <c r="B268" s="111"/>
       <c r="C268" s="112"/>
       <c r="D268" s="112" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E268" s="175" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="F268" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G268" s="114">
-        <v>44952</v>
+        <v>44951</v>
       </c>
       <c r="H268" s="115">
-        <v>44952</v>
-      </c>
-    </row>
-    <row r="269" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="B269" s="111"/>
       <c r="C269" s="112"/>
-      <c r="D269" s="112"/>
-      <c r="E269" s="171"/>
-      <c r="F269" s="113"/>
-      <c r="G269" s="114"/>
-      <c r="H269" s="115"/>
-    </row>
-    <row r="270" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D269" s="163"/>
+      <c r="E269" s="172"/>
+      <c r="F269" s="163"/>
+      <c r="G269" s="163"/>
+      <c r="H269" s="164"/>
+    </row>
+    <row r="270" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="B270" s="111"/>
       <c r="C270" s="112"/>
-      <c r="D270" s="112"/>
-      <c r="E270" s="171"/>
-      <c r="F270" s="113"/>
-      <c r="G270" s="114"/>
-      <c r="H270" s="115"/>
+      <c r="D270" s="112" t="s">
+        <v>341</v>
+      </c>
+      <c r="E270" s="175" t="s">
+        <v>342</v>
+      </c>
+      <c r="F270" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G270" s="114">
+        <v>44952</v>
+      </c>
+      <c r="H270" s="115">
+        <v>44952</v>
+      </c>
     </row>
     <row r="271" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
@@ -7820,114 +7852,104 @@
       <c r="G271" s="114"/>
       <c r="H271" s="115"/>
     </row>
-    <row r="272" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
       <c r="B272" s="111"/>
       <c r="C272" s="112"/>
-      <c r="D272" s="112" t="s">
-        <v>393</v>
-      </c>
-      <c r="E272" s="175" t="s">
-        <v>394</v>
-      </c>
-      <c r="F272" s="113" t="s">
-        <v>267</v>
-      </c>
-      <c r="G272" s="114">
-        <v>44957</v>
-      </c>
-      <c r="H272" s="115">
-        <v>42982</v>
-      </c>
-    </row>
-    <row r="273" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="D272" s="112"/>
+      <c r="E272" s="171"/>
+      <c r="F272" s="113"/>
+      <c r="G272" s="114"/>
+      <c r="H272" s="115"/>
+    </row>
+    <row r="273" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A273" s="1"/>
       <c r="B273" s="111"/>
       <c r="C273" s="112"/>
-      <c r="D273" s="112" t="s">
-        <v>392</v>
-      </c>
-      <c r="E273" s="175" t="s">
-        <v>395</v>
-      </c>
-      <c r="F273" s="113" t="s">
-        <v>281</v>
-      </c>
-      <c r="G273" s="114">
-        <v>44281</v>
-      </c>
-      <c r="H273" s="115">
-        <v>44557</v>
-      </c>
-    </row>
-    <row r="274" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D273" s="112"/>
+      <c r="E273" s="171"/>
+      <c r="F273" s="113"/>
+      <c r="G273" s="114"/>
+      <c r="H273" s="115"/>
+    </row>
+    <row r="274" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="B274" s="111"/>
       <c r="C274" s="112"/>
       <c r="D274" s="112" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E274" s="175" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="F274" s="113" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G274" s="114">
-        <v>43257</v>
+        <v>44957</v>
       </c>
       <c r="H274" s="115">
-        <v>43257</v>
-      </c>
-    </row>
-    <row r="275" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="B275" s="111"/>
       <c r="C275" s="112"/>
       <c r="D275" s="112" t="s">
-        <v>285</v>
+        <v>392</v>
       </c>
       <c r="E275" s="175" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F275" s="113" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G275" s="114">
-        <v>44949</v>
+        <v>44281</v>
       </c>
       <c r="H275" s="115">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44557</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="B276" s="111"/>
       <c r="C276" s="112"/>
-      <c r="D276" s="112"/>
-      <c r="E276" s="175"/>
-      <c r="F276" s="113"/>
-      <c r="G276" s="114"/>
-      <c r="H276" s="115"/>
+      <c r="D276" s="112" t="s">
+        <v>396</v>
+      </c>
+      <c r="E276" s="175" t="s">
+        <v>397</v>
+      </c>
+      <c r="F276" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G276" s="114">
+        <v>43257</v>
+      </c>
+      <c r="H276" s="115">
+        <v>43257</v>
+      </c>
     </row>
     <row r="277" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A277" s="1"/>
       <c r="B277" s="111"/>
       <c r="C277" s="112"/>
       <c r="D277" s="112" t="s">
-        <v>391</v>
+        <v>285</v>
       </c>
       <c r="E277" s="175" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F277" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G277" s="114">
-        <v>44957</v>
+        <v>44949</v>
       </c>
       <c r="H277" s="115">
-        <v>44957</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="278" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -7940,35 +7962,35 @@
       <c r="G278" s="114"/>
       <c r="H278" s="115"/>
     </row>
-    <row r="279" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="B279" s="111"/>
       <c r="C279" s="112"/>
-      <c r="D279" s="112"/>
-      <c r="E279" s="171"/>
-      <c r="F279" s="113"/>
-      <c r="G279" s="114"/>
-      <c r="H279" s="115"/>
+      <c r="D279" s="112" t="s">
+        <v>391</v>
+      </c>
+      <c r="E279" s="175" t="s">
+        <v>399</v>
+      </c>
+      <c r="F279" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G279" s="114">
+        <v>44957</v>
+      </c>
+      <c r="H279" s="115">
+        <v>44957</v>
+      </c>
     </row>
     <row r="280" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="B280" s="111"/>
       <c r="C280" s="112"/>
-      <c r="D280" s="112" t="s">
-        <v>329</v>
-      </c>
-      <c r="E280" s="171" t="s">
-        <v>330</v>
-      </c>
-      <c r="F280" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G280" s="114">
-        <v>44893</v>
-      </c>
-      <c r="H280" s="115">
-        <v>44893</v>
-      </c>
+      <c r="D280" s="112"/>
+      <c r="E280" s="175"/>
+      <c r="F280" s="113"/>
+      <c r="G280" s="114"/>
+      <c r="H280" s="115"/>
     </row>
     <row r="281" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
@@ -7980,110 +8002,118 @@
       <c r="G281" s="114"/>
       <c r="H281" s="115"/>
     </row>
-    <row r="282" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A282" s="154"/>
-      <c r="B282" s="188" t="s">
+    <row r="282" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A282" s="1"/>
+      <c r="B282" s="111"/>
+      <c r="C282" s="112"/>
+      <c r="D282" s="112" t="s">
+        <v>329</v>
+      </c>
+      <c r="E282" s="171" t="s">
+        <v>330</v>
+      </c>
+      <c r="F282" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G282" s="114">
+        <v>44893</v>
+      </c>
+      <c r="H282" s="115">
+        <v>44893</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A283" s="1"/>
+      <c r="B283" s="111"/>
+      <c r="C283" s="112"/>
+      <c r="D283" s="112"/>
+      <c r="E283" s="171"/>
+      <c r="F283" s="113"/>
+      <c r="G283" s="114"/>
+      <c r="H283" s="115"/>
+    </row>
+    <row r="284" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A284" s="154"/>
+      <c r="B284" s="185" t="s">
         <v>143</v>
       </c>
-      <c r="C282" s="152"/>
-      <c r="D282" s="152"/>
-      <c r="E282" s="170"/>
-      <c r="F282" s="152"/>
-      <c r="G282" s="152"/>
-      <c r="H282" s="153"/>
-    </row>
-    <row r="283" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A283" s="154"/>
-      <c r="B283" s="188"/>
-      <c r="C283" s="181" t="s">
+      <c r="C284" s="152"/>
+      <c r="D284" s="152"/>
+      <c r="E284" s="170"/>
+      <c r="F284" s="152"/>
+      <c r="G284" s="152"/>
+      <c r="H284" s="153"/>
+    </row>
+    <row r="285" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="154"/>
+      <c r="B285" s="185"/>
+      <c r="C285" s="186" t="s">
         <v>160</v>
       </c>
-      <c r="D283" s="152"/>
-      <c r="E283" s="170"/>
-      <c r="F283" s="152"/>
-      <c r="G283" s="152"/>
-      <c r="H283" s="153"/>
-    </row>
-    <row r="284" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A284" s="1"/>
-      <c r="B284" s="111"/>
-      <c r="C284" s="181"/>
-      <c r="D284" s="112"/>
-      <c r="E284" s="171"/>
-      <c r="F284" s="113"/>
-      <c r="G284" s="114"/>
-      <c r="H284" s="115"/>
-    </row>
-    <row r="285" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A285" s="1"/>
-      <c r="B285" s="111"/>
-      <c r="C285" s="112"/>
-      <c r="D285" s="112"/>
-      <c r="E285" s="171"/>
-      <c r="F285" s="113"/>
-      <c r="G285" s="114"/>
-      <c r="H285" s="115"/>
-    </row>
-    <row r="286" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A286" s="154"/>
-      <c r="B286" s="188" t="s">
+      <c r="D285" s="152"/>
+      <c r="E285" s="170"/>
+      <c r="F285" s="152"/>
+      <c r="G285" s="152"/>
+      <c r="H285" s="153"/>
+    </row>
+    <row r="286" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A286" s="1"/>
+      <c r="B286" s="111"/>
+      <c r="C286" s="186"/>
+      <c r="D286" s="112"/>
+      <c r="E286" s="171"/>
+      <c r="F286" s="113"/>
+      <c r="G286" s="114"/>
+      <c r="H286" s="115"/>
+    </row>
+    <row r="287" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A287" s="1"/>
+      <c r="B287" s="111"/>
+      <c r="C287" s="112"/>
+      <c r="D287" s="112"/>
+      <c r="E287" s="171"/>
+      <c r="F287" s="113"/>
+      <c r="G287" s="114"/>
+      <c r="H287" s="115"/>
+    </row>
+    <row r="288" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A288" s="154"/>
+      <c r="B288" s="185" t="s">
         <v>142</v>
       </c>
-      <c r="C286" s="152"/>
-      <c r="D286" s="152"/>
-      <c r="E286" s="170"/>
-      <c r="F286" s="152"/>
-      <c r="G286" s="152"/>
-      <c r="H286" s="153"/>
-    </row>
-    <row r="287" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A287" s="154"/>
-      <c r="B287" s="188"/>
-      <c r="C287" s="181" t="s">
+      <c r="C288" s="152"/>
+      <c r="D288" s="152"/>
+      <c r="E288" s="170"/>
+      <c r="F288" s="152"/>
+      <c r="G288" s="152"/>
+      <c r="H288" s="153"/>
+    </row>
+    <row r="289" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="154"/>
+      <c r="B289" s="185"/>
+      <c r="C289" s="186" t="s">
         <v>148</v>
       </c>
-      <c r="D287" s="152"/>
-      <c r="E287" s="170"/>
-      <c r="F287" s="152"/>
-      <c r="G287" s="152"/>
-      <c r="H287" s="153"/>
-    </row>
-    <row r="288" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A288" s="1"/>
-      <c r="B288" s="111"/>
-      <c r="C288" s="181"/>
-      <c r="D288" s="112"/>
-      <c r="E288" s="171"/>
-      <c r="F288" s="113"/>
-      <c r="G288" s="114"/>
-      <c r="H288" s="115"/>
-    </row>
-    <row r="289" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A289" s="1"/>
-      <c r="B289" s="111"/>
-      <c r="C289" s="112"/>
-      <c r="D289" s="112"/>
-      <c r="E289" s="171"/>
-      <c r="F289" s="113"/>
-      <c r="G289" s="114"/>
-      <c r="H289" s="115"/>
+      <c r="D289" s="152"/>
+      <c r="E289" s="170"/>
+      <c r="F289" s="152"/>
+      <c r="G289" s="152"/>
+      <c r="H289" s="153"/>
     </row>
     <row r="290" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A290" s="1"/>
       <c r="B290" s="111"/>
-      <c r="C290" s="181" t="s">
-        <v>149</v>
-      </c>
-      <c r="D290" s="152"/>
-      <c r="E290" s="170"/>
-      <c r="F290" s="152"/>
-      <c r="G290" s="152"/>
-      <c r="H290" s="153"/>
+      <c r="C290" s="186"/>
+      <c r="D290" s="112"/>
+      <c r="E290" s="171"/>
+      <c r="F290" s="113"/>
+      <c r="G290" s="114"/>
+      <c r="H290" s="115"/>
     </row>
     <row r="291" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="B291" s="111"/>
-      <c r="C291" s="181"/>
+      <c r="C291" s="112"/>
       <c r="D291" s="112"/>
       <c r="E291" s="171"/>
       <c r="F291" s="113"/>
@@ -8093,29 +8123,29 @@
     <row r="292" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="B292" s="111"/>
-      <c r="C292" s="112"/>
-      <c r="D292" s="112"/>
-      <c r="E292" s="171"/>
-      <c r="F292" s="113"/>
-      <c r="G292" s="114"/>
-      <c r="H292" s="115"/>
+      <c r="C292" s="186" t="s">
+        <v>149</v>
+      </c>
+      <c r="D292" s="152"/>
+      <c r="E292" s="170"/>
+      <c r="F292" s="152"/>
+      <c r="G292" s="152"/>
+      <c r="H292" s="153"/>
     </row>
     <row r="293" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="B293" s="111"/>
-      <c r="C293" s="181" t="s">
-        <v>150</v>
-      </c>
-      <c r="D293" s="152"/>
-      <c r="E293" s="170"/>
-      <c r="F293" s="152"/>
-      <c r="G293" s="152"/>
-      <c r="H293" s="153"/>
+      <c r="C293" s="186"/>
+      <c r="D293" s="112"/>
+      <c r="E293" s="171"/>
+      <c r="F293" s="113"/>
+      <c r="G293" s="114"/>
+      <c r="H293" s="115"/>
     </row>
     <row r="294" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="B294" s="111"/>
-      <c r="C294" s="181"/>
+      <c r="C294" s="112"/>
       <c r="D294" s="112"/>
       <c r="E294" s="171"/>
       <c r="F294" s="113"/>
@@ -8125,29 +8155,29 @@
     <row r="295" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="B295" s="111"/>
-      <c r="C295" s="112"/>
-      <c r="D295" s="112"/>
-      <c r="E295" s="171"/>
-      <c r="F295" s="113"/>
-      <c r="G295" s="114"/>
-      <c r="H295" s="115"/>
+      <c r="C295" s="186" t="s">
+        <v>150</v>
+      </c>
+      <c r="D295" s="152"/>
+      <c r="E295" s="170"/>
+      <c r="F295" s="152"/>
+      <c r="G295" s="152"/>
+      <c r="H295" s="153"/>
     </row>
     <row r="296" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="B296" s="111"/>
-      <c r="C296" s="181" t="s">
-        <v>151</v>
-      </c>
-      <c r="D296" s="152"/>
-      <c r="E296" s="170"/>
-      <c r="F296" s="152"/>
-      <c r="G296" s="152"/>
-      <c r="H296" s="153"/>
+      <c r="C296" s="186"/>
+      <c r="D296" s="112"/>
+      <c r="E296" s="171"/>
+      <c r="F296" s="113"/>
+      <c r="G296" s="114"/>
+      <c r="H296" s="115"/>
     </row>
     <row r="297" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="B297" s="111"/>
-      <c r="C297" s="181"/>
+      <c r="C297" s="112"/>
       <c r="D297" s="112"/>
       <c r="E297" s="171"/>
       <c r="F297" s="113"/>
@@ -8157,29 +8187,29 @@
     <row r="298" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="B298" s="111"/>
-      <c r="C298" s="112"/>
-      <c r="D298" s="112"/>
-      <c r="E298" s="171"/>
-      <c r="F298" s="113"/>
-      <c r="G298" s="114"/>
-      <c r="H298" s="115"/>
+      <c r="C298" s="186" t="s">
+        <v>151</v>
+      </c>
+      <c r="D298" s="152"/>
+      <c r="E298" s="170"/>
+      <c r="F298" s="152"/>
+      <c r="G298" s="152"/>
+      <c r="H298" s="153"/>
     </row>
     <row r="299" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="B299" s="111"/>
-      <c r="C299" s="181" t="s">
-        <v>152</v>
-      </c>
-      <c r="D299" s="152"/>
-      <c r="E299" s="170"/>
-      <c r="F299" s="152"/>
-      <c r="G299" s="152"/>
-      <c r="H299" s="153"/>
+      <c r="C299" s="186"/>
+      <c r="D299" s="112"/>
+      <c r="E299" s="171"/>
+      <c r="F299" s="113"/>
+      <c r="G299" s="114"/>
+      <c r="H299" s="115"/>
     </row>
     <row r="300" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="B300" s="111"/>
-      <c r="C300" s="181"/>
+      <c r="C300" s="112"/>
       <c r="D300" s="112"/>
       <c r="E300" s="171"/>
       <c r="F300" s="113"/>
@@ -8189,29 +8219,29 @@
     <row r="301" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="B301" s="111"/>
-      <c r="C301" s="112"/>
-      <c r="D301" s="112"/>
-      <c r="E301" s="171"/>
-      <c r="F301" s="113"/>
-      <c r="G301" s="114"/>
-      <c r="H301" s="115"/>
+      <c r="C301" s="186" t="s">
+        <v>152</v>
+      </c>
+      <c r="D301" s="152"/>
+      <c r="E301" s="170"/>
+      <c r="F301" s="152"/>
+      <c r="G301" s="152"/>
+      <c r="H301" s="153"/>
     </row>
     <row r="302" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="B302" s="111"/>
-      <c r="C302" s="181" t="s">
-        <v>153</v>
-      </c>
-      <c r="D302" s="152"/>
-      <c r="E302" s="170"/>
-      <c r="F302" s="152"/>
-      <c r="G302" s="152"/>
-      <c r="H302" s="153"/>
+      <c r="C302" s="186"/>
+      <c r="D302" s="112"/>
+      <c r="E302" s="171"/>
+      <c r="F302" s="113"/>
+      <c r="G302" s="114"/>
+      <c r="H302" s="115"/>
     </row>
     <row r="303" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="B303" s="111"/>
-      <c r="C303" s="181"/>
+      <c r="C303" s="112"/>
       <c r="D303" s="112"/>
       <c r="E303" s="171"/>
       <c r="F303" s="113"/>
@@ -8221,29 +8251,29 @@
     <row r="304" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="B304" s="111"/>
-      <c r="C304" s="112"/>
-      <c r="D304" s="112"/>
-      <c r="E304" s="171"/>
-      <c r="F304" s="113"/>
-      <c r="G304" s="114"/>
-      <c r="H304" s="115"/>
+      <c r="C304" s="186" t="s">
+        <v>153</v>
+      </c>
+      <c r="D304" s="152"/>
+      <c r="E304" s="170"/>
+      <c r="F304" s="152"/>
+      <c r="G304" s="152"/>
+      <c r="H304" s="153"/>
     </row>
     <row r="305" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A305" s="1"/>
       <c r="B305" s="111"/>
-      <c r="C305" s="181" t="s">
-        <v>154</v>
-      </c>
-      <c r="D305" s="152"/>
-      <c r="E305" s="170"/>
-      <c r="F305" s="152"/>
-      <c r="G305" s="152"/>
-      <c r="H305" s="153"/>
+      <c r="C305" s="186"/>
+      <c r="D305" s="112"/>
+      <c r="E305" s="171"/>
+      <c r="F305" s="113"/>
+      <c r="G305" s="114"/>
+      <c r="H305" s="115"/>
     </row>
     <row r="306" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A306" s="1"/>
       <c r="B306" s="111"/>
-      <c r="C306" s="181"/>
+      <c r="C306" s="112"/>
       <c r="D306" s="112"/>
       <c r="E306" s="171"/>
       <c r="F306" s="113"/>
@@ -8253,29 +8283,29 @@
     <row r="307" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A307" s="1"/>
       <c r="B307" s="111"/>
-      <c r="C307" s="112"/>
-      <c r="D307" s="112"/>
-      <c r="E307" s="171"/>
-      <c r="F307" s="113"/>
-      <c r="G307" s="114"/>
-      <c r="H307" s="115"/>
+      <c r="C307" s="186" t="s">
+        <v>154</v>
+      </c>
+      <c r="D307" s="152"/>
+      <c r="E307" s="170"/>
+      <c r="F307" s="152"/>
+      <c r="G307" s="152"/>
+      <c r="H307" s="153"/>
     </row>
     <row r="308" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A308" s="1"/>
       <c r="B308" s="111"/>
-      <c r="C308" s="181" t="s">
-        <v>155</v>
-      </c>
-      <c r="D308" s="152"/>
-      <c r="E308" s="170"/>
-      <c r="F308" s="152"/>
-      <c r="G308" s="152"/>
-      <c r="H308" s="153"/>
+      <c r="C308" s="186"/>
+      <c r="D308" s="112"/>
+      <c r="E308" s="171"/>
+      <c r="F308" s="113"/>
+      <c r="G308" s="114"/>
+      <c r="H308" s="115"/>
     </row>
     <row r="309" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A309" s="1"/>
       <c r="B309" s="111"/>
-      <c r="C309" s="181"/>
+      <c r="C309" s="112"/>
       <c r="D309" s="112"/>
       <c r="E309" s="171"/>
       <c r="F309" s="113"/>
@@ -8285,29 +8315,29 @@
     <row r="310" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A310" s="1"/>
       <c r="B310" s="111"/>
-      <c r="C310" s="112"/>
-      <c r="D310" s="112"/>
-      <c r="E310" s="171"/>
-      <c r="F310" s="113"/>
-      <c r="G310" s="114"/>
-      <c r="H310" s="115"/>
+      <c r="C310" s="186" t="s">
+        <v>155</v>
+      </c>
+      <c r="D310" s="152"/>
+      <c r="E310" s="170"/>
+      <c r="F310" s="152"/>
+      <c r="G310" s="152"/>
+      <c r="H310" s="153"/>
     </row>
     <row r="311" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A311" s="1"/>
       <c r="B311" s="111"/>
-      <c r="C311" s="181" t="s">
-        <v>156</v>
-      </c>
-      <c r="D311" s="152"/>
-      <c r="E311" s="170"/>
-      <c r="F311" s="152"/>
-      <c r="G311" s="152"/>
-      <c r="H311" s="153"/>
+      <c r="C311" s="186"/>
+      <c r="D311" s="112"/>
+      <c r="E311" s="171"/>
+      <c r="F311" s="113"/>
+      <c r="G311" s="114"/>
+      <c r="H311" s="115"/>
     </row>
     <row r="312" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A312" s="1"/>
       <c r="B312" s="111"/>
-      <c r="C312" s="181"/>
+      <c r="C312" s="112"/>
       <c r="D312" s="112"/>
       <c r="E312" s="171"/>
       <c r="F312" s="113"/>
@@ -8317,29 +8347,29 @@
     <row r="313" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A313" s="1"/>
       <c r="B313" s="111"/>
-      <c r="C313" s="112"/>
-      <c r="D313" s="112"/>
-      <c r="E313" s="171"/>
-      <c r="F313" s="113"/>
-      <c r="G313" s="114"/>
-      <c r="H313" s="115"/>
+      <c r="C313" s="186" t="s">
+        <v>156</v>
+      </c>
+      <c r="D313" s="152"/>
+      <c r="E313" s="170"/>
+      <c r="F313" s="152"/>
+      <c r="G313" s="152"/>
+      <c r="H313" s="153"/>
     </row>
     <row r="314" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A314" s="1"/>
       <c r="B314" s="111"/>
-      <c r="C314" s="181" t="s">
-        <v>157</v>
-      </c>
-      <c r="D314" s="152"/>
-      <c r="E314" s="170"/>
-      <c r="F314" s="152"/>
-      <c r="G314" s="152"/>
-      <c r="H314" s="153"/>
+      <c r="C314" s="186"/>
+      <c r="D314" s="112"/>
+      <c r="E314" s="171"/>
+      <c r="F314" s="113"/>
+      <c r="G314" s="114"/>
+      <c r="H314" s="115"/>
     </row>
     <row r="315" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A315" s="1"/>
       <c r="B315" s="111"/>
-      <c r="C315" s="181"/>
+      <c r="C315" s="112"/>
       <c r="D315" s="112"/>
       <c r="E315" s="171"/>
       <c r="F315" s="113"/>
@@ -8349,83 +8379,65 @@
     <row r="316" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A316" s="1"/>
       <c r="B316" s="111"/>
-      <c r="C316" s="112"/>
-      <c r="D316" s="112"/>
-      <c r="E316" s="171"/>
-      <c r="F316" s="113"/>
-      <c r="G316" s="114"/>
-      <c r="H316" s="115"/>
+      <c r="C316" s="186" t="s">
+        <v>157</v>
+      </c>
+      <c r="D316" s="152"/>
+      <c r="E316" s="170"/>
+      <c r="F316" s="152"/>
+      <c r="G316" s="152"/>
+      <c r="H316" s="153"/>
     </row>
     <row r="317" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A317" s="1"/>
       <c r="B317" s="111"/>
-      <c r="C317" s="181" t="s">
-        <v>158</v>
-      </c>
-      <c r="D317" s="152"/>
-      <c r="E317" s="170"/>
-      <c r="F317" s="152"/>
-      <c r="G317" s="152"/>
-      <c r="H317" s="153"/>
+      <c r="C317" s="186"/>
+      <c r="D317" s="112"/>
+      <c r="E317" s="171"/>
+      <c r="F317" s="113"/>
+      <c r="G317" s="114"/>
+      <c r="H317" s="115"/>
     </row>
     <row r="318" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
       <c r="B318" s="111"/>
-      <c r="C318" s="181"/>
-      <c r="D318" s="148" t="s">
-        <v>470</v>
-      </c>
-      <c r="E318" s="178" t="s">
-        <v>471</v>
-      </c>
-      <c r="F318" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G318" s="150">
-        <v>44663</v>
-      </c>
-      <c r="H318" s="151">
-        <v>44663</v>
-      </c>
+      <c r="C318" s="112"/>
+      <c r="D318" s="112"/>
+      <c r="E318" s="171"/>
+      <c r="F318" s="113"/>
+      <c r="G318" s="114"/>
+      <c r="H318" s="115"/>
     </row>
     <row r="319" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
       <c r="B319" s="111"/>
-      <c r="C319" s="112"/>
-      <c r="D319" s="143" t="s">
-        <v>472</v>
-      </c>
-      <c r="E319" s="176" t="s">
-        <v>473</v>
-      </c>
-      <c r="F319" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="G319" s="145">
-        <v>44663</v>
-      </c>
-      <c r="H319" s="146">
-        <v>44663</v>
-      </c>
+      <c r="C319" s="186" t="s">
+        <v>158</v>
+      </c>
+      <c r="D319" s="152"/>
+      <c r="E319" s="170"/>
+      <c r="F319" s="152"/>
+      <c r="G319" s="152"/>
+      <c r="H319" s="153"/>
     </row>
     <row r="320" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
       <c r="B320" s="111"/>
-      <c r="C320" s="112"/>
-      <c r="D320" s="143" t="s">
-        <v>475</v>
-      </c>
-      <c r="E320" s="176" t="s">
-        <v>474</v>
-      </c>
-      <c r="F320" s="144" t="s">
+      <c r="C320" s="186"/>
+      <c r="D320" s="148" t="s">
+        <v>470</v>
+      </c>
+      <c r="E320" s="178" t="s">
+        <v>471</v>
+      </c>
+      <c r="F320" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G320" s="145">
-        <v>44630</v>
-      </c>
-      <c r="H320" s="146">
-        <v>44630</v>
+      <c r="G320" s="150">
+        <v>44663</v>
+      </c>
+      <c r="H320" s="151">
+        <v>44663</v>
       </c>
     </row>
     <row r="321" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8433,19 +8445,19 @@
       <c r="B321" s="111"/>
       <c r="C321" s="112"/>
       <c r="D321" s="143" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="E321" s="176" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F321" s="144" t="s">
         <v>232</v>
       </c>
       <c r="G321" s="145">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="H321" s="146">
-        <v>44630</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="322" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8453,16 +8465,16 @@
       <c r="B322" s="111"/>
       <c r="C322" s="112"/>
       <c r="D322" s="143" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="E322" s="176" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="F322" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G322" s="145">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H322" s="146">
         <v>44630</v>
@@ -8473,16 +8485,16 @@
       <c r="B323" s="111"/>
       <c r="C323" s="112"/>
       <c r="D323" s="143" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="E323" s="176" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F323" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G323" s="145">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H323" s="146">
         <v>44630</v>
@@ -8493,19 +8505,19 @@
       <c r="B324" s="111"/>
       <c r="C324" s="112"/>
       <c r="D324" s="143" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E324" s="176" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F324" s="144" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G324" s="145">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H324" s="146">
-        <v>44824</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="325" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8513,19 +8525,19 @@
       <c r="B325" s="111"/>
       <c r="C325" s="112"/>
       <c r="D325" s="143" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E325" s="176" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="F325" s="144" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G325" s="145">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H325" s="146">
-        <v>44824</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="326" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8533,19 +8545,19 @@
       <c r="B326" s="111"/>
       <c r="C326" s="112"/>
       <c r="D326" s="143" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E326" s="176" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F326" s="144" t="s">
-        <v>463</v>
+        <v>256</v>
       </c>
       <c r="G326" s="145">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H326" s="146">
-        <v>44622</v>
+        <v>44824</v>
       </c>
     </row>
     <row r="327" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8553,19 +8565,19 @@
       <c r="B327" s="111"/>
       <c r="C327" s="112"/>
       <c r="D327" s="143" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E327" s="176" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="F327" s="144" t="s">
-        <v>463</v>
+        <v>256</v>
       </c>
       <c r="G327" s="145">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H327" s="146">
-        <v>44621</v>
+        <v>44824</v>
       </c>
     </row>
     <row r="328" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8573,19 +8585,19 @@
       <c r="B328" s="111"/>
       <c r="C328" s="112"/>
       <c r="D328" s="143" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E328" s="176" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="F328" s="144" t="s">
         <v>463</v>
       </c>
       <c r="G328" s="145">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H328" s="146">
-        <v>44732</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="329" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8593,19 +8605,19 @@
       <c r="B329" s="111"/>
       <c r="C329" s="112"/>
       <c r="D329" s="143" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E329" s="176" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F329" s="144" t="s">
         <v>463</v>
       </c>
       <c r="G329" s="145">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H329" s="146">
-        <v>44732</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="330" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8613,19 +8625,19 @@
       <c r="B330" s="111"/>
       <c r="C330" s="112"/>
       <c r="D330" s="143" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E330" s="176" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="F330" s="144" t="s">
-        <v>496</v>
+        <v>463</v>
       </c>
       <c r="G330" s="145">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H330" s="146">
-        <v>44621</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="331" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8633,19 +8645,19 @@
       <c r="B331" s="111"/>
       <c r="C331" s="112"/>
       <c r="D331" s="143" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="E331" s="176" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F331" s="144" t="s">
-        <v>496</v>
+        <v>463</v>
       </c>
       <c r="G331" s="145">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H331" s="146">
-        <v>44621</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="332" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8653,19 +8665,19 @@
       <c r="B332" s="111"/>
       <c r="C332" s="112"/>
       <c r="D332" s="143" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E332" s="176" t="s">
-        <v>501</v>
+        <v>495</v>
       </c>
       <c r="F332" s="144" t="s">
-        <v>267</v>
+        <v>496</v>
       </c>
       <c r="G332" s="145">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H332" s="146">
-        <v>44622</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="333" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8673,16 +8685,16 @@
       <c r="B333" s="111"/>
       <c r="C333" s="112"/>
       <c r="D333" s="143" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="E333" s="176" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="F333" s="144" t="s">
-        <v>267</v>
+        <v>496</v>
       </c>
       <c r="G333" s="145">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H333" s="146">
         <v>44621</v>
@@ -8693,19 +8705,19 @@
       <c r="B334" s="111"/>
       <c r="C334" s="112"/>
       <c r="D334" s="143" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="E334" s="176" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="F334" s="144" t="s">
-        <v>463</v>
+        <v>267</v>
       </c>
       <c r="G334" s="145">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H334" s="146">
-        <v>44621</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="335" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8713,16 +8725,16 @@
       <c r="B335" s="111"/>
       <c r="C335" s="112"/>
       <c r="D335" s="143" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="E335" s="176" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F335" s="144" t="s">
-        <v>463</v>
+        <v>267</v>
       </c>
       <c r="G335" s="145">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H335" s="146">
         <v>44621</v>
@@ -8733,19 +8745,19 @@
       <c r="B336" s="111"/>
       <c r="C336" s="112"/>
       <c r="D336" s="143" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="E336" s="176" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="F336" s="144" t="s">
-        <v>267</v>
+        <v>463</v>
       </c>
       <c r="G336" s="145">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H336" s="146">
-        <v>44627</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="337" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8753,19 +8765,19 @@
       <c r="B337" s="111"/>
       <c r="C337" s="112"/>
       <c r="D337" s="143" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E337" s="176" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F337" s="144" t="s">
-        <v>267</v>
+        <v>463</v>
       </c>
       <c r="G337" s="145">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H337" s="146">
-        <v>44627</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="338" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8773,19 +8785,19 @@
       <c r="B338" s="111"/>
       <c r="C338" s="112"/>
       <c r="D338" s="143" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E338" s="176" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="F338" s="144" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G338" s="145">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H338" s="146">
-        <v>44628</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="339" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8793,19 +8805,19 @@
       <c r="B339" s="111"/>
       <c r="C339" s="112"/>
       <c r="D339" s="143" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E339" s="176" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F339" s="144" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G339" s="145">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H339" s="146">
-        <v>44628</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="340" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8813,16 +8825,16 @@
       <c r="B340" s="111"/>
       <c r="C340" s="112"/>
       <c r="D340" s="143" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E340" s="176" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="F340" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G340" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H340" s="146">
         <v>44628</v>
@@ -8833,16 +8845,16 @@
       <c r="B341" s="111"/>
       <c r="C341" s="112"/>
       <c r="D341" s="143" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="E341" s="176" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F341" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G341" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H341" s="146">
         <v>44628</v>
@@ -8853,16 +8865,16 @@
       <c r="B342" s="111"/>
       <c r="C342" s="112"/>
       <c r="D342" s="143" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E342" s="176" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="F342" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G342" s="145">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H342" s="146">
         <v>44628</v>
@@ -8873,16 +8885,16 @@
       <c r="B343" s="111"/>
       <c r="C343" s="112"/>
       <c r="D343" s="143" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="E343" s="176" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="F343" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G343" s="145">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H343" s="146">
         <v>44628</v>
@@ -8893,16 +8905,16 @@
       <c r="B344" s="111"/>
       <c r="C344" s="112"/>
       <c r="D344" s="143" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E344" s="176" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="F344" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G344" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H344" s="146">
         <v>44628</v>
@@ -8913,16 +8925,16 @@
       <c r="B345" s="111"/>
       <c r="C345" s="112"/>
       <c r="D345" s="143" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E345" s="176" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="F345" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G345" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H345" s="146">
         <v>44628</v>
@@ -8933,19 +8945,19 @@
       <c r="B346" s="111"/>
       <c r="C346" s="112"/>
       <c r="D346" s="143" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E346" s="176" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="F346" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G346" s="145">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H346" s="146">
-        <v>44617</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="347" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8953,19 +8965,19 @@
       <c r="B347" s="111"/>
       <c r="C347" s="112"/>
       <c r="D347" s="143" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="E347" s="176" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F347" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G347" s="145">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H347" s="146">
-        <v>44617</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="348" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8973,19 +8985,19 @@
       <c r="B348" s="111"/>
       <c r="C348" s="112"/>
       <c r="D348" s="143" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="E348" s="176" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="F348" s="144" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G348" s="145">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H348" s="146">
-        <v>44662</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="349" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8993,182 +9005,182 @@
       <c r="B349" s="111"/>
       <c r="C349" s="112"/>
       <c r="D349" s="143" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="E349" s="176" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F349" s="144" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G349" s="145">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H349" s="146">
-        <v>44662</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="350" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A350" s="1"/>
       <c r="B350" s="111"/>
       <c r="C350" s="112"/>
-      <c r="D350" s="112"/>
-      <c r="E350" s="171"/>
-      <c r="F350" s="113"/>
-      <c r="G350" s="114"/>
-      <c r="H350" s="115"/>
+      <c r="D350" s="143" t="s">
+        <v>531</v>
+      </c>
+      <c r="E350" s="176" t="s">
+        <v>532</v>
+      </c>
+      <c r="F350" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G350" s="145">
+        <v>44740</v>
+      </c>
+      <c r="H350" s="146">
+        <v>44662</v>
+      </c>
     </row>
     <row r="351" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A351" s="1"/>
       <c r="B351" s="111"/>
-      <c r="C351" s="181" t="s">
-        <v>147</v>
-      </c>
-      <c r="D351" s="152"/>
-      <c r="E351" s="170"/>
-      <c r="F351" s="152"/>
-      <c r="G351" s="152"/>
-      <c r="H351" s="153"/>
+      <c r="C351" s="112"/>
+      <c r="D351" s="143" t="s">
+        <v>534</v>
+      </c>
+      <c r="E351" s="176" t="s">
+        <v>533</v>
+      </c>
+      <c r="F351" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G351" s="145">
+        <v>44740</v>
+      </c>
+      <c r="H351" s="146">
+        <v>44662</v>
+      </c>
     </row>
     <row r="352" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A352" s="1"/>
       <c r="B352" s="111"/>
-      <c r="C352" s="181"/>
-      <c r="D352" s="148" t="s">
-        <v>274</v>
-      </c>
-      <c r="E352" s="178" t="s">
-        <v>448</v>
-      </c>
-      <c r="F352" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G352" s="150">
-        <v>44167</v>
-      </c>
-      <c r="H352" s="151">
-        <v>44167</v>
-      </c>
+      <c r="C352" s="112"/>
+      <c r="D352" s="112"/>
+      <c r="E352" s="171"/>
+      <c r="F352" s="113"/>
+      <c r="G352" s="114"/>
+      <c r="H352" s="115"/>
     </row>
     <row r="353" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="B353" s="111"/>
-      <c r="C353" s="112"/>
-      <c r="D353" s="143" t="s">
-        <v>449</v>
-      </c>
-      <c r="E353" s="176" t="s">
-        <v>450</v>
-      </c>
-      <c r="F353" s="144" t="s">
-        <v>256</v>
-      </c>
-      <c r="G353" s="145">
-        <v>44575</v>
-      </c>
-      <c r="H353" s="146">
-        <v>44167</v>
-      </c>
-    </row>
-    <row r="354" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C353" s="186" t="s">
+        <v>147</v>
+      </c>
+      <c r="D353" s="152"/>
+      <c r="E353" s="170"/>
+      <c r="F353" s="152"/>
+      <c r="G353" s="152"/>
+      <c r="H353" s="153"/>
+    </row>
+    <row r="354" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="B354" s="111"/>
-      <c r="C354" s="112"/>
-      <c r="D354" s="143" t="s">
-        <v>452</v>
-      </c>
-      <c r="E354" s="174" t="s">
-        <v>451</v>
-      </c>
-      <c r="F354" s="144" t="s">
-        <v>281</v>
-      </c>
-      <c r="G354" s="145">
-        <v>44404</v>
-      </c>
-      <c r="H354" s="146">
-        <v>44404</v>
+      <c r="C354" s="186"/>
+      <c r="D354" s="148" t="s">
+        <v>274</v>
+      </c>
+      <c r="E354" s="178" t="s">
+        <v>448</v>
+      </c>
+      <c r="F354" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G354" s="150">
+        <v>44167</v>
+      </c>
+      <c r="H354" s="151">
+        <v>44167</v>
       </c>
     </row>
     <row r="355" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A355" s="1"/>
       <c r="B355" s="111"/>
       <c r="C355" s="112"/>
-      <c r="D355" s="112"/>
-      <c r="E355" s="171"/>
-      <c r="F355" s="113"/>
-      <c r="G355" s="114"/>
-      <c r="H355" s="115"/>
-    </row>
-    <row r="356" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D355" s="143" t="s">
+        <v>449</v>
+      </c>
+      <c r="E355" s="176" t="s">
+        <v>450</v>
+      </c>
+      <c r="F355" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G355" s="145">
+        <v>44575</v>
+      </c>
+      <c r="H355" s="146">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="B356" s="111"/>
-      <c r="C356" s="181" t="s">
-        <v>159</v>
-      </c>
-      <c r="D356" s="152"/>
-      <c r="E356" s="170"/>
-      <c r="F356" s="152"/>
-      <c r="G356" s="152"/>
-      <c r="H356" s="153"/>
+      <c r="C356" s="112"/>
+      <c r="D356" s="143" t="s">
+        <v>452</v>
+      </c>
+      <c r="E356" s="174" t="s">
+        <v>451</v>
+      </c>
+      <c r="F356" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="G356" s="145">
+        <v>44404</v>
+      </c>
+      <c r="H356" s="146">
+        <v>44404</v>
+      </c>
     </row>
     <row r="357" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="B357" s="111"/>
-      <c r="C357" s="181"/>
-      <c r="D357" s="148" t="s">
-        <v>454</v>
-      </c>
-      <c r="E357" s="178" t="s">
-        <v>453</v>
-      </c>
-      <c r="F357" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G357" s="150">
-        <v>44635</v>
-      </c>
-      <c r="H357" s="151">
-        <v>44635</v>
-      </c>
+      <c r="C357" s="112"/>
+      <c r="D357" s="112"/>
+      <c r="E357" s="171"/>
+      <c r="F357" s="113"/>
+      <c r="G357" s="114"/>
+      <c r="H357" s="115"/>
     </row>
     <row r="358" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="B358" s="111"/>
-      <c r="C358" s="112"/>
-      <c r="D358" s="143" t="s">
-        <v>456</v>
-      </c>
-      <c r="E358" s="176" t="s">
-        <v>455</v>
-      </c>
-      <c r="F358" s="144" t="s">
-        <v>232</v>
-      </c>
-      <c r="G358" s="145">
-        <v>44635</v>
-      </c>
-      <c r="H358" s="146">
-        <v>44635</v>
-      </c>
+      <c r="C358" s="186" t="s">
+        <v>159</v>
+      </c>
+      <c r="D358" s="152"/>
+      <c r="E358" s="170"/>
+      <c r="F358" s="152"/>
+      <c r="G358" s="152"/>
+      <c r="H358" s="153"/>
     </row>
     <row r="359" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A359" s="1"/>
       <c r="B359" s="111"/>
-      <c r="C359" s="112"/>
-      <c r="D359" s="143" t="s">
-        <v>457</v>
-      </c>
-      <c r="E359" s="176" t="s">
-        <v>459</v>
-      </c>
-      <c r="F359" s="144" t="s">
+      <c r="C359" s="186"/>
+      <c r="D359" s="148" t="s">
+        <v>454</v>
+      </c>
+      <c r="E359" s="178" t="s">
+        <v>453</v>
+      </c>
+      <c r="F359" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G359" s="145">
+      <c r="G359" s="150">
         <v>44635</v>
       </c>
-      <c r="H359" s="146">
+      <c r="H359" s="151">
         <v>44635</v>
       </c>
     </row>
@@ -9177,10 +9189,10 @@
       <c r="B360" s="111"/>
       <c r="C360" s="112"/>
       <c r="D360" s="143" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="E360" s="176" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F360" s="144" t="s">
         <v>232</v>
@@ -9197,19 +9209,19 @@
       <c r="B361" s="111"/>
       <c r="C361" s="112"/>
       <c r="D361" s="143" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E361" s="176" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="F361" s="144" t="s">
-        <v>463</v>
+        <v>232</v>
       </c>
       <c r="G361" s="145">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H361" s="146">
-        <v>44644</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="362" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9217,19 +9229,19 @@
       <c r="B362" s="111"/>
       <c r="C362" s="112"/>
       <c r="D362" s="143" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E362" s="176" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="F362" s="144" t="s">
-        <v>463</v>
+        <v>232</v>
       </c>
       <c r="G362" s="145">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H362" s="146">
-        <v>44644</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="363" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9237,19 +9249,19 @@
       <c r="B363" s="111"/>
       <c r="C363" s="112"/>
       <c r="D363" s="143" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="E363" s="176" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="F363" s="144" t="s">
-        <v>267</v>
+        <v>463</v>
       </c>
       <c r="G363" s="145">
+        <v>44701</v>
+      </c>
+      <c r="H363" s="146">
         <v>44644</v>
-      </c>
-      <c r="H363" s="146">
-        <v>44636</v>
       </c>
     </row>
     <row r="364" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9257,50 +9269,70 @@
       <c r="B364" s="111"/>
       <c r="C364" s="112"/>
       <c r="D364" s="143" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="E364" s="176" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F364" s="144" t="s">
+        <v>463</v>
+      </c>
+      <c r="G364" s="145">
+        <v>44701</v>
+      </c>
+      <c r="H364" s="146">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A365" s="1"/>
+      <c r="B365" s="111"/>
+      <c r="C365" s="112"/>
+      <c r="D365" s="143" t="s">
+        <v>466</v>
+      </c>
+      <c r="E365" s="176" t="s">
+        <v>467</v>
+      </c>
+      <c r="F365" s="144" t="s">
         <v>267</v>
       </c>
-      <c r="G364" s="145">
+      <c r="G365" s="145">
         <v>44644</v>
       </c>
-      <c r="H364" s="146">
+      <c r="H365" s="146">
         <v>44636</v>
       </c>
-    </row>
-    <row r="365" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A365" s="1"/>
-      <c r="B365" s="116"/>
-      <c r="C365" s="117"/>
-      <c r="D365" s="117"/>
-      <c r="E365" s="179"/>
-      <c r="F365" s="118"/>
-      <c r="G365" s="119"/>
-      <c r="H365" s="120"/>
     </row>
     <row r="366" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A366" s="1"/>
-      <c r="B366" s="1"/>
-      <c r="C366" s="1"/>
-      <c r="D366" s="1"/>
-      <c r="E366" s="180"/>
-      <c r="F366" s="121"/>
-      <c r="G366" s="122"/>
-      <c r="H366" s="122"/>
-    </row>
-    <row r="367" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B366" s="111"/>
+      <c r="C366" s="112"/>
+      <c r="D366" s="143" t="s">
+        <v>468</v>
+      </c>
+      <c r="E366" s="176" t="s">
+        <v>469</v>
+      </c>
+      <c r="F366" s="144" t="s">
+        <v>267</v>
+      </c>
+      <c r="G366" s="145">
+        <v>44644</v>
+      </c>
+      <c r="H366" s="146">
+        <v>44636</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A367" s="1"/>
-      <c r="B367" s="1"/>
-      <c r="C367" s="1"/>
-      <c r="D367" s="1"/>
-      <c r="E367" s="180"/>
-      <c r="F367" s="121"/>
-      <c r="G367" s="122"/>
-      <c r="H367" s="122"/>
+      <c r="B367" s="116"/>
+      <c r="C367" s="117"/>
+      <c r="D367" s="117"/>
+      <c r="E367" s="179"/>
+      <c r="F367" s="118"/>
+      <c r="G367" s="119"/>
+      <c r="H367" s="120"/>
     </row>
     <row r="368" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
@@ -9442,17 +9474,25 @@
       <c r="G381" s="122"/>
       <c r="H381" s="122"/>
     </row>
-    <row r="382" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E382" s="169"/>
-      <c r="F382" s="95"/>
-      <c r="G382" s="110"/>
-      <c r="H382" s="110"/>
-    </row>
-    <row r="383" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E383" s="169"/>
-      <c r="F383" s="95"/>
-      <c r="G383" s="110"/>
-      <c r="H383" s="110"/>
+    <row r="382" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A382" s="1"/>
+      <c r="B382" s="1"/>
+      <c r="C382" s="1"/>
+      <c r="D382" s="1"/>
+      <c r="E382" s="180"/>
+      <c r="F382" s="121"/>
+      <c r="G382" s="122"/>
+      <c r="H382" s="122"/>
+    </row>
+    <row r="383" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A383" s="1"/>
+      <c r="B383" s="1"/>
+      <c r="C383" s="1"/>
+      <c r="D383" s="1"/>
+      <c r="E383" s="180"/>
+      <c r="F383" s="121"/>
+      <c r="G383" s="122"/>
+      <c r="H383" s="122"/>
     </row>
     <row r="384" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="E384" s="169"/>
@@ -9460,21 +9500,32 @@
       <c r="G384" s="110"/>
       <c r="H384" s="110"/>
     </row>
+    <row r="385" spans="5:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E385" s="169"/>
+      <c r="F385" s="95"/>
+      <c r="G385" s="110"/>
+      <c r="H385" s="110"/>
+    </row>
+    <row r="386" spans="5:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E386" s="169"/>
+      <c r="F386" s="95"/>
+      <c r="G386" s="110"/>
+      <c r="H386" s="110"/>
+    </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B286:B287"/>
-    <mergeCell ref="C287:C288"/>
-    <mergeCell ref="C156:C157"/>
-    <mergeCell ref="B282:B283"/>
-    <mergeCell ref="C283:C284"/>
-    <mergeCell ref="C224:C225"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C290:C291"/>
-    <mergeCell ref="C293:C294"/>
+    <mergeCell ref="C313:C314"/>
+    <mergeCell ref="C316:C317"/>
+    <mergeCell ref="C319:C320"/>
+    <mergeCell ref="C353:C354"/>
+    <mergeCell ref="C358:C359"/>
+    <mergeCell ref="C298:C299"/>
+    <mergeCell ref="C301:C302"/>
+    <mergeCell ref="C304:C305"/>
+    <mergeCell ref="C307:C308"/>
+    <mergeCell ref="C310:C311"/>
+    <mergeCell ref="C292:C293"/>
+    <mergeCell ref="C295:C296"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C14:C15"/>
@@ -9487,16 +9538,17 @@
     <mergeCell ref="C101:C102"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="C137:C138"/>
-    <mergeCell ref="C296:C297"/>
-    <mergeCell ref="C299:C300"/>
-    <mergeCell ref="C302:C303"/>
-    <mergeCell ref="C305:C306"/>
-    <mergeCell ref="C308:C309"/>
-    <mergeCell ref="C311:C312"/>
-    <mergeCell ref="C314:C315"/>
-    <mergeCell ref="C317:C318"/>
-    <mergeCell ref="C351:C352"/>
-    <mergeCell ref="C356:C357"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B288:B289"/>
+    <mergeCell ref="C289:C290"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="B284:B285"/>
+    <mergeCell ref="C285:C286"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -9530,20 +9582,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="196" t="s">
+      <c r="B2" s="213" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="197"/>
-      <c r="D2" s="198"/>
-      <c r="E2" s="193" t="s">
+      <c r="C2" s="214"/>
+      <c r="D2" s="215"/>
+      <c r="E2" s="210" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="195"/>
-      <c r="G2" s="193" t="s">
+      <c r="F2" s="212"/>
+      <c r="G2" s="210" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="194"/>
-      <c r="I2" s="195"/>
+      <c r="H2" s="211"/>
+      <c r="I2" s="212"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -9564,10 +9616,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="199" t="s">
+      <c r="H3" s="216" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="200"/>
+      <c r="I3" s="217"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -9609,7 +9661,7 @@
       <c r="F5" s="207" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="210" t="s">
+      <c r="G5" s="198" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -9625,11 +9677,11 @@
       <c r="D6" s="205"/>
       <c r="E6" s="35"/>
       <c r="F6" s="208"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="191" t="s">
+      <c r="G6" s="199"/>
+      <c r="H6" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="192"/>
+      <c r="I6" s="194"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
@@ -9637,7 +9689,7 @@
       <c r="D7" s="206"/>
       <c r="E7" s="36"/>
       <c r="F7" s="209"/>
-      <c r="G7" s="212"/>
+      <c r="G7" s="200"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -9677,13 +9729,13 @@
       <c r="D9" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="215" t="s">
+      <c r="E9" s="195" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="207" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="210" t="s">
+      <c r="G9" s="198" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -9698,22 +9750,22 @@
       <c r="B10" s="61"/>
       <c r="C10" s="202"/>
       <c r="D10" s="205"/>
-      <c r="E10" s="216"/>
+      <c r="E10" s="196"/>
       <c r="F10" s="208"/>
-      <c r="G10" s="211"/>
-      <c r="H10" s="191" t="s">
+      <c r="G10" s="199"/>
+      <c r="H10" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="192"/>
+      <c r="I10" s="194"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
       <c r="C11" s="203"/>
       <c r="D11" s="206"/>
-      <c r="E11" s="217"/>
+      <c r="E11" s="197"/>
       <c r="F11" s="209"/>
-      <c r="G11" s="212"/>
+      <c r="G11" s="200"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -9735,7 +9787,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="210" t="s">
+      <c r="G12" s="198" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -9755,7 +9807,7 @@
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="212"/>
+      <c r="G13" s="200"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -9800,8 +9852,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="213"/>
-      <c r="I16" s="214"/>
+      <c r="H16" s="191"/>
+      <c r="I16" s="192"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -10221,13 +10273,13 @@
       <c r="D40" s="204" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="215" t="s">
+      <c r="E40" s="195" t="s">
         <v>45</v>
       </c>
       <c r="F40" s="207" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="210" t="s">
+      <c r="G40" s="198" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -10241,21 +10293,21 @@
       <c r="B41" s="61"/>
       <c r="C41" s="202"/>
       <c r="D41" s="205"/>
-      <c r="E41" s="216"/>
+      <c r="E41" s="196"/>
       <c r="F41" s="208"/>
-      <c r="G41" s="211"/>
-      <c r="H41" s="191" t="s">
+      <c r="G41" s="199"/>
+      <c r="H41" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="192"/>
+      <c r="I41" s="194"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
       <c r="C42" s="203"/>
       <c r="D42" s="206"/>
-      <c r="E42" s="217"/>
+      <c r="E42" s="197"/>
       <c r="F42" s="209"/>
-      <c r="G42" s="212"/>
+      <c r="G42" s="200"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -10295,13 +10347,13 @@
       <c r="D44" s="204" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="215" t="s">
+      <c r="E44" s="195" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="207" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="210" t="s">
+      <c r="G44" s="198" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -10315,21 +10367,21 @@
       <c r="B45" s="61"/>
       <c r="C45" s="202"/>
       <c r="D45" s="205"/>
-      <c r="E45" s="216"/>
+      <c r="E45" s="196"/>
       <c r="F45" s="208"/>
-      <c r="G45" s="211"/>
-      <c r="H45" s="191" t="s">
+      <c r="G45" s="199"/>
+      <c r="H45" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="192"/>
+      <c r="I45" s="194"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
       <c r="C46" s="203"/>
       <c r="D46" s="206"/>
-      <c r="E46" s="217"/>
+      <c r="E46" s="197"/>
       <c r="F46" s="209"/>
-      <c r="G46" s="212"/>
+      <c r="G46" s="200"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -10354,8 +10406,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="213"/>
-      <c r="I48" s="214"/>
+      <c r="H48" s="191"/>
+      <c r="I48" s="192"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -10418,10 +10470,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="191" t="s">
+      <c r="H52" s="193" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="192"/>
+      <c r="I52" s="194"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -10454,8 +10506,8 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="213"/>
-      <c r="I55" s="214"/>
+      <c r="H55" s="191"/>
+      <c r="I55" s="192"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="64" t="s">
@@ -10868,8 +10920,8 @@
       <c r="E83" s="25"/>
       <c r="F83" s="22"/>
       <c r="G83" s="25"/>
-      <c r="H83" s="213"/>
-      <c r="I83" s="214"/>
+      <c r="H83" s="191"/>
+      <c r="I83" s="192"/>
     </row>
     <row r="84" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="61"/>
@@ -11013,22 +11065,15 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -11039,15 +11084,22 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H55:I55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11080,10 +11132,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="219"/>
-      <c r="D2" s="194" t="s">
+      <c r="D2" s="211" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="195" t="s">
+      <c r="E2" s="212" t="s">
         <v>0</v>
       </c>
     </row>
@@ -11094,8 +11146,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="199"/>
-      <c r="E3" s="200"/>
+      <c r="D3" s="216"/>
+      <c r="E3" s="217"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 13 Februari 2023 18:56 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="970" uniqueCount="660">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -2085,10 +2085,17 @@
     <t xml:space="preserve">Mendapatkan Tahapan saat ini dan Tahapan selanjutnya pada Work Flow Dokumen Bisnis sesuai ID Dokumen Bisnis (varBusinessDocument_RefID) </t>
   </si>
   <si>
-    <t>Mendapatkan Jalur Work Flow berdasarkan ID Jenis Doumen Bisnis (varBusinessDocumentType_RefID) dan ID Entitas Submitter (varSubmitterEntity_RefID</t>
-  </si>
-  <si>
     <t>Func_General_GetBusinessDocumentTypeWorkFlowPath</t>
+  </si>
+  <si>
+    <t>Mendapatkan Jalur Work Flow berdasarkan ID Jenis Dokumen Bisnis (varBusinessDocumentType_RefID) dan ID Entitas Submitter (varSubmitterEntity_RefID</t>
+  </si>
+  <si>
+    <t>Func_General_GetBusinessDocumentWorkFlowPathApprovalHistory</t>
+  </si>
+  <si>
+    <t>Mendapatkan Riwayat Pengesahan Work Flow Dokumen Bisnis berdasarkan ID Branch (varBranch_RefID) dan ID Dokumen Bisnis (varBusinessDocument_RefID).
+Adapun Pick Statement (varPickStatement), Sort Statement (varSortStatement), Filter Statement (varFilterStatement), dan Paging Statement (varPagingStatement) merupakan parameter optional yang dapat digunakan ataupun tidak sesuai dengan kebutuhan</t>
   </si>
 </sst>
 </file>
@@ -3335,6 +3342,15 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3350,20 +3366,77 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -3371,12 +3444,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3385,66 +3452,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3769,13 +3776,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H386"/>
+  <dimension ref="A1:H387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E247" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E243" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E251" sqref="E251"/>
+      <selection pane="bottomRight" activeCell="E249" sqref="E249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3793,19 +3800,19 @@
   <sheetData>
     <row r="1" spans="1:8" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="189" t="s">
+      <c r="B2" s="182" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
-      <c r="E2" s="187" t="s">
+      <c r="C2" s="183"/>
+      <c r="D2" s="183"/>
+      <c r="E2" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="181" t="s">
+      <c r="F2" s="184" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="182"/>
-      <c r="H2" s="183"/>
+      <c r="G2" s="185"/>
+      <c r="H2" s="186"/>
     </row>
     <row r="3" spans="1:8" s="156" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="157" t="s">
@@ -3817,7 +3824,7 @@
       <c r="D3" s="159" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="188"/>
+      <c r="E3" s="190"/>
       <c r="F3" s="160" t="s">
         <v>228</v>
       </c>
@@ -3830,7 +3837,7 @@
     </row>
     <row r="4" spans="1:8" s="155" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="154"/>
-      <c r="B4" s="184" t="s">
+      <c r="B4" s="187" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="152"/>
@@ -3842,8 +3849,8 @@
     </row>
     <row r="5" spans="1:8" s="155" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="154"/>
-      <c r="B5" s="185"/>
-      <c r="C5" s="186" t="s">
+      <c r="B5" s="188"/>
+      <c r="C5" s="181" t="s">
         <v>160</v>
       </c>
       <c r="D5" s="152"/>
@@ -3855,7 +3862,7 @@
     <row r="6" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="111"/>
-      <c r="C6" s="186"/>
+      <c r="C6" s="181"/>
       <c r="D6" s="112"/>
       <c r="E6" s="171"/>
       <c r="F6" s="113"/>
@@ -3875,7 +3882,7 @@
     <row r="8" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="111"/>
-      <c r="C8" s="186" t="s">
+      <c r="C8" s="181" t="s">
         <v>161</v>
       </c>
       <c r="D8" s="152"/>
@@ -3887,7 +3894,7 @@
     <row r="9" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="111"/>
-      <c r="C9" s="186"/>
+      <c r="C9" s="181"/>
       <c r="D9" s="112"/>
       <c r="E9" s="171"/>
       <c r="F9" s="113"/>
@@ -3907,7 +3914,7 @@
     <row r="11" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="111"/>
-      <c r="C11" s="186" t="s">
+      <c r="C11" s="181" t="s">
         <v>162</v>
       </c>
       <c r="D11" s="152"/>
@@ -3919,7 +3926,7 @@
     <row r="12" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="111"/>
-      <c r="C12" s="186"/>
+      <c r="C12" s="181"/>
       <c r="D12" s="112"/>
       <c r="E12" s="171"/>
       <c r="F12" s="113"/>
@@ -3939,7 +3946,7 @@
     <row r="14" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="111"/>
-      <c r="C14" s="186" t="s">
+      <c r="C14" s="181" t="s">
         <v>163</v>
       </c>
       <c r="D14" s="152"/>
@@ -3951,7 +3958,7 @@
     <row r="15" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="111"/>
-      <c r="C15" s="186"/>
+      <c r="C15" s="181"/>
       <c r="D15" s="112"/>
       <c r="E15" s="171"/>
       <c r="F15" s="113"/>
@@ -3971,7 +3978,7 @@
     <row r="17" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="111"/>
-      <c r="C17" s="186" t="s">
+      <c r="C17" s="181" t="s">
         <v>164</v>
       </c>
       <c r="D17" s="152"/>
@@ -3983,7 +3990,7 @@
     <row r="18" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="111"/>
-      <c r="C18" s="186"/>
+      <c r="C18" s="181"/>
       <c r="D18" s="112"/>
       <c r="E18" s="171"/>
       <c r="F18" s="113"/>
@@ -4003,7 +4010,7 @@
     <row r="20" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="111"/>
-      <c r="C20" s="186" t="s">
+      <c r="C20" s="181" t="s">
         <v>4</v>
       </c>
       <c r="D20" s="152"/>
@@ -4015,7 +4022,7 @@
     <row r="21" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="111"/>
-      <c r="C21" s="186"/>
+      <c r="C21" s="181"/>
       <c r="D21" s="112"/>
       <c r="E21" s="171"/>
       <c r="F21" s="113"/>
@@ -4095,7 +4102,7 @@
     <row r="27" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="111"/>
-      <c r="C27" s="186" t="s">
+      <c r="C27" s="181" t="s">
         <v>165</v>
       </c>
       <c r="D27" s="152"/>
@@ -4107,7 +4114,7 @@
     <row r="28" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="111"/>
-      <c r="C28" s="186"/>
+      <c r="C28" s="181"/>
       <c r="D28" s="112"/>
       <c r="E28" s="171"/>
       <c r="F28" s="113"/>
@@ -4127,7 +4134,7 @@
     <row r="30" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="111"/>
-      <c r="C30" s="186" t="s">
+      <c r="C30" s="181" t="s">
         <v>166</v>
       </c>
       <c r="D30" s="152"/>
@@ -4139,7 +4146,7 @@
     <row r="31" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="111"/>
-      <c r="C31" s="186"/>
+      <c r="C31" s="181"/>
       <c r="D31" s="112"/>
       <c r="E31" s="171"/>
       <c r="F31" s="113"/>
@@ -4349,7 +4356,7 @@
     <row r="47" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
       <c r="B47" s="111"/>
-      <c r="C47" s="186" t="s">
+      <c r="C47" s="181" t="s">
         <v>75</v>
       </c>
       <c r="D47" s="152"/>
@@ -4361,7 +4368,7 @@
     <row r="48" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="111"/>
-      <c r="C48" s="186"/>
+      <c r="C48" s="181"/>
       <c r="D48" s="112" t="s">
         <v>566</v>
       </c>
@@ -5031,7 +5038,7 @@
     <row r="98" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="111"/>
-      <c r="C98" s="186" t="s">
+      <c r="C98" s="181" t="s">
         <v>167</v>
       </c>
       <c r="D98" s="152"/>
@@ -5043,7 +5050,7 @@
     <row r="99" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="111"/>
-      <c r="C99" s="186"/>
+      <c r="C99" s="181"/>
       <c r="D99" s="112"/>
       <c r="E99" s="171"/>
       <c r="F99" s="113"/>
@@ -5063,7 +5070,7 @@
     <row r="101" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="111"/>
-      <c r="C101" s="186" t="s">
+      <c r="C101" s="181" t="s">
         <v>168</v>
       </c>
       <c r="D101" s="152"/>
@@ -5075,7 +5082,7 @@
     <row r="102" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="111"/>
-      <c r="C102" s="186"/>
+      <c r="C102" s="181"/>
       <c r="D102" s="112"/>
       <c r="E102" s="171"/>
       <c r="F102" s="113"/>
@@ -5095,7 +5102,7 @@
     <row r="104" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="111"/>
-      <c r="C104" s="186" t="s">
+      <c r="C104" s="181" t="s">
         <v>169</v>
       </c>
       <c r="D104" s="152"/>
@@ -5107,7 +5114,7 @@
     <row r="105" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A105" s="1"/>
       <c r="B105" s="111"/>
-      <c r="C105" s="186"/>
+      <c r="C105" s="181"/>
       <c r="D105" s="148" t="s">
         <v>535</v>
       </c>
@@ -5587,7 +5594,7 @@
     <row r="137" spans="1:8" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1"/>
       <c r="B137" s="111"/>
-      <c r="C137" s="186" t="s">
+      <c r="C137" s="181" t="s">
         <v>57</v>
       </c>
       <c r="D137" s="152"/>
@@ -5599,7 +5606,7 @@
     <row r="138" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="111"/>
-      <c r="C138" s="186"/>
+      <c r="C138" s="181"/>
       <c r="D138" s="148" t="s">
         <v>423</v>
       </c>
@@ -5899,7 +5906,7 @@
     <row r="156" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="1"/>
       <c r="B156" s="111"/>
-      <c r="C156" s="186" t="s">
+      <c r="C156" s="181" t="s">
         <v>170</v>
       </c>
       <c r="D156" s="152"/>
@@ -5911,7 +5918,7 @@
     <row r="157" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A157" s="1"/>
       <c r="B157" s="111"/>
-      <c r="C157" s="186"/>
+      <c r="C157" s="181"/>
       <c r="D157" s="148" t="s">
         <v>651</v>
       </c>
@@ -7051,7 +7058,7 @@
     <row r="224" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A224" s="1"/>
       <c r="B224" s="111"/>
-      <c r="C224" s="186" t="s">
+      <c r="C224" s="181" t="s">
         <v>146</v>
       </c>
       <c r="D224" s="152"/>
@@ -7063,7 +7070,7 @@
     <row r="225" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A225" s="1"/>
       <c r="B225" s="111"/>
-      <c r="C225" s="186"/>
+      <c r="C225" s="181"/>
       <c r="D225" s="148" t="s">
         <v>274</v>
       </c>
@@ -7432,24 +7439,24 @@
         <v>44970</v>
       </c>
     </row>
-    <row r="249" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A249" s="1"/>
       <c r="B249" s="111"/>
       <c r="C249" s="112"/>
       <c r="D249" s="112" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E249" s="175" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="F249" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G249" s="114">
-        <v>44952</v>
+        <v>44998</v>
       </c>
       <c r="H249" s="115">
-        <v>44952</v>
+        <v>44998</v>
       </c>
     </row>
     <row r="250" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7457,19 +7464,19 @@
       <c r="B250" s="111"/>
       <c r="C250" s="112"/>
       <c r="D250" s="112" t="s">
-        <v>325</v>
+        <v>656</v>
       </c>
       <c r="E250" s="175" t="s">
-        <v>326</v>
+        <v>657</v>
       </c>
       <c r="F250" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G250" s="114">
-        <v>44902</v>
+        <v>44952</v>
       </c>
       <c r="H250" s="115">
-        <v>44902</v>
+        <v>44952</v>
       </c>
     </row>
     <row r="251" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7477,19 +7484,19 @@
       <c r="B251" s="111"/>
       <c r="C251" s="112"/>
       <c r="D251" s="112" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="E251" s="175" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="F251" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G251" s="114">
-        <v>44897</v>
+        <v>44902</v>
       </c>
       <c r="H251" s="115">
-        <v>44897</v>
+        <v>44902</v>
       </c>
     </row>
     <row r="252" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7497,19 +7504,19 @@
       <c r="B252" s="111"/>
       <c r="C252" s="112"/>
       <c r="D252" s="112" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="E252" s="175" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="F252" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G252" s="114">
-        <v>44951</v>
+        <v>44897</v>
       </c>
       <c r="H252" s="115">
-        <v>44951</v>
+        <v>44897</v>
       </c>
     </row>
     <row r="253" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7517,10 +7524,10 @@
       <c r="B253" s="111"/>
       <c r="C253" s="112"/>
       <c r="D253" s="112" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="E253" s="175" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="F253" s="113" t="s">
         <v>232</v>
@@ -7532,64 +7539,64 @@
         <v>44951</v>
       </c>
     </row>
-    <row r="254" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A254" s="1"/>
       <c r="B254" s="111"/>
       <c r="C254" s="112"/>
       <c r="D254" s="112" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="E254" s="175" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="F254" s="113" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G254" s="114">
-        <v>44900</v>
+        <v>44951</v>
       </c>
       <c r="H254" s="115">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="255" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A255" s="1"/>
       <c r="B255" s="111"/>
       <c r="C255" s="112"/>
       <c r="D255" s="112" t="s">
-        <v>327</v>
-      </c>
-      <c r="E255" s="171" t="s">
-        <v>328</v>
+        <v>320</v>
+      </c>
+      <c r="E255" s="175" t="s">
+        <v>324</v>
       </c>
       <c r="F255" s="113" t="s">
         <v>281</v>
       </c>
       <c r="G255" s="114">
-        <v>44896</v>
+        <v>44900</v>
       </c>
       <c r="H255" s="115">
-        <v>44896</v>
-      </c>
-    </row>
-    <row r="256" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A256" s="1"/>
       <c r="B256" s="111"/>
       <c r="C256" s="112"/>
       <c r="D256" s="112" t="s">
-        <v>321</v>
-      </c>
-      <c r="E256" s="175" t="s">
-        <v>338</v>
+        <v>327</v>
+      </c>
+      <c r="E256" s="171" t="s">
+        <v>328</v>
       </c>
       <c r="F256" s="113" t="s">
         <v>281</v>
       </c>
       <c r="G256" s="114">
-        <v>44945</v>
+        <v>44896</v>
       </c>
       <c r="H256" s="115">
-        <v>44949</v>
+        <v>44896</v>
       </c>
     </row>
     <row r="257" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7597,60 +7604,60 @@
       <c r="B257" s="111"/>
       <c r="C257" s="112"/>
       <c r="D257" s="112" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="E257" s="175" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="F257" s="113" t="s">
         <v>281</v>
       </c>
       <c r="G257" s="114">
-        <v>44910</v>
+        <v>44945</v>
       </c>
       <c r="H257" s="115">
-        <v>44910</v>
-      </c>
-    </row>
-    <row r="258" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A258" s="1"/>
       <c r="B258" s="111"/>
       <c r="C258" s="112"/>
-      <c r="D258" s="163"/>
-      <c r="E258" s="172"/>
-      <c r="F258" s="163"/>
-      <c r="G258" s="163"/>
-      <c r="H258" s="164"/>
-    </row>
-    <row r="259" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="D258" s="112" t="s">
+        <v>333</v>
+      </c>
+      <c r="E258" s="175" t="s">
+        <v>334</v>
+      </c>
+      <c r="F258" s="113" t="s">
+        <v>281</v>
+      </c>
+      <c r="G258" s="114">
+        <v>44910</v>
+      </c>
+      <c r="H258" s="115">
+        <v>44910</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="1"/>
       <c r="B259" s="111"/>
       <c r="C259" s="112"/>
-      <c r="D259" s="148" t="s">
-        <v>626</v>
-      </c>
-      <c r="E259" s="173" t="s">
-        <v>627</v>
-      </c>
-      <c r="F259" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G259" s="150">
-        <v>44965</v>
-      </c>
-      <c r="H259" s="151">
-        <v>44965</v>
-      </c>
+      <c r="D259" s="163"/>
+      <c r="E259" s="172"/>
+      <c r="F259" s="163"/>
+      <c r="G259" s="163"/>
+      <c r="H259" s="164"/>
     </row>
     <row r="260" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A260" s="1"/>
       <c r="B260" s="111"/>
       <c r="C260" s="112"/>
       <c r="D260" s="148" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="E260" s="173" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="F260" s="149" t="s">
         <v>232</v>
@@ -7667,10 +7674,10 @@
       <c r="B261" s="111"/>
       <c r="C261" s="112"/>
       <c r="D261" s="148" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="E261" s="173" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="F261" s="149" t="s">
         <v>232</v>
@@ -7687,70 +7694,70 @@
       <c r="B262" s="111"/>
       <c r="C262" s="112"/>
       <c r="D262" s="148" t="s">
-        <v>574</v>
+        <v>630</v>
       </c>
       <c r="E262" s="173" t="s">
-        <v>575</v>
+        <v>631</v>
       </c>
       <c r="F262" s="149" t="s">
         <v>232</v>
       </c>
       <c r="G262" s="150">
-        <v>44964</v>
+        <v>44965</v>
       </c>
       <c r="H262" s="151">
-        <v>44964</v>
+        <v>44965</v>
       </c>
     </row>
     <row r="263" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A263" s="1"/>
       <c r="B263" s="111"/>
       <c r="C263" s="112"/>
-      <c r="D263" s="143" t="s">
-        <v>591</v>
-      </c>
-      <c r="E263" s="174" t="s">
-        <v>592</v>
-      </c>
-      <c r="F263" s="144" t="s">
-        <v>281</v>
-      </c>
-      <c r="G263" s="145">
+      <c r="D263" s="148" t="s">
+        <v>574</v>
+      </c>
+      <c r="E263" s="173" t="s">
+        <v>575</v>
+      </c>
+      <c r="F263" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G263" s="150">
         <v>44964</v>
       </c>
-      <c r="H263" s="146">
-        <v>44901</v>
+      <c r="H263" s="151">
+        <v>44964</v>
       </c>
     </row>
     <row r="264" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A264" s="1"/>
       <c r="B264" s="111"/>
       <c r="C264" s="112"/>
-      <c r="D264" s="148" t="s">
-        <v>628</v>
-      </c>
-      <c r="E264" s="173" t="s">
-        <v>629</v>
-      </c>
-      <c r="F264" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G264" s="150">
-        <v>44965</v>
-      </c>
-      <c r="H264" s="151">
-        <v>44965</v>
-      </c>
-    </row>
-    <row r="265" spans="1:8" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="D264" s="143" t="s">
+        <v>591</v>
+      </c>
+      <c r="E264" s="174" t="s">
+        <v>592</v>
+      </c>
+      <c r="F264" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="G264" s="145">
+        <v>44964</v>
+      </c>
+      <c r="H264" s="146">
+        <v>44901</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A265" s="1"/>
       <c r="B265" s="111"/>
       <c r="C265" s="112"/>
       <c r="D265" s="148" t="s">
-        <v>620</v>
+        <v>628</v>
       </c>
       <c r="E265" s="173" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="F265" s="149" t="s">
         <v>232</v>
@@ -7766,91 +7773,101 @@
       <c r="A266" s="1"/>
       <c r="B266" s="111"/>
       <c r="C266" s="112"/>
-      <c r="D266" s="112" t="s">
-        <v>621</v>
-      </c>
-      <c r="E266" s="175" t="s">
-        <v>623</v>
-      </c>
-      <c r="F266" s="113" t="s">
+      <c r="D266" s="148" t="s">
+        <v>620</v>
+      </c>
+      <c r="E266" s="173" t="s">
+        <v>622</v>
+      </c>
+      <c r="F266" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G266" s="114">
+      <c r="G266" s="150">
         <v>44965</v>
       </c>
-      <c r="H266" s="115">
+      <c r="H266" s="151">
         <v>44965</v>
       </c>
     </row>
-    <row r="267" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A267" s="1"/>
       <c r="B267" s="111"/>
       <c r="C267" s="112"/>
-      <c r="D267" s="163"/>
-      <c r="E267" s="172"/>
-      <c r="F267" s="163"/>
-      <c r="G267" s="163"/>
-      <c r="H267" s="164"/>
-    </row>
-    <row r="268" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D267" s="112" t="s">
+        <v>621</v>
+      </c>
+      <c r="E267" s="175" t="s">
+        <v>623</v>
+      </c>
+      <c r="F267" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G267" s="114">
+        <v>44965</v>
+      </c>
+      <c r="H267" s="115">
+        <v>44965</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A268" s="1"/>
       <c r="B268" s="111"/>
       <c r="C268" s="112"/>
-      <c r="D268" s="112" t="s">
-        <v>339</v>
-      </c>
-      <c r="E268" s="175" t="s">
-        <v>340</v>
-      </c>
-      <c r="F268" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G268" s="114">
-        <v>44951</v>
-      </c>
-      <c r="H268" s="115">
-        <v>44951</v>
-      </c>
-    </row>
-    <row r="269" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D268" s="163"/>
+      <c r="E268" s="172"/>
+      <c r="F268" s="163"/>
+      <c r="G268" s="163"/>
+      <c r="H268" s="164"/>
+    </row>
+    <row r="269" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A269" s="1"/>
       <c r="B269" s="111"/>
       <c r="C269" s="112"/>
-      <c r="D269" s="163"/>
-      <c r="E269" s="172"/>
-      <c r="F269" s="163"/>
-      <c r="G269" s="163"/>
-      <c r="H269" s="164"/>
-    </row>
-    <row r="270" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D269" s="112" t="s">
+        <v>339</v>
+      </c>
+      <c r="E269" s="175" t="s">
+        <v>340</v>
+      </c>
+      <c r="F269" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G269" s="114">
+        <v>44951</v>
+      </c>
+      <c r="H269" s="115">
+        <v>44951</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A270" s="1"/>
       <c r="B270" s="111"/>
       <c r="C270" s="112"/>
-      <c r="D270" s="112" t="s">
-        <v>341</v>
-      </c>
-      <c r="E270" s="175" t="s">
-        <v>342</v>
-      </c>
-      <c r="F270" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G270" s="114">
-        <v>44952</v>
-      </c>
-      <c r="H270" s="115">
-        <v>44952</v>
-      </c>
-    </row>
-    <row r="271" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D270" s="163"/>
+      <c r="E270" s="172"/>
+      <c r="F270" s="163"/>
+      <c r="G270" s="163"/>
+      <c r="H270" s="164"/>
+    </row>
+    <row r="271" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A271" s="1"/>
       <c r="B271" s="111"/>
       <c r="C271" s="112"/>
-      <c r="D271" s="112"/>
-      <c r="E271" s="171"/>
-      <c r="F271" s="113"/>
-      <c r="G271" s="114"/>
-      <c r="H271" s="115"/>
+      <c r="D271" s="112" t="s">
+        <v>341</v>
+      </c>
+      <c r="E271" s="175" t="s">
+        <v>342</v>
+      </c>
+      <c r="F271" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G271" s="114">
+        <v>44952</v>
+      </c>
+      <c r="H271" s="115">
+        <v>44952</v>
+      </c>
     </row>
     <row r="272" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A272" s="1"/>
@@ -7872,64 +7889,54 @@
       <c r="G273" s="114"/>
       <c r="H273" s="115"/>
     </row>
-    <row r="274" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A274" s="1"/>
       <c r="B274" s="111"/>
       <c r="C274" s="112"/>
-      <c r="D274" s="112" t="s">
-        <v>393</v>
-      </c>
-      <c r="E274" s="175" t="s">
-        <v>394</v>
-      </c>
-      <c r="F274" s="113" t="s">
-        <v>267</v>
-      </c>
-      <c r="G274" s="114">
-        <v>44957</v>
-      </c>
-      <c r="H274" s="115">
-        <v>42982</v>
-      </c>
+      <c r="D274" s="112"/>
+      <c r="E274" s="171"/>
+      <c r="F274" s="113"/>
+      <c r="G274" s="114"/>
+      <c r="H274" s="115"/>
     </row>
     <row r="275" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A275" s="1"/>
       <c r="B275" s="111"/>
       <c r="C275" s="112"/>
       <c r="D275" s="112" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E275" s="175" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F275" s="113" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G275" s="114">
-        <v>44281</v>
+        <v>44957</v>
       </c>
       <c r="H275" s="115">
-        <v>44557</v>
-      </c>
-    </row>
-    <row r="276" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>42982</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A276" s="1"/>
       <c r="B276" s="111"/>
       <c r="C276" s="112"/>
       <c r="D276" s="112" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E276" s="175" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="F276" s="113" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G276" s="114">
-        <v>43257</v>
+        <v>44281</v>
       </c>
       <c r="H276" s="115">
-        <v>43257</v>
+        <v>44557</v>
       </c>
     </row>
     <row r="277" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -7937,67 +7944,77 @@
       <c r="B277" s="111"/>
       <c r="C277" s="112"/>
       <c r="D277" s="112" t="s">
-        <v>285</v>
+        <v>396</v>
       </c>
       <c r="E277" s="175" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F277" s="113" t="s">
         <v>232</v>
       </c>
       <c r="G277" s="114">
-        <v>44949</v>
+        <v>43257</v>
       </c>
       <c r="H277" s="115">
-        <v>44949</v>
-      </c>
-    </row>
-    <row r="278" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>43257</v>
+      </c>
+    </row>
+    <row r="278" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A278" s="1"/>
       <c r="B278" s="111"/>
       <c r="C278" s="112"/>
-      <c r="D278" s="112"/>
-      <c r="E278" s="175"/>
-      <c r="F278" s="113"/>
-      <c r="G278" s="114"/>
-      <c r="H278" s="115"/>
-    </row>
-    <row r="279" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D278" s="112" t="s">
+        <v>285</v>
+      </c>
+      <c r="E278" s="175" t="s">
+        <v>398</v>
+      </c>
+      <c r="F278" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G278" s="114">
+        <v>44949</v>
+      </c>
+      <c r="H278" s="115">
+        <v>44949</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A279" s="1"/>
       <c r="B279" s="111"/>
       <c r="C279" s="112"/>
-      <c r="D279" s="112" t="s">
-        <v>391</v>
-      </c>
-      <c r="E279" s="175" t="s">
-        <v>399</v>
-      </c>
-      <c r="F279" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G279" s="114">
-        <v>44957</v>
-      </c>
-      <c r="H279" s="115">
-        <v>44957</v>
-      </c>
-    </row>
-    <row r="280" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D279" s="112"/>
+      <c r="E279" s="175"/>
+      <c r="F279" s="113"/>
+      <c r="G279" s="114"/>
+      <c r="H279" s="115"/>
+    </row>
+    <row r="280" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A280" s="1"/>
       <c r="B280" s="111"/>
       <c r="C280" s="112"/>
-      <c r="D280" s="112"/>
-      <c r="E280" s="175"/>
-      <c r="F280" s="113"/>
-      <c r="G280" s="114"/>
-      <c r="H280" s="115"/>
+      <c r="D280" s="112" t="s">
+        <v>391</v>
+      </c>
+      <c r="E280" s="175" t="s">
+        <v>399</v>
+      </c>
+      <c r="F280" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G280" s="114">
+        <v>44957</v>
+      </c>
+      <c r="H280" s="115">
+        <v>44957</v>
+      </c>
     </row>
     <row r="281" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A281" s="1"/>
       <c r="B281" s="111"/>
       <c r="C281" s="112"/>
       <c r="D281" s="112"/>
-      <c r="E281" s="171"/>
+      <c r="E281" s="175"/>
       <c r="F281" s="113"/>
       <c r="G281" s="114"/>
       <c r="H281" s="115"/>
@@ -8006,114 +8023,114 @@
       <c r="A282" s="1"/>
       <c r="B282" s="111"/>
       <c r="C282" s="112"/>
-      <c r="D282" s="112" t="s">
-        <v>329</v>
-      </c>
-      <c r="E282" s="171" t="s">
-        <v>330</v>
-      </c>
-      <c r="F282" s="113" t="s">
-        <v>232</v>
-      </c>
-      <c r="G282" s="114">
-        <v>44893</v>
-      </c>
-      <c r="H282" s="115">
-        <v>44893</v>
-      </c>
+      <c r="D282" s="112"/>
+      <c r="E282" s="171"/>
+      <c r="F282" s="113"/>
+      <c r="G282" s="114"/>
+      <c r="H282" s="115"/>
     </row>
     <row r="283" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A283" s="1"/>
       <c r="B283" s="111"/>
       <c r="C283" s="112"/>
-      <c r="D283" s="112"/>
-      <c r="E283" s="171"/>
-      <c r="F283" s="113"/>
-      <c r="G283" s="114"/>
-      <c r="H283" s="115"/>
-    </row>
-    <row r="284" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A284" s="154"/>
-      <c r="B284" s="185" t="s">
+      <c r="D283" s="112" t="s">
+        <v>329</v>
+      </c>
+      <c r="E283" s="171" t="s">
+        <v>330</v>
+      </c>
+      <c r="F283" s="113" t="s">
+        <v>232</v>
+      </c>
+      <c r="G283" s="114">
+        <v>44893</v>
+      </c>
+      <c r="H283" s="115">
+        <v>44893</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A284" s="1"/>
+      <c r="B284" s="111"/>
+      <c r="C284" s="112"/>
+      <c r="D284" s="112"/>
+      <c r="E284" s="171"/>
+      <c r="F284" s="113"/>
+      <c r="G284" s="114"/>
+      <c r="H284" s="115"/>
+    </row>
+    <row r="285" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A285" s="154"/>
+      <c r="B285" s="188" t="s">
         <v>143</v>
       </c>
-      <c r="C284" s="152"/>
-      <c r="D284" s="152"/>
-      <c r="E284" s="170"/>
-      <c r="F284" s="152"/>
-      <c r="G284" s="152"/>
-      <c r="H284" s="153"/>
-    </row>
-    <row r="285" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A285" s="154"/>
-      <c r="B285" s="185"/>
-      <c r="C285" s="186" t="s">
-        <v>160</v>
-      </c>
+      <c r="C285" s="152"/>
       <c r="D285" s="152"/>
       <c r="E285" s="170"/>
       <c r="F285" s="152"/>
       <c r="G285" s="152"/>
       <c r="H285" s="153"/>
     </row>
-    <row r="286" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A286" s="1"/>
-      <c r="B286" s="111"/>
-      <c r="C286" s="186"/>
-      <c r="D286" s="112"/>
-      <c r="E286" s="171"/>
-      <c r="F286" s="113"/>
-      <c r="G286" s="114"/>
-      <c r="H286" s="115"/>
+    <row r="286" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="154"/>
+      <c r="B286" s="188"/>
+      <c r="C286" s="181" t="s">
+        <v>160</v>
+      </c>
+      <c r="D286" s="152"/>
+      <c r="E286" s="170"/>
+      <c r="F286" s="152"/>
+      <c r="G286" s="152"/>
+      <c r="H286" s="153"/>
     </row>
     <row r="287" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A287" s="1"/>
       <c r="B287" s="111"/>
-      <c r="C287" s="112"/>
+      <c r="C287" s="181"/>
       <c r="D287" s="112"/>
       <c r="E287" s="171"/>
       <c r="F287" s="113"/>
       <c r="G287" s="114"/>
       <c r="H287" s="115"/>
     </row>
-    <row r="288" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A288" s="154"/>
-      <c r="B288" s="185" t="s">
+    <row r="288" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A288" s="1"/>
+      <c r="B288" s="111"/>
+      <c r="C288" s="112"/>
+      <c r="D288" s="112"/>
+      <c r="E288" s="171"/>
+      <c r="F288" s="113"/>
+      <c r="G288" s="114"/>
+      <c r="H288" s="115"/>
+    </row>
+    <row r="289" spans="1:8" s="155" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A289" s="154"/>
+      <c r="B289" s="188" t="s">
         <v>142</v>
       </c>
-      <c r="C288" s="152"/>
-      <c r="D288" s="152"/>
-      <c r="E288" s="170"/>
-      <c r="F288" s="152"/>
-      <c r="G288" s="152"/>
-      <c r="H288" s="153"/>
-    </row>
-    <row r="289" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A289" s="154"/>
-      <c r="B289" s="185"/>
-      <c r="C289" s="186" t="s">
-        <v>148</v>
-      </c>
+      <c r="C289" s="152"/>
       <c r="D289" s="152"/>
       <c r="E289" s="170"/>
       <c r="F289" s="152"/>
       <c r="G289" s="152"/>
       <c r="H289" s="153"/>
     </row>
-    <row r="290" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A290" s="1"/>
-      <c r="B290" s="111"/>
-      <c r="C290" s="186"/>
-      <c r="D290" s="112"/>
-      <c r="E290" s="171"/>
-      <c r="F290" s="113"/>
-      <c r="G290" s="114"/>
-      <c r="H290" s="115"/>
+    <row r="290" spans="1:8" s="155" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="154"/>
+      <c r="B290" s="188"/>
+      <c r="C290" s="181" t="s">
+        <v>148</v>
+      </c>
+      <c r="D290" s="152"/>
+      <c r="E290" s="170"/>
+      <c r="F290" s="152"/>
+      <c r="G290" s="152"/>
+      <c r="H290" s="153"/>
     </row>
     <row r="291" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A291" s="1"/>
       <c r="B291" s="111"/>
-      <c r="C291" s="112"/>
+      <c r="C291" s="181"/>
       <c r="D291" s="112"/>
       <c r="E291" s="171"/>
       <c r="F291" s="113"/>
@@ -8123,29 +8140,29 @@
     <row r="292" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A292" s="1"/>
       <c r="B292" s="111"/>
-      <c r="C292" s="186" t="s">
-        <v>149</v>
-      </c>
-      <c r="D292" s="152"/>
-      <c r="E292" s="170"/>
-      <c r="F292" s="152"/>
-      <c r="G292" s="152"/>
-      <c r="H292" s="153"/>
+      <c r="C292" s="112"/>
+      <c r="D292" s="112"/>
+      <c r="E292" s="171"/>
+      <c r="F292" s="113"/>
+      <c r="G292" s="114"/>
+      <c r="H292" s="115"/>
     </row>
     <row r="293" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A293" s="1"/>
       <c r="B293" s="111"/>
-      <c r="C293" s="186"/>
-      <c r="D293" s="112"/>
-      <c r="E293" s="171"/>
-      <c r="F293" s="113"/>
-      <c r="G293" s="114"/>
-      <c r="H293" s="115"/>
+      <c r="C293" s="181" t="s">
+        <v>149</v>
+      </c>
+      <c r="D293" s="152"/>
+      <c r="E293" s="170"/>
+      <c r="F293" s="152"/>
+      <c r="G293" s="152"/>
+      <c r="H293" s="153"/>
     </row>
     <row r="294" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A294" s="1"/>
       <c r="B294" s="111"/>
-      <c r="C294" s="112"/>
+      <c r="C294" s="181"/>
       <c r="D294" s="112"/>
       <c r="E294" s="171"/>
       <c r="F294" s="113"/>
@@ -8155,29 +8172,29 @@
     <row r="295" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A295" s="1"/>
       <c r="B295" s="111"/>
-      <c r="C295" s="186" t="s">
-        <v>150</v>
-      </c>
-      <c r="D295" s="152"/>
-      <c r="E295" s="170"/>
-      <c r="F295" s="152"/>
-      <c r="G295" s="152"/>
-      <c r="H295" s="153"/>
+      <c r="C295" s="112"/>
+      <c r="D295" s="112"/>
+      <c r="E295" s="171"/>
+      <c r="F295" s="113"/>
+      <c r="G295" s="114"/>
+      <c r="H295" s="115"/>
     </row>
     <row r="296" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A296" s="1"/>
       <c r="B296" s="111"/>
-      <c r="C296" s="186"/>
-      <c r="D296" s="112"/>
-      <c r="E296" s="171"/>
-      <c r="F296" s="113"/>
-      <c r="G296" s="114"/>
-      <c r="H296" s="115"/>
+      <c r="C296" s="181" t="s">
+        <v>150</v>
+      </c>
+      <c r="D296" s="152"/>
+      <c r="E296" s="170"/>
+      <c r="F296" s="152"/>
+      <c r="G296" s="152"/>
+      <c r="H296" s="153"/>
     </row>
     <row r="297" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A297" s="1"/>
       <c r="B297" s="111"/>
-      <c r="C297" s="112"/>
+      <c r="C297" s="181"/>
       <c r="D297" s="112"/>
       <c r="E297" s="171"/>
       <c r="F297" s="113"/>
@@ -8187,29 +8204,29 @@
     <row r="298" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="B298" s="111"/>
-      <c r="C298" s="186" t="s">
-        <v>151</v>
-      </c>
-      <c r="D298" s="152"/>
-      <c r="E298" s="170"/>
-      <c r="F298" s="152"/>
-      <c r="G298" s="152"/>
-      <c r="H298" s="153"/>
+      <c r="C298" s="112"/>
+      <c r="D298" s="112"/>
+      <c r="E298" s="171"/>
+      <c r="F298" s="113"/>
+      <c r="G298" s="114"/>
+      <c r="H298" s="115"/>
     </row>
     <row r="299" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="B299" s="111"/>
-      <c r="C299" s="186"/>
-      <c r="D299" s="112"/>
-      <c r="E299" s="171"/>
-      <c r="F299" s="113"/>
-      <c r="G299" s="114"/>
-      <c r="H299" s="115"/>
+      <c r="C299" s="181" t="s">
+        <v>151</v>
+      </c>
+      <c r="D299" s="152"/>
+      <c r="E299" s="170"/>
+      <c r="F299" s="152"/>
+      <c r="G299" s="152"/>
+      <c r="H299" s="153"/>
     </row>
     <row r="300" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A300" s="1"/>
       <c r="B300" s="111"/>
-      <c r="C300" s="112"/>
+      <c r="C300" s="181"/>
       <c r="D300" s="112"/>
       <c r="E300" s="171"/>
       <c r="F300" s="113"/>
@@ -8219,29 +8236,29 @@
     <row r="301" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A301" s="1"/>
       <c r="B301" s="111"/>
-      <c r="C301" s="186" t="s">
-        <v>152</v>
-      </c>
-      <c r="D301" s="152"/>
-      <c r="E301" s="170"/>
-      <c r="F301" s="152"/>
-      <c r="G301" s="152"/>
-      <c r="H301" s="153"/>
+      <c r="C301" s="112"/>
+      <c r="D301" s="112"/>
+      <c r="E301" s="171"/>
+      <c r="F301" s="113"/>
+      <c r="G301" s="114"/>
+      <c r="H301" s="115"/>
     </row>
     <row r="302" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A302" s="1"/>
       <c r="B302" s="111"/>
-      <c r="C302" s="186"/>
-      <c r="D302" s="112"/>
-      <c r="E302" s="171"/>
-      <c r="F302" s="113"/>
-      <c r="G302" s="114"/>
-      <c r="H302" s="115"/>
+      <c r="C302" s="181" t="s">
+        <v>152</v>
+      </c>
+      <c r="D302" s="152"/>
+      <c r="E302" s="170"/>
+      <c r="F302" s="152"/>
+      <c r="G302" s="152"/>
+      <c r="H302" s="153"/>
     </row>
     <row r="303" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A303" s="1"/>
       <c r="B303" s="111"/>
-      <c r="C303" s="112"/>
+      <c r="C303" s="181"/>
       <c r="D303" s="112"/>
       <c r="E303" s="171"/>
       <c r="F303" s="113"/>
@@ -8251,29 +8268,29 @@
     <row r="304" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A304" s="1"/>
       <c r="B304" s="111"/>
-      <c r="C304" s="186" t="s">
-        <v>153</v>
-      </c>
-      <c r="D304" s="152"/>
-      <c r="E304" s="170"/>
-      <c r="F304" s="152"/>
-      <c r="G304" s="152"/>
-      <c r="H304" s="153"/>
+      <c r="C304" s="112"/>
+      <c r="D304" s="112"/>
+      <c r="E304" s="171"/>
+      <c r="F304" s="113"/>
+      <c r="G304" s="114"/>
+      <c r="H304" s="115"/>
     </row>
     <row r="305" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A305" s="1"/>
       <c r="B305" s="111"/>
-      <c r="C305" s="186"/>
-      <c r="D305" s="112"/>
-      <c r="E305" s="171"/>
-      <c r="F305" s="113"/>
-      <c r="G305" s="114"/>
-      <c r="H305" s="115"/>
+      <c r="C305" s="181" t="s">
+        <v>153</v>
+      </c>
+      <c r="D305" s="152"/>
+      <c r="E305" s="170"/>
+      <c r="F305" s="152"/>
+      <c r="G305" s="152"/>
+      <c r="H305" s="153"/>
     </row>
     <row r="306" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A306" s="1"/>
       <c r="B306" s="111"/>
-      <c r="C306" s="112"/>
+      <c r="C306" s="181"/>
       <c r="D306" s="112"/>
       <c r="E306" s="171"/>
       <c r="F306" s="113"/>
@@ -8283,29 +8300,29 @@
     <row r="307" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A307" s="1"/>
       <c r="B307" s="111"/>
-      <c r="C307" s="186" t="s">
-        <v>154</v>
-      </c>
-      <c r="D307" s="152"/>
-      <c r="E307" s="170"/>
-      <c r="F307" s="152"/>
-      <c r="G307" s="152"/>
-      <c r="H307" s="153"/>
+      <c r="C307" s="112"/>
+      <c r="D307" s="112"/>
+      <c r="E307" s="171"/>
+      <c r="F307" s="113"/>
+      <c r="G307" s="114"/>
+      <c r="H307" s="115"/>
     </row>
     <row r="308" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A308" s="1"/>
       <c r="B308" s="111"/>
-      <c r="C308" s="186"/>
-      <c r="D308" s="112"/>
-      <c r="E308" s="171"/>
-      <c r="F308" s="113"/>
-      <c r="G308" s="114"/>
-      <c r="H308" s="115"/>
+      <c r="C308" s="181" t="s">
+        <v>154</v>
+      </c>
+      <c r="D308" s="152"/>
+      <c r="E308" s="170"/>
+      <c r="F308" s="152"/>
+      <c r="G308" s="152"/>
+      <c r="H308" s="153"/>
     </row>
     <row r="309" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A309" s="1"/>
       <c r="B309" s="111"/>
-      <c r="C309" s="112"/>
+      <c r="C309" s="181"/>
       <c r="D309" s="112"/>
       <c r="E309" s="171"/>
       <c r="F309" s="113"/>
@@ -8315,29 +8332,29 @@
     <row r="310" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A310" s="1"/>
       <c r="B310" s="111"/>
-      <c r="C310" s="186" t="s">
-        <v>155</v>
-      </c>
-      <c r="D310" s="152"/>
-      <c r="E310" s="170"/>
-      <c r="F310" s="152"/>
-      <c r="G310" s="152"/>
-      <c r="H310" s="153"/>
+      <c r="C310" s="112"/>
+      <c r="D310" s="112"/>
+      <c r="E310" s="171"/>
+      <c r="F310" s="113"/>
+      <c r="G310" s="114"/>
+      <c r="H310" s="115"/>
     </row>
     <row r="311" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A311" s="1"/>
       <c r="B311" s="111"/>
-      <c r="C311" s="186"/>
-      <c r="D311" s="112"/>
-      <c r="E311" s="171"/>
-      <c r="F311" s="113"/>
-      <c r="G311" s="114"/>
-      <c r="H311" s="115"/>
+      <c r="C311" s="181" t="s">
+        <v>155</v>
+      </c>
+      <c r="D311" s="152"/>
+      <c r="E311" s="170"/>
+      <c r="F311" s="152"/>
+      <c r="G311" s="152"/>
+      <c r="H311" s="153"/>
     </row>
     <row r="312" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A312" s="1"/>
       <c r="B312" s="111"/>
-      <c r="C312" s="112"/>
+      <c r="C312" s="181"/>
       <c r="D312" s="112"/>
       <c r="E312" s="171"/>
       <c r="F312" s="113"/>
@@ -8347,29 +8364,29 @@
     <row r="313" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A313" s="1"/>
       <c r="B313" s="111"/>
-      <c r="C313" s="186" t="s">
-        <v>156</v>
-      </c>
-      <c r="D313" s="152"/>
-      <c r="E313" s="170"/>
-      <c r="F313" s="152"/>
-      <c r="G313" s="152"/>
-      <c r="H313" s="153"/>
+      <c r="C313" s="112"/>
+      <c r="D313" s="112"/>
+      <c r="E313" s="171"/>
+      <c r="F313" s="113"/>
+      <c r="G313" s="114"/>
+      <c r="H313" s="115"/>
     </row>
     <row r="314" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A314" s="1"/>
       <c r="B314" s="111"/>
-      <c r="C314" s="186"/>
-      <c r="D314" s="112"/>
-      <c r="E314" s="171"/>
-      <c r="F314" s="113"/>
-      <c r="G314" s="114"/>
-      <c r="H314" s="115"/>
+      <c r="C314" s="181" t="s">
+        <v>156</v>
+      </c>
+      <c r="D314" s="152"/>
+      <c r="E314" s="170"/>
+      <c r="F314" s="152"/>
+      <c r="G314" s="152"/>
+      <c r="H314" s="153"/>
     </row>
     <row r="315" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A315" s="1"/>
       <c r="B315" s="111"/>
-      <c r="C315" s="112"/>
+      <c r="C315" s="181"/>
       <c r="D315" s="112"/>
       <c r="E315" s="171"/>
       <c r="F315" s="113"/>
@@ -8379,29 +8396,29 @@
     <row r="316" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A316" s="1"/>
       <c r="B316" s="111"/>
-      <c r="C316" s="186" t="s">
-        <v>157</v>
-      </c>
-      <c r="D316" s="152"/>
-      <c r="E316" s="170"/>
-      <c r="F316" s="152"/>
-      <c r="G316" s="152"/>
-      <c r="H316" s="153"/>
+      <c r="C316" s="112"/>
+      <c r="D316" s="112"/>
+      <c r="E316" s="171"/>
+      <c r="F316" s="113"/>
+      <c r="G316" s="114"/>
+      <c r="H316" s="115"/>
     </row>
     <row r="317" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A317" s="1"/>
       <c r="B317" s="111"/>
-      <c r="C317" s="186"/>
-      <c r="D317" s="112"/>
-      <c r="E317" s="171"/>
-      <c r="F317" s="113"/>
-      <c r="G317" s="114"/>
-      <c r="H317" s="115"/>
+      <c r="C317" s="181" t="s">
+        <v>157</v>
+      </c>
+      <c r="D317" s="152"/>
+      <c r="E317" s="170"/>
+      <c r="F317" s="152"/>
+      <c r="G317" s="152"/>
+      <c r="H317" s="153"/>
     </row>
     <row r="318" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
       <c r="B318" s="111"/>
-      <c r="C318" s="112"/>
+      <c r="C318" s="181"/>
       <c r="D318" s="112"/>
       <c r="E318" s="171"/>
       <c r="F318" s="113"/>
@@ -8411,52 +8428,42 @@
     <row r="319" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
       <c r="B319" s="111"/>
-      <c r="C319" s="186" t="s">
-        <v>158</v>
-      </c>
-      <c r="D319" s="152"/>
-      <c r="E319" s="170"/>
-      <c r="F319" s="152"/>
-      <c r="G319" s="152"/>
-      <c r="H319" s="153"/>
+      <c r="C319" s="112"/>
+      <c r="D319" s="112"/>
+      <c r="E319" s="171"/>
+      <c r="F319" s="113"/>
+      <c r="G319" s="114"/>
+      <c r="H319" s="115"/>
     </row>
     <row r="320" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
       <c r="B320" s="111"/>
-      <c r="C320" s="186"/>
-      <c r="D320" s="148" t="s">
-        <v>470</v>
-      </c>
-      <c r="E320" s="178" t="s">
-        <v>471</v>
-      </c>
-      <c r="F320" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G320" s="150">
-        <v>44663</v>
-      </c>
-      <c r="H320" s="151">
-        <v>44663</v>
-      </c>
+      <c r="C320" s="181" t="s">
+        <v>158</v>
+      </c>
+      <c r="D320" s="152"/>
+      <c r="E320" s="170"/>
+      <c r="F320" s="152"/>
+      <c r="G320" s="152"/>
+      <c r="H320" s="153"/>
     </row>
     <row r="321" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A321" s="1"/>
       <c r="B321" s="111"/>
-      <c r="C321" s="112"/>
-      <c r="D321" s="143" t="s">
-        <v>472</v>
-      </c>
-      <c r="E321" s="176" t="s">
-        <v>473</v>
-      </c>
-      <c r="F321" s="144" t="s">
+      <c r="C321" s="181"/>
+      <c r="D321" s="148" t="s">
+        <v>470</v>
+      </c>
+      <c r="E321" s="178" t="s">
+        <v>471</v>
+      </c>
+      <c r="F321" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G321" s="145">
+      <c r="G321" s="150">
         <v>44663</v>
       </c>
-      <c r="H321" s="146">
+      <c r="H321" s="151">
         <v>44663</v>
       </c>
     </row>
@@ -8465,19 +8472,19 @@
       <c r="B322" s="111"/>
       <c r="C322" s="112"/>
       <c r="D322" s="143" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="E322" s="176" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F322" s="144" t="s">
         <v>232</v>
       </c>
       <c r="G322" s="145">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="H322" s="146">
-        <v>44630</v>
+        <v>44663</v>
       </c>
     </row>
     <row r="323" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8485,10 +8492,10 @@
       <c r="B323" s="111"/>
       <c r="C323" s="112"/>
       <c r="D323" s="143" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E323" s="176" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F323" s="144" t="s">
         <v>232</v>
@@ -8505,16 +8512,16 @@
       <c r="B324" s="111"/>
       <c r="C324" s="112"/>
       <c r="D324" s="143" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E324" s="176" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F324" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G324" s="145">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H324" s="146">
         <v>44630</v>
@@ -8525,10 +8532,10 @@
       <c r="B325" s="111"/>
       <c r="C325" s="112"/>
       <c r="D325" s="143" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E325" s="176" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F325" s="144" t="s">
         <v>281</v>
@@ -8545,19 +8552,19 @@
       <c r="B326" s="111"/>
       <c r="C326" s="112"/>
       <c r="D326" s="143" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E326" s="176" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F326" s="144" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G326" s="145">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H326" s="146">
-        <v>44824</v>
+        <v>44630</v>
       </c>
     </row>
     <row r="327" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8565,10 +8572,10 @@
       <c r="B327" s="111"/>
       <c r="C327" s="112"/>
       <c r="D327" s="143" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="E327" s="176" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F327" s="144" t="s">
         <v>256</v>
@@ -8585,19 +8592,19 @@
       <c r="B328" s="111"/>
       <c r="C328" s="112"/>
       <c r="D328" s="143" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E328" s="176" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F328" s="144" t="s">
-        <v>463</v>
+        <v>256</v>
       </c>
       <c r="G328" s="145">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H328" s="146">
-        <v>44622</v>
+        <v>44824</v>
       </c>
     </row>
     <row r="329" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8605,10 +8612,10 @@
       <c r="B329" s="111"/>
       <c r="C329" s="112"/>
       <c r="D329" s="143" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E329" s="176" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F329" s="144" t="s">
         <v>463</v>
@@ -8617,7 +8624,7 @@
         <v>44733</v>
       </c>
       <c r="H329" s="146">
-        <v>44621</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="330" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8625,19 +8632,19 @@
       <c r="B330" s="111"/>
       <c r="C330" s="112"/>
       <c r="D330" s="143" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E330" s="176" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F330" s="144" t="s">
         <v>463</v>
       </c>
       <c r="G330" s="145">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H330" s="146">
-        <v>44732</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="331" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8645,10 +8652,10 @@
       <c r="B331" s="111"/>
       <c r="C331" s="112"/>
       <c r="D331" s="143" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E331" s="176" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F331" s="144" t="s">
         <v>463</v>
@@ -8665,19 +8672,19 @@
       <c r="B332" s="111"/>
       <c r="C332" s="112"/>
       <c r="D332" s="143" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="E332" s="176" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F332" s="144" t="s">
-        <v>496</v>
+        <v>463</v>
       </c>
       <c r="G332" s="145">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H332" s="146">
-        <v>44621</v>
+        <v>44732</v>
       </c>
     </row>
     <row r="333" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8685,10 +8692,10 @@
       <c r="B333" s="111"/>
       <c r="C333" s="112"/>
       <c r="D333" s="143" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="E333" s="176" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="F333" s="144" t="s">
         <v>496</v>
@@ -8705,19 +8712,19 @@
       <c r="B334" s="111"/>
       <c r="C334" s="112"/>
       <c r="D334" s="143" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E334" s="176" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F334" s="144" t="s">
-        <v>267</v>
+        <v>496</v>
       </c>
       <c r="G334" s="145">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H334" s="146">
-        <v>44622</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="335" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8725,10 +8732,10 @@
       <c r="B335" s="111"/>
       <c r="C335" s="112"/>
       <c r="D335" s="143" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E335" s="176" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F335" s="144" t="s">
         <v>267</v>
@@ -8737,7 +8744,7 @@
         <v>44644</v>
       </c>
       <c r="H335" s="146">
-        <v>44621</v>
+        <v>44622</v>
       </c>
     </row>
     <row r="336" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8745,16 +8752,16 @@
       <c r="B336" s="111"/>
       <c r="C336" s="112"/>
       <c r="D336" s="143" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="E336" s="176" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F336" s="144" t="s">
-        <v>463</v>
+        <v>267</v>
       </c>
       <c r="G336" s="145">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H336" s="146">
         <v>44621</v>
@@ -8765,10 +8772,10 @@
       <c r="B337" s="111"/>
       <c r="C337" s="112"/>
       <c r="D337" s="143" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E337" s="176" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="F337" s="144" t="s">
         <v>463</v>
@@ -8785,19 +8792,19 @@
       <c r="B338" s="111"/>
       <c r="C338" s="112"/>
       <c r="D338" s="143" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E338" s="176" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F338" s="144" t="s">
-        <v>267</v>
+        <v>463</v>
       </c>
       <c r="G338" s="145">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H338" s="146">
-        <v>44627</v>
+        <v>44621</v>
       </c>
     </row>
     <row r="339" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8805,10 +8812,10 @@
       <c r="B339" s="111"/>
       <c r="C339" s="112"/>
       <c r="D339" s="143" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E339" s="176" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F339" s="144" t="s">
         <v>267</v>
@@ -8825,19 +8832,19 @@
       <c r="B340" s="111"/>
       <c r="C340" s="112"/>
       <c r="D340" s="143" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E340" s="176" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F340" s="144" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G340" s="145">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H340" s="146">
-        <v>44628</v>
+        <v>44627</v>
       </c>
     </row>
     <row r="341" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -8845,10 +8852,10 @@
       <c r="B341" s="111"/>
       <c r="C341" s="112"/>
       <c r="D341" s="143" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E341" s="176" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F341" s="144" t="s">
         <v>232</v>
@@ -8865,16 +8872,16 @@
       <c r="B342" s="111"/>
       <c r="C342" s="112"/>
       <c r="D342" s="143" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E342" s="176" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F342" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G342" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H342" s="146">
         <v>44628</v>
@@ -8885,10 +8892,10 @@
       <c r="B343" s="111"/>
       <c r="C343" s="112"/>
       <c r="D343" s="143" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E343" s="176" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F343" s="144" t="s">
         <v>281</v>
@@ -8905,16 +8912,16 @@
       <c r="B344" s="111"/>
       <c r="C344" s="112"/>
       <c r="D344" s="143" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="E344" s="176" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F344" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G344" s="145">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H344" s="146">
         <v>44628</v>
@@ -8925,10 +8932,10 @@
       <c r="B345" s="111"/>
       <c r="C345" s="112"/>
       <c r="D345" s="143" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="E345" s="176" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F345" s="144" t="s">
         <v>232</v>
@@ -8945,16 +8952,16 @@
       <c r="B346" s="111"/>
       <c r="C346" s="112"/>
       <c r="D346" s="143" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="E346" s="176" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F346" s="144" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G346" s="145">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H346" s="146">
         <v>44628</v>
@@ -8965,10 +8972,10 @@
       <c r="B347" s="111"/>
       <c r="C347" s="112"/>
       <c r="D347" s="143" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E347" s="176" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F347" s="144" t="s">
         <v>281</v>
@@ -8985,19 +8992,19 @@
       <c r="B348" s="111"/>
       <c r="C348" s="112"/>
       <c r="D348" s="143" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E348" s="176" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F348" s="144" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G348" s="145">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H348" s="146">
-        <v>44617</v>
+        <v>44628</v>
       </c>
     </row>
     <row r="349" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9005,10 +9012,10 @@
       <c r="B349" s="111"/>
       <c r="C349" s="112"/>
       <c r="D349" s="143" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="E349" s="176" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F349" s="144" t="s">
         <v>232</v>
@@ -9025,19 +9032,19 @@
       <c r="B350" s="111"/>
       <c r="C350" s="112"/>
       <c r="D350" s="143" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E350" s="176" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="F350" s="144" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G350" s="145">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H350" s="146">
-        <v>44662</v>
+        <v>44617</v>
       </c>
     </row>
     <row r="351" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9045,10 +9052,10 @@
       <c r="B351" s="111"/>
       <c r="C351" s="112"/>
       <c r="D351" s="143" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="E351" s="176" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F351" s="144" t="s">
         <v>256</v>
@@ -9064,143 +9071,143 @@
       <c r="A352" s="1"/>
       <c r="B352" s="111"/>
       <c r="C352" s="112"/>
-      <c r="D352" s="112"/>
-      <c r="E352" s="171"/>
-      <c r="F352" s="113"/>
-      <c r="G352" s="114"/>
-      <c r="H352" s="115"/>
+      <c r="D352" s="143" t="s">
+        <v>534</v>
+      </c>
+      <c r="E352" s="176" t="s">
+        <v>533</v>
+      </c>
+      <c r="F352" s="144" t="s">
+        <v>256</v>
+      </c>
+      <c r="G352" s="145">
+        <v>44740</v>
+      </c>
+      <c r="H352" s="146">
+        <v>44662</v>
+      </c>
     </row>
     <row r="353" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="B353" s="111"/>
-      <c r="C353" s="186" t="s">
-        <v>147</v>
-      </c>
-      <c r="D353" s="152"/>
-      <c r="E353" s="170"/>
-      <c r="F353" s="152"/>
-      <c r="G353" s="152"/>
-      <c r="H353" s="153"/>
+      <c r="C353" s="112"/>
+      <c r="D353" s="112"/>
+      <c r="E353" s="171"/>
+      <c r="F353" s="113"/>
+      <c r="G353" s="114"/>
+      <c r="H353" s="115"/>
     </row>
     <row r="354" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A354" s="1"/>
       <c r="B354" s="111"/>
-      <c r="C354" s="186"/>
-      <c r="D354" s="148" t="s">
-        <v>274</v>
-      </c>
-      <c r="E354" s="178" t="s">
-        <v>448</v>
-      </c>
-      <c r="F354" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G354" s="150">
-        <v>44167</v>
-      </c>
-      <c r="H354" s="151">
-        <v>44167</v>
-      </c>
+      <c r="C354" s="181" t="s">
+        <v>147</v>
+      </c>
+      <c r="D354" s="152"/>
+      <c r="E354" s="170"/>
+      <c r="F354" s="152"/>
+      <c r="G354" s="152"/>
+      <c r="H354" s="153"/>
     </row>
     <row r="355" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A355" s="1"/>
       <c r="B355" s="111"/>
-      <c r="C355" s="112"/>
-      <c r="D355" s="143" t="s">
-        <v>449</v>
-      </c>
-      <c r="E355" s="176" t="s">
-        <v>450</v>
-      </c>
-      <c r="F355" s="144" t="s">
-        <v>256</v>
-      </c>
-      <c r="G355" s="145">
-        <v>44575</v>
-      </c>
-      <c r="H355" s="146">
+      <c r="C355" s="181"/>
+      <c r="D355" s="148" t="s">
+        <v>274</v>
+      </c>
+      <c r="E355" s="178" t="s">
+        <v>448</v>
+      </c>
+      <c r="F355" s="149" t="s">
+        <v>232</v>
+      </c>
+      <c r="G355" s="150">
         <v>44167</v>
       </c>
-    </row>
-    <row r="356" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H355" s="151">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A356" s="1"/>
       <c r="B356" s="111"/>
       <c r="C356" s="112"/>
       <c r="D356" s="143" t="s">
-        <v>452</v>
-      </c>
-      <c r="E356" s="174" t="s">
-        <v>451</v>
+        <v>449</v>
+      </c>
+      <c r="E356" s="176" t="s">
+        <v>450</v>
       </c>
       <c r="F356" s="144" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G356" s="145">
-        <v>44404</v>
+        <v>44575</v>
       </c>
       <c r="H356" s="146">
-        <v>44404</v>
-      </c>
-    </row>
-    <row r="357" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="B357" s="111"/>
       <c r="C357" s="112"/>
-      <c r="D357" s="112"/>
-      <c r="E357" s="171"/>
-      <c r="F357" s="113"/>
-      <c r="G357" s="114"/>
-      <c r="H357" s="115"/>
+      <c r="D357" s="143" t="s">
+        <v>452</v>
+      </c>
+      <c r="E357" s="174" t="s">
+        <v>451</v>
+      </c>
+      <c r="F357" s="144" t="s">
+        <v>281</v>
+      </c>
+      <c r="G357" s="145">
+        <v>44404</v>
+      </c>
+      <c r="H357" s="146">
+        <v>44404</v>
+      </c>
     </row>
     <row r="358" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="B358" s="111"/>
-      <c r="C358" s="186" t="s">
-        <v>159</v>
-      </c>
-      <c r="D358" s="152"/>
-      <c r="E358" s="170"/>
-      <c r="F358" s="152"/>
-      <c r="G358" s="152"/>
-      <c r="H358" s="153"/>
+      <c r="C358" s="112"/>
+      <c r="D358" s="112"/>
+      <c r="E358" s="171"/>
+      <c r="F358" s="113"/>
+      <c r="G358" s="114"/>
+      <c r="H358" s="115"/>
     </row>
     <row r="359" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A359" s="1"/>
       <c r="B359" s="111"/>
-      <c r="C359" s="186"/>
-      <c r="D359" s="148" t="s">
-        <v>454</v>
-      </c>
-      <c r="E359" s="178" t="s">
-        <v>453</v>
-      </c>
-      <c r="F359" s="149" t="s">
-        <v>232</v>
-      </c>
-      <c r="G359" s="150">
-        <v>44635</v>
-      </c>
-      <c r="H359" s="151">
-        <v>44635</v>
-      </c>
+      <c r="C359" s="181" t="s">
+        <v>159</v>
+      </c>
+      <c r="D359" s="152"/>
+      <c r="E359" s="170"/>
+      <c r="F359" s="152"/>
+      <c r="G359" s="152"/>
+      <c r="H359" s="153"/>
     </row>
     <row r="360" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="B360" s="111"/>
-      <c r="C360" s="112"/>
-      <c r="D360" s="143" t="s">
-        <v>456</v>
-      </c>
-      <c r="E360" s="176" t="s">
-        <v>455</v>
-      </c>
-      <c r="F360" s="144" t="s">
+      <c r="C360" s="181"/>
+      <c r="D360" s="148" t="s">
+        <v>454</v>
+      </c>
+      <c r="E360" s="178" t="s">
+        <v>453</v>
+      </c>
+      <c r="F360" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="G360" s="145">
+      <c r="G360" s="150">
         <v>44635</v>
       </c>
-      <c r="H360" s="146">
+      <c r="H360" s="151">
         <v>44635</v>
       </c>
     </row>
@@ -9209,10 +9216,10 @@
       <c r="B361" s="111"/>
       <c r="C361" s="112"/>
       <c r="D361" s="143" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E361" s="176" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F361" s="144" t="s">
         <v>232</v>
@@ -9229,10 +9236,10 @@
       <c r="B362" s="111"/>
       <c r="C362" s="112"/>
       <c r="D362" s="143" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E362" s="176" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F362" s="144" t="s">
         <v>232</v>
@@ -9249,19 +9256,19 @@
       <c r="B363" s="111"/>
       <c r="C363" s="112"/>
       <c r="D363" s="143" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="E363" s="176" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="F363" s="144" t="s">
-        <v>463</v>
+        <v>232</v>
       </c>
       <c r="G363" s="145">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H363" s="146">
-        <v>44644</v>
+        <v>44635</v>
       </c>
     </row>
     <row r="364" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9269,10 +9276,10 @@
       <c r="B364" s="111"/>
       <c r="C364" s="112"/>
       <c r="D364" s="143" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E364" s="176" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F364" s="144" t="s">
         <v>463</v>
@@ -9289,19 +9296,19 @@
       <c r="B365" s="111"/>
       <c r="C365" s="112"/>
       <c r="D365" s="143" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="E365" s="176" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F365" s="144" t="s">
-        <v>267</v>
+        <v>463</v>
       </c>
       <c r="G365" s="145">
+        <v>44701</v>
+      </c>
+      <c r="H365" s="146">
         <v>44644</v>
-      </c>
-      <c r="H365" s="146">
-        <v>44636</v>
       </c>
     </row>
     <row r="366" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -9309,10 +9316,10 @@
       <c r="B366" s="111"/>
       <c r="C366" s="112"/>
       <c r="D366" s="143" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="E366" s="176" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F366" s="144" t="s">
         <v>267</v>
@@ -9324,25 +9331,35 @@
         <v>44636</v>
       </c>
     </row>
-    <row r="367" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A367" s="1"/>
-      <c r="B367" s="116"/>
-      <c r="C367" s="117"/>
-      <c r="D367" s="117"/>
-      <c r="E367" s="179"/>
-      <c r="F367" s="118"/>
-      <c r="G367" s="119"/>
-      <c r="H367" s="120"/>
-    </row>
-    <row r="368" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="B367" s="111"/>
+      <c r="C367" s="112"/>
+      <c r="D367" s="143" t="s">
+        <v>468</v>
+      </c>
+      <c r="E367" s="176" t="s">
+        <v>469</v>
+      </c>
+      <c r="F367" s="144" t="s">
+        <v>267</v>
+      </c>
+      <c r="G367" s="145">
+        <v>44644</v>
+      </c>
+      <c r="H367" s="146">
+        <v>44636</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" s="78" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
-      <c r="B368" s="1"/>
-      <c r="C368" s="1"/>
-      <c r="D368" s="1"/>
-      <c r="E368" s="180"/>
-      <c r="F368" s="121"/>
-      <c r="G368" s="122"/>
-      <c r="H368" s="122"/>
+      <c r="B368" s="116"/>
+      <c r="C368" s="117"/>
+      <c r="D368" s="117"/>
+      <c r="E368" s="179"/>
+      <c r="F368" s="118"/>
+      <c r="G368" s="119"/>
+      <c r="H368" s="120"/>
     </row>
     <row r="369" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A369" s="1"/>
@@ -9494,11 +9511,15 @@
       <c r="G383" s="122"/>
       <c r="H383" s="122"/>
     </row>
-    <row r="384" spans="1:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E384" s="169"/>
-      <c r="F384" s="95"/>
-      <c r="G384" s="110"/>
-      <c r="H384" s="110"/>
+    <row r="384" spans="1:8" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A384" s="1"/>
+      <c r="B384" s="1"/>
+      <c r="C384" s="1"/>
+      <c r="D384" s="1"/>
+      <c r="E384" s="180"/>
+      <c r="F384" s="121"/>
+      <c r="G384" s="122"/>
+      <c r="H384" s="122"/>
     </row>
     <row r="385" spans="5:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="E385" s="169"/>
@@ -9512,20 +9533,27 @@
       <c r="G386" s="110"/>
       <c r="H386" s="110"/>
     </row>
+    <row r="387" spans="5:8" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E387" s="169"/>
+      <c r="F387" s="95"/>
+      <c r="G387" s="110"/>
+      <c r="H387" s="110"/>
+    </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="C313:C314"/>
-    <mergeCell ref="C316:C317"/>
-    <mergeCell ref="C319:C320"/>
-    <mergeCell ref="C353:C354"/>
-    <mergeCell ref="C358:C359"/>
-    <mergeCell ref="C298:C299"/>
-    <mergeCell ref="C301:C302"/>
-    <mergeCell ref="C304:C305"/>
-    <mergeCell ref="C307:C308"/>
-    <mergeCell ref="C310:C311"/>
-    <mergeCell ref="C292:C293"/>
-    <mergeCell ref="C295:C296"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B289:B290"/>
+    <mergeCell ref="C290:C291"/>
+    <mergeCell ref="C156:C157"/>
+    <mergeCell ref="B285:B286"/>
+    <mergeCell ref="C286:C287"/>
+    <mergeCell ref="C224:C225"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C293:C294"/>
+    <mergeCell ref="C296:C297"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C14:C15"/>
@@ -9538,17 +9566,16 @@
     <mergeCell ref="C101:C102"/>
     <mergeCell ref="C104:C105"/>
     <mergeCell ref="C137:C138"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B288:B289"/>
-    <mergeCell ref="C289:C290"/>
-    <mergeCell ref="C156:C157"/>
-    <mergeCell ref="B284:B285"/>
-    <mergeCell ref="C285:C286"/>
-    <mergeCell ref="C224:C225"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C299:C300"/>
+    <mergeCell ref="C302:C303"/>
+    <mergeCell ref="C305:C306"/>
+    <mergeCell ref="C308:C309"/>
+    <mergeCell ref="C311:C312"/>
+    <mergeCell ref="C314:C315"/>
+    <mergeCell ref="C317:C318"/>
+    <mergeCell ref="C320:C321"/>
+    <mergeCell ref="C354:C355"/>
+    <mergeCell ref="C359:C360"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -9582,20 +9609,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="213" t="s">
+      <c r="B2" s="196" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="214"/>
-      <c r="D2" s="215"/>
-      <c r="E2" s="210" t="s">
+      <c r="C2" s="197"/>
+      <c r="D2" s="198"/>
+      <c r="E2" s="193" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="212"/>
-      <c r="G2" s="210" t="s">
+      <c r="F2" s="195"/>
+      <c r="G2" s="193" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="211"/>
-      <c r="I2" s="212"/>
+      <c r="H2" s="194"/>
+      <c r="I2" s="195"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -9616,10 +9643,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="216" t="s">
+      <c r="H3" s="199" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="217"/>
+      <c r="I3" s="200"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -9661,7 +9688,7 @@
       <c r="F5" s="207" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="198" t="s">
+      <c r="G5" s="210" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -9677,11 +9704,11 @@
       <c r="D6" s="205"/>
       <c r="E6" s="35"/>
       <c r="F6" s="208"/>
-      <c r="G6" s="199"/>
-      <c r="H6" s="193" t="s">
+      <c r="G6" s="211"/>
+      <c r="H6" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="194"/>
+      <c r="I6" s="192"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
@@ -9689,7 +9716,7 @@
       <c r="D7" s="206"/>
       <c r="E7" s="36"/>
       <c r="F7" s="209"/>
-      <c r="G7" s="200"/>
+      <c r="G7" s="212"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -9729,13 +9756,13 @@
       <c r="D9" s="204" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="195" t="s">
+      <c r="E9" s="215" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="207" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="198" t="s">
+      <c r="G9" s="210" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -9750,22 +9777,22 @@
       <c r="B10" s="61"/>
       <c r="C10" s="202"/>
       <c r="D10" s="205"/>
-      <c r="E10" s="196"/>
+      <c r="E10" s="216"/>
       <c r="F10" s="208"/>
-      <c r="G10" s="199"/>
-      <c r="H10" s="193" t="s">
+      <c r="G10" s="211"/>
+      <c r="H10" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="194"/>
+      <c r="I10" s="192"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
       <c r="C11" s="203"/>
       <c r="D11" s="206"/>
-      <c r="E11" s="197"/>
+      <c r="E11" s="217"/>
       <c r="F11" s="209"/>
-      <c r="G11" s="200"/>
+      <c r="G11" s="212"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -9787,7 +9814,7 @@
       <c r="F12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="198" t="s">
+      <c r="G12" s="210" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -9807,7 +9834,7 @@
       <c r="F13" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G13" s="200"/>
+      <c r="G13" s="212"/>
       <c r="H13" s="8"/>
       <c r="I13" s="17"/>
     </row>
@@ -9852,8 +9879,8 @@
       <c r="E16" s="25"/>
       <c r="F16" s="22"/>
       <c r="G16" s="25"/>
-      <c r="H16" s="191"/>
-      <c r="I16" s="192"/>
+      <c r="H16" s="213"/>
+      <c r="I16" s="214"/>
     </row>
     <row r="17" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
@@ -10273,13 +10300,13 @@
       <c r="D40" s="204" t="s">
         <v>43</v>
       </c>
-      <c r="E40" s="195" t="s">
+      <c r="E40" s="215" t="s">
         <v>45</v>
       </c>
       <c r="F40" s="207" t="s">
         <v>46</v>
       </c>
-      <c r="G40" s="198" t="s">
+      <c r="G40" s="210" t="s">
         <v>47</v>
       </c>
       <c r="H40" s="6" t="s">
@@ -10293,21 +10320,21 @@
       <c r="B41" s="61"/>
       <c r="C41" s="202"/>
       <c r="D41" s="205"/>
-      <c r="E41" s="196"/>
+      <c r="E41" s="216"/>
       <c r="F41" s="208"/>
-      <c r="G41" s="199"/>
-      <c r="H41" s="193" t="s">
+      <c r="G41" s="211"/>
+      <c r="H41" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="I41" s="194"/>
+      <c r="I41" s="192"/>
     </row>
     <row r="42" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B42" s="61"/>
       <c r="C42" s="203"/>
       <c r="D42" s="206"/>
-      <c r="E42" s="197"/>
+      <c r="E42" s="217"/>
       <c r="F42" s="209"/>
-      <c r="G42" s="200"/>
+      <c r="G42" s="212"/>
       <c r="H42" s="8" t="s">
         <v>23</v>
       </c>
@@ -10347,13 +10374,13 @@
       <c r="D44" s="204" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="195" t="s">
+      <c r="E44" s="215" t="s">
         <v>55</v>
       </c>
       <c r="F44" s="207" t="s">
         <v>56</v>
       </c>
-      <c r="G44" s="198" t="s">
+      <c r="G44" s="210" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="6" t="s">
@@ -10367,21 +10394,21 @@
       <c r="B45" s="61"/>
       <c r="C45" s="202"/>
       <c r="D45" s="205"/>
-      <c r="E45" s="196"/>
+      <c r="E45" s="216"/>
       <c r="F45" s="208"/>
-      <c r="G45" s="199"/>
-      <c r="H45" s="193" t="s">
+      <c r="G45" s="211"/>
+      <c r="H45" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="I45" s="194"/>
+      <c r="I45" s="192"/>
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
       <c r="C46" s="203"/>
       <c r="D46" s="206"/>
-      <c r="E46" s="197"/>
+      <c r="E46" s="217"/>
       <c r="F46" s="209"/>
-      <c r="G46" s="200"/>
+      <c r="G46" s="212"/>
       <c r="H46" s="8" t="s">
         <v>23</v>
       </c>
@@ -10406,8 +10433,8 @@
       <c r="E48" s="25"/>
       <c r="F48" s="22"/>
       <c r="G48" s="25"/>
-      <c r="H48" s="191"/>
-      <c r="I48" s="192"/>
+      <c r="H48" s="213"/>
+      <c r="I48" s="214"/>
     </row>
     <row r="49" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="61" t="s">
@@ -10470,10 +10497,10 @@
       <c r="E52" s="39"/>
       <c r="F52" s="12"/>
       <c r="G52" s="32"/>
-      <c r="H52" s="193" t="s">
+      <c r="H52" s="191" t="s">
         <v>32</v>
       </c>
-      <c r="I52" s="194"/>
+      <c r="I52" s="192"/>
     </row>
     <row r="53" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B53" s="61"/>
@@ -10506,8 +10533,8 @@
       <c r="E55" s="25"/>
       <c r="F55" s="22"/>
       <c r="G55" s="25"/>
-      <c r="H55" s="191"/>
-      <c r="I55" s="192"/>
+      <c r="H55" s="213"/>
+      <c r="I55" s="214"/>
     </row>
     <row r="56" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="64" t="s">
@@ -10920,8 +10947,8 @@
       <c r="E83" s="25"/>
       <c r="F83" s="22"/>
       <c r="G83" s="25"/>
-      <c r="H83" s="191"/>
-      <c r="I83" s="192"/>
+      <c r="H83" s="213"/>
+      <c r="I83" s="214"/>
     </row>
     <row r="84" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="61"/>
@@ -11065,15 +11092,22 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="H83:I83"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="E44:E46"/>
+    <mergeCell ref="G44:G46"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="F44:F46"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="E40:E42"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="G40:G42"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="G12:G13"/>
@@ -11084,22 +11118,15 @@
     <mergeCell ref="D9:D11"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C40:C42"/>
-    <mergeCell ref="D40:D42"/>
-    <mergeCell ref="E40:E42"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="G40:G42"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="H83:I83"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="G44:G46"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H55:I55"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11132,10 +11159,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="219"/>
-      <c r="D2" s="211" t="s">
+      <c r="D2" s="194" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="212" t="s">
+      <c r="E2" s="195" t="s">
         <v>0</v>
       </c>
     </row>
@@ -11146,8 +11173,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="216"/>
-      <c r="E3" s="217"/>
+      <c r="D3" s="199"/>
+      <c r="E3" s="200"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 2 Maret 2023 18:35 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1420" uniqueCount="875">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -2809,6 +2809,14 @@
   <si>
     <t>Mendapatkan Data List WorkFlow Path berdasarkan ID Branch (varBranch_RefID), ID Jenis Dokumen Bisnis (varBusinessDocumentType_RefID), ID Entitas Submitter (varSubmitterEntity_RefID), dan ID Combined Budget (varCombinedBudget_RefID).
 Adapun Pick Statement (varPickStatement), Sort Statement (varSortStatement), Filter Statement (varFilterStatement), dan Paging Statement (varPagingStatement) merupakan parameter optional yang dapat digunakan ataupun tidak sesuai dengan kebutuhan</t>
+  </si>
+  <si>
+    <t>Func_GetDataEntities_Mapper_BusinessDocumentTypeToWorkFlow</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Entities untuk Pemetaan Jenis Dokumen Bisnis pada WorkFlow berdasarkan ID (varID).
+Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
+Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
   </si>
 </sst>
 </file>
@@ -4206,6 +4214,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4224,20 +4247,71 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4245,12 +4319,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4259,66 +4327,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4643,13 +4651,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I483"/>
+  <dimension ref="A1:I484"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E329" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E324" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E332" sqref="E332"/>
+      <selection pane="bottomRight" activeCell="D324" sqref="D324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4668,20 +4676,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="218" t="s">
+      <c r="B2" s="212" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="219"/>
-      <c r="D2" s="220"/>
-      <c r="E2" s="214" t="s">
+      <c r="C2" s="213"/>
+      <c r="D2" s="214"/>
+      <c r="E2" s="219" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="210" t="s">
+      <c r="F2" s="215" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="211"/>
-      <c r="H2" s="212"/>
-      <c r="I2" s="216" t="s">
+      <c r="G2" s="216"/>
+      <c r="H2" s="217"/>
+      <c r="I2" s="210" t="s">
         <v>673</v>
       </c>
     </row>
@@ -4695,7 +4703,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="215"/>
+      <c r="E3" s="220"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -4705,11 +4713,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="217"/>
+      <c r="I3" s="211"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="213" t="s">
+      <c r="B4" s="218" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -10226,7 +10234,9 @@
       <c r="H316" s="203">
         <v>44965</v>
       </c>
-      <c r="I316" s="176"/>
+      <c r="I316" s="176" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="317" spans="1:9" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A317" s="1"/>
@@ -10247,7 +10257,9 @@
       <c r="H317" s="203">
         <v>44965</v>
       </c>
-      <c r="I317" s="176"/>
+      <c r="I317" s="176" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="318" spans="1:9" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A318" s="1"/>
@@ -10268,7 +10280,9 @@
       <c r="H318" s="203">
         <v>44965</v>
       </c>
-      <c r="I318" s="176"/>
+      <c r="I318" s="176" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="319" spans="1:9" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A319" s="1"/>
@@ -10289,7 +10303,9 @@
       <c r="H319" s="203">
         <v>44964</v>
       </c>
-      <c r="I319" s="176"/>
+      <c r="I319" s="176" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="320" spans="1:9" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A320" s="1"/>
@@ -10310,7 +10326,9 @@
       <c r="H320" s="204">
         <v>44901</v>
       </c>
-      <c r="I320" s="177"/>
+      <c r="I320" s="177" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="321" spans="1:9" s="78" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A321" s="1"/>
@@ -10331,7 +10349,9 @@
       <c r="H321" s="203">
         <v>44965</v>
       </c>
-      <c r="I321" s="176"/>
+      <c r="I321" s="176" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="322" spans="1:9" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A322" s="1"/>
@@ -10352,84 +10372,88 @@
       <c r="H322" s="203">
         <v>44965</v>
       </c>
-      <c r="I322" s="176"/>
+      <c r="I322" s="176" t="s">
+        <v>714</v>
+      </c>
     </row>
     <row r="323" spans="1:9" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A323" s="1"/>
       <c r="B323" s="109"/>
       <c r="C323" s="110"/>
-      <c r="D323" s="165" t="s">
+      <c r="D323" s="167" t="s">
         <v>618</v>
       </c>
-      <c r="E323" s="159" t="s">
+      <c r="E323" s="158" t="s">
         <v>620</v>
       </c>
-      <c r="F323" s="148" t="s">
+      <c r="F323" s="151" t="s">
         <v>232</v>
       </c>
-      <c r="G323" s="186">
+      <c r="G323" s="190">
         <v>44965</v>
       </c>
-      <c r="H323" s="201">
+      <c r="H323" s="204">
         <v>44965</v>
       </c>
-      <c r="I323" s="174"/>
-    </row>
-    <row r="324" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I323" s="177" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" s="78" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
       <c r="A324" s="1"/>
       <c r="B324" s="109"/>
       <c r="C324" s="110"/>
-      <c r="D324" s="144"/>
-      <c r="E324" s="156"/>
-      <c r="F324" s="149"/>
-      <c r="G324" s="187"/>
-      <c r="H324" s="202"/>
-      <c r="I324" s="175"/>
-    </row>
-    <row r="325" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="D324" s="165" t="s">
+        <v>873</v>
+      </c>
+      <c r="E324" s="159" t="s">
+        <v>874</v>
+      </c>
+      <c r="F324" s="148" t="s">
+        <v>232</v>
+      </c>
+      <c r="G324" s="186">
+        <v>44965</v>
+      </c>
+      <c r="H324" s="201">
+        <v>44965</v>
+      </c>
+      <c r="I324" s="174" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A325" s="1"/>
       <c r="B325" s="109"/>
       <c r="C325" s="110"/>
-      <c r="D325" s="166" t="s">
-        <v>676</v>
-      </c>
-      <c r="E325" s="157" t="s">
-        <v>686</v>
-      </c>
-      <c r="F325" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G325" s="188">
-        <v>44923</v>
-      </c>
-      <c r="H325" s="203">
-        <v>44923</v>
-      </c>
-      <c r="I325" s="171" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="326" spans="1:9" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="D325" s="144"/>
+      <c r="E325" s="156"/>
+      <c r="F325" s="149"/>
+      <c r="G325" s="187"/>
+      <c r="H325" s="202"/>
+      <c r="I325" s="175"/>
+    </row>
+    <row r="326" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A326" s="1"/>
       <c r="B326" s="109"/>
       <c r="C326" s="110"/>
       <c r="D326" s="166" t="s">
-        <v>338</v>
+        <v>676</v>
       </c>
       <c r="E326" s="157" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F326" s="150" t="s">
         <v>232</v>
       </c>
       <c r="G326" s="188">
-        <v>44951</v>
+        <v>44923</v>
       </c>
       <c r="H326" s="203">
-        <v>44951</v>
+        <v>44923</v>
       </c>
       <c r="I326" s="171" t="s">
-        <v>675</v>
+        <v>677</v>
       </c>
     </row>
     <row r="327" spans="1:9" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
@@ -10437,156 +10461,168 @@
       <c r="B327" s="109"/>
       <c r="C327" s="110"/>
       <c r="D327" s="166" t="s">
-        <v>672</v>
+        <v>338</v>
       </c>
       <c r="E327" s="157" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="F327" s="150" t="s">
         <v>232</v>
       </c>
       <c r="G327" s="188">
-        <v>44977</v>
+        <v>44951</v>
       </c>
       <c r="H327" s="203">
-        <v>44977</v>
+        <v>44951</v>
       </c>
       <c r="I327" s="171" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="328" spans="1:9" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A328" s="1"/>
       <c r="B328" s="109"/>
       <c r="C328" s="110"/>
-      <c r="D328" s="167" t="s">
-        <v>678</v>
-      </c>
-      <c r="E328" s="158" t="s">
-        <v>683</v>
-      </c>
-      <c r="F328" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G328" s="190">
-        <v>44951</v>
-      </c>
-      <c r="H328" s="204">
-        <v>44950</v>
-      </c>
-      <c r="I328" s="183" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="329" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="D328" s="166" t="s">
+        <v>672</v>
+      </c>
+      <c r="E328" s="157" t="s">
+        <v>684</v>
+      </c>
+      <c r="F328" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G328" s="188">
+        <v>44977</v>
+      </c>
+      <c r="H328" s="203">
+        <v>44977</v>
+      </c>
+      <c r="I328" s="171" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" s="78" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A329" s="1"/>
       <c r="B329" s="109"/>
       <c r="C329" s="110"/>
       <c r="D329" s="167" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="E329" s="158" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="F329" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G329" s="190">
-        <v>44923</v>
+        <v>44951</v>
       </c>
       <c r="H329" s="204">
-        <v>44923</v>
+        <v>44950</v>
       </c>
       <c r="I329" s="183" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="330" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A330" s="1"/>
       <c r="B330" s="109"/>
       <c r="C330" s="110"/>
-      <c r="D330" s="167"/>
-      <c r="E330" s="158"/>
-      <c r="F330" s="151"/>
-      <c r="G330" s="190"/>
-      <c r="H330" s="204"/>
-      <c r="I330" s="183"/>
-    </row>
-    <row r="331" spans="1:9" s="78" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="D330" s="167" t="s">
+        <v>680</v>
+      </c>
+      <c r="E330" s="158" t="s">
+        <v>682</v>
+      </c>
+      <c r="F330" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G330" s="190">
+        <v>44923</v>
+      </c>
+      <c r="H330" s="204">
+        <v>44923</v>
+      </c>
+      <c r="I330" s="183" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A331" s="1"/>
       <c r="B331" s="109"/>
       <c r="C331" s="110"/>
-      <c r="D331" s="167" t="s">
-        <v>870</v>
-      </c>
-      <c r="E331" s="158" t="s">
-        <v>872</v>
-      </c>
-      <c r="F331" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G331" s="190">
-        <v>44987</v>
-      </c>
-      <c r="H331" s="204">
-        <v>44952</v>
-      </c>
-      <c r="I331" s="183" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="332" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D331" s="167"/>
+      <c r="E331" s="158"/>
+      <c r="F331" s="151"/>
+      <c r="G331" s="190"/>
+      <c r="H331" s="204"/>
+      <c r="I331" s="183"/>
+    </row>
+    <row r="332" spans="1:9" s="78" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A332" s="1"/>
       <c r="B332" s="109"/>
       <c r="C332" s="110"/>
-      <c r="D332" s="165"/>
-      <c r="E332" s="159"/>
-      <c r="F332" s="148"/>
-      <c r="G332" s="186"/>
-      <c r="H332" s="201"/>
-      <c r="I332" s="182"/>
-    </row>
-    <row r="333" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D332" s="167" t="s">
+        <v>870</v>
+      </c>
+      <c r="E332" s="158" t="s">
+        <v>872</v>
+      </c>
+      <c r="F332" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G332" s="190">
+        <v>44987</v>
+      </c>
+      <c r="H332" s="204">
+        <v>44952</v>
+      </c>
+      <c r="I332" s="183" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A333" s="1"/>
       <c r="B333" s="109"/>
       <c r="C333" s="110"/>
-      <c r="D333" s="144"/>
-      <c r="E333" s="156"/>
-      <c r="F333" s="149"/>
-      <c r="G333" s="187"/>
-      <c r="H333" s="202"/>
-      <c r="I333" s="175"/>
-    </row>
-    <row r="334" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D333" s="165"/>
+      <c r="E333" s="159"/>
+      <c r="F333" s="148"/>
+      <c r="G333" s="186"/>
+      <c r="H333" s="201"/>
+      <c r="I333" s="182"/>
+    </row>
+    <row r="334" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A334" s="1"/>
       <c r="B334" s="109"/>
       <c r="C334" s="110"/>
-      <c r="D334" s="166" t="s">
-        <v>339</v>
-      </c>
-      <c r="E334" s="157" t="s">
-        <v>340</v>
-      </c>
-      <c r="F334" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G334" s="188">
-        <v>44952</v>
-      </c>
-      <c r="H334" s="203">
-        <v>44952</v>
-      </c>
-      <c r="I334" s="174"/>
-    </row>
-    <row r="335" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D334" s="144"/>
+      <c r="E334" s="156"/>
+      <c r="F334" s="149"/>
+      <c r="G334" s="187"/>
+      <c r="H334" s="202"/>
+      <c r="I334" s="175"/>
+    </row>
+    <row r="335" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A335" s="1"/>
       <c r="B335" s="109"/>
       <c r="C335" s="110"/>
-      <c r="D335" s="165"/>
-      <c r="E335" s="155"/>
-      <c r="F335" s="148"/>
-      <c r="G335" s="186"/>
-      <c r="H335" s="201"/>
+      <c r="D335" s="166" t="s">
+        <v>339</v>
+      </c>
+      <c r="E335" s="157" t="s">
+        <v>340</v>
+      </c>
+      <c r="F335" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G335" s="188">
+        <v>44952</v>
+      </c>
+      <c r="H335" s="203">
+        <v>44952</v>
+      </c>
       <c r="I335" s="174"/>
     </row>
     <row r="336" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10604,73 +10640,63 @@
       <c r="A337" s="1"/>
       <c r="B337" s="109"/>
       <c r="C337" s="110"/>
-      <c r="D337" s="166"/>
-      <c r="E337" s="162"/>
-      <c r="F337" s="150"/>
-      <c r="G337" s="188"/>
-      <c r="H337" s="203"/>
+      <c r="D337" s="165"/>
+      <c r="E337" s="155"/>
+      <c r="F337" s="148"/>
+      <c r="G337" s="186"/>
+      <c r="H337" s="201"/>
       <c r="I337" s="174"/>
     </row>
-    <row r="338" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A338" s="1"/>
       <c r="B338" s="109"/>
       <c r="C338" s="110"/>
-      <c r="D338" s="166" t="s">
-        <v>391</v>
-      </c>
-      <c r="E338" s="157" t="s">
-        <v>392</v>
-      </c>
-      <c r="F338" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G338" s="188">
-        <v>44957</v>
-      </c>
-      <c r="H338" s="203">
-        <v>42982</v>
-      </c>
+      <c r="D338" s="166"/>
+      <c r="E338" s="162"/>
+      <c r="F338" s="150"/>
+      <c r="G338" s="188"/>
+      <c r="H338" s="203"/>
       <c r="I338" s="174"/>
     </row>
     <row r="339" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A339" s="1"/>
       <c r="B339" s="109"/>
       <c r="C339" s="110"/>
-      <c r="D339" s="167" t="s">
-        <v>390</v>
-      </c>
-      <c r="E339" s="158" t="s">
-        <v>393</v>
-      </c>
-      <c r="F339" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G339" s="190">
-        <v>44281</v>
-      </c>
-      <c r="H339" s="204">
-        <v>44557</v>
+      <c r="D339" s="166" t="s">
+        <v>391</v>
+      </c>
+      <c r="E339" s="157" t="s">
+        <v>392</v>
+      </c>
+      <c r="F339" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G339" s="188">
+        <v>44957</v>
+      </c>
+      <c r="H339" s="203">
+        <v>42982</v>
       </c>
       <c r="I339" s="174"/>
     </row>
-    <row r="340" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A340" s="1"/>
       <c r="B340" s="109"/>
       <c r="C340" s="110"/>
       <c r="D340" s="167" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E340" s="158" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="F340" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G340" s="190">
-        <v>43257</v>
+        <v>44281</v>
       </c>
       <c r="H340" s="204">
-        <v>43257</v>
+        <v>44557</v>
       </c>
       <c r="I340" s="174"/>
     </row>
@@ -10679,63 +10705,73 @@
       <c r="B341" s="109"/>
       <c r="C341" s="110"/>
       <c r="D341" s="167" t="s">
-        <v>285</v>
+        <v>394</v>
       </c>
       <c r="E341" s="158" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F341" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G341" s="190">
-        <v>44949</v>
+        <v>43257</v>
       </c>
       <c r="H341" s="204">
-        <v>44949</v>
+        <v>43257</v>
       </c>
       <c r="I341" s="174"/>
     </row>
-    <row r="342" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A342" s="1"/>
       <c r="B342" s="109"/>
       <c r="C342" s="110"/>
-      <c r="D342" s="167"/>
-      <c r="E342" s="158"/>
-      <c r="F342" s="151"/>
-      <c r="G342" s="190"/>
-      <c r="H342" s="204"/>
+      <c r="D342" s="167" t="s">
+        <v>285</v>
+      </c>
+      <c r="E342" s="158" t="s">
+        <v>396</v>
+      </c>
+      <c r="F342" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G342" s="190">
+        <v>44949</v>
+      </c>
+      <c r="H342" s="204">
+        <v>44949</v>
+      </c>
       <c r="I342" s="174"/>
     </row>
-    <row r="343" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A343" s="1"/>
       <c r="B343" s="109"/>
       <c r="C343" s="110"/>
-      <c r="D343" s="167" t="s">
-        <v>389</v>
-      </c>
-      <c r="E343" s="158" t="s">
-        <v>397</v>
-      </c>
-      <c r="F343" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G343" s="190">
-        <v>44957</v>
-      </c>
-      <c r="H343" s="204">
-        <v>44957</v>
-      </c>
+      <c r="D343" s="167"/>
+      <c r="E343" s="158"/>
+      <c r="F343" s="151"/>
+      <c r="G343" s="190"/>
+      <c r="H343" s="204"/>
       <c r="I343" s="174"/>
     </row>
-    <row r="344" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A344" s="1"/>
       <c r="B344" s="109"/>
       <c r="C344" s="110"/>
-      <c r="D344" s="165"/>
-      <c r="E344" s="159"/>
-      <c r="F344" s="148"/>
-      <c r="G344" s="186"/>
-      <c r="H344" s="201"/>
+      <c r="D344" s="167" t="s">
+        <v>389</v>
+      </c>
+      <c r="E344" s="158" t="s">
+        <v>397</v>
+      </c>
+      <c r="F344" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G344" s="190">
+        <v>44957</v>
+      </c>
+      <c r="H344" s="204">
+        <v>44957</v>
+      </c>
       <c r="I344" s="174"/>
     </row>
     <row r="345" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -10743,99 +10779,97 @@
       <c r="B345" s="109"/>
       <c r="C345" s="110"/>
       <c r="D345" s="165"/>
-      <c r="E345" s="155"/>
+      <c r="E345" s="159"/>
       <c r="F345" s="148"/>
       <c r="G345" s="186"/>
       <c r="H345" s="201"/>
       <c r="I345" s="174"/>
     </row>
-    <row r="346" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A346" s="1"/>
       <c r="B346" s="109"/>
       <c r="C346" s="110"/>
-      <c r="D346" s="144"/>
-      <c r="E346" s="156"/>
-      <c r="F346" s="149"/>
-      <c r="G346" s="187"/>
-      <c r="H346" s="202"/>
-      <c r="I346" s="175"/>
-    </row>
-    <row r="347" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D346" s="165"/>
+      <c r="E346" s="155"/>
+      <c r="F346" s="148"/>
+      <c r="G346" s="186"/>
+      <c r="H346" s="201"/>
+      <c r="I346" s="174"/>
+    </row>
+    <row r="347" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A347" s="1"/>
       <c r="B347" s="109"/>
       <c r="C347" s="110"/>
-      <c r="D347" s="166" t="s">
-        <v>329</v>
-      </c>
-      <c r="E347" s="162" t="s">
-        <v>330</v>
-      </c>
-      <c r="F347" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G347" s="188">
-        <v>44893</v>
-      </c>
-      <c r="H347" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I347" s="171" t="s">
-        <v>730</v>
-      </c>
+      <c r="D347" s="144"/>
+      <c r="E347" s="156"/>
+      <c r="F347" s="149"/>
+      <c r="G347" s="187"/>
+      <c r="H347" s="202"/>
+      <c r="I347" s="175"/>
     </row>
     <row r="348" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A348" s="1"/>
       <c r="B348" s="109"/>
       <c r="C348" s="110"/>
-      <c r="D348" s="167" t="s">
-        <v>855</v>
-      </c>
-      <c r="E348" s="158" t="s">
-        <v>856</v>
-      </c>
-      <c r="F348" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G348" s="190">
-        <v>44986</v>
-      </c>
-      <c r="H348" s="204">
-        <v>44951</v>
-      </c>
-      <c r="I348" s="183" t="s">
+      <c r="D348" s="166" t="s">
+        <v>329</v>
+      </c>
+      <c r="E348" s="162" t="s">
+        <v>330</v>
+      </c>
+      <c r="F348" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G348" s="188">
+        <v>44893</v>
+      </c>
+      <c r="H348" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I348" s="171" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="349" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A349" s="1"/>
       <c r="B349" s="109"/>
       <c r="C349" s="110"/>
-      <c r="D349" s="165"/>
-      <c r="E349" s="155"/>
-      <c r="F349" s="148"/>
-      <c r="G349" s="186"/>
-      <c r="H349" s="201"/>
-      <c r="I349" s="174"/>
-    </row>
-    <row r="350" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A350" s="136"/>
-      <c r="B350" s="208" t="s">
+      <c r="D349" s="167" t="s">
+        <v>855</v>
+      </c>
+      <c r="E349" s="158" t="s">
+        <v>856</v>
+      </c>
+      <c r="F349" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G349" s="190">
+        <v>44986</v>
+      </c>
+      <c r="H349" s="204">
+        <v>44951</v>
+      </c>
+      <c r="I349" s="183" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="350" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A350" s="1"/>
+      <c r="B350" s="109"/>
+      <c r="C350" s="110"/>
+      <c r="D350" s="165"/>
+      <c r="E350" s="155"/>
+      <c r="F350" s="148"/>
+      <c r="G350" s="186"/>
+      <c r="H350" s="201"/>
+      <c r="I350" s="174"/>
+    </row>
+    <row r="351" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A351" s="136"/>
+      <c r="B351" s="208" t="s">
         <v>142</v>
       </c>
-      <c r="C350" s="134"/>
-      <c r="D350" s="135"/>
-      <c r="E350" s="154"/>
-      <c r="F350" s="147"/>
-      <c r="G350" s="185"/>
-      <c r="H350" s="200"/>
-      <c r="I350" s="173"/>
-    </row>
-    <row r="351" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A351" s="136"/>
-      <c r="B351" s="208"/>
-      <c r="C351" s="209" t="s">
-        <v>160</v>
-      </c>
+      <c r="C351" s="134"/>
       <c r="D351" s="135"/>
       <c r="E351" s="154"/>
       <c r="F351" s="147"/>
@@ -10843,21 +10877,23 @@
       <c r="H351" s="200"/>
       <c r="I351" s="173"/>
     </row>
-    <row r="352" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A352" s="1"/>
-      <c r="B352" s="109"/>
-      <c r="C352" s="209"/>
-      <c r="D352" s="165"/>
-      <c r="E352" s="155"/>
-      <c r="F352" s="148"/>
-      <c r="G352" s="186"/>
-      <c r="H352" s="201"/>
-      <c r="I352" s="174"/>
+    <row r="352" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A352" s="136"/>
+      <c r="B352" s="208"/>
+      <c r="C352" s="209" t="s">
+        <v>160</v>
+      </c>
+      <c r="D352" s="135"/>
+      <c r="E352" s="154"/>
+      <c r="F352" s="147"/>
+      <c r="G352" s="185"/>
+      <c r="H352" s="200"/>
+      <c r="I352" s="173"/>
     </row>
     <row r="353" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A353" s="1"/>
       <c r="B353" s="109"/>
-      <c r="C353" s="110"/>
+      <c r="C353" s="209"/>
       <c r="D353" s="165"/>
       <c r="E353" s="155"/>
       <c r="F353" s="148"/>
@@ -10865,25 +10901,23 @@
       <c r="H353" s="201"/>
       <c r="I353" s="174"/>
     </row>
-    <row r="354" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A354" s="136"/>
-      <c r="B354" s="208" t="s">
+    <row r="354" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A354" s="1"/>
+      <c r="B354" s="109"/>
+      <c r="C354" s="110"/>
+      <c r="D354" s="165"/>
+      <c r="E354" s="155"/>
+      <c r="F354" s="148"/>
+      <c r="G354" s="186"/>
+      <c r="H354" s="201"/>
+      <c r="I354" s="174"/>
+    </row>
+    <row r="355" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A355" s="136"/>
+      <c r="B355" s="208" t="s">
         <v>143</v>
       </c>
-      <c r="C354" s="134"/>
-      <c r="D354" s="135"/>
-      <c r="E354" s="154"/>
-      <c r="F354" s="147"/>
-      <c r="G354" s="185"/>
-      <c r="H354" s="200"/>
-      <c r="I354" s="173"/>
-    </row>
-    <row r="355" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A355" s="136"/>
-      <c r="B355" s="208"/>
-      <c r="C355" s="209" t="s">
-        <v>148</v>
-      </c>
+      <c r="C355" s="134"/>
       <c r="D355" s="135"/>
       <c r="E355" s="154"/>
       <c r="F355" s="147"/>
@@ -10891,21 +10925,23 @@
       <c r="H355" s="200"/>
       <c r="I355" s="173"/>
     </row>
-    <row r="356" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A356" s="1"/>
-      <c r="B356" s="109"/>
-      <c r="C356" s="209"/>
-      <c r="D356" s="165"/>
-      <c r="E356" s="155"/>
-      <c r="F356" s="148"/>
-      <c r="G356" s="186"/>
-      <c r="H356" s="201"/>
-      <c r="I356" s="174"/>
+    <row r="356" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A356" s="136"/>
+      <c r="B356" s="208"/>
+      <c r="C356" s="209" t="s">
+        <v>148</v>
+      </c>
+      <c r="D356" s="135"/>
+      <c r="E356" s="154"/>
+      <c r="F356" s="147"/>
+      <c r="G356" s="185"/>
+      <c r="H356" s="200"/>
+      <c r="I356" s="173"/>
     </row>
     <row r="357" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A357" s="1"/>
       <c r="B357" s="109"/>
-      <c r="C357" s="110"/>
+      <c r="C357" s="209"/>
       <c r="D357" s="165"/>
       <c r="E357" s="155"/>
       <c r="F357" s="148"/>
@@ -10916,31 +10952,31 @@
     <row r="358" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A358" s="1"/>
       <c r="B358" s="109"/>
-      <c r="C358" s="209" t="s">
-        <v>149</v>
-      </c>
-      <c r="D358" s="135"/>
-      <c r="E358" s="154"/>
-      <c r="F358" s="147"/>
-      <c r="G358" s="185"/>
-      <c r="H358" s="200"/>
-      <c r="I358" s="173"/>
+      <c r="C358" s="110"/>
+      <c r="D358" s="165"/>
+      <c r="E358" s="155"/>
+      <c r="F358" s="148"/>
+      <c r="G358" s="186"/>
+      <c r="H358" s="201"/>
+      <c r="I358" s="174"/>
     </row>
     <row r="359" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A359" s="1"/>
       <c r="B359" s="109"/>
-      <c r="C359" s="209"/>
-      <c r="D359" s="165"/>
-      <c r="E359" s="155"/>
-      <c r="F359" s="148"/>
-      <c r="G359" s="186"/>
-      <c r="H359" s="201"/>
-      <c r="I359" s="174"/>
+      <c r="C359" s="209" t="s">
+        <v>149</v>
+      </c>
+      <c r="D359" s="135"/>
+      <c r="E359" s="154"/>
+      <c r="F359" s="147"/>
+      <c r="G359" s="185"/>
+      <c r="H359" s="200"/>
+      <c r="I359" s="173"/>
     </row>
     <row r="360" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A360" s="1"/>
       <c r="B360" s="109"/>
-      <c r="C360" s="110"/>
+      <c r="C360" s="209"/>
       <c r="D360" s="165"/>
       <c r="E360" s="155"/>
       <c r="F360" s="148"/>
@@ -10951,31 +10987,31 @@
     <row r="361" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A361" s="1"/>
       <c r="B361" s="109"/>
-      <c r="C361" s="209" t="s">
-        <v>150</v>
-      </c>
-      <c r="D361" s="135"/>
-      <c r="E361" s="154"/>
-      <c r="F361" s="147"/>
-      <c r="G361" s="185"/>
-      <c r="H361" s="200"/>
-      <c r="I361" s="173"/>
+      <c r="C361" s="110"/>
+      <c r="D361" s="165"/>
+      <c r="E361" s="155"/>
+      <c r="F361" s="148"/>
+      <c r="G361" s="186"/>
+      <c r="H361" s="201"/>
+      <c r="I361" s="174"/>
     </row>
     <row r="362" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A362" s="1"/>
       <c r="B362" s="109"/>
-      <c r="C362" s="209"/>
-      <c r="D362" s="165"/>
-      <c r="E362" s="155"/>
-      <c r="F362" s="148"/>
-      <c r="G362" s="186"/>
-      <c r="H362" s="201"/>
-      <c r="I362" s="174"/>
+      <c r="C362" s="209" t="s">
+        <v>150</v>
+      </c>
+      <c r="D362" s="135"/>
+      <c r="E362" s="154"/>
+      <c r="F362" s="147"/>
+      <c r="G362" s="185"/>
+      <c r="H362" s="200"/>
+      <c r="I362" s="173"/>
     </row>
     <row r="363" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
       <c r="B363" s="109"/>
-      <c r="C363" s="110"/>
+      <c r="C363" s="209"/>
       <c r="D363" s="165"/>
       <c r="E363" s="155"/>
       <c r="F363" s="148"/>
@@ -10986,31 +11022,31 @@
     <row r="364" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="B364" s="109"/>
-      <c r="C364" s="209" t="s">
-        <v>151</v>
-      </c>
-      <c r="D364" s="135"/>
-      <c r="E364" s="154"/>
-      <c r="F364" s="147"/>
-      <c r="G364" s="185"/>
-      <c r="H364" s="200"/>
-      <c r="I364" s="173"/>
+      <c r="C364" s="110"/>
+      <c r="D364" s="165"/>
+      <c r="E364" s="155"/>
+      <c r="F364" s="148"/>
+      <c r="G364" s="186"/>
+      <c r="H364" s="201"/>
+      <c r="I364" s="174"/>
     </row>
     <row r="365" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A365" s="1"/>
       <c r="B365" s="109"/>
-      <c r="C365" s="209"/>
-      <c r="D365" s="165"/>
-      <c r="E365" s="155"/>
-      <c r="F365" s="148"/>
-      <c r="G365" s="186"/>
-      <c r="H365" s="201"/>
-      <c r="I365" s="174"/>
+      <c r="C365" s="209" t="s">
+        <v>151</v>
+      </c>
+      <c r="D365" s="135"/>
+      <c r="E365" s="154"/>
+      <c r="F365" s="147"/>
+      <c r="G365" s="185"/>
+      <c r="H365" s="200"/>
+      <c r="I365" s="173"/>
     </row>
     <row r="366" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A366" s="1"/>
       <c r="B366" s="109"/>
-      <c r="C366" s="110"/>
+      <c r="C366" s="209"/>
       <c r="D366" s="165"/>
       <c r="E366" s="155"/>
       <c r="F366" s="148"/>
@@ -11021,59 +11057,47 @@
     <row r="367" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A367" s="1"/>
       <c r="B367" s="109"/>
-      <c r="C367" s="209" t="s">
-        <v>152</v>
-      </c>
-      <c r="D367" s="135"/>
-      <c r="E367" s="154"/>
-      <c r="F367" s="147"/>
-      <c r="G367" s="185"/>
-      <c r="H367" s="200"/>
-      <c r="I367" s="173"/>
+      <c r="C367" s="110"/>
+      <c r="D367" s="165"/>
+      <c r="E367" s="155"/>
+      <c r="F367" s="148"/>
+      <c r="G367" s="186"/>
+      <c r="H367" s="201"/>
+      <c r="I367" s="174"/>
     </row>
     <row r="368" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
       <c r="B368" s="109"/>
-      <c r="C368" s="209"/>
-      <c r="D368" s="166" t="s">
-        <v>763</v>
-      </c>
-      <c r="E368" s="162" t="s">
-        <v>765</v>
-      </c>
-      <c r="F368" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G368" s="188">
-        <v>44721</v>
-      </c>
-      <c r="H368" s="204">
-        <v>44698</v>
-      </c>
-      <c r="I368" s="176" t="s">
-        <v>762</v>
-      </c>
+      <c r="C368" s="209" t="s">
+        <v>152</v>
+      </c>
+      <c r="D368" s="135"/>
+      <c r="E368" s="154"/>
+      <c r="F368" s="147"/>
+      <c r="G368" s="185"/>
+      <c r="H368" s="200"/>
+      <c r="I368" s="173"/>
     </row>
     <row r="369" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A369" s="1"/>
       <c r="B369" s="109"/>
-      <c r="C369" s="110"/>
-      <c r="D369" s="167" t="s">
-        <v>764</v>
-      </c>
-      <c r="E369" s="160" t="s">
-        <v>766</v>
-      </c>
-      <c r="F369" s="151" t="s">
+      <c r="C369" s="209"/>
+      <c r="D369" s="166" t="s">
+        <v>763</v>
+      </c>
+      <c r="E369" s="162" t="s">
+        <v>765</v>
+      </c>
+      <c r="F369" s="150" t="s">
         <v>267</v>
       </c>
-      <c r="G369" s="190">
+      <c r="G369" s="188">
         <v>44721</v>
       </c>
       <c r="H369" s="204">
         <v>44698</v>
       </c>
-      <c r="I369" s="177" t="s">
+      <c r="I369" s="176" t="s">
         <v>762</v>
       </c>
     </row>
@@ -11082,19 +11106,19 @@
       <c r="B370" s="109"/>
       <c r="C370" s="110"/>
       <c r="D370" s="167" t="s">
-        <v>758</v>
+        <v>764</v>
       </c>
       <c r="E370" s="160" t="s">
-        <v>760</v>
+        <v>766</v>
       </c>
       <c r="F370" s="151" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G370" s="190">
-        <v>44644</v>
+        <v>44721</v>
       </c>
       <c r="H370" s="204">
-        <v>44622</v>
+        <v>44698</v>
       </c>
       <c r="I370" s="177" t="s">
         <v>762</v>
@@ -11105,10 +11129,10 @@
       <c r="B371" s="109"/>
       <c r="C371" s="110"/>
       <c r="D371" s="167" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E371" s="160" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F371" s="151" t="s">
         <v>281</v>
@@ -11128,19 +11152,19 @@
       <c r="B372" s="109"/>
       <c r="C372" s="110"/>
       <c r="D372" s="167" t="s">
-        <v>767</v>
+        <v>759</v>
       </c>
       <c r="E372" s="160" t="s">
-        <v>769</v>
+        <v>761</v>
       </c>
       <c r="F372" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G372" s="190">
-        <v>44755</v>
+        <v>44644</v>
       </c>
       <c r="H372" s="204">
-        <v>44755</v>
+        <v>44622</v>
       </c>
       <c r="I372" s="177" t="s">
         <v>762</v>
@@ -11151,19 +11175,19 @@
       <c r="B373" s="109"/>
       <c r="C373" s="110"/>
       <c r="D373" s="167" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="E373" s="160" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F373" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G373" s="190">
-        <v>44756</v>
+        <v>44755</v>
       </c>
       <c r="H373" s="204">
-        <v>44756</v>
+        <v>44755</v>
       </c>
       <c r="I373" s="177" t="s">
         <v>762</v>
@@ -11174,19 +11198,19 @@
       <c r="B374" s="109"/>
       <c r="C374" s="110"/>
       <c r="D374" s="167" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
       <c r="E374" s="160" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
       <c r="F374" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G374" s="190">
-        <v>44755</v>
+        <v>44756</v>
       </c>
       <c r="H374" s="204">
-        <v>44755</v>
+        <v>44756</v>
       </c>
       <c r="I374" s="177" t="s">
         <v>762</v>
@@ -11197,10 +11221,10 @@
       <c r="B375" s="109"/>
       <c r="C375" s="110"/>
       <c r="D375" s="167" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="E375" s="160" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F375" s="151" t="s">
         <v>232</v>
@@ -11219,12 +11243,24 @@
       <c r="A376" s="1"/>
       <c r="B376" s="109"/>
       <c r="C376" s="110"/>
-      <c r="D376" s="167"/>
-      <c r="E376" s="160"/>
-      <c r="F376" s="151"/>
-      <c r="G376" s="190"/>
-      <c r="H376" s="204"/>
-      <c r="I376" s="177"/>
+      <c r="D376" s="167" t="s">
+        <v>772</v>
+      </c>
+      <c r="E376" s="160" t="s">
+        <v>774</v>
+      </c>
+      <c r="F376" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G376" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H376" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I376" s="177" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="377" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A377" s="1"/>
@@ -11285,19 +11321,11 @@
       <c r="A382" s="1"/>
       <c r="B382" s="109"/>
       <c r="C382" s="110"/>
-      <c r="D382" s="167" t="s">
-        <v>776</v>
-      </c>
+      <c r="D382" s="167"/>
       <c r="E382" s="160"/>
-      <c r="F382" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G382" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H382" s="204">
-        <v>44984</v>
-      </c>
+      <c r="F382" s="151"/>
+      <c r="G382" s="190"/>
+      <c r="H382" s="204"/>
       <c r="I382" s="177"/>
     </row>
     <row r="383" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -11305,7 +11333,7 @@
       <c r="B383" s="109"/>
       <c r="C383" s="110"/>
       <c r="D383" s="167" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="E383" s="160"/>
       <c r="F383" s="151" t="s">
@@ -11323,11 +11351,19 @@
       <c r="A384" s="1"/>
       <c r="B384" s="109"/>
       <c r="C384" s="110"/>
-      <c r="D384" s="167"/>
+      <c r="D384" s="167" t="s">
+        <v>775</v>
+      </c>
       <c r="E384" s="160"/>
-      <c r="F384" s="151"/>
-      <c r="G384" s="190"/>
-      <c r="H384" s="204"/>
+      <c r="F384" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G384" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H384" s="204">
+        <v>44984</v>
+      </c>
       <c r="I384" s="177"/>
     </row>
     <row r="385" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -11367,41 +11403,41 @@
       <c r="A388" s="1"/>
       <c r="B388" s="109"/>
       <c r="C388" s="110"/>
-      <c r="D388" s="165"/>
-      <c r="E388" s="155"/>
-      <c r="F388" s="148"/>
-      <c r="G388" s="186"/>
-      <c r="H388" s="201"/>
-      <c r="I388" s="174"/>
+      <c r="D388" s="167"/>
+      <c r="E388" s="160"/>
+      <c r="F388" s="151"/>
+      <c r="G388" s="190"/>
+      <c r="H388" s="204"/>
+      <c r="I388" s="177"/>
     </row>
     <row r="389" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A389" s="1"/>
       <c r="B389" s="109"/>
-      <c r="C389" s="209" t="s">
-        <v>153</v>
-      </c>
-      <c r="D389" s="135"/>
-      <c r="E389" s="154"/>
-      <c r="F389" s="147"/>
-      <c r="G389" s="185"/>
-      <c r="H389" s="200"/>
-      <c r="I389" s="173"/>
+      <c r="C389" s="110"/>
+      <c r="D389" s="165"/>
+      <c r="E389" s="155"/>
+      <c r="F389" s="148"/>
+      <c r="G389" s="186"/>
+      <c r="H389" s="201"/>
+      <c r="I389" s="174"/>
     </row>
     <row r="390" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A390" s="1"/>
       <c r="B390" s="109"/>
-      <c r="C390" s="209"/>
-      <c r="D390" s="165"/>
-      <c r="E390" s="155"/>
-      <c r="F390" s="148"/>
-      <c r="G390" s="186"/>
-      <c r="H390" s="201"/>
-      <c r="I390" s="174"/>
+      <c r="C390" s="209" t="s">
+        <v>153</v>
+      </c>
+      <c r="D390" s="135"/>
+      <c r="E390" s="154"/>
+      <c r="F390" s="147"/>
+      <c r="G390" s="185"/>
+      <c r="H390" s="200"/>
+      <c r="I390" s="173"/>
     </row>
     <row r="391" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A391" s="1"/>
       <c r="B391" s="109"/>
-      <c r="C391" s="110"/>
+      <c r="C391" s="209"/>
       <c r="D391" s="165"/>
       <c r="E391" s="155"/>
       <c r="F391" s="148"/>
@@ -11412,31 +11448,31 @@
     <row r="392" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A392" s="1"/>
       <c r="B392" s="109"/>
-      <c r="C392" s="209" t="s">
-        <v>154</v>
-      </c>
-      <c r="D392" s="135"/>
-      <c r="E392" s="154"/>
-      <c r="F392" s="147"/>
-      <c r="G392" s="185"/>
-      <c r="H392" s="200"/>
-      <c r="I392" s="173"/>
+      <c r="C392" s="110"/>
+      <c r="D392" s="165"/>
+      <c r="E392" s="155"/>
+      <c r="F392" s="148"/>
+      <c r="G392" s="186"/>
+      <c r="H392" s="201"/>
+      <c r="I392" s="174"/>
     </row>
     <row r="393" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A393" s="1"/>
       <c r="B393" s="109"/>
-      <c r="C393" s="209"/>
-      <c r="D393" s="165"/>
-      <c r="E393" s="155"/>
-      <c r="F393" s="148"/>
-      <c r="G393" s="186"/>
-      <c r="H393" s="201"/>
-      <c r="I393" s="174"/>
+      <c r="C393" s="209" t="s">
+        <v>154</v>
+      </c>
+      <c r="D393" s="135"/>
+      <c r="E393" s="154"/>
+      <c r="F393" s="147"/>
+      <c r="G393" s="185"/>
+      <c r="H393" s="200"/>
+      <c r="I393" s="173"/>
     </row>
     <row r="394" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A394" s="1"/>
       <c r="B394" s="109"/>
-      <c r="C394" s="110"/>
+      <c r="C394" s="209"/>
       <c r="D394" s="165"/>
       <c r="E394" s="155"/>
       <c r="F394" s="148"/>
@@ -11447,31 +11483,31 @@
     <row r="395" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A395" s="1"/>
       <c r="B395" s="109"/>
-      <c r="C395" s="209" t="s">
-        <v>155</v>
-      </c>
-      <c r="D395" s="135"/>
-      <c r="E395" s="154"/>
-      <c r="F395" s="147"/>
-      <c r="G395" s="185"/>
-      <c r="H395" s="200"/>
-      <c r="I395" s="173"/>
+      <c r="C395" s="110"/>
+      <c r="D395" s="165"/>
+      <c r="E395" s="155"/>
+      <c r="F395" s="148"/>
+      <c r="G395" s="186"/>
+      <c r="H395" s="201"/>
+      <c r="I395" s="174"/>
     </row>
     <row r="396" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A396" s="1"/>
       <c r="B396" s="109"/>
-      <c r="C396" s="209"/>
-      <c r="D396" s="165"/>
-      <c r="E396" s="155"/>
-      <c r="F396" s="148"/>
-      <c r="G396" s="186"/>
-      <c r="H396" s="201"/>
-      <c r="I396" s="174"/>
+      <c r="C396" s="209" t="s">
+        <v>155</v>
+      </c>
+      <c r="D396" s="135"/>
+      <c r="E396" s="154"/>
+      <c r="F396" s="147"/>
+      <c r="G396" s="185"/>
+      <c r="H396" s="200"/>
+      <c r="I396" s="173"/>
     </row>
     <row r="397" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A397" s="1"/>
       <c r="B397" s="109"/>
-      <c r="C397" s="110"/>
+      <c r="C397" s="209"/>
       <c r="D397" s="165"/>
       <c r="E397" s="155"/>
       <c r="F397" s="148"/>
@@ -11482,31 +11518,31 @@
     <row r="398" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A398" s="1"/>
       <c r="B398" s="109"/>
-      <c r="C398" s="209" t="s">
-        <v>156</v>
-      </c>
-      <c r="D398" s="135"/>
-      <c r="E398" s="154"/>
-      <c r="F398" s="147"/>
-      <c r="G398" s="185"/>
-      <c r="H398" s="200"/>
-      <c r="I398" s="173"/>
+      <c r="C398" s="110"/>
+      <c r="D398" s="165"/>
+      <c r="E398" s="155"/>
+      <c r="F398" s="148"/>
+      <c r="G398" s="186"/>
+      <c r="H398" s="201"/>
+      <c r="I398" s="174"/>
     </row>
     <row r="399" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A399" s="1"/>
       <c r="B399" s="109"/>
-      <c r="C399" s="209"/>
-      <c r="D399" s="165"/>
-      <c r="E399" s="155"/>
-      <c r="F399" s="148"/>
-      <c r="G399" s="186"/>
-      <c r="H399" s="201"/>
-      <c r="I399" s="174"/>
+      <c r="C399" s="209" t="s">
+        <v>156</v>
+      </c>
+      <c r="D399" s="135"/>
+      <c r="E399" s="154"/>
+      <c r="F399" s="147"/>
+      <c r="G399" s="185"/>
+      <c r="H399" s="200"/>
+      <c r="I399" s="173"/>
     </row>
     <row r="400" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A400" s="1"/>
       <c r="B400" s="109"/>
-      <c r="C400" s="110"/>
+      <c r="C400" s="209"/>
       <c r="D400" s="165"/>
       <c r="E400" s="155"/>
       <c r="F400" s="148"/>
@@ -11517,31 +11553,31 @@
     <row r="401" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A401" s="1"/>
       <c r="B401" s="109"/>
-      <c r="C401" s="209" t="s">
-        <v>157</v>
-      </c>
-      <c r="D401" s="135"/>
-      <c r="E401" s="154"/>
-      <c r="F401" s="147"/>
-      <c r="G401" s="185"/>
-      <c r="H401" s="200"/>
-      <c r="I401" s="173"/>
+      <c r="C401" s="110"/>
+      <c r="D401" s="165"/>
+      <c r="E401" s="155"/>
+      <c r="F401" s="148"/>
+      <c r="G401" s="186"/>
+      <c r="H401" s="201"/>
+      <c r="I401" s="174"/>
     </row>
     <row r="402" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A402" s="1"/>
       <c r="B402" s="109"/>
-      <c r="C402" s="209"/>
-      <c r="D402" s="165"/>
-      <c r="E402" s="155"/>
-      <c r="F402" s="148"/>
-      <c r="G402" s="186"/>
-      <c r="H402" s="201"/>
-      <c r="I402" s="174"/>
+      <c r="C402" s="209" t="s">
+        <v>157</v>
+      </c>
+      <c r="D402" s="135"/>
+      <c r="E402" s="154"/>
+      <c r="F402" s="147"/>
+      <c r="G402" s="185"/>
+      <c r="H402" s="200"/>
+      <c r="I402" s="173"/>
     </row>
     <row r="403" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A403" s="1"/>
       <c r="B403" s="109"/>
-      <c r="C403" s="110"/>
+      <c r="C403" s="209"/>
       <c r="D403" s="165"/>
       <c r="E403" s="155"/>
       <c r="F403" s="148"/>
@@ -11552,59 +11588,47 @@
     <row r="404" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A404" s="1"/>
       <c r="B404" s="109"/>
-      <c r="C404" s="209" t="s">
-        <v>158</v>
-      </c>
-      <c r="D404" s="135"/>
-      <c r="E404" s="154"/>
-      <c r="F404" s="147"/>
-      <c r="G404" s="185"/>
-      <c r="H404" s="200"/>
-      <c r="I404" s="173"/>
+      <c r="C404" s="110"/>
+      <c r="D404" s="165"/>
+      <c r="E404" s="155"/>
+      <c r="F404" s="148"/>
+      <c r="G404" s="186"/>
+      <c r="H404" s="201"/>
+      <c r="I404" s="174"/>
     </row>
     <row r="405" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A405" s="1"/>
       <c r="B405" s="109"/>
-      <c r="C405" s="209"/>
-      <c r="D405" s="166" t="s">
-        <v>468</v>
-      </c>
-      <c r="E405" s="162" t="s">
-        <v>469</v>
-      </c>
-      <c r="F405" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G405" s="188">
-        <v>44663</v>
-      </c>
-      <c r="H405" s="203">
-        <v>44663</v>
-      </c>
-      <c r="I405" s="198" t="s">
-        <v>762</v>
-      </c>
+      <c r="C405" s="209" t="s">
+        <v>158</v>
+      </c>
+      <c r="D405" s="135"/>
+      <c r="E405" s="154"/>
+      <c r="F405" s="147"/>
+      <c r="G405" s="185"/>
+      <c r="H405" s="200"/>
+      <c r="I405" s="173"/>
     </row>
     <row r="406" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A406" s="1"/>
       <c r="B406" s="109"/>
-      <c r="C406" s="110"/>
-      <c r="D406" s="167" t="s">
-        <v>470</v>
-      </c>
-      <c r="E406" s="160" t="s">
-        <v>471</v>
-      </c>
-      <c r="F406" s="151" t="s">
+      <c r="C406" s="209"/>
+      <c r="D406" s="166" t="s">
+        <v>468</v>
+      </c>
+      <c r="E406" s="162" t="s">
+        <v>469</v>
+      </c>
+      <c r="F406" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="G406" s="190">
+      <c r="G406" s="188">
         <v>44663</v>
       </c>
-      <c r="H406" s="204">
+      <c r="H406" s="203">
         <v>44663</v>
       </c>
-      <c r="I406" s="199" t="s">
+      <c r="I406" s="198" t="s">
         <v>762</v>
       </c>
     </row>
@@ -11613,19 +11637,19 @@
       <c r="B407" s="109"/>
       <c r="C407" s="110"/>
       <c r="D407" s="167" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="E407" s="160" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F407" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G407" s="190">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="H407" s="204">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="I407" s="199" t="s">
         <v>762</v>
@@ -11636,10 +11660,10 @@
       <c r="B408" s="109"/>
       <c r="C408" s="110"/>
       <c r="D408" s="167" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E408" s="160" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F408" s="151" t="s">
         <v>232</v>
@@ -11659,16 +11683,16 @@
       <c r="B409" s="109"/>
       <c r="C409" s="110"/>
       <c r="D409" s="167" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E409" s="160" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F409" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G409" s="190">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H409" s="204">
         <v>44630</v>
@@ -11682,10 +11706,10 @@
       <c r="B410" s="109"/>
       <c r="C410" s="110"/>
       <c r="D410" s="167" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E410" s="160" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F410" s="151" t="s">
         <v>281</v>
@@ -11705,19 +11729,19 @@
       <c r="B411" s="109"/>
       <c r="C411" s="110"/>
       <c r="D411" s="167" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E411" s="160" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F411" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G411" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H411" s="204">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I411" s="199" t="s">
         <v>762</v>
@@ -11728,10 +11752,10 @@
       <c r="B412" s="109"/>
       <c r="C412" s="110"/>
       <c r="D412" s="167" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="E412" s="160" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F412" s="151" t="s">
         <v>256</v>
@@ -11751,19 +11775,19 @@
       <c r="B413" s="109"/>
       <c r="C413" s="110"/>
       <c r="D413" s="167" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E413" s="160" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F413" s="151" t="s">
-        <v>461</v>
+        <v>256</v>
       </c>
       <c r="G413" s="190">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H413" s="204">
-        <v>44622</v>
+        <v>44824</v>
       </c>
       <c r="I413" s="199" t="s">
         <v>762</v>
@@ -11774,10 +11798,10 @@
       <c r="B414" s="109"/>
       <c r="C414" s="110"/>
       <c r="D414" s="167" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="E414" s="160" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F414" s="151" t="s">
         <v>461</v>
@@ -11786,7 +11810,7 @@
         <v>44733</v>
       </c>
       <c r="H414" s="204">
-        <v>44621</v>
+        <v>44622</v>
       </c>
       <c r="I414" s="199" t="s">
         <v>762</v>
@@ -11797,19 +11821,19 @@
       <c r="B415" s="109"/>
       <c r="C415" s="110"/>
       <c r="D415" s="167" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E415" s="160" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F415" s="151" t="s">
         <v>461</v>
       </c>
       <c r="G415" s="190">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H415" s="204">
-        <v>44732</v>
+        <v>44621</v>
       </c>
       <c r="I415" s="199" t="s">
         <v>762</v>
@@ -11820,10 +11844,10 @@
       <c r="B416" s="109"/>
       <c r="C416" s="110"/>
       <c r="D416" s="167" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E416" s="160" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F416" s="151" t="s">
         <v>461</v>
@@ -11843,19 +11867,19 @@
       <c r="B417" s="109"/>
       <c r="C417" s="110"/>
       <c r="D417" s="167" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="E417" s="160" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="F417" s="151" t="s">
-        <v>494</v>
+        <v>461</v>
       </c>
       <c r="G417" s="190">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H417" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I417" s="199" t="s">
         <v>762</v>
@@ -11866,10 +11890,10 @@
       <c r="B418" s="109"/>
       <c r="C418" s="110"/>
       <c r="D418" s="167" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E418" s="160" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="F418" s="151" t="s">
         <v>494</v>
@@ -11889,19 +11913,19 @@
       <c r="B419" s="109"/>
       <c r="C419" s="110"/>
       <c r="D419" s="167" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E419" s="160" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="F419" s="151" t="s">
-        <v>267</v>
+        <v>494</v>
       </c>
       <c r="G419" s="190">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H419" s="204">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="I419" s="199" t="s">
         <v>762</v>
@@ -11912,10 +11936,10 @@
       <c r="B420" s="109"/>
       <c r="C420" s="110"/>
       <c r="D420" s="167" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E420" s="160" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F420" s="151" t="s">
         <v>267</v>
@@ -11924,7 +11948,7 @@
         <v>44644</v>
       </c>
       <c r="H420" s="204">
-        <v>44621</v>
+        <v>44622</v>
       </c>
       <c r="I420" s="199" t="s">
         <v>762</v>
@@ -11935,16 +11959,16 @@
       <c r="B421" s="109"/>
       <c r="C421" s="110"/>
       <c r="D421" s="167" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E421" s="160" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F421" s="151" t="s">
-        <v>461</v>
+        <v>267</v>
       </c>
       <c r="G421" s="190">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H421" s="204">
         <v>44621</v>
@@ -11958,10 +11982,10 @@
       <c r="B422" s="109"/>
       <c r="C422" s="110"/>
       <c r="D422" s="167" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E422" s="160" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="F422" s="151" t="s">
         <v>461</v>
@@ -11981,19 +12005,19 @@
       <c r="B423" s="109"/>
       <c r="C423" s="110"/>
       <c r="D423" s="167" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="E423" s="160" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F423" s="151" t="s">
-        <v>267</v>
+        <v>461</v>
       </c>
       <c r="G423" s="190">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H423" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I423" s="199" t="s">
         <v>762</v>
@@ -12004,10 +12028,10 @@
       <c r="B424" s="109"/>
       <c r="C424" s="110"/>
       <c r="D424" s="167" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="E424" s="160" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F424" s="151" t="s">
         <v>267</v>
@@ -12027,19 +12051,19 @@
       <c r="B425" s="109"/>
       <c r="C425" s="110"/>
       <c r="D425" s="167" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E425" s="160" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="F425" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G425" s="190">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H425" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I425" s="199" t="s">
         <v>762</v>
@@ -12050,10 +12074,10 @@
       <c r="B426" s="109"/>
       <c r="C426" s="110"/>
       <c r="D426" s="167" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="E426" s="160" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F426" s="151" t="s">
         <v>232</v>
@@ -12073,16 +12097,16 @@
       <c r="B427" s="109"/>
       <c r="C427" s="110"/>
       <c r="D427" s="167" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="E427" s="160" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F427" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G427" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H427" s="204">
         <v>44628</v>
@@ -12096,10 +12120,10 @@
       <c r="B428" s="109"/>
       <c r="C428" s="110"/>
       <c r="D428" s="167" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E428" s="160" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="F428" s="151" t="s">
         <v>281</v>
@@ -12119,16 +12143,16 @@
       <c r="B429" s="109"/>
       <c r="C429" s="110"/>
       <c r="D429" s="167" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="E429" s="160" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="F429" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G429" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H429" s="204">
         <v>44628</v>
@@ -12142,10 +12166,10 @@
       <c r="B430" s="109"/>
       <c r="C430" s="110"/>
       <c r="D430" s="167" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E430" s="160" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F430" s="151" t="s">
         <v>232</v>
@@ -12165,16 +12189,16 @@
       <c r="B431" s="109"/>
       <c r="C431" s="110"/>
       <c r="D431" s="167" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="E431" s="160" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F431" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G431" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H431" s="204">
         <v>44628</v>
@@ -12188,10 +12212,10 @@
       <c r="B432" s="109"/>
       <c r="C432" s="110"/>
       <c r="D432" s="167" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E432" s="160" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F432" s="151" t="s">
         <v>281</v>
@@ -12211,19 +12235,19 @@
       <c r="B433" s="109"/>
       <c r="C433" s="110"/>
       <c r="D433" s="167" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="E433" s="160" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F433" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G433" s="190">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H433" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I433" s="199" t="s">
         <v>762</v>
@@ -12234,10 +12258,10 @@
       <c r="B434" s="109"/>
       <c r="C434" s="110"/>
       <c r="D434" s="167" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="E434" s="160" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F434" s="151" t="s">
         <v>232</v>
@@ -12257,19 +12281,19 @@
       <c r="B435" s="109"/>
       <c r="C435" s="110"/>
       <c r="D435" s="167" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E435" s="160" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="F435" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G435" s="190">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H435" s="204">
-        <v>44662</v>
+        <v>44617</v>
       </c>
       <c r="I435" s="199" t="s">
         <v>762</v>
@@ -12280,10 +12304,10 @@
       <c r="B436" s="109"/>
       <c r="C436" s="110"/>
       <c r="D436" s="167" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="E436" s="160" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F436" s="151" t="s">
         <v>256</v>
@@ -12302,164 +12326,166 @@
       <c r="A437" s="1"/>
       <c r="B437" s="109"/>
       <c r="C437" s="110"/>
-      <c r="D437" s="165"/>
-      <c r="E437" s="155"/>
-      <c r="F437" s="148"/>
-      <c r="G437" s="186"/>
-      <c r="H437" s="201"/>
-      <c r="I437" s="174"/>
+      <c r="D437" s="167" t="s">
+        <v>532</v>
+      </c>
+      <c r="E437" s="160" t="s">
+        <v>531</v>
+      </c>
+      <c r="F437" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G437" s="190">
+        <v>44740</v>
+      </c>
+      <c r="H437" s="204">
+        <v>44662</v>
+      </c>
+      <c r="I437" s="199" t="s">
+        <v>762</v>
+      </c>
     </row>
     <row r="438" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A438" s="1"/>
       <c r="B438" s="109"/>
-      <c r="C438" s="209" t="s">
-        <v>147</v>
-      </c>
-      <c r="D438" s="135"/>
-      <c r="E438" s="154"/>
-      <c r="F438" s="147"/>
-      <c r="G438" s="185"/>
-      <c r="H438" s="200"/>
-      <c r="I438" s="173"/>
+      <c r="C438" s="110"/>
+      <c r="D438" s="165"/>
+      <c r="E438" s="155"/>
+      <c r="F438" s="148"/>
+      <c r="G438" s="186"/>
+      <c r="H438" s="201"/>
+      <c r="I438" s="174"/>
     </row>
     <row r="439" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A439" s="1"/>
       <c r="B439" s="109"/>
-      <c r="C439" s="209"/>
-      <c r="D439" s="166" t="s">
-        <v>274</v>
-      </c>
-      <c r="E439" s="162" t="s">
-        <v>446</v>
-      </c>
-      <c r="F439" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G439" s="188">
-        <v>44167</v>
-      </c>
-      <c r="H439" s="203">
-        <v>44167</v>
-      </c>
-      <c r="I439" s="176"/>
+      <c r="C439" s="209" t="s">
+        <v>147</v>
+      </c>
+      <c r="D439" s="135"/>
+      <c r="E439" s="154"/>
+      <c r="F439" s="147"/>
+      <c r="G439" s="185"/>
+      <c r="H439" s="200"/>
+      <c r="I439" s="173"/>
     </row>
     <row r="440" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A440" s="1"/>
       <c r="B440" s="109"/>
-      <c r="C440" s="110"/>
-      <c r="D440" s="167" t="s">
-        <v>447</v>
-      </c>
-      <c r="E440" s="160" t="s">
-        <v>448</v>
-      </c>
-      <c r="F440" s="151" t="s">
-        <v>256</v>
-      </c>
-      <c r="G440" s="190">
-        <v>44575</v>
-      </c>
-      <c r="H440" s="204">
+      <c r="C440" s="209"/>
+      <c r="D440" s="166" t="s">
+        <v>274</v>
+      </c>
+      <c r="E440" s="162" t="s">
+        <v>446</v>
+      </c>
+      <c r="F440" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G440" s="188">
         <v>44167</v>
       </c>
-      <c r="I440" s="177"/>
-    </row>
-    <row r="441" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="H440" s="203">
+        <v>44167</v>
+      </c>
+      <c r="I440" s="176"/>
+    </row>
+    <row r="441" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A441" s="1"/>
       <c r="B441" s="109"/>
       <c r="C441" s="110"/>
       <c r="D441" s="167" t="s">
-        <v>450</v>
-      </c>
-      <c r="E441" s="158" t="s">
-        <v>449</v>
+        <v>447</v>
+      </c>
+      <c r="E441" s="160" t="s">
+        <v>448</v>
       </c>
       <c r="F441" s="151" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G441" s="190">
-        <v>44404</v>
+        <v>44575</v>
       </c>
       <c r="H441" s="204">
-        <v>44404</v>
+        <v>44167</v>
       </c>
       <c r="I441" s="177"/>
     </row>
-    <row r="442" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A442" s="1"/>
       <c r="B442" s="109"/>
       <c r="C442" s="110"/>
-      <c r="D442" s="165"/>
-      <c r="E442" s="155"/>
-      <c r="F442" s="148"/>
-      <c r="G442" s="186"/>
-      <c r="H442" s="201"/>
-      <c r="I442" s="174"/>
+      <c r="D442" s="167" t="s">
+        <v>450</v>
+      </c>
+      <c r="E442" s="158" t="s">
+        <v>449</v>
+      </c>
+      <c r="F442" s="151" t="s">
+        <v>281</v>
+      </c>
+      <c r="G442" s="190">
+        <v>44404</v>
+      </c>
+      <c r="H442" s="204">
+        <v>44404</v>
+      </c>
+      <c r="I442" s="177"/>
     </row>
     <row r="443" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A443" s="1"/>
       <c r="B443" s="109"/>
-      <c r="C443" s="209" t="s">
-        <v>159</v>
-      </c>
-      <c r="D443" s="135"/>
-      <c r="E443" s="154"/>
-      <c r="F443" s="147"/>
-      <c r="G443" s="185"/>
-      <c r="H443" s="200"/>
-      <c r="I443" s="173"/>
+      <c r="C443" s="110"/>
+      <c r="D443" s="165"/>
+      <c r="E443" s="155"/>
+      <c r="F443" s="148"/>
+      <c r="G443" s="186"/>
+      <c r="H443" s="201"/>
+      <c r="I443" s="174"/>
     </row>
     <row r="444" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A444" s="1"/>
       <c r="B444" s="109"/>
-      <c r="C444" s="209"/>
-      <c r="D444" s="166" t="s">
-        <v>452</v>
-      </c>
-      <c r="E444" s="162" t="s">
-        <v>451</v>
-      </c>
-      <c r="F444" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G444" s="188">
-        <v>44635</v>
-      </c>
-      <c r="H444" s="203">
-        <v>44635</v>
-      </c>
-      <c r="I444" s="176"/>
+      <c r="C444" s="209" t="s">
+        <v>159</v>
+      </c>
+      <c r="D444" s="135"/>
+      <c r="E444" s="154"/>
+      <c r="F444" s="147"/>
+      <c r="G444" s="185"/>
+      <c r="H444" s="200"/>
+      <c r="I444" s="173"/>
     </row>
     <row r="445" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A445" s="1"/>
       <c r="B445" s="109"/>
-      <c r="C445" s="110"/>
-      <c r="D445" s="167" t="s">
-        <v>454</v>
-      </c>
-      <c r="E445" s="160" t="s">
-        <v>453</v>
-      </c>
-      <c r="F445" s="151" t="s">
+      <c r="C445" s="209"/>
+      <c r="D445" s="166" t="s">
+        <v>452</v>
+      </c>
+      <c r="E445" s="162" t="s">
+        <v>451</v>
+      </c>
+      <c r="F445" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="G445" s="190">
+      <c r="G445" s="188">
         <v>44635</v>
       </c>
-      <c r="H445" s="204">
+      <c r="H445" s="203">
         <v>44635</v>
       </c>
-      <c r="I445" s="177"/>
+      <c r="I445" s="176"/>
     </row>
     <row r="446" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A446" s="1"/>
       <c r="B446" s="109"/>
       <c r="C446" s="110"/>
       <c r="D446" s="167" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E446" s="160" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F446" s="151" t="s">
         <v>232</v>
@@ -12477,10 +12503,10 @@
       <c r="B447" s="109"/>
       <c r="C447" s="110"/>
       <c r="D447" s="167" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E447" s="160" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="F447" s="151" t="s">
         <v>232</v>
@@ -12498,19 +12524,19 @@
       <c r="B448" s="109"/>
       <c r="C448" s="110"/>
       <c r="D448" s="167" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="E448" s="160" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F448" s="151" t="s">
-        <v>461</v>
+        <v>232</v>
       </c>
       <c r="G448" s="190">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H448" s="204">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="I448" s="177"/>
     </row>
@@ -12519,10 +12545,10 @@
       <c r="B449" s="109"/>
       <c r="C449" s="110"/>
       <c r="D449" s="167" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E449" s="160" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F449" s="151" t="s">
         <v>461</v>
@@ -12540,19 +12566,19 @@
       <c r="B450" s="109"/>
       <c r="C450" s="110"/>
       <c r="D450" s="167" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E450" s="160" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F450" s="151" t="s">
-        <v>267</v>
+        <v>461</v>
       </c>
       <c r="G450" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H450" s="204">
         <v>44644</v>
-      </c>
-      <c r="H450" s="204">
-        <v>44636</v>
       </c>
       <c r="I450" s="177"/>
     </row>
@@ -12561,10 +12587,10 @@
       <c r="B451" s="109"/>
       <c r="C451" s="110"/>
       <c r="D451" s="167" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E451" s="160" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F451" s="151" t="s">
         <v>267</v>
@@ -12581,32 +12607,40 @@
       <c r="A452" s="1"/>
       <c r="B452" s="109"/>
       <c r="C452" s="110"/>
-      <c r="D452" s="165"/>
-      <c r="E452" s="155"/>
-      <c r="F452" s="148"/>
-      <c r="G452" s="186"/>
-      <c r="H452" s="201"/>
-      <c r="I452" s="174"/>
-    </row>
-    <row r="453" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A453" s="136"/>
-      <c r="B453" s="208" t="s">
+      <c r="D452" s="167" t="s">
+        <v>466</v>
+      </c>
+      <c r="E452" s="160" t="s">
+        <v>467</v>
+      </c>
+      <c r="F452" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G452" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H452" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I452" s="177"/>
+    </row>
+    <row r="453" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A453" s="1"/>
+      <c r="B453" s="109"/>
+      <c r="C453" s="110"/>
+      <c r="D453" s="165"/>
+      <c r="E453" s="155"/>
+      <c r="F453" s="148"/>
+      <c r="G453" s="186"/>
+      <c r="H453" s="201"/>
+      <c r="I453" s="174"/>
+    </row>
+    <row r="454" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A454" s="136"/>
+      <c r="B454" s="208" t="s">
         <v>144</v>
       </c>
-      <c r="C453" s="134"/>
-      <c r="D453" s="135"/>
-      <c r="E453" s="154"/>
-      <c r="F453" s="147"/>
-      <c r="G453" s="185"/>
-      <c r="H453" s="200"/>
-      <c r="I453" s="173"/>
-    </row>
-    <row r="454" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A454" s="136"/>
-      <c r="B454" s="208"/>
-      <c r="C454" s="209" t="s">
-        <v>146</v>
-      </c>
+      <c r="C454" s="134"/>
       <c r="D454" s="135"/>
       <c r="E454" s="154"/>
       <c r="F454" s="147"/>
@@ -12614,21 +12648,23 @@
       <c r="H454" s="200"/>
       <c r="I454" s="173"/>
     </row>
-    <row r="455" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A455" s="1"/>
-      <c r="B455" s="109"/>
-      <c r="C455" s="209"/>
-      <c r="D455" s="165"/>
-      <c r="E455" s="155"/>
-      <c r="F455" s="148"/>
-      <c r="G455" s="186"/>
-      <c r="H455" s="201"/>
-      <c r="I455" s="174"/>
+    <row r="455" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A455" s="136"/>
+      <c r="B455" s="208"/>
+      <c r="C455" s="209" t="s">
+        <v>146</v>
+      </c>
+      <c r="D455" s="135"/>
+      <c r="E455" s="154"/>
+      <c r="F455" s="147"/>
+      <c r="G455" s="185"/>
+      <c r="H455" s="200"/>
+      <c r="I455" s="173"/>
     </row>
     <row r="456" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A456" s="1"/>
       <c r="B456" s="109"/>
-      <c r="C456" s="110"/>
+      <c r="C456" s="209"/>
       <c r="D456" s="165"/>
       <c r="E456" s="155"/>
       <c r="F456" s="148"/>
@@ -12636,57 +12672,45 @@
       <c r="H456" s="201"/>
       <c r="I456" s="174"/>
     </row>
-    <row r="457" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A457" s="1"/>
       <c r="B457" s="109"/>
       <c r="C457" s="110"/>
-      <c r="D457" s="144"/>
-      <c r="E457" s="156"/>
-      <c r="F457" s="149"/>
-      <c r="G457" s="187"/>
-      <c r="H457" s="202"/>
-      <c r="I457" s="175"/>
-    </row>
-    <row r="458" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A458" s="136"/>
+      <c r="D457" s="165"/>
+      <c r="E457" s="155"/>
+      <c r="F457" s="148"/>
+      <c r="G457" s="186"/>
+      <c r="H457" s="201"/>
+      <c r="I457" s="174"/>
+    </row>
+    <row r="458" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A458" s="1"/>
       <c r="B458" s="109"/>
       <c r="C458" s="110"/>
-      <c r="D458" s="166" t="s">
-        <v>861</v>
-      </c>
-      <c r="E458" s="162" t="s">
-        <v>863</v>
-      </c>
-      <c r="F458" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G458" s="188">
-        <v>44950</v>
-      </c>
-      <c r="H458" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I458" s="171" t="s">
-        <v>730</v>
-      </c>
+      <c r="D458" s="144"/>
+      <c r="E458" s="156"/>
+      <c r="F458" s="149"/>
+      <c r="G458" s="187"/>
+      <c r="H458" s="202"/>
+      <c r="I458" s="175"/>
     </row>
     <row r="459" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A459" s="136"/>
       <c r="B459" s="109"/>
       <c r="C459" s="110"/>
-      <c r="D459" s="167" t="s">
-        <v>862</v>
-      </c>
-      <c r="E459" s="158" t="s">
-        <v>864</v>
-      </c>
-      <c r="F459" s="151" t="s">
+      <c r="D459" s="166" t="s">
+        <v>861</v>
+      </c>
+      <c r="E459" s="162" t="s">
+        <v>863</v>
+      </c>
+      <c r="F459" s="150" t="s">
         <v>267</v>
       </c>
-      <c r="G459" s="190">
+      <c r="G459" s="188">
         <v>44950</v>
       </c>
-      <c r="H459" s="204">
+      <c r="H459" s="203">
         <v>44893</v>
       </c>
       <c r="I459" s="171" t="s">
@@ -12697,19 +12721,19 @@
       <c r="A460" s="136"/>
       <c r="B460" s="109"/>
       <c r="C460" s="110"/>
-      <c r="D460" s="166" t="s">
-        <v>865</v>
-      </c>
-      <c r="E460" s="157" t="s">
-        <v>867</v>
-      </c>
-      <c r="F460" s="150" t="s">
-        <v>550</v>
-      </c>
-      <c r="G460" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H460" s="203">
+      <c r="D460" s="167" t="s">
+        <v>862</v>
+      </c>
+      <c r="E460" s="158" t="s">
+        <v>864</v>
+      </c>
+      <c r="F460" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G460" s="190">
+        <v>44950</v>
+      </c>
+      <c r="H460" s="204">
         <v>44893</v>
       </c>
       <c r="I460" s="171" t="s">
@@ -12721,10 +12745,10 @@
       <c r="B461" s="109"/>
       <c r="C461" s="110"/>
       <c r="D461" s="166" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E461" s="157" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F461" s="150" t="s">
         <v>550</v>
@@ -12744,19 +12768,19 @@
       <c r="B462" s="109"/>
       <c r="C462" s="110"/>
       <c r="D462" s="166" t="s">
-        <v>857</v>
-      </c>
-      <c r="E462" s="162" t="s">
-        <v>860</v>
+        <v>866</v>
+      </c>
+      <c r="E462" s="157" t="s">
+        <v>868</v>
       </c>
       <c r="F462" s="150" t="s">
-        <v>267</v>
+        <v>550</v>
       </c>
       <c r="G462" s="188">
-        <v>44986</v>
+        <v>44970</v>
       </c>
       <c r="H462" s="203">
-        <v>44951</v>
+        <v>44893</v>
       </c>
       <c r="I462" s="171" t="s">
         <v>730</v>
@@ -12766,46 +12790,58 @@
       <c r="A463" s="136"/>
       <c r="B463" s="109"/>
       <c r="C463" s="110"/>
-      <c r="D463" s="167" t="s">
-        <v>858</v>
-      </c>
-      <c r="E463" s="158" t="s">
-        <v>859</v>
-      </c>
-      <c r="F463" s="151" t="s">
+      <c r="D463" s="166" t="s">
+        <v>857</v>
+      </c>
+      <c r="E463" s="162" t="s">
+        <v>860</v>
+      </c>
+      <c r="F463" s="150" t="s">
         <v>267</v>
       </c>
-      <c r="G463" s="190">
+      <c r="G463" s="188">
         <v>44986</v>
       </c>
-      <c r="H463" s="204">
+      <c r="H463" s="203">
         <v>44951</v>
       </c>
       <c r="I463" s="171" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="464" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A464" s="136"/>
-      <c r="B464" s="111"/>
-      <c r="C464" s="112"/>
-      <c r="D464" s="170"/>
-      <c r="E464" s="163"/>
-      <c r="F464" s="153"/>
-      <c r="G464" s="191"/>
-      <c r="H464" s="206"/>
-      <c r="I464" s="179"/>
-    </row>
-    <row r="465" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A465" s="1"/>
-      <c r="B465" s="1"/>
-      <c r="C465" s="1"/>
-      <c r="D465" s="1"/>
-      <c r="E465" s="146"/>
-      <c r="F465" s="113"/>
-      <c r="G465" s="192"/>
-      <c r="H465" s="192"/>
-      <c r="I465" s="180"/>
+      <c r="B464" s="109"/>
+      <c r="C464" s="110"/>
+      <c r="D464" s="167" t="s">
+        <v>858</v>
+      </c>
+      <c r="E464" s="158" t="s">
+        <v>859</v>
+      </c>
+      <c r="F464" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G464" s="190">
+        <v>44986</v>
+      </c>
+      <c r="H464" s="204">
+        <v>44951</v>
+      </c>
+      <c r="I464" s="171" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="465" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A465" s="136"/>
+      <c r="B465" s="111"/>
+      <c r="C465" s="112"/>
+      <c r="D465" s="170"/>
+      <c r="E465" s="163"/>
+      <c r="F465" s="153"/>
+      <c r="G465" s="191"/>
+      <c r="H465" s="206"/>
+      <c r="I465" s="179"/>
     </row>
     <row r="466" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A466" s="1"/>
@@ -12972,38 +13008,71 @@
       <c r="H480" s="192"/>
       <c r="I480" s="180"/>
     </row>
-    <row r="481" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E481" s="145"/>
-      <c r="F481" s="95"/>
-      <c r="G481" s="193"/>
-      <c r="H481" s="193"/>
-      <c r="I481" s="181"/>
-    </row>
-    <row r="482" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A481" s="1"/>
+      <c r="B481" s="1"/>
+      <c r="C481" s="1"/>
+      <c r="D481" s="1"/>
+      <c r="E481" s="146"/>
+      <c r="F481" s="113"/>
+      <c r="G481" s="192"/>
+      <c r="H481" s="192"/>
+      <c r="I481" s="180"/>
+    </row>
+    <row r="482" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="E482" s="145"/>
       <c r="F482" s="95"/>
       <c r="G482" s="193"/>
       <c r="H482" s="193"/>
       <c r="I482" s="181"/>
     </row>
-    <row r="483" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="E483" s="145"/>
       <c r="F483" s="95"/>
       <c r="G483" s="193"/>
       <c r="H483" s="193"/>
       <c r="I483" s="181"/>
     </row>
+    <row r="484" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E484" s="145"/>
+      <c r="F484" s="95"/>
+      <c r="G484" s="193"/>
+      <c r="H484" s="193"/>
+      <c r="I484" s="181"/>
+    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B453:B454"/>
-    <mergeCell ref="C454:C455"/>
+    <mergeCell ref="B355:B356"/>
+    <mergeCell ref="C356:C357"/>
+    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="B351:B352"/>
+    <mergeCell ref="C352:C353"/>
+    <mergeCell ref="C278:C279"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C128:C129"/>
+    <mergeCell ref="C444:C445"/>
+    <mergeCell ref="C365:C366"/>
+    <mergeCell ref="C368:C369"/>
+    <mergeCell ref="C390:C391"/>
+    <mergeCell ref="C393:C394"/>
+    <mergeCell ref="C396:C397"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="C140:C141"/>
+    <mergeCell ref="C181:C182"/>
+    <mergeCell ref="B454:B455"/>
+    <mergeCell ref="C455:C456"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C398:C399"/>
-    <mergeCell ref="C401:C402"/>
-    <mergeCell ref="C404:C405"/>
-    <mergeCell ref="C438:C439"/>
-    <mergeCell ref="C358:C359"/>
-    <mergeCell ref="C361:C362"/>
+    <mergeCell ref="C399:C400"/>
+    <mergeCell ref="C402:C403"/>
+    <mergeCell ref="C405:C406"/>
+    <mergeCell ref="C439:C440"/>
+    <mergeCell ref="C359:C360"/>
+    <mergeCell ref="C362:C363"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C14:C15"/>
@@ -13011,28 +13080,6 @@
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="C54:C55"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="C443:C444"/>
-    <mergeCell ref="C364:C365"/>
-    <mergeCell ref="C367:C368"/>
-    <mergeCell ref="C389:C390"/>
-    <mergeCell ref="C392:C393"/>
-    <mergeCell ref="C395:C396"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="C181:C182"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B354:B355"/>
-    <mergeCell ref="C355:C356"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="B350:B351"/>
-    <mergeCell ref="C351:C352"/>
-    <mergeCell ref="C278:C279"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -13066,20 +13113,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="243" t="s">
+      <c r="B2" s="226" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="244"/>
-      <c r="D2" s="245"/>
-      <c r="E2" s="240" t="s">
+      <c r="C2" s="227"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="223" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="242"/>
-      <c r="G2" s="240" t="s">
+      <c r="F2" s="225"/>
+      <c r="G2" s="223" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="241"/>
-      <c r="I2" s="242"/>
+      <c r="H2" s="224"/>
+      <c r="I2" s="225"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -13100,10 +13147,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="246" t="s">
+      <c r="H3" s="229" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="247"/>
+      <c r="I3" s="230"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -13145,7 +13192,7 @@
       <c r="F5" s="237" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="228" t="s">
+      <c r="G5" s="240" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -13161,11 +13208,11 @@
       <c r="D6" s="235"/>
       <c r="E6" s="35"/>
       <c r="F6" s="238"/>
-      <c r="G6" s="229"/>
-      <c r="H6" s="223" t="s">
+      <c r="G6" s="241"/>
+      <c r="H6" s="221" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="224"/>
+      <c r="I6" s="222"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
@@ -13173,7 +13220,7 @@
       <c r="D7" s="236"/>
       <c r="E7" s="36"/>
       <c r="F7" s="239"/>
-      <c r="G7" s="230"/>
+      <c r="G7" s="242"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -13213,13 +13260,13 @@
       <c r="D9" s="234" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="225" t="s">
+      <c r="E9" s="245" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="237" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="228" t="s">
+      <c r="G9" s="240" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -13234,22 +13281,22 @@
       <c r="B10" s="61"/>
       <c r="C10" s="232"/>
       <c r="D10" s="235"/>
-      <c r="E10" s="226"/>
+      <c r="E10" s="246"/>
       <c r="F10" s="238"/>
-      <c r="G10" s="229"/>
-      <c r="H10" s="223" t="s">
+      <c r="G10" s="241"/>
+      <c r="H10" s="221" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="224"/>
+      <c r="I10" s="222"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
       <c r="C11" s="233"/>
       <c r="D11" s="236"/>
-      <c r="E11" s="227"/>
+      <c r="E11" s="247"/>
       <c r="F11" s="239"/>
-      <c r="G11" s="230"/>
+      <c r="G11" s="242"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -13359,7 +13406,7 @@
       <c r="F18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="228" t="s">
+      <c r="G18" s="240" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="6" t="s">
@@ -13379,7 +13426,7 @@
       <c r="F19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="230"/>
+      <c r="G19" s="242"/>
       <c r="H19" s="8"/>
       <c r="I19" s="17"/>
     </row>
@@ -13424,8 +13471,8 @@
       <c r="E22" s="25"/>
       <c r="F22" s="22"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="221"/>
-      <c r="I22" s="222"/>
+      <c r="H22" s="243"/>
+      <c r="I22" s="244"/>
     </row>
     <row r="23" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="67" t="s">
@@ -13845,13 +13892,13 @@
       <c r="D46" s="234" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="225" t="s">
+      <c r="E46" s="245" t="s">
         <v>45</v>
       </c>
       <c r="F46" s="237" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="228" t="s">
+      <c r="G46" s="240" t="s">
         <v>47</v>
       </c>
       <c r="H46" s="6" t="s">
@@ -13865,21 +13912,21 @@
       <c r="B47" s="61"/>
       <c r="C47" s="232"/>
       <c r="D47" s="235"/>
-      <c r="E47" s="226"/>
+      <c r="E47" s="246"/>
       <c r="F47" s="238"/>
-      <c r="G47" s="229"/>
-      <c r="H47" s="223" t="s">
+      <c r="G47" s="241"/>
+      <c r="H47" s="221" t="s">
         <v>32</v>
       </c>
-      <c r="I47" s="224"/>
+      <c r="I47" s="222"/>
     </row>
     <row r="48" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B48" s="61"/>
       <c r="C48" s="233"/>
       <c r="D48" s="236"/>
-      <c r="E48" s="227"/>
+      <c r="E48" s="247"/>
       <c r="F48" s="239"/>
-      <c r="G48" s="230"/>
+      <c r="G48" s="242"/>
       <c r="H48" s="8" t="s">
         <v>23</v>
       </c>
@@ -13919,13 +13966,13 @@
       <c r="D50" s="234" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="225" t="s">
+      <c r="E50" s="245" t="s">
         <v>55</v>
       </c>
       <c r="F50" s="237" t="s">
         <v>56</v>
       </c>
-      <c r="G50" s="228" t="s">
+      <c r="G50" s="240" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="6" t="s">
@@ -13939,21 +13986,21 @@
       <c r="B51" s="61"/>
       <c r="C51" s="232"/>
       <c r="D51" s="235"/>
-      <c r="E51" s="226"/>
+      <c r="E51" s="246"/>
       <c r="F51" s="238"/>
-      <c r="G51" s="229"/>
-      <c r="H51" s="223" t="s">
+      <c r="G51" s="241"/>
+      <c r="H51" s="221" t="s">
         <v>32</v>
       </c>
-      <c r="I51" s="224"/>
+      <c r="I51" s="222"/>
     </row>
     <row r="52" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B52" s="61"/>
       <c r="C52" s="233"/>
       <c r="D52" s="236"/>
-      <c r="E52" s="227"/>
+      <c r="E52" s="247"/>
       <c r="F52" s="239"/>
-      <c r="G52" s="230"/>
+      <c r="G52" s="242"/>
       <c r="H52" s="8" t="s">
         <v>23</v>
       </c>
@@ -13978,8 +14025,8 @@
       <c r="E54" s="25"/>
       <c r="F54" s="22"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="221"/>
-      <c r="I54" s="222"/>
+      <c r="H54" s="243"/>
+      <c r="I54" s="244"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="61" t="s">
@@ -14042,10 +14089,10 @@
       <c r="E58" s="39"/>
       <c r="F58" s="12"/>
       <c r="G58" s="32"/>
-      <c r="H58" s="223" t="s">
+      <c r="H58" s="221" t="s">
         <v>32</v>
       </c>
-      <c r="I58" s="224"/>
+      <c r="I58" s="222"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
@@ -14078,8 +14125,8 @@
       <c r="E61" s="25"/>
       <c r="F61" s="22"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="221"/>
-      <c r="I61" s="222"/>
+      <c r="H61" s="243"/>
+      <c r="I61" s="244"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="64" t="s">
@@ -14492,8 +14539,8 @@
       <c r="E89" s="25"/>
       <c r="F89" s="22"/>
       <c r="G89" s="25"/>
-      <c r="H89" s="221"/>
-      <c r="I89" s="222"/>
+      <c r="H89" s="243"/>
+      <c r="I89" s="244"/>
     </row>
     <row r="90" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="61"/>
@@ -14637,15 +14684,22 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="G18:G19"/>
@@ -14658,22 +14712,15 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="D14:D16"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -14707,10 +14754,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="249"/>
-      <c r="D2" s="241" t="s">
+      <c r="D2" s="224" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="242" t="s">
+      <c r="E2" s="225" t="s">
         <v>0</v>
       </c>
     </row>
@@ -14721,8 +14768,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="246"/>
-      <c r="E3" s="247"/>
+      <c r="D3" s="229"/>
+      <c r="E3" s="230"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 24 Maret 2023 14:51 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1508" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="939">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -3008,6 +3008,40 @@
   </si>
   <si>
     <t>Memperbaharui satu atau beberapa field yang didefiniskan pada Array Data (varData) pada Record Table yang diidentifikasi melalui Record ID (varID)</t>
+  </si>
+  <si>
+    <t>Mendapatkan Signature Snapshot Data Content dari suatu Table berdasarkan Nama Schema (varSchemaName) dan Nama Table (varTableName)</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetTableSnapshotSignature</t>
+  </si>
+  <si>
+    <t>SchSysConfig.
+FuncSys_General_GetTableStatistics</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetTableStatistics</t>
+  </si>
+  <si>
+    <t>Mendapatkan Informasi Statistik Data dari Table berdasarkan Nama Schema (varSchemaName) dan Nama Table (varTableName)</t>
+  </si>
+  <si>
+    <t>Func_TblLog_TableSnapshotSignature_UPDATE</t>
+  </si>
+  <si>
+    <t>Func_TblLog_TableSnapshotSignature_INSERT</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblLog_TableSnapshotSignature</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblLog_TableSnapshotSignature</t>
+  </si>
+  <si>
+    <t>Func_TblLog_TableSnapshotSignature_SET</t>
+  </si>
+  <si>
+    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblLog_TableSnapshotSignature</t>
   </si>
 </sst>
 </file>
@@ -4417,6 +4451,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4435,20 +4484,71 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4456,12 +4556,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4470,66 +4564,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4854,13 +4888,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I506"/>
+  <dimension ref="A1:I515"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F364" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E365" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J364" sqref="J364"/>
+      <selection pane="bottomRight" activeCell="E375" sqref="E375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4879,20 +4913,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="216" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="218" t="s">
+      <c r="C2" s="217"/>
+      <c r="D2" s="218"/>
+      <c r="E2" s="223" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="214" t="s">
+      <c r="F2" s="219" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="215"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="220" t="s">
+      <c r="G2" s="220"/>
+      <c r="H2" s="221"/>
+      <c r="I2" s="214" t="s">
         <v>670</v>
       </c>
     </row>
@@ -4906,7 +4940,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="219"/>
+      <c r="E3" s="224"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -4916,11 +4950,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="221"/>
+      <c r="I3" s="215"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="222" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -11387,197 +11421,227 @@
         <v>926</v>
       </c>
     </row>
-    <row r="363" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
       <c r="B363" s="109"/>
       <c r="C363" s="110"/>
-      <c r="D363" s="167"/>
-      <c r="E363" s="158"/>
-      <c r="F363" s="151"/>
-      <c r="G363" s="190"/>
-      <c r="H363" s="204"/>
-      <c r="I363" s="199"/>
+      <c r="D363" s="167" t="s">
+        <v>931</v>
+      </c>
+      <c r="E363" s="158" t="s">
+        <v>932</v>
+      </c>
+      <c r="F363" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G363" s="190">
+        <v>45009</v>
+      </c>
+      <c r="H363" s="204">
+        <v>45009</v>
+      </c>
+      <c r="I363" s="209" t="s">
+        <v>930</v>
+      </c>
     </row>
     <row r="364" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A364" s="1"/>
       <c r="B364" s="109"/>
       <c r="C364" s="110"/>
       <c r="D364" s="167" t="s">
-        <v>388</v>
+        <v>929</v>
       </c>
       <c r="E364" s="158" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="F364" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G364" s="190">
-        <v>44957</v>
+        <v>45009</v>
       </c>
       <c r="H364" s="204">
-        <v>44957</v>
-      </c>
-      <c r="I364" s="199" t="s">
-        <v>892</v>
+        <v>45009</v>
+      </c>
+      <c r="I364" s="209" t="s">
+        <v>735</v>
       </c>
     </row>
     <row r="365" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A365" s="1"/>
       <c r="B365" s="109"/>
       <c r="C365" s="110"/>
-      <c r="D365" s="165"/>
-      <c r="E365" s="159"/>
-      <c r="F365" s="148"/>
-      <c r="G365" s="186"/>
-      <c r="H365" s="201"/>
-      <c r="I365" s="174"/>
-    </row>
-    <row r="366" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D365" s="167"/>
+      <c r="E365" s="158"/>
+      <c r="F365" s="151"/>
+      <c r="G365" s="190"/>
+      <c r="H365" s="204"/>
+      <c r="I365" s="199"/>
+    </row>
+    <row r="366" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A366" s="1"/>
       <c r="B366" s="109"/>
       <c r="C366" s="110"/>
-      <c r="D366" s="165"/>
-      <c r="E366" s="155"/>
-      <c r="F366" s="148"/>
-      <c r="G366" s="186"/>
-      <c r="H366" s="201"/>
-      <c r="I366" s="174"/>
-    </row>
-    <row r="367" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D366" s="167" t="s">
+        <v>388</v>
+      </c>
+      <c r="E366" s="158" t="s">
+        <v>927</v>
+      </c>
+      <c r="F366" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G366" s="190">
+        <v>44957</v>
+      </c>
+      <c r="H366" s="204">
+        <v>44957</v>
+      </c>
+      <c r="I366" s="199" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="367" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A367" s="1"/>
       <c r="B367" s="109"/>
       <c r="C367" s="110"/>
-      <c r="D367" s="144"/>
-      <c r="E367" s="156"/>
-      <c r="F367" s="149"/>
-      <c r="G367" s="187"/>
-      <c r="H367" s="202"/>
-      <c r="I367" s="175"/>
-    </row>
-    <row r="368" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D367" s="165"/>
+      <c r="E367" s="159"/>
+      <c r="F367" s="148"/>
+      <c r="G367" s="186"/>
+      <c r="H367" s="201"/>
+      <c r="I367" s="174"/>
+    </row>
+    <row r="368" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
       <c r="B368" s="109"/>
       <c r="C368" s="110"/>
-      <c r="D368" s="166" t="s">
-        <v>329</v>
-      </c>
-      <c r="E368" s="162" t="s">
-        <v>330</v>
-      </c>
-      <c r="F368" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G368" s="188">
-        <v>44893</v>
-      </c>
-      <c r="H368" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I368" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="369" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D368" s="165"/>
+      <c r="E368" s="155"/>
+      <c r="F368" s="148"/>
+      <c r="G368" s="186"/>
+      <c r="H368" s="201"/>
+      <c r="I368" s="174"/>
+    </row>
+    <row r="369" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A369" s="1"/>
       <c r="B369" s="109"/>
       <c r="C369" s="110"/>
-      <c r="D369" s="167" t="s">
-        <v>852</v>
-      </c>
-      <c r="E369" s="158" t="s">
-        <v>853</v>
-      </c>
-      <c r="F369" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G369" s="190">
-        <v>44986</v>
-      </c>
-      <c r="H369" s="204">
-        <v>44951</v>
-      </c>
-      <c r="I369" s="183" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="370" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D369" s="144"/>
+      <c r="E369" s="156"/>
+      <c r="F369" s="149"/>
+      <c r="G369" s="187"/>
+      <c r="H369" s="202"/>
+      <c r="I369" s="175"/>
+    </row>
+    <row r="370" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A370" s="1"/>
       <c r="B370" s="109"/>
       <c r="C370" s="110"/>
-      <c r="D370" s="165"/>
-      <c r="E370" s="155"/>
-      <c r="F370" s="148"/>
-      <c r="G370" s="186"/>
-      <c r="H370" s="201"/>
-      <c r="I370" s="174"/>
-    </row>
-    <row r="371" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A371" s="136"/>
-      <c r="B371" s="212" t="s">
-        <v>142</v>
-      </c>
-      <c r="C371" s="134"/>
-      <c r="D371" s="135"/>
-      <c r="E371" s="154"/>
-      <c r="F371" s="147"/>
-      <c r="G371" s="185"/>
-      <c r="H371" s="200"/>
-      <c r="I371" s="173"/>
-    </row>
-    <row r="372" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A372" s="136"/>
-      <c r="B372" s="212"/>
-      <c r="C372" s="213" t="s">
-        <v>160</v>
-      </c>
-      <c r="D372" s="135"/>
-      <c r="E372" s="154"/>
-      <c r="F372" s="147"/>
-      <c r="G372" s="185"/>
-      <c r="H372" s="200"/>
-      <c r="I372" s="173"/>
+      <c r="D370" s="166" t="s">
+        <v>329</v>
+      </c>
+      <c r="E370" s="162" t="s">
+        <v>330</v>
+      </c>
+      <c r="F370" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G370" s="188">
+        <v>44893</v>
+      </c>
+      <c r="H370" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I370" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="371" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A371" s="1"/>
+      <c r="B371" s="109"/>
+      <c r="C371" s="110"/>
+      <c r="D371" s="166"/>
+      <c r="E371" s="162"/>
+      <c r="F371" s="150"/>
+      <c r="G371" s="188"/>
+      <c r="H371" s="203"/>
+      <c r="I371" s="171"/>
+    </row>
+    <row r="372" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A372" s="1"/>
+      <c r="B372" s="109"/>
+      <c r="C372" s="110"/>
+      <c r="D372" s="166" t="s">
+        <v>937</v>
+      </c>
+      <c r="E372" s="162" t="s">
+        <v>938</v>
+      </c>
+      <c r="F372" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G372" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H372" s="203">
+        <v>45009</v>
+      </c>
+      <c r="I372" s="183" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="373" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A373" s="1"/>
       <c r="B373" s="109"/>
-      <c r="C373" s="213"/>
-      <c r="D373" s="165"/>
-      <c r="E373" s="155"/>
-      <c r="F373" s="148"/>
-      <c r="G373" s="186"/>
-      <c r="H373" s="201"/>
-      <c r="I373" s="174"/>
-    </row>
-    <row r="374" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C373" s="110"/>
+      <c r="D373" s="166"/>
+      <c r="E373" s="162"/>
+      <c r="F373" s="150"/>
+      <c r="G373" s="188"/>
+      <c r="H373" s="203"/>
+      <c r="I373" s="171"/>
+    </row>
+    <row r="374" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A374" s="1"/>
       <c r="B374" s="109"/>
       <c r="C374" s="110"/>
-      <c r="D374" s="165"/>
-      <c r="E374" s="155"/>
-      <c r="F374" s="148"/>
-      <c r="G374" s="186"/>
-      <c r="H374" s="201"/>
-      <c r="I374" s="174"/>
-    </row>
-    <row r="375" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A375" s="136"/>
-      <c r="B375" s="212" t="s">
-        <v>143</v>
-      </c>
-      <c r="C375" s="134"/>
-      <c r="D375" s="135"/>
-      <c r="E375" s="154"/>
-      <c r="F375" s="147"/>
-      <c r="G375" s="185"/>
-      <c r="H375" s="200"/>
-      <c r="I375" s="173"/>
-    </row>
-    <row r="376" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D374" s="167" t="s">
+        <v>852</v>
+      </c>
+      <c r="E374" s="158" t="s">
+        <v>853</v>
+      </c>
+      <c r="F374" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G374" s="190">
+        <v>44986</v>
+      </c>
+      <c r="H374" s="204">
+        <v>44951</v>
+      </c>
+      <c r="I374" s="183" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="375" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A375" s="1"/>
+      <c r="B375" s="109"/>
+      <c r="C375" s="110"/>
+      <c r="D375" s="165"/>
+      <c r="E375" s="155"/>
+      <c r="F375" s="148"/>
+      <c r="G375" s="186"/>
+      <c r="H375" s="201"/>
+      <c r="I375" s="174"/>
+    </row>
+    <row r="376" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A376" s="136"/>
-      <c r="B376" s="212"/>
-      <c r="C376" s="213" t="s">
-        <v>148</v>
-      </c>
+      <c r="B376" s="212" t="s">
+        <v>142</v>
+      </c>
+      <c r="C376" s="134"/>
       <c r="D376" s="135"/>
       <c r="E376" s="154"/>
       <c r="F376" s="147"/>
@@ -11585,21 +11649,23 @@
       <c r="H376" s="200"/>
       <c r="I376" s="173"/>
     </row>
-    <row r="377" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A377" s="1"/>
-      <c r="B377" s="109"/>
-      <c r="C377" s="213"/>
-      <c r="D377" s="165"/>
-      <c r="E377" s="155"/>
-      <c r="F377" s="148"/>
-      <c r="G377" s="186"/>
-      <c r="H377" s="201"/>
-      <c r="I377" s="174"/>
+    <row r="377" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A377" s="136"/>
+      <c r="B377" s="212"/>
+      <c r="C377" s="213" t="s">
+        <v>160</v>
+      </c>
+      <c r="D377" s="135"/>
+      <c r="E377" s="154"/>
+      <c r="F377" s="147"/>
+      <c r="G377" s="185"/>
+      <c r="H377" s="200"/>
+      <c r="I377" s="173"/>
     </row>
     <row r="378" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A378" s="1"/>
       <c r="B378" s="109"/>
-      <c r="C378" s="110"/>
+      <c r="C378" s="213"/>
       <c r="D378" s="165"/>
       <c r="E378" s="155"/>
       <c r="F378" s="148"/>
@@ -11610,54 +11676,44 @@
     <row r="379" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A379" s="1"/>
       <c r="B379" s="109"/>
-      <c r="C379" s="213" t="s">
-        <v>149</v>
-      </c>
-      <c r="D379" s="135"/>
-      <c r="E379" s="154"/>
-      <c r="F379" s="147"/>
-      <c r="G379" s="185"/>
-      <c r="H379" s="200"/>
-      <c r="I379" s="173"/>
-    </row>
-    <row r="380" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A380" s="1"/>
-      <c r="B380" s="109"/>
-      <c r="C380" s="213"/>
-      <c r="D380" s="165"/>
-      <c r="E380" s="155"/>
-      <c r="F380" s="148"/>
-      <c r="G380" s="186"/>
-      <c r="H380" s="201"/>
-      <c r="I380" s="174"/>
-    </row>
-    <row r="381" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A381" s="1"/>
-      <c r="B381" s="109"/>
-      <c r="C381" s="110"/>
-      <c r="D381" s="166" t="s">
-        <v>915</v>
-      </c>
-      <c r="E381" s="157" t="s">
-        <v>917</v>
-      </c>
-      <c r="F381" s="150" t="s">
-        <v>689</v>
-      </c>
-      <c r="G381" s="188">
-        <v>44860</v>
-      </c>
-      <c r="H381" s="203">
-        <v>44503</v>
-      </c>
-      <c r="I381" s="171" t="s">
-        <v>916</v>
-      </c>
+      <c r="C379" s="110"/>
+      <c r="D379" s="165"/>
+      <c r="E379" s="155"/>
+      <c r="F379" s="148"/>
+      <c r="G379" s="186"/>
+      <c r="H379" s="201"/>
+      <c r="I379" s="174"/>
+    </row>
+    <row r="380" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A380" s="136"/>
+      <c r="B380" s="212" t="s">
+        <v>143</v>
+      </c>
+      <c r="C380" s="134"/>
+      <c r="D380" s="135"/>
+      <c r="E380" s="154"/>
+      <c r="F380" s="147"/>
+      <c r="G380" s="185"/>
+      <c r="H380" s="200"/>
+      <c r="I380" s="173"/>
+    </row>
+    <row r="381" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A381" s="136"/>
+      <c r="B381" s="212"/>
+      <c r="C381" s="213" t="s">
+        <v>148</v>
+      </c>
+      <c r="D381" s="135"/>
+      <c r="E381" s="154"/>
+      <c r="F381" s="147"/>
+      <c r="G381" s="185"/>
+      <c r="H381" s="200"/>
+      <c r="I381" s="173"/>
     </row>
     <row r="382" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A382" s="1"/>
       <c r="B382" s="109"/>
-      <c r="C382" s="110"/>
+      <c r="C382" s="213"/>
       <c r="D382" s="165"/>
       <c r="E382" s="155"/>
       <c r="F382" s="148"/>
@@ -11668,31 +11724,31 @@
     <row r="383" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A383" s="1"/>
       <c r="B383" s="109"/>
-      <c r="C383" s="213" t="s">
-        <v>150</v>
-      </c>
-      <c r="D383" s="135"/>
-      <c r="E383" s="154"/>
-      <c r="F383" s="147"/>
-      <c r="G383" s="185"/>
-      <c r="H383" s="200"/>
-      <c r="I383" s="173"/>
+      <c r="C383" s="110"/>
+      <c r="D383" s="165"/>
+      <c r="E383" s="155"/>
+      <c r="F383" s="148"/>
+      <c r="G383" s="186"/>
+      <c r="H383" s="201"/>
+      <c r="I383" s="174"/>
     </row>
     <row r="384" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A384" s="1"/>
       <c r="B384" s="109"/>
-      <c r="C384" s="213"/>
-      <c r="D384" s="165"/>
-      <c r="E384" s="155"/>
-      <c r="F384" s="148"/>
-      <c r="G384" s="186"/>
-      <c r="H384" s="201"/>
-      <c r="I384" s="174"/>
+      <c r="C384" s="213" t="s">
+        <v>149</v>
+      </c>
+      <c r="D384" s="135"/>
+      <c r="E384" s="154"/>
+      <c r="F384" s="147"/>
+      <c r="G384" s="185"/>
+      <c r="H384" s="200"/>
+      <c r="I384" s="173"/>
     </row>
     <row r="385" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A385" s="1"/>
       <c r="B385" s="109"/>
-      <c r="C385" s="110"/>
+      <c r="C385" s="213"/>
       <c r="D385" s="165"/>
       <c r="E385" s="155"/>
       <c r="F385" s="148"/>
@@ -11700,23 +11756,33 @@
       <c r="H385" s="201"/>
       <c r="I385" s="174"/>
     </row>
-    <row r="386" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A386" s="1"/>
       <c r="B386" s="109"/>
-      <c r="C386" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="D386" s="135"/>
-      <c r="E386" s="154"/>
-      <c r="F386" s="147"/>
-      <c r="G386" s="185"/>
-      <c r="H386" s="200"/>
-      <c r="I386" s="173"/>
+      <c r="C386" s="110"/>
+      <c r="D386" s="166" t="s">
+        <v>915</v>
+      </c>
+      <c r="E386" s="157" t="s">
+        <v>917</v>
+      </c>
+      <c r="F386" s="150" t="s">
+        <v>689</v>
+      </c>
+      <c r="G386" s="188">
+        <v>44860</v>
+      </c>
+      <c r="H386" s="203">
+        <v>44503</v>
+      </c>
+      <c r="I386" s="171" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="387" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A387" s="1"/>
       <c r="B387" s="109"/>
-      <c r="C387" s="213"/>
+      <c r="C387" s="110"/>
       <c r="D387" s="165"/>
       <c r="E387" s="155"/>
       <c r="F387" s="148"/>
@@ -11727,162 +11793,106 @@
     <row r="388" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A388" s="1"/>
       <c r="B388" s="109"/>
-      <c r="C388" s="110"/>
-      <c r="D388" s="165"/>
-      <c r="E388" s="155"/>
-      <c r="F388" s="148"/>
-      <c r="G388" s="186"/>
-      <c r="H388" s="201"/>
-      <c r="I388" s="174"/>
+      <c r="C388" s="213" t="s">
+        <v>150</v>
+      </c>
+      <c r="D388" s="135"/>
+      <c r="E388" s="154"/>
+      <c r="F388" s="147"/>
+      <c r="G388" s="185"/>
+      <c r="H388" s="200"/>
+      <c r="I388" s="173"/>
     </row>
     <row r="389" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A389" s="1"/>
       <c r="B389" s="109"/>
-      <c r="C389" s="213" t="s">
-        <v>152</v>
-      </c>
-      <c r="D389" s="135"/>
-      <c r="E389" s="154"/>
-      <c r="F389" s="147"/>
-      <c r="G389" s="185"/>
-      <c r="H389" s="200"/>
-      <c r="I389" s="173"/>
+      <c r="C389" s="213"/>
+      <c r="D389" s="165"/>
+      <c r="E389" s="155"/>
+      <c r="F389" s="148"/>
+      <c r="G389" s="186"/>
+      <c r="H389" s="201"/>
+      <c r="I389" s="174"/>
     </row>
     <row r="390" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A390" s="1"/>
       <c r="B390" s="109"/>
-      <c r="C390" s="213"/>
-      <c r="D390" s="166" t="s">
-        <v>760</v>
-      </c>
-      <c r="E390" s="162" t="s">
-        <v>762</v>
-      </c>
-      <c r="F390" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G390" s="188">
-        <v>44721</v>
-      </c>
-      <c r="H390" s="204">
-        <v>44698</v>
-      </c>
-      <c r="I390" s="176" t="s">
-        <v>759</v>
-      </c>
+      <c r="C390" s="110"/>
+      <c r="D390" s="165"/>
+      <c r="E390" s="155"/>
+      <c r="F390" s="148"/>
+      <c r="G390" s="186"/>
+      <c r="H390" s="201"/>
+      <c r="I390" s="174"/>
     </row>
     <row r="391" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A391" s="1"/>
       <c r="B391" s="109"/>
-      <c r="C391" s="110"/>
-      <c r="D391" s="167" t="s">
-        <v>761</v>
-      </c>
-      <c r="E391" s="160" t="s">
-        <v>763</v>
-      </c>
-      <c r="F391" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G391" s="190">
-        <v>44721</v>
-      </c>
-      <c r="H391" s="204">
-        <v>44698</v>
-      </c>
-      <c r="I391" s="177" t="s">
-        <v>759</v>
-      </c>
+      <c r="C391" s="213" t="s">
+        <v>151</v>
+      </c>
+      <c r="D391" s="135"/>
+      <c r="E391" s="154"/>
+      <c r="F391" s="147"/>
+      <c r="G391" s="185"/>
+      <c r="H391" s="200"/>
+      <c r="I391" s="173"/>
     </row>
     <row r="392" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A392" s="1"/>
       <c r="B392" s="109"/>
-      <c r="C392" s="110"/>
-      <c r="D392" s="167" t="s">
-        <v>755</v>
-      </c>
-      <c r="E392" s="160" t="s">
-        <v>757</v>
-      </c>
-      <c r="F392" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G392" s="190">
-        <v>44644</v>
-      </c>
-      <c r="H392" s="204">
-        <v>44622</v>
-      </c>
-      <c r="I392" s="177" t="s">
-        <v>759</v>
-      </c>
+      <c r="C392" s="213"/>
+      <c r="D392" s="165"/>
+      <c r="E392" s="155"/>
+      <c r="F392" s="148"/>
+      <c r="G392" s="186"/>
+      <c r="H392" s="201"/>
+      <c r="I392" s="174"/>
     </row>
     <row r="393" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A393" s="1"/>
       <c r="B393" s="109"/>
       <c r="C393" s="110"/>
-      <c r="D393" s="167" t="s">
-        <v>756</v>
-      </c>
-      <c r="E393" s="160" t="s">
-        <v>758</v>
-      </c>
-      <c r="F393" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G393" s="190">
-        <v>44644</v>
-      </c>
-      <c r="H393" s="204">
-        <v>44622</v>
-      </c>
-      <c r="I393" s="177" t="s">
-        <v>759</v>
-      </c>
+      <c r="D393" s="165"/>
+      <c r="E393" s="155"/>
+      <c r="F393" s="148"/>
+      <c r="G393" s="186"/>
+      <c r="H393" s="201"/>
+      <c r="I393" s="174"/>
     </row>
     <row r="394" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A394" s="1"/>
       <c r="B394" s="109"/>
-      <c r="C394" s="110"/>
-      <c r="D394" s="167" t="s">
-        <v>764</v>
-      </c>
-      <c r="E394" s="160" t="s">
-        <v>766</v>
-      </c>
-      <c r="F394" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G394" s="190">
-        <v>44755</v>
-      </c>
-      <c r="H394" s="204">
-        <v>44755</v>
-      </c>
-      <c r="I394" s="177" t="s">
-        <v>759</v>
-      </c>
+      <c r="C394" s="213" t="s">
+        <v>152</v>
+      </c>
+      <c r="D394" s="135"/>
+      <c r="E394" s="154"/>
+      <c r="F394" s="147"/>
+      <c r="G394" s="185"/>
+      <c r="H394" s="200"/>
+      <c r="I394" s="173"/>
     </row>
     <row r="395" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A395" s="1"/>
       <c r="B395" s="109"/>
-      <c r="C395" s="110"/>
-      <c r="D395" s="167" t="s">
-        <v>765</v>
-      </c>
-      <c r="E395" s="160" t="s">
-        <v>767</v>
-      </c>
-      <c r="F395" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G395" s="190">
-        <v>44756</v>
+      <c r="C395" s="213"/>
+      <c r="D395" s="166" t="s">
+        <v>760</v>
+      </c>
+      <c r="E395" s="162" t="s">
+        <v>762</v>
+      </c>
+      <c r="F395" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G395" s="188">
+        <v>44721</v>
       </c>
       <c r="H395" s="204">
-        <v>44756</v>
-      </c>
-      <c r="I395" s="177" t="s">
+        <v>44698</v>
+      </c>
+      <c r="I395" s="176" t="s">
         <v>759</v>
       </c>
     </row>
@@ -11891,19 +11901,19 @@
       <c r="B396" s="109"/>
       <c r="C396" s="110"/>
       <c r="D396" s="167" t="s">
-        <v>768</v>
+        <v>761</v>
       </c>
       <c r="E396" s="160" t="s">
-        <v>770</v>
+        <v>763</v>
       </c>
       <c r="F396" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G396" s="190">
-        <v>44755</v>
+        <v>44721</v>
       </c>
       <c r="H396" s="204">
-        <v>44755</v>
+        <v>44698</v>
       </c>
       <c r="I396" s="177" t="s">
         <v>759</v>
@@ -11914,19 +11924,19 @@
       <c r="B397" s="109"/>
       <c r="C397" s="110"/>
       <c r="D397" s="167" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="E397" s="160" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="F397" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G397" s="190">
-        <v>44755</v>
+        <v>44644</v>
       </c>
       <c r="H397" s="204">
-        <v>44755</v>
+        <v>44622</v>
       </c>
       <c r="I397" s="177" t="s">
         <v>759</v>
@@ -11936,56 +11946,116 @@
       <c r="A398" s="1"/>
       <c r="B398" s="109"/>
       <c r="C398" s="110"/>
-      <c r="D398" s="167"/>
-      <c r="E398" s="160"/>
-      <c r="F398" s="151"/>
-      <c r="G398" s="190"/>
-      <c r="H398" s="204"/>
-      <c r="I398" s="177"/>
+      <c r="D398" s="167" t="s">
+        <v>756</v>
+      </c>
+      <c r="E398" s="160" t="s">
+        <v>758</v>
+      </c>
+      <c r="F398" s="151" t="s">
+        <v>281</v>
+      </c>
+      <c r="G398" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H398" s="204">
+        <v>44622</v>
+      </c>
+      <c r="I398" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="399" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A399" s="1"/>
       <c r="B399" s="109"/>
       <c r="C399" s="110"/>
-      <c r="D399" s="167"/>
-      <c r="E399" s="160"/>
-      <c r="F399" s="151"/>
-      <c r="G399" s="190"/>
-      <c r="H399" s="204"/>
-      <c r="I399" s="177"/>
+      <c r="D399" s="167" t="s">
+        <v>764</v>
+      </c>
+      <c r="E399" s="160" t="s">
+        <v>766</v>
+      </c>
+      <c r="F399" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G399" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H399" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I399" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="400" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A400" s="1"/>
       <c r="B400" s="109"/>
       <c r="C400" s="110"/>
-      <c r="D400" s="167"/>
-      <c r="E400" s="160"/>
-      <c r="F400" s="151"/>
-      <c r="G400" s="190"/>
-      <c r="H400" s="204"/>
-      <c r="I400" s="177"/>
+      <c r="D400" s="167" t="s">
+        <v>765</v>
+      </c>
+      <c r="E400" s="160" t="s">
+        <v>767</v>
+      </c>
+      <c r="F400" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G400" s="190">
+        <v>44756</v>
+      </c>
+      <c r="H400" s="204">
+        <v>44756</v>
+      </c>
+      <c r="I400" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="401" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A401" s="1"/>
       <c r="B401" s="109"/>
       <c r="C401" s="110"/>
-      <c r="D401" s="167"/>
-      <c r="E401" s="160"/>
-      <c r="F401" s="151"/>
-      <c r="G401" s="190"/>
-      <c r="H401" s="204"/>
-      <c r="I401" s="177"/>
+      <c r="D401" s="167" t="s">
+        <v>768</v>
+      </c>
+      <c r="E401" s="160" t="s">
+        <v>770</v>
+      </c>
+      <c r="F401" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G401" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H401" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I401" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="402" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A402" s="1"/>
       <c r="B402" s="109"/>
       <c r="C402" s="110"/>
-      <c r="D402" s="167"/>
-      <c r="E402" s="160"/>
-      <c r="F402" s="151"/>
-      <c r="G402" s="190"/>
-      <c r="H402" s="204"/>
-      <c r="I402" s="177"/>
+      <c r="D402" s="167" t="s">
+        <v>769</v>
+      </c>
+      <c r="E402" s="160" t="s">
+        <v>771</v>
+      </c>
+      <c r="F402" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G402" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H402" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I402" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="403" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A403" s="1"/>
@@ -12002,38 +12072,22 @@
       <c r="A404" s="1"/>
       <c r="B404" s="109"/>
       <c r="C404" s="110"/>
-      <c r="D404" s="167" t="s">
-        <v>773</v>
-      </c>
+      <c r="D404" s="167"/>
       <c r="E404" s="160"/>
-      <c r="F404" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G404" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H404" s="204">
-        <v>44984</v>
-      </c>
+      <c r="F404" s="151"/>
+      <c r="G404" s="190"/>
+      <c r="H404" s="204"/>
       <c r="I404" s="177"/>
     </row>
     <row r="405" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A405" s="1"/>
       <c r="B405" s="109"/>
       <c r="C405" s="110"/>
-      <c r="D405" s="167" t="s">
-        <v>772</v>
-      </c>
+      <c r="D405" s="167"/>
       <c r="E405" s="160"/>
-      <c r="F405" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G405" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H405" s="204">
-        <v>44984</v>
-      </c>
+      <c r="F405" s="151"/>
+      <c r="G405" s="190"/>
+      <c r="H405" s="204"/>
       <c r="I405" s="177"/>
     </row>
     <row r="406" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -12073,76 +12127,88 @@
       <c r="A409" s="1"/>
       <c r="B409" s="109"/>
       <c r="C409" s="110"/>
-      <c r="D409" s="167"/>
+      <c r="D409" s="167" t="s">
+        <v>773</v>
+      </c>
       <c r="E409" s="160"/>
-      <c r="F409" s="151"/>
-      <c r="G409" s="190"/>
-      <c r="H409" s="204"/>
+      <c r="F409" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G409" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H409" s="204">
+        <v>44984</v>
+      </c>
       <c r="I409" s="177"/>
     </row>
     <row r="410" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A410" s="1"/>
       <c r="B410" s="109"/>
       <c r="C410" s="110"/>
-      <c r="D410" s="165"/>
-      <c r="E410" s="155"/>
-      <c r="F410" s="148"/>
-      <c r="G410" s="186"/>
-      <c r="H410" s="201"/>
-      <c r="I410" s="174"/>
+      <c r="D410" s="167" t="s">
+        <v>772</v>
+      </c>
+      <c r="E410" s="160"/>
+      <c r="F410" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G410" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H410" s="204">
+        <v>44984</v>
+      </c>
+      <c r="I410" s="177"/>
     </row>
     <row r="411" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A411" s="1"/>
       <c r="B411" s="109"/>
-      <c r="C411" s="213" t="s">
-        <v>153</v>
-      </c>
-      <c r="D411" s="135"/>
-      <c r="E411" s="154"/>
-      <c r="F411" s="147"/>
-      <c r="G411" s="185"/>
-      <c r="H411" s="200"/>
-      <c r="I411" s="173"/>
+      <c r="C411" s="110"/>
+      <c r="D411" s="167"/>
+      <c r="E411" s="160"/>
+      <c r="F411" s="151"/>
+      <c r="G411" s="190"/>
+      <c r="H411" s="204"/>
+      <c r="I411" s="177"/>
     </row>
     <row r="412" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A412" s="1"/>
       <c r="B412" s="109"/>
-      <c r="C412" s="213"/>
-      <c r="D412" s="165"/>
-      <c r="E412" s="155"/>
-      <c r="F412" s="148"/>
-      <c r="G412" s="186"/>
-      <c r="H412" s="201"/>
-      <c r="I412" s="174"/>
+      <c r="C412" s="110"/>
+      <c r="D412" s="167"/>
+      <c r="E412" s="160"/>
+      <c r="F412" s="151"/>
+      <c r="G412" s="190"/>
+      <c r="H412" s="204"/>
+      <c r="I412" s="177"/>
     </row>
     <row r="413" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A413" s="1"/>
       <c r="B413" s="109"/>
       <c r="C413" s="110"/>
-      <c r="D413" s="165"/>
-      <c r="E413" s="155"/>
-      <c r="F413" s="148"/>
-      <c r="G413" s="186"/>
-      <c r="H413" s="201"/>
-      <c r="I413" s="174"/>
+      <c r="D413" s="167"/>
+      <c r="E413" s="160"/>
+      <c r="F413" s="151"/>
+      <c r="G413" s="190"/>
+      <c r="H413" s="204"/>
+      <c r="I413" s="177"/>
     </row>
     <row r="414" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A414" s="1"/>
       <c r="B414" s="109"/>
-      <c r="C414" s="213" t="s">
-        <v>154</v>
-      </c>
-      <c r="D414" s="135"/>
-      <c r="E414" s="154"/>
-      <c r="F414" s="147"/>
-      <c r="G414" s="185"/>
-      <c r="H414" s="200"/>
-      <c r="I414" s="173"/>
+      <c r="C414" s="110"/>
+      <c r="D414" s="167"/>
+      <c r="E414" s="160"/>
+      <c r="F414" s="151"/>
+      <c r="G414" s="190"/>
+      <c r="H414" s="204"/>
+      <c r="I414" s="177"/>
     </row>
     <row r="415" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A415" s="1"/>
       <c r="B415" s="109"/>
-      <c r="C415" s="213"/>
+      <c r="C415" s="110"/>
       <c r="D415" s="165"/>
       <c r="E415" s="155"/>
       <c r="F415" s="148"/>
@@ -12153,31 +12219,31 @@
     <row r="416" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A416" s="1"/>
       <c r="B416" s="109"/>
-      <c r="C416" s="110"/>
-      <c r="D416" s="165"/>
-      <c r="E416" s="155"/>
-      <c r="F416" s="148"/>
-      <c r="G416" s="186"/>
-      <c r="H416" s="201"/>
-      <c r="I416" s="174"/>
+      <c r="C416" s="213" t="s">
+        <v>153</v>
+      </c>
+      <c r="D416" s="135"/>
+      <c r="E416" s="154"/>
+      <c r="F416" s="147"/>
+      <c r="G416" s="185"/>
+      <c r="H416" s="200"/>
+      <c r="I416" s="173"/>
     </row>
     <row r="417" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A417" s="1"/>
       <c r="B417" s="109"/>
-      <c r="C417" s="213" t="s">
-        <v>155</v>
-      </c>
-      <c r="D417" s="135"/>
-      <c r="E417" s="154"/>
-      <c r="F417" s="147"/>
-      <c r="G417" s="185"/>
-      <c r="H417" s="200"/>
-      <c r="I417" s="173"/>
+      <c r="C417" s="213"/>
+      <c r="D417" s="165"/>
+      <c r="E417" s="155"/>
+      <c r="F417" s="148"/>
+      <c r="G417" s="186"/>
+      <c r="H417" s="201"/>
+      <c r="I417" s="174"/>
     </row>
     <row r="418" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A418" s="1"/>
       <c r="B418" s="109"/>
-      <c r="C418" s="213"/>
+      <c r="C418" s="110"/>
       <c r="D418" s="165"/>
       <c r="E418" s="155"/>
       <c r="F418" s="148"/>
@@ -12188,31 +12254,31 @@
     <row r="419" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A419" s="1"/>
       <c r="B419" s="109"/>
-      <c r="C419" s="110"/>
-      <c r="D419" s="165"/>
-      <c r="E419" s="155"/>
-      <c r="F419" s="148"/>
-      <c r="G419" s="186"/>
-      <c r="H419" s="201"/>
-      <c r="I419" s="174"/>
+      <c r="C419" s="213" t="s">
+        <v>154</v>
+      </c>
+      <c r="D419" s="135"/>
+      <c r="E419" s="154"/>
+      <c r="F419" s="147"/>
+      <c r="G419" s="185"/>
+      <c r="H419" s="200"/>
+      <c r="I419" s="173"/>
     </row>
     <row r="420" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A420" s="1"/>
       <c r="B420" s="109"/>
-      <c r="C420" s="213" t="s">
-        <v>156</v>
-      </c>
-      <c r="D420" s="135"/>
-      <c r="E420" s="154"/>
-      <c r="F420" s="147"/>
-      <c r="G420" s="185"/>
-      <c r="H420" s="200"/>
-      <c r="I420" s="173"/>
+      <c r="C420" s="213"/>
+      <c r="D420" s="165"/>
+      <c r="E420" s="155"/>
+      <c r="F420" s="148"/>
+      <c r="G420" s="186"/>
+      <c r="H420" s="201"/>
+      <c r="I420" s="174"/>
     </row>
     <row r="421" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A421" s="1"/>
       <c r="B421" s="109"/>
-      <c r="C421" s="213"/>
+      <c r="C421" s="110"/>
       <c r="D421" s="165"/>
       <c r="E421" s="155"/>
       <c r="F421" s="148"/>
@@ -12223,31 +12289,31 @@
     <row r="422" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A422" s="1"/>
       <c r="B422" s="109"/>
-      <c r="C422" s="110"/>
-      <c r="D422" s="165"/>
-      <c r="E422" s="155"/>
-      <c r="F422" s="148"/>
-      <c r="G422" s="186"/>
-      <c r="H422" s="201"/>
-      <c r="I422" s="174"/>
+      <c r="C422" s="213" t="s">
+        <v>155</v>
+      </c>
+      <c r="D422" s="135"/>
+      <c r="E422" s="154"/>
+      <c r="F422" s="147"/>
+      <c r="G422" s="185"/>
+      <c r="H422" s="200"/>
+      <c r="I422" s="173"/>
     </row>
     <row r="423" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A423" s="1"/>
       <c r="B423" s="109"/>
-      <c r="C423" s="213" t="s">
-        <v>157</v>
-      </c>
-      <c r="D423" s="135"/>
-      <c r="E423" s="154"/>
-      <c r="F423" s="147"/>
-      <c r="G423" s="185"/>
-      <c r="H423" s="200"/>
-      <c r="I423" s="173"/>
+      <c r="C423" s="213"/>
+      <c r="D423" s="165"/>
+      <c r="E423" s="155"/>
+      <c r="F423" s="148"/>
+      <c r="G423" s="186"/>
+      <c r="H423" s="201"/>
+      <c r="I423" s="174"/>
     </row>
     <row r="424" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A424" s="1"/>
       <c r="B424" s="109"/>
-      <c r="C424" s="213"/>
+      <c r="C424" s="110"/>
       <c r="D424" s="165"/>
       <c r="E424" s="155"/>
       <c r="F424" s="148"/>
@@ -12255,33 +12321,23 @@
       <c r="H424" s="201"/>
       <c r="I424" s="174"/>
     </row>
-    <row r="425" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A425" s="1"/>
       <c r="B425" s="109"/>
-      <c r="C425" s="110"/>
-      <c r="D425" s="166" t="s">
-        <v>697</v>
-      </c>
-      <c r="E425" s="157" t="s">
-        <v>698</v>
-      </c>
-      <c r="F425" s="150" t="s">
-        <v>699</v>
-      </c>
-      <c r="G425" s="188">
-        <v>44859</v>
-      </c>
-      <c r="H425" s="203">
-        <v>44477</v>
-      </c>
-      <c r="I425" s="171" t="s">
-        <v>700</v>
-      </c>
+      <c r="C425" s="213" t="s">
+        <v>156</v>
+      </c>
+      <c r="D425" s="135"/>
+      <c r="E425" s="154"/>
+      <c r="F425" s="147"/>
+      <c r="G425" s="185"/>
+      <c r="H425" s="200"/>
+      <c r="I425" s="173"/>
     </row>
     <row r="426" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A426" s="1"/>
       <c r="B426" s="109"/>
-      <c r="C426" s="110"/>
+      <c r="C426" s="213"/>
       <c r="D426" s="165"/>
       <c r="E426" s="155"/>
       <c r="F426" s="148"/>
@@ -12292,151 +12348,105 @@
     <row r="427" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A427" s="1"/>
       <c r="B427" s="109"/>
-      <c r="C427" s="213" t="s">
-        <v>158</v>
-      </c>
-      <c r="D427" s="135"/>
-      <c r="E427" s="154"/>
-      <c r="F427" s="147"/>
-      <c r="G427" s="185"/>
-      <c r="H427" s="200"/>
-      <c r="I427" s="173"/>
+      <c r="C427" s="110"/>
+      <c r="D427" s="165"/>
+      <c r="E427" s="155"/>
+      <c r="F427" s="148"/>
+      <c r="G427" s="186"/>
+      <c r="H427" s="201"/>
+      <c r="I427" s="174"/>
     </row>
     <row r="428" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A428" s="1"/>
       <c r="B428" s="109"/>
-      <c r="C428" s="213"/>
-      <c r="D428" s="166" t="s">
-        <v>466</v>
-      </c>
-      <c r="E428" s="162" t="s">
-        <v>467</v>
-      </c>
-      <c r="F428" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G428" s="188">
-        <v>44663</v>
-      </c>
-      <c r="H428" s="203">
-        <v>44663</v>
-      </c>
-      <c r="I428" s="198" t="s">
-        <v>759</v>
-      </c>
+      <c r="C428" s="213" t="s">
+        <v>157</v>
+      </c>
+      <c r="D428" s="135"/>
+      <c r="E428" s="154"/>
+      <c r="F428" s="147"/>
+      <c r="G428" s="185"/>
+      <c r="H428" s="200"/>
+      <c r="I428" s="173"/>
     </row>
     <row r="429" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A429" s="1"/>
       <c r="B429" s="109"/>
-      <c r="C429" s="110"/>
-      <c r="D429" s="167" t="s">
-        <v>468</v>
-      </c>
-      <c r="E429" s="160" t="s">
-        <v>469</v>
-      </c>
-      <c r="F429" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G429" s="190">
-        <v>44663</v>
-      </c>
-      <c r="H429" s="204">
-        <v>44663</v>
-      </c>
-      <c r="I429" s="199" t="s">
-        <v>759</v>
-      </c>
-    </row>
-    <row r="430" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C429" s="213"/>
+      <c r="D429" s="165"/>
+      <c r="E429" s="155"/>
+      <c r="F429" s="148"/>
+      <c r="G429" s="186"/>
+      <c r="H429" s="201"/>
+      <c r="I429" s="174"/>
+    </row>
+    <row r="430" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A430" s="1"/>
       <c r="B430" s="109"/>
       <c r="C430" s="110"/>
-      <c r="D430" s="167" t="s">
-        <v>471</v>
-      </c>
-      <c r="E430" s="160" t="s">
-        <v>470</v>
-      </c>
-      <c r="F430" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G430" s="190">
-        <v>44630</v>
-      </c>
-      <c r="H430" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I430" s="199" t="s">
-        <v>759</v>
+      <c r="D430" s="166" t="s">
+        <v>697</v>
+      </c>
+      <c r="E430" s="157" t="s">
+        <v>698</v>
+      </c>
+      <c r="F430" s="150" t="s">
+        <v>699</v>
+      </c>
+      <c r="G430" s="188">
+        <v>44859</v>
+      </c>
+      <c r="H430" s="203">
+        <v>44477</v>
+      </c>
+      <c r="I430" s="171" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="431" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A431" s="1"/>
       <c r="B431" s="109"/>
       <c r="C431" s="110"/>
-      <c r="D431" s="167" t="s">
-        <v>472</v>
-      </c>
-      <c r="E431" s="160" t="s">
-        <v>473</v>
-      </c>
-      <c r="F431" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G431" s="190">
-        <v>44630</v>
-      </c>
-      <c r="H431" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I431" s="199" t="s">
-        <v>759</v>
-      </c>
+      <c r="D431" s="165"/>
+      <c r="E431" s="155"/>
+      <c r="F431" s="148"/>
+      <c r="G431" s="186"/>
+      <c r="H431" s="201"/>
+      <c r="I431" s="174"/>
     </row>
     <row r="432" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A432" s="1"/>
       <c r="B432" s="109"/>
-      <c r="C432" s="110"/>
-      <c r="D432" s="167" t="s">
-        <v>474</v>
-      </c>
-      <c r="E432" s="160" t="s">
-        <v>475</v>
-      </c>
-      <c r="F432" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G432" s="190">
-        <v>44698</v>
-      </c>
-      <c r="H432" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I432" s="199" t="s">
-        <v>759</v>
-      </c>
+      <c r="C432" s="213" t="s">
+        <v>158</v>
+      </c>
+      <c r="D432" s="135"/>
+      <c r="E432" s="154"/>
+      <c r="F432" s="147"/>
+      <c r="G432" s="185"/>
+      <c r="H432" s="200"/>
+      <c r="I432" s="173"/>
     </row>
     <row r="433" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A433" s="1"/>
       <c r="B433" s="109"/>
-      <c r="C433" s="110"/>
-      <c r="D433" s="167" t="s">
-        <v>476</v>
-      </c>
-      <c r="E433" s="160" t="s">
-        <v>477</v>
-      </c>
-      <c r="F433" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G433" s="190">
-        <v>44698</v>
-      </c>
-      <c r="H433" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I433" s="199" t="s">
+      <c r="C433" s="213"/>
+      <c r="D433" s="166" t="s">
+        <v>466</v>
+      </c>
+      <c r="E433" s="162" t="s">
+        <v>467</v>
+      </c>
+      <c r="F433" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G433" s="188">
+        <v>44663</v>
+      </c>
+      <c r="H433" s="203">
+        <v>44663</v>
+      </c>
+      <c r="I433" s="198" t="s">
         <v>759</v>
       </c>
     </row>
@@ -12445,19 +12455,19 @@
       <c r="B434" s="109"/>
       <c r="C434" s="110"/>
       <c r="D434" s="167" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="E434" s="160" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="F434" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G434" s="190">
-        <v>44669</v>
+        <v>44663</v>
       </c>
       <c r="H434" s="204">
-        <v>44824</v>
+        <v>44663</v>
       </c>
       <c r="I434" s="199" t="s">
         <v>759</v>
@@ -12468,19 +12478,19 @@
       <c r="B435" s="109"/>
       <c r="C435" s="110"/>
       <c r="D435" s="167" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="E435" s="160" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="F435" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G435" s="190">
-        <v>44669</v>
+        <v>44630</v>
       </c>
       <c r="H435" s="204">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I435" s="199" t="s">
         <v>759</v>
@@ -12491,19 +12501,19 @@
       <c r="B436" s="109"/>
       <c r="C436" s="110"/>
       <c r="D436" s="167" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="E436" s="160" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="F436" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G436" s="190">
-        <v>44733</v>
+        <v>44630</v>
       </c>
       <c r="H436" s="204">
-        <v>44622</v>
+        <v>44630</v>
       </c>
       <c r="I436" s="199" t="s">
         <v>759</v>
@@ -12514,19 +12524,19 @@
       <c r="B437" s="109"/>
       <c r="C437" s="110"/>
       <c r="D437" s="167" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="E437" s="160" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="F437" s="151" t="s">
-        <v>459</v>
+        <v>281</v>
       </c>
       <c r="G437" s="190">
-        <v>44733</v>
+        <v>44698</v>
       </c>
       <c r="H437" s="204">
-        <v>44621</v>
+        <v>44630</v>
       </c>
       <c r="I437" s="199" t="s">
         <v>759</v>
@@ -12537,19 +12547,19 @@
       <c r="B438" s="109"/>
       <c r="C438" s="110"/>
       <c r="D438" s="167" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="E438" s="160" t="s">
-        <v>488</v>
+        <v>477</v>
       </c>
       <c r="F438" s="151" t="s">
-        <v>459</v>
+        <v>281</v>
       </c>
       <c r="G438" s="190">
-        <v>44671</v>
+        <v>44698</v>
       </c>
       <c r="H438" s="204">
-        <v>44732</v>
+        <v>44630</v>
       </c>
       <c r="I438" s="199" t="s">
         <v>759</v>
@@ -12560,19 +12570,19 @@
       <c r="B439" s="109"/>
       <c r="C439" s="110"/>
       <c r="D439" s="167" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="E439" s="160" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="F439" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G439" s="190">
-        <v>44671</v>
+        <v>44669</v>
       </c>
       <c r="H439" s="204">
-        <v>44732</v>
+        <v>44824</v>
       </c>
       <c r="I439" s="199" t="s">
         <v>759</v>
@@ -12583,19 +12593,19 @@
       <c r="B440" s="109"/>
       <c r="C440" s="110"/>
       <c r="D440" s="167" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="E440" s="160" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="F440" s="151" t="s">
-        <v>492</v>
+        <v>256</v>
       </c>
       <c r="G440" s="190">
-        <v>44698</v>
+        <v>44669</v>
       </c>
       <c r="H440" s="204">
-        <v>44621</v>
+        <v>44824</v>
       </c>
       <c r="I440" s="199" t="s">
         <v>759</v>
@@ -12606,19 +12616,19 @@
       <c r="B441" s="109"/>
       <c r="C441" s="110"/>
       <c r="D441" s="167" t="s">
-        <v>494</v>
+        <v>482</v>
       </c>
       <c r="E441" s="160" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="F441" s="151" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="G441" s="190">
-        <v>44698</v>
+        <v>44733</v>
       </c>
       <c r="H441" s="204">
-        <v>44621</v>
+        <v>44622</v>
       </c>
       <c r="I441" s="199" t="s">
         <v>759</v>
@@ -12629,19 +12639,19 @@
       <c r="B442" s="109"/>
       <c r="C442" s="110"/>
       <c r="D442" s="167" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="E442" s="160" t="s">
-        <v>497</v>
+        <v>485</v>
       </c>
       <c r="F442" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G442" s="190">
-        <v>44644</v>
+        <v>44733</v>
       </c>
       <c r="H442" s="204">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="I442" s="199" t="s">
         <v>759</v>
@@ -12652,19 +12662,19 @@
       <c r="B443" s="109"/>
       <c r="C443" s="110"/>
       <c r="D443" s="167" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="E443" s="160" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="F443" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G443" s="190">
-        <v>44644</v>
+        <v>44671</v>
       </c>
       <c r="H443" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I443" s="199" t="s">
         <v>759</v>
@@ -12675,19 +12685,19 @@
       <c r="B444" s="109"/>
       <c r="C444" s="110"/>
       <c r="D444" s="167" t="s">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="E444" s="160" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="F444" s="151" t="s">
         <v>459</v>
       </c>
       <c r="G444" s="190">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H444" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I444" s="199" t="s">
         <v>759</v>
@@ -12698,13 +12708,13 @@
       <c r="B445" s="109"/>
       <c r="C445" s="110"/>
       <c r="D445" s="167" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="E445" s="160" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="F445" s="151" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="G445" s="190">
         <v>44698</v>
@@ -12721,19 +12731,19 @@
       <c r="B446" s="109"/>
       <c r="C446" s="110"/>
       <c r="D446" s="167" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="E446" s="160" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
       <c r="F446" s="151" t="s">
-        <v>267</v>
+        <v>492</v>
       </c>
       <c r="G446" s="190">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H446" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I446" s="199" t="s">
         <v>759</v>
@@ -12744,19 +12754,19 @@
       <c r="B447" s="109"/>
       <c r="C447" s="110"/>
       <c r="D447" s="167" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="E447" s="160" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="F447" s="151" t="s">
         <v>267</v>
       </c>
       <c r="G447" s="190">
-        <v>44846</v>
+        <v>44644</v>
       </c>
       <c r="H447" s="204">
-        <v>44627</v>
+        <v>44622</v>
       </c>
       <c r="I447" s="199" t="s">
         <v>759</v>
@@ -12767,19 +12777,19 @@
       <c r="B448" s="109"/>
       <c r="C448" s="110"/>
       <c r="D448" s="167" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="E448" s="160" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="F448" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G448" s="190">
-        <v>44628</v>
+        <v>44644</v>
       </c>
       <c r="H448" s="204">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I448" s="199" t="s">
         <v>759</v>
@@ -12790,19 +12800,19 @@
       <c r="B449" s="109"/>
       <c r="C449" s="110"/>
       <c r="D449" s="167" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="E449" s="160" t="s">
-        <v>510</v>
+        <v>499</v>
       </c>
       <c r="F449" s="151" t="s">
-        <v>232</v>
+        <v>459</v>
       </c>
       <c r="G449" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H449" s="204">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I449" s="199" t="s">
         <v>759</v>
@@ -12813,19 +12823,19 @@
       <c r="B450" s="109"/>
       <c r="C450" s="110"/>
       <c r="D450" s="167" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="E450" s="160" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="F450" s="151" t="s">
-        <v>281</v>
+        <v>459</v>
       </c>
       <c r="G450" s="190">
         <v>44698</v>
       </c>
       <c r="H450" s="204">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I450" s="199" t="s">
         <v>759</v>
@@ -12836,19 +12846,19 @@
       <c r="B451" s="109"/>
       <c r="C451" s="110"/>
       <c r="D451" s="167" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="E451" s="160" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="F451" s="151" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G451" s="190">
-        <v>44698</v>
+        <v>44846</v>
       </c>
       <c r="H451" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I451" s="199" t="s">
         <v>759</v>
@@ -12859,19 +12869,19 @@
       <c r="B452" s="109"/>
       <c r="C452" s="110"/>
       <c r="D452" s="167" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="E452" s="160" t="s">
-        <v>517</v>
+        <v>506</v>
       </c>
       <c r="F452" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G452" s="190">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H452" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I452" s="199" t="s">
         <v>759</v>
@@ -12882,10 +12892,10 @@
       <c r="B453" s="109"/>
       <c r="C453" s="110"/>
       <c r="D453" s="167" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="E453" s="160" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="F453" s="151" t="s">
         <v>232</v>
@@ -12905,16 +12915,16 @@
       <c r="B454" s="109"/>
       <c r="C454" s="110"/>
       <c r="D454" s="167" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="E454" s="160" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="F454" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G454" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H454" s="204">
         <v>44628</v>
@@ -12928,10 +12938,10 @@
       <c r="B455" s="109"/>
       <c r="C455" s="110"/>
       <c r="D455" s="167" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="E455" s="160" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="F455" s="151" t="s">
         <v>281</v>
@@ -12951,19 +12961,19 @@
       <c r="B456" s="109"/>
       <c r="C456" s="110"/>
       <c r="D456" s="167" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="E456" s="160" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="F456" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G456" s="190">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H456" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I456" s="199" t="s">
         <v>759</v>
@@ -12974,19 +12984,19 @@
       <c r="B457" s="109"/>
       <c r="C457" s="110"/>
       <c r="D457" s="167" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="E457" s="160" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="F457" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G457" s="190">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="H457" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I457" s="199" t="s">
         <v>759</v>
@@ -12997,19 +13007,19 @@
       <c r="B458" s="109"/>
       <c r="C458" s="110"/>
       <c r="D458" s="167" t="s">
-        <v>527</v>
+        <v>516</v>
       </c>
       <c r="E458" s="160" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="F458" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G458" s="190">
-        <v>44740</v>
+        <v>44628</v>
       </c>
       <c r="H458" s="204">
-        <v>44662</v>
+        <v>44628</v>
       </c>
       <c r="I458" s="199" t="s">
         <v>759</v>
@@ -13020,19 +13030,19 @@
       <c r="B459" s="109"/>
       <c r="C459" s="110"/>
       <c r="D459" s="167" t="s">
-        <v>530</v>
+        <v>519</v>
       </c>
       <c r="E459" s="160" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="F459" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G459" s="190">
-        <v>44740</v>
+        <v>44698</v>
       </c>
       <c r="H459" s="204">
-        <v>44662</v>
+        <v>44628</v>
       </c>
       <c r="I459" s="199" t="s">
         <v>759</v>
@@ -13042,88 +13052,116 @@
       <c r="A460" s="1"/>
       <c r="B460" s="109"/>
       <c r="C460" s="110"/>
-      <c r="D460" s="165"/>
-      <c r="E460" s="155"/>
-      <c r="F460" s="148"/>
-      <c r="G460" s="186"/>
-      <c r="H460" s="201"/>
-      <c r="I460" s="174"/>
+      <c r="D460" s="167" t="s">
+        <v>521</v>
+      </c>
+      <c r="E460" s="160" t="s">
+        <v>522</v>
+      </c>
+      <c r="F460" s="151" t="s">
+        <v>281</v>
+      </c>
+      <c r="G460" s="190">
+        <v>44698</v>
+      </c>
+      <c r="H460" s="204">
+        <v>44628</v>
+      </c>
+      <c r="I460" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="461" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A461" s="1"/>
       <c r="B461" s="109"/>
-      <c r="C461" s="213" t="s">
-        <v>147</v>
-      </c>
-      <c r="D461" s="135"/>
-      <c r="E461" s="154"/>
-      <c r="F461" s="147"/>
-      <c r="G461" s="185"/>
-      <c r="H461" s="200"/>
-      <c r="I461" s="173"/>
+      <c r="C461" s="110"/>
+      <c r="D461" s="167" t="s">
+        <v>523</v>
+      </c>
+      <c r="E461" s="160" t="s">
+        <v>524</v>
+      </c>
+      <c r="F461" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G461" s="190">
+        <v>44617</v>
+      </c>
+      <c r="H461" s="204">
+        <v>44617</v>
+      </c>
+      <c r="I461" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="462" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A462" s="1"/>
       <c r="B462" s="109"/>
-      <c r="C462" s="213"/>
-      <c r="D462" s="166" t="s">
-        <v>274</v>
-      </c>
-      <c r="E462" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="F462" s="150" t="s">
+      <c r="C462" s="110"/>
+      <c r="D462" s="167" t="s">
+        <v>526</v>
+      </c>
+      <c r="E462" s="160" t="s">
+        <v>525</v>
+      </c>
+      <c r="F462" s="151" t="s">
         <v>232</v>
       </c>
-      <c r="G462" s="188">
-        <v>44167</v>
-      </c>
-      <c r="H462" s="203">
-        <v>44167</v>
-      </c>
-      <c r="I462" s="176"/>
+      <c r="G462" s="190">
+        <v>44617</v>
+      </c>
+      <c r="H462" s="204">
+        <v>44617</v>
+      </c>
+      <c r="I462" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="463" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A463" s="1"/>
       <c r="B463" s="109"/>
       <c r="C463" s="110"/>
       <c r="D463" s="167" t="s">
-        <v>445</v>
+        <v>527</v>
       </c>
       <c r="E463" s="160" t="s">
-        <v>446</v>
+        <v>528</v>
       </c>
       <c r="F463" s="151" t="s">
         <v>256</v>
       </c>
       <c r="G463" s="190">
-        <v>44575</v>
+        <v>44740</v>
       </c>
       <c r="H463" s="204">
-        <v>44167</v>
-      </c>
-      <c r="I463" s="177"/>
-    </row>
-    <row r="464" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>44662</v>
+      </c>
+      <c r="I463" s="199" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="464" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A464" s="1"/>
       <c r="B464" s="109"/>
       <c r="C464" s="110"/>
       <c r="D464" s="167" t="s">
-        <v>448</v>
-      </c>
-      <c r="E464" s="158" t="s">
-        <v>447</v>
+        <v>530</v>
+      </c>
+      <c r="E464" s="160" t="s">
+        <v>529</v>
       </c>
       <c r="F464" s="151" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G464" s="190">
-        <v>44404</v>
+        <v>44740</v>
       </c>
       <c r="H464" s="204">
-        <v>44404</v>
-      </c>
-      <c r="I464" s="177"/>
+        <v>44662</v>
+      </c>
+      <c r="I464" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="465" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A465" s="1"/>
@@ -13140,7 +13178,7 @@
       <c r="A466" s="1"/>
       <c r="B466" s="109"/>
       <c r="C466" s="213" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D466" s="135"/>
       <c r="E466" s="154"/>
@@ -13154,19 +13192,19 @@
       <c r="B467" s="109"/>
       <c r="C467" s="213"/>
       <c r="D467" s="166" t="s">
-        <v>450</v>
+        <v>274</v>
       </c>
       <c r="E467" s="162" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="F467" s="150" t="s">
         <v>232</v>
       </c>
       <c r="G467" s="188">
-        <v>44635</v>
+        <v>44167</v>
       </c>
       <c r="H467" s="203">
-        <v>44635</v>
+        <v>44167</v>
       </c>
       <c r="I467" s="176"/>
     </row>
@@ -13175,40 +13213,40 @@
       <c r="B468" s="109"/>
       <c r="C468" s="110"/>
       <c r="D468" s="167" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="E468" s="160" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="F468" s="151" t="s">
-        <v>232</v>
+        <v>256</v>
       </c>
       <c r="G468" s="190">
-        <v>44635</v>
+        <v>44575</v>
       </c>
       <c r="H468" s="204">
-        <v>44635</v>
+        <v>44167</v>
       </c>
       <c r="I468" s="177"/>
     </row>
-    <row r="469" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A469" s="1"/>
       <c r="B469" s="109"/>
       <c r="C469" s="110"/>
       <c r="D469" s="167" t="s">
-        <v>453</v>
-      </c>
-      <c r="E469" s="160" t="s">
-        <v>455</v>
+        <v>448</v>
+      </c>
+      <c r="E469" s="158" t="s">
+        <v>447</v>
       </c>
       <c r="F469" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G469" s="190">
-        <v>44635</v>
+        <v>44404</v>
       </c>
       <c r="H469" s="204">
-        <v>44635</v>
+        <v>44404</v>
       </c>
       <c r="I469" s="177"/>
     </row>
@@ -13216,83 +13254,65 @@
       <c r="A470" s="1"/>
       <c r="B470" s="109"/>
       <c r="C470" s="110"/>
-      <c r="D470" s="167" t="s">
-        <v>454</v>
-      </c>
-      <c r="E470" s="160" t="s">
-        <v>456</v>
-      </c>
-      <c r="F470" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G470" s="190">
-        <v>44635</v>
-      </c>
-      <c r="H470" s="204">
-        <v>44635</v>
-      </c>
-      <c r="I470" s="177"/>
+      <c r="D470" s="165"/>
+      <c r="E470" s="155"/>
+      <c r="F470" s="148"/>
+      <c r="G470" s="186"/>
+      <c r="H470" s="201"/>
+      <c r="I470" s="174"/>
     </row>
     <row r="471" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A471" s="1"/>
       <c r="B471" s="109"/>
-      <c r="C471" s="110"/>
-      <c r="D471" s="167" t="s">
-        <v>457</v>
-      </c>
-      <c r="E471" s="160" t="s">
-        <v>460</v>
-      </c>
-      <c r="F471" s="151" t="s">
-        <v>459</v>
-      </c>
-      <c r="G471" s="190">
-        <v>44701</v>
-      </c>
-      <c r="H471" s="204">
-        <v>44644</v>
-      </c>
-      <c r="I471" s="177"/>
+      <c r="C471" s="213" t="s">
+        <v>159</v>
+      </c>
+      <c r="D471" s="135"/>
+      <c r="E471" s="154"/>
+      <c r="F471" s="147"/>
+      <c r="G471" s="185"/>
+      <c r="H471" s="200"/>
+      <c r="I471" s="173"/>
     </row>
     <row r="472" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A472" s="1"/>
       <c r="B472" s="109"/>
-      <c r="C472" s="110"/>
-      <c r="D472" s="167" t="s">
-        <v>458</v>
-      </c>
-      <c r="E472" s="160" t="s">
-        <v>461</v>
-      </c>
-      <c r="F472" s="151" t="s">
-        <v>459</v>
-      </c>
-      <c r="G472" s="190">
-        <v>44701</v>
-      </c>
-      <c r="H472" s="204">
-        <v>44644</v>
-      </c>
-      <c r="I472" s="177"/>
+      <c r="C472" s="213"/>
+      <c r="D472" s="166" t="s">
+        <v>450</v>
+      </c>
+      <c r="E472" s="162" t="s">
+        <v>449</v>
+      </c>
+      <c r="F472" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G472" s="188">
+        <v>44635</v>
+      </c>
+      <c r="H472" s="203">
+        <v>44635</v>
+      </c>
+      <c r="I472" s="176"/>
     </row>
     <row r="473" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A473" s="1"/>
       <c r="B473" s="109"/>
       <c r="C473" s="110"/>
       <c r="D473" s="167" t="s">
-        <v>462</v>
+        <v>452</v>
       </c>
       <c r="E473" s="160" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="F473" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G473" s="190">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H473" s="204">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="I473" s="177"/>
     </row>
@@ -13301,19 +13321,19 @@
       <c r="B474" s="109"/>
       <c r="C474" s="110"/>
       <c r="D474" s="167" t="s">
-        <v>464</v>
+        <v>453</v>
       </c>
       <c r="E474" s="160" t="s">
-        <v>465</v>
+        <v>455</v>
       </c>
       <c r="F474" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G474" s="190">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H474" s="204">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="I474" s="177"/>
     </row>
@@ -13321,319 +13341,393 @@
       <c r="A475" s="1"/>
       <c r="B475" s="109"/>
       <c r="C475" s="110"/>
-      <c r="D475" s="165"/>
-      <c r="E475" s="155"/>
-      <c r="F475" s="148"/>
-      <c r="G475" s="186"/>
-      <c r="H475" s="201"/>
-      <c r="I475" s="174"/>
-    </row>
-    <row r="476" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A476" s="136"/>
-      <c r="B476" s="212" t="s">
-        <v>144</v>
-      </c>
-      <c r="C476" s="134"/>
-      <c r="D476" s="135"/>
-      <c r="E476" s="154"/>
-      <c r="F476" s="147"/>
-      <c r="G476" s="185"/>
-      <c r="H476" s="200"/>
-      <c r="I476" s="173"/>
-    </row>
-    <row r="477" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A477" s="136"/>
-      <c r="B477" s="212"/>
-      <c r="C477" s="213" t="s">
-        <v>146</v>
-      </c>
-      <c r="D477" s="135"/>
-      <c r="E477" s="154"/>
-      <c r="F477" s="147"/>
-      <c r="G477" s="185"/>
-      <c r="H477" s="200"/>
-      <c r="I477" s="173"/>
+      <c r="D475" s="167" t="s">
+        <v>454</v>
+      </c>
+      <c r="E475" s="160" t="s">
+        <v>456</v>
+      </c>
+      <c r="F475" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G475" s="190">
+        <v>44635</v>
+      </c>
+      <c r="H475" s="204">
+        <v>44635</v>
+      </c>
+      <c r="I475" s="177"/>
+    </row>
+    <row r="476" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A476" s="1"/>
+      <c r="B476" s="109"/>
+      <c r="C476" s="110"/>
+      <c r="D476" s="167" t="s">
+        <v>457</v>
+      </c>
+      <c r="E476" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="F476" s="151" t="s">
+        <v>459</v>
+      </c>
+      <c r="G476" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H476" s="204">
+        <v>44644</v>
+      </c>
+      <c r="I476" s="177"/>
+    </row>
+    <row r="477" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A477" s="1"/>
+      <c r="B477" s="109"/>
+      <c r="C477" s="110"/>
+      <c r="D477" s="167" t="s">
+        <v>458</v>
+      </c>
+      <c r="E477" s="160" t="s">
+        <v>461</v>
+      </c>
+      <c r="F477" s="151" t="s">
+        <v>459</v>
+      </c>
+      <c r="G477" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H477" s="204">
+        <v>44644</v>
+      </c>
+      <c r="I477" s="177"/>
     </row>
     <row r="478" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A478" s="1"/>
       <c r="B478" s="109"/>
-      <c r="C478" s="213"/>
-      <c r="D478" s="165"/>
-      <c r="E478" s="155"/>
-      <c r="F478" s="148"/>
-      <c r="G478" s="186"/>
-      <c r="H478" s="201"/>
-      <c r="I478" s="174"/>
+      <c r="C478" s="110"/>
+      <c r="D478" s="167" t="s">
+        <v>462</v>
+      </c>
+      <c r="E478" s="160" t="s">
+        <v>463</v>
+      </c>
+      <c r="F478" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G478" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H478" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I478" s="177"/>
     </row>
     <row r="479" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A479" s="1"/>
       <c r="B479" s="109"/>
       <c r="C479" s="110"/>
-      <c r="D479" s="165"/>
-      <c r="E479" s="155"/>
-      <c r="F479" s="148"/>
-      <c r="G479" s="186"/>
-      <c r="H479" s="201"/>
-      <c r="I479" s="174"/>
-    </row>
-    <row r="480" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D479" s="167" t="s">
+        <v>464</v>
+      </c>
+      <c r="E479" s="160" t="s">
+        <v>465</v>
+      </c>
+      <c r="F479" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G479" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H479" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I479" s="177"/>
+    </row>
+    <row r="480" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A480" s="1"/>
       <c r="B480" s="109"/>
       <c r="C480" s="110"/>
-      <c r="D480" s="144"/>
-      <c r="E480" s="156"/>
-      <c r="F480" s="149"/>
-      <c r="G480" s="187"/>
-      <c r="H480" s="202"/>
-      <c r="I480" s="175"/>
-    </row>
-    <row r="481" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D480" s="165"/>
+      <c r="E480" s="155"/>
+      <c r="F480" s="148"/>
+      <c r="G480" s="186"/>
+      <c r="H480" s="201"/>
+      <c r="I480" s="174"/>
+    </row>
+    <row r="481" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A481" s="136"/>
-      <c r="B481" s="109"/>
-      <c r="C481" s="110"/>
-      <c r="D481" s="166" t="s">
-        <v>858</v>
-      </c>
-      <c r="E481" s="162" t="s">
-        <v>860</v>
-      </c>
-      <c r="F481" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G481" s="188">
-        <v>44950</v>
-      </c>
-      <c r="H481" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I481" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="482" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B481" s="212" t="s">
+        <v>144</v>
+      </c>
+      <c r="C481" s="134"/>
+      <c r="D481" s="135"/>
+      <c r="E481" s="154"/>
+      <c r="F481" s="147"/>
+      <c r="G481" s="185"/>
+      <c r="H481" s="200"/>
+      <c r="I481" s="173"/>
+    </row>
+    <row r="482" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A482" s="136"/>
-      <c r="B482" s="109"/>
-      <c r="C482" s="110"/>
-      <c r="D482" s="167" t="s">
-        <v>859</v>
-      </c>
-      <c r="E482" s="158" t="s">
-        <v>861</v>
-      </c>
-      <c r="F482" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G482" s="190">
-        <v>44950</v>
-      </c>
-      <c r="H482" s="204">
-        <v>44893</v>
-      </c>
-      <c r="I482" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="483" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A483" s="136"/>
+      <c r="B482" s="212"/>
+      <c r="C482" s="213" t="s">
+        <v>146</v>
+      </c>
+      <c r="D482" s="135"/>
+      <c r="E482" s="154"/>
+      <c r="F482" s="147"/>
+      <c r="G482" s="185"/>
+      <c r="H482" s="200"/>
+      <c r="I482" s="173"/>
+    </row>
+    <row r="483" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A483" s="1"/>
       <c r="B483" s="109"/>
-      <c r="C483" s="110"/>
-      <c r="D483" s="166" t="s">
-        <v>862</v>
-      </c>
-      <c r="E483" s="157" t="s">
-        <v>864</v>
-      </c>
-      <c r="F483" s="150" t="s">
-        <v>548</v>
-      </c>
-      <c r="G483" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H483" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I483" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="484" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A484" s="136"/>
+      <c r="C483" s="213"/>
+      <c r="D483" s="165"/>
+      <c r="E483" s="155"/>
+      <c r="F483" s="148"/>
+      <c r="G483" s="186"/>
+      <c r="H483" s="201"/>
+      <c r="I483" s="174"/>
+    </row>
+    <row r="484" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A484" s="1"/>
       <c r="B484" s="109"/>
       <c r="C484" s="110"/>
-      <c r="D484" s="166" t="s">
-        <v>863</v>
-      </c>
-      <c r="E484" s="157" t="s">
-        <v>865</v>
-      </c>
-      <c r="F484" s="150" t="s">
-        <v>548</v>
-      </c>
-      <c r="G484" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H484" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I484" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="485" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A485" s="136"/>
+      <c r="D484" s="165"/>
+      <c r="E484" s="155"/>
+      <c r="F484" s="148"/>
+      <c r="G484" s="186"/>
+      <c r="H484" s="201"/>
+      <c r="I484" s="174"/>
+    </row>
+    <row r="485" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A485" s="1"/>
       <c r="B485" s="109"/>
       <c r="C485" s="110"/>
-      <c r="D485" s="166" t="s">
-        <v>854</v>
-      </c>
-      <c r="E485" s="162" t="s">
-        <v>857</v>
-      </c>
-      <c r="F485" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G485" s="188">
-        <v>44986</v>
-      </c>
-      <c r="H485" s="203">
-        <v>44951</v>
-      </c>
-      <c r="I485" s="171" t="s">
-        <v>727</v>
-      </c>
+      <c r="D485" s="144"/>
+      <c r="E485" s="156"/>
+      <c r="F485" s="149"/>
+      <c r="G485" s="187"/>
+      <c r="H485" s="202"/>
+      <c r="I485" s="175"/>
     </row>
     <row r="486" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A486" s="136"/>
       <c r="B486" s="109"/>
       <c r="C486" s="110"/>
-      <c r="D486" s="167" t="s">
-        <v>855</v>
-      </c>
-      <c r="E486" s="158" t="s">
-        <v>856</v>
-      </c>
-      <c r="F486" s="151" t="s">
+      <c r="D486" s="166" t="s">
+        <v>858</v>
+      </c>
+      <c r="E486" s="162" t="s">
+        <v>860</v>
+      </c>
+      <c r="F486" s="150" t="s">
         <v>267</v>
       </c>
-      <c r="G486" s="190">
-        <v>44986</v>
-      </c>
-      <c r="H486" s="204">
-        <v>44951</v>
+      <c r="G486" s="188">
+        <v>44950</v>
+      </c>
+      <c r="H486" s="203">
+        <v>44893</v>
       </c>
       <c r="I486" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="487" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A487" s="136"/>
-      <c r="B487" s="111"/>
-      <c r="C487" s="112"/>
-      <c r="D487" s="170"/>
-      <c r="E487" s="163"/>
-      <c r="F487" s="153"/>
-      <c r="G487" s="191"/>
-      <c r="H487" s="206"/>
-      <c r="I487" s="179"/>
-    </row>
-    <row r="488" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A488" s="1"/>
-      <c r="B488" s="1"/>
-      <c r="C488" s="1"/>
-      <c r="D488" s="1"/>
-      <c r="E488" s="146"/>
-      <c r="F488" s="113"/>
-      <c r="G488" s="192"/>
-      <c r="H488" s="192"/>
-      <c r="I488" s="180"/>
-    </row>
-    <row r="489" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A489" s="1"/>
-      <c r="B489" s="1"/>
-      <c r="C489" s="1"/>
-      <c r="D489" s="1"/>
-      <c r="E489" s="146"/>
-      <c r="F489" s="113"/>
-      <c r="G489" s="192"/>
-      <c r="H489" s="192"/>
-      <c r="I489" s="180"/>
-    </row>
-    <row r="490" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A490" s="1"/>
-      <c r="B490" s="1"/>
-      <c r="C490" s="1"/>
-      <c r="D490" s="1"/>
-      <c r="E490" s="146"/>
-      <c r="F490" s="113"/>
-      <c r="G490" s="192"/>
-      <c r="H490" s="192"/>
-      <c r="I490" s="180"/>
-    </row>
-    <row r="491" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A491" s="1"/>
-      <c r="B491" s="1"/>
-      <c r="C491" s="1"/>
-      <c r="D491" s="1"/>
-      <c r="E491" s="146"/>
-      <c r="F491" s="113"/>
-      <c r="G491" s="192"/>
-      <c r="H491" s="192"/>
-      <c r="I491" s="180"/>
-    </row>
-    <row r="492" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A492" s="1"/>
-      <c r="B492" s="1"/>
-      <c r="C492" s="1"/>
-      <c r="D492" s="1"/>
-      <c r="E492" s="146"/>
-      <c r="F492" s="113"/>
-      <c r="G492" s="192"/>
-      <c r="H492" s="192"/>
-      <c r="I492" s="180"/>
-    </row>
-    <row r="493" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A493" s="1"/>
-      <c r="B493" s="1"/>
-      <c r="C493" s="1"/>
-      <c r="D493" s="1"/>
-      <c r="E493" s="146"/>
-      <c r="F493" s="113"/>
-      <c r="G493" s="192"/>
-      <c r="H493" s="192"/>
-      <c r="I493" s="180"/>
-    </row>
-    <row r="494" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A494" s="1"/>
-      <c r="B494" s="1"/>
-      <c r="C494" s="1"/>
-      <c r="D494" s="1"/>
-      <c r="E494" s="146"/>
-      <c r="F494" s="113"/>
-      <c r="G494" s="192"/>
-      <c r="H494" s="192"/>
-      <c r="I494" s="180"/>
-    </row>
-    <row r="495" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A495" s="1"/>
-      <c r="B495" s="1"/>
-      <c r="C495" s="1"/>
-      <c r="D495" s="1"/>
-      <c r="E495" s="146"/>
-      <c r="F495" s="113"/>
-      <c r="G495" s="192"/>
-      <c r="H495" s="192"/>
-      <c r="I495" s="180"/>
-    </row>
-    <row r="496" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A496" s="1"/>
-      <c r="B496" s="1"/>
-      <c r="C496" s="1"/>
-      <c r="D496" s="1"/>
-      <c r="E496" s="146"/>
-      <c r="F496" s="113"/>
-      <c r="G496" s="192"/>
-      <c r="H496" s="192"/>
-      <c r="I496" s="180"/>
+      <c r="B487" s="109"/>
+      <c r="C487" s="110"/>
+      <c r="D487" s="167" t="s">
+        <v>859</v>
+      </c>
+      <c r="E487" s="158" t="s">
+        <v>861</v>
+      </c>
+      <c r="F487" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G487" s="190">
+        <v>44950</v>
+      </c>
+      <c r="H487" s="204">
+        <v>44893</v>
+      </c>
+      <c r="I487" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="488" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A488" s="136"/>
+      <c r="B488" s="109"/>
+      <c r="C488" s="110"/>
+      <c r="D488" s="166" t="s">
+        <v>862</v>
+      </c>
+      <c r="E488" s="157" t="s">
+        <v>864</v>
+      </c>
+      <c r="F488" s="150" t="s">
+        <v>548</v>
+      </c>
+      <c r="G488" s="188">
+        <v>44970</v>
+      </c>
+      <c r="H488" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I488" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="489" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A489" s="136"/>
+      <c r="B489" s="109"/>
+      <c r="C489" s="110"/>
+      <c r="D489" s="166" t="s">
+        <v>863</v>
+      </c>
+      <c r="E489" s="157" t="s">
+        <v>865</v>
+      </c>
+      <c r="F489" s="150" t="s">
+        <v>548</v>
+      </c>
+      <c r="G489" s="188">
+        <v>44970</v>
+      </c>
+      <c r="H489" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I489" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="490" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A490" s="136"/>
+      <c r="B490" s="109"/>
+      <c r="C490" s="110"/>
+      <c r="D490" s="166"/>
+      <c r="E490" s="157"/>
+      <c r="F490" s="150"/>
+      <c r="G490" s="188"/>
+      <c r="H490" s="203"/>
+      <c r="I490" s="171"/>
+    </row>
+    <row r="491" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A491" s="136"/>
+      <c r="B491" s="109"/>
+      <c r="C491" s="110"/>
+      <c r="D491" s="166" t="s">
+        <v>934</v>
+      </c>
+      <c r="E491" s="157" t="s">
+        <v>936</v>
+      </c>
+      <c r="F491" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G491" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H491" s="203">
+        <v>45009</v>
+      </c>
+      <c r="I491" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="492" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A492" s="136"/>
+      <c r="B492" s="109"/>
+      <c r="C492" s="110"/>
+      <c r="D492" s="166" t="s">
+        <v>933</v>
+      </c>
+      <c r="E492" s="157" t="s">
+        <v>935</v>
+      </c>
+      <c r="F492" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G492" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H492" s="203">
+        <v>45009</v>
+      </c>
+      <c r="I492" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="493" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A493" s="136"/>
+      <c r="B493" s="109"/>
+      <c r="C493" s="110"/>
+      <c r="D493" s="166"/>
+      <c r="E493" s="157"/>
+      <c r="F493" s="150"/>
+      <c r="G493" s="188"/>
+      <c r="H493" s="203"/>
+      <c r="I493" s="171"/>
+    </row>
+    <row r="494" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A494" s="136"/>
+      <c r="B494" s="109"/>
+      <c r="C494" s="110"/>
+      <c r="D494" s="166" t="s">
+        <v>854</v>
+      </c>
+      <c r="E494" s="162" t="s">
+        <v>857</v>
+      </c>
+      <c r="F494" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G494" s="188">
+        <v>44986</v>
+      </c>
+      <c r="H494" s="203">
+        <v>44951</v>
+      </c>
+      <c r="I494" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="495" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A495" s="136"/>
+      <c r="B495" s="109"/>
+      <c r="C495" s="110"/>
+      <c r="D495" s="167" t="s">
+        <v>855</v>
+      </c>
+      <c r="E495" s="158" t="s">
+        <v>856</v>
+      </c>
+      <c r="F495" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G495" s="190">
+        <v>44986</v>
+      </c>
+      <c r="H495" s="204">
+        <v>44951</v>
+      </c>
+      <c r="I495" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="496" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A496" s="136"/>
+      <c r="B496" s="111"/>
+      <c r="C496" s="112"/>
+      <c r="D496" s="170"/>
+      <c r="E496" s="163"/>
+      <c r="F496" s="153"/>
+      <c r="G496" s="191"/>
+      <c r="H496" s="206"/>
+      <c r="I496" s="179"/>
     </row>
     <row r="497" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A497" s="1"/>
@@ -13712,38 +13806,159 @@
       <c r="H503" s="192"/>
       <c r="I503" s="180"/>
     </row>
-    <row r="504" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E504" s="145"/>
-      <c r="F504" s="95"/>
-      <c r="G504" s="193"/>
-      <c r="H504" s="193"/>
-      <c r="I504" s="181"/>
-    </row>
-    <row r="505" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E505" s="145"/>
-      <c r="F505" s="95"/>
-      <c r="G505" s="193"/>
-      <c r="H505" s="193"/>
-      <c r="I505" s="181"/>
-    </row>
-    <row r="506" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E506" s="145"/>
-      <c r="F506" s="95"/>
-      <c r="G506" s="193"/>
-      <c r="H506" s="193"/>
-      <c r="I506" s="181"/>
+    <row r="504" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A504" s="1"/>
+      <c r="B504" s="1"/>
+      <c r="C504" s="1"/>
+      <c r="D504" s="1"/>
+      <c r="E504" s="146"/>
+      <c r="F504" s="113"/>
+      <c r="G504" s="192"/>
+      <c r="H504" s="192"/>
+      <c r="I504" s="180"/>
+    </row>
+    <row r="505" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A505" s="1"/>
+      <c r="B505" s="1"/>
+      <c r="C505" s="1"/>
+      <c r="D505" s="1"/>
+      <c r="E505" s="146"/>
+      <c r="F505" s="113"/>
+      <c r="G505" s="192"/>
+      <c r="H505" s="192"/>
+      <c r="I505" s="180"/>
+    </row>
+    <row r="506" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A506" s="1"/>
+      <c r="B506" s="1"/>
+      <c r="C506" s="1"/>
+      <c r="D506" s="1"/>
+      <c r="E506" s="146"/>
+      <c r="F506" s="113"/>
+      <c r="G506" s="192"/>
+      <c r="H506" s="192"/>
+      <c r="I506" s="180"/>
+    </row>
+    <row r="507" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A507" s="1"/>
+      <c r="B507" s="1"/>
+      <c r="C507" s="1"/>
+      <c r="D507" s="1"/>
+      <c r="E507" s="146"/>
+      <c r="F507" s="113"/>
+      <c r="G507" s="192"/>
+      <c r="H507" s="192"/>
+      <c r="I507" s="180"/>
+    </row>
+    <row r="508" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A508" s="1"/>
+      <c r="B508" s="1"/>
+      <c r="C508" s="1"/>
+      <c r="D508" s="1"/>
+      <c r="E508" s="146"/>
+      <c r="F508" s="113"/>
+      <c r="G508" s="192"/>
+      <c r="H508" s="192"/>
+      <c r="I508" s="180"/>
+    </row>
+    <row r="509" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A509" s="1"/>
+      <c r="B509" s="1"/>
+      <c r="C509" s="1"/>
+      <c r="D509" s="1"/>
+      <c r="E509" s="146"/>
+      <c r="F509" s="113"/>
+      <c r="G509" s="192"/>
+      <c r="H509" s="192"/>
+      <c r="I509" s="180"/>
+    </row>
+    <row r="510" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A510" s="1"/>
+      <c r="B510" s="1"/>
+      <c r="C510" s="1"/>
+      <c r="D510" s="1"/>
+      <c r="E510" s="146"/>
+      <c r="F510" s="113"/>
+      <c r="G510" s="192"/>
+      <c r="H510" s="192"/>
+      <c r="I510" s="180"/>
+    </row>
+    <row r="511" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A511" s="1"/>
+      <c r="B511" s="1"/>
+      <c r="C511" s="1"/>
+      <c r="D511" s="1"/>
+      <c r="E511" s="146"/>
+      <c r="F511" s="113"/>
+      <c r="G511" s="192"/>
+      <c r="H511" s="192"/>
+      <c r="I511" s="180"/>
+    </row>
+    <row r="512" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A512" s="1"/>
+      <c r="B512" s="1"/>
+      <c r="C512" s="1"/>
+      <c r="D512" s="1"/>
+      <c r="E512" s="146"/>
+      <c r="F512" s="113"/>
+      <c r="G512" s="192"/>
+      <c r="H512" s="192"/>
+      <c r="I512" s="180"/>
+    </row>
+    <row r="513" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E513" s="145"/>
+      <c r="F513" s="95"/>
+      <c r="G513" s="193"/>
+      <c r="H513" s="193"/>
+      <c r="I513" s="181"/>
+    </row>
+    <row r="514" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E514" s="145"/>
+      <c r="F514" s="95"/>
+      <c r="G514" s="193"/>
+      <c r="H514" s="193"/>
+      <c r="I514" s="181"/>
+    </row>
+    <row r="515" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E515" s="145"/>
+      <c r="F515" s="95"/>
+      <c r="G515" s="193"/>
+      <c r="H515" s="193"/>
+      <c r="I515" s="181"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B476:B477"/>
-    <mergeCell ref="C477:C478"/>
+    <mergeCell ref="B380:B381"/>
+    <mergeCell ref="C381:C382"/>
+    <mergeCell ref="C204:C205"/>
+    <mergeCell ref="B376:B377"/>
+    <mergeCell ref="C377:C378"/>
+    <mergeCell ref="C282:C283"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="C132:C133"/>
+    <mergeCell ref="C471:C472"/>
+    <mergeCell ref="C391:C392"/>
+    <mergeCell ref="C394:C395"/>
+    <mergeCell ref="C416:C417"/>
+    <mergeCell ref="C419:C420"/>
+    <mergeCell ref="C422:C423"/>
+    <mergeCell ref="C135:C136"/>
+    <mergeCell ref="C144:C145"/>
+    <mergeCell ref="C185:C186"/>
+    <mergeCell ref="B481:B482"/>
+    <mergeCell ref="C482:C483"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C420:C421"/>
-    <mergeCell ref="C423:C424"/>
-    <mergeCell ref="C427:C428"/>
-    <mergeCell ref="C461:C462"/>
-    <mergeCell ref="C379:C380"/>
-    <mergeCell ref="C383:C384"/>
+    <mergeCell ref="C425:C426"/>
+    <mergeCell ref="C428:C429"/>
+    <mergeCell ref="C432:C433"/>
+    <mergeCell ref="C466:C467"/>
+    <mergeCell ref="C384:C385"/>
+    <mergeCell ref="C388:C389"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C15:C16"/>
@@ -13751,28 +13966,6 @@
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="C466:C467"/>
-    <mergeCell ref="C386:C387"/>
-    <mergeCell ref="C389:C390"/>
-    <mergeCell ref="C411:C412"/>
-    <mergeCell ref="C414:C415"/>
-    <mergeCell ref="C417:C418"/>
-    <mergeCell ref="C135:C136"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="C185:C186"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B375:B376"/>
-    <mergeCell ref="C376:C377"/>
-    <mergeCell ref="C204:C205"/>
-    <mergeCell ref="B371:B372"/>
-    <mergeCell ref="C372:C373"/>
-    <mergeCell ref="C282:C283"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -13806,20 +13999,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="247" t="s">
+      <c r="B2" s="230" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="248"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="244" t="s">
+      <c r="C2" s="231"/>
+      <c r="D2" s="232"/>
+      <c r="E2" s="227" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="246"/>
-      <c r="G2" s="244" t="s">
+      <c r="F2" s="229"/>
+      <c r="G2" s="227" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="245"/>
-      <c r="I2" s="246"/>
+      <c r="H2" s="228"/>
+      <c r="I2" s="229"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -13840,10 +14033,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="250" t="s">
+      <c r="H3" s="233" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="251"/>
+      <c r="I3" s="234"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -13885,7 +14078,7 @@
       <c r="F5" s="241" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="232" t="s">
+      <c r="G5" s="244" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -13901,11 +14094,11 @@
       <c r="D6" s="239"/>
       <c r="E6" s="35"/>
       <c r="F6" s="242"/>
-      <c r="G6" s="233"/>
-      <c r="H6" s="227" t="s">
+      <c r="G6" s="245"/>
+      <c r="H6" s="225" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="228"/>
+      <c r="I6" s="226"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
@@ -13913,7 +14106,7 @@
       <c r="D7" s="240"/>
       <c r="E7" s="36"/>
       <c r="F7" s="243"/>
-      <c r="G7" s="234"/>
+      <c r="G7" s="246"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -13953,13 +14146,13 @@
       <c r="D9" s="238" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="229" t="s">
+      <c r="E9" s="249" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="241" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="232" t="s">
+      <c r="G9" s="244" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -13974,22 +14167,22 @@
       <c r="B10" s="61"/>
       <c r="C10" s="236"/>
       <c r="D10" s="239"/>
-      <c r="E10" s="230"/>
+      <c r="E10" s="250"/>
       <c r="F10" s="242"/>
-      <c r="G10" s="233"/>
-      <c r="H10" s="227" t="s">
+      <c r="G10" s="245"/>
+      <c r="H10" s="225" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="228"/>
+      <c r="I10" s="226"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
       <c r="C11" s="237"/>
       <c r="D11" s="240"/>
-      <c r="E11" s="231"/>
+      <c r="E11" s="251"/>
       <c r="F11" s="243"/>
-      <c r="G11" s="234"/>
+      <c r="G11" s="246"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -14099,7 +14292,7 @@
       <c r="F18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="232" t="s">
+      <c r="G18" s="244" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="6" t="s">
@@ -14119,7 +14312,7 @@
       <c r="F19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="234"/>
+      <c r="G19" s="246"/>
       <c r="H19" s="8"/>
       <c r="I19" s="17"/>
     </row>
@@ -14164,8 +14357,8 @@
       <c r="E22" s="25"/>
       <c r="F22" s="22"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="225"/>
-      <c r="I22" s="226"/>
+      <c r="H22" s="247"/>
+      <c r="I22" s="248"/>
     </row>
     <row r="23" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="67" t="s">
@@ -14585,13 +14778,13 @@
       <c r="D46" s="238" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="229" t="s">
+      <c r="E46" s="249" t="s">
         <v>45</v>
       </c>
       <c r="F46" s="241" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="232" t="s">
+      <c r="G46" s="244" t="s">
         <v>47</v>
       </c>
       <c r="H46" s="6" t="s">
@@ -14605,21 +14798,21 @@
       <c r="B47" s="61"/>
       <c r="C47" s="236"/>
       <c r="D47" s="239"/>
-      <c r="E47" s="230"/>
+      <c r="E47" s="250"/>
       <c r="F47" s="242"/>
-      <c r="G47" s="233"/>
-      <c r="H47" s="227" t="s">
+      <c r="G47" s="245"/>
+      <c r="H47" s="225" t="s">
         <v>32</v>
       </c>
-      <c r="I47" s="228"/>
+      <c r="I47" s="226"/>
     </row>
     <row r="48" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B48" s="61"/>
       <c r="C48" s="237"/>
       <c r="D48" s="240"/>
-      <c r="E48" s="231"/>
+      <c r="E48" s="251"/>
       <c r="F48" s="243"/>
-      <c r="G48" s="234"/>
+      <c r="G48" s="246"/>
       <c r="H48" s="8" t="s">
         <v>23</v>
       </c>
@@ -14659,13 +14852,13 @@
       <c r="D50" s="238" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="229" t="s">
+      <c r="E50" s="249" t="s">
         <v>55</v>
       </c>
       <c r="F50" s="241" t="s">
         <v>56</v>
       </c>
-      <c r="G50" s="232" t="s">
+      <c r="G50" s="244" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="6" t="s">
@@ -14679,21 +14872,21 @@
       <c r="B51" s="61"/>
       <c r="C51" s="236"/>
       <c r="D51" s="239"/>
-      <c r="E51" s="230"/>
+      <c r="E51" s="250"/>
       <c r="F51" s="242"/>
-      <c r="G51" s="233"/>
-      <c r="H51" s="227" t="s">
+      <c r="G51" s="245"/>
+      <c r="H51" s="225" t="s">
         <v>32</v>
       </c>
-      <c r="I51" s="228"/>
+      <c r="I51" s="226"/>
     </row>
     <row r="52" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B52" s="61"/>
       <c r="C52" s="237"/>
       <c r="D52" s="240"/>
-      <c r="E52" s="231"/>
+      <c r="E52" s="251"/>
       <c r="F52" s="243"/>
-      <c r="G52" s="234"/>
+      <c r="G52" s="246"/>
       <c r="H52" s="8" t="s">
         <v>23</v>
       </c>
@@ -14718,8 +14911,8 @@
       <c r="E54" s="25"/>
       <c r="F54" s="22"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="225"/>
-      <c r="I54" s="226"/>
+      <c r="H54" s="247"/>
+      <c r="I54" s="248"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="61" t="s">
@@ -14782,10 +14975,10 @@
       <c r="E58" s="39"/>
       <c r="F58" s="12"/>
       <c r="G58" s="32"/>
-      <c r="H58" s="227" t="s">
+      <c r="H58" s="225" t="s">
         <v>32</v>
       </c>
-      <c r="I58" s="228"/>
+      <c r="I58" s="226"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
@@ -14818,8 +15011,8 @@
       <c r="E61" s="25"/>
       <c r="F61" s="22"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="225"/>
-      <c r="I61" s="226"/>
+      <c r="H61" s="247"/>
+      <c r="I61" s="248"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="64" t="s">
@@ -15232,8 +15425,8 @@
       <c r="E89" s="25"/>
       <c r="F89" s="22"/>
       <c r="G89" s="25"/>
-      <c r="H89" s="225"/>
-      <c r="I89" s="226"/>
+      <c r="H89" s="247"/>
+      <c r="I89" s="248"/>
     </row>
     <row r="90" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="61"/>
@@ -15377,15 +15570,22 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="G18:G19"/>
@@ -15398,22 +15598,15 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="D14:D16"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -15447,10 +15640,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="253"/>
-      <c r="D2" s="245" t="s">
+      <c r="D2" s="228" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="246" t="s">
+      <c r="E2" s="229" t="s">
         <v>0</v>
       </c>
     </row>
@@ -15461,8 +15654,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="250"/>
-      <c r="E3" s="251"/>
+      <c r="D3" s="233"/>
+      <c r="E3" s="234"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 30 Maret 2023 16:34 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1528" uniqueCount="939">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="942">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -3042,6 +3042,16 @@
   </si>
   <si>
     <t>Mengeset data (INSERT dan UPDATE) pada tabel TblLog_TableSnapshotSignature</t>
+  </si>
+  <si>
+    <t>FuncSys_General_GetUserIdentityByLDAPUserID</t>
+  </si>
+  <si>
+    <t>Mendapatkan identitas utama pengguna berdasarkan ID Pengguna LDAP (varLDAPUserID)</t>
+  </si>
+  <si>
+    <t>SchSysConfig.
+HoldFuncSys_General_GetUserIdentityByLDAPUserID</t>
   </si>
 </sst>
 </file>
@@ -4888,13 +4898,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I515"/>
+  <dimension ref="A1:I517"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E365" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="F362" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E375" sqref="E375"/>
+      <selection pane="bottomRight" activeCell="H366" sqref="H366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11483,111 +11493,111 @@
       <c r="B366" s="109"/>
       <c r="C366" s="110"/>
       <c r="D366" s="167" t="s">
-        <v>388</v>
+        <v>939</v>
       </c>
       <c r="E366" s="158" t="s">
-        <v>927</v>
+        <v>940</v>
       </c>
       <c r="F366" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G366" s="190">
-        <v>44957</v>
+        <v>45014</v>
       </c>
       <c r="H366" s="204">
-        <v>44957</v>
-      </c>
-      <c r="I366" s="199" t="s">
-        <v>892</v>
+        <v>45014</v>
+      </c>
+      <c r="I366" s="209" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="367" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A367" s="1"/>
       <c r="B367" s="109"/>
       <c r="C367" s="110"/>
-      <c r="D367" s="165"/>
-      <c r="E367" s="159"/>
-      <c r="F367" s="148"/>
-      <c r="G367" s="186"/>
-      <c r="H367" s="201"/>
-      <c r="I367" s="174"/>
-    </row>
-    <row r="368" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D367" s="167"/>
+      <c r="E367" s="158"/>
+      <c r="F367" s="151"/>
+      <c r="G367" s="190"/>
+      <c r="H367" s="204"/>
+      <c r="I367" s="199"/>
+    </row>
+    <row r="368" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A368" s="1"/>
       <c r="B368" s="109"/>
       <c r="C368" s="110"/>
-      <c r="D368" s="165"/>
-      <c r="E368" s="155"/>
-      <c r="F368" s="148"/>
-      <c r="G368" s="186"/>
-      <c r="H368" s="201"/>
-      <c r="I368" s="174"/>
-    </row>
-    <row r="369" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D368" s="167" t="s">
+        <v>388</v>
+      </c>
+      <c r="E368" s="158" t="s">
+        <v>927</v>
+      </c>
+      <c r="F368" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G368" s="190">
+        <v>44957</v>
+      </c>
+      <c r="H368" s="204">
+        <v>44957</v>
+      </c>
+      <c r="I368" s="199" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="369" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A369" s="1"/>
       <c r="B369" s="109"/>
       <c r="C369" s="110"/>
-      <c r="D369" s="144"/>
-      <c r="E369" s="156"/>
-      <c r="F369" s="149"/>
-      <c r="G369" s="187"/>
-      <c r="H369" s="202"/>
-      <c r="I369" s="175"/>
-    </row>
-    <row r="370" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D369" s="165"/>
+      <c r="E369" s="159"/>
+      <c r="F369" s="148"/>
+      <c r="G369" s="186"/>
+      <c r="H369" s="201"/>
+      <c r="I369" s="174"/>
+    </row>
+    <row r="370" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A370" s="1"/>
       <c r="B370" s="109"/>
       <c r="C370" s="110"/>
-      <c r="D370" s="166" t="s">
-        <v>329</v>
-      </c>
-      <c r="E370" s="162" t="s">
-        <v>330</v>
-      </c>
-      <c r="F370" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G370" s="188">
-        <v>44893</v>
-      </c>
-      <c r="H370" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I370" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="371" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D370" s="165"/>
+      <c r="E370" s="155"/>
+      <c r="F370" s="148"/>
+      <c r="G370" s="186"/>
+      <c r="H370" s="201"/>
+      <c r="I370" s="174"/>
+    </row>
+    <row r="371" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A371" s="1"/>
       <c r="B371" s="109"/>
       <c r="C371" s="110"/>
-      <c r="D371" s="166"/>
-      <c r="E371" s="162"/>
-      <c r="F371" s="150"/>
-      <c r="G371" s="188"/>
-      <c r="H371" s="203"/>
-      <c r="I371" s="171"/>
+      <c r="D371" s="144"/>
+      <c r="E371" s="156"/>
+      <c r="F371" s="149"/>
+      <c r="G371" s="187"/>
+      <c r="H371" s="202"/>
+      <c r="I371" s="175"/>
     </row>
     <row r="372" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A372" s="1"/>
       <c r="B372" s="109"/>
       <c r="C372" s="110"/>
       <c r="D372" s="166" t="s">
-        <v>937</v>
+        <v>329</v>
       </c>
       <c r="E372" s="162" t="s">
-        <v>938</v>
+        <v>330</v>
       </c>
       <c r="F372" s="150" t="s">
         <v>232</v>
       </c>
       <c r="G372" s="188">
-        <v>45009</v>
+        <v>44893</v>
       </c>
       <c r="H372" s="203">
-        <v>45009</v>
-      </c>
-      <c r="I372" s="183" t="s">
+        <v>44893</v>
+      </c>
+      <c r="I372" s="171" t="s">
         <v>727</v>
       </c>
     </row>
@@ -11606,20 +11616,20 @@
       <c r="A374" s="1"/>
       <c r="B374" s="109"/>
       <c r="C374" s="110"/>
-      <c r="D374" s="167" t="s">
-        <v>852</v>
-      </c>
-      <c r="E374" s="158" t="s">
-        <v>853</v>
-      </c>
-      <c r="F374" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G374" s="190">
-        <v>44986</v>
-      </c>
-      <c r="H374" s="204">
-        <v>44951</v>
+      <c r="D374" s="166" t="s">
+        <v>937</v>
+      </c>
+      <c r="E374" s="162" t="s">
+        <v>938</v>
+      </c>
+      <c r="F374" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G374" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H374" s="203">
+        <v>45009</v>
       </c>
       <c r="I374" s="183" t="s">
         <v>727</v>
@@ -11629,126 +11639,136 @@
       <c r="A375" s="1"/>
       <c r="B375" s="109"/>
       <c r="C375" s="110"/>
-      <c r="D375" s="165"/>
-      <c r="E375" s="155"/>
-      <c r="F375" s="148"/>
-      <c r="G375" s="186"/>
-      <c r="H375" s="201"/>
-      <c r="I375" s="174"/>
-    </row>
-    <row r="376" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A376" s="136"/>
-      <c r="B376" s="212" t="s">
+      <c r="D375" s="166"/>
+      <c r="E375" s="162"/>
+      <c r="F375" s="150"/>
+      <c r="G375" s="188"/>
+      <c r="H375" s="203"/>
+      <c r="I375" s="171"/>
+    </row>
+    <row r="376" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A376" s="1"/>
+      <c r="B376" s="109"/>
+      <c r="C376" s="110"/>
+      <c r="D376" s="167" t="s">
+        <v>852</v>
+      </c>
+      <c r="E376" s="158" t="s">
+        <v>853</v>
+      </c>
+      <c r="F376" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G376" s="190">
+        <v>44986</v>
+      </c>
+      <c r="H376" s="204">
+        <v>44951</v>
+      </c>
+      <c r="I376" s="183" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="377" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A377" s="1"/>
+      <c r="B377" s="109"/>
+      <c r="C377" s="110"/>
+      <c r="D377" s="165"/>
+      <c r="E377" s="155"/>
+      <c r="F377" s="148"/>
+      <c r="G377" s="186"/>
+      <c r="H377" s="201"/>
+      <c r="I377" s="174"/>
+    </row>
+    <row r="378" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A378" s="136"/>
+      <c r="B378" s="212" t="s">
         <v>142</v>
       </c>
-      <c r="C376" s="134"/>
-      <c r="D376" s="135"/>
-      <c r="E376" s="154"/>
-      <c r="F376" s="147"/>
-      <c r="G376" s="185"/>
-      <c r="H376" s="200"/>
-      <c r="I376" s="173"/>
-    </row>
-    <row r="377" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A377" s="136"/>
-      <c r="B377" s="212"/>
-      <c r="C377" s="213" t="s">
+      <c r="C378" s="134"/>
+      <c r="D378" s="135"/>
+      <c r="E378" s="154"/>
+      <c r="F378" s="147"/>
+      <c r="G378" s="185"/>
+      <c r="H378" s="200"/>
+      <c r="I378" s="173"/>
+    </row>
+    <row r="379" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A379" s="136"/>
+      <c r="B379" s="212"/>
+      <c r="C379" s="213" t="s">
         <v>160</v>
       </c>
-      <c r="D377" s="135"/>
-      <c r="E377" s="154"/>
-      <c r="F377" s="147"/>
-      <c r="G377" s="185"/>
-      <c r="H377" s="200"/>
-      <c r="I377" s="173"/>
-    </row>
-    <row r="378" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A378" s="1"/>
-      <c r="B378" s="109"/>
-      <c r="C378" s="213"/>
-      <c r="D378" s="165"/>
-      <c r="E378" s="155"/>
-      <c r="F378" s="148"/>
-      <c r="G378" s="186"/>
-      <c r="H378" s="201"/>
-      <c r="I378" s="174"/>
-    </row>
-    <row r="379" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A379" s="1"/>
-      <c r="B379" s="109"/>
-      <c r="C379" s="110"/>
-      <c r="D379" s="165"/>
-      <c r="E379" s="155"/>
-      <c r="F379" s="148"/>
-      <c r="G379" s="186"/>
-      <c r="H379" s="201"/>
-      <c r="I379" s="174"/>
-    </row>
-    <row r="380" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A380" s="136"/>
-      <c r="B380" s="212" t="s">
+      <c r="D379" s="135"/>
+      <c r="E379" s="154"/>
+      <c r="F379" s="147"/>
+      <c r="G379" s="185"/>
+      <c r="H379" s="200"/>
+      <c r="I379" s="173"/>
+    </row>
+    <row r="380" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A380" s="1"/>
+      <c r="B380" s="109"/>
+      <c r="C380" s="213"/>
+      <c r="D380" s="165"/>
+      <c r="E380" s="155"/>
+      <c r="F380" s="148"/>
+      <c r="G380" s="186"/>
+      <c r="H380" s="201"/>
+      <c r="I380" s="174"/>
+    </row>
+    <row r="381" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A381" s="1"/>
+      <c r="B381" s="109"/>
+      <c r="C381" s="110"/>
+      <c r="D381" s="165"/>
+      <c r="E381" s="155"/>
+      <c r="F381" s="148"/>
+      <c r="G381" s="186"/>
+      <c r="H381" s="201"/>
+      <c r="I381" s="174"/>
+    </row>
+    <row r="382" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A382" s="136"/>
+      <c r="B382" s="212" t="s">
         <v>143</v>
       </c>
-      <c r="C380" s="134"/>
-      <c r="D380" s="135"/>
-      <c r="E380" s="154"/>
-      <c r="F380" s="147"/>
-      <c r="G380" s="185"/>
-      <c r="H380" s="200"/>
-      <c r="I380" s="173"/>
-    </row>
-    <row r="381" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A381" s="136"/>
-      <c r="B381" s="212"/>
-      <c r="C381" s="213" t="s">
+      <c r="C382" s="134"/>
+      <c r="D382" s="135"/>
+      <c r="E382" s="154"/>
+      <c r="F382" s="147"/>
+      <c r="G382" s="185"/>
+      <c r="H382" s="200"/>
+      <c r="I382" s="173"/>
+    </row>
+    <row r="383" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A383" s="136"/>
+      <c r="B383" s="212"/>
+      <c r="C383" s="213" t="s">
         <v>148</v>
       </c>
-      <c r="D381" s="135"/>
-      <c r="E381" s="154"/>
-      <c r="F381" s="147"/>
-      <c r="G381" s="185"/>
-      <c r="H381" s="200"/>
-      <c r="I381" s="173"/>
-    </row>
-    <row r="382" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A382" s="1"/>
-      <c r="B382" s="109"/>
-      <c r="C382" s="213"/>
-      <c r="D382" s="165"/>
-      <c r="E382" s="155"/>
-      <c r="F382" s="148"/>
-      <c r="G382" s="186"/>
-      <c r="H382" s="201"/>
-      <c r="I382" s="174"/>
-    </row>
-    <row r="383" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A383" s="1"/>
-      <c r="B383" s="109"/>
-      <c r="C383" s="110"/>
-      <c r="D383" s="165"/>
-      <c r="E383" s="155"/>
-      <c r="F383" s="148"/>
-      <c r="G383" s="186"/>
-      <c r="H383" s="201"/>
-      <c r="I383" s="174"/>
+      <c r="D383" s="135"/>
+      <c r="E383" s="154"/>
+      <c r="F383" s="147"/>
+      <c r="G383" s="185"/>
+      <c r="H383" s="200"/>
+      <c r="I383" s="173"/>
     </row>
     <row r="384" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A384" s="1"/>
       <c r="B384" s="109"/>
-      <c r="C384" s="213" t="s">
-        <v>149</v>
-      </c>
-      <c r="D384" s="135"/>
-      <c r="E384" s="154"/>
-      <c r="F384" s="147"/>
-      <c r="G384" s="185"/>
-      <c r="H384" s="200"/>
-      <c r="I384" s="173"/>
+      <c r="C384" s="213"/>
+      <c r="D384" s="165"/>
+      <c r="E384" s="155"/>
+      <c r="F384" s="148"/>
+      <c r="G384" s="186"/>
+      <c r="H384" s="201"/>
+      <c r="I384" s="174"/>
     </row>
     <row r="385" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A385" s="1"/>
       <c r="B385" s="109"/>
-      <c r="C385" s="213"/>
+      <c r="C385" s="110"/>
       <c r="D385" s="165"/>
       <c r="E385" s="155"/>
       <c r="F385" s="148"/>
@@ -11756,33 +11776,23 @@
       <c r="H385" s="201"/>
       <c r="I385" s="174"/>
     </row>
-    <row r="386" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A386" s="1"/>
       <c r="B386" s="109"/>
-      <c r="C386" s="110"/>
-      <c r="D386" s="166" t="s">
-        <v>915</v>
-      </c>
-      <c r="E386" s="157" t="s">
-        <v>917</v>
-      </c>
-      <c r="F386" s="150" t="s">
-        <v>689</v>
-      </c>
-      <c r="G386" s="188">
-        <v>44860</v>
-      </c>
-      <c r="H386" s="203">
-        <v>44503</v>
-      </c>
-      <c r="I386" s="171" t="s">
-        <v>916</v>
-      </c>
+      <c r="C386" s="213" t="s">
+        <v>149</v>
+      </c>
+      <c r="D386" s="135"/>
+      <c r="E386" s="154"/>
+      <c r="F386" s="147"/>
+      <c r="G386" s="185"/>
+      <c r="H386" s="200"/>
+      <c r="I386" s="173"/>
     </row>
     <row r="387" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A387" s="1"/>
       <c r="B387" s="109"/>
-      <c r="C387" s="110"/>
+      <c r="C387" s="213"/>
       <c r="D387" s="165"/>
       <c r="E387" s="155"/>
       <c r="F387" s="148"/>
@@ -11790,23 +11800,33 @@
       <c r="H387" s="201"/>
       <c r="I387" s="174"/>
     </row>
-    <row r="388" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A388" s="1"/>
       <c r="B388" s="109"/>
-      <c r="C388" s="213" t="s">
-        <v>150</v>
-      </c>
-      <c r="D388" s="135"/>
-      <c r="E388" s="154"/>
-      <c r="F388" s="147"/>
-      <c r="G388" s="185"/>
-      <c r="H388" s="200"/>
-      <c r="I388" s="173"/>
+      <c r="C388" s="110"/>
+      <c r="D388" s="166" t="s">
+        <v>915</v>
+      </c>
+      <c r="E388" s="157" t="s">
+        <v>917</v>
+      </c>
+      <c r="F388" s="150" t="s">
+        <v>689</v>
+      </c>
+      <c r="G388" s="188">
+        <v>44860</v>
+      </c>
+      <c r="H388" s="203">
+        <v>44503</v>
+      </c>
+      <c r="I388" s="171" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="389" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A389" s="1"/>
       <c r="B389" s="109"/>
-      <c r="C389" s="213"/>
+      <c r="C389" s="110"/>
       <c r="D389" s="165"/>
       <c r="E389" s="155"/>
       <c r="F389" s="148"/>
@@ -11817,31 +11837,31 @@
     <row r="390" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A390" s="1"/>
       <c r="B390" s="109"/>
-      <c r="C390" s="110"/>
-      <c r="D390" s="165"/>
-      <c r="E390" s="155"/>
-      <c r="F390" s="148"/>
-      <c r="G390" s="186"/>
-      <c r="H390" s="201"/>
-      <c r="I390" s="174"/>
+      <c r="C390" s="213" t="s">
+        <v>150</v>
+      </c>
+      <c r="D390" s="135"/>
+      <c r="E390" s="154"/>
+      <c r="F390" s="147"/>
+      <c r="G390" s="185"/>
+      <c r="H390" s="200"/>
+      <c r="I390" s="173"/>
     </row>
     <row r="391" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A391" s="1"/>
       <c r="B391" s="109"/>
-      <c r="C391" s="213" t="s">
-        <v>151</v>
-      </c>
-      <c r="D391" s="135"/>
-      <c r="E391" s="154"/>
-      <c r="F391" s="147"/>
-      <c r="G391" s="185"/>
-      <c r="H391" s="200"/>
-      <c r="I391" s="173"/>
+      <c r="C391" s="213"/>
+      <c r="D391" s="165"/>
+      <c r="E391" s="155"/>
+      <c r="F391" s="148"/>
+      <c r="G391" s="186"/>
+      <c r="H391" s="201"/>
+      <c r="I391" s="174"/>
     </row>
     <row r="392" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A392" s="1"/>
       <c r="B392" s="109"/>
-      <c r="C392" s="213"/>
+      <c r="C392" s="110"/>
       <c r="D392" s="165"/>
       <c r="E392" s="155"/>
       <c r="F392" s="148"/>
@@ -11852,93 +11872,71 @@
     <row r="393" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A393" s="1"/>
       <c r="B393" s="109"/>
-      <c r="C393" s="110"/>
-      <c r="D393" s="165"/>
-      <c r="E393" s="155"/>
-      <c r="F393" s="148"/>
-      <c r="G393" s="186"/>
-      <c r="H393" s="201"/>
-      <c r="I393" s="174"/>
+      <c r="C393" s="213" t="s">
+        <v>151</v>
+      </c>
+      <c r="D393" s="135"/>
+      <c r="E393" s="154"/>
+      <c r="F393" s="147"/>
+      <c r="G393" s="185"/>
+      <c r="H393" s="200"/>
+      <c r="I393" s="173"/>
     </row>
     <row r="394" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A394" s="1"/>
       <c r="B394" s="109"/>
-      <c r="C394" s="213" t="s">
-        <v>152</v>
-      </c>
-      <c r="D394" s="135"/>
-      <c r="E394" s="154"/>
-      <c r="F394" s="147"/>
-      <c r="G394" s="185"/>
-      <c r="H394" s="200"/>
-      <c r="I394" s="173"/>
+      <c r="C394" s="213"/>
+      <c r="D394" s="165"/>
+      <c r="E394" s="155"/>
+      <c r="F394" s="148"/>
+      <c r="G394" s="186"/>
+      <c r="H394" s="201"/>
+      <c r="I394" s="174"/>
     </row>
     <row r="395" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A395" s="1"/>
       <c r="B395" s="109"/>
-      <c r="C395" s="213"/>
-      <c r="D395" s="166" t="s">
-        <v>760</v>
-      </c>
-      <c r="E395" s="162" t="s">
-        <v>762</v>
-      </c>
-      <c r="F395" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G395" s="188">
-        <v>44721</v>
-      </c>
-      <c r="H395" s="204">
-        <v>44698</v>
-      </c>
-      <c r="I395" s="176" t="s">
-        <v>759</v>
-      </c>
+      <c r="C395" s="110"/>
+      <c r="D395" s="165"/>
+      <c r="E395" s="155"/>
+      <c r="F395" s="148"/>
+      <c r="G395" s="186"/>
+      <c r="H395" s="201"/>
+      <c r="I395" s="174"/>
     </row>
     <row r="396" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A396" s="1"/>
       <c r="B396" s="109"/>
-      <c r="C396" s="110"/>
-      <c r="D396" s="167" t="s">
-        <v>761</v>
-      </c>
-      <c r="E396" s="160" t="s">
-        <v>763</v>
-      </c>
-      <c r="F396" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G396" s="190">
-        <v>44721</v>
-      </c>
-      <c r="H396" s="204">
-        <v>44698</v>
-      </c>
-      <c r="I396" s="177" t="s">
-        <v>759</v>
-      </c>
+      <c r="C396" s="213" t="s">
+        <v>152</v>
+      </c>
+      <c r="D396" s="135"/>
+      <c r="E396" s="154"/>
+      <c r="F396" s="147"/>
+      <c r="G396" s="185"/>
+      <c r="H396" s="200"/>
+      <c r="I396" s="173"/>
     </row>
     <row r="397" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A397" s="1"/>
       <c r="B397" s="109"/>
-      <c r="C397" s="110"/>
-      <c r="D397" s="167" t="s">
-        <v>755</v>
-      </c>
-      <c r="E397" s="160" t="s">
-        <v>757</v>
-      </c>
-      <c r="F397" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G397" s="190">
-        <v>44644</v>
+      <c r="C397" s="213"/>
+      <c r="D397" s="166" t="s">
+        <v>760</v>
+      </c>
+      <c r="E397" s="162" t="s">
+        <v>762</v>
+      </c>
+      <c r="F397" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G397" s="188">
+        <v>44721</v>
       </c>
       <c r="H397" s="204">
-        <v>44622</v>
-      </c>
-      <c r="I397" s="177" t="s">
+        <v>44698</v>
+      </c>
+      <c r="I397" s="176" t="s">
         <v>759</v>
       </c>
     </row>
@@ -11947,19 +11945,19 @@
       <c r="B398" s="109"/>
       <c r="C398" s="110"/>
       <c r="D398" s="167" t="s">
-        <v>756</v>
+        <v>761</v>
       </c>
       <c r="E398" s="160" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="F398" s="151" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G398" s="190">
-        <v>44644</v>
+        <v>44721</v>
       </c>
       <c r="H398" s="204">
-        <v>44622</v>
+        <v>44698</v>
       </c>
       <c r="I398" s="177" t="s">
         <v>759</v>
@@ -11970,19 +11968,19 @@
       <c r="B399" s="109"/>
       <c r="C399" s="110"/>
       <c r="D399" s="167" t="s">
-        <v>764</v>
+        <v>755</v>
       </c>
       <c r="E399" s="160" t="s">
-        <v>766</v>
+        <v>757</v>
       </c>
       <c r="F399" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G399" s="190">
-        <v>44755</v>
+        <v>44644</v>
       </c>
       <c r="H399" s="204">
-        <v>44755</v>
+        <v>44622</v>
       </c>
       <c r="I399" s="177" t="s">
         <v>759</v>
@@ -11993,19 +11991,19 @@
       <c r="B400" s="109"/>
       <c r="C400" s="110"/>
       <c r="D400" s="167" t="s">
-        <v>765</v>
+        <v>756</v>
       </c>
       <c r="E400" s="160" t="s">
-        <v>767</v>
+        <v>758</v>
       </c>
       <c r="F400" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G400" s="190">
-        <v>44756</v>
+        <v>44644</v>
       </c>
       <c r="H400" s="204">
-        <v>44756</v>
+        <v>44622</v>
       </c>
       <c r="I400" s="177" t="s">
         <v>759</v>
@@ -12016,10 +12014,10 @@
       <c r="B401" s="109"/>
       <c r="C401" s="110"/>
       <c r="D401" s="167" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="E401" s="160" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="F401" s="151" t="s">
         <v>232</v>
@@ -12039,19 +12037,19 @@
       <c r="B402" s="109"/>
       <c r="C402" s="110"/>
       <c r="D402" s="167" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="E402" s="160" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
       <c r="F402" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G402" s="190">
-        <v>44755</v>
+        <v>44756</v>
       </c>
       <c r="H402" s="204">
-        <v>44755</v>
+        <v>44756</v>
       </c>
       <c r="I402" s="177" t="s">
         <v>759</v>
@@ -12061,23 +12059,47 @@
       <c r="A403" s="1"/>
       <c r="B403" s="109"/>
       <c r="C403" s="110"/>
-      <c r="D403" s="167"/>
-      <c r="E403" s="160"/>
-      <c r="F403" s="151"/>
-      <c r="G403" s="190"/>
-      <c r="H403" s="204"/>
-      <c r="I403" s="177"/>
+      <c r="D403" s="167" t="s">
+        <v>768</v>
+      </c>
+      <c r="E403" s="160" t="s">
+        <v>770</v>
+      </c>
+      <c r="F403" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G403" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H403" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I403" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="404" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A404" s="1"/>
       <c r="B404" s="109"/>
       <c r="C404" s="110"/>
-      <c r="D404" s="167"/>
-      <c r="E404" s="160"/>
-      <c r="F404" s="151"/>
-      <c r="G404" s="190"/>
-      <c r="H404" s="204"/>
-      <c r="I404" s="177"/>
+      <c r="D404" s="167" t="s">
+        <v>769</v>
+      </c>
+      <c r="E404" s="160" t="s">
+        <v>771</v>
+      </c>
+      <c r="F404" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G404" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H404" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I404" s="177" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="405" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A405" s="1"/>
@@ -12127,60 +12149,60 @@
       <c r="A409" s="1"/>
       <c r="B409" s="109"/>
       <c r="C409" s="110"/>
-      <c r="D409" s="167" t="s">
-        <v>773</v>
-      </c>
+      <c r="D409" s="167"/>
       <c r="E409" s="160"/>
-      <c r="F409" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G409" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H409" s="204">
-        <v>44984</v>
-      </c>
+      <c r="F409" s="151"/>
+      <c r="G409" s="190"/>
+      <c r="H409" s="204"/>
       <c r="I409" s="177"/>
     </row>
     <row r="410" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A410" s="1"/>
       <c r="B410" s="109"/>
       <c r="C410" s="110"/>
-      <c r="D410" s="167" t="s">
-        <v>772</v>
-      </c>
+      <c r="D410" s="167"/>
       <c r="E410" s="160"/>
-      <c r="F410" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G410" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H410" s="204">
-        <v>44984</v>
-      </c>
+      <c r="F410" s="151"/>
+      <c r="G410" s="190"/>
+      <c r="H410" s="204"/>
       <c r="I410" s="177"/>
     </row>
     <row r="411" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A411" s="1"/>
       <c r="B411" s="109"/>
       <c r="C411" s="110"/>
-      <c r="D411" s="167"/>
+      <c r="D411" s="167" t="s">
+        <v>773</v>
+      </c>
       <c r="E411" s="160"/>
-      <c r="F411" s="151"/>
-      <c r="G411" s="190"/>
-      <c r="H411" s="204"/>
+      <c r="F411" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G411" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H411" s="204">
+        <v>44984</v>
+      </c>
       <c r="I411" s="177"/>
     </row>
     <row r="412" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A412" s="1"/>
       <c r="B412" s="109"/>
       <c r="C412" s="110"/>
-      <c r="D412" s="167"/>
+      <c r="D412" s="167" t="s">
+        <v>772</v>
+      </c>
       <c r="E412" s="160"/>
-      <c r="F412" s="151"/>
-      <c r="G412" s="190"/>
-      <c r="H412" s="204"/>
+      <c r="F412" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G412" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H412" s="204">
+        <v>44984</v>
+      </c>
       <c r="I412" s="177"/>
     </row>
     <row r="413" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -12209,30 +12231,28 @@
       <c r="A415" s="1"/>
       <c r="B415" s="109"/>
       <c r="C415" s="110"/>
-      <c r="D415" s="165"/>
-      <c r="E415" s="155"/>
-      <c r="F415" s="148"/>
-      <c r="G415" s="186"/>
-      <c r="H415" s="201"/>
-      <c r="I415" s="174"/>
+      <c r="D415" s="167"/>
+      <c r="E415" s="160"/>
+      <c r="F415" s="151"/>
+      <c r="G415" s="190"/>
+      <c r="H415" s="204"/>
+      <c r="I415" s="177"/>
     </row>
     <row r="416" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A416" s="1"/>
       <c r="B416" s="109"/>
-      <c r="C416" s="213" t="s">
-        <v>153</v>
-      </c>
-      <c r="D416" s="135"/>
-      <c r="E416" s="154"/>
-      <c r="F416" s="147"/>
-      <c r="G416" s="185"/>
-      <c r="H416" s="200"/>
-      <c r="I416" s="173"/>
+      <c r="C416" s="110"/>
+      <c r="D416" s="167"/>
+      <c r="E416" s="160"/>
+      <c r="F416" s="151"/>
+      <c r="G416" s="190"/>
+      <c r="H416" s="204"/>
+      <c r="I416" s="177"/>
     </row>
     <row r="417" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A417" s="1"/>
       <c r="B417" s="109"/>
-      <c r="C417" s="213"/>
+      <c r="C417" s="110"/>
       <c r="D417" s="165"/>
       <c r="E417" s="155"/>
       <c r="F417" s="148"/>
@@ -12243,31 +12263,31 @@
     <row r="418" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A418" s="1"/>
       <c r="B418" s="109"/>
-      <c r="C418" s="110"/>
-      <c r="D418" s="165"/>
-      <c r="E418" s="155"/>
-      <c r="F418" s="148"/>
-      <c r="G418" s="186"/>
-      <c r="H418" s="201"/>
-      <c r="I418" s="174"/>
+      <c r="C418" s="213" t="s">
+        <v>153</v>
+      </c>
+      <c r="D418" s="135"/>
+      <c r="E418" s="154"/>
+      <c r="F418" s="147"/>
+      <c r="G418" s="185"/>
+      <c r="H418" s="200"/>
+      <c r="I418" s="173"/>
     </row>
     <row r="419" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A419" s="1"/>
       <c r="B419" s="109"/>
-      <c r="C419" s="213" t="s">
-        <v>154</v>
-      </c>
-      <c r="D419" s="135"/>
-      <c r="E419" s="154"/>
-      <c r="F419" s="147"/>
-      <c r="G419" s="185"/>
-      <c r="H419" s="200"/>
-      <c r="I419" s="173"/>
+      <c r="C419" s="213"/>
+      <c r="D419" s="165"/>
+      <c r="E419" s="155"/>
+      <c r="F419" s="148"/>
+      <c r="G419" s="186"/>
+      <c r="H419" s="201"/>
+      <c r="I419" s="174"/>
     </row>
     <row r="420" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A420" s="1"/>
       <c r="B420" s="109"/>
-      <c r="C420" s="213"/>
+      <c r="C420" s="110"/>
       <c r="D420" s="165"/>
       <c r="E420" s="155"/>
       <c r="F420" s="148"/>
@@ -12278,31 +12298,31 @@
     <row r="421" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A421" s="1"/>
       <c r="B421" s="109"/>
-      <c r="C421" s="110"/>
-      <c r="D421" s="165"/>
-      <c r="E421" s="155"/>
-      <c r="F421" s="148"/>
-      <c r="G421" s="186"/>
-      <c r="H421" s="201"/>
-      <c r="I421" s="174"/>
+      <c r="C421" s="213" t="s">
+        <v>154</v>
+      </c>
+      <c r="D421" s="135"/>
+      <c r="E421" s="154"/>
+      <c r="F421" s="147"/>
+      <c r="G421" s="185"/>
+      <c r="H421" s="200"/>
+      <c r="I421" s="173"/>
     </row>
     <row r="422" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A422" s="1"/>
       <c r="B422" s="109"/>
-      <c r="C422" s="213" t="s">
-        <v>155</v>
-      </c>
-      <c r="D422" s="135"/>
-      <c r="E422" s="154"/>
-      <c r="F422" s="147"/>
-      <c r="G422" s="185"/>
-      <c r="H422" s="200"/>
-      <c r="I422" s="173"/>
+      <c r="C422" s="213"/>
+      <c r="D422" s="165"/>
+      <c r="E422" s="155"/>
+      <c r="F422" s="148"/>
+      <c r="G422" s="186"/>
+      <c r="H422" s="201"/>
+      <c r="I422" s="174"/>
     </row>
     <row r="423" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A423" s="1"/>
       <c r="B423" s="109"/>
-      <c r="C423" s="213"/>
+      <c r="C423" s="110"/>
       <c r="D423" s="165"/>
       <c r="E423" s="155"/>
       <c r="F423" s="148"/>
@@ -12313,31 +12333,31 @@
     <row r="424" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A424" s="1"/>
       <c r="B424" s="109"/>
-      <c r="C424" s="110"/>
-      <c r="D424" s="165"/>
-      <c r="E424" s="155"/>
-      <c r="F424" s="148"/>
-      <c r="G424" s="186"/>
-      <c r="H424" s="201"/>
-      <c r="I424" s="174"/>
+      <c r="C424" s="213" t="s">
+        <v>155</v>
+      </c>
+      <c r="D424" s="135"/>
+      <c r="E424" s="154"/>
+      <c r="F424" s="147"/>
+      <c r="G424" s="185"/>
+      <c r="H424" s="200"/>
+      <c r="I424" s="173"/>
     </row>
     <row r="425" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A425" s="1"/>
       <c r="B425" s="109"/>
-      <c r="C425" s="213" t="s">
-        <v>156</v>
-      </c>
-      <c r="D425" s="135"/>
-      <c r="E425" s="154"/>
-      <c r="F425" s="147"/>
-      <c r="G425" s="185"/>
-      <c r="H425" s="200"/>
-      <c r="I425" s="173"/>
+      <c r="C425" s="213"/>
+      <c r="D425" s="165"/>
+      <c r="E425" s="155"/>
+      <c r="F425" s="148"/>
+      <c r="G425" s="186"/>
+      <c r="H425" s="201"/>
+      <c r="I425" s="174"/>
     </row>
     <row r="426" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A426" s="1"/>
       <c r="B426" s="109"/>
-      <c r="C426" s="213"/>
+      <c r="C426" s="110"/>
       <c r="D426" s="165"/>
       <c r="E426" s="155"/>
       <c r="F426" s="148"/>
@@ -12348,31 +12368,31 @@
     <row r="427" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A427" s="1"/>
       <c r="B427" s="109"/>
-      <c r="C427" s="110"/>
-      <c r="D427" s="165"/>
-      <c r="E427" s="155"/>
-      <c r="F427" s="148"/>
-      <c r="G427" s="186"/>
-      <c r="H427" s="201"/>
-      <c r="I427" s="174"/>
+      <c r="C427" s="213" t="s">
+        <v>156</v>
+      </c>
+      <c r="D427" s="135"/>
+      <c r="E427" s="154"/>
+      <c r="F427" s="147"/>
+      <c r="G427" s="185"/>
+      <c r="H427" s="200"/>
+      <c r="I427" s="173"/>
     </row>
     <row r="428" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A428" s="1"/>
       <c r="B428" s="109"/>
-      <c r="C428" s="213" t="s">
-        <v>157</v>
-      </c>
-      <c r="D428" s="135"/>
-      <c r="E428" s="154"/>
-      <c r="F428" s="147"/>
-      <c r="G428" s="185"/>
-      <c r="H428" s="200"/>
-      <c r="I428" s="173"/>
+      <c r="C428" s="213"/>
+      <c r="D428" s="165"/>
+      <c r="E428" s="155"/>
+      <c r="F428" s="148"/>
+      <c r="G428" s="186"/>
+      <c r="H428" s="201"/>
+      <c r="I428" s="174"/>
     </row>
     <row r="429" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A429" s="1"/>
       <c r="B429" s="109"/>
-      <c r="C429" s="213"/>
+      <c r="C429" s="110"/>
       <c r="D429" s="165"/>
       <c r="E429" s="155"/>
       <c r="F429" s="148"/>
@@ -12380,33 +12400,23 @@
       <c r="H429" s="201"/>
       <c r="I429" s="174"/>
     </row>
-    <row r="430" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A430" s="1"/>
       <c r="B430" s="109"/>
-      <c r="C430" s="110"/>
-      <c r="D430" s="166" t="s">
-        <v>697</v>
-      </c>
-      <c r="E430" s="157" t="s">
-        <v>698</v>
-      </c>
-      <c r="F430" s="150" t="s">
-        <v>699</v>
-      </c>
-      <c r="G430" s="188">
-        <v>44859</v>
-      </c>
-      <c r="H430" s="203">
-        <v>44477</v>
-      </c>
-      <c r="I430" s="171" t="s">
-        <v>700</v>
-      </c>
+      <c r="C430" s="213" t="s">
+        <v>157</v>
+      </c>
+      <c r="D430" s="135"/>
+      <c r="E430" s="154"/>
+      <c r="F430" s="147"/>
+      <c r="G430" s="185"/>
+      <c r="H430" s="200"/>
+      <c r="I430" s="173"/>
     </row>
     <row r="431" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A431" s="1"/>
       <c r="B431" s="109"/>
-      <c r="C431" s="110"/>
+      <c r="C431" s="213"/>
       <c r="D431" s="165"/>
       <c r="E431" s="155"/>
       <c r="F431" s="148"/>
@@ -12414,85 +12424,73 @@
       <c r="H431" s="201"/>
       <c r="I431" s="174"/>
     </row>
-    <row r="432" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A432" s="1"/>
       <c r="B432" s="109"/>
-      <c r="C432" s="213" t="s">
-        <v>158</v>
-      </c>
-      <c r="D432" s="135"/>
-      <c r="E432" s="154"/>
-      <c r="F432" s="147"/>
-      <c r="G432" s="185"/>
-      <c r="H432" s="200"/>
-      <c r="I432" s="173"/>
+      <c r="C432" s="110"/>
+      <c r="D432" s="166" t="s">
+        <v>697</v>
+      </c>
+      <c r="E432" s="157" t="s">
+        <v>698</v>
+      </c>
+      <c r="F432" s="150" t="s">
+        <v>699</v>
+      </c>
+      <c r="G432" s="188">
+        <v>44859</v>
+      </c>
+      <c r="H432" s="203">
+        <v>44477</v>
+      </c>
+      <c r="I432" s="171" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="433" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A433" s="1"/>
       <c r="B433" s="109"/>
-      <c r="C433" s="213"/>
-      <c r="D433" s="166" t="s">
-        <v>466</v>
-      </c>
-      <c r="E433" s="162" t="s">
-        <v>467</v>
-      </c>
-      <c r="F433" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G433" s="188">
-        <v>44663</v>
-      </c>
-      <c r="H433" s="203">
-        <v>44663</v>
-      </c>
-      <c r="I433" s="198" t="s">
-        <v>759</v>
-      </c>
+      <c r="C433" s="110"/>
+      <c r="D433" s="165"/>
+      <c r="E433" s="155"/>
+      <c r="F433" s="148"/>
+      <c r="G433" s="186"/>
+      <c r="H433" s="201"/>
+      <c r="I433" s="174"/>
     </row>
     <row r="434" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A434" s="1"/>
       <c r="B434" s="109"/>
-      <c r="C434" s="110"/>
-      <c r="D434" s="167" t="s">
-        <v>468</v>
-      </c>
-      <c r="E434" s="160" t="s">
-        <v>469</v>
-      </c>
-      <c r="F434" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G434" s="190">
-        <v>44663</v>
-      </c>
-      <c r="H434" s="204">
-        <v>44663</v>
-      </c>
-      <c r="I434" s="199" t="s">
-        <v>759</v>
-      </c>
+      <c r="C434" s="213" t="s">
+        <v>158</v>
+      </c>
+      <c r="D434" s="135"/>
+      <c r="E434" s="154"/>
+      <c r="F434" s="147"/>
+      <c r="G434" s="185"/>
+      <c r="H434" s="200"/>
+      <c r="I434" s="173"/>
     </row>
     <row r="435" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A435" s="1"/>
       <c r="B435" s="109"/>
-      <c r="C435" s="110"/>
-      <c r="D435" s="167" t="s">
-        <v>471</v>
-      </c>
-      <c r="E435" s="160" t="s">
-        <v>470</v>
-      </c>
-      <c r="F435" s="151" t="s">
+      <c r="C435" s="213"/>
+      <c r="D435" s="166" t="s">
+        <v>466</v>
+      </c>
+      <c r="E435" s="162" t="s">
+        <v>467</v>
+      </c>
+      <c r="F435" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="G435" s="190">
-        <v>44630</v>
-      </c>
-      <c r="H435" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I435" s="199" t="s">
+      <c r="G435" s="188">
+        <v>44663</v>
+      </c>
+      <c r="H435" s="203">
+        <v>44663</v>
+      </c>
+      <c r="I435" s="198" t="s">
         <v>759</v>
       </c>
     </row>
@@ -12501,19 +12499,19 @@
       <c r="B436" s="109"/>
       <c r="C436" s="110"/>
       <c r="D436" s="167" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E436" s="160" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F436" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G436" s="190">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="H436" s="204">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="I436" s="199" t="s">
         <v>759</v>
@@ -12524,16 +12522,16 @@
       <c r="B437" s="109"/>
       <c r="C437" s="110"/>
       <c r="D437" s="167" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="E437" s="160" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="F437" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G437" s="190">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H437" s="204">
         <v>44630</v>
@@ -12547,16 +12545,16 @@
       <c r="B438" s="109"/>
       <c r="C438" s="110"/>
       <c r="D438" s="167" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="E438" s="160" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F438" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G438" s="190">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H438" s="204">
         <v>44630</v>
@@ -12570,19 +12568,19 @@
       <c r="B439" s="109"/>
       <c r="C439" s="110"/>
       <c r="D439" s="167" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="E439" s="160" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F439" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G439" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H439" s="204">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I439" s="199" t="s">
         <v>759</v>
@@ -12593,19 +12591,19 @@
       <c r="B440" s="109"/>
       <c r="C440" s="110"/>
       <c r="D440" s="167" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E440" s="160" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F440" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G440" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H440" s="204">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I440" s="199" t="s">
         <v>759</v>
@@ -12616,19 +12614,19 @@
       <c r="B441" s="109"/>
       <c r="C441" s="110"/>
       <c r="D441" s="167" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E441" s="160" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F441" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G441" s="190">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H441" s="204">
-        <v>44622</v>
+        <v>44824</v>
       </c>
       <c r="I441" s="199" t="s">
         <v>759</v>
@@ -12639,19 +12637,19 @@
       <c r="B442" s="109"/>
       <c r="C442" s="110"/>
       <c r="D442" s="167" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E442" s="160" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="F442" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G442" s="190">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H442" s="204">
-        <v>44621</v>
+        <v>44824</v>
       </c>
       <c r="I442" s="199" t="s">
         <v>759</v>
@@ -12662,19 +12660,19 @@
       <c r="B443" s="109"/>
       <c r="C443" s="110"/>
       <c r="D443" s="167" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E443" s="160" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="F443" s="151" t="s">
         <v>459</v>
       </c>
       <c r="G443" s="190">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H443" s="204">
-        <v>44732</v>
+        <v>44622</v>
       </c>
       <c r="I443" s="199" t="s">
         <v>759</v>
@@ -12685,19 +12683,19 @@
       <c r="B444" s="109"/>
       <c r="C444" s="110"/>
       <c r="D444" s="167" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E444" s="160" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F444" s="151" t="s">
         <v>459</v>
       </c>
       <c r="G444" s="190">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H444" s="204">
-        <v>44732</v>
+        <v>44621</v>
       </c>
       <c r="I444" s="199" t="s">
         <v>759</v>
@@ -12708,19 +12706,19 @@
       <c r="B445" s="109"/>
       <c r="C445" s="110"/>
       <c r="D445" s="167" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E445" s="160" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F445" s="151" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="G445" s="190">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H445" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I445" s="199" t="s">
         <v>759</v>
@@ -12731,19 +12729,19 @@
       <c r="B446" s="109"/>
       <c r="C446" s="110"/>
       <c r="D446" s="167" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="E446" s="160" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F446" s="151" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="G446" s="190">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H446" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I446" s="199" t="s">
         <v>759</v>
@@ -12754,19 +12752,19 @@
       <c r="B447" s="109"/>
       <c r="C447" s="110"/>
       <c r="D447" s="167" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E447" s="160" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="F447" s="151" t="s">
-        <v>267</v>
+        <v>492</v>
       </c>
       <c r="G447" s="190">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H447" s="204">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="I447" s="199" t="s">
         <v>759</v>
@@ -12777,16 +12775,16 @@
       <c r="B448" s="109"/>
       <c r="C448" s="110"/>
       <c r="D448" s="167" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E448" s="160" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="F448" s="151" t="s">
-        <v>267</v>
+        <v>492</v>
       </c>
       <c r="G448" s="190">
-        <v>44644</v>
+        <v>44698</v>
       </c>
       <c r="H448" s="204">
         <v>44621</v>
@@ -12800,19 +12798,19 @@
       <c r="B449" s="109"/>
       <c r="C449" s="110"/>
       <c r="D449" s="167" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E449" s="160" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F449" s="151" t="s">
-        <v>459</v>
+        <v>267</v>
       </c>
       <c r="G449" s="190">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H449" s="204">
-        <v>44621</v>
+        <v>44622</v>
       </c>
       <c r="I449" s="199" t="s">
         <v>759</v>
@@ -12823,16 +12821,16 @@
       <c r="B450" s="109"/>
       <c r="C450" s="110"/>
       <c r="D450" s="167" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E450" s="160" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F450" s="151" t="s">
-        <v>459</v>
+        <v>267</v>
       </c>
       <c r="G450" s="190">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H450" s="204">
         <v>44621</v>
@@ -12846,19 +12844,19 @@
       <c r="B451" s="109"/>
       <c r="C451" s="110"/>
       <c r="D451" s="167" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E451" s="160" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F451" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G451" s="190">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H451" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I451" s="199" t="s">
         <v>759</v>
@@ -12869,19 +12867,19 @@
       <c r="B452" s="109"/>
       <c r="C452" s="110"/>
       <c r="D452" s="167" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="E452" s="160" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F452" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G452" s="190">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H452" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I452" s="199" t="s">
         <v>759</v>
@@ -12892,19 +12890,19 @@
       <c r="B453" s="109"/>
       <c r="C453" s="110"/>
       <c r="D453" s="167" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E453" s="160" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F453" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G453" s="190">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H453" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I453" s="199" t="s">
         <v>759</v>
@@ -12915,19 +12913,19 @@
       <c r="B454" s="109"/>
       <c r="C454" s="110"/>
       <c r="D454" s="167" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E454" s="160" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F454" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G454" s="190">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H454" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I454" s="199" t="s">
         <v>759</v>
@@ -12938,16 +12936,16 @@
       <c r="B455" s="109"/>
       <c r="C455" s="110"/>
       <c r="D455" s="167" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E455" s="160" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="F455" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G455" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H455" s="204">
         <v>44628</v>
@@ -12961,16 +12959,16 @@
       <c r="B456" s="109"/>
       <c r="C456" s="110"/>
       <c r="D456" s="167" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E456" s="160" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F456" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G456" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H456" s="204">
         <v>44628</v>
@@ -12984,16 +12982,16 @@
       <c r="B457" s="109"/>
       <c r="C457" s="110"/>
       <c r="D457" s="167" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E457" s="160" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F457" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G457" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H457" s="204">
         <v>44628</v>
@@ -13007,16 +13005,16 @@
       <c r="B458" s="109"/>
       <c r="C458" s="110"/>
       <c r="D458" s="167" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E458" s="160" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F458" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G458" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H458" s="204">
         <v>44628</v>
@@ -13030,16 +13028,16 @@
       <c r="B459" s="109"/>
       <c r="C459" s="110"/>
       <c r="D459" s="167" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E459" s="160" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F459" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G459" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H459" s="204">
         <v>44628</v>
@@ -13053,16 +13051,16 @@
       <c r="B460" s="109"/>
       <c r="C460" s="110"/>
       <c r="D460" s="167" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="E460" s="160" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="F460" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G460" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H460" s="204">
         <v>44628</v>
@@ -13076,19 +13074,19 @@
       <c r="B461" s="109"/>
       <c r="C461" s="110"/>
       <c r="D461" s="167" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E461" s="160" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F461" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G461" s="190">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H461" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I461" s="199" t="s">
         <v>759</v>
@@ -13099,19 +13097,19 @@
       <c r="B462" s="109"/>
       <c r="C462" s="110"/>
       <c r="D462" s="167" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="E462" s="160" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F462" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G462" s="190">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H462" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I462" s="199" t="s">
         <v>759</v>
@@ -13122,19 +13120,19 @@
       <c r="B463" s="109"/>
       <c r="C463" s="110"/>
       <c r="D463" s="167" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E463" s="160" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="F463" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G463" s="190">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H463" s="204">
-        <v>44662</v>
+        <v>44617</v>
       </c>
       <c r="I463" s="199" t="s">
         <v>759</v>
@@ -13145,19 +13143,19 @@
       <c r="B464" s="109"/>
       <c r="C464" s="110"/>
       <c r="D464" s="167" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E464" s="160" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="F464" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G464" s="190">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H464" s="204">
-        <v>44662</v>
+        <v>44617</v>
       </c>
       <c r="I464" s="199" t="s">
         <v>759</v>
@@ -13167,185 +13165,189 @@
       <c r="A465" s="1"/>
       <c r="B465" s="109"/>
       <c r="C465" s="110"/>
-      <c r="D465" s="165"/>
-      <c r="E465" s="155"/>
-      <c r="F465" s="148"/>
-      <c r="G465" s="186"/>
-      <c r="H465" s="201"/>
-      <c r="I465" s="174"/>
+      <c r="D465" s="167" t="s">
+        <v>527</v>
+      </c>
+      <c r="E465" s="160" t="s">
+        <v>528</v>
+      </c>
+      <c r="F465" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G465" s="190">
+        <v>44740</v>
+      </c>
+      <c r="H465" s="204">
+        <v>44662</v>
+      </c>
+      <c r="I465" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="466" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A466" s="1"/>
       <c r="B466" s="109"/>
-      <c r="C466" s="213" t="s">
-        <v>147</v>
-      </c>
-      <c r="D466" s="135"/>
-      <c r="E466" s="154"/>
-      <c r="F466" s="147"/>
-      <c r="G466" s="185"/>
-      <c r="H466" s="200"/>
-      <c r="I466" s="173"/>
+      <c r="C466" s="110"/>
+      <c r="D466" s="167" t="s">
+        <v>530</v>
+      </c>
+      <c r="E466" s="160" t="s">
+        <v>529</v>
+      </c>
+      <c r="F466" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G466" s="190">
+        <v>44740</v>
+      </c>
+      <c r="H466" s="204">
+        <v>44662</v>
+      </c>
+      <c r="I466" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="467" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A467" s="1"/>
       <c r="B467" s="109"/>
-      <c r="C467" s="213"/>
-      <c r="D467" s="166" t="s">
-        <v>274</v>
-      </c>
-      <c r="E467" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="F467" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G467" s="188">
-        <v>44167</v>
-      </c>
-      <c r="H467" s="203">
-        <v>44167</v>
-      </c>
-      <c r="I467" s="176"/>
+      <c r="C467" s="110"/>
+      <c r="D467" s="165"/>
+      <c r="E467" s="155"/>
+      <c r="F467" s="148"/>
+      <c r="G467" s="186"/>
+      <c r="H467" s="201"/>
+      <c r="I467" s="174"/>
     </row>
     <row r="468" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A468" s="1"/>
       <c r="B468" s="109"/>
-      <c r="C468" s="110"/>
-      <c r="D468" s="167" t="s">
-        <v>445</v>
-      </c>
-      <c r="E468" s="160" t="s">
-        <v>446</v>
-      </c>
-      <c r="F468" s="151" t="s">
-        <v>256</v>
-      </c>
-      <c r="G468" s="190">
-        <v>44575</v>
-      </c>
-      <c r="H468" s="204">
-        <v>44167</v>
-      </c>
-      <c r="I468" s="177"/>
-    </row>
-    <row r="469" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C468" s="213" t="s">
+        <v>147</v>
+      </c>
+      <c r="D468" s="135"/>
+      <c r="E468" s="154"/>
+      <c r="F468" s="147"/>
+      <c r="G468" s="185"/>
+      <c r="H468" s="200"/>
+      <c r="I468" s="173"/>
+    </row>
+    <row r="469" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A469" s="1"/>
       <c r="B469" s="109"/>
-      <c r="C469" s="110"/>
-      <c r="D469" s="167" t="s">
-        <v>448</v>
-      </c>
-      <c r="E469" s="158" t="s">
-        <v>447</v>
-      </c>
-      <c r="F469" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G469" s="190">
-        <v>44404</v>
-      </c>
-      <c r="H469" s="204">
-        <v>44404</v>
-      </c>
-      <c r="I469" s="177"/>
+      <c r="C469" s="213"/>
+      <c r="D469" s="166" t="s">
+        <v>274</v>
+      </c>
+      <c r="E469" s="162" t="s">
+        <v>444</v>
+      </c>
+      <c r="F469" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G469" s="188">
+        <v>44167</v>
+      </c>
+      <c r="H469" s="203">
+        <v>44167</v>
+      </c>
+      <c r="I469" s="176"/>
     </row>
     <row r="470" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A470" s="1"/>
       <c r="B470" s="109"/>
       <c r="C470" s="110"/>
-      <c r="D470" s="165"/>
-      <c r="E470" s="155"/>
-      <c r="F470" s="148"/>
-      <c r="G470" s="186"/>
-      <c r="H470" s="201"/>
-      <c r="I470" s="174"/>
-    </row>
-    <row r="471" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D470" s="167" t="s">
+        <v>445</v>
+      </c>
+      <c r="E470" s="160" t="s">
+        <v>446</v>
+      </c>
+      <c r="F470" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G470" s="190">
+        <v>44575</v>
+      </c>
+      <c r="H470" s="204">
+        <v>44167</v>
+      </c>
+      <c r="I470" s="177"/>
+    </row>
+    <row r="471" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A471" s="1"/>
       <c r="B471" s="109"/>
-      <c r="C471" s="213" t="s">
-        <v>159</v>
-      </c>
-      <c r="D471" s="135"/>
-      <c r="E471" s="154"/>
-      <c r="F471" s="147"/>
-      <c r="G471" s="185"/>
-      <c r="H471" s="200"/>
-      <c r="I471" s="173"/>
+      <c r="C471" s="110"/>
+      <c r="D471" s="167" t="s">
+        <v>448</v>
+      </c>
+      <c r="E471" s="158" t="s">
+        <v>447</v>
+      </c>
+      <c r="F471" s="151" t="s">
+        <v>281</v>
+      </c>
+      <c r="G471" s="190">
+        <v>44404</v>
+      </c>
+      <c r="H471" s="204">
+        <v>44404</v>
+      </c>
+      <c r="I471" s="177"/>
     </row>
     <row r="472" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A472" s="1"/>
       <c r="B472" s="109"/>
-      <c r="C472" s="213"/>
-      <c r="D472" s="166" t="s">
-        <v>450</v>
-      </c>
-      <c r="E472" s="162" t="s">
-        <v>449</v>
-      </c>
-      <c r="F472" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G472" s="188">
-        <v>44635</v>
-      </c>
-      <c r="H472" s="203">
-        <v>44635</v>
-      </c>
-      <c r="I472" s="176"/>
+      <c r="C472" s="110"/>
+      <c r="D472" s="165"/>
+      <c r="E472" s="155"/>
+      <c r="F472" s="148"/>
+      <c r="G472" s="186"/>
+      <c r="H472" s="201"/>
+      <c r="I472" s="174"/>
     </row>
     <row r="473" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A473" s="1"/>
       <c r="B473" s="109"/>
-      <c r="C473" s="110"/>
-      <c r="D473" s="167" t="s">
-        <v>452</v>
-      </c>
-      <c r="E473" s="160" t="s">
-        <v>451</v>
-      </c>
-      <c r="F473" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G473" s="190">
-        <v>44635</v>
-      </c>
-      <c r="H473" s="204">
-        <v>44635</v>
-      </c>
-      <c r="I473" s="177"/>
+      <c r="C473" s="213" t="s">
+        <v>159</v>
+      </c>
+      <c r="D473" s="135"/>
+      <c r="E473" s="154"/>
+      <c r="F473" s="147"/>
+      <c r="G473" s="185"/>
+      <c r="H473" s="200"/>
+      <c r="I473" s="173"/>
     </row>
     <row r="474" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A474" s="1"/>
       <c r="B474" s="109"/>
-      <c r="C474" s="110"/>
-      <c r="D474" s="167" t="s">
-        <v>453</v>
-      </c>
-      <c r="E474" s="160" t="s">
-        <v>455</v>
-      </c>
-      <c r="F474" s="151" t="s">
+      <c r="C474" s="213"/>
+      <c r="D474" s="166" t="s">
+        <v>450</v>
+      </c>
+      <c r="E474" s="162" t="s">
+        <v>449</v>
+      </c>
+      <c r="F474" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="G474" s="190">
+      <c r="G474" s="188">
         <v>44635</v>
       </c>
-      <c r="H474" s="204">
+      <c r="H474" s="203">
         <v>44635</v>
       </c>
-      <c r="I474" s="177"/>
+      <c r="I474" s="176"/>
     </row>
     <row r="475" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A475" s="1"/>
       <c r="B475" s="109"/>
       <c r="C475" s="110"/>
       <c r="D475" s="167" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E475" s="160" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F475" s="151" t="s">
         <v>232</v>
@@ -13363,19 +13365,19 @@
       <c r="B476" s="109"/>
       <c r="C476" s="110"/>
       <c r="D476" s="167" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E476" s="160" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F476" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G476" s="190">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H476" s="204">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="I476" s="177"/>
     </row>
@@ -13384,19 +13386,19 @@
       <c r="B477" s="109"/>
       <c r="C477" s="110"/>
       <c r="D477" s="167" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E477" s="160" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="F477" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G477" s="190">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H477" s="204">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="I477" s="177"/>
     </row>
@@ -13405,19 +13407,19 @@
       <c r="B478" s="109"/>
       <c r="C478" s="110"/>
       <c r="D478" s="167" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E478" s="160" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F478" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G478" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H478" s="204">
         <v>44644</v>
-      </c>
-      <c r="H478" s="204">
-        <v>44636</v>
       </c>
       <c r="I478" s="177"/>
     </row>
@@ -13426,19 +13428,19 @@
       <c r="B479" s="109"/>
       <c r="C479" s="110"/>
       <c r="D479" s="167" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="E479" s="160" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F479" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G479" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H479" s="204">
         <v>44644</v>
-      </c>
-      <c r="H479" s="204">
-        <v>44636</v>
       </c>
       <c r="I479" s="177"/>
     </row>
@@ -13446,133 +13448,129 @@
       <c r="A480" s="1"/>
       <c r="B480" s="109"/>
       <c r="C480" s="110"/>
-      <c r="D480" s="165"/>
-      <c r="E480" s="155"/>
-      <c r="F480" s="148"/>
-      <c r="G480" s="186"/>
-      <c r="H480" s="201"/>
-      <c r="I480" s="174"/>
-    </row>
-    <row r="481" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A481" s="136"/>
-      <c r="B481" s="212" t="s">
+      <c r="D480" s="167" t="s">
+        <v>462</v>
+      </c>
+      <c r="E480" s="160" t="s">
+        <v>463</v>
+      </c>
+      <c r="F480" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G480" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H480" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I480" s="177"/>
+    </row>
+    <row r="481" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A481" s="1"/>
+      <c r="B481" s="109"/>
+      <c r="C481" s="110"/>
+      <c r="D481" s="167" t="s">
+        <v>464</v>
+      </c>
+      <c r="E481" s="160" t="s">
+        <v>465</v>
+      </c>
+      <c r="F481" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G481" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H481" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I481" s="177"/>
+    </row>
+    <row r="482" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A482" s="1"/>
+      <c r="B482" s="109"/>
+      <c r="C482" s="110"/>
+      <c r="D482" s="165"/>
+      <c r="E482" s="155"/>
+      <c r="F482" s="148"/>
+      <c r="G482" s="186"/>
+      <c r="H482" s="201"/>
+      <c r="I482" s="174"/>
+    </row>
+    <row r="483" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A483" s="136"/>
+      <c r="B483" s="212" t="s">
         <v>144</v>
       </c>
-      <c r="C481" s="134"/>
-      <c r="D481" s="135"/>
-      <c r="E481" s="154"/>
-      <c r="F481" s="147"/>
-      <c r="G481" s="185"/>
-      <c r="H481" s="200"/>
-      <c r="I481" s="173"/>
-    </row>
-    <row r="482" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A482" s="136"/>
-      <c r="B482" s="212"/>
-      <c r="C482" s="213" t="s">
+      <c r="C483" s="134"/>
+      <c r="D483" s="135"/>
+      <c r="E483" s="154"/>
+      <c r="F483" s="147"/>
+      <c r="G483" s="185"/>
+      <c r="H483" s="200"/>
+      <c r="I483" s="173"/>
+    </row>
+    <row r="484" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A484" s="136"/>
+      <c r="B484" s="212"/>
+      <c r="C484" s="213" t="s">
         <v>146</v>
       </c>
-      <c r="D482" s="135"/>
-      <c r="E482" s="154"/>
-      <c r="F482" s="147"/>
-      <c r="G482" s="185"/>
-      <c r="H482" s="200"/>
-      <c r="I482" s="173"/>
-    </row>
-    <row r="483" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A483" s="1"/>
-      <c r="B483" s="109"/>
-      <c r="C483" s="213"/>
-      <c r="D483" s="165"/>
-      <c r="E483" s="155"/>
-      <c r="F483" s="148"/>
-      <c r="G483" s="186"/>
-      <c r="H483" s="201"/>
-      <c r="I483" s="174"/>
-    </row>
-    <row r="484" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A484" s="1"/>
-      <c r="B484" s="109"/>
-      <c r="C484" s="110"/>
-      <c r="D484" s="165"/>
-      <c r="E484" s="155"/>
-      <c r="F484" s="148"/>
-      <c r="G484" s="186"/>
-      <c r="H484" s="201"/>
-      <c r="I484" s="174"/>
-    </row>
-    <row r="485" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D484" s="135"/>
+      <c r="E484" s="154"/>
+      <c r="F484" s="147"/>
+      <c r="G484" s="185"/>
+      <c r="H484" s="200"/>
+      <c r="I484" s="173"/>
+    </row>
+    <row r="485" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A485" s="1"/>
       <c r="B485" s="109"/>
-      <c r="C485" s="110"/>
-      <c r="D485" s="144"/>
-      <c r="E485" s="156"/>
-      <c r="F485" s="149"/>
-      <c r="G485" s="187"/>
-      <c r="H485" s="202"/>
-      <c r="I485" s="175"/>
-    </row>
-    <row r="486" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A486" s="136"/>
+      <c r="C485" s="213"/>
+      <c r="D485" s="165"/>
+      <c r="E485" s="155"/>
+      <c r="F485" s="148"/>
+      <c r="G485" s="186"/>
+      <c r="H485" s="201"/>
+      <c r="I485" s="174"/>
+    </row>
+    <row r="486" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A486" s="1"/>
       <c r="B486" s="109"/>
       <c r="C486" s="110"/>
-      <c r="D486" s="166" t="s">
-        <v>858</v>
-      </c>
-      <c r="E486" s="162" t="s">
-        <v>860</v>
-      </c>
-      <c r="F486" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G486" s="188">
-        <v>44950</v>
-      </c>
-      <c r="H486" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I486" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="487" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A487" s="136"/>
+      <c r="D486" s="165"/>
+      <c r="E486" s="155"/>
+      <c r="F486" s="148"/>
+      <c r="G486" s="186"/>
+      <c r="H486" s="201"/>
+      <c r="I486" s="174"/>
+    </row>
+    <row r="487" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A487" s="1"/>
       <c r="B487" s="109"/>
       <c r="C487" s="110"/>
-      <c r="D487" s="167" t="s">
-        <v>859</v>
-      </c>
-      <c r="E487" s="158" t="s">
-        <v>861</v>
-      </c>
-      <c r="F487" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G487" s="190">
-        <v>44950</v>
-      </c>
-      <c r="H487" s="204">
-        <v>44893</v>
-      </c>
-      <c r="I487" s="171" t="s">
-        <v>727</v>
-      </c>
+      <c r="D487" s="144"/>
+      <c r="E487" s="156"/>
+      <c r="F487" s="149"/>
+      <c r="G487" s="187"/>
+      <c r="H487" s="202"/>
+      <c r="I487" s="175"/>
     </row>
     <row r="488" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A488" s="136"/>
       <c r="B488" s="109"/>
       <c r="C488" s="110"/>
       <c r="D488" s="166" t="s">
-        <v>862</v>
-      </c>
-      <c r="E488" s="157" t="s">
-        <v>864</v>
+        <v>858</v>
+      </c>
+      <c r="E488" s="162" t="s">
+        <v>860</v>
       </c>
       <c r="F488" s="150" t="s">
-        <v>548</v>
+        <v>267</v>
       </c>
       <c r="G488" s="188">
-        <v>44970</v>
+        <v>44950</v>
       </c>
       <c r="H488" s="203">
         <v>44893</v>
@@ -13585,171 +13583,195 @@
       <c r="A489" s="136"/>
       <c r="B489" s="109"/>
       <c r="C489" s="110"/>
-      <c r="D489" s="166" t="s">
-        <v>863</v>
-      </c>
-      <c r="E489" s="157" t="s">
-        <v>865</v>
-      </c>
-      <c r="F489" s="150" t="s">
-        <v>548</v>
-      </c>
-      <c r="G489" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H489" s="203">
+      <c r="D489" s="167" t="s">
+        <v>859</v>
+      </c>
+      <c r="E489" s="158" t="s">
+        <v>861</v>
+      </c>
+      <c r="F489" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G489" s="190">
+        <v>44950</v>
+      </c>
+      <c r="H489" s="204">
         <v>44893</v>
       </c>
       <c r="I489" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="490" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A490" s="136"/>
       <c r="B490" s="109"/>
       <c r="C490" s="110"/>
-      <c r="D490" s="166"/>
-      <c r="E490" s="157"/>
-      <c r="F490" s="150"/>
-      <c r="G490" s="188"/>
-      <c r="H490" s="203"/>
-      <c r="I490" s="171"/>
+      <c r="D490" s="166" t="s">
+        <v>862</v>
+      </c>
+      <c r="E490" s="157" t="s">
+        <v>864</v>
+      </c>
+      <c r="F490" s="150" t="s">
+        <v>548</v>
+      </c>
+      <c r="G490" s="188">
+        <v>44970</v>
+      </c>
+      <c r="H490" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I490" s="171" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="491" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A491" s="136"/>
       <c r="B491" s="109"/>
       <c r="C491" s="110"/>
       <c r="D491" s="166" t="s">
-        <v>934</v>
+        <v>863</v>
       </c>
       <c r="E491" s="157" t="s">
-        <v>936</v>
+        <v>865</v>
       </c>
       <c r="F491" s="150" t="s">
-        <v>232</v>
+        <v>548</v>
       </c>
       <c r="G491" s="188">
-        <v>45009</v>
+        <v>44970</v>
       </c>
       <c r="H491" s="203">
-        <v>45009</v>
+        <v>44893</v>
       </c>
       <c r="I491" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="492" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A492" s="136"/>
       <c r="B492" s="109"/>
       <c r="C492" s="110"/>
-      <c r="D492" s="166" t="s">
-        <v>933</v>
-      </c>
-      <c r="E492" s="157" t="s">
-        <v>935</v>
-      </c>
-      <c r="F492" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G492" s="188">
-        <v>45009</v>
-      </c>
-      <c r="H492" s="203">
-        <v>45009</v>
-      </c>
-      <c r="I492" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="493" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D492" s="166"/>
+      <c r="E492" s="157"/>
+      <c r="F492" s="150"/>
+      <c r="G492" s="188"/>
+      <c r="H492" s="203"/>
+      <c r="I492" s="171"/>
+    </row>
+    <row r="493" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A493" s="136"/>
       <c r="B493" s="109"/>
       <c r="C493" s="110"/>
-      <c r="D493" s="166"/>
-      <c r="E493" s="157"/>
-      <c r="F493" s="150"/>
-      <c r="G493" s="188"/>
-      <c r="H493" s="203"/>
-      <c r="I493" s="171"/>
+      <c r="D493" s="166" t="s">
+        <v>934</v>
+      </c>
+      <c r="E493" s="157" t="s">
+        <v>936</v>
+      </c>
+      <c r="F493" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G493" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H493" s="203">
+        <v>45009</v>
+      </c>
+      <c r="I493" s="171" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="494" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A494" s="136"/>
       <c r="B494" s="109"/>
       <c r="C494" s="110"/>
       <c r="D494" s="166" t="s">
-        <v>854</v>
-      </c>
-      <c r="E494" s="162" t="s">
-        <v>857</v>
+        <v>933</v>
+      </c>
+      <c r="E494" s="157" t="s">
+        <v>935</v>
       </c>
       <c r="F494" s="150" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G494" s="188">
-        <v>44986</v>
+        <v>45009</v>
       </c>
       <c r="H494" s="203">
-        <v>44951</v>
+        <v>45009</v>
       </c>
       <c r="I494" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="495" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A495" s="136"/>
       <c r="B495" s="109"/>
       <c r="C495" s="110"/>
-      <c r="D495" s="167" t="s">
+      <c r="D495" s="166"/>
+      <c r="E495" s="157"/>
+      <c r="F495" s="150"/>
+      <c r="G495" s="188"/>
+      <c r="H495" s="203"/>
+      <c r="I495" s="171"/>
+    </row>
+    <row r="496" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A496" s="136"/>
+      <c r="B496" s="109"/>
+      <c r="C496" s="110"/>
+      <c r="D496" s="166" t="s">
+        <v>854</v>
+      </c>
+      <c r="E496" s="162" t="s">
+        <v>857</v>
+      </c>
+      <c r="F496" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G496" s="188">
+        <v>44986</v>
+      </c>
+      <c r="H496" s="203">
+        <v>44951</v>
+      </c>
+      <c r="I496" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="497" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A497" s="136"/>
+      <c r="B497" s="109"/>
+      <c r="C497" s="110"/>
+      <c r="D497" s="167" t="s">
         <v>855</v>
       </c>
-      <c r="E495" s="158" t="s">
+      <c r="E497" s="158" t="s">
         <v>856</v>
       </c>
-      <c r="F495" s="151" t="s">
+      <c r="F497" s="151" t="s">
         <v>267</v>
       </c>
-      <c r="G495" s="190">
+      <c r="G497" s="190">
         <v>44986</v>
       </c>
-      <c r="H495" s="204">
+      <c r="H497" s="204">
         <v>44951</v>
       </c>
-      <c r="I495" s="171" t="s">
+      <c r="I497" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="496" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A496" s="136"/>
-      <c r="B496" s="111"/>
-      <c r="C496" s="112"/>
-      <c r="D496" s="170"/>
-      <c r="E496" s="163"/>
-      <c r="F496" s="153"/>
-      <c r="G496" s="191"/>
-      <c r="H496" s="206"/>
-      <c r="I496" s="179"/>
-    </row>
-    <row r="497" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A497" s="1"/>
-      <c r="B497" s="1"/>
-      <c r="C497" s="1"/>
-      <c r="D497" s="1"/>
-      <c r="E497" s="146"/>
-      <c r="F497" s="113"/>
-      <c r="G497" s="192"/>
-      <c r="H497" s="192"/>
-      <c r="I497" s="180"/>
-    </row>
-    <row r="498" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A498" s="1"/>
-      <c r="B498" s="1"/>
-      <c r="C498" s="1"/>
-      <c r="D498" s="1"/>
-      <c r="E498" s="146"/>
-      <c r="F498" s="113"/>
-      <c r="G498" s="192"/>
-      <c r="H498" s="192"/>
-      <c r="I498" s="180"/>
+    <row r="498" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A498" s="136"/>
+      <c r="B498" s="111"/>
+      <c r="C498" s="112"/>
+      <c r="D498" s="170"/>
+      <c r="E498" s="163"/>
+      <c r="F498" s="153"/>
+      <c r="G498" s="191"/>
+      <c r="H498" s="206"/>
+      <c r="I498" s="179"/>
     </row>
     <row r="499" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A499" s="1"/>
@@ -13905,34 +13927,56 @@
       <c r="H512" s="192"/>
       <c r="I512" s="180"/>
     </row>
-    <row r="513" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E513" s="145"/>
-      <c r="F513" s="95"/>
-      <c r="G513" s="193"/>
-      <c r="H513" s="193"/>
-      <c r="I513" s="181"/>
-    </row>
-    <row r="514" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E514" s="145"/>
-      <c r="F514" s="95"/>
-      <c r="G514" s="193"/>
-      <c r="H514" s="193"/>
-      <c r="I514" s="181"/>
-    </row>
-    <row r="515" spans="5:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+    <row r="513" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A513" s="1"/>
+      <c r="B513" s="1"/>
+      <c r="C513" s="1"/>
+      <c r="D513" s="1"/>
+      <c r="E513" s="146"/>
+      <c r="F513" s="113"/>
+      <c r="G513" s="192"/>
+      <c r="H513" s="192"/>
+      <c r="I513" s="180"/>
+    </row>
+    <row r="514" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A514" s="1"/>
+      <c r="B514" s="1"/>
+      <c r="C514" s="1"/>
+      <c r="D514" s="1"/>
+      <c r="E514" s="146"/>
+      <c r="F514" s="113"/>
+      <c r="G514" s="192"/>
+      <c r="H514" s="192"/>
+      <c r="I514" s="180"/>
+    </row>
+    <row r="515" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="E515" s="145"/>
       <c r="F515" s="95"/>
       <c r="G515" s="193"/>
       <c r="H515" s="193"/>
       <c r="I515" s="181"/>
     </row>
+    <row r="516" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E516" s="145"/>
+      <c r="F516" s="95"/>
+      <c r="G516" s="193"/>
+      <c r="H516" s="193"/>
+      <c r="I516" s="181"/>
+    </row>
+    <row r="517" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E517" s="145"/>
+      <c r="F517" s="95"/>
+      <c r="G517" s="193"/>
+      <c r="H517" s="193"/>
+      <c r="I517" s="181"/>
+    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B380:B381"/>
-    <mergeCell ref="C381:C382"/>
+    <mergeCell ref="B382:B383"/>
+    <mergeCell ref="C383:C384"/>
     <mergeCell ref="C204:C205"/>
-    <mergeCell ref="B376:B377"/>
-    <mergeCell ref="C377:C378"/>
+    <mergeCell ref="B378:B379"/>
+    <mergeCell ref="C379:C380"/>
     <mergeCell ref="C282:C283"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="B4:B5"/>
@@ -13941,24 +13985,24 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C72:C73"/>
     <mergeCell ref="C132:C133"/>
-    <mergeCell ref="C471:C472"/>
-    <mergeCell ref="C391:C392"/>
-    <mergeCell ref="C394:C395"/>
-    <mergeCell ref="C416:C417"/>
-    <mergeCell ref="C419:C420"/>
-    <mergeCell ref="C422:C423"/>
+    <mergeCell ref="C473:C474"/>
+    <mergeCell ref="C393:C394"/>
+    <mergeCell ref="C396:C397"/>
+    <mergeCell ref="C418:C419"/>
+    <mergeCell ref="C421:C422"/>
+    <mergeCell ref="C424:C425"/>
     <mergeCell ref="C135:C136"/>
     <mergeCell ref="C144:C145"/>
     <mergeCell ref="C185:C186"/>
-    <mergeCell ref="B481:B482"/>
-    <mergeCell ref="C482:C483"/>
+    <mergeCell ref="B483:B484"/>
+    <mergeCell ref="C484:C485"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C425:C426"/>
-    <mergeCell ref="C428:C429"/>
-    <mergeCell ref="C432:C433"/>
-    <mergeCell ref="C466:C467"/>
-    <mergeCell ref="C384:C385"/>
-    <mergeCell ref="C388:C389"/>
+    <mergeCell ref="C427:C428"/>
+    <mergeCell ref="C430:C431"/>
+    <mergeCell ref="C434:C435"/>
+    <mergeCell ref="C468:C469"/>
+    <mergeCell ref="C386:C387"/>
+    <mergeCell ref="C390:C391"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C15:C16"/>

</xml_diff>

<commit_message>
Update Pertanggal 5 Mei 2023 10:30 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="968">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1584" uniqueCount="972">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -3134,6 +3134,18 @@
   <si>
     <t>SchData-OLTP-Budgeting.
 HoldFunc_GetDataList_CombinedBudgetSectionDetail</t>
+  </si>
+  <si>
+    <t>Func_TblPurchaseOrderPaymentTermDetail_INSERT</t>
+  </si>
+  <si>
+    <t>Func_TblPurchaseOrderPaymentTermDetail_UPDATE</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblPurchaseOrderPaymentTermDetail</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblPurchaseOrderPaymentTermDetail</t>
   </si>
 </sst>
 </file>
@@ -4537,12 +4549,30 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4561,20 +4591,71 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4582,12 +4663,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -4597,66 +4672,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4668,9 +4683,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4983,13 +4995,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I533"/>
+  <dimension ref="A1:I535"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E456" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomRight" activeCell="D466" sqref="D466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5008,20 +5020,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="217" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="223"/>
-      <c r="D2" s="224"/>
-      <c r="E2" s="218" t="s">
+      <c r="C2" s="218"/>
+      <c r="D2" s="219"/>
+      <c r="E2" s="224" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="214" t="s">
+      <c r="F2" s="220" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="215"/>
-      <c r="H2" s="216"/>
-      <c r="I2" s="220" t="s">
+      <c r="G2" s="221"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="215" t="s">
         <v>670</v>
       </c>
     </row>
@@ -5035,7 +5047,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="219"/>
+      <c r="E3" s="225"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -5045,11 +5057,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="221"/>
+      <c r="I3" s="216"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="217" t="s">
+      <c r="B4" s="223" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -5062,8 +5074,8 @@
     </row>
     <row r="5" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="136"/>
-      <c r="B5" s="212"/>
-      <c r="C5" s="213" t="s">
+      <c r="B5" s="213"/>
+      <c r="C5" s="214" t="s">
         <v>160</v>
       </c>
       <c r="D5" s="135"/>
@@ -5076,7 +5088,7 @@
     <row r="6" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="109"/>
-      <c r="C6" s="213"/>
+      <c r="C6" s="214"/>
       <c r="D6" s="165"/>
       <c r="E6" s="155"/>
       <c r="F6" s="148"/>
@@ -5098,7 +5110,7 @@
     <row r="8" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="109"/>
-      <c r="C8" s="213" t="s">
+      <c r="C8" s="214" t="s">
         <v>161</v>
       </c>
       <c r="D8" s="135"/>
@@ -5111,7 +5123,7 @@
     <row r="9" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="109"/>
-      <c r="C9" s="213"/>
+      <c r="C9" s="214"/>
       <c r="D9" s="165"/>
       <c r="E9" s="155"/>
       <c r="F9" s="148"/>
@@ -5133,7 +5145,7 @@
     <row r="11" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="109"/>
-      <c r="C11" s="213" t="s">
+      <c r="C11" s="214" t="s">
         <v>162</v>
       </c>
       <c r="D11" s="135"/>
@@ -5146,7 +5158,7 @@
     <row r="12" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="109"/>
-      <c r="C12" s="213"/>
+      <c r="C12" s="214"/>
       <c r="D12" s="165"/>
       <c r="E12" s="155"/>
       <c r="F12" s="148"/>
@@ -5215,7 +5227,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="109"/>
       <c r="C16" s="110"/>
-      <c r="D16" s="256" t="s">
+      <c r="D16" s="212" t="s">
         <v>965</v>
       </c>
       <c r="E16" s="158" t="s">
@@ -5248,7 +5260,7 @@
     <row r="18" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="109"/>
-      <c r="C18" s="213" t="s">
+      <c r="C18" s="214" t="s">
         <v>163</v>
       </c>
       <c r="D18" s="135"/>
@@ -5261,7 +5273,7 @@
     <row r="19" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="109"/>
-      <c r="C19" s="213"/>
+      <c r="C19" s="214"/>
       <c r="D19" s="165"/>
       <c r="E19" s="155"/>
       <c r="F19" s="148"/>
@@ -5283,7 +5295,7 @@
     <row r="21" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="109"/>
-      <c r="C21" s="213" t="s">
+      <c r="C21" s="214" t="s">
         <v>164</v>
       </c>
       <c r="D21" s="135"/>
@@ -5296,7 +5308,7 @@
     <row r="22" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="109"/>
-      <c r="C22" s="213"/>
+      <c r="C22" s="214"/>
       <c r="D22" s="165"/>
       <c r="E22" s="155"/>
       <c r="F22" s="148"/>
@@ -5318,7 +5330,7 @@
     <row r="24" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="109"/>
-      <c r="C24" s="213" t="s">
+      <c r="C24" s="214" t="s">
         <v>4</v>
       </c>
       <c r="D24" s="135"/>
@@ -5331,7 +5343,7 @@
     <row r="25" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="109"/>
-      <c r="C25" s="213"/>
+      <c r="C25" s="214"/>
       <c r="D25" s="165"/>
       <c r="E25" s="155"/>
       <c r="F25" s="148"/>
@@ -5925,7 +5937,7 @@
     <row r="55" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
       <c r="B55" s="109"/>
-      <c r="C55" s="213" t="s">
+      <c r="C55" s="214" t="s">
         <v>165</v>
       </c>
       <c r="D55" s="135"/>
@@ -5938,7 +5950,7 @@
     <row r="56" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
       <c r="B56" s="109"/>
-      <c r="C56" s="213"/>
+      <c r="C56" s="214"/>
       <c r="D56" s="165"/>
       <c r="E56" s="155"/>
       <c r="F56" s="148"/>
@@ -5960,7 +5972,7 @@
     <row r="58" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
       <c r="B58" s="109"/>
-      <c r="C58" s="213" t="s">
+      <c r="C58" s="214" t="s">
         <v>166</v>
       </c>
       <c r="D58" s="135"/>
@@ -5973,7 +5985,7 @@
     <row r="59" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="B59" s="109"/>
-      <c r="C59" s="213"/>
+      <c r="C59" s="214"/>
       <c r="D59" s="165"/>
       <c r="E59" s="155"/>
       <c r="F59" s="148"/>
@@ -6209,7 +6221,7 @@
     <row r="75" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="109"/>
-      <c r="C75" s="213" t="s">
+      <c r="C75" s="214" t="s">
         <v>75</v>
       </c>
       <c r="D75" s="135"/>
@@ -6222,7 +6234,7 @@
     <row r="76" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="109"/>
-      <c r="C76" s="213"/>
+      <c r="C76" s="214"/>
       <c r="D76" s="165" t="s">
         <v>561</v>
       </c>
@@ -7191,7 +7203,7 @@
     <row r="135" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1"/>
       <c r="B135" s="109"/>
-      <c r="C135" s="213" t="s">
+      <c r="C135" s="214" t="s">
         <v>167</v>
       </c>
       <c r="D135" s="135"/>
@@ -7204,7 +7216,7 @@
     <row r="136" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="1"/>
       <c r="B136" s="109"/>
-      <c r="C136" s="213"/>
+      <c r="C136" s="214"/>
       <c r="D136" s="165"/>
       <c r="E136" s="155"/>
       <c r="F136" s="148"/>
@@ -7226,7 +7238,7 @@
     <row r="138" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1"/>
       <c r="B138" s="109"/>
-      <c r="C138" s="213" t="s">
+      <c r="C138" s="214" t="s">
         <v>168</v>
       </c>
       <c r="D138" s="135"/>
@@ -7239,7 +7251,7 @@
     <row r="139" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="1"/>
       <c r="B139" s="109"/>
-      <c r="C139" s="213"/>
+      <c r="C139" s="214"/>
       <c r="D139" s="165"/>
       <c r="E139" s="155"/>
       <c r="F139" s="148"/>
@@ -7375,7 +7387,7 @@
     <row r="147" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1"/>
       <c r="B147" s="109"/>
-      <c r="C147" s="213" t="s">
+      <c r="C147" s="214" t="s">
         <v>169</v>
       </c>
       <c r="D147" s="135"/>
@@ -7388,7 +7400,7 @@
     <row r="148" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A148" s="1"/>
       <c r="B148" s="109"/>
-      <c r="C148" s="213"/>
+      <c r="C148" s="214"/>
       <c r="D148" s="166" t="s">
         <v>531</v>
       </c>
@@ -8140,7 +8152,7 @@
     <row r="188" spans="1:9" s="78" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1"/>
       <c r="B188" s="109"/>
-      <c r="C188" s="213" t="s">
+      <c r="C188" s="214" t="s">
         <v>57</v>
       </c>
       <c r="D188" s="135"/>
@@ -8153,7 +8165,7 @@
     <row r="189" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A189" s="1"/>
       <c r="B189" s="109"/>
-      <c r="C189" s="213"/>
+      <c r="C189" s="214"/>
       <c r="D189" s="166" t="s">
         <v>419</v>
       </c>
@@ -8495,7 +8507,7 @@
     <row r="207" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A207" s="1"/>
       <c r="B207" s="109"/>
-      <c r="C207" s="213" t="s">
+      <c r="C207" s="214" t="s">
         <v>170</v>
       </c>
       <c r="D207" s="135"/>
@@ -8508,7 +8520,7 @@
     <row r="208" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A208" s="1"/>
       <c r="B208" s="109"/>
-      <c r="C208" s="213"/>
+      <c r="C208" s="214"/>
       <c r="D208" s="166" t="s">
         <v>643</v>
       </c>
@@ -10278,7 +10290,7 @@
     <row r="298" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A298" s="1"/>
       <c r="B298" s="109"/>
-      <c r="C298" s="213" t="s">
+      <c r="C298" s="214" t="s">
         <v>146</v>
       </c>
       <c r="D298" s="135"/>
@@ -10291,7 +10303,7 @@
     <row r="299" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A299" s="1"/>
       <c r="B299" s="109"/>
-      <c r="C299" s="213"/>
+      <c r="C299" s="214"/>
       <c r="D299" s="166" t="s">
         <v>274</v>
       </c>
@@ -12075,7 +12087,7 @@
     </row>
     <row r="394" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A394" s="136"/>
-      <c r="B394" s="212" t="s">
+      <c r="B394" s="213" t="s">
         <v>142</v>
       </c>
       <c r="C394" s="134"/>
@@ -12088,8 +12100,8 @@
     </row>
     <row r="395" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A395" s="136"/>
-      <c r="B395" s="212"/>
-      <c r="C395" s="213" t="s">
+      <c r="B395" s="213"/>
+      <c r="C395" s="214" t="s">
         <v>160</v>
       </c>
       <c r="D395" s="135"/>
@@ -12102,7 +12114,7 @@
     <row r="396" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A396" s="1"/>
       <c r="B396" s="109"/>
-      <c r="C396" s="213"/>
+      <c r="C396" s="214"/>
       <c r="D396" s="165"/>
       <c r="E396" s="155"/>
       <c r="F396" s="148"/>
@@ -12123,7 +12135,7 @@
     </row>
     <row r="398" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A398" s="136"/>
-      <c r="B398" s="212" t="s">
+      <c r="B398" s="213" t="s">
         <v>143</v>
       </c>
       <c r="C398" s="134"/>
@@ -12136,8 +12148,8 @@
     </row>
     <row r="399" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A399" s="136"/>
-      <c r="B399" s="212"/>
-      <c r="C399" s="213" t="s">
+      <c r="B399" s="213"/>
+      <c r="C399" s="214" t="s">
         <v>148</v>
       </c>
       <c r="D399" s="135"/>
@@ -12150,7 +12162,7 @@
     <row r="400" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A400" s="1"/>
       <c r="B400" s="109"/>
-      <c r="C400" s="213"/>
+      <c r="C400" s="214"/>
       <c r="D400" s="165"/>
       <c r="E400" s="155"/>
       <c r="F400" s="148"/>
@@ -12172,7 +12184,7 @@
     <row r="402" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A402" s="1"/>
       <c r="B402" s="109"/>
-      <c r="C402" s="213" t="s">
+      <c r="C402" s="214" t="s">
         <v>149</v>
       </c>
       <c r="D402" s="135"/>
@@ -12185,7 +12197,7 @@
     <row r="403" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A403" s="1"/>
       <c r="B403" s="109"/>
-      <c r="C403" s="213"/>
+      <c r="C403" s="214"/>
       <c r="D403" s="165"/>
       <c r="E403" s="155"/>
       <c r="F403" s="148"/>
@@ -12230,7 +12242,7 @@
     <row r="406" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A406" s="1"/>
       <c r="B406" s="109"/>
-      <c r="C406" s="213" t="s">
+      <c r="C406" s="214" t="s">
         <v>150</v>
       </c>
       <c r="D406" s="135"/>
@@ -12243,7 +12255,7 @@
     <row r="407" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A407" s="1"/>
       <c r="B407" s="109"/>
-      <c r="C407" s="213"/>
+      <c r="C407" s="214"/>
       <c r="D407" s="165"/>
       <c r="E407" s="155"/>
       <c r="F407" s="148"/>
@@ -12265,7 +12277,7 @@
     <row r="409" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A409" s="1"/>
       <c r="B409" s="109"/>
-      <c r="C409" s="213" t="s">
+      <c r="C409" s="214" t="s">
         <v>151</v>
       </c>
       <c r="D409" s="135"/>
@@ -12278,7 +12290,7 @@
     <row r="410" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A410" s="1"/>
       <c r="B410" s="109"/>
-      <c r="C410" s="213"/>
+      <c r="C410" s="214"/>
       <c r="D410" s="165"/>
       <c r="E410" s="155"/>
       <c r="F410" s="148"/>
@@ -12300,7 +12312,7 @@
     <row r="412" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A412" s="1"/>
       <c r="B412" s="109"/>
-      <c r="C412" s="213" t="s">
+      <c r="C412" s="214" t="s">
         <v>152</v>
       </c>
       <c r="D412" s="135"/>
@@ -12313,7 +12325,7 @@
     <row r="413" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A413" s="1"/>
       <c r="B413" s="109"/>
-      <c r="C413" s="213"/>
+      <c r="C413" s="214"/>
       <c r="D413" s="166" t="s">
         <v>760</v>
       </c>
@@ -12656,7 +12668,7 @@
     <row r="434" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A434" s="1"/>
       <c r="B434" s="109"/>
-      <c r="C434" s="213" t="s">
+      <c r="C434" s="214" t="s">
         <v>153</v>
       </c>
       <c r="D434" s="135"/>
@@ -12669,7 +12681,7 @@
     <row r="435" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A435" s="1"/>
       <c r="B435" s="109"/>
-      <c r="C435" s="213"/>
+      <c r="C435" s="214"/>
       <c r="D435" s="165"/>
       <c r="E435" s="155"/>
       <c r="F435" s="148"/>
@@ -12691,7 +12703,7 @@
     <row r="437" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A437" s="1"/>
       <c r="B437" s="109"/>
-      <c r="C437" s="213" t="s">
+      <c r="C437" s="214" t="s">
         <v>154</v>
       </c>
       <c r="D437" s="135"/>
@@ -12704,7 +12716,7 @@
     <row r="438" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A438" s="1"/>
       <c r="B438" s="109"/>
-      <c r="C438" s="213"/>
+      <c r="C438" s="214"/>
       <c r="D438" s="165"/>
       <c r="E438" s="155"/>
       <c r="F438" s="148"/>
@@ -12726,7 +12738,7 @@
     <row r="440" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A440" s="1"/>
       <c r="B440" s="109"/>
-      <c r="C440" s="213" t="s">
+      <c r="C440" s="214" t="s">
         <v>155</v>
       </c>
       <c r="D440" s="135"/>
@@ -12739,7 +12751,7 @@
     <row r="441" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A441" s="1"/>
       <c r="B441" s="109"/>
-      <c r="C441" s="213"/>
+      <c r="C441" s="214"/>
       <c r="D441" s="165"/>
       <c r="E441" s="155"/>
       <c r="F441" s="148"/>
@@ -12761,7 +12773,7 @@
     <row r="443" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A443" s="1"/>
       <c r="B443" s="109"/>
-      <c r="C443" s="213" t="s">
+      <c r="C443" s="214" t="s">
         <v>156</v>
       </c>
       <c r="D443" s="135"/>
@@ -12774,7 +12786,7 @@
     <row r="444" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A444" s="1"/>
       <c r="B444" s="109"/>
-      <c r="C444" s="213"/>
+      <c r="C444" s="214"/>
       <c r="D444" s="165"/>
       <c r="E444" s="155"/>
       <c r="F444" s="148"/>
@@ -12796,7 +12808,7 @@
     <row r="446" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A446" s="1"/>
       <c r="B446" s="109"/>
-      <c r="C446" s="213" t="s">
+      <c r="C446" s="214" t="s">
         <v>157</v>
       </c>
       <c r="D446" s="135"/>
@@ -12809,7 +12821,7 @@
     <row r="447" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A447" s="1"/>
       <c r="B447" s="109"/>
-      <c r="C447" s="213"/>
+      <c r="C447" s="214"/>
       <c r="D447" s="165"/>
       <c r="E447" s="155"/>
       <c r="F447" s="148"/>
@@ -12854,7 +12866,7 @@
     <row r="450" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A450" s="1"/>
       <c r="B450" s="109"/>
-      <c r="C450" s="213" t="s">
+      <c r="C450" s="214" t="s">
         <v>158</v>
       </c>
       <c r="D450" s="135"/>
@@ -12867,7 +12879,7 @@
     <row r="451" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A451" s="1"/>
       <c r="B451" s="109"/>
-      <c r="C451" s="213"/>
+      <c r="C451" s="214"/>
       <c r="D451" s="166" t="s">
         <v>466</v>
       </c>
@@ -13007,19 +13019,19 @@
       <c r="B457" s="109"/>
       <c r="C457" s="110"/>
       <c r="D457" s="167" t="s">
-        <v>478</v>
+        <v>490</v>
       </c>
       <c r="E457" s="160" t="s">
-        <v>479</v>
+        <v>491</v>
       </c>
       <c r="F457" s="151" t="s">
-        <v>256</v>
+        <v>492</v>
       </c>
       <c r="G457" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H457" s="204">
-        <v>44824</v>
+        <v>44621</v>
       </c>
       <c r="I457" s="199" t="s">
         <v>759</v>
@@ -13030,19 +13042,19 @@
       <c r="B458" s="109"/>
       <c r="C458" s="110"/>
       <c r="D458" s="167" t="s">
-        <v>481</v>
+        <v>494</v>
       </c>
       <c r="E458" s="160" t="s">
-        <v>480</v>
+        <v>493</v>
       </c>
       <c r="F458" s="151" t="s">
-        <v>256</v>
+        <v>492</v>
       </c>
       <c r="G458" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H458" s="204">
-        <v>44824</v>
+        <v>44621</v>
       </c>
       <c r="I458" s="199" t="s">
         <v>759</v>
@@ -13053,19 +13065,19 @@
       <c r="B459" s="109"/>
       <c r="C459" s="110"/>
       <c r="D459" s="167" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E459" s="160" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F459" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G459" s="190">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H459" s="204">
-        <v>44622</v>
+        <v>44824</v>
       </c>
       <c r="I459" s="199" t="s">
         <v>759</v>
@@ -13076,19 +13088,19 @@
       <c r="B460" s="109"/>
       <c r="C460" s="110"/>
       <c r="D460" s="167" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="E460" s="160" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="F460" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G460" s="190">
-        <v>44733</v>
+        <v>44669</v>
       </c>
       <c r="H460" s="204">
-        <v>44621</v>
+        <v>44824</v>
       </c>
       <c r="I460" s="199" t="s">
         <v>759</v>
@@ -13099,19 +13111,19 @@
       <c r="B461" s="109"/>
       <c r="C461" s="110"/>
       <c r="D461" s="167" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E461" s="160" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="F461" s="151" t="s">
         <v>459</v>
       </c>
       <c r="G461" s="190">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H461" s="204">
-        <v>44732</v>
+        <v>44622</v>
       </c>
       <c r="I461" s="199" t="s">
         <v>759</v>
@@ -13122,19 +13134,19 @@
       <c r="B462" s="109"/>
       <c r="C462" s="110"/>
       <c r="D462" s="167" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="E462" s="160" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F462" s="151" t="s">
         <v>459</v>
       </c>
       <c r="G462" s="190">
-        <v>44671</v>
+        <v>44733</v>
       </c>
       <c r="H462" s="204">
-        <v>44732</v>
+        <v>44621</v>
       </c>
       <c r="I462" s="199" t="s">
         <v>759</v>
@@ -13145,19 +13157,19 @@
       <c r="B463" s="109"/>
       <c r="C463" s="110"/>
       <c r="D463" s="167" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E463" s="160" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F463" s="151" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="G463" s="190">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H463" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I463" s="199" t="s">
         <v>759</v>
@@ -13168,19 +13180,19 @@
       <c r="B464" s="109"/>
       <c r="C464" s="110"/>
       <c r="D464" s="167" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="E464" s="160" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F464" s="151" t="s">
-        <v>492</v>
+        <v>459</v>
       </c>
       <c r="G464" s="190">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H464" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I464" s="199" t="s">
         <v>759</v>
@@ -13191,19 +13203,19 @@
       <c r="B465" s="109"/>
       <c r="C465" s="110"/>
       <c r="D465" s="167" t="s">
-        <v>495</v>
+        <v>968</v>
       </c>
       <c r="E465" s="160" t="s">
-        <v>497</v>
+        <v>970</v>
       </c>
       <c r="F465" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G465" s="190">
-        <v>44644</v>
+        <v>45048</v>
       </c>
       <c r="H465" s="204">
-        <v>44622</v>
+        <v>45048</v>
       </c>
       <c r="I465" s="199" t="s">
         <v>759</v>
@@ -13214,19 +13226,19 @@
       <c r="B466" s="109"/>
       <c r="C466" s="110"/>
       <c r="D466" s="167" t="s">
-        <v>496</v>
+        <v>969</v>
       </c>
       <c r="E466" s="160" t="s">
-        <v>498</v>
+        <v>971</v>
       </c>
       <c r="F466" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G466" s="190">
-        <v>44644</v>
+        <v>45048</v>
       </c>
       <c r="H466" s="204">
-        <v>44621</v>
+        <v>45048</v>
       </c>
       <c r="I466" s="199" t="s">
         <v>759</v>
@@ -13237,19 +13249,19 @@
       <c r="B467" s="109"/>
       <c r="C467" s="110"/>
       <c r="D467" s="167" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="E467" s="160" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="F467" s="151" t="s">
-        <v>459</v>
+        <v>267</v>
       </c>
       <c r="G467" s="190">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H467" s="204">
-        <v>44621</v>
+        <v>44622</v>
       </c>
       <c r="I467" s="199" t="s">
         <v>759</v>
@@ -13260,16 +13272,16 @@
       <c r="B468" s="109"/>
       <c r="C468" s="110"/>
       <c r="D468" s="167" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="E468" s="160" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="F468" s="151" t="s">
-        <v>459</v>
+        <v>267</v>
       </c>
       <c r="G468" s="190">
-        <v>44698</v>
+        <v>44644</v>
       </c>
       <c r="H468" s="204">
         <v>44621</v>
@@ -13283,19 +13295,19 @@
       <c r="B469" s="109"/>
       <c r="C469" s="110"/>
       <c r="D469" s="167" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E469" s="160" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="F469" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G469" s="190">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H469" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I469" s="199" t="s">
         <v>759</v>
@@ -13306,19 +13318,19 @@
       <c r="B470" s="109"/>
       <c r="C470" s="110"/>
       <c r="D470" s="167" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="E470" s="160" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F470" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G470" s="190">
-        <v>44846</v>
+        <v>44698</v>
       </c>
       <c r="H470" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I470" s="199" t="s">
         <v>759</v>
@@ -13329,19 +13341,19 @@
       <c r="B471" s="109"/>
       <c r="C471" s="110"/>
       <c r="D471" s="167" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="E471" s="160" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="F471" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G471" s="190">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H471" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I471" s="199" t="s">
         <v>759</v>
@@ -13352,19 +13364,19 @@
       <c r="B472" s="109"/>
       <c r="C472" s="110"/>
       <c r="D472" s="167" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E472" s="160" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F472" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G472" s="190">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H472" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I472" s="199" t="s">
         <v>759</v>
@@ -13375,16 +13387,16 @@
       <c r="B473" s="109"/>
       <c r="C473" s="110"/>
       <c r="D473" s="167" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E473" s="160" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="F473" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G473" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H473" s="204">
         <v>44628</v>
@@ -13398,16 +13410,16 @@
       <c r="B474" s="109"/>
       <c r="C474" s="110"/>
       <c r="D474" s="167" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E474" s="160" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F474" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G474" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H474" s="204">
         <v>44628</v>
@@ -13421,16 +13433,16 @@
       <c r="B475" s="109"/>
       <c r="C475" s="110"/>
       <c r="D475" s="167" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E475" s="160" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="F475" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G475" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H475" s="204">
         <v>44628</v>
@@ -13444,16 +13456,16 @@
       <c r="B476" s="109"/>
       <c r="C476" s="110"/>
       <c r="D476" s="167" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="E476" s="160" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F476" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G476" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H476" s="204">
         <v>44628</v>
@@ -13467,16 +13479,16 @@
       <c r="B477" s="109"/>
       <c r="C477" s="110"/>
       <c r="D477" s="167" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E477" s="160" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="F477" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G477" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H477" s="204">
         <v>44628</v>
@@ -13490,16 +13502,16 @@
       <c r="B478" s="109"/>
       <c r="C478" s="110"/>
       <c r="D478" s="167" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="E478" s="160" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="F478" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G478" s="190">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H478" s="204">
         <v>44628</v>
@@ -13513,19 +13525,19 @@
       <c r="B479" s="109"/>
       <c r="C479" s="110"/>
       <c r="D479" s="167" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E479" s="160" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F479" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G479" s="190">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H479" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I479" s="199" t="s">
         <v>759</v>
@@ -13536,19 +13548,19 @@
       <c r="B480" s="109"/>
       <c r="C480" s="110"/>
       <c r="D480" s="167" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="E480" s="160" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F480" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G480" s="190">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H480" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I480" s="199" t="s">
         <v>759</v>
@@ -13559,19 +13571,19 @@
       <c r="B481" s="109"/>
       <c r="C481" s="110"/>
       <c r="D481" s="167" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="E481" s="160" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="F481" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G481" s="190">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H481" s="204">
-        <v>44662</v>
+        <v>44617</v>
       </c>
       <c r="I481" s="199" t="s">
         <v>759</v>
@@ -13582,19 +13594,19 @@
       <c r="B482" s="109"/>
       <c r="C482" s="110"/>
       <c r="D482" s="167" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="E482" s="160" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="F482" s="151" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G482" s="190">
-        <v>44740</v>
+        <v>44617</v>
       </c>
       <c r="H482" s="204">
-        <v>44662</v>
+        <v>44617</v>
       </c>
       <c r="I482" s="199" t="s">
         <v>759</v>
@@ -13604,185 +13616,189 @@
       <c r="A483" s="1"/>
       <c r="B483" s="109"/>
       <c r="C483" s="110"/>
-      <c r="D483" s="165"/>
-      <c r="E483" s="155"/>
-      <c r="F483" s="148"/>
-      <c r="G483" s="186"/>
-      <c r="H483" s="201"/>
-      <c r="I483" s="174"/>
+      <c r="D483" s="167" t="s">
+        <v>527</v>
+      </c>
+      <c r="E483" s="160" t="s">
+        <v>528</v>
+      </c>
+      <c r="F483" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G483" s="190">
+        <v>44740</v>
+      </c>
+      <c r="H483" s="204">
+        <v>44662</v>
+      </c>
+      <c r="I483" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="484" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A484" s="1"/>
       <c r="B484" s="109"/>
-      <c r="C484" s="213" t="s">
-        <v>147</v>
-      </c>
-      <c r="D484" s="135"/>
-      <c r="E484" s="154"/>
-      <c r="F484" s="147"/>
-      <c r="G484" s="185"/>
-      <c r="H484" s="200"/>
-      <c r="I484" s="173"/>
+      <c r="C484" s="110"/>
+      <c r="D484" s="167" t="s">
+        <v>530</v>
+      </c>
+      <c r="E484" s="160" t="s">
+        <v>529</v>
+      </c>
+      <c r="F484" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G484" s="190">
+        <v>44740</v>
+      </c>
+      <c r="H484" s="204">
+        <v>44662</v>
+      </c>
+      <c r="I484" s="199" t="s">
+        <v>759</v>
+      </c>
     </row>
     <row r="485" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A485" s="1"/>
       <c r="B485" s="109"/>
-      <c r="C485" s="213"/>
-      <c r="D485" s="166" t="s">
-        <v>274</v>
-      </c>
-      <c r="E485" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="F485" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G485" s="188">
-        <v>44167</v>
-      </c>
-      <c r="H485" s="203">
-        <v>44167</v>
-      </c>
-      <c r="I485" s="176"/>
+      <c r="C485" s="110"/>
+      <c r="D485" s="165"/>
+      <c r="E485" s="155"/>
+      <c r="F485" s="148"/>
+      <c r="G485" s="186"/>
+      <c r="H485" s="201"/>
+      <c r="I485" s="174"/>
     </row>
     <row r="486" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A486" s="1"/>
       <c r="B486" s="109"/>
-      <c r="C486" s="110"/>
-      <c r="D486" s="167" t="s">
-        <v>445</v>
-      </c>
-      <c r="E486" s="160" t="s">
-        <v>446</v>
-      </c>
-      <c r="F486" s="151" t="s">
-        <v>256</v>
-      </c>
-      <c r="G486" s="190">
-        <v>44575</v>
-      </c>
-      <c r="H486" s="204">
-        <v>44167</v>
-      </c>
-      <c r="I486" s="177"/>
-    </row>
-    <row r="487" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C486" s="214" t="s">
+        <v>147</v>
+      </c>
+      <c r="D486" s="135"/>
+      <c r="E486" s="154"/>
+      <c r="F486" s="147"/>
+      <c r="G486" s="185"/>
+      <c r="H486" s="200"/>
+      <c r="I486" s="173"/>
+    </row>
+    <row r="487" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A487" s="1"/>
       <c r="B487" s="109"/>
-      <c r="C487" s="110"/>
-      <c r="D487" s="167" t="s">
-        <v>448</v>
-      </c>
-      <c r="E487" s="158" t="s">
-        <v>447</v>
-      </c>
-      <c r="F487" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G487" s="190">
-        <v>44404</v>
-      </c>
-      <c r="H487" s="204">
-        <v>44404</v>
-      </c>
-      <c r="I487" s="177"/>
+      <c r="C487" s="214"/>
+      <c r="D487" s="166" t="s">
+        <v>274</v>
+      </c>
+      <c r="E487" s="162" t="s">
+        <v>444</v>
+      </c>
+      <c r="F487" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G487" s="188">
+        <v>44167</v>
+      </c>
+      <c r="H487" s="203">
+        <v>44167</v>
+      </c>
+      <c r="I487" s="176"/>
     </row>
     <row r="488" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A488" s="1"/>
       <c r="B488" s="109"/>
       <c r="C488" s="110"/>
-      <c r="D488" s="165"/>
-      <c r="E488" s="155"/>
-      <c r="F488" s="148"/>
-      <c r="G488" s="186"/>
-      <c r="H488" s="201"/>
-      <c r="I488" s="174"/>
-    </row>
-    <row r="489" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D488" s="167" t="s">
+        <v>445</v>
+      </c>
+      <c r="E488" s="160" t="s">
+        <v>446</v>
+      </c>
+      <c r="F488" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G488" s="190">
+        <v>44575</v>
+      </c>
+      <c r="H488" s="204">
+        <v>44167</v>
+      </c>
+      <c r="I488" s="177"/>
+    </row>
+    <row r="489" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A489" s="1"/>
       <c r="B489" s="109"/>
-      <c r="C489" s="213" t="s">
-        <v>159</v>
-      </c>
-      <c r="D489" s="135"/>
-      <c r="E489" s="154"/>
-      <c r="F489" s="147"/>
-      <c r="G489" s="185"/>
-      <c r="H489" s="200"/>
-      <c r="I489" s="173"/>
+      <c r="C489" s="110"/>
+      <c r="D489" s="167" t="s">
+        <v>448</v>
+      </c>
+      <c r="E489" s="158" t="s">
+        <v>447</v>
+      </c>
+      <c r="F489" s="151" t="s">
+        <v>281</v>
+      </c>
+      <c r="G489" s="190">
+        <v>44404</v>
+      </c>
+      <c r="H489" s="204">
+        <v>44404</v>
+      </c>
+      <c r="I489" s="177"/>
     </row>
     <row r="490" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A490" s="1"/>
       <c r="B490" s="109"/>
-      <c r="C490" s="213"/>
-      <c r="D490" s="166" t="s">
-        <v>450</v>
-      </c>
-      <c r="E490" s="162" t="s">
-        <v>449</v>
-      </c>
-      <c r="F490" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G490" s="188">
-        <v>44635</v>
-      </c>
-      <c r="H490" s="203">
-        <v>44635</v>
-      </c>
-      <c r="I490" s="176"/>
+      <c r="C490" s="110"/>
+      <c r="D490" s="165"/>
+      <c r="E490" s="155"/>
+      <c r="F490" s="148"/>
+      <c r="G490" s="186"/>
+      <c r="H490" s="201"/>
+      <c r="I490" s="174"/>
     </row>
     <row r="491" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A491" s="1"/>
       <c r="B491" s="109"/>
-      <c r="C491" s="110"/>
-      <c r="D491" s="167" t="s">
-        <v>452</v>
-      </c>
-      <c r="E491" s="160" t="s">
-        <v>451</v>
-      </c>
-      <c r="F491" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G491" s="190">
-        <v>44635</v>
-      </c>
-      <c r="H491" s="204">
-        <v>44635</v>
-      </c>
-      <c r="I491" s="177"/>
+      <c r="C491" s="214" t="s">
+        <v>159</v>
+      </c>
+      <c r="D491" s="135"/>
+      <c r="E491" s="154"/>
+      <c r="F491" s="147"/>
+      <c r="G491" s="185"/>
+      <c r="H491" s="200"/>
+      <c r="I491" s="173"/>
     </row>
     <row r="492" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A492" s="1"/>
       <c r="B492" s="109"/>
-      <c r="C492" s="110"/>
-      <c r="D492" s="167" t="s">
-        <v>453</v>
-      </c>
-      <c r="E492" s="160" t="s">
-        <v>455</v>
-      </c>
-      <c r="F492" s="151" t="s">
+      <c r="C492" s="214"/>
+      <c r="D492" s="166" t="s">
+        <v>450</v>
+      </c>
+      <c r="E492" s="162" t="s">
+        <v>449</v>
+      </c>
+      <c r="F492" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="G492" s="190">
+      <c r="G492" s="188">
         <v>44635</v>
       </c>
-      <c r="H492" s="204">
+      <c r="H492" s="203">
         <v>44635</v>
       </c>
-      <c r="I492" s="177"/>
+      <c r="I492" s="176"/>
     </row>
     <row r="493" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A493" s="1"/>
       <c r="B493" s="109"/>
       <c r="C493" s="110"/>
       <c r="D493" s="167" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="E493" s="160" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="F493" s="151" t="s">
         <v>232</v>
@@ -13800,19 +13816,19 @@
       <c r="B494" s="109"/>
       <c r="C494" s="110"/>
       <c r="D494" s="167" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="E494" s="160" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="F494" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G494" s="190">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H494" s="204">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="I494" s="177"/>
     </row>
@@ -13821,19 +13837,19 @@
       <c r="B495" s="109"/>
       <c r="C495" s="110"/>
       <c r="D495" s="167" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E495" s="160" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="F495" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G495" s="190">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H495" s="204">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="I495" s="177"/>
     </row>
@@ -13842,19 +13858,19 @@
       <c r="B496" s="109"/>
       <c r="C496" s="110"/>
       <c r="D496" s="167" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="E496" s="160" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="F496" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G496" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H496" s="204">
         <v>44644</v>
-      </c>
-      <c r="H496" s="204">
-        <v>44636</v>
       </c>
       <c r="I496" s="177"/>
     </row>
@@ -13863,19 +13879,19 @@
       <c r="B497" s="109"/>
       <c r="C497" s="110"/>
       <c r="D497" s="167" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="E497" s="160" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F497" s="151" t="s">
-        <v>267</v>
+        <v>459</v>
       </c>
       <c r="G497" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H497" s="204">
         <v>44644</v>
-      </c>
-      <c r="H497" s="204">
-        <v>44636</v>
       </c>
       <c r="I497" s="177"/>
     </row>
@@ -13883,133 +13899,129 @@
       <c r="A498" s="1"/>
       <c r="B498" s="109"/>
       <c r="C498" s="110"/>
-      <c r="D498" s="165"/>
-      <c r="E498" s="155"/>
-      <c r="F498" s="148"/>
-      <c r="G498" s="186"/>
-      <c r="H498" s="201"/>
-      <c r="I498" s="174"/>
-    </row>
-    <row r="499" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A499" s="136"/>
-      <c r="B499" s="212" t="s">
+      <c r="D498" s="167" t="s">
+        <v>462</v>
+      </c>
+      <c r="E498" s="160" t="s">
+        <v>463</v>
+      </c>
+      <c r="F498" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G498" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H498" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I498" s="177"/>
+    </row>
+    <row r="499" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A499" s="1"/>
+      <c r="B499" s="109"/>
+      <c r="C499" s="110"/>
+      <c r="D499" s="167" t="s">
+        <v>464</v>
+      </c>
+      <c r="E499" s="160" t="s">
+        <v>465</v>
+      </c>
+      <c r="F499" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G499" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H499" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I499" s="177"/>
+    </row>
+    <row r="500" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A500" s="1"/>
+      <c r="B500" s="109"/>
+      <c r="C500" s="110"/>
+      <c r="D500" s="165"/>
+      <c r="E500" s="155"/>
+      <c r="F500" s="148"/>
+      <c r="G500" s="186"/>
+      <c r="H500" s="201"/>
+      <c r="I500" s="174"/>
+    </row>
+    <row r="501" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A501" s="136"/>
+      <c r="B501" s="213" t="s">
         <v>144</v>
       </c>
-      <c r="C499" s="134"/>
-      <c r="D499" s="135"/>
-      <c r="E499" s="154"/>
-      <c r="F499" s="147"/>
-      <c r="G499" s="185"/>
-      <c r="H499" s="200"/>
-      <c r="I499" s="173"/>
-    </row>
-    <row r="500" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A500" s="136"/>
-      <c r="B500" s="212"/>
-      <c r="C500" s="213" t="s">
+      <c r="C501" s="134"/>
+      <c r="D501" s="135"/>
+      <c r="E501" s="154"/>
+      <c r="F501" s="147"/>
+      <c r="G501" s="185"/>
+      <c r="H501" s="200"/>
+      <c r="I501" s="173"/>
+    </row>
+    <row r="502" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A502" s="136"/>
+      <c r="B502" s="213"/>
+      <c r="C502" s="214" t="s">
         <v>146</v>
       </c>
-      <c r="D500" s="135"/>
-      <c r="E500" s="154"/>
-      <c r="F500" s="147"/>
-      <c r="G500" s="185"/>
-      <c r="H500" s="200"/>
-      <c r="I500" s="173"/>
-    </row>
-    <row r="501" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A501" s="1"/>
-      <c r="B501" s="109"/>
-      <c r="C501" s="213"/>
-      <c r="D501" s="165"/>
-      <c r="E501" s="155"/>
-      <c r="F501" s="148"/>
-      <c r="G501" s="186"/>
-      <c r="H501" s="201"/>
-      <c r="I501" s="174"/>
-    </row>
-    <row r="502" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A502" s="1"/>
-      <c r="B502" s="109"/>
-      <c r="C502" s="110"/>
-      <c r="D502" s="165"/>
-      <c r="E502" s="155"/>
-      <c r="F502" s="148"/>
-      <c r="G502" s="186"/>
-      <c r="H502" s="201"/>
-      <c r="I502" s="174"/>
-    </row>
-    <row r="503" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D502" s="135"/>
+      <c r="E502" s="154"/>
+      <c r="F502" s="147"/>
+      <c r="G502" s="185"/>
+      <c r="H502" s="200"/>
+      <c r="I502" s="173"/>
+    </row>
+    <row r="503" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A503" s="1"/>
       <c r="B503" s="109"/>
-      <c r="C503" s="110"/>
-      <c r="D503" s="144"/>
-      <c r="E503" s="156"/>
-      <c r="F503" s="149"/>
-      <c r="G503" s="187"/>
-      <c r="H503" s="202"/>
-      <c r="I503" s="175"/>
-    </row>
-    <row r="504" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A504" s="136"/>
+      <c r="C503" s="214"/>
+      <c r="D503" s="165"/>
+      <c r="E503" s="155"/>
+      <c r="F503" s="148"/>
+      <c r="G503" s="186"/>
+      <c r="H503" s="201"/>
+      <c r="I503" s="174"/>
+    </row>
+    <row r="504" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A504" s="1"/>
       <c r="B504" s="109"/>
       <c r="C504" s="110"/>
-      <c r="D504" s="166" t="s">
-        <v>858</v>
-      </c>
-      <c r="E504" s="162" t="s">
-        <v>860</v>
-      </c>
-      <c r="F504" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G504" s="188">
-        <v>44950</v>
-      </c>
-      <c r="H504" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I504" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="505" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A505" s="136"/>
+      <c r="D504" s="165"/>
+      <c r="E504" s="155"/>
+      <c r="F504" s="148"/>
+      <c r="G504" s="186"/>
+      <c r="H504" s="201"/>
+      <c r="I504" s="174"/>
+    </row>
+    <row r="505" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A505" s="1"/>
       <c r="B505" s="109"/>
       <c r="C505" s="110"/>
-      <c r="D505" s="167" t="s">
-        <v>859</v>
-      </c>
-      <c r="E505" s="158" t="s">
-        <v>861</v>
-      </c>
-      <c r="F505" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G505" s="190">
-        <v>44950</v>
-      </c>
-      <c r="H505" s="204">
-        <v>44893</v>
-      </c>
-      <c r="I505" s="171" t="s">
-        <v>727</v>
-      </c>
+      <c r="D505" s="144"/>
+      <c r="E505" s="156"/>
+      <c r="F505" s="149"/>
+      <c r="G505" s="187"/>
+      <c r="H505" s="202"/>
+      <c r="I505" s="175"/>
     </row>
     <row r="506" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A506" s="136"/>
       <c r="B506" s="109"/>
       <c r="C506" s="110"/>
       <c r="D506" s="166" t="s">
-        <v>862</v>
-      </c>
-      <c r="E506" s="157" t="s">
-        <v>864</v>
+        <v>858</v>
+      </c>
+      <c r="E506" s="162" t="s">
+        <v>860</v>
       </c>
       <c r="F506" s="150" t="s">
-        <v>548</v>
+        <v>267</v>
       </c>
       <c r="G506" s="188">
-        <v>44970</v>
+        <v>44950</v>
       </c>
       <c r="H506" s="203">
         <v>44893</v>
@@ -14022,171 +14034,195 @@
       <c r="A507" s="136"/>
       <c r="B507" s="109"/>
       <c r="C507" s="110"/>
-      <c r="D507" s="166" t="s">
-        <v>863</v>
-      </c>
-      <c r="E507" s="157" t="s">
-        <v>865</v>
-      </c>
-      <c r="F507" s="150" t="s">
-        <v>548</v>
-      </c>
-      <c r="G507" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H507" s="203">
+      <c r="D507" s="167" t="s">
+        <v>859</v>
+      </c>
+      <c r="E507" s="158" t="s">
+        <v>861</v>
+      </c>
+      <c r="F507" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G507" s="190">
+        <v>44950</v>
+      </c>
+      <c r="H507" s="204">
         <v>44893</v>
       </c>
       <c r="I507" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="508" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="508" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A508" s="136"/>
       <c r="B508" s="109"/>
       <c r="C508" s="110"/>
-      <c r="D508" s="166"/>
-      <c r="E508" s="157"/>
-      <c r="F508" s="150"/>
-      <c r="G508" s="188"/>
-      <c r="H508" s="203"/>
-      <c r="I508" s="171"/>
+      <c r="D508" s="166" t="s">
+        <v>862</v>
+      </c>
+      <c r="E508" s="157" t="s">
+        <v>864</v>
+      </c>
+      <c r="F508" s="150" t="s">
+        <v>548</v>
+      </c>
+      <c r="G508" s="188">
+        <v>44970</v>
+      </c>
+      <c r="H508" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I508" s="171" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="509" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A509" s="136"/>
       <c r="B509" s="109"/>
       <c r="C509" s="110"/>
       <c r="D509" s="166" t="s">
-        <v>934</v>
+        <v>863</v>
       </c>
       <c r="E509" s="157" t="s">
-        <v>936</v>
+        <v>865</v>
       </c>
       <c r="F509" s="150" t="s">
-        <v>232</v>
+        <v>548</v>
       </c>
       <c r="G509" s="188">
-        <v>45009</v>
+        <v>44970</v>
       </c>
       <c r="H509" s="203">
-        <v>45009</v>
+        <v>44893</v>
       </c>
       <c r="I509" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="510" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="510" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A510" s="136"/>
       <c r="B510" s="109"/>
       <c r="C510" s="110"/>
-      <c r="D510" s="166" t="s">
-        <v>933</v>
-      </c>
-      <c r="E510" s="157" t="s">
-        <v>935</v>
-      </c>
-      <c r="F510" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G510" s="188">
-        <v>45009</v>
-      </c>
-      <c r="H510" s="203">
-        <v>45009</v>
-      </c>
-      <c r="I510" s="171" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="511" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D510" s="166"/>
+      <c r="E510" s="157"/>
+      <c r="F510" s="150"/>
+      <c r="G510" s="188"/>
+      <c r="H510" s="203"/>
+      <c r="I510" s="171"/>
+    </row>
+    <row r="511" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A511" s="136"/>
       <c r="B511" s="109"/>
       <c r="C511" s="110"/>
-      <c r="D511" s="166"/>
-      <c r="E511" s="157"/>
-      <c r="F511" s="150"/>
-      <c r="G511" s="188"/>
-      <c r="H511" s="203"/>
-      <c r="I511" s="171"/>
+      <c r="D511" s="166" t="s">
+        <v>934</v>
+      </c>
+      <c r="E511" s="157" t="s">
+        <v>936</v>
+      </c>
+      <c r="F511" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G511" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H511" s="203">
+        <v>45009</v>
+      </c>
+      <c r="I511" s="171" t="s">
+        <v>727</v>
+      </c>
     </row>
     <row r="512" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A512" s="136"/>
       <c r="B512" s="109"/>
       <c r="C512" s="110"/>
       <c r="D512" s="166" t="s">
-        <v>854</v>
-      </c>
-      <c r="E512" s="162" t="s">
-        <v>857</v>
+        <v>933</v>
+      </c>
+      <c r="E512" s="157" t="s">
+        <v>935</v>
       </c>
       <c r="F512" s="150" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G512" s="188">
-        <v>44986</v>
+        <v>45009</v>
       </c>
       <c r="H512" s="203">
-        <v>44951</v>
+        <v>45009</v>
       </c>
       <c r="I512" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="513" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="513" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A513" s="136"/>
       <c r="B513" s="109"/>
       <c r="C513" s="110"/>
-      <c r="D513" s="167" t="s">
+      <c r="D513" s="166"/>
+      <c r="E513" s="157"/>
+      <c r="F513" s="150"/>
+      <c r="G513" s="188"/>
+      <c r="H513" s="203"/>
+      <c r="I513" s="171"/>
+    </row>
+    <row r="514" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A514" s="136"/>
+      <c r="B514" s="109"/>
+      <c r="C514" s="110"/>
+      <c r="D514" s="166" t="s">
+        <v>854</v>
+      </c>
+      <c r="E514" s="162" t="s">
+        <v>857</v>
+      </c>
+      <c r="F514" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G514" s="188">
+        <v>44986</v>
+      </c>
+      <c r="H514" s="203">
+        <v>44951</v>
+      </c>
+      <c r="I514" s="171" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="515" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A515" s="136"/>
+      <c r="B515" s="109"/>
+      <c r="C515" s="110"/>
+      <c r="D515" s="167" t="s">
         <v>855</v>
       </c>
-      <c r="E513" s="158" t="s">
+      <c r="E515" s="158" t="s">
         <v>856</v>
       </c>
-      <c r="F513" s="151" t="s">
+      <c r="F515" s="151" t="s">
         <v>267</v>
       </c>
-      <c r="G513" s="190">
+      <c r="G515" s="190">
         <v>44986</v>
       </c>
-      <c r="H513" s="204">
+      <c r="H515" s="204">
         <v>44951</v>
       </c>
-      <c r="I513" s="171" t="s">
+      <c r="I515" s="171" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="514" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A514" s="136"/>
-      <c r="B514" s="111"/>
-      <c r="C514" s="112"/>
-      <c r="D514" s="170"/>
-      <c r="E514" s="163"/>
-      <c r="F514" s="153"/>
-      <c r="G514" s="191"/>
-      <c r="H514" s="206"/>
-      <c r="I514" s="179"/>
-    </row>
-    <row r="515" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A515" s="1"/>
-      <c r="B515" s="1"/>
-      <c r="C515" s="1"/>
-      <c r="D515" s="1"/>
-      <c r="E515" s="146"/>
-      <c r="F515" s="113"/>
-      <c r="G515" s="192"/>
-      <c r="H515" s="192"/>
-      <c r="I515" s="180"/>
-    </row>
-    <row r="516" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A516" s="1"/>
-      <c r="B516" s="1"/>
-      <c r="C516" s="1"/>
-      <c r="D516" s="1"/>
-      <c r="E516" s="146"/>
-      <c r="F516" s="113"/>
-      <c r="G516" s="192"/>
-      <c r="H516" s="192"/>
-      <c r="I516" s="180"/>
+    <row r="516" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A516" s="136"/>
+      <c r="B516" s="111"/>
+      <c r="C516" s="112"/>
+      <c r="D516" s="170"/>
+      <c r="E516" s="163"/>
+      <c r="F516" s="153"/>
+      <c r="G516" s="191"/>
+      <c r="H516" s="206"/>
+      <c r="I516" s="179"/>
     </row>
     <row r="517" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A517" s="1"/>
@@ -14342,19 +14378,27 @@
       <c r="H530" s="192"/>
       <c r="I530" s="180"/>
     </row>
-    <row r="531" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E531" s="145"/>
-      <c r="F531" s="95"/>
-      <c r="G531" s="193"/>
-      <c r="H531" s="193"/>
-      <c r="I531" s="181"/>
-    </row>
-    <row r="532" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E532" s="145"/>
-      <c r="F532" s="95"/>
-      <c r="G532" s="193"/>
-      <c r="H532" s="193"/>
-      <c r="I532" s="181"/>
+    <row r="531" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A531" s="1"/>
+      <c r="B531" s="1"/>
+      <c r="C531" s="1"/>
+      <c r="D531" s="1"/>
+      <c r="E531" s="146"/>
+      <c r="F531" s="113"/>
+      <c r="G531" s="192"/>
+      <c r="H531" s="192"/>
+      <c r="I531" s="180"/>
+    </row>
+    <row r="532" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A532" s="1"/>
+      <c r="B532" s="1"/>
+      <c r="C532" s="1"/>
+      <c r="D532" s="1"/>
+      <c r="E532" s="146"/>
+      <c r="F532" s="113"/>
+      <c r="G532" s="192"/>
+      <c r="H532" s="192"/>
+      <c r="I532" s="180"/>
     </row>
     <row r="533" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
       <c r="E533" s="145"/>
@@ -14363,15 +14407,51 @@
       <c r="H533" s="193"/>
       <c r="I533" s="181"/>
     </row>
+    <row r="534" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E534" s="145"/>
+      <c r="F534" s="95"/>
+      <c r="G534" s="193"/>
+      <c r="H534" s="193"/>
+      <c r="I534" s="181"/>
+    </row>
+    <row r="535" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E535" s="145"/>
+      <c r="F535" s="95"/>
+      <c r="G535" s="193"/>
+      <c r="H535" s="193"/>
+      <c r="I535" s="181"/>
+    </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="B499:B500"/>
-    <mergeCell ref="C500:C501"/>
+    <mergeCell ref="B398:B399"/>
+    <mergeCell ref="C399:C400"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="B394:B395"/>
+    <mergeCell ref="C395:C396"/>
+    <mergeCell ref="C298:C299"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C135:C136"/>
+    <mergeCell ref="C491:C492"/>
+    <mergeCell ref="C409:C410"/>
+    <mergeCell ref="C412:C413"/>
+    <mergeCell ref="C434:C435"/>
+    <mergeCell ref="C437:C438"/>
+    <mergeCell ref="C440:C441"/>
+    <mergeCell ref="C138:C139"/>
+    <mergeCell ref="C147:C148"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="B501:B502"/>
+    <mergeCell ref="C502:C503"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="C443:C444"/>
     <mergeCell ref="C446:C447"/>
     <mergeCell ref="C450:C451"/>
-    <mergeCell ref="C484:C485"/>
+    <mergeCell ref="C486:C487"/>
     <mergeCell ref="C402:C403"/>
     <mergeCell ref="C406:C407"/>
     <mergeCell ref="B2:D2"/>
@@ -14381,28 +14461,6 @@
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C55:C56"/>
     <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C135:C136"/>
-    <mergeCell ref="C489:C490"/>
-    <mergeCell ref="C409:C410"/>
-    <mergeCell ref="C412:C413"/>
-    <mergeCell ref="C434:C435"/>
-    <mergeCell ref="C437:C438"/>
-    <mergeCell ref="C440:C441"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="C147:C148"/>
-    <mergeCell ref="C188:C189"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B398:B399"/>
-    <mergeCell ref="C399:C400"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="B394:B395"/>
-    <mergeCell ref="C395:C396"/>
-    <mergeCell ref="C298:C299"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -14436,20 +14494,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="247" t="s">
+      <c r="B2" s="231" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="248"/>
-      <c r="D2" s="249"/>
-      <c r="E2" s="244" t="s">
+      <c r="C2" s="232"/>
+      <c r="D2" s="233"/>
+      <c r="E2" s="228" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="246"/>
-      <c r="G2" s="244" t="s">
+      <c r="F2" s="230"/>
+      <c r="G2" s="228" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="245"/>
-      <c r="I2" s="246"/>
+      <c r="H2" s="229"/>
+      <c r="I2" s="230"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -14470,10 +14528,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="250" t="s">
+      <c r="H3" s="234" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="251"/>
+      <c r="I3" s="235"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -14503,19 +14561,19 @@
     </row>
     <row r="5" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B5" s="61"/>
-      <c r="C5" s="235" t="s">
+      <c r="C5" s="236" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="238" t="s">
+      <c r="D5" s="239" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="241" t="s">
+      <c r="F5" s="242" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="232" t="s">
+      <c r="G5" s="245" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="6" t="s">
@@ -14527,23 +14585,23 @@
     </row>
     <row r="6" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="61"/>
-      <c r="C6" s="236"/>
-      <c r="D6" s="239"/>
+      <c r="C6" s="237"/>
+      <c r="D6" s="240"/>
       <c r="E6" s="35"/>
-      <c r="F6" s="242"/>
-      <c r="G6" s="233"/>
-      <c r="H6" s="227" t="s">
+      <c r="F6" s="243"/>
+      <c r="G6" s="246"/>
+      <c r="H6" s="226" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="228"/>
+      <c r="I6" s="227"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61"/>
-      <c r="C7" s="237"/>
-      <c r="D7" s="240"/>
+      <c r="C7" s="238"/>
+      <c r="D7" s="241"/>
       <c r="E7" s="36"/>
-      <c r="F7" s="243"/>
-      <c r="G7" s="234"/>
+      <c r="F7" s="244"/>
+      <c r="G7" s="247"/>
       <c r="H7" s="8" t="s">
         <v>23</v>
       </c>
@@ -14577,19 +14635,19 @@
     </row>
     <row r="9" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B9" s="61"/>
-      <c r="C9" s="235" t="s">
+      <c r="C9" s="236" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="238" t="s">
+      <c r="D9" s="239" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="229" t="s">
+      <c r="E9" s="250" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="241" t="s">
+      <c r="F9" s="242" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="232" t="s">
+      <c r="G9" s="245" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -14602,24 +14660,24 @@
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
-      <c r="C10" s="236"/>
-      <c r="D10" s="239"/>
-      <c r="E10" s="230"/>
-      <c r="F10" s="242"/>
-      <c r="G10" s="233"/>
-      <c r="H10" s="227" t="s">
+      <c r="C10" s="237"/>
+      <c r="D10" s="240"/>
+      <c r="E10" s="251"/>
+      <c r="F10" s="243"/>
+      <c r="G10" s="246"/>
+      <c r="H10" s="226" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="228"/>
+      <c r="I10" s="227"/>
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B11" s="61"/>
-      <c r="C11" s="237"/>
-      <c r="D11" s="240"/>
-      <c r="E11" s="231"/>
-      <c r="F11" s="243"/>
-      <c r="G11" s="234"/>
+      <c r="C11" s="238"/>
+      <c r="D11" s="241"/>
+      <c r="E11" s="252"/>
+      <c r="F11" s="244"/>
+      <c r="G11" s="247"/>
       <c r="H11" s="8" t="s">
         <v>23</v>
       </c>
@@ -14657,10 +14715,10 @@
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
-      <c r="C14" s="235" t="s">
+      <c r="C14" s="236" t="s">
         <v>794</v>
       </c>
-      <c r="D14" s="238" t="s">
+      <c r="D14" s="239" t="s">
         <v>797</v>
       </c>
       <c r="E14" s="37" t="s">
@@ -14675,8 +14733,8 @@
     </row>
     <row r="15" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="61"/>
-      <c r="C15" s="236"/>
-      <c r="D15" s="239"/>
+      <c r="C15" s="237"/>
+      <c r="D15" s="240"/>
       <c r="E15" s="37" t="s">
         <v>801</v>
       </c>
@@ -14689,8 +14747,8 @@
     </row>
     <row r="16" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="61"/>
-      <c r="C16" s="237"/>
-      <c r="D16" s="240"/>
+      <c r="C16" s="238"/>
+      <c r="D16" s="241"/>
       <c r="E16" s="37" t="s">
         <v>802</v>
       </c>
@@ -14717,10 +14775,10 @@
     </row>
     <row r="18" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B18" s="61"/>
-      <c r="C18" s="235" t="s">
+      <c r="C18" s="236" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="238" t="s">
+      <c r="D18" s="239" t="s">
         <v>28</v>
       </c>
       <c r="E18" s="37" t="s">
@@ -14729,7 +14787,7 @@
       <c r="F18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="232" t="s">
+      <c r="G18" s="245" t="s">
         <v>24</v>
       </c>
       <c r="H18" s="6" t="s">
@@ -14741,15 +14799,15 @@
     </row>
     <row r="19" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B19" s="61"/>
-      <c r="C19" s="237"/>
-      <c r="D19" s="240"/>
+      <c r="C19" s="238"/>
+      <c r="D19" s="241"/>
       <c r="E19" s="37" t="s">
         <v>35</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G19" s="234"/>
+      <c r="G19" s="247"/>
       <c r="H19" s="8"/>
       <c r="I19" s="17"/>
     </row>
@@ -14794,8 +14852,8 @@
       <c r="E22" s="25"/>
       <c r="F22" s="22"/>
       <c r="G22" s="25"/>
-      <c r="H22" s="225"/>
-      <c r="I22" s="226"/>
+      <c r="H22" s="248"/>
+      <c r="I22" s="249"/>
     </row>
     <row r="23" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="67" t="s">
@@ -15209,19 +15267,19 @@
     </row>
     <row r="46" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B46" s="61"/>
-      <c r="C46" s="235" t="s">
+      <c r="C46" s="236" t="s">
         <v>42</v>
       </c>
-      <c r="D46" s="238" t="s">
+      <c r="D46" s="239" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="229" t="s">
+      <c r="E46" s="250" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="241" t="s">
+      <c r="F46" s="242" t="s">
         <v>46</v>
       </c>
-      <c r="G46" s="232" t="s">
+      <c r="G46" s="245" t="s">
         <v>47</v>
       </c>
       <c r="H46" s="6" t="s">
@@ -15233,23 +15291,23 @@
     </row>
     <row r="47" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="61"/>
-      <c r="C47" s="236"/>
-      <c r="D47" s="239"/>
-      <c r="E47" s="230"/>
-      <c r="F47" s="242"/>
-      <c r="G47" s="233"/>
-      <c r="H47" s="227" t="s">
+      <c r="C47" s="237"/>
+      <c r="D47" s="240"/>
+      <c r="E47" s="251"/>
+      <c r="F47" s="243"/>
+      <c r="G47" s="246"/>
+      <c r="H47" s="226" t="s">
         <v>32</v>
       </c>
-      <c r="I47" s="228"/>
+      <c r="I47" s="227"/>
     </row>
     <row r="48" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B48" s="61"/>
-      <c r="C48" s="237"/>
-      <c r="D48" s="240"/>
-      <c r="E48" s="231"/>
-      <c r="F48" s="243"/>
-      <c r="G48" s="234"/>
+      <c r="C48" s="238"/>
+      <c r="D48" s="241"/>
+      <c r="E48" s="252"/>
+      <c r="F48" s="244"/>
+      <c r="G48" s="247"/>
       <c r="H48" s="8" t="s">
         <v>23</v>
       </c>
@@ -15283,19 +15341,19 @@
     </row>
     <row r="50" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B50" s="61"/>
-      <c r="C50" s="235" t="s">
+      <c r="C50" s="236" t="s">
         <v>52</v>
       </c>
-      <c r="D50" s="238" t="s">
+      <c r="D50" s="239" t="s">
         <v>53</v>
       </c>
-      <c r="E50" s="229" t="s">
+      <c r="E50" s="250" t="s">
         <v>55</v>
       </c>
-      <c r="F50" s="241" t="s">
+      <c r="F50" s="242" t="s">
         <v>56</v>
       </c>
-      <c r="G50" s="232" t="s">
+      <c r="G50" s="245" t="s">
         <v>9</v>
       </c>
       <c r="H50" s="6" t="s">
@@ -15307,23 +15365,23 @@
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="61"/>
-      <c r="C51" s="236"/>
-      <c r="D51" s="239"/>
-      <c r="E51" s="230"/>
-      <c r="F51" s="242"/>
-      <c r="G51" s="233"/>
-      <c r="H51" s="227" t="s">
+      <c r="C51" s="237"/>
+      <c r="D51" s="240"/>
+      <c r="E51" s="251"/>
+      <c r="F51" s="243"/>
+      <c r="G51" s="246"/>
+      <c r="H51" s="226" t="s">
         <v>32</v>
       </c>
-      <c r="I51" s="228"/>
+      <c r="I51" s="227"/>
     </row>
     <row r="52" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B52" s="61"/>
-      <c r="C52" s="237"/>
-      <c r="D52" s="240"/>
-      <c r="E52" s="231"/>
-      <c r="F52" s="243"/>
-      <c r="G52" s="234"/>
+      <c r="C52" s="238"/>
+      <c r="D52" s="241"/>
+      <c r="E52" s="252"/>
+      <c r="F52" s="244"/>
+      <c r="G52" s="247"/>
       <c r="H52" s="8" t="s">
         <v>23</v>
       </c>
@@ -15348,8 +15406,8 @@
       <c r="E54" s="25"/>
       <c r="F54" s="22"/>
       <c r="G54" s="25"/>
-      <c r="H54" s="225"/>
-      <c r="I54" s="226"/>
+      <c r="H54" s="248"/>
+      <c r="I54" s="249"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="61" t="s">
@@ -15412,10 +15470,10 @@
       <c r="E58" s="39"/>
       <c r="F58" s="12"/>
       <c r="G58" s="32"/>
-      <c r="H58" s="227" t="s">
+      <c r="H58" s="226" t="s">
         <v>32</v>
       </c>
-      <c r="I58" s="228"/>
+      <c r="I58" s="227"/>
     </row>
     <row r="59" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B59" s="61"/>
@@ -15448,8 +15506,8 @@
       <c r="E61" s="25"/>
       <c r="F61" s="22"/>
       <c r="G61" s="25"/>
-      <c r="H61" s="225"/>
-      <c r="I61" s="226"/>
+      <c r="H61" s="248"/>
+      <c r="I61" s="249"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="64" t="s">
@@ -15862,8 +15920,8 @@
       <c r="E89" s="25"/>
       <c r="F89" s="22"/>
       <c r="G89" s="25"/>
-      <c r="H89" s="225"/>
-      <c r="I89" s="226"/>
+      <c r="H89" s="248"/>
+      <c r="I89" s="249"/>
     </row>
     <row r="90" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="61"/>
@@ -16007,15 +16065,22 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="E50:E52"/>
+    <mergeCell ref="G50:G52"/>
+    <mergeCell ref="H51:I51"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="D50:D52"/>
+    <mergeCell ref="F50:F52"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="C46:C48"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="F46:F48"/>
+    <mergeCell ref="G46:G48"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="G18:G19"/>
@@ -16028,22 +16093,15 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="D14:D16"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="F50:F52"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="C46:C48"/>
-    <mergeCell ref="D46:D48"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="F46:F48"/>
-    <mergeCell ref="G46:G48"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="G50:G52"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -16073,14 +16131,14 @@
   <sheetData>
     <row r="1" spans="2:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="252" t="s">
+      <c r="B2" s="253" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="253"/>
-      <c r="D2" s="245" t="s">
+      <c r="C2" s="254"/>
+      <c r="D2" s="229" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="246" t="s">
+      <c r="E2" s="230" t="s">
         <v>0</v>
       </c>
     </row>
@@ -16091,8 +16149,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="250"/>
-      <c r="E3" s="251"/>
+      <c r="D3" s="234"/>
+      <c r="E3" s="235"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">
@@ -16552,7 +16610,7 @@
       <c r="B2" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="254" t="s">
+      <c r="C2" s="255" t="s">
         <v>0</v>
       </c>
     </row>
@@ -16560,7 +16618,7 @@
       <c r="B3" s="90" t="s">
         <v>145</v>
       </c>
-      <c r="C3" s="255"/>
+      <c r="C3" s="256"/>
     </row>
     <row r="4" spans="2:3" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="89" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 23 Mei 2023 18:02 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -13,12 +13,11 @@
     <sheet name="Database" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="1074">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="1075">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -3481,6 +3480,9 @@
   <si>
     <t>Mendapatkan Data List Jenis Posisi Jabatan Pekerja saat ini berdasarkan ID Branch (varBranch_RefID) dan ID Worker (varWorker_RefID).
 Adapun Pick Statement (varPickStatement), Sort Statement (varSortStatement), Filter Statement (varFilterStatement), dan Paging Statement (varPagingStatement) merupakan parameter optional yang dapat digunakan ataupun tidak sesuai dengan kebutuhan</t>
+  </si>
+  <si>
+    <t>1.03.0000</t>
   </si>
 </sst>
 </file>
@@ -4920,6 +4922,24 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4935,23 +4955,11 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4959,6 +4967,51 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4982,57 +5035,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5363,7 +5365,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D91" sqref="D91"/>
+      <selection pane="bottomRight" activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5382,20 +5384,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="226" t="s">
+      <c r="B2" s="232" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="227"/>
-      <c r="D2" s="228"/>
-      <c r="E2" s="233" t="s">
+      <c r="C2" s="233"/>
+      <c r="D2" s="234"/>
+      <c r="E2" s="228" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="229" t="s">
+      <c r="F2" s="224" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="230"/>
-      <c r="H2" s="231"/>
-      <c r="I2" s="224" t="s">
+      <c r="G2" s="225"/>
+      <c r="H2" s="226"/>
+      <c r="I2" s="230" t="s">
         <v>669</v>
       </c>
     </row>
@@ -5409,7 +5411,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="234"/>
+      <c r="E3" s="229"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -5419,11 +5421,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="225"/>
+      <c r="I3" s="231"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="232" t="s">
+      <c r="B4" s="227" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -6923,10 +6925,10 @@
         <v>1069</v>
       </c>
       <c r="F91" s="150" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G91" s="188">
-        <v>45068</v>
+        <v>45069</v>
       </c>
       <c r="H91" s="203">
         <v>44490</v>
@@ -6946,10 +6948,10 @@
         <v>1066</v>
       </c>
       <c r="F92" s="150" t="s">
-        <v>547</v>
+        <v>1074</v>
       </c>
       <c r="G92" s="188">
-        <v>44937</v>
+        <v>45069</v>
       </c>
       <c r="H92" s="203">
         <v>44705</v>
@@ -15906,30 +15908,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B450:B451"/>
-    <mergeCell ref="C451:C452"/>
-    <mergeCell ref="C227:C228"/>
-    <mergeCell ref="B446:B447"/>
-    <mergeCell ref="C447:C448"/>
-    <mergeCell ref="C327:C328"/>
-    <mergeCell ref="C442:C443"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="C548:C549"/>
-    <mergeCell ref="C466:C467"/>
-    <mergeCell ref="C469:C470"/>
-    <mergeCell ref="C491:C492"/>
-    <mergeCell ref="C494:C495"/>
-    <mergeCell ref="C497:C498"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="C208:C209"/>
-    <mergeCell ref="C438:C439"/>
     <mergeCell ref="B558:B559"/>
     <mergeCell ref="C559:C560"/>
     <mergeCell ref="I2:I3"/>
@@ -15946,6 +15924,30 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C76:C77"/>
     <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="C160:C161"/>
+    <mergeCell ref="C548:C549"/>
+    <mergeCell ref="C466:C467"/>
+    <mergeCell ref="C469:C470"/>
+    <mergeCell ref="C491:C492"/>
+    <mergeCell ref="C494:C495"/>
+    <mergeCell ref="C497:C498"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="C208:C209"/>
+    <mergeCell ref="C438:C439"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B450:B451"/>
+    <mergeCell ref="C451:C452"/>
+    <mergeCell ref="C227:C228"/>
+    <mergeCell ref="B446:B447"/>
+    <mergeCell ref="C447:C448"/>
+    <mergeCell ref="C327:C328"/>
+    <mergeCell ref="C442:C443"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -15979,20 +15981,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="240" t="s">
+      <c r="B2" s="257" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="241"/>
-      <c r="D2" s="242"/>
-      <c r="E2" s="237" t="s">
+      <c r="C2" s="258"/>
+      <c r="D2" s="259"/>
+      <c r="E2" s="254" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="239"/>
-      <c r="G2" s="237" t="s">
+      <c r="F2" s="256"/>
+      <c r="G2" s="254" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="238"/>
-      <c r="I2" s="239"/>
+      <c r="H2" s="255"/>
+      <c r="I2" s="256"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -16013,10 +16015,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="243" t="s">
+      <c r="H3" s="260" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="244"/>
+      <c r="I3" s="261"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -16051,8 +16053,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="257"/>
-      <c r="I6" s="258"/>
+      <c r="H6" s="235"/>
+      <c r="I6" s="236"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -16094,7 +16096,7 @@
       <c r="F8" s="251" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="254" t="s">
+      <c r="G8" s="242" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -16110,11 +16112,11 @@
       <c r="D9" s="249"/>
       <c r="E9" s="35"/>
       <c r="F9" s="252"/>
-      <c r="G9" s="255"/>
-      <c r="H9" s="235" t="s">
+      <c r="G9" s="243"/>
+      <c r="H9" s="237" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="236"/>
+      <c r="I9" s="238"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -16122,7 +16124,7 @@
       <c r="D10" s="250"/>
       <c r="E10" s="36"/>
       <c r="F10" s="253"/>
-      <c r="G10" s="256"/>
+      <c r="G10" s="244"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -16162,13 +16164,13 @@
       <c r="D12" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="259" t="s">
+      <c r="E12" s="239" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="251" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="254" t="s">
+      <c r="G12" s="242" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -16183,22 +16185,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="246"/>
       <c r="D13" s="249"/>
-      <c r="E13" s="260"/>
+      <c r="E13" s="240"/>
       <c r="F13" s="252"/>
-      <c r="G13" s="255"/>
-      <c r="H13" s="235" t="s">
+      <c r="G13" s="243"/>
+      <c r="H13" s="237" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="236"/>
+      <c r="I13" s="238"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="247"/>
       <c r="D14" s="250"/>
-      <c r="E14" s="261"/>
+      <c r="E14" s="241"/>
       <c r="F14" s="253"/>
-      <c r="G14" s="256"/>
+      <c r="G14" s="244"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -16308,7 +16310,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="254" t="s">
+      <c r="G21" s="242" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -16328,7 +16330,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="256"/>
+      <c r="G22" s="244"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -16373,8 +16375,8 @@
       <c r="E25" s="25"/>
       <c r="F25" s="22"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="257"/>
-      <c r="I25" s="258"/>
+      <c r="H25" s="235"/>
+      <c r="I25" s="236"/>
     </row>
     <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="67" t="s">
@@ -16794,13 +16796,13 @@
       <c r="D49" s="248" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="259" t="s">
+      <c r="E49" s="239" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="251" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="254" t="s">
+      <c r="G49" s="242" t="s">
         <v>47</v>
       </c>
       <c r="H49" s="6" t="s">
@@ -16814,21 +16816,21 @@
       <c r="B50" s="61"/>
       <c r="C50" s="246"/>
       <c r="D50" s="249"/>
-      <c r="E50" s="260"/>
+      <c r="E50" s="240"/>
       <c r="F50" s="252"/>
-      <c r="G50" s="255"/>
-      <c r="H50" s="235" t="s">
+      <c r="G50" s="243"/>
+      <c r="H50" s="237" t="s">
         <v>32</v>
       </c>
-      <c r="I50" s="236"/>
+      <c r="I50" s="238"/>
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B51" s="61"/>
       <c r="C51" s="247"/>
       <c r="D51" s="250"/>
-      <c r="E51" s="261"/>
+      <c r="E51" s="241"/>
       <c r="F51" s="253"/>
-      <c r="G51" s="256"/>
+      <c r="G51" s="244"/>
       <c r="H51" s="8" t="s">
         <v>23</v>
       </c>
@@ -16868,13 +16870,13 @@
       <c r="D53" s="248" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="259" t="s">
+      <c r="E53" s="239" t="s">
         <v>55</v>
       </c>
       <c r="F53" s="251" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="254" t="s">
+      <c r="G53" s="242" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -16888,21 +16890,21 @@
       <c r="B54" s="61"/>
       <c r="C54" s="246"/>
       <c r="D54" s="249"/>
-      <c r="E54" s="260"/>
+      <c r="E54" s="240"/>
       <c r="F54" s="252"/>
-      <c r="G54" s="255"/>
-      <c r="H54" s="235" t="s">
+      <c r="G54" s="243"/>
+      <c r="H54" s="237" t="s">
         <v>32</v>
       </c>
-      <c r="I54" s="236"/>
+      <c r="I54" s="238"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
       <c r="C55" s="247"/>
       <c r="D55" s="250"/>
-      <c r="E55" s="261"/>
+      <c r="E55" s="241"/>
       <c r="F55" s="253"/>
-      <c r="G55" s="256"/>
+      <c r="G55" s="244"/>
       <c r="H55" s="8" t="s">
         <v>23</v>
       </c>
@@ -16927,8 +16929,8 @@
       <c r="E57" s="25"/>
       <c r="F57" s="22"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="257"/>
-      <c r="I57" s="258"/>
+      <c r="H57" s="235"/>
+      <c r="I57" s="236"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="61" t="s">
@@ -16991,10 +16993,10 @@
       <c r="E61" s="39"/>
       <c r="F61" s="12"/>
       <c r="G61" s="32"/>
-      <c r="H61" s="235" t="s">
+      <c r="H61" s="237" t="s">
         <v>32</v>
       </c>
-      <c r="I61" s="236"/>
+      <c r="I61" s="238"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -17027,8 +17029,8 @@
       <c r="E64" s="25"/>
       <c r="F64" s="22"/>
       <c r="G64" s="25"/>
-      <c r="H64" s="257"/>
-      <c r="I64" s="258"/>
+      <c r="H64" s="235"/>
+      <c r="I64" s="236"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64" t="s">
@@ -17441,8 +17443,8 @@
       <c r="E92" s="25"/>
       <c r="F92" s="22"/>
       <c r="G92" s="25"/>
-      <c r="H92" s="257"/>
-      <c r="I92" s="258"/>
+      <c r="H92" s="235"/>
+      <c r="I92" s="236"/>
     </row>
     <row r="93" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="61"/>
@@ -17586,22 +17588,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -17614,16 +17610,22 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H64:I64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -17657,10 +17659,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="263"/>
-      <c r="D2" s="238" t="s">
+      <c r="D2" s="255" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="239" t="s">
+      <c r="E2" s="256" t="s">
         <v>0</v>
       </c>
     </row>
@@ -17671,8 +17673,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="243"/>
-      <c r="E3" s="244"/>
+      <c r="D3" s="260"/>
+      <c r="E3" s="261"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 26 Mei 2023 19:55 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -5030,6 +5030,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5048,20 +5063,71 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5069,12 +5135,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5083,66 +5143,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5470,10 +5470,10 @@
   <dimension ref="A1:I604"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D151" sqref="D151"/>
+      <selection pane="bottomRight" activeCell="G88" sqref="G88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5492,20 +5492,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="232" t="s">
+      <c r="B2" s="226" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="233"/>
-      <c r="D2" s="234"/>
-      <c r="E2" s="228" t="s">
+      <c r="C2" s="227"/>
+      <c r="D2" s="228"/>
+      <c r="E2" s="233" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="224" t="s">
+      <c r="F2" s="229" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="225"/>
-      <c r="H2" s="226"/>
-      <c r="I2" s="230" t="s">
+      <c r="G2" s="230"/>
+      <c r="H2" s="231"/>
+      <c r="I2" s="224" t="s">
         <v>669</v>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="229"/>
+      <c r="E3" s="234"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -5529,11 +5529,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="231"/>
+      <c r="I3" s="225"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="227" t="s">
+      <c r="B4" s="232" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -6965,10 +6965,10 @@
         <v>584</v>
       </c>
       <c r="F87" s="151" t="s">
-        <v>547</v>
+        <v>591</v>
       </c>
       <c r="G87" s="190">
-        <v>44964</v>
+        <v>45072</v>
       </c>
       <c r="H87" s="204">
         <v>44722</v>
@@ -16308,6 +16308,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B459:B460"/>
+    <mergeCell ref="C460:C461"/>
+    <mergeCell ref="C234:C235"/>
+    <mergeCell ref="B455:B456"/>
+    <mergeCell ref="C456:C457"/>
+    <mergeCell ref="C334:C335"/>
+    <mergeCell ref="C451:C452"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="C560:C561"/>
+    <mergeCell ref="C475:C476"/>
+    <mergeCell ref="C478:C479"/>
+    <mergeCell ref="C500:C501"/>
+    <mergeCell ref="C503:C504"/>
+    <mergeCell ref="C506:C507"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="C183:C184"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="C445:C446"/>
     <mergeCell ref="B570:B571"/>
     <mergeCell ref="C571:C572"/>
     <mergeCell ref="I2:I3"/>
@@ -16324,30 +16348,6 @@
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C76:C77"/>
     <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="C560:C561"/>
-    <mergeCell ref="C475:C476"/>
-    <mergeCell ref="C478:C479"/>
-    <mergeCell ref="C500:C501"/>
-    <mergeCell ref="C503:C504"/>
-    <mergeCell ref="C506:C507"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="C183:C184"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="C445:C446"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B459:B460"/>
-    <mergeCell ref="C460:C461"/>
-    <mergeCell ref="C234:C235"/>
-    <mergeCell ref="B455:B456"/>
-    <mergeCell ref="C456:C457"/>
-    <mergeCell ref="C334:C335"/>
-    <mergeCell ref="C451:C452"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -16381,20 +16381,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="257" t="s">
+      <c r="B2" s="240" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="258"/>
-      <c r="D2" s="259"/>
-      <c r="E2" s="254" t="s">
+      <c r="C2" s="241"/>
+      <c r="D2" s="242"/>
+      <c r="E2" s="237" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="256"/>
-      <c r="G2" s="254" t="s">
+      <c r="F2" s="239"/>
+      <c r="G2" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="255"/>
-      <c r="I2" s="256"/>
+      <c r="H2" s="238"/>
+      <c r="I2" s="239"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -16415,10 +16415,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="260" t="s">
+      <c r="H3" s="243" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="261"/>
+      <c r="I3" s="244"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -16453,8 +16453,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="235"/>
-      <c r="I6" s="236"/>
+      <c r="H6" s="257"/>
+      <c r="I6" s="258"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -16496,7 +16496,7 @@
       <c r="F8" s="251" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="242" t="s">
+      <c r="G8" s="254" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -16512,11 +16512,11 @@
       <c r="D9" s="249"/>
       <c r="E9" s="35"/>
       <c r="F9" s="252"/>
-      <c r="G9" s="243"/>
-      <c r="H9" s="237" t="s">
+      <c r="G9" s="255"/>
+      <c r="H9" s="235" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="238"/>
+      <c r="I9" s="236"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -16524,7 +16524,7 @@
       <c r="D10" s="250"/>
       <c r="E10" s="36"/>
       <c r="F10" s="253"/>
-      <c r="G10" s="244"/>
+      <c r="G10" s="256"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -16564,13 +16564,13 @@
       <c r="D12" s="248" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="239" t="s">
+      <c r="E12" s="259" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="251" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="242" t="s">
+      <c r="G12" s="254" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -16585,22 +16585,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="246"/>
       <c r="D13" s="249"/>
-      <c r="E13" s="240"/>
+      <c r="E13" s="260"/>
       <c r="F13" s="252"/>
-      <c r="G13" s="243"/>
-      <c r="H13" s="237" t="s">
+      <c r="G13" s="255"/>
+      <c r="H13" s="235" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="238"/>
+      <c r="I13" s="236"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="247"/>
       <c r="D14" s="250"/>
-      <c r="E14" s="241"/>
+      <c r="E14" s="261"/>
       <c r="F14" s="253"/>
-      <c r="G14" s="244"/>
+      <c r="G14" s="256"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -16710,7 +16710,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="242" t="s">
+      <c r="G21" s="254" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -16730,7 +16730,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="244"/>
+      <c r="G22" s="256"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -16775,8 +16775,8 @@
       <c r="E25" s="25"/>
       <c r="F25" s="22"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="235"/>
-      <c r="I25" s="236"/>
+      <c r="H25" s="257"/>
+      <c r="I25" s="258"/>
     </row>
     <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="67" t="s">
@@ -17196,13 +17196,13 @@
       <c r="D49" s="248" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="239" t="s">
+      <c r="E49" s="259" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="251" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="242" t="s">
+      <c r="G49" s="254" t="s">
         <v>47</v>
       </c>
       <c r="H49" s="6" t="s">
@@ -17216,21 +17216,21 @@
       <c r="B50" s="61"/>
       <c r="C50" s="246"/>
       <c r="D50" s="249"/>
-      <c r="E50" s="240"/>
+      <c r="E50" s="260"/>
       <c r="F50" s="252"/>
-      <c r="G50" s="243"/>
-      <c r="H50" s="237" t="s">
+      <c r="G50" s="255"/>
+      <c r="H50" s="235" t="s">
         <v>32</v>
       </c>
-      <c r="I50" s="238"/>
+      <c r="I50" s="236"/>
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B51" s="61"/>
       <c r="C51" s="247"/>
       <c r="D51" s="250"/>
-      <c r="E51" s="241"/>
+      <c r="E51" s="261"/>
       <c r="F51" s="253"/>
-      <c r="G51" s="244"/>
+      <c r="G51" s="256"/>
       <c r="H51" s="8" t="s">
         <v>23</v>
       </c>
@@ -17270,13 +17270,13 @@
       <c r="D53" s="248" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="239" t="s">
+      <c r="E53" s="259" t="s">
         <v>55</v>
       </c>
       <c r="F53" s="251" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="242" t="s">
+      <c r="G53" s="254" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -17290,21 +17290,21 @@
       <c r="B54" s="61"/>
       <c r="C54" s="246"/>
       <c r="D54" s="249"/>
-      <c r="E54" s="240"/>
+      <c r="E54" s="260"/>
       <c r="F54" s="252"/>
-      <c r="G54" s="243"/>
-      <c r="H54" s="237" t="s">
+      <c r="G54" s="255"/>
+      <c r="H54" s="235" t="s">
         <v>32</v>
       </c>
-      <c r="I54" s="238"/>
+      <c r="I54" s="236"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
       <c r="C55" s="247"/>
       <c r="D55" s="250"/>
-      <c r="E55" s="241"/>
+      <c r="E55" s="261"/>
       <c r="F55" s="253"/>
-      <c r="G55" s="244"/>
+      <c r="G55" s="256"/>
       <c r="H55" s="8" t="s">
         <v>23</v>
       </c>
@@ -17329,8 +17329,8 @@
       <c r="E57" s="25"/>
       <c r="F57" s="22"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="235"/>
-      <c r="I57" s="236"/>
+      <c r="H57" s="257"/>
+      <c r="I57" s="258"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="61" t="s">
@@ -17393,10 +17393,10 @@
       <c r="E61" s="39"/>
       <c r="F61" s="12"/>
       <c r="G61" s="32"/>
-      <c r="H61" s="237" t="s">
+      <c r="H61" s="235" t="s">
         <v>32</v>
       </c>
-      <c r="I61" s="238"/>
+      <c r="I61" s="236"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -17429,8 +17429,8 @@
       <c r="E64" s="25"/>
       <c r="F64" s="22"/>
       <c r="G64" s="25"/>
-      <c r="H64" s="235"/>
-      <c r="I64" s="236"/>
+      <c r="H64" s="257"/>
+      <c r="I64" s="258"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64" t="s">
@@ -17843,8 +17843,8 @@
       <c r="E92" s="25"/>
       <c r="F92" s="22"/>
       <c r="G92" s="25"/>
-      <c r="H92" s="235"/>
-      <c r="I92" s="236"/>
+      <c r="H92" s="257"/>
+      <c r="I92" s="258"/>
     </row>
     <row r="93" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="61"/>
@@ -17988,16 +17988,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -18010,22 +18016,16 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -18059,10 +18059,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="263"/>
-      <c r="D2" s="255" t="s">
+      <c r="D2" s="238" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="256" t="s">
+      <c r="E2" s="239" t="s">
         <v>0</v>
       </c>
     </row>
@@ -18073,8 +18073,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="260"/>
-      <c r="E3" s="261"/>
+      <c r="D3" s="243"/>
+      <c r="E3" s="244"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 19 Juni 2023 13:38 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3330" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Function" sheetId="3" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Table" sheetId="1" r:id="rId3"/>
     <sheet name="Schema" sheetId="2" r:id="rId4"/>
     <sheet name="Database" sheetId="4" r:id="rId5"/>
+    <sheet name="Transalation Formula" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1911" uniqueCount="1160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="1162">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -3858,6 +3859,12 @@
   <si>
     <t>SchSysConfig.
 HoldFuncSys_General_GetSubOrdinatArrayIDFromSuperOrdinatArrayID</t>
+  </si>
+  <si>
+    <t>Get PID</t>
+  </si>
+  <si>
+    <t>((("AnyID"/1000000000000)%10000)*1000000000000) + ("AnyID"%1000000000000))</t>
   </si>
 </sst>
 </file>
@@ -5306,6 +5313,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5324,20 +5346,71 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5345,12 +5418,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5359,66 +5426,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6286,6 +6293,60 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="14" name="Elbow Connector 13"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="88" idx="2"/>
+          <a:endCxn id="75" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5274469" y="88107"/>
+          <a:ext cx="928688" cy="1990725"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6578,7 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I642"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="F387" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -6601,20 +6662,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="235" t="s">
+      <c r="B2" s="229" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="236"/>
-      <c r="D2" s="237"/>
-      <c r="E2" s="231" t="s">
+      <c r="C2" s="230"/>
+      <c r="D2" s="231"/>
+      <c r="E2" s="236" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="227" t="s">
+      <c r="F2" s="232" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="228"/>
-      <c r="H2" s="229"/>
-      <c r="I2" s="233" t="s">
+      <c r="G2" s="233"/>
+      <c r="H2" s="234"/>
+      <c r="I2" s="227" t="s">
         <v>667</v>
       </c>
     </row>
@@ -6628,7 +6689,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="232"/>
+      <c r="E3" s="237"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -6638,11 +6699,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="234"/>
+      <c r="I3" s="228"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="230" t="s">
+      <c r="B4" s="235" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -18145,6 +18206,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B497:B498"/>
+    <mergeCell ref="C498:C499"/>
+    <mergeCell ref="C257:C258"/>
+    <mergeCell ref="B493:B494"/>
+    <mergeCell ref="C494:C495"/>
+    <mergeCell ref="C360:C361"/>
+    <mergeCell ref="C489:C490"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C116:C117"/>
+    <mergeCell ref="C190:C191"/>
+    <mergeCell ref="C598:C599"/>
+    <mergeCell ref="C513:C514"/>
+    <mergeCell ref="C516:C517"/>
+    <mergeCell ref="C538:C539"/>
+    <mergeCell ref="C541:C542"/>
+    <mergeCell ref="C544:C545"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="C206:C207"/>
+    <mergeCell ref="C238:C239"/>
+    <mergeCell ref="C478:C479"/>
     <mergeCell ref="B608:B609"/>
     <mergeCell ref="C609:C610"/>
     <mergeCell ref="I2:I3"/>
@@ -18161,30 +18246,6 @@
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="C91:C92"/>
     <mergeCell ref="C94:C95"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="C598:C599"/>
-    <mergeCell ref="C513:C514"/>
-    <mergeCell ref="C516:C517"/>
-    <mergeCell ref="C538:C539"/>
-    <mergeCell ref="C541:C542"/>
-    <mergeCell ref="C544:C545"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="C206:C207"/>
-    <mergeCell ref="C238:C239"/>
-    <mergeCell ref="C478:C479"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B497:B498"/>
-    <mergeCell ref="C498:C499"/>
-    <mergeCell ref="C257:C258"/>
-    <mergeCell ref="B493:B494"/>
-    <mergeCell ref="C494:C495"/>
-    <mergeCell ref="C360:C361"/>
-    <mergeCell ref="C489:C490"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -18196,7 +18257,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18237,20 +18298,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="260" t="s">
+      <c r="B2" s="243" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="261"/>
-      <c r="D2" s="262"/>
-      <c r="E2" s="257" t="s">
+      <c r="C2" s="244"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="240" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="259"/>
-      <c r="G2" s="257" t="s">
+      <c r="F2" s="242"/>
+      <c r="G2" s="240" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="258"/>
-      <c r="I2" s="259"/>
+      <c r="H2" s="241"/>
+      <c r="I2" s="242"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -18271,10 +18332,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="263" t="s">
+      <c r="H3" s="246" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="264"/>
+      <c r="I3" s="247"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -18309,8 +18370,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="238"/>
-      <c r="I6" s="239"/>
+      <c r="H6" s="260"/>
+      <c r="I6" s="261"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -18352,7 +18413,7 @@
       <c r="F8" s="254" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="245" t="s">
+      <c r="G8" s="257" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -18368,11 +18429,11 @@
       <c r="D9" s="252"/>
       <c r="E9" s="35"/>
       <c r="F9" s="255"/>
-      <c r="G9" s="246"/>
-      <c r="H9" s="240" t="s">
+      <c r="G9" s="258"/>
+      <c r="H9" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="241"/>
+      <c r="I9" s="239"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -18380,7 +18441,7 @@
       <c r="D10" s="253"/>
       <c r="E10" s="36"/>
       <c r="F10" s="256"/>
-      <c r="G10" s="247"/>
+      <c r="G10" s="259"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -18420,13 +18481,13 @@
       <c r="D12" s="251" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="242" t="s">
+      <c r="E12" s="262" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="254" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="245" t="s">
+      <c r="G12" s="257" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -18441,22 +18502,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="249"/>
       <c r="D13" s="252"/>
-      <c r="E13" s="243"/>
+      <c r="E13" s="263"/>
       <c r="F13" s="255"/>
-      <c r="G13" s="246"/>
-      <c r="H13" s="240" t="s">
+      <c r="G13" s="258"/>
+      <c r="H13" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="241"/>
+      <c r="I13" s="239"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="250"/>
       <c r="D14" s="253"/>
-      <c r="E14" s="244"/>
+      <c r="E14" s="264"/>
       <c r="F14" s="256"/>
-      <c r="G14" s="247"/>
+      <c r="G14" s="259"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -18566,7 +18627,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="245" t="s">
+      <c r="G21" s="257" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -18586,7 +18647,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="247"/>
+      <c r="G22" s="259"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -18631,8 +18692,8 @@
       <c r="E25" s="25"/>
       <c r="F25" s="22"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="238"/>
-      <c r="I25" s="239"/>
+      <c r="H25" s="260"/>
+      <c r="I25" s="261"/>
     </row>
     <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="67" t="s">
@@ -19052,13 +19113,13 @@
       <c r="D49" s="251" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="242" t="s">
+      <c r="E49" s="262" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="254" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="245" t="s">
+      <c r="G49" s="257" t="s">
         <v>47</v>
       </c>
       <c r="H49" s="6" t="s">
@@ -19072,21 +19133,21 @@
       <c r="B50" s="61"/>
       <c r="C50" s="249"/>
       <c r="D50" s="252"/>
-      <c r="E50" s="243"/>
+      <c r="E50" s="263"/>
       <c r="F50" s="255"/>
-      <c r="G50" s="246"/>
-      <c r="H50" s="240" t="s">
+      <c r="G50" s="258"/>
+      <c r="H50" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="I50" s="241"/>
+      <c r="I50" s="239"/>
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B51" s="61"/>
       <c r="C51" s="250"/>
       <c r="D51" s="253"/>
-      <c r="E51" s="244"/>
+      <c r="E51" s="264"/>
       <c r="F51" s="256"/>
-      <c r="G51" s="247"/>
+      <c r="G51" s="259"/>
       <c r="H51" s="8" t="s">
         <v>23</v>
       </c>
@@ -19126,13 +19187,13 @@
       <c r="D53" s="251" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="242" t="s">
+      <c r="E53" s="262" t="s">
         <v>55</v>
       </c>
       <c r="F53" s="254" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="245" t="s">
+      <c r="G53" s="257" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -19146,21 +19207,21 @@
       <c r="B54" s="61"/>
       <c r="C54" s="249"/>
       <c r="D54" s="252"/>
-      <c r="E54" s="243"/>
+      <c r="E54" s="263"/>
       <c r="F54" s="255"/>
-      <c r="G54" s="246"/>
-      <c r="H54" s="240" t="s">
+      <c r="G54" s="258"/>
+      <c r="H54" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="I54" s="241"/>
+      <c r="I54" s="239"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
       <c r="C55" s="250"/>
       <c r="D55" s="253"/>
-      <c r="E55" s="244"/>
+      <c r="E55" s="264"/>
       <c r="F55" s="256"/>
-      <c r="G55" s="247"/>
+      <c r="G55" s="259"/>
       <c r="H55" s="8" t="s">
         <v>23</v>
       </c>
@@ -19185,8 +19246,8 @@
       <c r="E57" s="25"/>
       <c r="F57" s="22"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="238"/>
-      <c r="I57" s="239"/>
+      <c r="H57" s="260"/>
+      <c r="I57" s="261"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="61" t="s">
@@ -19249,10 +19310,10 @@
       <c r="E61" s="39"/>
       <c r="F61" s="12"/>
       <c r="G61" s="32"/>
-      <c r="H61" s="240" t="s">
+      <c r="H61" s="238" t="s">
         <v>32</v>
       </c>
-      <c r="I61" s="241"/>
+      <c r="I61" s="239"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -19285,8 +19346,8 @@
       <c r="E64" s="25"/>
       <c r="F64" s="22"/>
       <c r="G64" s="25"/>
-      <c r="H64" s="238"/>
-      <c r="I64" s="239"/>
+      <c r="H64" s="260"/>
+      <c r="I64" s="261"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64" t="s">
@@ -19699,8 +19760,8 @@
       <c r="E92" s="25"/>
       <c r="F92" s="22"/>
       <c r="G92" s="25"/>
-      <c r="H92" s="238"/>
-      <c r="I92" s="239"/>
+      <c r="H92" s="260"/>
+      <c r="I92" s="261"/>
     </row>
     <row r="93" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="61"/>
@@ -19844,16 +19905,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -19866,22 +19933,16 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -19915,10 +19976,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="266"/>
-      <c r="D2" s="258" t="s">
+      <c r="D2" s="241" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="259" t="s">
+      <c r="E2" s="242" t="s">
         <v>0</v>
       </c>
     </row>
@@ -19929,8 +19990,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="263"/>
-      <c r="E3" s="264"/>
+      <c r="D3" s="246"/>
+      <c r="E3" s="247"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">
@@ -20438,4 +20499,33 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="78"/>
+    <col min="3" max="3" width="62.28515625" style="78" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="78"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="78" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C2" s="78" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Pertanggal 4 September 2023 15:23 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2145" uniqueCount="1312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2161" uniqueCount="1320">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -4397,6 +4397,30 @@
   <si>
     <t>SchSysAsset.
 HoldFunc_DataAnalysis_FncRprt_Profitability_ReturnOnInvestment</t>
+  </si>
+  <si>
+    <t>Func_TblLog_FileContent_INSERT</t>
+  </si>
+  <si>
+    <t>Func_TblLog_FileContent_UPDATE</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblLog_FileContent</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblLog_FileContent</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblLog_FileContentDetail</t>
+  </si>
+  <si>
+    <t>Func_TblLog_FileContentDetail_INSERT</t>
+  </si>
+  <si>
+    <t>Func_TblLog_FileContentDetail_UPDATE</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblLog_FileContentDetail</t>
   </si>
 </sst>
 </file>
@@ -5859,6 +5883,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5877,20 +5916,71 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -5898,12 +5988,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -5912,66 +5996,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7183,13 +7207,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I725"/>
+  <dimension ref="A1:I729"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F307" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E591" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D312" sqref="D312"/>
+      <selection pane="bottomRight" activeCell="D595" sqref="D595"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7208,20 +7232,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="236" t="s">
+      <c r="B2" s="230" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="237"/>
-      <c r="D2" s="238"/>
-      <c r="E2" s="232" t="s">
+      <c r="C2" s="231"/>
+      <c r="D2" s="232"/>
+      <c r="E2" s="237" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="228" t="s">
+      <c r="F2" s="233" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="229"/>
-      <c r="H2" s="230"/>
-      <c r="I2" s="234" t="s">
+      <c r="G2" s="234"/>
+      <c r="H2" s="235"/>
+      <c r="I2" s="228" t="s">
         <v>667</v>
       </c>
     </row>
@@ -7235,7 +7259,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="233"/>
+      <c r="E3" s="238"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -7245,11 +7269,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="235"/>
+      <c r="I3" s="229"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="231" t="s">
+      <c r="B4" s="236" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="134"/>
@@ -18088,55 +18112,77 @@
       <c r="A593" s="1"/>
       <c r="B593" s="109"/>
       <c r="C593" s="227"/>
-      <c r="D593" s="165"/>
-      <c r="E593" s="155"/>
-      <c r="F593" s="148"/>
-      <c r="G593" s="186"/>
-      <c r="H593" s="201"/>
-      <c r="I593" s="174"/>
-    </row>
-    <row r="594" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D593" s="166"/>
+      <c r="E593" s="162"/>
+      <c r="F593" s="150"/>
+      <c r="G593" s="188"/>
+      <c r="H593" s="203"/>
+      <c r="I593" s="176"/>
+    </row>
+    <row r="594" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A594" s="1"/>
       <c r="B594" s="109"/>
       <c r="C594" s="110"/>
-      <c r="D594" s="165"/>
-      <c r="E594" s="155"/>
-      <c r="F594" s="148"/>
-      <c r="G594" s="186"/>
-      <c r="H594" s="201"/>
-      <c r="I594" s="174"/>
-    </row>
-    <row r="595" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D594" s="166" t="s">
+        <v>1312</v>
+      </c>
+      <c r="E594" s="162" t="s">
+        <v>1314</v>
+      </c>
+      <c r="F594" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G594" s="188">
+        <v>45173</v>
+      </c>
+      <c r="H594" s="203">
+        <v>45173</v>
+      </c>
+      <c r="I594" s="183" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="595" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A595" s="1"/>
       <c r="B595" s="109"/>
-      <c r="C595" s="227" t="s">
-        <v>152</v>
-      </c>
-      <c r="D595" s="135"/>
-      <c r="E595" s="154"/>
-      <c r="F595" s="147"/>
-      <c r="G595" s="185"/>
-      <c r="H595" s="200"/>
-      <c r="I595" s="173"/>
+      <c r="C595" s="110"/>
+      <c r="D595" s="167" t="s">
+        <v>1313</v>
+      </c>
+      <c r="E595" s="160" t="s">
+        <v>1315</v>
+      </c>
+      <c r="F595" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G595" s="190">
+        <v>45173</v>
+      </c>
+      <c r="H595" s="204">
+        <v>45173</v>
+      </c>
+      <c r="I595" s="183" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="596" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A596" s="1"/>
       <c r="B596" s="109"/>
-      <c r="C596" s="227"/>
-      <c r="D596" s="166" t="s">
-        <v>757</v>
-      </c>
-      <c r="E596" s="162" t="s">
-        <v>759</v>
-      </c>
-      <c r="F596" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G596" s="188">
-        <v>44721</v>
+      <c r="C596" s="110"/>
+      <c r="D596" s="167" t="s">
+        <v>1317</v>
+      </c>
+      <c r="E596" s="160" t="s">
+        <v>1316</v>
+      </c>
+      <c r="F596" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G596" s="190">
+        <v>45173</v>
       </c>
       <c r="H596" s="204">
-        <v>44698</v>
+        <v>45173</v>
       </c>
       <c r="I596" s="183" t="s">
         <v>724</v>
@@ -18147,88 +18193,66 @@
       <c r="B597" s="109"/>
       <c r="C597" s="110"/>
       <c r="D597" s="167" t="s">
-        <v>758</v>
+        <v>1318</v>
       </c>
       <c r="E597" s="160" t="s">
-        <v>760</v>
+        <v>1319</v>
       </c>
       <c r="F597" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G597" s="190">
-        <v>44721</v>
+        <v>45173</v>
       </c>
       <c r="H597" s="204">
-        <v>44698</v>
+        <v>45173</v>
       </c>
       <c r="I597" s="183" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="598" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="598" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A598" s="1"/>
       <c r="B598" s="109"/>
       <c r="C598" s="110"/>
-      <c r="D598" s="167" t="s">
-        <v>752</v>
-      </c>
-      <c r="E598" s="160" t="s">
-        <v>754</v>
-      </c>
-      <c r="F598" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G598" s="190">
-        <v>44644</v>
-      </c>
-      <c r="H598" s="204">
-        <v>44622</v>
-      </c>
-      <c r="I598" s="183" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="599" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D598" s="167"/>
+      <c r="E598" s="160"/>
+      <c r="F598" s="151"/>
+      <c r="G598" s="190"/>
+      <c r="H598" s="204"/>
+      <c r="I598" s="177"/>
+    </row>
+    <row r="599" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A599" s="1"/>
       <c r="B599" s="109"/>
-      <c r="C599" s="110"/>
-      <c r="D599" s="167" t="s">
-        <v>753</v>
-      </c>
-      <c r="E599" s="160" t="s">
-        <v>755</v>
-      </c>
-      <c r="F599" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G599" s="190">
-        <v>44644</v>
-      </c>
-      <c r="H599" s="204">
-        <v>44622</v>
-      </c>
-      <c r="I599" s="183" t="s">
-        <v>724</v>
-      </c>
+      <c r="C599" s="227" t="s">
+        <v>152</v>
+      </c>
+      <c r="D599" s="135"/>
+      <c r="E599" s="154"/>
+      <c r="F599" s="147"/>
+      <c r="G599" s="185"/>
+      <c r="H599" s="200"/>
+      <c r="I599" s="173"/>
     </row>
     <row r="600" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A600" s="1"/>
       <c r="B600" s="109"/>
-      <c r="C600" s="110"/>
-      <c r="D600" s="167" t="s">
-        <v>761</v>
-      </c>
-      <c r="E600" s="160" t="s">
-        <v>763</v>
-      </c>
-      <c r="F600" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G600" s="190">
-        <v>44755</v>
+      <c r="C600" s="227"/>
+      <c r="D600" s="166" t="s">
+        <v>757</v>
+      </c>
+      <c r="E600" s="162" t="s">
+        <v>759</v>
+      </c>
+      <c r="F600" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G600" s="188">
+        <v>44721</v>
       </c>
       <c r="H600" s="204">
-        <v>44755</v>
+        <v>44698</v>
       </c>
       <c r="I600" s="183" t="s">
         <v>724</v>
@@ -18239,19 +18263,19 @@
       <c r="B601" s="109"/>
       <c r="C601" s="110"/>
       <c r="D601" s="167" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="E601" s="160" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="F601" s="151" t="s">
-        <v>232</v>
+        <v>267</v>
       </c>
       <c r="G601" s="190">
-        <v>44756</v>
+        <v>44721</v>
       </c>
       <c r="H601" s="204">
-        <v>44756</v>
+        <v>44698</v>
       </c>
       <c r="I601" s="183" t="s">
         <v>724</v>
@@ -18262,19 +18286,19 @@
       <c r="B602" s="109"/>
       <c r="C602" s="110"/>
       <c r="D602" s="167" t="s">
-        <v>765</v>
+        <v>752</v>
       </c>
       <c r="E602" s="160" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="F602" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G602" s="190">
-        <v>44755</v>
+        <v>44644</v>
       </c>
       <c r="H602" s="204">
-        <v>44755</v>
+        <v>44622</v>
       </c>
       <c r="I602" s="183" t="s">
         <v>724</v>
@@ -18285,67 +18309,115 @@
       <c r="B603" s="109"/>
       <c r="C603" s="110"/>
       <c r="D603" s="167" t="s">
-        <v>766</v>
+        <v>753</v>
       </c>
       <c r="E603" s="160" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="F603" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G603" s="190">
-        <v>44755</v>
+        <v>44644</v>
       </c>
       <c r="H603" s="204">
-        <v>44755</v>
+        <v>44622</v>
       </c>
       <c r="I603" s="183" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="604" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="604" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A604" s="1"/>
       <c r="B604" s="109"/>
       <c r="C604" s="110"/>
-      <c r="D604" s="167"/>
-      <c r="E604" s="160"/>
-      <c r="F604" s="151"/>
-      <c r="G604" s="190"/>
-      <c r="H604" s="204"/>
-      <c r="I604" s="177"/>
-    </row>
-    <row r="605" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D604" s="167" t="s">
+        <v>761</v>
+      </c>
+      <c r="E604" s="160" t="s">
+        <v>763</v>
+      </c>
+      <c r="F604" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G604" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H604" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I604" s="183" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="605" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A605" s="1"/>
       <c r="B605" s="109"/>
       <c r="C605" s="110"/>
-      <c r="D605" s="167"/>
-      <c r="E605" s="160"/>
-      <c r="F605" s="151"/>
-      <c r="G605" s="190"/>
-      <c r="H605" s="204"/>
-      <c r="I605" s="177"/>
-    </row>
-    <row r="606" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D605" s="167" t="s">
+        <v>762</v>
+      </c>
+      <c r="E605" s="160" t="s">
+        <v>764</v>
+      </c>
+      <c r="F605" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G605" s="190">
+        <v>44756</v>
+      </c>
+      <c r="H605" s="204">
+        <v>44756</v>
+      </c>
+      <c r="I605" s="183" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="606" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A606" s="1"/>
       <c r="B606" s="109"/>
       <c r="C606" s="110"/>
-      <c r="D606" s="167"/>
-      <c r="E606" s="160"/>
-      <c r="F606" s="151"/>
-      <c r="G606" s="190"/>
-      <c r="H606" s="204"/>
-      <c r="I606" s="177"/>
-    </row>
-    <row r="607" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D606" s="167" t="s">
+        <v>765</v>
+      </c>
+      <c r="E606" s="160" t="s">
+        <v>767</v>
+      </c>
+      <c r="F606" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G606" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H606" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I606" s="183" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="607" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A607" s="1"/>
       <c r="B607" s="109"/>
       <c r="C607" s="110"/>
-      <c r="D607" s="167"/>
-      <c r="E607" s="160"/>
-      <c r="F607" s="151"/>
-      <c r="G607" s="190"/>
-      <c r="H607" s="204"/>
-      <c r="I607" s="177"/>
+      <c r="D607" s="167" t="s">
+        <v>766</v>
+      </c>
+      <c r="E607" s="160" t="s">
+        <v>768</v>
+      </c>
+      <c r="F607" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G607" s="190">
+        <v>44755</v>
+      </c>
+      <c r="H607" s="204">
+        <v>44755</v>
+      </c>
+      <c r="I607" s="183" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="608" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A608" s="1"/>
@@ -18369,47 +18441,27 @@
       <c r="H609" s="204"/>
       <c r="I609" s="177"/>
     </row>
-    <row r="610" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A610" s="1"/>
       <c r="B610" s="109"/>
       <c r="C610" s="110"/>
-      <c r="D610" s="167" t="s">
-        <v>770</v>
-      </c>
+      <c r="D610" s="167"/>
       <c r="E610" s="160"/>
-      <c r="F610" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G610" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H610" s="204">
-        <v>44984</v>
-      </c>
-      <c r="I610" s="183" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="611" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="F610" s="151"/>
+      <c r="G610" s="190"/>
+      <c r="H610" s="204"/>
+      <c r="I610" s="177"/>
+    </row>
+    <row r="611" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A611" s="1"/>
       <c r="B611" s="109"/>
       <c r="C611" s="110"/>
-      <c r="D611" s="167" t="s">
-        <v>769</v>
-      </c>
+      <c r="D611" s="167"/>
       <c r="E611" s="160"/>
-      <c r="F611" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G611" s="190">
-        <v>44984</v>
-      </c>
-      <c r="H611" s="204">
-        <v>44984</v>
-      </c>
-      <c r="I611" s="183" t="s">
-        <v>724</v>
-      </c>
+      <c r="F611" s="151"/>
+      <c r="G611" s="190"/>
+      <c r="H611" s="204"/>
+      <c r="I611" s="177"/>
     </row>
     <row r="612" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A612" s="1"/>
@@ -18433,124 +18485,120 @@
       <c r="H613" s="204"/>
       <c r="I613" s="177"/>
     </row>
-    <row r="614" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A614" s="1"/>
       <c r="B614" s="109"/>
       <c r="C614" s="110"/>
-      <c r="D614" s="167"/>
+      <c r="D614" s="167" t="s">
+        <v>770</v>
+      </c>
       <c r="E614" s="160"/>
-      <c r="F614" s="151"/>
-      <c r="G614" s="190"/>
-      <c r="H614" s="204"/>
-      <c r="I614" s="177"/>
-    </row>
-    <row r="615" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="F614" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G614" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H614" s="204">
+        <v>44984</v>
+      </c>
+      <c r="I614" s="183" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="615" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A615" s="1"/>
       <c r="B615" s="109"/>
       <c r="C615" s="110"/>
-      <c r="D615" s="167"/>
+      <c r="D615" s="167" t="s">
+        <v>769</v>
+      </c>
       <c r="E615" s="160"/>
-      <c r="F615" s="151"/>
-      <c r="G615" s="190"/>
-      <c r="H615" s="204"/>
-      <c r="I615" s="177"/>
+      <c r="F615" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G615" s="190">
+        <v>44984</v>
+      </c>
+      <c r="H615" s="204">
+        <v>44984</v>
+      </c>
+      <c r="I615" s="183" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="616" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A616" s="1"/>
       <c r="B616" s="109"/>
       <c r="C616" s="110"/>
-      <c r="D616" s="165"/>
-      <c r="E616" s="155"/>
-      <c r="F616" s="148"/>
-      <c r="G616" s="186"/>
-      <c r="H616" s="201"/>
-      <c r="I616" s="174"/>
+      <c r="D616" s="167"/>
+      <c r="E616" s="160"/>
+      <c r="F616" s="151"/>
+      <c r="G616" s="190"/>
+      <c r="H616" s="204"/>
+      <c r="I616" s="177"/>
     </row>
     <row r="617" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A617" s="1"/>
       <c r="B617" s="109"/>
-      <c r="C617" s="227" t="s">
-        <v>153</v>
-      </c>
-      <c r="D617" s="135"/>
-      <c r="E617" s="154"/>
-      <c r="F617" s="147"/>
-      <c r="G617" s="185"/>
-      <c r="H617" s="200"/>
-      <c r="I617" s="173"/>
+      <c r="C617" s="110"/>
+      <c r="D617" s="167"/>
+      <c r="E617" s="160"/>
+      <c r="F617" s="151"/>
+      <c r="G617" s="190"/>
+      <c r="H617" s="204"/>
+      <c r="I617" s="177"/>
     </row>
     <row r="618" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A618" s="1"/>
       <c r="B618" s="109"/>
-      <c r="C618" s="227"/>
-      <c r="D618" s="165"/>
-      <c r="E618" s="155"/>
-      <c r="F618" s="148"/>
-      <c r="G618" s="186"/>
-      <c r="H618" s="201"/>
-      <c r="I618" s="174"/>
+      <c r="C618" s="110"/>
+      <c r="D618" s="167"/>
+      <c r="E618" s="160"/>
+      <c r="F618" s="151"/>
+      <c r="G618" s="190"/>
+      <c r="H618" s="204"/>
+      <c r="I618" s="177"/>
     </row>
     <row r="619" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A619" s="1"/>
       <c r="B619" s="109"/>
       <c r="C619" s="110"/>
-      <c r="D619" s="166"/>
-      <c r="E619" s="162"/>
-      <c r="F619" s="150"/>
-      <c r="G619" s="188"/>
-      <c r="H619" s="203"/>
-      <c r="I619" s="171"/>
-    </row>
-    <row r="620" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D619" s="167"/>
+      <c r="E619" s="160"/>
+      <c r="F619" s="151"/>
+      <c r="G619" s="190"/>
+      <c r="H619" s="204"/>
+      <c r="I619" s="177"/>
+    </row>
+    <row r="620" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A620" s="1"/>
       <c r="B620" s="109"/>
       <c r="C620" s="110"/>
-      <c r="D620" s="166" t="s">
-        <v>1237</v>
-      </c>
-      <c r="E620" s="162" t="s">
-        <v>1239</v>
-      </c>
-      <c r="F620" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G620" s="188">
-        <v>45156</v>
-      </c>
-      <c r="H620" s="203">
-        <v>44525</v>
-      </c>
-      <c r="I620" s="171" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="621" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D620" s="165"/>
+      <c r="E620" s="155"/>
+      <c r="F620" s="148"/>
+      <c r="G620" s="186"/>
+      <c r="H620" s="201"/>
+      <c r="I620" s="174"/>
+    </row>
+    <row r="621" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A621" s="1"/>
       <c r="B621" s="109"/>
-      <c r="C621" s="110"/>
-      <c r="D621" s="167" t="s">
-        <v>1238</v>
-      </c>
-      <c r="E621" s="160" t="s">
-        <v>1240</v>
-      </c>
-      <c r="F621" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G621" s="190">
-        <v>45156</v>
-      </c>
-      <c r="H621" s="204">
-        <v>44525</v>
-      </c>
-      <c r="I621" s="183" t="s">
-        <v>724</v>
-      </c>
+      <c r="C621" s="227" t="s">
+        <v>153</v>
+      </c>
+      <c r="D621" s="135"/>
+      <c r="E621" s="154"/>
+      <c r="F621" s="147"/>
+      <c r="G621" s="185"/>
+      <c r="H621" s="200"/>
+      <c r="I621" s="173"/>
     </row>
     <row r="622" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A622" s="1"/>
       <c r="B622" s="109"/>
-      <c r="C622" s="110"/>
+      <c r="C622" s="227"/>
       <c r="D622" s="165"/>
       <c r="E622" s="155"/>
       <c r="F622" s="148"/>
@@ -18561,37 +18609,59 @@
     <row r="623" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A623" s="1"/>
       <c r="B623" s="109"/>
-      <c r="C623" s="227" t="s">
-        <v>154</v>
-      </c>
-      <c r="D623" s="135"/>
-      <c r="E623" s="154"/>
-      <c r="F623" s="147"/>
-      <c r="G623" s="185"/>
-      <c r="H623" s="200"/>
-      <c r="I623" s="173"/>
-    </row>
-    <row r="624" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C623" s="110"/>
+      <c r="D623" s="166"/>
+      <c r="E623" s="162"/>
+      <c r="F623" s="150"/>
+      <c r="G623" s="188"/>
+      <c r="H623" s="203"/>
+      <c r="I623" s="171"/>
+    </row>
+    <row r="624" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A624" s="1"/>
       <c r="B624" s="109"/>
-      <c r="C624" s="227"/>
-      <c r="D624" s="165"/>
-      <c r="E624" s="155"/>
-      <c r="F624" s="148"/>
-      <c r="G624" s="186"/>
-      <c r="H624" s="201"/>
-      <c r="I624" s="174"/>
-    </row>
-    <row r="625" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C624" s="110"/>
+      <c r="D624" s="166" t="s">
+        <v>1237</v>
+      </c>
+      <c r="E624" s="162" t="s">
+        <v>1239</v>
+      </c>
+      <c r="F624" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G624" s="188">
+        <v>45156</v>
+      </c>
+      <c r="H624" s="203">
+        <v>44525</v>
+      </c>
+      <c r="I624" s="171" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="625" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A625" s="1"/>
       <c r="B625" s="109"/>
       <c r="C625" s="110"/>
-      <c r="D625" s="166"/>
-      <c r="E625" s="162"/>
-      <c r="F625" s="150"/>
-      <c r="G625" s="188"/>
-      <c r="H625" s="203"/>
-      <c r="I625" s="176"/>
+      <c r="D625" s="167" t="s">
+        <v>1238</v>
+      </c>
+      <c r="E625" s="160" t="s">
+        <v>1240</v>
+      </c>
+      <c r="F625" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G625" s="190">
+        <v>45156</v>
+      </c>
+      <c r="H625" s="204">
+        <v>44525</v>
+      </c>
+      <c r="I625" s="183" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="626" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A626" s="1"/>
@@ -18608,7 +18678,7 @@
       <c r="A627" s="1"/>
       <c r="B627" s="109"/>
       <c r="C627" s="227" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D627" s="135"/>
       <c r="E627" s="154"/>
@@ -18632,63 +18702,41 @@
       <c r="A629" s="1"/>
       <c r="B629" s="109"/>
       <c r="C629" s="110"/>
-      <c r="D629" s="165"/>
-      <c r="E629" s="155"/>
-      <c r="F629" s="148"/>
-      <c r="G629" s="186"/>
-      <c r="H629" s="201"/>
-      <c r="I629" s="174"/>
-    </row>
-    <row r="630" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D629" s="166"/>
+      <c r="E629" s="162"/>
+      <c r="F629" s="150"/>
+      <c r="G629" s="188"/>
+      <c r="H629" s="203"/>
+      <c r="I629" s="176"/>
+    </row>
+    <row r="630" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A630" s="1"/>
       <c r="B630" s="109"/>
       <c r="C630" s="110"/>
-      <c r="D630" s="167" t="s">
-        <v>1088</v>
-      </c>
-      <c r="E630" s="160" t="s">
-        <v>1090</v>
-      </c>
-      <c r="F630" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G630" s="190">
-        <v>45071</v>
-      </c>
-      <c r="H630" s="204">
-        <v>45071</v>
-      </c>
-      <c r="I630" s="183" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="631" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D630" s="165"/>
+      <c r="E630" s="155"/>
+      <c r="F630" s="148"/>
+      <c r="G630" s="186"/>
+      <c r="H630" s="201"/>
+      <c r="I630" s="174"/>
+    </row>
+    <row r="631" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A631" s="1"/>
       <c r="B631" s="109"/>
-      <c r="C631" s="110"/>
-      <c r="D631" s="166" t="s">
-        <v>1089</v>
-      </c>
-      <c r="E631" s="162" t="s">
-        <v>1091</v>
-      </c>
-      <c r="F631" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G631" s="188">
-        <v>45071</v>
-      </c>
-      <c r="H631" s="203">
-        <v>45071</v>
-      </c>
-      <c r="I631" s="171" t="s">
-        <v>724</v>
-      </c>
+      <c r="C631" s="227" t="s">
+        <v>155</v>
+      </c>
+      <c r="D631" s="135"/>
+      <c r="E631" s="154"/>
+      <c r="F631" s="147"/>
+      <c r="G631" s="185"/>
+      <c r="H631" s="200"/>
+      <c r="I631" s="173"/>
     </row>
     <row r="632" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A632" s="1"/>
       <c r="B632" s="109"/>
-      <c r="C632" s="110"/>
+      <c r="C632" s="227"/>
       <c r="D632" s="165"/>
       <c r="E632" s="155"/>
       <c r="F632" s="148"/>
@@ -18699,84 +18747,94 @@
     <row r="633" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A633" s="1"/>
       <c r="B633" s="109"/>
-      <c r="C633" s="227" t="s">
-        <v>156</v>
-      </c>
-      <c r="D633" s="135"/>
-      <c r="E633" s="154"/>
-      <c r="F633" s="147"/>
-      <c r="G633" s="185"/>
-      <c r="H633" s="200"/>
-      <c r="I633" s="173"/>
-    </row>
-    <row r="634" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C633" s="110"/>
+      <c r="D633" s="165"/>
+      <c r="E633" s="155"/>
+      <c r="F633" s="148"/>
+      <c r="G633" s="186"/>
+      <c r="H633" s="201"/>
+      <c r="I633" s="174"/>
+    </row>
+    <row r="634" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A634" s="1"/>
       <c r="B634" s="109"/>
-      <c r="C634" s="227"/>
-      <c r="D634" s="165"/>
-      <c r="E634" s="155"/>
-      <c r="F634" s="148"/>
-      <c r="G634" s="186"/>
-      <c r="H634" s="201"/>
-      <c r="I634" s="174"/>
-    </row>
-    <row r="635" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C634" s="110"/>
+      <c r="D634" s="167" t="s">
+        <v>1088</v>
+      </c>
+      <c r="E634" s="160" t="s">
+        <v>1090</v>
+      </c>
+      <c r="F634" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G634" s="190">
+        <v>45071</v>
+      </c>
+      <c r="H634" s="204">
+        <v>45071</v>
+      </c>
+      <c r="I634" s="183" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="635" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A635" s="1"/>
       <c r="B635" s="109"/>
       <c r="C635" s="110"/>
-      <c r="D635" s="165"/>
-      <c r="E635" s="155"/>
-      <c r="F635" s="148"/>
-      <c r="G635" s="186"/>
-      <c r="H635" s="201"/>
-      <c r="I635" s="174"/>
+      <c r="D635" s="166" t="s">
+        <v>1089</v>
+      </c>
+      <c r="E635" s="162" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F635" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G635" s="188">
+        <v>45071</v>
+      </c>
+      <c r="H635" s="203">
+        <v>45071</v>
+      </c>
+      <c r="I635" s="171" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="636" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A636" s="1"/>
       <c r="B636" s="109"/>
-      <c r="C636" s="227" t="s">
-        <v>157</v>
-      </c>
-      <c r="D636" s="135"/>
-      <c r="E636" s="154"/>
-      <c r="F636" s="147"/>
-      <c r="G636" s="185"/>
-      <c r="H636" s="200"/>
-      <c r="I636" s="173"/>
+      <c r="C636" s="110"/>
+      <c r="D636" s="165"/>
+      <c r="E636" s="155"/>
+      <c r="F636" s="148"/>
+      <c r="G636" s="186"/>
+      <c r="H636" s="201"/>
+      <c r="I636" s="174"/>
     </row>
     <row r="637" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A637" s="1"/>
       <c r="B637" s="109"/>
-      <c r="C637" s="227"/>
-      <c r="D637" s="165"/>
-      <c r="E637" s="155"/>
-      <c r="F637" s="148"/>
-      <c r="G637" s="186"/>
-      <c r="H637" s="201"/>
-      <c r="I637" s="174"/>
-    </row>
-    <row r="638" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="C637" s="227" t="s">
+        <v>156</v>
+      </c>
+      <c r="D637" s="135"/>
+      <c r="E637" s="154"/>
+      <c r="F637" s="147"/>
+      <c r="G637" s="185"/>
+      <c r="H637" s="200"/>
+      <c r="I637" s="173"/>
+    </row>
+    <row r="638" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A638" s="1"/>
       <c r="B638" s="109"/>
-      <c r="C638" s="110"/>
-      <c r="D638" s="166" t="s">
-        <v>694</v>
-      </c>
-      <c r="E638" s="157" t="s">
-        <v>695</v>
-      </c>
-      <c r="F638" s="150" t="s">
-        <v>696</v>
-      </c>
-      <c r="G638" s="188">
-        <v>44859</v>
-      </c>
-      <c r="H638" s="203">
-        <v>44477</v>
-      </c>
-      <c r="I638" s="171" t="s">
-        <v>697</v>
-      </c>
+      <c r="C638" s="227"/>
+      <c r="D638" s="165"/>
+      <c r="E638" s="155"/>
+      <c r="F638" s="148"/>
+      <c r="G638" s="186"/>
+      <c r="H638" s="201"/>
+      <c r="I638" s="174"/>
     </row>
     <row r="639" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A639" s="1"/>
@@ -18793,7 +18851,7 @@
       <c r="A640" s="1"/>
       <c r="B640" s="109"/>
       <c r="C640" s="227" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D640" s="135"/>
       <c r="E640" s="154"/>
@@ -18806,114 +18864,80 @@
       <c r="A641" s="1"/>
       <c r="B641" s="109"/>
       <c r="C641" s="227"/>
-      <c r="D641" s="166" t="s">
-        <v>466</v>
-      </c>
-      <c r="E641" s="162" t="s">
-        <v>467</v>
-      </c>
-      <c r="F641" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G641" s="188">
-        <v>44663</v>
-      </c>
-      <c r="H641" s="203">
-        <v>44663</v>
-      </c>
-      <c r="I641" s="198" t="s">
-        <v>756</v>
-      </c>
-    </row>
-    <row r="642" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D641" s="165"/>
+      <c r="E641" s="155"/>
+      <c r="F641" s="148"/>
+      <c r="G641" s="186"/>
+      <c r="H641" s="201"/>
+      <c r="I641" s="174"/>
+    </row>
+    <row r="642" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A642" s="1"/>
       <c r="B642" s="109"/>
       <c r="C642" s="110"/>
-      <c r="D642" s="167" t="s">
-        <v>468</v>
-      </c>
-      <c r="E642" s="160" t="s">
-        <v>469</v>
-      </c>
-      <c r="F642" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G642" s="190">
-        <v>44663</v>
-      </c>
-      <c r="H642" s="204">
-        <v>44663</v>
-      </c>
-      <c r="I642" s="199" t="s">
-        <v>756</v>
+      <c r="D642" s="166" t="s">
+        <v>694</v>
+      </c>
+      <c r="E642" s="157" t="s">
+        <v>695</v>
+      </c>
+      <c r="F642" s="150" t="s">
+        <v>696</v>
+      </c>
+      <c r="G642" s="188">
+        <v>44859</v>
+      </c>
+      <c r="H642" s="203">
+        <v>44477</v>
+      </c>
+      <c r="I642" s="171" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="643" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A643" s="1"/>
       <c r="B643" s="109"/>
       <c r="C643" s="110"/>
-      <c r="D643" s="167" t="s">
-        <v>471</v>
-      </c>
-      <c r="E643" s="160" t="s">
-        <v>470</v>
-      </c>
-      <c r="F643" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G643" s="190">
-        <v>44630</v>
-      </c>
-      <c r="H643" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I643" s="199" t="s">
-        <v>756</v>
-      </c>
+      <c r="D643" s="165"/>
+      <c r="E643" s="155"/>
+      <c r="F643" s="148"/>
+      <c r="G643" s="186"/>
+      <c r="H643" s="201"/>
+      <c r="I643" s="174"/>
     </row>
     <row r="644" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A644" s="1"/>
       <c r="B644" s="109"/>
-      <c r="C644" s="110"/>
-      <c r="D644" s="167" t="s">
-        <v>472</v>
-      </c>
-      <c r="E644" s="160" t="s">
-        <v>473</v>
-      </c>
-      <c r="F644" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G644" s="190">
-        <v>44630</v>
-      </c>
-      <c r="H644" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I644" s="199" t="s">
-        <v>756</v>
-      </c>
+      <c r="C644" s="227" t="s">
+        <v>158</v>
+      </c>
+      <c r="D644" s="135"/>
+      <c r="E644" s="154"/>
+      <c r="F644" s="147"/>
+      <c r="G644" s="185"/>
+      <c r="H644" s="200"/>
+      <c r="I644" s="173"/>
     </row>
     <row r="645" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A645" s="1"/>
       <c r="B645" s="109"/>
-      <c r="C645" s="110"/>
-      <c r="D645" s="167" t="s">
-        <v>474</v>
-      </c>
-      <c r="E645" s="160" t="s">
-        <v>475</v>
-      </c>
-      <c r="F645" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G645" s="190">
-        <v>44698</v>
-      </c>
-      <c r="H645" s="204">
-        <v>44630</v>
-      </c>
-      <c r="I645" s="199" t="s">
+      <c r="C645" s="227"/>
+      <c r="D645" s="166" t="s">
+        <v>466</v>
+      </c>
+      <c r="E645" s="162" t="s">
+        <v>467</v>
+      </c>
+      <c r="F645" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G645" s="188">
+        <v>44663</v>
+      </c>
+      <c r="H645" s="203">
+        <v>44663</v>
+      </c>
+      <c r="I645" s="198" t="s">
         <v>756</v>
       </c>
     </row>
@@ -18922,19 +18946,19 @@
       <c r="B646" s="109"/>
       <c r="C646" s="110"/>
       <c r="D646" s="167" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="E646" s="160" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="F646" s="151" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
       <c r="G646" s="190">
-        <v>44698</v>
+        <v>44663</v>
       </c>
       <c r="H646" s="204">
-        <v>44630</v>
+        <v>44663</v>
       </c>
       <c r="I646" s="199" t="s">
         <v>756</v>
@@ -18945,19 +18969,19 @@
       <c r="B647" s="109"/>
       <c r="C647" s="110"/>
       <c r="D647" s="167" t="s">
-        <v>490</v>
+        <v>471</v>
       </c>
       <c r="E647" s="160" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="F647" s="151" t="s">
-        <v>492</v>
+        <v>232</v>
       </c>
       <c r="G647" s="190">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H647" s="204">
-        <v>44621</v>
+        <v>44630</v>
       </c>
       <c r="I647" s="199" t="s">
         <v>756</v>
@@ -18968,19 +18992,19 @@
       <c r="B648" s="109"/>
       <c r="C648" s="110"/>
       <c r="D648" s="167" t="s">
-        <v>494</v>
+        <v>472</v>
       </c>
       <c r="E648" s="160" t="s">
-        <v>493</v>
+        <v>473</v>
       </c>
       <c r="F648" s="151" t="s">
-        <v>492</v>
+        <v>232</v>
       </c>
       <c r="G648" s="190">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H648" s="204">
-        <v>44621</v>
+        <v>44630</v>
       </c>
       <c r="I648" s="199" t="s">
         <v>756</v>
@@ -18991,19 +19015,19 @@
       <c r="B649" s="109"/>
       <c r="C649" s="110"/>
       <c r="D649" s="167" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="E649" s="160" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F649" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G649" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H649" s="204">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I649" s="199" t="s">
         <v>756</v>
@@ -19014,19 +19038,19 @@
       <c r="B650" s="109"/>
       <c r="C650" s="110"/>
       <c r="D650" s="167" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="E650" s="160" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="F650" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G650" s="190">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H650" s="204">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I650" s="199" t="s">
         <v>756</v>
@@ -19037,19 +19061,19 @@
       <c r="B651" s="109"/>
       <c r="C651" s="110"/>
       <c r="D651" s="167" t="s">
-        <v>482</v>
+        <v>490</v>
       </c>
       <c r="E651" s="160" t="s">
-        <v>483</v>
+        <v>491</v>
       </c>
       <c r="F651" s="151" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="G651" s="190">
-        <v>44733</v>
+        <v>44698</v>
       </c>
       <c r="H651" s="204">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="I651" s="199" t="s">
         <v>756</v>
@@ -19060,16 +19084,16 @@
       <c r="B652" s="109"/>
       <c r="C652" s="110"/>
       <c r="D652" s="167" t="s">
-        <v>484</v>
+        <v>494</v>
       </c>
       <c r="E652" s="160" t="s">
-        <v>485</v>
+        <v>493</v>
       </c>
       <c r="F652" s="151" t="s">
-        <v>459</v>
+        <v>492</v>
       </c>
       <c r="G652" s="190">
-        <v>44733</v>
+        <v>44698</v>
       </c>
       <c r="H652" s="204">
         <v>44621</v>
@@ -19083,19 +19107,19 @@
       <c r="B653" s="109"/>
       <c r="C653" s="110"/>
       <c r="D653" s="167" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E653" s="160" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="F653" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G653" s="190">
-        <v>44671</v>
+        <v>44669</v>
       </c>
       <c r="H653" s="204">
-        <v>44732</v>
+        <v>44824</v>
       </c>
       <c r="I653" s="199" t="s">
         <v>756</v>
@@ -19106,19 +19130,19 @@
       <c r="B654" s="109"/>
       <c r="C654" s="110"/>
       <c r="D654" s="167" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
       <c r="E654" s="160" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="F654" s="151" t="s">
-        <v>459</v>
+        <v>256</v>
       </c>
       <c r="G654" s="190">
-        <v>44671</v>
+        <v>44669</v>
       </c>
       <c r="H654" s="204">
-        <v>44732</v>
+        <v>44824</v>
       </c>
       <c r="I654" s="199" t="s">
         <v>756</v>
@@ -19129,19 +19153,19 @@
       <c r="B655" s="109"/>
       <c r="C655" s="110"/>
       <c r="D655" s="167" t="s">
-        <v>965</v>
+        <v>482</v>
       </c>
       <c r="E655" s="160" t="s">
-        <v>967</v>
+        <v>483</v>
       </c>
       <c r="F655" s="151" t="s">
-        <v>232</v>
+        <v>459</v>
       </c>
       <c r="G655" s="190">
-        <v>45048</v>
+        <v>44733</v>
       </c>
       <c r="H655" s="204">
-        <v>45048</v>
+        <v>44622</v>
       </c>
       <c r="I655" s="199" t="s">
         <v>756</v>
@@ -19152,19 +19176,19 @@
       <c r="B656" s="109"/>
       <c r="C656" s="110"/>
       <c r="D656" s="167" t="s">
-        <v>966</v>
+        <v>484</v>
       </c>
       <c r="E656" s="160" t="s">
-        <v>968</v>
+        <v>485</v>
       </c>
       <c r="F656" s="151" t="s">
-        <v>232</v>
+        <v>459</v>
       </c>
       <c r="G656" s="190">
-        <v>45048</v>
+        <v>44733</v>
       </c>
       <c r="H656" s="204">
-        <v>45048</v>
+        <v>44621</v>
       </c>
       <c r="I656" s="199" t="s">
         <v>756</v>
@@ -19175,19 +19199,19 @@
       <c r="B657" s="109"/>
       <c r="C657" s="110"/>
       <c r="D657" s="167" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="E657" s="160" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="F657" s="151" t="s">
-        <v>547</v>
+        <v>459</v>
       </c>
       <c r="G657" s="190">
-        <v>45145</v>
+        <v>44671</v>
       </c>
       <c r="H657" s="204">
-        <v>44622</v>
+        <v>44732</v>
       </c>
       <c r="I657" s="199" t="s">
         <v>756</v>
@@ -19198,19 +19222,19 @@
       <c r="B658" s="109"/>
       <c r="C658" s="110"/>
       <c r="D658" s="167" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="E658" s="160" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="F658" s="151" t="s">
-        <v>547</v>
+        <v>459</v>
       </c>
       <c r="G658" s="190">
-        <v>45145</v>
+        <v>44671</v>
       </c>
       <c r="H658" s="204">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I658" s="199" t="s">
         <v>756</v>
@@ -19221,19 +19245,19 @@
       <c r="B659" s="109"/>
       <c r="C659" s="110"/>
       <c r="D659" s="167" t="s">
-        <v>500</v>
+        <v>965</v>
       </c>
       <c r="E659" s="160" t="s">
-        <v>499</v>
+        <v>967</v>
       </c>
       <c r="F659" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G659" s="190">
-        <v>44698</v>
+        <v>45048</v>
       </c>
       <c r="H659" s="204">
-        <v>44621</v>
+        <v>45048</v>
       </c>
       <c r="I659" s="199" t="s">
         <v>756</v>
@@ -19244,19 +19268,19 @@
       <c r="B660" s="109"/>
       <c r="C660" s="110"/>
       <c r="D660" s="167" t="s">
-        <v>501</v>
+        <v>966</v>
       </c>
       <c r="E660" s="160" t="s">
-        <v>502</v>
+        <v>968</v>
       </c>
       <c r="F660" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G660" s="190">
-        <v>44698</v>
+        <v>45048</v>
       </c>
       <c r="H660" s="204">
-        <v>44621</v>
+        <v>45048</v>
       </c>
       <c r="I660" s="199" t="s">
         <v>756</v>
@@ -19267,19 +19291,19 @@
       <c r="B661" s="109"/>
       <c r="C661" s="110"/>
       <c r="D661" s="167" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="E661" s="160" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="F661" s="151" t="s">
-        <v>267</v>
+        <v>547</v>
       </c>
       <c r="G661" s="190">
-        <v>44846</v>
+        <v>45145</v>
       </c>
       <c r="H661" s="204">
-        <v>44627</v>
+        <v>44622</v>
       </c>
       <c r="I661" s="199" t="s">
         <v>756</v>
@@ -19290,19 +19314,19 @@
       <c r="B662" s="109"/>
       <c r="C662" s="110"/>
       <c r="D662" s="167" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="E662" s="160" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="F662" s="151" t="s">
-        <v>267</v>
+        <v>547</v>
       </c>
       <c r="G662" s="190">
-        <v>44846</v>
+        <v>45145</v>
       </c>
       <c r="H662" s="204">
-        <v>44627</v>
+        <v>44621</v>
       </c>
       <c r="I662" s="199" t="s">
         <v>756</v>
@@ -19313,19 +19337,19 @@
       <c r="B663" s="109"/>
       <c r="C663" s="110"/>
       <c r="D663" s="167" t="s">
-        <v>507</v>
+        <v>500</v>
       </c>
       <c r="E663" s="160" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="F663" s="151" t="s">
-        <v>232</v>
+        <v>459</v>
       </c>
       <c r="G663" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H663" s="204">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I663" s="199" t="s">
         <v>756</v>
@@ -19336,19 +19360,19 @@
       <c r="B664" s="109"/>
       <c r="C664" s="110"/>
       <c r="D664" s="167" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="E664" s="160" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="F664" s="151" t="s">
-        <v>232</v>
+        <v>459</v>
       </c>
       <c r="G664" s="190">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H664" s="204">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I664" s="199" t="s">
         <v>756</v>
@@ -19359,19 +19383,19 @@
       <c r="B665" s="109"/>
       <c r="C665" s="110"/>
       <c r="D665" s="167" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="E665" s="160" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="F665" s="151" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G665" s="190">
-        <v>44698</v>
+        <v>44846</v>
       </c>
       <c r="H665" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I665" s="199" t="s">
         <v>756</v>
@@ -19382,19 +19406,19 @@
       <c r="B666" s="109"/>
       <c r="C666" s="110"/>
       <c r="D666" s="167" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="E666" s="160" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="F666" s="151" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="G666" s="190">
-        <v>44698</v>
+        <v>44846</v>
       </c>
       <c r="H666" s="204">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I666" s="199" t="s">
         <v>756</v>
@@ -19405,10 +19429,10 @@
       <c r="B667" s="109"/>
       <c r="C667" s="110"/>
       <c r="D667" s="167" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="E667" s="160" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="F667" s="151" t="s">
         <v>232</v>
@@ -19428,10 +19452,10 @@
       <c r="B668" s="109"/>
       <c r="C668" s="110"/>
       <c r="D668" s="167" t="s">
-        <v>516</v>
+        <v>509</v>
       </c>
       <c r="E668" s="160" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="F668" s="151" t="s">
         <v>232</v>
@@ -19451,10 +19475,10 @@
       <c r="B669" s="109"/>
       <c r="C669" s="110"/>
       <c r="D669" s="167" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="E669" s="160" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="F669" s="151" t="s">
         <v>281</v>
@@ -19474,10 +19498,10 @@
       <c r="B670" s="109"/>
       <c r="C670" s="110"/>
       <c r="D670" s="167" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="E670" s="160" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="F670" s="151" t="s">
         <v>281</v>
@@ -19497,19 +19521,19 @@
       <c r="B671" s="109"/>
       <c r="C671" s="110"/>
       <c r="D671" s="167" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="E671" s="160" t="s">
-        <v>524</v>
+        <v>517</v>
       </c>
       <c r="F671" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G671" s="190">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="H671" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I671" s="199" t="s">
         <v>756</v>
@@ -19520,19 +19544,19 @@
       <c r="B672" s="109"/>
       <c r="C672" s="110"/>
       <c r="D672" s="167" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="E672" s="160" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
       <c r="F672" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G672" s="190">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="H672" s="204">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I672" s="199" t="s">
         <v>756</v>
@@ -19543,19 +19567,19 @@
       <c r="B673" s="109"/>
       <c r="C673" s="110"/>
       <c r="D673" s="167" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="E673" s="160" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="F673" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G673" s="190">
-        <v>44740</v>
+        <v>44698</v>
       </c>
       <c r="H673" s="204">
-        <v>44662</v>
+        <v>44628</v>
       </c>
       <c r="I673" s="199" t="s">
         <v>756</v>
@@ -19566,19 +19590,19 @@
       <c r="B674" s="109"/>
       <c r="C674" s="110"/>
       <c r="D674" s="167" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="E674" s="160" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
       <c r="F674" s="151" t="s">
-        <v>256</v>
+        <v>281</v>
       </c>
       <c r="G674" s="190">
-        <v>44740</v>
+        <v>44698</v>
       </c>
       <c r="H674" s="204">
-        <v>44662</v>
+        <v>44628</v>
       </c>
       <c r="I674" s="199" t="s">
         <v>756</v>
@@ -19588,152 +19612,178 @@
       <c r="A675" s="1"/>
       <c r="B675" s="109"/>
       <c r="C675" s="110"/>
-      <c r="D675" s="165"/>
-      <c r="E675" s="155"/>
-      <c r="F675" s="148"/>
-      <c r="G675" s="186"/>
-      <c r="H675" s="201"/>
-      <c r="I675" s="174"/>
+      <c r="D675" s="167" t="s">
+        <v>523</v>
+      </c>
+      <c r="E675" s="160" t="s">
+        <v>524</v>
+      </c>
+      <c r="F675" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G675" s="190">
+        <v>44617</v>
+      </c>
+      <c r="H675" s="204">
+        <v>44617</v>
+      </c>
+      <c r="I675" s="199" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="676" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A676" s="1"/>
       <c r="B676" s="109"/>
-      <c r="C676" s="227" t="s">
-        <v>147</v>
-      </c>
-      <c r="D676" s="135"/>
-      <c r="E676" s="154"/>
-      <c r="F676" s="147"/>
-      <c r="G676" s="185"/>
-      <c r="H676" s="200"/>
-      <c r="I676" s="173"/>
+      <c r="C676" s="110"/>
+      <c r="D676" s="167" t="s">
+        <v>526</v>
+      </c>
+      <c r="E676" s="160" t="s">
+        <v>525</v>
+      </c>
+      <c r="F676" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G676" s="190">
+        <v>44617</v>
+      </c>
+      <c r="H676" s="204">
+        <v>44617</v>
+      </c>
+      <c r="I676" s="199" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="677" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A677" s="1"/>
       <c r="B677" s="109"/>
-      <c r="C677" s="227"/>
-      <c r="D677" s="166" t="s">
-        <v>274</v>
-      </c>
-      <c r="E677" s="162" t="s">
-        <v>444</v>
-      </c>
-      <c r="F677" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G677" s="188">
-        <v>44167</v>
-      </c>
-      <c r="H677" s="203">
-        <v>44167</v>
-      </c>
-      <c r="I677" s="176"/>
+      <c r="C677" s="110"/>
+      <c r="D677" s="167" t="s">
+        <v>527</v>
+      </c>
+      <c r="E677" s="160" t="s">
+        <v>528</v>
+      </c>
+      <c r="F677" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G677" s="190">
+        <v>44740</v>
+      </c>
+      <c r="H677" s="204">
+        <v>44662</v>
+      </c>
+      <c r="I677" s="199" t="s">
+        <v>756</v>
+      </c>
     </row>
     <row r="678" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A678" s="1"/>
       <c r="B678" s="109"/>
       <c r="C678" s="110"/>
       <c r="D678" s="167" t="s">
-        <v>445</v>
+        <v>530</v>
       </c>
       <c r="E678" s="160" t="s">
-        <v>446</v>
+        <v>529</v>
       </c>
       <c r="F678" s="151" t="s">
         <v>256</v>
       </c>
       <c r="G678" s="190">
-        <v>44575</v>
+        <v>44740</v>
       </c>
       <c r="H678" s="204">
-        <v>44167</v>
-      </c>
-      <c r="I678" s="177"/>
-    </row>
-    <row r="679" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>44662</v>
+      </c>
+      <c r="I678" s="199" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="679" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A679" s="1"/>
       <c r="B679" s="109"/>
       <c r="C679" s="110"/>
-      <c r="D679" s="167" t="s">
-        <v>448</v>
-      </c>
-      <c r="E679" s="158" t="s">
-        <v>447</v>
-      </c>
-      <c r="F679" s="151" t="s">
-        <v>281</v>
-      </c>
-      <c r="G679" s="190">
-        <v>44404</v>
-      </c>
-      <c r="H679" s="204">
-        <v>44404</v>
-      </c>
-      <c r="I679" s="177"/>
+      <c r="D679" s="165"/>
+      <c r="E679" s="155"/>
+      <c r="F679" s="148"/>
+      <c r="G679" s="186"/>
+      <c r="H679" s="201"/>
+      <c r="I679" s="174"/>
     </row>
     <row r="680" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A680" s="1"/>
       <c r="B680" s="109"/>
-      <c r="C680" s="110"/>
-      <c r="D680" s="165"/>
-      <c r="E680" s="155"/>
-      <c r="F680" s="148"/>
-      <c r="G680" s="186"/>
-      <c r="H680" s="201"/>
-      <c r="I680" s="174"/>
+      <c r="C680" s="227" t="s">
+        <v>147</v>
+      </c>
+      <c r="D680" s="135"/>
+      <c r="E680" s="154"/>
+      <c r="F680" s="147"/>
+      <c r="G680" s="185"/>
+      <c r="H680" s="200"/>
+      <c r="I680" s="173"/>
     </row>
     <row r="681" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A681" s="1"/>
       <c r="B681" s="109"/>
-      <c r="C681" s="227" t="s">
-        <v>159</v>
-      </c>
-      <c r="D681" s="135"/>
-      <c r="E681" s="154"/>
-      <c r="F681" s="147"/>
-      <c r="G681" s="185"/>
-      <c r="H681" s="200"/>
-      <c r="I681" s="173"/>
+      <c r="C681" s="227"/>
+      <c r="D681" s="166" t="s">
+        <v>274</v>
+      </c>
+      <c r="E681" s="162" t="s">
+        <v>444</v>
+      </c>
+      <c r="F681" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G681" s="188">
+        <v>44167</v>
+      </c>
+      <c r="H681" s="203">
+        <v>44167</v>
+      </c>
+      <c r="I681" s="176"/>
     </row>
     <row r="682" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A682" s="1"/>
       <c r="B682" s="109"/>
-      <c r="C682" s="227"/>
-      <c r="D682" s="166" t="s">
-        <v>450</v>
-      </c>
-      <c r="E682" s="162" t="s">
-        <v>449</v>
-      </c>
-      <c r="F682" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G682" s="188">
-        <v>44635</v>
-      </c>
-      <c r="H682" s="203">
-        <v>44635</v>
-      </c>
-      <c r="I682" s="176"/>
-    </row>
-    <row r="683" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C682" s="110"/>
+      <c r="D682" s="167" t="s">
+        <v>445</v>
+      </c>
+      <c r="E682" s="160" t="s">
+        <v>446</v>
+      </c>
+      <c r="F682" s="151" t="s">
+        <v>256</v>
+      </c>
+      <c r="G682" s="190">
+        <v>44575</v>
+      </c>
+      <c r="H682" s="204">
+        <v>44167</v>
+      </c>
+      <c r="I682" s="177"/>
+    </row>
+    <row r="683" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A683" s="1"/>
       <c r="B683" s="109"/>
       <c r="C683" s="110"/>
       <c r="D683" s="167" t="s">
-        <v>452</v>
-      </c>
-      <c r="E683" s="160" t="s">
-        <v>451</v>
+        <v>448</v>
+      </c>
+      <c r="E683" s="158" t="s">
+        <v>447</v>
       </c>
       <c r="F683" s="151" t="s">
-        <v>232</v>
+        <v>281</v>
       </c>
       <c r="G683" s="190">
-        <v>44635</v>
+        <v>44404</v>
       </c>
       <c r="H683" s="204">
-        <v>44635</v>
+        <v>44404</v>
       </c>
       <c r="I683" s="177"/>
     </row>
@@ -19741,83 +19791,65 @@
       <c r="A684" s="1"/>
       <c r="B684" s="109"/>
       <c r="C684" s="110"/>
-      <c r="D684" s="167" t="s">
-        <v>453</v>
-      </c>
-      <c r="E684" s="160" t="s">
-        <v>455</v>
-      </c>
-      <c r="F684" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G684" s="190">
-        <v>44635</v>
-      </c>
-      <c r="H684" s="204">
-        <v>44635</v>
-      </c>
-      <c r="I684" s="177"/>
+      <c r="D684" s="165"/>
+      <c r="E684" s="155"/>
+      <c r="F684" s="148"/>
+      <c r="G684" s="186"/>
+      <c r="H684" s="201"/>
+      <c r="I684" s="174"/>
     </row>
     <row r="685" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A685" s="1"/>
       <c r="B685" s="109"/>
-      <c r="C685" s="110"/>
-      <c r="D685" s="167" t="s">
-        <v>454</v>
-      </c>
-      <c r="E685" s="160" t="s">
-        <v>456</v>
-      </c>
-      <c r="F685" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G685" s="190">
-        <v>44635</v>
-      </c>
-      <c r="H685" s="204">
-        <v>44635</v>
-      </c>
-      <c r="I685" s="177"/>
+      <c r="C685" s="227" t="s">
+        <v>159</v>
+      </c>
+      <c r="D685" s="135"/>
+      <c r="E685" s="154"/>
+      <c r="F685" s="147"/>
+      <c r="G685" s="185"/>
+      <c r="H685" s="200"/>
+      <c r="I685" s="173"/>
     </row>
     <row r="686" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A686" s="1"/>
       <c r="B686" s="109"/>
-      <c r="C686" s="110"/>
-      <c r="D686" s="167" t="s">
-        <v>457</v>
-      </c>
-      <c r="E686" s="160" t="s">
-        <v>460</v>
-      </c>
-      <c r="F686" s="151" t="s">
-        <v>459</v>
-      </c>
-      <c r="G686" s="190">
-        <v>44701</v>
-      </c>
-      <c r="H686" s="204">
-        <v>44644</v>
-      </c>
-      <c r="I686" s="177"/>
+      <c r="C686" s="227"/>
+      <c r="D686" s="166" t="s">
+        <v>450</v>
+      </c>
+      <c r="E686" s="162" t="s">
+        <v>449</v>
+      </c>
+      <c r="F686" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G686" s="188">
+        <v>44635</v>
+      </c>
+      <c r="H686" s="203">
+        <v>44635</v>
+      </c>
+      <c r="I686" s="176"/>
     </row>
     <row r="687" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A687" s="1"/>
       <c r="B687" s="109"/>
       <c r="C687" s="110"/>
       <c r="D687" s="167" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
       <c r="E687" s="160" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
       <c r="F687" s="151" t="s">
-        <v>459</v>
+        <v>232</v>
       </c>
       <c r="G687" s="190">
-        <v>44701</v>
+        <v>44635</v>
       </c>
       <c r="H687" s="204">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="I687" s="177"/>
     </row>
@@ -19826,19 +19858,19 @@
       <c r="B688" s="109"/>
       <c r="C688" s="110"/>
       <c r="D688" s="167" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
       <c r="E688" s="160" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="F688" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G688" s="190">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H688" s="204">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="I688" s="177"/>
     </row>
@@ -19847,19 +19879,19 @@
       <c r="B689" s="109"/>
       <c r="C689" s="110"/>
       <c r="D689" s="167" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="E689" s="160" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="F689" s="151" t="s">
-        <v>267</v>
+        <v>232</v>
       </c>
       <c r="G689" s="190">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H689" s="204">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="I689" s="177"/>
     </row>
@@ -19867,49 +19899,85 @@
       <c r="A690" s="1"/>
       <c r="B690" s="109"/>
       <c r="C690" s="110"/>
-      <c r="D690" s="165"/>
-      <c r="E690" s="155"/>
-      <c r="F690" s="148"/>
-      <c r="G690" s="186"/>
-      <c r="H690" s="201"/>
-      <c r="I690" s="174"/>
-    </row>
-    <row r="691" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A691" s="136"/>
-      <c r="B691" s="226" t="s">
-        <v>144</v>
-      </c>
-      <c r="C691" s="134"/>
-      <c r="D691" s="135"/>
-      <c r="E691" s="154"/>
-      <c r="F691" s="147"/>
-      <c r="G691" s="185"/>
-      <c r="H691" s="200"/>
-      <c r="I691" s="173"/>
-    </row>
-    <row r="692" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A692" s="136"/>
-      <c r="B692" s="226"/>
-      <c r="C692" s="227" t="s">
-        <v>146</v>
-      </c>
-      <c r="D692" s="135"/>
-      <c r="E692" s="154"/>
-      <c r="F692" s="147"/>
-      <c r="G692" s="185"/>
-      <c r="H692" s="200"/>
-      <c r="I692" s="173"/>
+      <c r="D690" s="167" t="s">
+        <v>457</v>
+      </c>
+      <c r="E690" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="F690" s="151" t="s">
+        <v>459</v>
+      </c>
+      <c r="G690" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H690" s="204">
+        <v>44644</v>
+      </c>
+      <c r="I690" s="177"/>
+    </row>
+    <row r="691" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A691" s="1"/>
+      <c r="B691" s="109"/>
+      <c r="C691" s="110"/>
+      <c r="D691" s="167" t="s">
+        <v>458</v>
+      </c>
+      <c r="E691" s="160" t="s">
+        <v>461</v>
+      </c>
+      <c r="F691" s="151" t="s">
+        <v>459</v>
+      </c>
+      <c r="G691" s="190">
+        <v>44701</v>
+      </c>
+      <c r="H691" s="204">
+        <v>44644</v>
+      </c>
+      <c r="I691" s="177"/>
+    </row>
+    <row r="692" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A692" s="1"/>
+      <c r="B692" s="109"/>
+      <c r="C692" s="110"/>
+      <c r="D692" s="167" t="s">
+        <v>462</v>
+      </c>
+      <c r="E692" s="160" t="s">
+        <v>463</v>
+      </c>
+      <c r="F692" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G692" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H692" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I692" s="177"/>
     </row>
     <row r="693" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A693" s="1"/>
       <c r="B693" s="109"/>
-      <c r="C693" s="227"/>
-      <c r="D693" s="165"/>
-      <c r="E693" s="155"/>
-      <c r="F693" s="148"/>
-      <c r="G693" s="186"/>
-      <c r="H693" s="201"/>
-      <c r="I693" s="174"/>
+      <c r="C693" s="110"/>
+      <c r="D693" s="167" t="s">
+        <v>464</v>
+      </c>
+      <c r="E693" s="160" t="s">
+        <v>465</v>
+      </c>
+      <c r="F693" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G693" s="190">
+        <v>44644</v>
+      </c>
+      <c r="H693" s="204">
+        <v>44636</v>
+      </c>
+      <c r="I693" s="177"/>
     </row>
     <row r="694" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A694" s="1"/>
@@ -19922,138 +19990,106 @@
       <c r="H694" s="201"/>
       <c r="I694" s="174"/>
     </row>
-    <row r="695" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A695" s="1"/>
-      <c r="B695" s="109"/>
-      <c r="C695" s="110"/>
-      <c r="D695" s="144"/>
-      <c r="E695" s="156"/>
-      <c r="F695" s="149"/>
-      <c r="G695" s="187"/>
-      <c r="H695" s="202"/>
-      <c r="I695" s="175"/>
-    </row>
-    <row r="696" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="695" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A695" s="136"/>
+      <c r="B695" s="226" t="s">
+        <v>144</v>
+      </c>
+      <c r="C695" s="134"/>
+      <c r="D695" s="135"/>
+      <c r="E695" s="154"/>
+      <c r="F695" s="147"/>
+      <c r="G695" s="185"/>
+      <c r="H695" s="200"/>
+      <c r="I695" s="173"/>
+    </row>
+    <row r="696" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A696" s="136"/>
-      <c r="B696" s="109"/>
-      <c r="C696" s="110"/>
-      <c r="D696" s="166" t="s">
-        <v>855</v>
-      </c>
-      <c r="E696" s="162" t="s">
-        <v>857</v>
-      </c>
-      <c r="F696" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G696" s="188">
-        <v>44950</v>
-      </c>
-      <c r="H696" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I696" s="171" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="697" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A697" s="136"/>
+      <c r="B696" s="226"/>
+      <c r="C696" s="227" t="s">
+        <v>146</v>
+      </c>
+      <c r="D696" s="135"/>
+      <c r="E696" s="154"/>
+      <c r="F696" s="147"/>
+      <c r="G696" s="185"/>
+      <c r="H696" s="200"/>
+      <c r="I696" s="173"/>
+    </row>
+    <row r="697" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A697" s="1"/>
       <c r="B697" s="109"/>
-      <c r="C697" s="110"/>
-      <c r="D697" s="167" t="s">
-        <v>856</v>
-      </c>
-      <c r="E697" s="158" t="s">
-        <v>858</v>
-      </c>
-      <c r="F697" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G697" s="190">
-        <v>44950</v>
-      </c>
-      <c r="H697" s="204">
-        <v>44893</v>
-      </c>
-      <c r="I697" s="171" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="698" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A698" s="136"/>
+      <c r="C697" s="227"/>
+      <c r="D697" s="165"/>
+      <c r="E697" s="155"/>
+      <c r="F697" s="148"/>
+      <c r="G697" s="186"/>
+      <c r="H697" s="201"/>
+      <c r="I697" s="174"/>
+    </row>
+    <row r="698" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A698" s="1"/>
       <c r="B698" s="109"/>
       <c r="C698" s="110"/>
-      <c r="D698" s="166" t="s">
-        <v>859</v>
-      </c>
-      <c r="E698" s="157" t="s">
-        <v>861</v>
-      </c>
-      <c r="F698" s="150" t="s">
-        <v>547</v>
-      </c>
-      <c r="G698" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H698" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I698" s="171" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="699" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A699" s="136"/>
+      <c r="D698" s="165"/>
+      <c r="E698" s="155"/>
+      <c r="F698" s="148"/>
+      <c r="G698" s="186"/>
+      <c r="H698" s="201"/>
+      <c r="I698" s="174"/>
+    </row>
+    <row r="699" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A699" s="1"/>
       <c r="B699" s="109"/>
       <c r="C699" s="110"/>
-      <c r="D699" s="166" t="s">
-        <v>860</v>
-      </c>
-      <c r="E699" s="157" t="s">
-        <v>862</v>
-      </c>
-      <c r="F699" s="150" t="s">
-        <v>547</v>
-      </c>
-      <c r="G699" s="188">
-        <v>44970</v>
-      </c>
-      <c r="H699" s="203">
-        <v>44893</v>
-      </c>
-      <c r="I699" s="171" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="700" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D699" s="144"/>
+      <c r="E699" s="156"/>
+      <c r="F699" s="149"/>
+      <c r="G699" s="187"/>
+      <c r="H699" s="202"/>
+      <c r="I699" s="175"/>
+    </row>
+    <row r="700" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A700" s="136"/>
       <c r="B700" s="109"/>
       <c r="C700" s="110"/>
-      <c r="D700" s="166"/>
-      <c r="E700" s="157"/>
-      <c r="F700" s="150"/>
-      <c r="G700" s="188"/>
-      <c r="H700" s="203"/>
-      <c r="I700" s="171"/>
+      <c r="D700" s="166" t="s">
+        <v>855</v>
+      </c>
+      <c r="E700" s="162" t="s">
+        <v>857</v>
+      </c>
+      <c r="F700" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G700" s="188">
+        <v>44950</v>
+      </c>
+      <c r="H700" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I700" s="171" t="s">
+        <v>724</v>
+      </c>
     </row>
     <row r="701" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A701" s="136"/>
       <c r="B701" s="109"/>
       <c r="C701" s="110"/>
-      <c r="D701" s="166" t="s">
-        <v>931</v>
-      </c>
-      <c r="E701" s="157" t="s">
-        <v>933</v>
-      </c>
-      <c r="F701" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G701" s="188">
-        <v>45009</v>
-      </c>
-      <c r="H701" s="203">
-        <v>45009</v>
+      <c r="D701" s="167" t="s">
+        <v>856</v>
+      </c>
+      <c r="E701" s="158" t="s">
+        <v>858</v>
+      </c>
+      <c r="F701" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G701" s="190">
+        <v>44950</v>
+      </c>
+      <c r="H701" s="204">
+        <v>44893</v>
       </c>
       <c r="I701" s="171" t="s">
         <v>724</v>
@@ -20064,135 +20100,171 @@
       <c r="B702" s="109"/>
       <c r="C702" s="110"/>
       <c r="D702" s="166" t="s">
-        <v>930</v>
+        <v>859</v>
       </c>
       <c r="E702" s="157" t="s">
-        <v>932</v>
+        <v>861</v>
       </c>
       <c r="F702" s="150" t="s">
-        <v>232</v>
+        <v>547</v>
       </c>
       <c r="G702" s="188">
-        <v>45009</v>
+        <v>44970</v>
       </c>
       <c r="H702" s="203">
-        <v>45009</v>
+        <v>44893</v>
       </c>
       <c r="I702" s="171" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="703" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="703" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A703" s="136"/>
       <c r="B703" s="109"/>
       <c r="C703" s="110"/>
-      <c r="D703" s="166"/>
-      <c r="E703" s="157"/>
-      <c r="F703" s="150"/>
-      <c r="G703" s="188"/>
-      <c r="H703" s="203"/>
-      <c r="I703" s="171"/>
-    </row>
-    <row r="704" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D703" s="166" t="s">
+        <v>860</v>
+      </c>
+      <c r="E703" s="157" t="s">
+        <v>862</v>
+      </c>
+      <c r="F703" s="150" t="s">
+        <v>547</v>
+      </c>
+      <c r="G703" s="188">
+        <v>44970</v>
+      </c>
+      <c r="H703" s="203">
+        <v>44893</v>
+      </c>
+      <c r="I703" s="171" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="704" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A704" s="136"/>
       <c r="B704" s="109"/>
       <c r="C704" s="110"/>
-      <c r="D704" s="166" t="s">
-        <v>851</v>
-      </c>
-      <c r="E704" s="162" t="s">
-        <v>854</v>
-      </c>
-      <c r="F704" s="150" t="s">
-        <v>267</v>
-      </c>
-      <c r="G704" s="188">
-        <v>44986</v>
-      </c>
-      <c r="H704" s="203">
-        <v>44951</v>
-      </c>
-      <c r="I704" s="171" t="s">
-        <v>724</v>
-      </c>
+      <c r="D704" s="166"/>
+      <c r="E704" s="157"/>
+      <c r="F704" s="150"/>
+      <c r="G704" s="188"/>
+      <c r="H704" s="203"/>
+      <c r="I704" s="171"/>
     </row>
     <row r="705" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A705" s="136"/>
       <c r="B705" s="109"/>
       <c r="C705" s="110"/>
-      <c r="D705" s="167" t="s">
-        <v>852</v>
-      </c>
-      <c r="E705" s="158" t="s">
-        <v>853</v>
-      </c>
-      <c r="F705" s="151" t="s">
-        <v>267</v>
-      </c>
-      <c r="G705" s="190">
-        <v>44986</v>
-      </c>
-      <c r="H705" s="204">
-        <v>44951</v>
+      <c r="D705" s="166" t="s">
+        <v>931</v>
+      </c>
+      <c r="E705" s="157" t="s">
+        <v>933</v>
+      </c>
+      <c r="F705" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G705" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H705" s="203">
+        <v>45009</v>
       </c>
       <c r="I705" s="171" t="s">
         <v>724</v>
       </c>
     </row>
-    <row r="706" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="706" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A706" s="136"/>
-      <c r="B706" s="111"/>
-      <c r="C706" s="112"/>
-      <c r="D706" s="170"/>
-      <c r="E706" s="163"/>
-      <c r="F706" s="153"/>
-      <c r="G706" s="191"/>
-      <c r="H706" s="206"/>
-      <c r="I706" s="179"/>
-    </row>
-    <row r="707" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A707" s="1"/>
-      <c r="B707" s="1"/>
-      <c r="C707" s="1"/>
-      <c r="D707" s="1"/>
-      <c r="E707" s="146"/>
-      <c r="F707" s="113"/>
-      <c r="G707" s="192"/>
-      <c r="H707" s="192"/>
-      <c r="I707" s="180"/>
-    </row>
-    <row r="708" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A708" s="1"/>
-      <c r="B708" s="1"/>
-      <c r="C708" s="1"/>
-      <c r="D708" s="1"/>
-      <c r="E708" s="146"/>
-      <c r="F708" s="113"/>
-      <c r="G708" s="192"/>
-      <c r="H708" s="192"/>
-      <c r="I708" s="180"/>
-    </row>
-    <row r="709" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A709" s="1"/>
-      <c r="B709" s="1"/>
-      <c r="C709" s="1"/>
-      <c r="D709" s="1"/>
-      <c r="E709" s="146"/>
-      <c r="F709" s="113"/>
-      <c r="G709" s="192"/>
-      <c r="H709" s="192"/>
-      <c r="I709" s="180"/>
-    </row>
-    <row r="710" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A710" s="1"/>
-      <c r="B710" s="1"/>
-      <c r="C710" s="1"/>
-      <c r="D710" s="1"/>
-      <c r="E710" s="146"/>
-      <c r="F710" s="113"/>
-      <c r="G710" s="192"/>
-      <c r="H710" s="192"/>
-      <c r="I710" s="180"/>
+      <c r="B706" s="109"/>
+      <c r="C706" s="110"/>
+      <c r="D706" s="166" t="s">
+        <v>930</v>
+      </c>
+      <c r="E706" s="157" t="s">
+        <v>932</v>
+      </c>
+      <c r="F706" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G706" s="188">
+        <v>45009</v>
+      </c>
+      <c r="H706" s="203">
+        <v>45009</v>
+      </c>
+      <c r="I706" s="171" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="707" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A707" s="136"/>
+      <c r="B707" s="109"/>
+      <c r="C707" s="110"/>
+      <c r="D707" s="166"/>
+      <c r="E707" s="157"/>
+      <c r="F707" s="150"/>
+      <c r="G707" s="188"/>
+      <c r="H707" s="203"/>
+      <c r="I707" s="171"/>
+    </row>
+    <row r="708" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A708" s="136"/>
+      <c r="B708" s="109"/>
+      <c r="C708" s="110"/>
+      <c r="D708" s="166" t="s">
+        <v>851</v>
+      </c>
+      <c r="E708" s="162" t="s">
+        <v>854</v>
+      </c>
+      <c r="F708" s="150" t="s">
+        <v>267</v>
+      </c>
+      <c r="G708" s="188">
+        <v>44986</v>
+      </c>
+      <c r="H708" s="203">
+        <v>44951</v>
+      </c>
+      <c r="I708" s="171" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="709" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A709" s="136"/>
+      <c r="B709" s="109"/>
+      <c r="C709" s="110"/>
+      <c r="D709" s="167" t="s">
+        <v>852</v>
+      </c>
+      <c r="E709" s="158" t="s">
+        <v>853</v>
+      </c>
+      <c r="F709" s="151" t="s">
+        <v>267</v>
+      </c>
+      <c r="G709" s="190">
+        <v>44986</v>
+      </c>
+      <c r="H709" s="204">
+        <v>44951</v>
+      </c>
+      <c r="I709" s="171" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="710" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A710" s="136"/>
+      <c r="B710" s="111"/>
+      <c r="C710" s="112"/>
+      <c r="D710" s="170"/>
+      <c r="E710" s="163"/>
+      <c r="F710" s="153"/>
+      <c r="G710" s="191"/>
+      <c r="H710" s="206"/>
+      <c r="I710" s="179"/>
     </row>
     <row r="711" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A711" s="1"/>
@@ -20326,36 +20398,104 @@
       <c r="H722" s="192"/>
       <c r="I722" s="180"/>
     </row>
-    <row r="723" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E723" s="145"/>
-      <c r="F723" s="95"/>
-      <c r="G723" s="193"/>
-      <c r="H723" s="193"/>
-      <c r="I723" s="181"/>
-    </row>
-    <row r="724" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E724" s="145"/>
-      <c r="F724" s="95"/>
-      <c r="G724" s="193"/>
-      <c r="H724" s="193"/>
-      <c r="I724" s="181"/>
-    </row>
-    <row r="725" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E725" s="145"/>
-      <c r="F725" s="95"/>
-      <c r="G725" s="193"/>
-      <c r="H725" s="193"/>
-      <c r="I725" s="181"/>
+    <row r="723" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A723" s="1"/>
+      <c r="B723" s="1"/>
+      <c r="C723" s="1"/>
+      <c r="D723" s="1"/>
+      <c r="E723" s="146"/>
+      <c r="F723" s="113"/>
+      <c r="G723" s="192"/>
+      <c r="H723" s="192"/>
+      <c r="I723" s="180"/>
+    </row>
+    <row r="724" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A724" s="1"/>
+      <c r="B724" s="1"/>
+      <c r="C724" s="1"/>
+      <c r="D724" s="1"/>
+      <c r="E724" s="146"/>
+      <c r="F724" s="113"/>
+      <c r="G724" s="192"/>
+      <c r="H724" s="192"/>
+      <c r="I724" s="180"/>
+    </row>
+    <row r="725" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A725" s="1"/>
+      <c r="B725" s="1"/>
+      <c r="C725" s="1"/>
+      <c r="D725" s="1"/>
+      <c r="E725" s="146"/>
+      <c r="F725" s="113"/>
+      <c r="G725" s="192"/>
+      <c r="H725" s="192"/>
+      <c r="I725" s="180"/>
+    </row>
+    <row r="726" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A726" s="1"/>
+      <c r="B726" s="1"/>
+      <c r="C726" s="1"/>
+      <c r="D726" s="1"/>
+      <c r="E726" s="146"/>
+      <c r="F726" s="113"/>
+      <c r="G726" s="192"/>
+      <c r="H726" s="192"/>
+      <c r="I726" s="180"/>
+    </row>
+    <row r="727" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E727" s="145"/>
+      <c r="F727" s="95"/>
+      <c r="G727" s="193"/>
+      <c r="H727" s="193"/>
+      <c r="I727" s="181"/>
+    </row>
+    <row r="728" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E728" s="145"/>
+      <c r="F728" s="95"/>
+      <c r="G728" s="193"/>
+      <c r="H728" s="193"/>
+      <c r="I728" s="181"/>
+    </row>
+    <row r="729" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E729" s="145"/>
+      <c r="F729" s="95"/>
+      <c r="G729" s="193"/>
+      <c r="H729" s="193"/>
+      <c r="I729" s="181"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B691:B692"/>
-    <mergeCell ref="C692:C693"/>
+    <mergeCell ref="B576:B577"/>
+    <mergeCell ref="C577:C578"/>
+    <mergeCell ref="C296:C297"/>
+    <mergeCell ref="B572:B573"/>
+    <mergeCell ref="C573:C574"/>
+    <mergeCell ref="C416:C417"/>
+    <mergeCell ref="C566:C567"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C135:C136"/>
+    <mergeCell ref="C222:C223"/>
+    <mergeCell ref="C685:C686"/>
+    <mergeCell ref="C592:C593"/>
+    <mergeCell ref="C599:C600"/>
+    <mergeCell ref="C621:C622"/>
+    <mergeCell ref="C627:C628"/>
+    <mergeCell ref="C631:C632"/>
+    <mergeCell ref="C229:C230"/>
+    <mergeCell ref="C238:C239"/>
+    <mergeCell ref="C277:C278"/>
+    <mergeCell ref="C551:C552"/>
+    <mergeCell ref="B695:B696"/>
+    <mergeCell ref="C696:C697"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C633:C634"/>
-    <mergeCell ref="C636:C637"/>
+    <mergeCell ref="C637:C638"/>
     <mergeCell ref="C640:C641"/>
-    <mergeCell ref="C676:C677"/>
+    <mergeCell ref="C644:C645"/>
+    <mergeCell ref="C680:C681"/>
     <mergeCell ref="C580:C581"/>
     <mergeCell ref="C589:C590"/>
     <mergeCell ref="B2:D2"/>
@@ -20365,30 +20505,6 @@
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="C95:C96"/>
     <mergeCell ref="C110:C111"/>
-    <mergeCell ref="C135:C136"/>
-    <mergeCell ref="C222:C223"/>
-    <mergeCell ref="C681:C682"/>
-    <mergeCell ref="C592:C593"/>
-    <mergeCell ref="C595:C596"/>
-    <mergeCell ref="C617:C618"/>
-    <mergeCell ref="C623:C624"/>
-    <mergeCell ref="C627:C628"/>
-    <mergeCell ref="C229:C230"/>
-    <mergeCell ref="C238:C239"/>
-    <mergeCell ref="C277:C278"/>
-    <mergeCell ref="C551:C552"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B576:B577"/>
-    <mergeCell ref="C577:C578"/>
-    <mergeCell ref="C296:C297"/>
-    <mergeCell ref="B572:B573"/>
-    <mergeCell ref="C573:C574"/>
-    <mergeCell ref="C416:C417"/>
-    <mergeCell ref="C566:C567"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -20441,20 +20557,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="261" t="s">
+      <c r="B2" s="244" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="262"/>
-      <c r="D2" s="263"/>
-      <c r="E2" s="258" t="s">
+      <c r="C2" s="245"/>
+      <c r="D2" s="246"/>
+      <c r="E2" s="241" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="260"/>
-      <c r="G2" s="258" t="s">
+      <c r="F2" s="243"/>
+      <c r="G2" s="241" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="259"/>
-      <c r="I2" s="260"/>
+      <c r="H2" s="242"/>
+      <c r="I2" s="243"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -20475,10 +20591,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="264" t="s">
+      <c r="H3" s="247" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="265"/>
+      <c r="I3" s="248"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -20513,8 +20629,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="239"/>
-      <c r="I6" s="240"/>
+      <c r="H6" s="261"/>
+      <c r="I6" s="262"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -20556,7 +20672,7 @@
       <c r="F8" s="255" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="246" t="s">
+      <c r="G8" s="258" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -20572,11 +20688,11 @@
       <c r="D9" s="253"/>
       <c r="E9" s="35"/>
       <c r="F9" s="256"/>
-      <c r="G9" s="247"/>
-      <c r="H9" s="241" t="s">
+      <c r="G9" s="259"/>
+      <c r="H9" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="242"/>
+      <c r="I9" s="240"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -20584,7 +20700,7 @@
       <c r="D10" s="254"/>
       <c r="E10" s="36"/>
       <c r="F10" s="257"/>
-      <c r="G10" s="248"/>
+      <c r="G10" s="260"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -20624,13 +20740,13 @@
       <c r="D12" s="252" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="243" t="s">
+      <c r="E12" s="263" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="255" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="246" t="s">
+      <c r="G12" s="258" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -20645,22 +20761,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="250"/>
       <c r="D13" s="253"/>
-      <c r="E13" s="244"/>
+      <c r="E13" s="264"/>
       <c r="F13" s="256"/>
-      <c r="G13" s="247"/>
-      <c r="H13" s="241" t="s">
+      <c r="G13" s="259"/>
+      <c r="H13" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="242"/>
+      <c r="I13" s="240"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="251"/>
       <c r="D14" s="254"/>
-      <c r="E14" s="245"/>
+      <c r="E14" s="265"/>
       <c r="F14" s="257"/>
-      <c r="G14" s="248"/>
+      <c r="G14" s="260"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -20770,7 +20886,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="246" t="s">
+      <c r="G21" s="258" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -20790,7 +20906,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="248"/>
+      <c r="G22" s="260"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -20835,8 +20951,8 @@
       <c r="E25" s="25"/>
       <c r="F25" s="22"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="239"/>
-      <c r="I25" s="240"/>
+      <c r="H25" s="261"/>
+      <c r="I25" s="262"/>
     </row>
     <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="67" t="s">
@@ -21256,13 +21372,13 @@
       <c r="D49" s="252" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="243" t="s">
+      <c r="E49" s="263" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="255" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="246" t="s">
+      <c r="G49" s="258" t="s">
         <v>47</v>
       </c>
       <c r="H49" s="6" t="s">
@@ -21276,21 +21392,21 @@
       <c r="B50" s="61"/>
       <c r="C50" s="250"/>
       <c r="D50" s="253"/>
-      <c r="E50" s="244"/>
+      <c r="E50" s="264"/>
       <c r="F50" s="256"/>
-      <c r="G50" s="247"/>
-      <c r="H50" s="241" t="s">
+      <c r="G50" s="259"/>
+      <c r="H50" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="I50" s="242"/>
+      <c r="I50" s="240"/>
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B51" s="61"/>
       <c r="C51" s="251"/>
       <c r="D51" s="254"/>
-      <c r="E51" s="245"/>
+      <c r="E51" s="265"/>
       <c r="F51" s="257"/>
-      <c r="G51" s="248"/>
+      <c r="G51" s="260"/>
       <c r="H51" s="8" t="s">
         <v>23</v>
       </c>
@@ -21330,13 +21446,13 @@
       <c r="D53" s="252" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="243" t="s">
+      <c r="E53" s="263" t="s">
         <v>55</v>
       </c>
       <c r="F53" s="255" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="246" t="s">
+      <c r="G53" s="258" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -21350,21 +21466,21 @@
       <c r="B54" s="61"/>
       <c r="C54" s="250"/>
       <c r="D54" s="253"/>
-      <c r="E54" s="244"/>
+      <c r="E54" s="264"/>
       <c r="F54" s="256"/>
-      <c r="G54" s="247"/>
-      <c r="H54" s="241" t="s">
+      <c r="G54" s="259"/>
+      <c r="H54" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="I54" s="242"/>
+      <c r="I54" s="240"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
       <c r="C55" s="251"/>
       <c r="D55" s="254"/>
-      <c r="E55" s="245"/>
+      <c r="E55" s="265"/>
       <c r="F55" s="257"/>
-      <c r="G55" s="248"/>
+      <c r="G55" s="260"/>
       <c r="H55" s="8" t="s">
         <v>23</v>
       </c>
@@ -21389,8 +21505,8 @@
       <c r="E57" s="25"/>
       <c r="F57" s="22"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="239"/>
-      <c r="I57" s="240"/>
+      <c r="H57" s="261"/>
+      <c r="I57" s="262"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="61" t="s">
@@ -21453,10 +21569,10 @@
       <c r="E61" s="39"/>
       <c r="F61" s="12"/>
       <c r="G61" s="32"/>
-      <c r="H61" s="241" t="s">
+      <c r="H61" s="239" t="s">
         <v>32</v>
       </c>
-      <c r="I61" s="242"/>
+      <c r="I61" s="240"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -21489,8 +21605,8 @@
       <c r="E64" s="25"/>
       <c r="F64" s="22"/>
       <c r="G64" s="25"/>
-      <c r="H64" s="239"/>
-      <c r="I64" s="240"/>
+      <c r="H64" s="261"/>
+      <c r="I64" s="262"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64" t="s">
@@ -21903,8 +22019,8 @@
       <c r="E92" s="25"/>
       <c r="F92" s="22"/>
       <c r="G92" s="25"/>
-      <c r="H92" s="239"/>
-      <c r="I92" s="240"/>
+      <c r="H92" s="261"/>
+      <c r="I92" s="262"/>
     </row>
     <row r="93" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="61"/>
@@ -22048,16 +22164,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -22070,22 +22192,16 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -22119,10 +22235,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="267"/>
-      <c r="D2" s="259" t="s">
+      <c r="D2" s="242" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="260" t="s">
+      <c r="E2" s="243" t="s">
         <v>0</v>
       </c>
     </row>
@@ -22133,8 +22249,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="264"/>
-      <c r="E3" s="265"/>
+      <c r="D3" s="247"/>
+      <c r="E3" s="248"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 27 Oktober 2023 11:24 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -4090,13 +4090,6 @@
     <t>Func_GetDataPickSet_BusinessDocumentIssuanceDisposition</t>
   </si>
   <si>
-    <t>Func_GetDataList_CodeOfAccounting</t>
-  </si>
-  <si>
-    <t>SchData-OLTP-Accounting.
-Func_GetDataList_CodeOfAccounting</t>
-  </si>
-  <si>
     <t>Func_General_GetPersonByWorkerCareerInternalArrayID</t>
   </si>
   <si>
@@ -4105,9 +4098,6 @@
   <si>
     <t>SchData-OLTP-HumanResource.
 HoldFunc_General_GetPersonByWorkerCareerInternalArrayID</t>
-  </si>
-  <si>
-    <t>Func_GetDataPickList_CodeOfAccounting</t>
   </si>
   <si>
     <t xml:space="preserve">Mendapatkan Data Pick List Code Of Accounting (COA) berdasarkan ID Branch (varBranch_RefID) dan Tanggal Efektif (varEffectiveDate). </t>
@@ -4695,14 +4685,6 @@
     </r>
   </si>
   <si>
-    <t>Func_GetDataEntities_CodeOfAccounting</t>
-  </si>
-  <si>
-    <t>Mendapatkan Data Entities untuk CodeOfAccounting berdasarkan ID (varID).
-Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
-Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
-  </si>
-  <si>
     <t>Func_GetDataEntities_Journal</t>
   </si>
   <si>
@@ -5102,60 +5084,6 @@
 HoldFunc_GetDataFastEntities_Product</t>
   </si>
   <si>
-    <t>Func_TblCodeOfAccounting_SET</t>
-  </si>
-  <si>
-    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblCodeOfAccounting</t>
-  </si>
-  <si>
-    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblCodeOfAccountingLinkage</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccountingLinkage_SET</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccountingLinkageSchema_SET</t>
-  </si>
-  <si>
-    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblCodeOfAccountingLinkageSchema</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccounting_INSERT</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccounting_UPDATE</t>
-  </si>
-  <si>
-    <t>Memutakhirkan data (UPDATE) pada tabel TblCodeOfAccounting</t>
-  </si>
-  <si>
-    <t>Memasukan data (INSERT) pada tabel TblCodeOfAccounting</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccountingLinkage_INSERT</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccountingLinkage_UPDATE</t>
-  </si>
-  <si>
-    <t>Memasukan data (INSERT) pada tabel TblCodeOfAccountingLinkage</t>
-  </si>
-  <si>
-    <t>Memutakhirkan data (UPDATE) pada tabel TblCodeOfAccountingLinkage</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccountingLinkageSchema_INSERT</t>
-  </si>
-  <si>
-    <t>Func_TblCodeOfAccountingLinkageSchema_UPDATE</t>
-  </si>
-  <si>
-    <t>Memutakhirkan data (UPDATE) pada tabel TblCodeOfAccountingLinkageSchema</t>
-  </si>
-  <si>
-    <t>Memasukan data (INSERT) pada tabel TblCodeOfAccountingLinkageSchema</t>
-  </si>
-  <si>
     <t>Func_GetDataFastEntities_Person</t>
   </si>
   <si>
@@ -5216,6 +5144,78 @@
   </si>
   <si>
     <t>Memutakhirkan data (UPDATE) pada tabel TblAdvanceSettlementDetail</t>
+  </si>
+  <si>
+    <t>Func_GetDataEntities_ChartOfAccount</t>
+  </si>
+  <si>
+    <t>Mendapatkan Data Entities untuk ChartOfAccount berdasarkan ID (varID).
+Seluruh Field Reference secara default akan dieksplorasi untuk pencarian data, kecuali bila termasuk pada daftar yang dikecualikan (varListExcludeReferenceFieldDataSearch).
+Depth Level (varDepthLevel) digunakan untuk menentukan tingkat kedalaman pencarian Field Reference. Dengan semakin kecilnya nilai yang dimasukkan maka akan mempersingkat pula waktu pencarian (Pencarian tidak sampai terlalu dalam). Bila Depth Level tidak didefinisikan (NULL) maka seluruh Node Field Reference akan diekspansi sampai pada titik terakhir.</t>
+  </si>
+  <si>
+    <t>Func_GetDataList_ChartOfAccount</t>
+  </si>
+  <si>
+    <t>SchData-OLTP-Accounting.
+Func_GetDataList_ChartOfAccount</t>
+  </si>
+  <si>
+    <t>Func_GetDataPickList_ChartOfAccount</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccount_SET</t>
+  </si>
+  <si>
+    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblChartOfAccount</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccountLinkage_SET</t>
+  </si>
+  <si>
+    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblChartOfAccountLinkage</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccountLinkageSchema_SET</t>
+  </si>
+  <si>
+    <t>Mengeset data (INSERT dan UPDATE) pada tabel TblChartOfAccountLinkageSchema</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccount_INSERT</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblChartOfAccount</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccount_UPDATE</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblChartOfAccount</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccountLinkage_INSERT</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblChartOfAccountLinkage</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccountLinkage_UPDATE</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblChartOfAccountLinkage</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccountLinkageSchema_INSERT</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblChartOfAccountLinkageSchema</t>
+  </si>
+  <si>
+    <t>Func_TblChartOfAccountLinkageSchema_UPDATE</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblChartOfAccountLinkageSchema</t>
   </si>
 </sst>
 </file>
@@ -6768,21 +6768,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6801,35 +6786,50 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -6858,29 +6858,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8095,10 +8095,10 @@
   <dimension ref="A1:I846"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E722" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="F18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D723" sqref="D723"/>
+      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8117,20 +8117,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="237" t="s">
+      <c r="B2" s="243" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="238"/>
-      <c r="D2" s="239"/>
-      <c r="E2" s="244" t="s">
+      <c r="C2" s="244"/>
+      <c r="D2" s="245"/>
+      <c r="E2" s="239" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="240" t="s">
+      <c r="F2" s="235" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="241"/>
-      <c r="H2" s="242"/>
-      <c r="I2" s="235" t="s">
+      <c r="G2" s="236"/>
+      <c r="H2" s="237"/>
+      <c r="I2" s="241" t="s">
         <v>667</v>
       </c>
     </row>
@@ -8144,7 +8144,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="245"/>
+      <c r="E3" s="240"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -8154,11 +8154,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="236"/>
+      <c r="I3" s="242"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="243" t="s">
+      <c r="B4" s="238" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="221"/>
@@ -8233,10 +8233,10 @@
       <c r="B10" s="109"/>
       <c r="C10" s="110"/>
       <c r="D10" s="166" t="s">
-        <v>1481</v>
+        <v>1476</v>
       </c>
       <c r="E10" s="157" t="s">
-        <v>1483</v>
+        <v>1478</v>
       </c>
       <c r="F10" s="150" t="s">
         <v>232</v>
@@ -8248,7 +8248,7 @@
         <v>45204</v>
       </c>
       <c r="I10" s="195" t="s">
-        <v>1482</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -8256,10 +8256,10 @@
       <c r="B11" s="109"/>
       <c r="C11" s="110"/>
       <c r="D11" s="166" t="s">
-        <v>1484</v>
+        <v>1479</v>
       </c>
       <c r="E11" s="157" t="s">
-        <v>1485</v>
+        <v>1480</v>
       </c>
       <c r="F11" s="150" t="s">
         <v>232</v>
@@ -8271,7 +8271,7 @@
         <v>45204</v>
       </c>
       <c r="I11" s="195" t="s">
-        <v>1486</v>
+        <v>1481</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -8279,10 +8279,10 @@
       <c r="B12" s="109"/>
       <c r="C12" s="110"/>
       <c r="D12" s="166" t="s">
-        <v>1487</v>
+        <v>1482</v>
       </c>
       <c r="E12" s="157" t="s">
-        <v>1488</v>
+        <v>1483</v>
       </c>
       <c r="F12" s="150" t="s">
         <v>232</v>
@@ -8294,7 +8294,7 @@
         <v>45204</v>
       </c>
       <c r="I12" s="195" t="s">
-        <v>1489</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8313,10 +8313,10 @@
       <c r="B14" s="109"/>
       <c r="C14" s="110"/>
       <c r="D14" s="166" t="s">
-        <v>1396</v>
+        <v>1517</v>
       </c>
       <c r="E14" s="157" t="s">
-        <v>1397</v>
+        <v>1518</v>
       </c>
       <c r="F14" s="150" t="s">
         <v>267</v>
@@ -8336,10 +8336,10 @@
       <c r="B15" s="109"/>
       <c r="C15" s="110"/>
       <c r="D15" s="167" t="s">
-        <v>1398</v>
+        <v>1393</v>
       </c>
       <c r="E15" s="158" t="s">
-        <v>1399</v>
+        <v>1394</v>
       </c>
       <c r="F15" s="151" t="s">
         <v>267</v>
@@ -8359,10 +8359,10 @@
       <c r="B16" s="109"/>
       <c r="C16" s="110"/>
       <c r="D16" s="167" t="s">
-        <v>1404</v>
+        <v>1399</v>
       </c>
       <c r="E16" s="158" t="s">
-        <v>1405</v>
+        <v>1400</v>
       </c>
       <c r="F16" s="151" t="s">
         <v>267</v>
@@ -8382,10 +8382,10 @@
       <c r="B17" s="109"/>
       <c r="C17" s="110"/>
       <c r="D17" s="167" t="s">
-        <v>1400</v>
+        <v>1395</v>
       </c>
       <c r="E17" s="158" t="s">
-        <v>1401</v>
+        <v>1396</v>
       </c>
       <c r="F17" s="151" t="s">
         <v>267</v>
@@ -8427,10 +8427,10 @@
       <c r="B20" s="109"/>
       <c r="C20" s="110"/>
       <c r="D20" s="166" t="s">
-        <v>1227</v>
+        <v>1519</v>
       </c>
       <c r="E20" s="157" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="F20" s="150" t="s">
         <v>267</v>
@@ -8442,7 +8442,7 @@
         <v>1173</v>
       </c>
       <c r="I20" s="195" t="s">
-        <v>1228</v>
+        <v>1520</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -8461,10 +8461,10 @@
       <c r="B22" s="109"/>
       <c r="C22" s="110"/>
       <c r="D22" s="166" t="s">
-        <v>1232</v>
+        <v>1521</v>
       </c>
       <c r="E22" s="157" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="F22" s="150" t="s">
         <v>232</v>
@@ -8506,10 +8506,10 @@
       <c r="B25" s="109"/>
       <c r="C25" s="110"/>
       <c r="D25" s="166" t="s">
-        <v>1502</v>
+        <v>1522</v>
       </c>
       <c r="E25" s="157" t="s">
-        <v>1503</v>
+        <v>1523</v>
       </c>
       <c r="F25" s="150" t="s">
         <v>232</v>
@@ -8529,10 +8529,10 @@
       <c r="B26" s="109"/>
       <c r="C26" s="110"/>
       <c r="D26" s="166" t="s">
-        <v>1505</v>
+        <v>1524</v>
       </c>
       <c r="E26" s="157" t="s">
-        <v>1504</v>
+        <v>1525</v>
       </c>
       <c r="F26" s="150" t="s">
         <v>232</v>
@@ -8552,10 +8552,10 @@
       <c r="B27" s="109"/>
       <c r="C27" s="110"/>
       <c r="D27" s="166" t="s">
-        <v>1506</v>
+        <v>1526</v>
       </c>
       <c r="E27" s="157" t="s">
-        <v>1507</v>
+        <v>1527</v>
       </c>
       <c r="F27" s="150" t="s">
         <v>232</v>
@@ -8758,10 +8758,10 @@
       <c r="B39" s="109"/>
       <c r="C39" s="110"/>
       <c r="D39" s="166" t="s">
-        <v>1402</v>
+        <v>1397</v>
       </c>
       <c r="E39" s="157" t="s">
-        <v>1403</v>
+        <v>1398</v>
       </c>
       <c r="F39" s="150" t="s">
         <v>267</v>
@@ -8781,10 +8781,10 @@
       <c r="B40" s="109"/>
       <c r="C40" s="110"/>
       <c r="D40" s="166" t="s">
-        <v>1406</v>
+        <v>1401</v>
       </c>
       <c r="E40" s="157" t="s">
-        <v>1407</v>
+        <v>1402</v>
       </c>
       <c r="F40" s="150" t="s">
         <v>547</v>
@@ -8804,10 +8804,10 @@
       <c r="B41" s="109"/>
       <c r="C41" s="110"/>
       <c r="D41" s="166" t="s">
-        <v>1408</v>
+        <v>1403</v>
       </c>
       <c r="E41" s="157" t="s">
-        <v>1409</v>
+        <v>1404</v>
       </c>
       <c r="F41" s="150" t="s">
         <v>547</v>
@@ -8827,10 +8827,10 @@
       <c r="B42" s="109"/>
       <c r="C42" s="110"/>
       <c r="D42" s="166" t="s">
-        <v>1410</v>
+        <v>1405</v>
       </c>
       <c r="E42" s="157" t="s">
-        <v>1411</v>
+        <v>1406</v>
       </c>
       <c r="F42" s="150" t="s">
         <v>547</v>
@@ -8850,10 +8850,10 @@
       <c r="B43" s="109"/>
       <c r="C43" s="110"/>
       <c r="D43" s="166" t="s">
-        <v>1412</v>
+        <v>1407</v>
       </c>
       <c r="E43" s="157" t="s">
-        <v>1413</v>
+        <v>1408</v>
       </c>
       <c r="F43" s="150" t="s">
         <v>232</v>
@@ -8873,10 +8873,10 @@
       <c r="B44" s="109"/>
       <c r="C44" s="110"/>
       <c r="D44" s="166" t="s">
-        <v>1414</v>
+        <v>1409</v>
       </c>
       <c r="E44" s="157" t="s">
-        <v>1415</v>
+        <v>1410</v>
       </c>
       <c r="F44" s="150" t="s">
         <v>232</v>
@@ -8896,10 +8896,10 @@
       <c r="B45" s="109"/>
       <c r="C45" s="110"/>
       <c r="D45" s="166" t="s">
-        <v>1416</v>
+        <v>1411</v>
       </c>
       <c r="E45" s="157" t="s">
-        <v>1417</v>
+        <v>1412</v>
       </c>
       <c r="F45" s="150" t="s">
         <v>232</v>
@@ -8919,10 +8919,10 @@
       <c r="B46" s="109"/>
       <c r="C46" s="110"/>
       <c r="D46" s="166" t="s">
-        <v>1418</v>
+        <v>1413</v>
       </c>
       <c r="E46" s="157" t="s">
-        <v>1419</v>
+        <v>1414</v>
       </c>
       <c r="F46" s="150" t="s">
         <v>232</v>
@@ -8942,10 +8942,10 @@
       <c r="B47" s="109"/>
       <c r="C47" s="110"/>
       <c r="D47" s="166" t="s">
-        <v>1420</v>
+        <v>1415</v>
       </c>
       <c r="E47" s="157" t="s">
-        <v>1421</v>
+        <v>1416</v>
       </c>
       <c r="F47" s="150" t="s">
         <v>232</v>
@@ -8988,10 +8988,10 @@
       <c r="B49" s="109"/>
       <c r="C49" s="110"/>
       <c r="D49" s="166" t="s">
-        <v>1494</v>
+        <v>1489</v>
       </c>
       <c r="E49" s="157" t="s">
-        <v>1495</v>
+        <v>1490</v>
       </c>
       <c r="F49" s="150" t="s">
         <v>232</v>
@@ -9011,10 +9011,10 @@
       <c r="B50" s="109"/>
       <c r="C50" s="110"/>
       <c r="D50" s="198" t="s">
-        <v>1422</v>
+        <v>1417</v>
       </c>
       <c r="E50" s="158" t="s">
-        <v>1424</v>
+        <v>1419</v>
       </c>
       <c r="F50" s="151" t="s">
         <v>232</v>
@@ -9034,10 +9034,10 @@
       <c r="B51" s="109"/>
       <c r="C51" s="110"/>
       <c r="D51" s="198" t="s">
-        <v>1423</v>
+        <v>1418</v>
       </c>
       <c r="E51" s="158" t="s">
-        <v>1425</v>
+        <v>1420</v>
       </c>
       <c r="F51" s="151" t="s">
         <v>232</v>
@@ -9500,10 +9500,10 @@
       <c r="B79" s="109"/>
       <c r="C79" s="110"/>
       <c r="D79" s="167" t="s">
-        <v>1426</v>
+        <v>1421</v>
       </c>
       <c r="E79" s="158" t="s">
-        <v>1427</v>
+        <v>1422</v>
       </c>
       <c r="F79" s="151" t="s">
         <v>267</v>
@@ -9523,10 +9523,10 @@
       <c r="B80" s="109"/>
       <c r="C80" s="110"/>
       <c r="D80" s="167" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="E80" s="158" t="s">
-        <v>1429</v>
+        <v>1424</v>
       </c>
       <c r="F80" s="151" t="s">
         <v>267</v>
@@ -9546,10 +9546,10 @@
       <c r="B81" s="109"/>
       <c r="C81" s="110"/>
       <c r="D81" s="167" t="s">
-        <v>1428</v>
+        <v>1423</v>
       </c>
       <c r="E81" s="158" t="s">
-        <v>1429</v>
+        <v>1424</v>
       </c>
       <c r="F81" s="151" t="s">
         <v>267</v>
@@ -9569,10 +9569,10 @@
       <c r="B82" s="109"/>
       <c r="C82" s="110"/>
       <c r="D82" s="167" t="s">
-        <v>1430</v>
+        <v>1425</v>
       </c>
       <c r="E82" s="158" t="s">
-        <v>1431</v>
+        <v>1426</v>
       </c>
       <c r="F82" s="151" t="s">
         <v>267</v>
@@ -9592,10 +9592,10 @@
       <c r="B83" s="109"/>
       <c r="C83" s="110"/>
       <c r="D83" s="167" t="s">
-        <v>1432</v>
+        <v>1427</v>
       </c>
       <c r="E83" s="158" t="s">
-        <v>1433</v>
+        <v>1428</v>
       </c>
       <c r="F83" s="151" t="s">
         <v>547</v>
@@ -9615,10 +9615,10 @@
       <c r="B84" s="109"/>
       <c r="C84" s="110"/>
       <c r="D84" s="167" t="s">
-        <v>1434</v>
+        <v>1429</v>
       </c>
       <c r="E84" s="158" t="s">
-        <v>1435</v>
+        <v>1430</v>
       </c>
       <c r="F84" s="151" t="s">
         <v>267</v>
@@ -9638,10 +9638,10 @@
       <c r="B85" s="109"/>
       <c r="C85" s="110"/>
       <c r="D85" s="167" t="s">
-        <v>1436</v>
+        <v>1431</v>
       </c>
       <c r="E85" s="158" t="s">
-        <v>1437</v>
+        <v>1432</v>
       </c>
       <c r="F85" s="151" t="s">
         <v>267</v>
@@ -9661,10 +9661,10 @@
       <c r="B86" s="109"/>
       <c r="C86" s="110"/>
       <c r="D86" s="167" t="s">
-        <v>1438</v>
+        <v>1433</v>
       </c>
       <c r="E86" s="158" t="s">
-        <v>1439</v>
+        <v>1434</v>
       </c>
       <c r="F86" s="151" t="s">
         <v>547</v>
@@ -9706,10 +9706,10 @@
       <c r="B89" s="109"/>
       <c r="C89" s="110"/>
       <c r="D89" s="167" t="s">
-        <v>1460</v>
+        <v>1455</v>
       </c>
       <c r="E89" s="158" t="s">
-        <v>1461</v>
+        <v>1456</v>
       </c>
       <c r="F89" s="151" t="s">
         <v>232</v>
@@ -9751,10 +9751,10 @@
       <c r="B92" s="109"/>
       <c r="C92" s="110"/>
       <c r="D92" s="167" t="s">
-        <v>1316</v>
+        <v>1313</v>
       </c>
       <c r="E92" s="160" t="s">
-        <v>1317</v>
+        <v>1314</v>
       </c>
       <c r="F92" s="151" t="s">
         <v>232</v>
@@ -9774,10 +9774,10 @@
       <c r="B93" s="109"/>
       <c r="C93" s="110"/>
       <c r="D93" s="167" t="s">
-        <v>1319</v>
+        <v>1316</v>
       </c>
       <c r="E93" s="160" t="s">
-        <v>1318</v>
+        <v>1315</v>
       </c>
       <c r="F93" s="151" t="s">
         <v>232</v>
@@ -9992,10 +9992,10 @@
       <c r="B105" s="109"/>
       <c r="C105" s="110"/>
       <c r="D105" s="167" t="s">
-        <v>1440</v>
+        <v>1435</v>
       </c>
       <c r="E105" s="158" t="s">
-        <v>1450</v>
+        <v>1445</v>
       </c>
       <c r="F105" s="151" t="s">
         <v>267</v>
@@ -10015,10 +10015,10 @@
       <c r="B106" s="109"/>
       <c r="C106" s="110"/>
       <c r="D106" s="167" t="s">
-        <v>1441</v>
+        <v>1436</v>
       </c>
       <c r="E106" s="158" t="s">
-        <v>1451</v>
+        <v>1446</v>
       </c>
       <c r="F106" s="151" t="s">
         <v>547</v>
@@ -10038,10 +10038,10 @@
       <c r="B107" s="109"/>
       <c r="C107" s="110"/>
       <c r="D107" s="167" t="s">
-        <v>1442</v>
+        <v>1437</v>
       </c>
       <c r="E107" s="158" t="s">
-        <v>1443</v>
+        <v>1438</v>
       </c>
       <c r="F107" s="151" t="s">
         <v>547</v>
@@ -10061,10 +10061,10 @@
       <c r="B108" s="109"/>
       <c r="C108" s="110"/>
       <c r="D108" s="167" t="s">
+        <v>1439</v>
+      </c>
+      <c r="E108" s="158" t="s">
         <v>1444</v>
-      </c>
-      <c r="E108" s="158" t="s">
-        <v>1449</v>
       </c>
       <c r="F108" s="151"/>
       <c r="G108" s="180">
@@ -10080,10 +10080,10 @@
       <c r="B109" s="109"/>
       <c r="C109" s="110"/>
       <c r="D109" s="167" t="s">
-        <v>1445</v>
+        <v>1440</v>
       </c>
       <c r="E109" s="158" t="s">
-        <v>1447</v>
+        <v>1442</v>
       </c>
       <c r="F109" s="151" t="s">
         <v>267</v>
@@ -10103,10 +10103,10 @@
       <c r="B110" s="109"/>
       <c r="C110" s="110"/>
       <c r="D110" s="167" t="s">
-        <v>1446</v>
+        <v>1441</v>
       </c>
       <c r="E110" s="158" t="s">
-        <v>1448</v>
+        <v>1443</v>
       </c>
       <c r="F110" s="151" t="s">
         <v>267</v>
@@ -10126,10 +10126,10 @@
       <c r="B111" s="109"/>
       <c r="C111" s="110"/>
       <c r="D111" s="167" t="s">
-        <v>1452</v>
+        <v>1447</v>
       </c>
       <c r="E111" s="158" t="s">
-        <v>1453</v>
+        <v>1448</v>
       </c>
       <c r="F111" s="151" t="s">
         <v>267</v>
@@ -10195,10 +10195,10 @@
       <c r="B114" s="109"/>
       <c r="C114" s="110"/>
       <c r="D114" s="167" t="s">
-        <v>1454</v>
+        <v>1449</v>
       </c>
       <c r="E114" s="158" t="s">
-        <v>1455</v>
+        <v>1450</v>
       </c>
       <c r="F114" s="151"/>
       <c r="G114" s="180"/>
@@ -10210,10 +10210,10 @@
       <c r="B115" s="109"/>
       <c r="C115" s="110"/>
       <c r="D115" s="167" t="s">
-        <v>1456</v>
+        <v>1451</v>
       </c>
       <c r="E115" s="158" t="s">
-        <v>1457</v>
+        <v>1452</v>
       </c>
       <c r="F115" s="151" t="s">
         <v>267</v>
@@ -10233,10 +10233,10 @@
       <c r="B116" s="109"/>
       <c r="C116" s="110"/>
       <c r="D116" s="167" t="s">
-        <v>1458</v>
+        <v>1453</v>
       </c>
       <c r="E116" s="158" t="s">
-        <v>1459</v>
+        <v>1454</v>
       </c>
       <c r="F116" s="151" t="s">
         <v>267</v>
@@ -10653,10 +10653,10 @@
       <c r="B140" s="109"/>
       <c r="C140" s="110"/>
       <c r="D140" s="166" t="s">
-        <v>1526</v>
+        <v>1503</v>
       </c>
       <c r="E140" s="162" t="s">
-        <v>1527</v>
+        <v>1504</v>
       </c>
       <c r="F140" s="150" t="s">
         <v>232</v>
@@ -10676,10 +10676,10 @@
       <c r="B141" s="109"/>
       <c r="C141" s="110"/>
       <c r="D141" s="166" t="s">
-        <v>1528</v>
+        <v>1505</v>
       </c>
       <c r="E141" s="162" t="s">
-        <v>1529</v>
+        <v>1506</v>
       </c>
       <c r="F141" s="150" t="s">
         <v>281</v>
@@ -10917,10 +10917,10 @@
       <c r="B154" s="109"/>
       <c r="C154" s="110"/>
       <c r="D154" s="166" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="E154" s="157" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="F154" s="150" t="s">
         <v>547</v>
@@ -10962,10 +10962,10 @@
       <c r="B157" s="109"/>
       <c r="C157" s="110"/>
       <c r="D157" s="166" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
       <c r="E157" s="157" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="F157" s="150" t="s">
         <v>256</v>
@@ -10977,7 +10977,7 @@
         <v>44427</v>
       </c>
       <c r="I157" s="195" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="158" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -11007,10 +11007,10 @@
       <c r="B160" s="109"/>
       <c r="C160" s="110"/>
       <c r="D160" s="166" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="E160" s="157" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="F160" s="150" t="s">
         <v>232</v>
@@ -11052,10 +11052,10 @@
       <c r="B163" s="109"/>
       <c r="C163" s="110"/>
       <c r="D163" s="166" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="E163" s="162" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="F163" s="150" t="s">
         <v>267</v>
@@ -11121,10 +11121,10 @@
       <c r="B168" s="109"/>
       <c r="C168" s="110"/>
       <c r="D168" s="166" t="s">
-        <v>1229</v>
+        <v>1227</v>
       </c>
       <c r="E168" s="157" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
       <c r="F168" s="150" t="s">
         <v>232</v>
@@ -11136,7 +11136,7 @@
         <v>45160</v>
       </c>
       <c r="I168" s="195" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="169" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -11462,10 +11462,10 @@
       <c r="B187" s="109"/>
       <c r="C187" s="110"/>
       <c r="D187" s="166" t="s">
-        <v>1355</v>
+        <v>1352</v>
       </c>
       <c r="E187" s="157" t="s">
-        <v>1354</v>
+        <v>1351</v>
       </c>
       <c r="F187" s="150" t="s">
         <v>232</v>
@@ -11477,7 +11477,7 @@
         <v>45189</v>
       </c>
       <c r="I187" s="195" t="s">
-        <v>1356</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="188" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11632,10 +11632,10 @@
       <c r="B197" s="109"/>
       <c r="C197" s="110"/>
       <c r="D197" s="166" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="E197" s="157" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="F197" s="150" t="s">
         <v>232</v>
@@ -12202,10 +12202,10 @@
       <c r="B225" s="109"/>
       <c r="C225" s="110"/>
       <c r="D225" s="166" t="s">
-        <v>1462</v>
+        <v>1457</v>
       </c>
       <c r="E225" s="158" t="s">
-        <v>1463</v>
+        <v>1458</v>
       </c>
       <c r="F225" s="150" t="s">
         <v>267</v>
@@ -12282,10 +12282,10 @@
       <c r="B229" s="109"/>
       <c r="C229" s="110"/>
       <c r="D229" s="166" t="s">
-        <v>1375</v>
+        <v>1372</v>
       </c>
       <c r="E229" s="216" t="s">
-        <v>1376</v>
+        <v>1373</v>
       </c>
       <c r="F229" s="151" t="s">
         <v>547</v>
@@ -12305,10 +12305,10 @@
       <c r="B230" s="109"/>
       <c r="C230" s="110"/>
       <c r="D230" s="166" t="s">
-        <v>1371</v>
+        <v>1368</v>
       </c>
       <c r="E230" s="216" t="s">
-        <v>1372</v>
+        <v>1369</v>
       </c>
       <c r="F230" s="151" t="s">
         <v>267</v>
@@ -12328,10 +12328,10 @@
       <c r="B231" s="109"/>
       <c r="C231" s="110"/>
       <c r="D231" s="166" t="s">
-        <v>1369</v>
+        <v>1366</v>
       </c>
       <c r="E231" s="216" t="s">
-        <v>1370</v>
+        <v>1367</v>
       </c>
       <c r="F231" s="151" t="s">
         <v>267</v>
@@ -12351,10 +12351,10 @@
       <c r="B232" s="109"/>
       <c r="C232" s="110"/>
       <c r="D232" s="166" t="s">
-        <v>1367</v>
+        <v>1364</v>
       </c>
       <c r="E232" s="216" t="s">
-        <v>1368</v>
+        <v>1365</v>
       </c>
       <c r="F232" s="151" t="s">
         <v>547</v>
@@ -12374,10 +12374,10 @@
       <c r="B233" s="109"/>
       <c r="C233" s="110"/>
       <c r="D233" s="166" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
       <c r="E233" s="216" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="F233" s="151" t="s">
         <v>232</v>
@@ -12397,10 +12397,10 @@
       <c r="B234" s="109"/>
       <c r="C234" s="110"/>
       <c r="D234" s="166" t="s">
-        <v>1365</v>
+        <v>1362</v>
       </c>
       <c r="E234" s="216" t="s">
-        <v>1366</v>
+        <v>1363</v>
       </c>
       <c r="F234" s="151" t="s">
         <v>547</v>
@@ -12466,10 +12466,10 @@
       <c r="B237" s="109"/>
       <c r="C237" s="110"/>
       <c r="D237" s="166" t="s">
-        <v>1363</v>
+        <v>1360</v>
       </c>
       <c r="E237" s="216" t="s">
-        <v>1364</v>
+        <v>1361</v>
       </c>
       <c r="F237" s="151" t="s">
         <v>547</v>
@@ -12489,10 +12489,10 @@
       <c r="B238" s="109"/>
       <c r="C238" s="110"/>
       <c r="D238" s="166" t="s">
-        <v>1324</v>
+        <v>1321</v>
       </c>
       <c r="E238" s="216" t="s">
-        <v>1325</v>
+        <v>1322</v>
       </c>
       <c r="F238" s="151" t="s">
         <v>267</v>
@@ -12512,10 +12512,10 @@
       <c r="B239" s="109"/>
       <c r="C239" s="110"/>
       <c r="D239" s="166" t="s">
-        <v>1361</v>
+        <v>1358</v>
       </c>
       <c r="E239" s="216" t="s">
-        <v>1362</v>
+        <v>1359</v>
       </c>
       <c r="F239" s="151" t="s">
         <v>547</v>
@@ -12535,10 +12535,10 @@
       <c r="B240" s="109"/>
       <c r="C240" s="110"/>
       <c r="D240" s="167" t="s">
-        <v>1357</v>
+        <v>1354</v>
       </c>
       <c r="E240" s="157" t="s">
-        <v>1358</v>
+        <v>1355</v>
       </c>
       <c r="F240" s="150" t="s">
         <v>547</v>
@@ -12558,10 +12558,10 @@
       <c r="B241" s="109"/>
       <c r="C241" s="110"/>
       <c r="D241" s="167" t="s">
-        <v>1360</v>
+        <v>1357</v>
       </c>
       <c r="E241" s="157" t="s">
-        <v>1359</v>
+        <v>1356</v>
       </c>
       <c r="F241" s="150" t="s">
         <v>267</v>
@@ -12581,10 +12581,10 @@
       <c r="B242" s="109"/>
       <c r="C242" s="110"/>
       <c r="D242" s="165" t="s">
-        <v>1345</v>
+        <v>1342</v>
       </c>
       <c r="E242" s="157" t="s">
-        <v>1346</v>
+        <v>1343</v>
       </c>
       <c r="F242" s="150" t="s">
         <v>267</v>
@@ -12615,10 +12615,10 @@
       <c r="B244" s="109"/>
       <c r="C244" s="110"/>
       <c r="D244" s="166" t="s">
+        <v>1344</v>
+      </c>
+      <c r="E244" s="157" t="s">
         <v>1347</v>
-      </c>
-      <c r="E244" s="157" t="s">
-        <v>1350</v>
       </c>
       <c r="F244" s="150" t="s">
         <v>232</v>
@@ -12630,7 +12630,7 @@
         <v>44859</v>
       </c>
       <c r="I244" s="195" t="s">
-        <v>1351</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="245" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12638,10 +12638,10 @@
       <c r="B245" s="109"/>
       <c r="C245" s="110"/>
       <c r="D245" s="166" t="s">
-        <v>1349</v>
+        <v>1346</v>
       </c>
       <c r="E245" s="157" t="s">
-        <v>1373</v>
+        <v>1370</v>
       </c>
       <c r="F245" s="150" t="s">
         <v>232</v>
@@ -12653,7 +12653,7 @@
         <v>45188</v>
       </c>
       <c r="I245" s="195" t="s">
-        <v>1353</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="246" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12661,10 +12661,10 @@
       <c r="B246" s="109"/>
       <c r="C246" s="110"/>
       <c r="D246" s="166" t="s">
-        <v>1348</v>
+        <v>1345</v>
       </c>
       <c r="E246" s="157" t="s">
-        <v>1374</v>
+        <v>1371</v>
       </c>
       <c r="F246" s="150" t="s">
         <v>232</v>
@@ -12676,7 +12676,7 @@
         <v>44859</v>
       </c>
       <c r="I246" s="195" t="s">
-        <v>1352</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="247" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12684,10 +12684,10 @@
       <c r="B247" s="109"/>
       <c r="C247" s="110"/>
       <c r="D247" s="166" t="s">
-        <v>1520</v>
+        <v>1497</v>
       </c>
       <c r="E247" s="157" t="s">
-        <v>1524</v>
+        <v>1501</v>
       </c>
       <c r="F247" s="150" t="s">
         <v>232</v>
@@ -12699,7 +12699,7 @@
         <v>45218</v>
       </c>
       <c r="I247" s="195" t="s">
-        <v>1521</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="248" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12707,10 +12707,10 @@
       <c r="B248" s="109"/>
       <c r="C248" s="110"/>
       <c r="D248" s="166" t="s">
-        <v>1523</v>
+        <v>1500</v>
       </c>
       <c r="E248" s="157" t="s">
-        <v>1525</v>
+        <v>1502</v>
       </c>
       <c r="F248" s="150" t="s">
         <v>232</v>
@@ -12722,7 +12722,7 @@
         <v>45218</v>
       </c>
       <c r="I248" s="195" t="s">
-        <v>1522</v>
+        <v>1499</v>
       </c>
     </row>
     <row r="249" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12730,10 +12730,10 @@
       <c r="B249" s="109"/>
       <c r="C249" s="110"/>
       <c r="D249" s="166" t="s">
-        <v>1499</v>
+        <v>1494</v>
       </c>
       <c r="E249" s="157" t="s">
-        <v>1500</v>
+        <v>1495</v>
       </c>
       <c r="F249" s="150" t="s">
         <v>232</v>
@@ -12745,7 +12745,7 @@
         <v>45205</v>
       </c>
       <c r="I249" s="195" t="s">
-        <v>1501</v>
+        <v>1496</v>
       </c>
     </row>
     <row r="250" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -12753,10 +12753,10 @@
       <c r="B250" s="109"/>
       <c r="C250" s="110"/>
       <c r="D250" s="166" t="s">
-        <v>1496</v>
+        <v>1491</v>
       </c>
       <c r="E250" s="157" t="s">
-        <v>1497</v>
+        <v>1492</v>
       </c>
       <c r="F250" s="150" t="s">
         <v>232</v>
@@ -12768,7 +12768,7 @@
         <v>45216</v>
       </c>
       <c r="I250" s="195" t="s">
-        <v>1498</v>
+        <v>1493</v>
       </c>
     </row>
     <row r="251" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -12993,10 +12993,10 @@
       <c r="B262" s="109"/>
       <c r="C262" s="110"/>
       <c r="D262" s="167" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="E262" s="158" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="F262" s="151" t="s">
         <v>281</v>
@@ -13008,7 +13008,7 @@
         <v>44851</v>
       </c>
       <c r="I262" s="196" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="263" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -13038,10 +13038,10 @@
       <c r="B265" s="109"/>
       <c r="C265" s="110"/>
       <c r="D265" s="167" t="s">
-        <v>1394</v>
+        <v>1391</v>
       </c>
       <c r="E265" s="158" t="s">
-        <v>1395</v>
+        <v>1392</v>
       </c>
       <c r="F265" s="151" t="s">
         <v>232</v>
@@ -13061,10 +13061,10 @@
       <c r="B266" s="109"/>
       <c r="C266" s="110"/>
       <c r="D266" s="167" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="E266" s="158" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="F266" s="151" t="s">
         <v>232</v>
@@ -13221,10 +13221,10 @@
       <c r="B274" s="109"/>
       <c r="C274" s="110"/>
       <c r="D274" s="166" t="s">
-        <v>1378</v>
+        <v>1375</v>
       </c>
       <c r="E274" s="157" t="s">
-        <v>1379</v>
+        <v>1376</v>
       </c>
       <c r="F274" s="150" t="s">
         <v>232</v>
@@ -13236,7 +13236,7 @@
         <v>45190</v>
       </c>
       <c r="I274" s="195" t="s">
-        <v>1377</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="275" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13255,10 +13255,10 @@
       <c r="B276" s="109"/>
       <c r="C276" s="110"/>
       <c r="D276" s="166" t="s">
-        <v>1387</v>
+        <v>1384</v>
       </c>
       <c r="E276" s="162" t="s">
-        <v>1388</v>
+        <v>1385</v>
       </c>
       <c r="F276" s="150" t="s">
         <v>232</v>
@@ -13324,7 +13324,7 @@
       <c r="B279" s="109"/>
       <c r="C279" s="110"/>
       <c r="D279" s="167" t="s">
-        <v>1389</v>
+        <v>1386</v>
       </c>
       <c r="E279" s="158" t="s">
         <v>1140</v>
@@ -13347,10 +13347,10 @@
       <c r="B280" s="109"/>
       <c r="C280" s="110"/>
       <c r="D280" s="167" t="s">
-        <v>1390</v>
+        <v>1387</v>
       </c>
       <c r="E280" s="158" t="s">
-        <v>1391</v>
+        <v>1388</v>
       </c>
       <c r="F280" s="151" t="s">
         <v>267</v>
@@ -13370,10 +13370,10 @@
       <c r="B281" s="109"/>
       <c r="C281" s="110"/>
       <c r="D281" s="167" t="s">
-        <v>1392</v>
+        <v>1389</v>
       </c>
       <c r="E281" s="158" t="s">
-        <v>1393</v>
+        <v>1390</v>
       </c>
       <c r="F281" s="151" t="s">
         <v>232</v>
@@ -14382,10 +14382,10 @@
       <c r="B341" s="109"/>
       <c r="C341" s="110"/>
       <c r="D341" s="167" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="E341" s="158" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="F341" s="151" t="s">
         <v>232</v>
@@ -14450,10 +14450,10 @@
       <c r="B345" s="109"/>
       <c r="C345" s="110"/>
       <c r="D345" s="167" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="E345" s="158" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="F345" s="151" t="s">
         <v>232</v>
@@ -15080,7 +15080,7 @@
       <c r="B379" s="109"/>
       <c r="C379" s="110"/>
       <c r="D379" s="167" t="s">
-        <v>1476</v>
+        <v>1471</v>
       </c>
       <c r="E379" s="160" t="s">
         <v>237</v>
@@ -15126,10 +15126,10 @@
       <c r="B381" s="109"/>
       <c r="C381" s="110"/>
       <c r="D381" s="167" t="s">
-        <v>1467</v>
+        <v>1462</v>
       </c>
       <c r="E381" s="160" t="s">
-        <v>1468</v>
+        <v>1463</v>
       </c>
       <c r="F381" s="151" t="s">
         <v>232</v>
@@ -15160,10 +15160,10 @@
       <c r="B383" s="109"/>
       <c r="C383" s="110"/>
       <c r="D383" s="167" t="s">
-        <v>1278</v>
+        <v>1275</v>
       </c>
       <c r="E383" s="158" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="F383" s="151" t="s">
         <v>232</v>
@@ -15175,7 +15175,7 @@
         <v>45169</v>
       </c>
       <c r="I383" s="196" t="s">
-        <v>1275</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="384" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15183,10 +15183,10 @@
       <c r="B384" s="109"/>
       <c r="C384" s="110"/>
       <c r="D384" s="167" t="s">
-        <v>1279</v>
+        <v>1276</v>
       </c>
       <c r="E384" s="158" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="F384" s="151" t="s">
         <v>232</v>
@@ -15198,7 +15198,7 @@
         <v>45169</v>
       </c>
       <c r="I384" s="196" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="385" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15206,10 +15206,10 @@
       <c r="B385" s="109"/>
       <c r="C385" s="110"/>
       <c r="D385" s="167" t="s">
-        <v>1280</v>
+        <v>1277</v>
       </c>
       <c r="E385" s="158" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="F385" s="151" t="s">
         <v>232</v>
@@ -15221,7 +15221,7 @@
         <v>45169</v>
       </c>
       <c r="I385" s="196" t="s">
-        <v>1277</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="386" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15229,10 +15229,10 @@
       <c r="B386" s="109"/>
       <c r="C386" s="110"/>
       <c r="D386" s="167" t="s">
-        <v>1281</v>
+        <v>1278</v>
       </c>
       <c r="E386" s="158" t="s">
-        <v>1283</v>
+        <v>1280</v>
       </c>
       <c r="F386" s="151" t="s">
         <v>232</v>
@@ -15244,7 +15244,7 @@
         <v>45169</v>
       </c>
       <c r="I386" s="196" t="s">
-        <v>1285</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="387" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15252,10 +15252,10 @@
       <c r="B387" s="109"/>
       <c r="C387" s="110"/>
       <c r="D387" s="167" t="s">
-        <v>1282</v>
+        <v>1279</v>
       </c>
       <c r="E387" s="158" t="s">
-        <v>1284</v>
+        <v>1281</v>
       </c>
       <c r="F387" s="151" t="s">
         <v>232</v>
@@ -15267,7 +15267,7 @@
         <v>45169</v>
       </c>
       <c r="I387" s="196" t="s">
-        <v>1286</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="388" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15275,10 +15275,10 @@
       <c r="B388" s="109"/>
       <c r="C388" s="110"/>
       <c r="D388" s="167" t="s">
-        <v>1287</v>
+        <v>1284</v>
       </c>
       <c r="E388" s="158" t="s">
-        <v>1288</v>
+        <v>1285</v>
       </c>
       <c r="F388" s="151" t="s">
         <v>232</v>
@@ -15290,7 +15290,7 @@
         <v>45169</v>
       </c>
       <c r="I388" s="196" t="s">
-        <v>1289</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="389" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15298,10 +15298,10 @@
       <c r="B389" s="109"/>
       <c r="C389" s="110"/>
       <c r="D389" s="167" t="s">
-        <v>1290</v>
+        <v>1287</v>
       </c>
       <c r="E389" s="158" t="s">
-        <v>1291</v>
+        <v>1288</v>
       </c>
       <c r="F389" s="151" t="s">
         <v>232</v>
@@ -15313,7 +15313,7 @@
         <v>45169</v>
       </c>
       <c r="I389" s="196" t="s">
-        <v>1292</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="390" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15321,10 +15321,10 @@
       <c r="B390" s="109"/>
       <c r="C390" s="110"/>
       <c r="D390" s="167" t="s">
-        <v>1299</v>
+        <v>1296</v>
       </c>
       <c r="E390" s="158" t="s">
-        <v>1304</v>
+        <v>1301</v>
       </c>
       <c r="F390" s="151" t="s">
         <v>232</v>
@@ -15336,7 +15336,7 @@
         <v>45169</v>
       </c>
       <c r="I390" s="196" t="s">
-        <v>1305</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="391" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15344,10 +15344,10 @@
       <c r="B391" s="109"/>
       <c r="C391" s="110"/>
       <c r="D391" s="167" t="s">
-        <v>1301</v>
+        <v>1298</v>
       </c>
       <c r="E391" s="158" t="s">
-        <v>1303</v>
+        <v>1300</v>
       </c>
       <c r="F391" s="151" t="s">
         <v>232</v>
@@ -15359,7 +15359,7 @@
         <v>45169</v>
       </c>
       <c r="I391" s="196" t="s">
-        <v>1306</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="392" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15367,10 +15367,10 @@
       <c r="B392" s="109"/>
       <c r="C392" s="110"/>
       <c r="D392" s="167" t="s">
-        <v>1300</v>
+        <v>1297</v>
       </c>
       <c r="E392" s="158" t="s">
-        <v>1302</v>
+        <v>1299</v>
       </c>
       <c r="F392" s="151" t="s">
         <v>232</v>
@@ -15382,7 +15382,7 @@
         <v>45169</v>
       </c>
       <c r="I392" s="196" t="s">
-        <v>1307</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="393" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15390,10 +15390,10 @@
       <c r="B393" s="109"/>
       <c r="C393" s="110"/>
       <c r="D393" s="167" t="s">
-        <v>1296</v>
+        <v>1293</v>
       </c>
       <c r="E393" s="158" t="s">
-        <v>1297</v>
+        <v>1294</v>
       </c>
       <c r="F393" s="151" t="s">
         <v>232</v>
@@ -15405,7 +15405,7 @@
         <v>45169</v>
       </c>
       <c r="I393" s="196" t="s">
-        <v>1298</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="394" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15413,10 +15413,10 @@
       <c r="B394" s="109"/>
       <c r="C394" s="110"/>
       <c r="D394" s="167" t="s">
-        <v>1293</v>
+        <v>1290</v>
       </c>
       <c r="E394" s="158" t="s">
-        <v>1294</v>
+        <v>1291</v>
       </c>
       <c r="F394" s="151" t="s">
         <v>232</v>
@@ -15428,7 +15428,7 @@
         <v>45169</v>
       </c>
       <c r="I394" s="196" t="s">
-        <v>1295</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="395" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15436,10 +15436,10 @@
       <c r="B395" s="109"/>
       <c r="C395" s="110"/>
       <c r="D395" s="167" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="E395" s="158" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="F395" s="151" t="s">
         <v>232</v>
@@ -15451,7 +15451,7 @@
         <v>45163</v>
       </c>
       <c r="I395" s="196" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="396" spans="1:9" s="78" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -15459,10 +15459,10 @@
       <c r="B396" s="109"/>
       <c r="C396" s="110"/>
       <c r="D396" s="167" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="E396" s="158" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="F396" s="151" t="s">
         <v>232</v>
@@ -15474,7 +15474,7 @@
         <v>45166</v>
       </c>
       <c r="I396" s="196" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="397" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -15482,10 +15482,10 @@
       <c r="B397" s="109"/>
       <c r="C397" s="110"/>
       <c r="D397" s="165" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="E397" s="159" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="F397" s="150" t="s">
         <v>232</v>
@@ -15497,7 +15497,7 @@
         <v>45162</v>
       </c>
       <c r="I397" s="209" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="398" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -15516,10 +15516,10 @@
       <c r="B399" s="109"/>
       <c r="C399" s="110"/>
       <c r="D399" s="165" t="s">
-        <v>1337</v>
+        <v>1334</v>
       </c>
       <c r="E399" s="159" t="s">
-        <v>1338</v>
+        <v>1335</v>
       </c>
       <c r="F399" s="151" t="s">
         <v>232</v>
@@ -15562,10 +15562,10 @@
       <c r="B401" s="109"/>
       <c r="C401" s="110"/>
       <c r="D401" s="165" t="s">
-        <v>1339</v>
+        <v>1336</v>
       </c>
       <c r="E401" s="159" t="s">
-        <v>1340</v>
+        <v>1337</v>
       </c>
       <c r="F401" s="151" t="s">
         <v>232</v>
@@ -15608,10 +15608,10 @@
       <c r="B403" s="109"/>
       <c r="C403" s="110"/>
       <c r="D403" s="167" t="s">
-        <v>1333</v>
+        <v>1330</v>
       </c>
       <c r="E403" s="158" t="s">
-        <v>1335</v>
+        <v>1332</v>
       </c>
       <c r="F403" s="151" t="s">
         <v>232</v>
@@ -15631,10 +15631,10 @@
       <c r="B404" s="109"/>
       <c r="C404" s="110"/>
       <c r="D404" s="167" t="s">
-        <v>1320</v>
+        <v>1317</v>
       </c>
       <c r="E404" s="217" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="F404" s="151" t="s">
         <v>232</v>
@@ -15654,10 +15654,10 @@
       <c r="B405" s="109"/>
       <c r="C405" s="110"/>
       <c r="D405" s="167" t="s">
-        <v>1343</v>
+        <v>1340</v>
       </c>
       <c r="E405" s="217" t="s">
-        <v>1344</v>
+        <v>1341</v>
       </c>
       <c r="F405" s="151" t="s">
         <v>232</v>
@@ -15677,10 +15677,10 @@
       <c r="B406" s="109"/>
       <c r="C406" s="110"/>
       <c r="D406" s="167" t="s">
-        <v>1334</v>
+        <v>1331</v>
       </c>
       <c r="E406" s="217" t="s">
-        <v>1336</v>
+        <v>1333</v>
       </c>
       <c r="F406" s="151" t="s">
         <v>232</v>
@@ -15700,10 +15700,10 @@
       <c r="B407" s="109"/>
       <c r="C407" s="110"/>
       <c r="D407" s="165" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="E407" s="159" t="s">
-        <v>1323</v>
+        <v>1320</v>
       </c>
       <c r="F407" s="151" t="s">
         <v>232</v>
@@ -15814,10 +15814,10 @@
       <c r="B413" s="109"/>
       <c r="C413" s="110"/>
       <c r="D413" s="167" t="s">
-        <v>1477</v>
+        <v>1472</v>
       </c>
       <c r="E413" s="160" t="s">
-        <v>1480</v>
+        <v>1475</v>
       </c>
       <c r="F413" s="150" t="s">
         <v>232</v>
@@ -15837,10 +15837,10 @@
       <c r="B414" s="109"/>
       <c r="C414" s="110"/>
       <c r="D414" s="167" t="s">
-        <v>1478</v>
+        <v>1473</v>
       </c>
       <c r="E414" s="160" t="s">
-        <v>1479</v>
+        <v>1474</v>
       </c>
       <c r="F414" s="150" t="s">
         <v>232</v>
@@ -15940,10 +15940,10 @@
       <c r="B419" s="109"/>
       <c r="C419" s="110"/>
       <c r="D419" s="167" t="s">
-        <v>1327</v>
+        <v>1324</v>
       </c>
       <c r="E419" s="160" t="s">
-        <v>1326</v>
+        <v>1323</v>
       </c>
       <c r="F419" s="151" t="s">
         <v>232</v>
@@ -16066,10 +16066,10 @@
       <c r="B425" s="109"/>
       <c r="C425" s="110"/>
       <c r="D425" s="167" t="s">
-        <v>1473</v>
+        <v>1468</v>
       </c>
       <c r="E425" s="158" t="s">
-        <v>1474</v>
+        <v>1469</v>
       </c>
       <c r="F425" s="151" t="s">
         <v>232</v>
@@ -16081,7 +16081,7 @@
         <v>45203</v>
       </c>
       <c r="I425" s="196" t="s">
-        <v>1475</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="426" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
@@ -16513,10 +16513,10 @@
       <c r="B446" s="109"/>
       <c r="C446" s="110"/>
       <c r="D446" s="167" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="E446" s="158" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="F446" s="151" t="s">
         <v>232</v>
@@ -16536,10 +16536,10 @@
       <c r="B447" s="109"/>
       <c r="C447" s="110"/>
       <c r="D447" s="167" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
       <c r="E447" s="158" t="s">
-        <v>1330</v>
+        <v>1327</v>
       </c>
       <c r="F447" s="151" t="s">
         <v>232</v>
@@ -16559,10 +16559,10 @@
       <c r="B448" s="109"/>
       <c r="C448" s="110"/>
       <c r="D448" s="167" t="s">
-        <v>1328</v>
+        <v>1325</v>
       </c>
       <c r="E448" s="158" t="s">
-        <v>1329</v>
+        <v>1326</v>
       </c>
       <c r="F448" s="151" t="s">
         <v>232</v>
@@ -16582,10 +16582,10 @@
       <c r="B449" s="109"/>
       <c r="C449" s="110"/>
       <c r="D449" s="167" t="s">
-        <v>1490</v>
+        <v>1485</v>
       </c>
       <c r="E449" s="158" t="s">
-        <v>1491</v>
+        <v>1486</v>
       </c>
       <c r="F449" s="151" t="s">
         <v>281</v>
@@ -16605,10 +16605,10 @@
       <c r="B450" s="109"/>
       <c r="C450" s="110"/>
       <c r="D450" s="167" t="s">
-        <v>1492</v>
+        <v>1487</v>
       </c>
       <c r="E450" s="158" t="s">
-        <v>1493</v>
+        <v>1488</v>
       </c>
       <c r="F450" s="151" t="s">
         <v>686</v>
@@ -16628,10 +16628,10 @@
       <c r="B451" s="109"/>
       <c r="C451" s="110"/>
       <c r="D451" s="165" t="s">
-        <v>1331</v>
+        <v>1328</v>
       </c>
       <c r="E451" s="159" t="s">
-        <v>1332</v>
+        <v>1329</v>
       </c>
       <c r="F451" s="151" t="s">
         <v>232</v>
@@ -16662,10 +16662,10 @@
       <c r="B453" s="109"/>
       <c r="C453" s="110"/>
       <c r="D453" s="167" t="s">
-        <v>1469</v>
+        <v>1464</v>
       </c>
       <c r="E453" s="158" t="s">
-        <v>1470</v>
+        <v>1465</v>
       </c>
       <c r="F453" s="151" t="s">
         <v>232</v>
@@ -16685,10 +16685,10 @@
       <c r="B454" s="109"/>
       <c r="C454" s="110"/>
       <c r="D454" s="167" t="s">
-        <v>1471</v>
+        <v>1466</v>
       </c>
       <c r="E454" s="158" t="s">
-        <v>1472</v>
+        <v>1467</v>
       </c>
       <c r="F454" s="151" t="s">
         <v>232</v>
@@ -17153,10 +17153,10 @@
       <c r="B478" s="109"/>
       <c r="C478" s="110"/>
       <c r="D478" s="166" t="s">
-        <v>1464</v>
+        <v>1459</v>
       </c>
       <c r="E478" s="157" t="s">
-        <v>1465</v>
+        <v>1460</v>
       </c>
       <c r="F478" s="150" t="s">
         <v>232</v>
@@ -17168,7 +17168,7 @@
         <v>45203</v>
       </c>
       <c r="I478" s="195" t="s">
-        <v>1466</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="479" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -17176,10 +17176,10 @@
       <c r="B479" s="109"/>
       <c r="C479" s="110"/>
       <c r="D479" s="166" t="s">
-        <v>1342</v>
+        <v>1339</v>
       </c>
       <c r="E479" s="157" t="s">
-        <v>1341</v>
+        <v>1338</v>
       </c>
       <c r="F479" s="150" t="s">
         <v>232</v>
@@ -17884,10 +17884,10 @@
       <c r="B515" s="109"/>
       <c r="C515" s="110"/>
       <c r="D515" s="167" t="s">
-        <v>1382</v>
+        <v>1379</v>
       </c>
       <c r="E515" s="158" t="s">
-        <v>1383</v>
+        <v>1380</v>
       </c>
       <c r="F515" s="151" t="s">
         <v>232</v>
@@ -17907,10 +17907,10 @@
       <c r="B516" s="109"/>
       <c r="C516" s="110"/>
       <c r="D516" s="167" t="s">
-        <v>1381</v>
+        <v>1378</v>
       </c>
       <c r="E516" s="158" t="s">
-        <v>1380</v>
+        <v>1377</v>
       </c>
       <c r="F516" s="151" t="s">
         <v>232</v>
@@ -19484,10 +19484,10 @@
       <c r="B595" s="109"/>
       <c r="C595" s="110"/>
       <c r="D595" s="165" t="s">
-        <v>1384</v>
+        <v>1381</v>
       </c>
       <c r="E595" s="159" t="s">
-        <v>1385</v>
+        <v>1382</v>
       </c>
       <c r="F595" s="148" t="s">
         <v>232</v>
@@ -19499,7 +19499,7 @@
         <v>45194</v>
       </c>
       <c r="I595" s="209" t="s">
-        <v>1386</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="596" spans="1:9" s="78" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21106,10 +21106,10 @@
       <c r="B687" s="109"/>
       <c r="C687" s="110"/>
       <c r="D687" s="167" t="s">
-        <v>1508</v>
+        <v>1528</v>
       </c>
       <c r="E687" s="158" t="s">
-        <v>1511</v>
+        <v>1529</v>
       </c>
       <c r="F687" s="151" t="s">
         <v>232</v>
@@ -21129,10 +21129,10 @@
       <c r="B688" s="109"/>
       <c r="C688" s="110"/>
       <c r="D688" s="167" t="s">
-        <v>1509</v>
+        <v>1530</v>
       </c>
       <c r="E688" s="158" t="s">
-        <v>1510</v>
+        <v>1531</v>
       </c>
       <c r="F688" s="151" t="s">
         <v>232</v>
@@ -21152,10 +21152,10 @@
       <c r="B689" s="109"/>
       <c r="C689" s="110"/>
       <c r="D689" s="167" t="s">
-        <v>1512</v>
+        <v>1532</v>
       </c>
       <c r="E689" s="158" t="s">
-        <v>1514</v>
+        <v>1533</v>
       </c>
       <c r="F689" s="151" t="s">
         <v>232</v>
@@ -21175,10 +21175,10 @@
       <c r="B690" s="109"/>
       <c r="C690" s="110"/>
       <c r="D690" s="167" t="s">
-        <v>1513</v>
+        <v>1534</v>
       </c>
       <c r="E690" s="158" t="s">
-        <v>1515</v>
+        <v>1535</v>
       </c>
       <c r="F690" s="151" t="s">
         <v>232</v>
@@ -21198,10 +21198,10 @@
       <c r="B691" s="109"/>
       <c r="C691" s="110"/>
       <c r="D691" s="167" t="s">
-        <v>1516</v>
+        <v>1536</v>
       </c>
       <c r="E691" s="158" t="s">
-        <v>1519</v>
+        <v>1537</v>
       </c>
       <c r="F691" s="151" t="s">
         <v>232</v>
@@ -21221,10 +21221,10 @@
       <c r="B692" s="109"/>
       <c r="C692" s="110"/>
       <c r="D692" s="167" t="s">
-        <v>1517</v>
+        <v>1538</v>
       </c>
       <c r="E692" s="158" t="s">
-        <v>1518</v>
+        <v>1539</v>
       </c>
       <c r="F692" s="151" t="s">
         <v>232</v>
@@ -21463,10 +21463,10 @@
       <c r="B708" s="109"/>
       <c r="C708" s="110"/>
       <c r="D708" s="166" t="s">
-        <v>1308</v>
+        <v>1305</v>
       </c>
       <c r="E708" s="162" t="s">
-        <v>1310</v>
+        <v>1307</v>
       </c>
       <c r="F708" s="150" t="s">
         <v>232</v>
@@ -21486,10 +21486,10 @@
       <c r="B709" s="109"/>
       <c r="C709" s="110"/>
       <c r="D709" s="167" t="s">
-        <v>1309</v>
+        <v>1306</v>
       </c>
       <c r="E709" s="160" t="s">
-        <v>1311</v>
+        <v>1308</v>
       </c>
       <c r="F709" s="151" t="s">
         <v>232</v>
@@ -21509,10 +21509,10 @@
       <c r="B710" s="109"/>
       <c r="C710" s="110"/>
       <c r="D710" s="167" t="s">
-        <v>1313</v>
+        <v>1310</v>
       </c>
       <c r="E710" s="160" t="s">
-        <v>1312</v>
+        <v>1309</v>
       </c>
       <c r="F710" s="151" t="s">
         <v>232</v>
@@ -21532,10 +21532,10 @@
       <c r="B711" s="109"/>
       <c r="C711" s="110"/>
       <c r="D711" s="167" t="s">
-        <v>1314</v>
+        <v>1311</v>
       </c>
       <c r="E711" s="160" t="s">
-        <v>1315</v>
+        <v>1312</v>
       </c>
       <c r="F711" s="151" t="s">
         <v>232</v>
@@ -21694,7 +21694,7 @@
       <c r="B719" s="109"/>
       <c r="C719" s="110"/>
       <c r="D719" s="167" t="s">
-        <v>1530</v>
+        <v>1507</v>
       </c>
       <c r="E719" s="160" t="s">
         <v>763</v>
@@ -21740,7 +21740,7 @@
       <c r="B721" s="109"/>
       <c r="C721" s="110"/>
       <c r="D721" s="167" t="s">
-        <v>1531</v>
+        <v>1508</v>
       </c>
       <c r="E721" s="160" t="s">
         <v>766</v>
@@ -21763,10 +21763,10 @@
       <c r="B722" s="109"/>
       <c r="C722" s="110"/>
       <c r="D722" s="167" t="s">
-        <v>1532</v>
+        <v>1509</v>
       </c>
       <c r="E722" s="160" t="s">
-        <v>1534</v>
+        <v>1511</v>
       </c>
       <c r="F722" s="151" t="s">
         <v>232</v>
@@ -21786,10 +21786,10 @@
       <c r="B723" s="109"/>
       <c r="C723" s="110"/>
       <c r="D723" s="167" t="s">
-        <v>1533</v>
+        <v>1510</v>
       </c>
       <c r="E723" s="160" t="s">
-        <v>1535</v>
+        <v>1512</v>
       </c>
       <c r="F723" s="151" t="s">
         <v>232</v>
@@ -21809,10 +21809,10 @@
       <c r="B724" s="109"/>
       <c r="C724" s="110"/>
       <c r="D724" s="167" t="s">
-        <v>1536</v>
+        <v>1513</v>
       </c>
       <c r="E724" s="160" t="s">
-        <v>1538</v>
+        <v>1515</v>
       </c>
       <c r="F724" s="151" t="s">
         <v>281</v>
@@ -21832,10 +21832,10 @@
       <c r="B725" s="109"/>
       <c r="C725" s="110"/>
       <c r="D725" s="167" t="s">
-        <v>1537</v>
+        <v>1514</v>
       </c>
       <c r="E725" s="160" t="s">
-        <v>1539</v>
+        <v>1516</v>
       </c>
       <c r="F725" s="151" t="s">
         <v>281</v>
@@ -22042,10 +22042,10 @@
       <c r="B741" s="109"/>
       <c r="C741" s="110"/>
       <c r="D741" s="166" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="E741" s="162" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="F741" s="150" t="s">
         <v>267</v>
@@ -22065,10 +22065,10 @@
       <c r="B742" s="109"/>
       <c r="C742" s="110"/>
       <c r="D742" s="167" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="E742" s="160" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="F742" s="151" t="s">
         <v>267</v>
@@ -23885,30 +23885,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B682:B683"/>
-    <mergeCell ref="C683:C684"/>
-    <mergeCell ref="C374:C375"/>
-    <mergeCell ref="B678:B679"/>
-    <mergeCell ref="C679:C680"/>
-    <mergeCell ref="C520:C521"/>
-    <mergeCell ref="C672:C673"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="C300:C301"/>
-    <mergeCell ref="C802:C803"/>
-    <mergeCell ref="C706:C707"/>
-    <mergeCell ref="C713:C714"/>
-    <mergeCell ref="C738:C739"/>
-    <mergeCell ref="C744:C745"/>
-    <mergeCell ref="C748:C749"/>
-    <mergeCell ref="C307:C308"/>
-    <mergeCell ref="C316:C317"/>
-    <mergeCell ref="C355:C356"/>
-    <mergeCell ref="C657:C658"/>
     <mergeCell ref="B812:B813"/>
     <mergeCell ref="C813:C814"/>
     <mergeCell ref="I2:I3"/>
@@ -23925,6 +23901,30 @@
     <mergeCell ref="C95:C96"/>
     <mergeCell ref="C150:C151"/>
     <mergeCell ref="C165:C166"/>
+    <mergeCell ref="C192:C193"/>
+    <mergeCell ref="C300:C301"/>
+    <mergeCell ref="C802:C803"/>
+    <mergeCell ref="C706:C707"/>
+    <mergeCell ref="C713:C714"/>
+    <mergeCell ref="C738:C739"/>
+    <mergeCell ref="C744:C745"/>
+    <mergeCell ref="C748:C749"/>
+    <mergeCell ref="C307:C308"/>
+    <mergeCell ref="C316:C317"/>
+    <mergeCell ref="C355:C356"/>
+    <mergeCell ref="C657:C658"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B682:B683"/>
+    <mergeCell ref="C683:C684"/>
+    <mergeCell ref="C374:C375"/>
+    <mergeCell ref="B678:B679"/>
+    <mergeCell ref="C679:C680"/>
+    <mergeCell ref="C520:C521"/>
+    <mergeCell ref="C672:C673"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -23977,20 +23977,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="251" t="s">
+      <c r="B2" s="268" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="252"/>
-      <c r="D2" s="253"/>
-      <c r="E2" s="248" t="s">
+      <c r="C2" s="269"/>
+      <c r="D2" s="270"/>
+      <c r="E2" s="265" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="250"/>
-      <c r="G2" s="248" t="s">
+      <c r="F2" s="267"/>
+      <c r="G2" s="265" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="249"/>
-      <c r="I2" s="250"/>
+      <c r="H2" s="266"/>
+      <c r="I2" s="267"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -24011,10 +24011,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="254" t="s">
+      <c r="H3" s="271" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="255"/>
+      <c r="I3" s="272"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -24049,8 +24049,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="268"/>
-      <c r="I6" s="269"/>
+      <c r="H6" s="246"/>
+      <c r="I6" s="247"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -24092,7 +24092,7 @@
       <c r="F8" s="262" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="265" t="s">
+      <c r="G8" s="253" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -24108,11 +24108,11 @@
       <c r="D9" s="260"/>
       <c r="E9" s="35"/>
       <c r="F9" s="263"/>
-      <c r="G9" s="266"/>
-      <c r="H9" s="246" t="s">
+      <c r="G9" s="254"/>
+      <c r="H9" s="248" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="247"/>
+      <c r="I9" s="249"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -24120,7 +24120,7 @@
       <c r="D10" s="261"/>
       <c r="E10" s="36"/>
       <c r="F10" s="264"/>
-      <c r="G10" s="267"/>
+      <c r="G10" s="255"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -24160,13 +24160,13 @@
       <c r="D12" s="259" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="270" t="s">
+      <c r="E12" s="250" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="262" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="265" t="s">
+      <c r="G12" s="253" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -24181,22 +24181,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="257"/>
       <c r="D13" s="260"/>
-      <c r="E13" s="271"/>
+      <c r="E13" s="251"/>
       <c r="F13" s="263"/>
-      <c r="G13" s="266"/>
-      <c r="H13" s="246" t="s">
+      <c r="G13" s="254"/>
+      <c r="H13" s="248" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="247"/>
+      <c r="I13" s="249"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="258"/>
       <c r="D14" s="261"/>
-      <c r="E14" s="272"/>
+      <c r="E14" s="252"/>
       <c r="F14" s="264"/>
-      <c r="G14" s="267"/>
+      <c r="G14" s="255"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -24306,7 +24306,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="265" t="s">
+      <c r="G21" s="253" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -24326,7 +24326,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="267"/>
+      <c r="G22" s="255"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -24371,8 +24371,8 @@
       <c r="E25" s="25"/>
       <c r="F25" s="22"/>
       <c r="G25" s="25"/>
-      <c r="H25" s="268"/>
-      <c r="I25" s="269"/>
+      <c r="H25" s="246"/>
+      <c r="I25" s="247"/>
     </row>
     <row r="26" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="67" t="s">
@@ -24792,13 +24792,13 @@
       <c r="D49" s="259" t="s">
         <v>43</v>
       </c>
-      <c r="E49" s="270" t="s">
+      <c r="E49" s="250" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="262" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="265" t="s">
+      <c r="G49" s="253" t="s">
         <v>47</v>
       </c>
       <c r="H49" s="6" t="s">
@@ -24812,21 +24812,21 @@
       <c r="B50" s="61"/>
       <c r="C50" s="257"/>
       <c r="D50" s="260"/>
-      <c r="E50" s="271"/>
+      <c r="E50" s="251"/>
       <c r="F50" s="263"/>
-      <c r="G50" s="266"/>
-      <c r="H50" s="246" t="s">
+      <c r="G50" s="254"/>
+      <c r="H50" s="248" t="s">
         <v>32</v>
       </c>
-      <c r="I50" s="247"/>
+      <c r="I50" s="249"/>
     </row>
     <row r="51" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B51" s="61"/>
       <c r="C51" s="258"/>
       <c r="D51" s="261"/>
-      <c r="E51" s="272"/>
+      <c r="E51" s="252"/>
       <c r="F51" s="264"/>
-      <c r="G51" s="267"/>
+      <c r="G51" s="255"/>
       <c r="H51" s="8" t="s">
         <v>23</v>
       </c>
@@ -24866,13 +24866,13 @@
       <c r="D53" s="259" t="s">
         <v>53</v>
       </c>
-      <c r="E53" s="270" t="s">
+      <c r="E53" s="250" t="s">
         <v>55</v>
       </c>
       <c r="F53" s="262" t="s">
         <v>56</v>
       </c>
-      <c r="G53" s="265" t="s">
+      <c r="G53" s="253" t="s">
         <v>9</v>
       </c>
       <c r="H53" s="6" t="s">
@@ -24886,21 +24886,21 @@
       <c r="B54" s="61"/>
       <c r="C54" s="257"/>
       <c r="D54" s="260"/>
-      <c r="E54" s="271"/>
+      <c r="E54" s="251"/>
       <c r="F54" s="263"/>
-      <c r="G54" s="266"/>
-      <c r="H54" s="246" t="s">
+      <c r="G54" s="254"/>
+      <c r="H54" s="248" t="s">
         <v>32</v>
       </c>
-      <c r="I54" s="247"/>
+      <c r="I54" s="249"/>
     </row>
     <row r="55" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B55" s="61"/>
       <c r="C55" s="258"/>
       <c r="D55" s="261"/>
-      <c r="E55" s="272"/>
+      <c r="E55" s="252"/>
       <c r="F55" s="264"/>
-      <c r="G55" s="267"/>
+      <c r="G55" s="255"/>
       <c r="H55" s="8" t="s">
         <v>23</v>
       </c>
@@ -24925,8 +24925,8 @@
       <c r="E57" s="25"/>
       <c r="F57" s="22"/>
       <c r="G57" s="25"/>
-      <c r="H57" s="268"/>
-      <c r="I57" s="269"/>
+      <c r="H57" s="246"/>
+      <c r="I57" s="247"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="61" t="s">
@@ -24989,10 +24989,10 @@
       <c r="E61" s="39"/>
       <c r="F61" s="12"/>
       <c r="G61" s="32"/>
-      <c r="H61" s="246" t="s">
+      <c r="H61" s="248" t="s">
         <v>32</v>
       </c>
-      <c r="I61" s="247"/>
+      <c r="I61" s="249"/>
     </row>
     <row r="62" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B62" s="61"/>
@@ -25025,8 +25025,8 @@
       <c r="E64" s="25"/>
       <c r="F64" s="22"/>
       <c r="G64" s="25"/>
-      <c r="H64" s="268"/>
-      <c r="I64" s="269"/>
+      <c r="H64" s="246"/>
+      <c r="I64" s="247"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="64" t="s">
@@ -25439,8 +25439,8 @@
       <c r="E92" s="25"/>
       <c r="F92" s="22"/>
       <c r="G92" s="25"/>
-      <c r="H92" s="268"/>
-      <c r="I92" s="269"/>
+      <c r="H92" s="246"/>
+      <c r="I92" s="247"/>
     </row>
     <row r="93" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="61"/>
@@ -25584,22 +25584,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H92:I92"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="G53:G55"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="F53:F55"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="F49:F51"/>
-    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -25612,16 +25606,22 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="D53:D55"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="G49:G51"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H92:I92"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="E53:E55"/>
+    <mergeCell ref="G53:G55"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="H64:I64"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -25655,10 +25655,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="274"/>
-      <c r="D2" s="249" t="s">
+      <c r="D2" s="266" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="250" t="s">
+      <c r="E2" s="267" t="s">
         <v>0</v>
       </c>
     </row>
@@ -25669,8 +25669,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="254"/>
-      <c r="E3" s="255"/>
+      <c r="D3" s="271"/>
+      <c r="E3" s="272"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 7 Desember 2023 17:26 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2781" uniqueCount="1646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="1650">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -5577,6 +5577,18 @@
   <si>
     <t>SchData-Warehouse-Log.
 HoldFunc_GetDataList_Log_TransactionHistory</t>
+  </si>
+  <si>
+    <t>Func_General_GetJSONOfTableRecordByID</t>
+  </si>
+  <si>
+    <t>Func_General_SetTransactionHistory</t>
+  </si>
+  <si>
+    <t>Menyimpan Transaction History</t>
+  </si>
+  <si>
+    <t>Menampilkan JSON dari Record Table berdasarkan ID (varID)</t>
   </si>
 </sst>
 </file>
@@ -7144,21 +7156,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7177,35 +7174,50 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -7234,29 +7246,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8474,7 +8486,7 @@
       <pane xSplit="4" ySplit="3" topLeftCell="E404" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D410" sqref="D410"/>
+      <selection pane="bottomRight" activeCell="E407" sqref="E407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8493,20 +8505,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="242" t="s">
+      <c r="B2" s="248" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="243"/>
-      <c r="D2" s="244"/>
-      <c r="E2" s="249" t="s">
+      <c r="C2" s="249"/>
+      <c r="D2" s="250"/>
+      <c r="E2" s="244" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="245" t="s">
+      <c r="F2" s="240" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="246"/>
-      <c r="H2" s="247"/>
-      <c r="I2" s="240" t="s">
+      <c r="G2" s="241"/>
+      <c r="H2" s="242"/>
+      <c r="I2" s="246" t="s">
         <v>662</v>
       </c>
     </row>
@@ -8520,7 +8532,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="250"/>
+      <c r="E3" s="245"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -8530,11 +8542,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="241"/>
+      <c r="I3" s="247"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="248" t="s">
+      <c r="B4" s="243" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="221"/>
@@ -16019,23 +16031,47 @@
       <c r="A407" s="1"/>
       <c r="B407" s="109"/>
       <c r="C407" s="110"/>
-      <c r="D407" s="167"/>
-      <c r="E407" s="160"/>
-      <c r="F407" s="151"/>
-      <c r="G407" s="180"/>
-      <c r="H407" s="192"/>
-      <c r="I407" s="196"/>
+      <c r="D407" s="167" t="s">
+        <v>1646</v>
+      </c>
+      <c r="E407" s="160" t="s">
+        <v>1649</v>
+      </c>
+      <c r="F407" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G407" s="180">
+        <v>45260</v>
+      </c>
+      <c r="H407" s="192">
+        <v>45260</v>
+      </c>
+      <c r="I407" s="196" t="s">
+        <v>703</v>
+      </c>
     </row>
     <row r="408" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A408" s="1"/>
       <c r="B408" s="109"/>
       <c r="C408" s="110"/>
-      <c r="D408" s="167"/>
-      <c r="E408" s="160"/>
-      <c r="F408" s="151"/>
-      <c r="G408" s="180"/>
-      <c r="H408" s="192"/>
-      <c r="I408" s="196"/>
+      <c r="D408" s="167" t="s">
+        <v>1647</v>
+      </c>
+      <c r="E408" s="160" t="s">
+        <v>1648</v>
+      </c>
+      <c r="F408" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G408" s="180">
+        <v>45266</v>
+      </c>
+      <c r="H408" s="192">
+        <v>45266</v>
+      </c>
+      <c r="I408" s="196" t="s">
+        <v>722</v>
+      </c>
     </row>
     <row r="409" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A409" s="1"/>
@@ -25559,31 +25595,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B728:B729"/>
-    <mergeCell ref="C729:C730"/>
-    <mergeCell ref="C415:C416"/>
-    <mergeCell ref="B724:B725"/>
-    <mergeCell ref="C725:C726"/>
-    <mergeCell ref="C566:C567"/>
-    <mergeCell ref="C718:C719"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="C216:C217"/>
-    <mergeCell ref="C325:C326"/>
-    <mergeCell ref="C866:C867"/>
-    <mergeCell ref="C756:C757"/>
-    <mergeCell ref="C763:C764"/>
-    <mergeCell ref="C802:C803"/>
-    <mergeCell ref="C808:C809"/>
-    <mergeCell ref="C812:C813"/>
-    <mergeCell ref="C332:C333"/>
-    <mergeCell ref="C341:C342"/>
-    <mergeCell ref="C381:C382"/>
-    <mergeCell ref="C703:C704"/>
-    <mergeCell ref="C405:C406"/>
     <mergeCell ref="B876:B877"/>
     <mergeCell ref="C877:C878"/>
     <mergeCell ref="I2:I3"/>
@@ -25600,6 +25611,31 @@
     <mergeCell ref="C101:C102"/>
     <mergeCell ref="C174:C175"/>
     <mergeCell ref="C189:C190"/>
+    <mergeCell ref="C216:C217"/>
+    <mergeCell ref="C325:C326"/>
+    <mergeCell ref="C866:C867"/>
+    <mergeCell ref="C756:C757"/>
+    <mergeCell ref="C763:C764"/>
+    <mergeCell ref="C802:C803"/>
+    <mergeCell ref="C808:C809"/>
+    <mergeCell ref="C812:C813"/>
+    <mergeCell ref="C332:C333"/>
+    <mergeCell ref="C341:C342"/>
+    <mergeCell ref="C381:C382"/>
+    <mergeCell ref="C703:C704"/>
+    <mergeCell ref="C405:C406"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B728:B729"/>
+    <mergeCell ref="C729:C730"/>
+    <mergeCell ref="C415:C416"/>
+    <mergeCell ref="B724:B725"/>
+    <mergeCell ref="C725:C726"/>
+    <mergeCell ref="C566:C567"/>
+    <mergeCell ref="C718:C719"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -25652,20 +25688,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="256" t="s">
+      <c r="B2" s="273" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="257"/>
-      <c r="D2" s="258"/>
-      <c r="E2" s="253" t="s">
+      <c r="C2" s="274"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="270" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="255"/>
-      <c r="G2" s="253" t="s">
+      <c r="F2" s="272"/>
+      <c r="G2" s="270" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="254"/>
-      <c r="I2" s="255"/>
+      <c r="H2" s="271"/>
+      <c r="I2" s="272"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -25686,10 +25722,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="259" t="s">
+      <c r="H3" s="276" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="260"/>
+      <c r="I3" s="277"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -25724,8 +25760,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="273"/>
-      <c r="I6" s="274"/>
+      <c r="H6" s="251"/>
+      <c r="I6" s="252"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -25767,7 +25803,7 @@
       <c r="F8" s="267" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="270" t="s">
+      <c r="G8" s="258" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -25783,11 +25819,11 @@
       <c r="D9" s="265"/>
       <c r="E9" s="35"/>
       <c r="F9" s="268"/>
-      <c r="G9" s="271"/>
-      <c r="H9" s="251" t="s">
+      <c r="G9" s="259"/>
+      <c r="H9" s="253" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="252"/>
+      <c r="I9" s="254"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -25795,7 +25831,7 @@
       <c r="D10" s="266"/>
       <c r="E10" s="36"/>
       <c r="F10" s="269"/>
-      <c r="G10" s="272"/>
+      <c r="G10" s="260"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -25835,13 +25871,13 @@
       <c r="D12" s="264" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="275" t="s">
+      <c r="E12" s="255" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="267" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="270" t="s">
+      <c r="G12" s="258" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -25856,22 +25892,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="262"/>
       <c r="D13" s="265"/>
-      <c r="E13" s="276"/>
+      <c r="E13" s="256"/>
       <c r="F13" s="268"/>
-      <c r="G13" s="271"/>
-      <c r="H13" s="251" t="s">
+      <c r="G13" s="259"/>
+      <c r="H13" s="253" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="252"/>
+      <c r="I13" s="254"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="263"/>
       <c r="D14" s="266"/>
-      <c r="E14" s="277"/>
+      <c r="E14" s="257"/>
       <c r="F14" s="269"/>
-      <c r="G14" s="272"/>
+      <c r="G14" s="260"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -25981,7 +26017,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="270" t="s">
+      <c r="G21" s="258" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -26001,7 +26037,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="272"/>
+      <c r="G22" s="260"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -26084,8 +26120,8 @@
       <c r="E28" s="25"/>
       <c r="F28" s="22"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="273"/>
-      <c r="I28" s="274"/>
+      <c r="H28" s="251"/>
+      <c r="I28" s="252"/>
     </row>
     <row r="29" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="67" t="s">
@@ -26505,13 +26541,13 @@
       <c r="D52" s="264" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="275" t="s">
+      <c r="E52" s="255" t="s">
         <v>45</v>
       </c>
       <c r="F52" s="267" t="s">
         <v>46</v>
       </c>
-      <c r="G52" s="270" t="s">
+      <c r="G52" s="258" t="s">
         <v>47</v>
       </c>
       <c r="H52" s="6" t="s">
@@ -26525,21 +26561,21 @@
       <c r="B53" s="61"/>
       <c r="C53" s="262"/>
       <c r="D53" s="265"/>
-      <c r="E53" s="276"/>
+      <c r="E53" s="256"/>
       <c r="F53" s="268"/>
-      <c r="G53" s="271"/>
-      <c r="H53" s="251" t="s">
+      <c r="G53" s="259"/>
+      <c r="H53" s="253" t="s">
         <v>32</v>
       </c>
-      <c r="I53" s="252"/>
+      <c r="I53" s="254"/>
     </row>
     <row r="54" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B54" s="61"/>
       <c r="C54" s="263"/>
       <c r="D54" s="266"/>
-      <c r="E54" s="277"/>
+      <c r="E54" s="257"/>
       <c r="F54" s="269"/>
-      <c r="G54" s="272"/>
+      <c r="G54" s="260"/>
       <c r="H54" s="8" t="s">
         <v>23</v>
       </c>
@@ -26579,13 +26615,13 @@
       <c r="D56" s="264" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="275" t="s">
+      <c r="E56" s="255" t="s">
         <v>55</v>
       </c>
       <c r="F56" s="267" t="s">
         <v>56</v>
       </c>
-      <c r="G56" s="270" t="s">
+      <c r="G56" s="258" t="s">
         <v>9</v>
       </c>
       <c r="H56" s="6" t="s">
@@ -26599,21 +26635,21 @@
       <c r="B57" s="61"/>
       <c r="C57" s="262"/>
       <c r="D57" s="265"/>
-      <c r="E57" s="276"/>
+      <c r="E57" s="256"/>
       <c r="F57" s="268"/>
-      <c r="G57" s="271"/>
-      <c r="H57" s="251" t="s">
+      <c r="G57" s="259"/>
+      <c r="H57" s="253" t="s">
         <v>32</v>
       </c>
-      <c r="I57" s="252"/>
+      <c r="I57" s="254"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B58" s="61"/>
       <c r="C58" s="263"/>
       <c r="D58" s="266"/>
-      <c r="E58" s="277"/>
+      <c r="E58" s="257"/>
       <c r="F58" s="269"/>
-      <c r="G58" s="272"/>
+      <c r="G58" s="260"/>
       <c r="H58" s="8" t="s">
         <v>23</v>
       </c>
@@ -26638,8 +26674,8 @@
       <c r="E60" s="25"/>
       <c r="F60" s="22"/>
       <c r="G60" s="25"/>
-      <c r="H60" s="273"/>
-      <c r="I60" s="274"/>
+      <c r="H60" s="251"/>
+      <c r="I60" s="252"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="61" t="s">
@@ -26702,10 +26738,10 @@
       <c r="E64" s="39"/>
       <c r="F64" s="12"/>
       <c r="G64" s="32"/>
-      <c r="H64" s="251" t="s">
+      <c r="H64" s="253" t="s">
         <v>32</v>
       </c>
-      <c r="I64" s="252"/>
+      <c r="I64" s="254"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B65" s="61"/>
@@ -26738,8 +26774,8 @@
       <c r="E67" s="25"/>
       <c r="F67" s="22"/>
       <c r="G67" s="25"/>
-      <c r="H67" s="273"/>
-      <c r="I67" s="274"/>
+      <c r="H67" s="251"/>
+      <c r="I67" s="252"/>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="64" t="s">
@@ -27152,8 +27188,8 @@
       <c r="E95" s="25"/>
       <c r="F95" s="22"/>
       <c r="G95" s="25"/>
-      <c r="H95" s="273"/>
-      <c r="I95" s="274"/>
+      <c r="H95" s="251"/>
+      <c r="I95" s="252"/>
     </row>
     <row r="96" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="61"/>
@@ -27297,22 +27333,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -27325,16 +27355,22 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H67:I67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -27368,10 +27404,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="279"/>
-      <c r="D2" s="254" t="s">
+      <c r="D2" s="271" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="255" t="s">
+      <c r="E2" s="272" t="s">
         <v>0</v>
       </c>
     </row>
@@ -27382,8 +27418,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="259"/>
-      <c r="E3" s="260"/>
+      <c r="D3" s="276"/>
+      <c r="E3" s="277"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 24 Januari 2023 09:53 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -8602,10 +8602,10 @@
   <dimension ref="A1:I910"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E508" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E511" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D515" sqref="D515"/>
+      <selection pane="bottomRight" activeCell="F520" sqref="F520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update Pertanggal 3 April 2024 10:41 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -7481,6 +7481,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7499,50 +7514,35 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -7571,29 +7571,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -8892,10 +8892,10 @@
   <dimension ref="A1:I936"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="F96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E314" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I101" sqref="I101"/>
+      <selection pane="bottomRight" activeCell="E317" sqref="E317"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -8914,20 +8914,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="244" t="s">
+      <c r="B2" s="238" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="245"/>
-      <c r="D2" s="246"/>
-      <c r="E2" s="240" t="s">
+      <c r="C2" s="239"/>
+      <c r="D2" s="240"/>
+      <c r="E2" s="245" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="236" t="s">
+      <c r="F2" s="241" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="237"/>
-      <c r="H2" s="238"/>
-      <c r="I2" s="242" t="s">
+      <c r="G2" s="242"/>
+      <c r="H2" s="243"/>
+      <c r="I2" s="236" t="s">
         <v>662</v>
       </c>
     </row>
@@ -8941,7 +8941,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="241"/>
+      <c r="E3" s="246"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -8951,11 +8951,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="243"/>
+      <c r="I3" s="237"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="239" t="s">
+      <c r="B4" s="244" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="221"/>
@@ -26566,6 +26566,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B754:B755"/>
+    <mergeCell ref="C755:C756"/>
+    <mergeCell ref="C420:C421"/>
+    <mergeCell ref="B750:B751"/>
+    <mergeCell ref="C751:C752"/>
+    <mergeCell ref="C578:C579"/>
+    <mergeCell ref="C744:C745"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="C227:C228"/>
+    <mergeCell ref="C338:C339"/>
+    <mergeCell ref="C892:C893"/>
+    <mergeCell ref="C782:C783"/>
+    <mergeCell ref="C789:C790"/>
+    <mergeCell ref="C828:C829"/>
+    <mergeCell ref="C834:C835"/>
+    <mergeCell ref="C838:C839"/>
+    <mergeCell ref="C345:C346"/>
+    <mergeCell ref="C354:C355"/>
+    <mergeCell ref="C394:C395"/>
+    <mergeCell ref="C729:C730"/>
     <mergeCell ref="B902:B903"/>
     <mergeCell ref="C903:C904"/>
     <mergeCell ref="I2:I3"/>
@@ -26582,30 +26606,6 @@
     <mergeCell ref="C112:C113"/>
     <mergeCell ref="C185:C186"/>
     <mergeCell ref="C200:C201"/>
-    <mergeCell ref="C227:C228"/>
-    <mergeCell ref="C338:C339"/>
-    <mergeCell ref="C892:C893"/>
-    <mergeCell ref="C782:C783"/>
-    <mergeCell ref="C789:C790"/>
-    <mergeCell ref="C828:C829"/>
-    <mergeCell ref="C834:C835"/>
-    <mergeCell ref="C838:C839"/>
-    <mergeCell ref="C345:C346"/>
-    <mergeCell ref="C354:C355"/>
-    <mergeCell ref="C394:C395"/>
-    <mergeCell ref="C729:C730"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="B754:B755"/>
-    <mergeCell ref="C755:C756"/>
-    <mergeCell ref="C420:C421"/>
-    <mergeCell ref="B750:B751"/>
-    <mergeCell ref="C751:C752"/>
-    <mergeCell ref="C578:C579"/>
-    <mergeCell ref="C744:C745"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -26658,20 +26658,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="269" t="s">
+      <c r="B2" s="252" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="270"/>
-      <c r="D2" s="271"/>
-      <c r="E2" s="266" t="s">
+      <c r="C2" s="253"/>
+      <c r="D2" s="254"/>
+      <c r="E2" s="249" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="268"/>
-      <c r="G2" s="266" t="s">
+      <c r="F2" s="251"/>
+      <c r="G2" s="249" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="267"/>
-      <c r="I2" s="268"/>
+      <c r="H2" s="250"/>
+      <c r="I2" s="251"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -26692,10 +26692,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="272" t="s">
+      <c r="H3" s="255" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="273"/>
+      <c r="I3" s="256"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -26730,8 +26730,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="247"/>
-      <c r="I6" s="248"/>
+      <c r="H6" s="269"/>
+      <c r="I6" s="270"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -26773,7 +26773,7 @@
       <c r="F8" s="263" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="254" t="s">
+      <c r="G8" s="266" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -26789,11 +26789,11 @@
       <c r="D9" s="261"/>
       <c r="E9" s="35"/>
       <c r="F9" s="264"/>
-      <c r="G9" s="255"/>
-      <c r="H9" s="249" t="s">
+      <c r="G9" s="267"/>
+      <c r="H9" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="250"/>
+      <c r="I9" s="248"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -26801,7 +26801,7 @@
       <c r="D10" s="262"/>
       <c r="E10" s="36"/>
       <c r="F10" s="265"/>
-      <c r="G10" s="256"/>
+      <c r="G10" s="268"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -26841,13 +26841,13 @@
       <c r="D12" s="260" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="251" t="s">
+      <c r="E12" s="271" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="263" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="254" t="s">
+      <c r="G12" s="266" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -26862,22 +26862,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="258"/>
       <c r="D13" s="261"/>
-      <c r="E13" s="252"/>
+      <c r="E13" s="272"/>
       <c r="F13" s="264"/>
-      <c r="G13" s="255"/>
-      <c r="H13" s="249" t="s">
+      <c r="G13" s="267"/>
+      <c r="H13" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="250"/>
+      <c r="I13" s="248"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="259"/>
       <c r="D14" s="262"/>
-      <c r="E14" s="253"/>
+      <c r="E14" s="273"/>
       <c r="F14" s="265"/>
-      <c r="G14" s="256"/>
+      <c r="G14" s="268"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -26987,7 +26987,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="254" t="s">
+      <c r="G21" s="266" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -27007,7 +27007,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="256"/>
+      <c r="G22" s="268"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -27090,8 +27090,8 @@
       <c r="E28" s="25"/>
       <c r="F28" s="22"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="247"/>
-      <c r="I28" s="248"/>
+      <c r="H28" s="269"/>
+      <c r="I28" s="270"/>
     </row>
     <row r="29" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="67" t="s">
@@ -27511,13 +27511,13 @@
       <c r="D52" s="260" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="251" t="s">
+      <c r="E52" s="271" t="s">
         <v>45</v>
       </c>
       <c r="F52" s="263" t="s">
         <v>46</v>
       </c>
-      <c r="G52" s="254" t="s">
+      <c r="G52" s="266" t="s">
         <v>47</v>
       </c>
       <c r="H52" s="6" t="s">
@@ -27531,21 +27531,21 @@
       <c r="B53" s="61"/>
       <c r="C53" s="258"/>
       <c r="D53" s="261"/>
-      <c r="E53" s="252"/>
+      <c r="E53" s="272"/>
       <c r="F53" s="264"/>
-      <c r="G53" s="255"/>
-      <c r="H53" s="249" t="s">
+      <c r="G53" s="267"/>
+      <c r="H53" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="I53" s="250"/>
+      <c r="I53" s="248"/>
     </row>
     <row r="54" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B54" s="61"/>
       <c r="C54" s="259"/>
       <c r="D54" s="262"/>
-      <c r="E54" s="253"/>
+      <c r="E54" s="273"/>
       <c r="F54" s="265"/>
-      <c r="G54" s="256"/>
+      <c r="G54" s="268"/>
       <c r="H54" s="8" t="s">
         <v>23</v>
       </c>
@@ -27585,13 +27585,13 @@
       <c r="D56" s="260" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="251" t="s">
+      <c r="E56" s="271" t="s">
         <v>55</v>
       </c>
       <c r="F56" s="263" t="s">
         <v>56</v>
       </c>
-      <c r="G56" s="254" t="s">
+      <c r="G56" s="266" t="s">
         <v>9</v>
       </c>
       <c r="H56" s="6" t="s">
@@ -27605,21 +27605,21 @@
       <c r="B57" s="61"/>
       <c r="C57" s="258"/>
       <c r="D57" s="261"/>
-      <c r="E57" s="252"/>
+      <c r="E57" s="272"/>
       <c r="F57" s="264"/>
-      <c r="G57" s="255"/>
-      <c r="H57" s="249" t="s">
+      <c r="G57" s="267"/>
+      <c r="H57" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="I57" s="250"/>
+      <c r="I57" s="248"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B58" s="61"/>
       <c r="C58" s="259"/>
       <c r="D58" s="262"/>
-      <c r="E58" s="253"/>
+      <c r="E58" s="273"/>
       <c r="F58" s="265"/>
-      <c r="G58" s="256"/>
+      <c r="G58" s="268"/>
       <c r="H58" s="8" t="s">
         <v>23</v>
       </c>
@@ -27644,8 +27644,8 @@
       <c r="E60" s="25"/>
       <c r="F60" s="22"/>
       <c r="G60" s="25"/>
-      <c r="H60" s="247"/>
-      <c r="I60" s="248"/>
+      <c r="H60" s="269"/>
+      <c r="I60" s="270"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="61" t="s">
@@ -27708,10 +27708,10 @@
       <c r="E64" s="39"/>
       <c r="F64" s="12"/>
       <c r="G64" s="32"/>
-      <c r="H64" s="249" t="s">
+      <c r="H64" s="247" t="s">
         <v>32</v>
       </c>
-      <c r="I64" s="250"/>
+      <c r="I64" s="248"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B65" s="61"/>
@@ -27744,8 +27744,8 @@
       <c r="E67" s="25"/>
       <c r="F67" s="22"/>
       <c r="G67" s="25"/>
-      <c r="H67" s="247"/>
-      <c r="I67" s="248"/>
+      <c r="H67" s="269"/>
+      <c r="I67" s="270"/>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="64" t="s">
@@ -28158,8 +28158,8 @@
       <c r="E95" s="25"/>
       <c r="F95" s="22"/>
       <c r="G95" s="25"/>
-      <c r="H95" s="247"/>
-      <c r="I95" s="248"/>
+      <c r="H95" s="269"/>
+      <c r="I95" s="270"/>
     </row>
     <row r="96" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="61"/>
@@ -28303,16 +28303,22 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -28325,22 +28331,16 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -28374,10 +28374,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="275"/>
-      <c r="D2" s="267" t="s">
+      <c r="D2" s="250" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="268" t="s">
+      <c r="E2" s="251" t="s">
         <v>0</v>
       </c>
     </row>
@@ -28388,8 +28388,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="272"/>
-      <c r="E3" s="273"/>
+      <c r="D3" s="255"/>
+      <c r="E3" s="256"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>

<commit_message>
Update Pertanggal 15 Mei 2024 11:30 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
+++ b/Documentation/Documents/Blue Print/Documents - Model/Model-Catalogue.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3001" uniqueCount="1759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3009" uniqueCount="1763">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -6097,6 +6097,18 @@
   </si>
   <si>
     <t>Menginisialisasi ulang data pada tabel TblProjectSectionType</t>
+  </si>
+  <si>
+    <t>Func_TblMaterialProductComponent_INSERT</t>
+  </si>
+  <si>
+    <t>Func_TblMaterialProductComponent_UPDATE</t>
+  </si>
+  <si>
+    <t>Memasukan data (INSERT) pada tabel TblMaterialProductComponent</t>
+  </si>
+  <si>
+    <t>Memutakhirkan data (UPDATE) pada tabel TblMaterialProductComponent</t>
   </si>
 </sst>
 </file>
@@ -7655,21 +7667,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7688,35 +7685,50 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -7745,29 +7757,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -9063,13 +9075,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I968"/>
+  <dimension ref="A1:I973"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E744" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="E864" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D753" sqref="D753"/>
+      <selection pane="bottomRight" activeCell="D870" sqref="D870"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9088,20 +9100,20 @@
   <sheetData>
     <row r="1" spans="1:9" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="239" t="s">
+      <c r="B2" s="245" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="240"/>
-      <c r="D2" s="241"/>
-      <c r="E2" s="246" t="s">
+      <c r="C2" s="246"/>
+      <c r="D2" s="247"/>
+      <c r="E2" s="241" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="242" t="s">
+      <c r="F2" s="237" t="s">
         <v>231</v>
       </c>
-      <c r="G2" s="243"/>
-      <c r="H2" s="244"/>
-      <c r="I2" s="237" t="s">
+      <c r="G2" s="238"/>
+      <c r="H2" s="239"/>
+      <c r="I2" s="243" t="s">
         <v>662</v>
       </c>
     </row>
@@ -9115,7 +9127,7 @@
       <c r="D3" s="164" t="s">
         <v>226</v>
       </c>
-      <c r="E3" s="247"/>
+      <c r="E3" s="242"/>
       <c r="F3" s="141" t="s">
         <v>228</v>
       </c>
@@ -9125,11 +9137,11 @@
       <c r="H3" s="143" t="s">
         <v>230</v>
       </c>
-      <c r="I3" s="238"/>
+      <c r="I3" s="244"/>
     </row>
     <row r="4" spans="1:9" s="137" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="136"/>
-      <c r="B4" s="245" t="s">
+      <c r="B4" s="240" t="s">
         <v>141</v>
       </c>
       <c r="C4" s="221"/>
@@ -25582,199 +25594,163 @@
       <c r="H866" s="189"/>
       <c r="I866" s="212"/>
     </row>
-    <row r="867" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="867" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A867" s="1"/>
       <c r="B867" s="109"/>
-      <c r="C867" s="110"/>
-      <c r="D867" s="165"/>
-      <c r="E867" s="155"/>
-      <c r="F867" s="148"/>
-      <c r="G867" s="176"/>
-      <c r="H867" s="189"/>
-      <c r="I867" s="212"/>
+      <c r="C867" s="223"/>
+      <c r="D867" s="224"/>
+      <c r="E867" s="226"/>
+      <c r="F867" s="225"/>
+      <c r="G867" s="224"/>
+      <c r="H867" s="226"/>
+      <c r="I867" s="227"/>
     </row>
     <row r="868" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A868" s="1"/>
       <c r="B868" s="109"/>
-      <c r="C868" s="236" t="s">
-        <v>157</v>
-      </c>
-      <c r="D868" s="135"/>
-      <c r="E868" s="154"/>
-      <c r="F868" s="147"/>
-      <c r="G868" s="175"/>
-      <c r="H868" s="188"/>
-      <c r="I868" s="211"/>
+      <c r="C868" s="110"/>
+      <c r="D868" s="167"/>
+      <c r="E868" s="160"/>
+      <c r="F868" s="151"/>
+      <c r="G868" s="180"/>
+      <c r="H868" s="192"/>
+      <c r="I868" s="196"/>
     </row>
     <row r="869" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A869" s="1"/>
       <c r="B869" s="109"/>
-      <c r="C869" s="236"/>
-      <c r="D869" s="165"/>
-      <c r="E869" s="155"/>
-      <c r="F869" s="148"/>
-      <c r="G869" s="176"/>
-      <c r="H869" s="189"/>
-      <c r="I869" s="212"/>
-    </row>
-    <row r="870" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="C869" s="110"/>
+      <c r="D869" s="167"/>
+      <c r="E869" s="160"/>
+      <c r="F869" s="151"/>
+      <c r="G869" s="180"/>
+      <c r="H869" s="192"/>
+      <c r="I869" s="196"/>
+    </row>
+    <row r="870" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A870" s="1"/>
       <c r="B870" s="109"/>
       <c r="C870" s="110"/>
       <c r="D870" s="167" t="s">
-        <v>689</v>
-      </c>
-      <c r="E870" s="158" t="s">
-        <v>690</v>
+        <v>1759</v>
+      </c>
+      <c r="E870" s="160" t="s">
+        <v>1761</v>
       </c>
       <c r="F870" s="151" t="s">
-        <v>691</v>
+        <v>232</v>
       </c>
       <c r="G870" s="180">
-        <v>44859</v>
+        <v>44382</v>
       </c>
       <c r="H870" s="192">
-        <v>44477</v>
+        <v>44382</v>
       </c>
       <c r="I870" s="196" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="871" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="871" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A871" s="1"/>
       <c r="B871" s="109"/>
-      <c r="C871" s="223"/>
-      <c r="D871" s="224"/>
-      <c r="E871" s="226"/>
-      <c r="F871" s="225"/>
-      <c r="G871" s="224"/>
-      <c r="H871" s="226"/>
-      <c r="I871" s="227"/>
-    </row>
-    <row r="872" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C871" s="110"/>
+      <c r="D871" s="167" t="s">
+        <v>1760</v>
+      </c>
+      <c r="E871" s="160" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F871" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G871" s="180">
+        <v>44382</v>
+      </c>
+      <c r="H871" s="192">
+        <v>44382</v>
+      </c>
+      <c r="I871" s="196" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="872" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A872" s="1"/>
       <c r="B872" s="109"/>
       <c r="C872" s="110"/>
-      <c r="D872" s="167" t="s">
-        <v>1729</v>
-      </c>
-      <c r="E872" s="160" t="s">
-        <v>1731</v>
-      </c>
-      <c r="F872" s="151" t="s">
-        <v>266</v>
-      </c>
-      <c r="G872" s="180">
-        <v>45422</v>
-      </c>
-      <c r="H872" s="192">
-        <v>44384</v>
-      </c>
-      <c r="I872" s="196" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="873" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D872" s="165"/>
+      <c r="E872" s="155"/>
+      <c r="F872" s="148"/>
+      <c r="G872" s="176"/>
+      <c r="H872" s="189"/>
+      <c r="I872" s="212"/>
+    </row>
+    <row r="873" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A873" s="1"/>
       <c r="B873" s="109"/>
-      <c r="C873" s="110"/>
-      <c r="D873" s="167" t="s">
-        <v>1730</v>
-      </c>
-      <c r="E873" s="160" t="s">
-        <v>1732</v>
-      </c>
-      <c r="F873" s="151" t="s">
-        <v>266</v>
-      </c>
-      <c r="G873" s="180">
-        <v>45422</v>
-      </c>
-      <c r="H873" s="192">
-        <v>44384</v>
-      </c>
-      <c r="I873" s="196" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="874" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C873" s="236" t="s">
+        <v>157</v>
+      </c>
+      <c r="D873" s="135"/>
+      <c r="E873" s="154"/>
+      <c r="F873" s="147"/>
+      <c r="G873" s="175"/>
+      <c r="H873" s="188"/>
+      <c r="I873" s="211"/>
+    </row>
+    <row r="874" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A874" s="1"/>
       <c r="B874" s="109"/>
-      <c r="C874" s="110"/>
-      <c r="D874" s="167" t="s">
-        <v>1733</v>
-      </c>
-      <c r="E874" s="160" t="s">
-        <v>1735</v>
-      </c>
-      <c r="F874" s="151" t="s">
-        <v>266</v>
-      </c>
-      <c r="G874" s="180">
-        <v>45422</v>
-      </c>
-      <c r="H874" s="192">
-        <v>44308</v>
-      </c>
-      <c r="I874" s="196" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="875" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C874" s="236"/>
+      <c r="D874" s="165"/>
+      <c r="E874" s="155"/>
+      <c r="F874" s="148"/>
+      <c r="G874" s="176"/>
+      <c r="H874" s="189"/>
+      <c r="I874" s="212"/>
+    </row>
+    <row r="875" spans="1:9" s="78" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A875" s="1"/>
       <c r="B875" s="109"/>
       <c r="C875" s="110"/>
       <c r="D875" s="167" t="s">
-        <v>1734</v>
-      </c>
-      <c r="E875" s="160" t="s">
-        <v>1736</v>
+        <v>689</v>
+      </c>
+      <c r="E875" s="158" t="s">
+        <v>690</v>
       </c>
       <c r="F875" s="151" t="s">
-        <v>266</v>
+        <v>691</v>
       </c>
       <c r="G875" s="180">
-        <v>45422</v>
+        <v>44859</v>
       </c>
       <c r="H875" s="192">
-        <v>44308</v>
+        <v>44477</v>
       </c>
       <c r="I875" s="196" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="876" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="876" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A876" s="1"/>
       <c r="B876" s="109"/>
-      <c r="C876" s="110"/>
-      <c r="D876" s="167" t="s">
-        <v>1737</v>
-      </c>
-      <c r="E876" s="160" t="s">
-        <v>1739</v>
-      </c>
-      <c r="F876" s="151" t="s">
-        <v>266</v>
-      </c>
-      <c r="G876" s="180">
-        <v>45422</v>
-      </c>
-      <c r="H876" s="192">
-        <v>44308</v>
-      </c>
-      <c r="I876" s="196" t="s">
-        <v>719</v>
-      </c>
+      <c r="C876" s="223"/>
+      <c r="D876" s="224"/>
+      <c r="E876" s="226"/>
+      <c r="F876" s="225"/>
+      <c r="G876" s="224"/>
+      <c r="H876" s="226"/>
+      <c r="I876" s="227"/>
     </row>
     <row r="877" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A877" s="1"/>
       <c r="B877" s="109"/>
       <c r="C877" s="110"/>
       <c r="D877" s="167" t="s">
-        <v>1738</v>
+        <v>1729</v>
       </c>
       <c r="E877" s="160" t="s">
-        <v>1740</v>
+        <v>1731</v>
       </c>
       <c r="F877" s="151" t="s">
         <v>266</v>
@@ -25783,7 +25759,7 @@
         <v>45422</v>
       </c>
       <c r="H877" s="192">
-        <v>44308</v>
+        <v>44384</v>
       </c>
       <c r="I877" s="196" t="s">
         <v>719</v>
@@ -25794,10 +25770,10 @@
       <c r="B878" s="109"/>
       <c r="C878" s="110"/>
       <c r="D878" s="167" t="s">
-        <v>1741</v>
+        <v>1730</v>
       </c>
       <c r="E878" s="160" t="s">
-        <v>1743</v>
+        <v>1732</v>
       </c>
       <c r="F878" s="151" t="s">
         <v>266</v>
@@ -25806,7 +25782,7 @@
         <v>45422</v>
       </c>
       <c r="H878" s="192">
-        <v>44711</v>
+        <v>44384</v>
       </c>
       <c r="I878" s="196" t="s">
         <v>719</v>
@@ -25817,10 +25793,10 @@
       <c r="B879" s="109"/>
       <c r="C879" s="110"/>
       <c r="D879" s="167" t="s">
-        <v>1742</v>
+        <v>1733</v>
       </c>
       <c r="E879" s="160" t="s">
-        <v>1744</v>
+        <v>1735</v>
       </c>
       <c r="F879" s="151" t="s">
         <v>266</v>
@@ -25829,7 +25805,7 @@
         <v>45422</v>
       </c>
       <c r="H879" s="192">
-        <v>44711</v>
+        <v>44308</v>
       </c>
       <c r="I879" s="196" t="s">
         <v>719</v>
@@ -25840,10 +25816,10 @@
       <c r="B880" s="109"/>
       <c r="C880" s="110"/>
       <c r="D880" s="167" t="s">
-        <v>1745</v>
+        <v>1734</v>
       </c>
       <c r="E880" s="160" t="s">
-        <v>1747</v>
+        <v>1736</v>
       </c>
       <c r="F880" s="151" t="s">
         <v>266</v>
@@ -25863,10 +25839,10 @@
       <c r="B881" s="109"/>
       <c r="C881" s="110"/>
       <c r="D881" s="167" t="s">
-        <v>1746</v>
+        <v>1737</v>
       </c>
       <c r="E881" s="160" t="s">
-        <v>1748</v>
+        <v>1739</v>
       </c>
       <c r="F881" s="151" t="s">
         <v>266</v>
@@ -25881,48 +25857,70 @@
         <v>719</v>
       </c>
     </row>
-    <row r="882" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="882" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A882" s="1"/>
       <c r="B882" s="109"/>
       <c r="C882" s="110"/>
-      <c r="D882" s="165"/>
-      <c r="E882" s="155"/>
-      <c r="F882" s="148"/>
-      <c r="G882" s="176"/>
-      <c r="H882" s="189"/>
-      <c r="I882" s="212"/>
-    </row>
-    <row r="883" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D882" s="167" t="s">
+        <v>1738</v>
+      </c>
+      <c r="E882" s="160" t="s">
+        <v>1740</v>
+      </c>
+      <c r="F882" s="151" t="s">
+        <v>266</v>
+      </c>
+      <c r="G882" s="180">
+        <v>45422</v>
+      </c>
+      <c r="H882" s="192">
+        <v>44308</v>
+      </c>
+      <c r="I882" s="196" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="883" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A883" s="1"/>
       <c r="B883" s="109"/>
-      <c r="C883" s="236" t="s">
-        <v>158</v>
-      </c>
-      <c r="D883" s="135"/>
-      <c r="E883" s="154"/>
-      <c r="F883" s="147"/>
-      <c r="G883" s="175"/>
-      <c r="H883" s="188"/>
-      <c r="I883" s="211"/>
+      <c r="C883" s="110"/>
+      <c r="D883" s="167" t="s">
+        <v>1741</v>
+      </c>
+      <c r="E883" s="160" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F883" s="151" t="s">
+        <v>266</v>
+      </c>
+      <c r="G883" s="180">
+        <v>45422</v>
+      </c>
+      <c r="H883" s="192">
+        <v>44711</v>
+      </c>
+      <c r="I883" s="196" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="884" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A884" s="1"/>
       <c r="B884" s="109"/>
-      <c r="C884" s="236"/>
-      <c r="D884" s="166" t="s">
-        <v>461</v>
-      </c>
-      <c r="E884" s="162" t="s">
-        <v>462</v>
-      </c>
-      <c r="F884" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G884" s="178">
-        <v>44663</v>
-      </c>
-      <c r="H884" s="191">
-        <v>44663</v>
+      <c r="C884" s="110"/>
+      <c r="D884" s="167" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E884" s="160" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F884" s="151" t="s">
+        <v>266</v>
+      </c>
+      <c r="G884" s="180">
+        <v>45422</v>
+      </c>
+      <c r="H884" s="192">
+        <v>44711</v>
       </c>
       <c r="I884" s="196" t="s">
         <v>719</v>
@@ -25933,19 +25931,19 @@
       <c r="B885" s="109"/>
       <c r="C885" s="110"/>
       <c r="D885" s="167" t="s">
-        <v>463</v>
+        <v>1745</v>
       </c>
       <c r="E885" s="160" t="s">
-        <v>464</v>
+        <v>1747</v>
       </c>
       <c r="F885" s="151" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="G885" s="180">
-        <v>44663</v>
+        <v>45422</v>
       </c>
       <c r="H885" s="192">
-        <v>44663</v>
+        <v>44308</v>
       </c>
       <c r="I885" s="196" t="s">
         <v>719</v>
@@ -25956,88 +25954,66 @@
       <c r="B886" s="109"/>
       <c r="C886" s="110"/>
       <c r="D886" s="167" t="s">
-        <v>466</v>
+        <v>1746</v>
       </c>
       <c r="E886" s="160" t="s">
-        <v>465</v>
+        <v>1748</v>
       </c>
       <c r="F886" s="151" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="G886" s="180">
-        <v>44630</v>
+        <v>45422</v>
       </c>
       <c r="H886" s="192">
-        <v>44630</v>
+        <v>44308</v>
       </c>
       <c r="I886" s="196" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="887" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="887" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A887" s="1"/>
       <c r="B887" s="109"/>
       <c r="C887" s="110"/>
-      <c r="D887" s="167" t="s">
-        <v>467</v>
-      </c>
-      <c r="E887" s="160" t="s">
-        <v>468</v>
-      </c>
-      <c r="F887" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G887" s="180">
-        <v>44630</v>
-      </c>
-      <c r="H887" s="192">
-        <v>44630</v>
-      </c>
-      <c r="I887" s="196" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="888" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="D887" s="165"/>
+      <c r="E887" s="155"/>
+      <c r="F887" s="148"/>
+      <c r="G887" s="176"/>
+      <c r="H887" s="189"/>
+      <c r="I887" s="212"/>
+    </row>
+    <row r="888" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A888" s="1"/>
       <c r="B888" s="109"/>
-      <c r="C888" s="110"/>
-      <c r="D888" s="167" t="s">
-        <v>469</v>
-      </c>
-      <c r="E888" s="160" t="s">
-        <v>470</v>
-      </c>
-      <c r="F888" s="151" t="s">
-        <v>280</v>
-      </c>
-      <c r="G888" s="180">
-        <v>44698</v>
-      </c>
-      <c r="H888" s="192">
-        <v>44630</v>
-      </c>
-      <c r="I888" s="196" t="s">
-        <v>719</v>
-      </c>
+      <c r="C888" s="236" t="s">
+        <v>158</v>
+      </c>
+      <c r="D888" s="135"/>
+      <c r="E888" s="154"/>
+      <c r="F888" s="147"/>
+      <c r="G888" s="175"/>
+      <c r="H888" s="188"/>
+      <c r="I888" s="211"/>
     </row>
     <row r="889" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A889" s="1"/>
       <c r="B889" s="109"/>
-      <c r="C889" s="110"/>
-      <c r="D889" s="167" t="s">
-        <v>471</v>
-      </c>
-      <c r="E889" s="160" t="s">
-        <v>472</v>
-      </c>
-      <c r="F889" s="151" t="s">
-        <v>280</v>
-      </c>
-      <c r="G889" s="180">
-        <v>44698</v>
-      </c>
-      <c r="H889" s="192">
-        <v>44630</v>
+      <c r="C889" s="236"/>
+      <c r="D889" s="166" t="s">
+        <v>461</v>
+      </c>
+      <c r="E889" s="162" t="s">
+        <v>462</v>
+      </c>
+      <c r="F889" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G889" s="178">
+        <v>44663</v>
+      </c>
+      <c r="H889" s="191">
+        <v>44663</v>
       </c>
       <c r="I889" s="196" t="s">
         <v>719</v>
@@ -26048,19 +26024,19 @@
       <c r="B890" s="109"/>
       <c r="C890" s="110"/>
       <c r="D890" s="167" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
       <c r="E890" s="160" t="s">
-        <v>486</v>
+        <v>464</v>
       </c>
       <c r="F890" s="151" t="s">
-        <v>487</v>
+        <v>232</v>
       </c>
       <c r="G890" s="180">
-        <v>44698</v>
+        <v>44663</v>
       </c>
       <c r="H890" s="192">
-        <v>44621</v>
+        <v>44663</v>
       </c>
       <c r="I890" s="196" t="s">
         <v>719</v>
@@ -26071,19 +26047,19 @@
       <c r="B891" s="109"/>
       <c r="C891" s="110"/>
       <c r="D891" s="167" t="s">
-        <v>489</v>
+        <v>466</v>
       </c>
       <c r="E891" s="160" t="s">
-        <v>488</v>
+        <v>465</v>
       </c>
       <c r="F891" s="151" t="s">
-        <v>487</v>
+        <v>232</v>
       </c>
       <c r="G891" s="180">
-        <v>44698</v>
+        <v>44630</v>
       </c>
       <c r="H891" s="192">
-        <v>44621</v>
+        <v>44630</v>
       </c>
       <c r="I891" s="196" t="s">
         <v>719</v>
@@ -26094,19 +26070,19 @@
       <c r="B892" s="109"/>
       <c r="C892" s="110"/>
       <c r="D892" s="167" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="E892" s="160" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="F892" s="151" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="G892" s="180">
-        <v>44669</v>
+        <v>44630</v>
       </c>
       <c r="H892" s="192">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I892" s="196" t="s">
         <v>719</v>
@@ -26117,19 +26093,19 @@
       <c r="B893" s="109"/>
       <c r="C893" s="110"/>
       <c r="D893" s="167" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="E893" s="160" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="F893" s="151" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="G893" s="180">
-        <v>44669</v>
+        <v>44698</v>
       </c>
       <c r="H893" s="192">
-        <v>44824</v>
+        <v>44630</v>
       </c>
       <c r="I893" s="196" t="s">
         <v>719</v>
@@ -26140,19 +26116,19 @@
       <c r="B894" s="109"/>
       <c r="C894" s="110"/>
       <c r="D894" s="167" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="E894" s="160" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="F894" s="151" t="s">
-        <v>454</v>
+        <v>280</v>
       </c>
       <c r="G894" s="180">
-        <v>44733</v>
+        <v>44698</v>
       </c>
       <c r="H894" s="192">
-        <v>44622</v>
+        <v>44630</v>
       </c>
       <c r="I894" s="196" t="s">
         <v>719</v>
@@ -26163,16 +26139,16 @@
       <c r="B895" s="109"/>
       <c r="C895" s="110"/>
       <c r="D895" s="167" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="E895" s="160" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="F895" s="151" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="G895" s="180">
-        <v>44733</v>
+        <v>44698</v>
       </c>
       <c r="H895" s="192">
         <v>44621</v>
@@ -26186,19 +26162,19 @@
       <c r="B896" s="109"/>
       <c r="C896" s="110"/>
       <c r="D896" s="167" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="E896" s="160" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="F896" s="151" t="s">
-        <v>454</v>
+        <v>487</v>
       </c>
       <c r="G896" s="180">
-        <v>44671</v>
+        <v>44698</v>
       </c>
       <c r="H896" s="192">
-        <v>44732</v>
+        <v>44621</v>
       </c>
       <c r="I896" s="196" t="s">
         <v>719</v>
@@ -26209,19 +26185,19 @@
       <c r="B897" s="109"/>
       <c r="C897" s="110"/>
       <c r="D897" s="167" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
       <c r="E897" s="160" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="F897" s="151" t="s">
-        <v>454</v>
+        <v>255</v>
       </c>
       <c r="G897" s="180">
-        <v>44671</v>
+        <v>44669</v>
       </c>
       <c r="H897" s="192">
-        <v>44732</v>
+        <v>44824</v>
       </c>
       <c r="I897" s="196" t="s">
         <v>719</v>
@@ -26232,19 +26208,19 @@
       <c r="B898" s="109"/>
       <c r="C898" s="110"/>
       <c r="D898" s="167" t="s">
-        <v>957</v>
+        <v>476</v>
       </c>
       <c r="E898" s="160" t="s">
-        <v>959</v>
+        <v>475</v>
       </c>
       <c r="F898" s="151" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="G898" s="180">
-        <v>45048</v>
+        <v>44669</v>
       </c>
       <c r="H898" s="192">
-        <v>45048</v>
+        <v>44824</v>
       </c>
       <c r="I898" s="196" t="s">
         <v>719</v>
@@ -26255,19 +26231,19 @@
       <c r="B899" s="109"/>
       <c r="C899" s="110"/>
       <c r="D899" s="167" t="s">
-        <v>958</v>
+        <v>477</v>
       </c>
       <c r="E899" s="160" t="s">
-        <v>960</v>
+        <v>478</v>
       </c>
       <c r="F899" s="151" t="s">
-        <v>232</v>
+        <v>454</v>
       </c>
       <c r="G899" s="180">
-        <v>45048</v>
+        <v>44733</v>
       </c>
       <c r="H899" s="192">
-        <v>45048</v>
+        <v>44622</v>
       </c>
       <c r="I899" s="196" t="s">
         <v>719</v>
@@ -26278,19 +26254,19 @@
       <c r="B900" s="109"/>
       <c r="C900" s="110"/>
       <c r="D900" s="167" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="E900" s="160" t="s">
-        <v>492</v>
+        <v>480</v>
       </c>
       <c r="F900" s="151" t="s">
-        <v>542</v>
+        <v>454</v>
       </c>
       <c r="G900" s="180">
-        <v>45145</v>
+        <v>44733</v>
       </c>
       <c r="H900" s="192">
-        <v>44622</v>
+        <v>44621</v>
       </c>
       <c r="I900" s="196" t="s">
         <v>719</v>
@@ -26301,19 +26277,19 @@
       <c r="B901" s="109"/>
       <c r="C901" s="110"/>
       <c r="D901" s="167" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="E901" s="160" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="F901" s="151" t="s">
-        <v>542</v>
+        <v>454</v>
       </c>
       <c r="G901" s="180">
-        <v>45145</v>
+        <v>44671</v>
       </c>
       <c r="H901" s="192">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I901" s="196" t="s">
         <v>719</v>
@@ -26324,19 +26300,19 @@
       <c r="B902" s="109"/>
       <c r="C902" s="110"/>
       <c r="D902" s="167" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="E902" s="160" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="F902" s="151" t="s">
         <v>454</v>
       </c>
       <c r="G902" s="180">
-        <v>44698</v>
+        <v>44671</v>
       </c>
       <c r="H902" s="192">
-        <v>44621</v>
+        <v>44732</v>
       </c>
       <c r="I902" s="196" t="s">
         <v>719</v>
@@ -26347,19 +26323,19 @@
       <c r="B903" s="109"/>
       <c r="C903" s="110"/>
       <c r="D903" s="167" t="s">
-        <v>496</v>
+        <v>957</v>
       </c>
       <c r="E903" s="160" t="s">
-        <v>497</v>
+        <v>959</v>
       </c>
       <c r="F903" s="151" t="s">
-        <v>454</v>
+        <v>232</v>
       </c>
       <c r="G903" s="180">
-        <v>44698</v>
+        <v>45048</v>
       </c>
       <c r="H903" s="192">
-        <v>44621</v>
+        <v>45048</v>
       </c>
       <c r="I903" s="196" t="s">
         <v>719</v>
@@ -26370,19 +26346,19 @@
       <c r="B904" s="109"/>
       <c r="C904" s="110"/>
       <c r="D904" s="167" t="s">
-        <v>498</v>
+        <v>958</v>
       </c>
       <c r="E904" s="160" t="s">
-        <v>499</v>
+        <v>960</v>
       </c>
       <c r="F904" s="151" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="G904" s="180">
-        <v>44846</v>
+        <v>45048</v>
       </c>
       <c r="H904" s="192">
-        <v>44627</v>
+        <v>45048</v>
       </c>
       <c r="I904" s="196" t="s">
         <v>719</v>
@@ -26393,19 +26369,19 @@
       <c r="B905" s="109"/>
       <c r="C905" s="110"/>
       <c r="D905" s="167" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="E905" s="160" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="F905" s="151" t="s">
-        <v>266</v>
+        <v>542</v>
       </c>
       <c r="G905" s="180">
-        <v>44846</v>
+        <v>45145</v>
       </c>
       <c r="H905" s="192">
-        <v>44627</v>
+        <v>44622</v>
       </c>
       <c r="I905" s="196" t="s">
         <v>719</v>
@@ -26416,19 +26392,19 @@
       <c r="B906" s="109"/>
       <c r="C906" s="110"/>
       <c r="D906" s="167" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="E906" s="160" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="F906" s="151" t="s">
-        <v>232</v>
+        <v>542</v>
       </c>
       <c r="G906" s="180">
-        <v>44628</v>
+        <v>45145</v>
       </c>
       <c r="H906" s="192">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I906" s="196" t="s">
         <v>719</v>
@@ -26439,19 +26415,19 @@
       <c r="B907" s="109"/>
       <c r="C907" s="110"/>
       <c r="D907" s="167" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="E907" s="160" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="F907" s="151" t="s">
-        <v>232</v>
+        <v>454</v>
       </c>
       <c r="G907" s="180">
-        <v>44628</v>
+        <v>44698</v>
       </c>
       <c r="H907" s="192">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I907" s="196" t="s">
         <v>719</v>
@@ -26462,19 +26438,19 @@
       <c r="B908" s="109"/>
       <c r="C908" s="110"/>
       <c r="D908" s="167" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="E908" s="160" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="F908" s="151" t="s">
-        <v>280</v>
+        <v>454</v>
       </c>
       <c r="G908" s="180">
         <v>44698</v>
       </c>
       <c r="H908" s="192">
-        <v>44628</v>
+        <v>44621</v>
       </c>
       <c r="I908" s="196" t="s">
         <v>719</v>
@@ -26485,19 +26461,19 @@
       <c r="B909" s="109"/>
       <c r="C909" s="110"/>
       <c r="D909" s="167" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="E909" s="160" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="F909" s="151" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="G909" s="180">
-        <v>44698</v>
+        <v>44846</v>
       </c>
       <c r="H909" s="192">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I909" s="196" t="s">
         <v>719</v>
@@ -26508,19 +26484,19 @@
       <c r="B910" s="109"/>
       <c r="C910" s="110"/>
       <c r="D910" s="167" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="E910" s="160" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="F910" s="151" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="G910" s="180">
-        <v>44628</v>
+        <v>44846</v>
       </c>
       <c r="H910" s="192">
-        <v>44628</v>
+        <v>44627</v>
       </c>
       <c r="I910" s="196" t="s">
         <v>719</v>
@@ -26531,10 +26507,10 @@
       <c r="B911" s="109"/>
       <c r="C911" s="110"/>
       <c r="D911" s="167" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="E911" s="160" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="F911" s="151" t="s">
         <v>232</v>
@@ -26554,16 +26530,16 @@
       <c r="B912" s="109"/>
       <c r="C912" s="110"/>
       <c r="D912" s="167" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="E912" s="160" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="F912" s="151" t="s">
-        <v>280</v>
+        <v>232</v>
       </c>
       <c r="G912" s="180">
-        <v>44698</v>
+        <v>44628</v>
       </c>
       <c r="H912" s="192">
         <v>44628</v>
@@ -26577,10 +26553,10 @@
       <c r="B913" s="109"/>
       <c r="C913" s="110"/>
       <c r="D913" s="167" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="E913" s="160" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="F913" s="151" t="s">
         <v>280</v>
@@ -26600,19 +26576,19 @@
       <c r="B914" s="109"/>
       <c r="C914" s="110"/>
       <c r="D914" s="167" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="E914" s="160" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="F914" s="151" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="G914" s="180">
-        <v>44617</v>
+        <v>44698</v>
       </c>
       <c r="H914" s="192">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I914" s="196" t="s">
         <v>719</v>
@@ -26623,19 +26599,19 @@
       <c r="B915" s="109"/>
       <c r="C915" s="110"/>
       <c r="D915" s="167" t="s">
-        <v>521</v>
+        <v>510</v>
       </c>
       <c r="E915" s="160" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="F915" s="151" t="s">
         <v>232</v>
       </c>
       <c r="G915" s="180">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="H915" s="192">
-        <v>44617</v>
+        <v>44628</v>
       </c>
       <c r="I915" s="196" t="s">
         <v>719</v>
@@ -26646,19 +26622,19 @@
       <c r="B916" s="109"/>
       <c r="C916" s="110"/>
       <c r="D916" s="167" t="s">
-        <v>522</v>
+        <v>511</v>
       </c>
       <c r="E916" s="160" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="F916" s="151" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="G916" s="180">
-        <v>44740</v>
+        <v>44628</v>
       </c>
       <c r="H916" s="192">
-        <v>44662</v>
+        <v>44628</v>
       </c>
       <c r="I916" s="196" t="s">
         <v>719</v>
@@ -26669,110 +26645,138 @@
       <c r="B917" s="109"/>
       <c r="C917" s="110"/>
       <c r="D917" s="167" t="s">
-        <v>525</v>
+        <v>514</v>
       </c>
       <c r="E917" s="160" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="F917" s="151" t="s">
-        <v>255</v>
+        <v>280</v>
       </c>
       <c r="G917" s="180">
-        <v>44740</v>
+        <v>44698</v>
       </c>
       <c r="H917" s="192">
-        <v>44662</v>
+        <v>44628</v>
       </c>
       <c r="I917" s="196" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="918" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="918" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A918" s="1"/>
       <c r="B918" s="109"/>
       <c r="C918" s="110"/>
-      <c r="D918" s="165"/>
-      <c r="E918" s="155"/>
-      <c r="F918" s="148"/>
-      <c r="G918" s="176"/>
-      <c r="H918" s="189"/>
-      <c r="I918" s="212"/>
-    </row>
-    <row r="919" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="D918" s="167" t="s">
+        <v>516</v>
+      </c>
+      <c r="E918" s="160" t="s">
+        <v>517</v>
+      </c>
+      <c r="F918" s="151" t="s">
+        <v>280</v>
+      </c>
+      <c r="G918" s="180">
+        <v>44698</v>
+      </c>
+      <c r="H918" s="192">
+        <v>44628</v>
+      </c>
+      <c r="I918" s="196" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="919" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A919" s="1"/>
       <c r="B919" s="109"/>
-      <c r="C919" s="236" t="s">
-        <v>147</v>
-      </c>
-      <c r="D919" s="135"/>
-      <c r="E919" s="154"/>
-      <c r="F919" s="147"/>
-      <c r="G919" s="175"/>
-      <c r="H919" s="188"/>
-      <c r="I919" s="211"/>
-    </row>
-    <row r="920" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C919" s="110"/>
+      <c r="D919" s="167" t="s">
+        <v>518</v>
+      </c>
+      <c r="E919" s="160" t="s">
+        <v>519</v>
+      </c>
+      <c r="F919" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G919" s="180">
+        <v>44617</v>
+      </c>
+      <c r="H919" s="192">
+        <v>44617</v>
+      </c>
+      <c r="I919" s="196" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="920" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A920" s="1"/>
       <c r="B920" s="109"/>
-      <c r="C920" s="236"/>
-      <c r="D920" s="166" t="s">
-        <v>273</v>
-      </c>
-      <c r="E920" s="162" t="s">
-        <v>439</v>
-      </c>
-      <c r="F920" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G920" s="178">
-        <v>44167</v>
-      </c>
-      <c r="H920" s="191">
-        <v>44167</v>
-      </c>
-      <c r="I920" s="186"/>
-    </row>
-    <row r="921" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C920" s="110"/>
+      <c r="D920" s="167" t="s">
+        <v>521</v>
+      </c>
+      <c r="E920" s="160" t="s">
+        <v>520</v>
+      </c>
+      <c r="F920" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G920" s="180">
+        <v>44617</v>
+      </c>
+      <c r="H920" s="192">
+        <v>44617</v>
+      </c>
+      <c r="I920" s="196" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="921" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A921" s="1"/>
       <c r="B921" s="109"/>
       <c r="C921" s="110"/>
       <c r="D921" s="167" t="s">
-        <v>440</v>
+        <v>522</v>
       </c>
       <c r="E921" s="160" t="s">
-        <v>441</v>
+        <v>523</v>
       </c>
       <c r="F921" s="151" t="s">
         <v>255</v>
       </c>
       <c r="G921" s="180">
-        <v>44575</v>
+        <v>44740</v>
       </c>
       <c r="H921" s="192">
-        <v>44167</v>
-      </c>
-      <c r="I921" s="187"/>
+        <v>44662</v>
+      </c>
+      <c r="I921" s="196" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="922" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A922" s="1"/>
       <c r="B922" s="109"/>
       <c r="C922" s="110"/>
       <c r="D922" s="167" t="s">
-        <v>443</v>
-      </c>
-      <c r="E922" s="158" t="s">
-        <v>442</v>
+        <v>525</v>
+      </c>
+      <c r="E922" s="160" t="s">
+        <v>524</v>
       </c>
       <c r="F922" s="151" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="G922" s="180">
-        <v>44404</v>
+        <v>44740</v>
       </c>
       <c r="H922" s="192">
-        <v>44404</v>
-      </c>
-      <c r="I922" s="187"/>
+        <v>44662</v>
+      </c>
+      <c r="I922" s="196" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="923" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A923" s="1"/>
@@ -26789,7 +26793,7 @@
       <c r="A924" s="1"/>
       <c r="B924" s="109"/>
       <c r="C924" s="236" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="D924" s="135"/>
       <c r="E924" s="154"/>
@@ -26803,19 +26807,19 @@
       <c r="B925" s="109"/>
       <c r="C925" s="236"/>
       <c r="D925" s="166" t="s">
-        <v>445</v>
+        <v>273</v>
       </c>
       <c r="E925" s="162" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="F925" s="150" t="s">
         <v>232</v>
       </c>
       <c r="G925" s="178">
-        <v>44635</v>
+        <v>44167</v>
       </c>
       <c r="H925" s="191">
-        <v>44635</v>
+        <v>44167</v>
       </c>
       <c r="I925" s="186"/>
     </row>
@@ -26824,40 +26828,40 @@
       <c r="B926" s="109"/>
       <c r="C926" s="110"/>
       <c r="D926" s="167" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="E926" s="160" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="F926" s="151" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
       <c r="G926" s="180">
-        <v>44635</v>
+        <v>44575</v>
       </c>
       <c r="H926" s="192">
-        <v>44635</v>
+        <v>44167</v>
       </c>
       <c r="I926" s="187"/>
     </row>
-    <row r="927" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="927" spans="1:9" s="78" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A927" s="1"/>
       <c r="B927" s="109"/>
       <c r="C927" s="110"/>
       <c r="D927" s="167" t="s">
-        <v>448</v>
-      </c>
-      <c r="E927" s="160" t="s">
-        <v>450</v>
+        <v>443</v>
+      </c>
+      <c r="E927" s="158" t="s">
+        <v>442</v>
       </c>
       <c r="F927" s="151" t="s">
-        <v>232</v>
+        <v>280</v>
       </c>
       <c r="G927" s="180">
-        <v>44635</v>
+        <v>44404</v>
       </c>
       <c r="H927" s="192">
-        <v>44635</v>
+        <v>44404</v>
       </c>
       <c r="I927" s="187"/>
     </row>
@@ -26865,83 +26869,65 @@
       <c r="A928" s="1"/>
       <c r="B928" s="109"/>
       <c r="C928" s="110"/>
-      <c r="D928" s="167" t="s">
-        <v>449</v>
-      </c>
-      <c r="E928" s="160" t="s">
-        <v>451</v>
-      </c>
-      <c r="F928" s="151" t="s">
-        <v>232</v>
-      </c>
-      <c r="G928" s="180">
-        <v>44635</v>
-      </c>
-      <c r="H928" s="192">
-        <v>44635</v>
-      </c>
-      <c r="I928" s="187"/>
+      <c r="D928" s="165"/>
+      <c r="E928" s="155"/>
+      <c r="F928" s="148"/>
+      <c r="G928" s="176"/>
+      <c r="H928" s="189"/>
+      <c r="I928" s="212"/>
     </row>
     <row r="929" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A929" s="1"/>
       <c r="B929" s="109"/>
-      <c r="C929" s="110"/>
-      <c r="D929" s="167" t="s">
-        <v>452</v>
-      </c>
-      <c r="E929" s="160" t="s">
-        <v>455</v>
-      </c>
-      <c r="F929" s="151" t="s">
-        <v>454</v>
-      </c>
-      <c r="G929" s="180">
-        <v>44701</v>
-      </c>
-      <c r="H929" s="192">
-        <v>44644</v>
-      </c>
-      <c r="I929" s="187"/>
+      <c r="C929" s="236" t="s">
+        <v>159</v>
+      </c>
+      <c r="D929" s="135"/>
+      <c r="E929" s="154"/>
+      <c r="F929" s="147"/>
+      <c r="G929" s="175"/>
+      <c r="H929" s="188"/>
+      <c r="I929" s="211"/>
     </row>
     <row r="930" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A930" s="1"/>
       <c r="B930" s="109"/>
-      <c r="C930" s="110"/>
-      <c r="D930" s="167" t="s">
-        <v>453</v>
-      </c>
-      <c r="E930" s="160" t="s">
-        <v>456</v>
-      </c>
-      <c r="F930" s="151" t="s">
-        <v>454</v>
-      </c>
-      <c r="G930" s="180">
-        <v>44701</v>
-      </c>
-      <c r="H930" s="192">
-        <v>44644</v>
-      </c>
-      <c r="I930" s="187"/>
+      <c r="C930" s="236"/>
+      <c r="D930" s="166" t="s">
+        <v>445</v>
+      </c>
+      <c r="E930" s="162" t="s">
+        <v>444</v>
+      </c>
+      <c r="F930" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G930" s="178">
+        <v>44635</v>
+      </c>
+      <c r="H930" s="191">
+        <v>44635</v>
+      </c>
+      <c r="I930" s="186"/>
     </row>
     <row r="931" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A931" s="1"/>
       <c r="B931" s="109"/>
       <c r="C931" s="110"/>
       <c r="D931" s="167" t="s">
-        <v>457</v>
+        <v>447</v>
       </c>
       <c r="E931" s="160" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="F931" s="151" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="G931" s="180">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H931" s="192">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="I931" s="187"/>
     </row>
@@ -26950,19 +26936,19 @@
       <c r="B932" s="109"/>
       <c r="C932" s="110"/>
       <c r="D932" s="167" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="E932" s="160" t="s">
-        <v>460</v>
+        <v>450</v>
       </c>
       <c r="F932" s="151" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="G932" s="180">
-        <v>44644</v>
+        <v>44635</v>
       </c>
       <c r="H932" s="192">
-        <v>44636</v>
+        <v>44635</v>
       </c>
       <c r="I932" s="187"/>
     </row>
@@ -26970,193 +26956,195 @@
       <c r="A933" s="1"/>
       <c r="B933" s="109"/>
       <c r="C933" s="110"/>
-      <c r="D933" s="165"/>
-      <c r="E933" s="155"/>
-      <c r="F933" s="148"/>
-      <c r="G933" s="176"/>
-      <c r="H933" s="189"/>
-      <c r="I933" s="212"/>
-    </row>
-    <row r="934" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A934" s="136"/>
-      <c r="B934" s="235" t="s">
-        <v>144</v>
-      </c>
-      <c r="C934" s="134"/>
-      <c r="D934" s="135"/>
-      <c r="E934" s="154"/>
-      <c r="F934" s="147"/>
-      <c r="G934" s="175"/>
-      <c r="H934" s="188"/>
-      <c r="I934" s="211"/>
-    </row>
-    <row r="935" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A935" s="136"/>
-      <c r="B935" s="235"/>
-      <c r="C935" s="236" t="s">
-        <v>146</v>
-      </c>
-      <c r="D935" s="135"/>
-      <c r="E935" s="154"/>
-      <c r="F935" s="147"/>
-      <c r="G935" s="175"/>
-      <c r="H935" s="188"/>
-      <c r="I935" s="211"/>
+      <c r="D933" s="167" t="s">
+        <v>449</v>
+      </c>
+      <c r="E933" s="160" t="s">
+        <v>451</v>
+      </c>
+      <c r="F933" s="151" t="s">
+        <v>232</v>
+      </c>
+      <c r="G933" s="180">
+        <v>44635</v>
+      </c>
+      <c r="H933" s="192">
+        <v>44635</v>
+      </c>
+      <c r="I933" s="187"/>
+    </row>
+    <row r="934" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A934" s="1"/>
+      <c r="B934" s="109"/>
+      <c r="C934" s="110"/>
+      <c r="D934" s="167" t="s">
+        <v>452</v>
+      </c>
+      <c r="E934" s="160" t="s">
+        <v>455</v>
+      </c>
+      <c r="F934" s="151" t="s">
+        <v>454</v>
+      </c>
+      <c r="G934" s="180">
+        <v>44701</v>
+      </c>
+      <c r="H934" s="192">
+        <v>44644</v>
+      </c>
+      <c r="I934" s="187"/>
+    </row>
+    <row r="935" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A935" s="1"/>
+      <c r="B935" s="109"/>
+      <c r="C935" s="110"/>
+      <c r="D935" s="167" t="s">
+        <v>453</v>
+      </c>
+      <c r="E935" s="160" t="s">
+        <v>456</v>
+      </c>
+      <c r="F935" s="151" t="s">
+        <v>454</v>
+      </c>
+      <c r="G935" s="180">
+        <v>44701</v>
+      </c>
+      <c r="H935" s="192">
+        <v>44644</v>
+      </c>
+      <c r="I935" s="187"/>
     </row>
     <row r="936" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A936" s="1"/>
       <c r="B936" s="109"/>
-      <c r="C936" s="236"/>
-      <c r="D936" s="165"/>
-      <c r="E936" s="155"/>
-      <c r="F936" s="148"/>
-      <c r="G936" s="176"/>
-      <c r="H936" s="189"/>
-      <c r="I936" s="212"/>
+      <c r="C936" s="110"/>
+      <c r="D936" s="167" t="s">
+        <v>457</v>
+      </c>
+      <c r="E936" s="160" t="s">
+        <v>458</v>
+      </c>
+      <c r="F936" s="151" t="s">
+        <v>266</v>
+      </c>
+      <c r="G936" s="180">
+        <v>44644</v>
+      </c>
+      <c r="H936" s="192">
+        <v>44636</v>
+      </c>
+      <c r="I936" s="187"/>
     </row>
     <row r="937" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A937" s="1"/>
       <c r="B937" s="109"/>
       <c r="C937" s="110"/>
-      <c r="D937" s="165"/>
-      <c r="E937" s="155"/>
-      <c r="F937" s="148"/>
-      <c r="G937" s="176"/>
-      <c r="H937" s="189"/>
-      <c r="I937" s="212"/>
-    </row>
-    <row r="938" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D937" s="167" t="s">
+        <v>459</v>
+      </c>
+      <c r="E937" s="160" t="s">
+        <v>460</v>
+      </c>
+      <c r="F937" s="151" t="s">
+        <v>266</v>
+      </c>
+      <c r="G937" s="180">
+        <v>44644</v>
+      </c>
+      <c r="H937" s="192">
+        <v>44636</v>
+      </c>
+      <c r="I937" s="187"/>
+    </row>
+    <row r="938" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A938" s="1"/>
       <c r="B938" s="109"/>
-      <c r="C938" s="223"/>
-      <c r="D938" s="224"/>
-      <c r="E938" s="226"/>
-      <c r="F938" s="225"/>
-      <c r="G938" s="224"/>
-      <c r="H938" s="226"/>
-      <c r="I938" s="227"/>
-    </row>
-    <row r="939" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C938" s="110"/>
+      <c r="D938" s="165"/>
+      <c r="E938" s="155"/>
+      <c r="F938" s="148"/>
+      <c r="G938" s="176"/>
+      <c r="H938" s="189"/>
+      <c r="I938" s="212"/>
+    </row>
+    <row r="939" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A939" s="136"/>
-      <c r="B939" s="109"/>
-      <c r="C939" s="110"/>
-      <c r="D939" s="166" t="s">
-        <v>847</v>
-      </c>
-      <c r="E939" s="162" t="s">
-        <v>849</v>
-      </c>
-      <c r="F939" s="150" t="s">
-        <v>266</v>
-      </c>
-      <c r="G939" s="178">
-        <v>44950</v>
-      </c>
-      <c r="H939" s="191">
-        <v>44893</v>
-      </c>
-      <c r="I939" s="195" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="940" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B939" s="235" t="s">
+        <v>144</v>
+      </c>
+      <c r="C939" s="134"/>
+      <c r="D939" s="135"/>
+      <c r="E939" s="154"/>
+      <c r="F939" s="147"/>
+      <c r="G939" s="175"/>
+      <c r="H939" s="188"/>
+      <c r="I939" s="211"/>
+    </row>
+    <row r="940" spans="1:9" s="137" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A940" s="136"/>
-      <c r="B940" s="109"/>
-      <c r="C940" s="110"/>
-      <c r="D940" s="167" t="s">
-        <v>848</v>
-      </c>
-      <c r="E940" s="158" t="s">
-        <v>850</v>
-      </c>
-      <c r="F940" s="151" t="s">
-        <v>266</v>
-      </c>
-      <c r="G940" s="180">
-        <v>44950</v>
-      </c>
-      <c r="H940" s="192">
-        <v>44893</v>
-      </c>
-      <c r="I940" s="195" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="941" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A941" s="136"/>
+      <c r="B940" s="235"/>
+      <c r="C940" s="236" t="s">
+        <v>146</v>
+      </c>
+      <c r="D940" s="135"/>
+      <c r="E940" s="154"/>
+      <c r="F940" s="147"/>
+      <c r="G940" s="175"/>
+      <c r="H940" s="188"/>
+      <c r="I940" s="211"/>
+    </row>
+    <row r="941" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A941" s="1"/>
       <c r="B941" s="109"/>
-      <c r="C941" s="110"/>
-      <c r="D941" s="166" t="s">
-        <v>851</v>
-      </c>
-      <c r="E941" s="157" t="s">
-        <v>853</v>
-      </c>
-      <c r="F941" s="150" t="s">
-        <v>542</v>
-      </c>
-      <c r="G941" s="178">
-        <v>44970</v>
-      </c>
-      <c r="H941" s="191">
-        <v>44893</v>
-      </c>
-      <c r="I941" s="195" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="942" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A942" s="136"/>
+      <c r="C941" s="236"/>
+      <c r="D941" s="165"/>
+      <c r="E941" s="155"/>
+      <c r="F941" s="148"/>
+      <c r="G941" s="176"/>
+      <c r="H941" s="189"/>
+      <c r="I941" s="212"/>
+    </row>
+    <row r="942" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A942" s="1"/>
       <c r="B942" s="109"/>
       <c r="C942" s="110"/>
-      <c r="D942" s="166" t="s">
-        <v>852</v>
-      </c>
-      <c r="E942" s="157" t="s">
-        <v>854</v>
-      </c>
-      <c r="F942" s="150" t="s">
-        <v>542</v>
-      </c>
-      <c r="G942" s="178">
-        <v>44970</v>
-      </c>
-      <c r="H942" s="191">
-        <v>44893</v>
-      </c>
-      <c r="I942" s="195" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="943" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A943" s="136"/>
+      <c r="D942" s="165"/>
+      <c r="E942" s="155"/>
+      <c r="F942" s="148"/>
+      <c r="G942" s="176"/>
+      <c r="H942" s="189"/>
+      <c r="I942" s="212"/>
+    </row>
+    <row r="943" spans="1:9" s="78" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A943" s="1"/>
       <c r="B943" s="109"/>
-      <c r="C943" s="110"/>
-      <c r="D943" s="166"/>
-      <c r="E943" s="157"/>
-      <c r="F943" s="150"/>
-      <c r="G943" s="178"/>
-      <c r="H943" s="191"/>
-      <c r="I943" s="195"/>
+      <c r="C943" s="223"/>
+      <c r="D943" s="224"/>
+      <c r="E943" s="226"/>
+      <c r="F943" s="225"/>
+      <c r="G943" s="224"/>
+      <c r="H943" s="226"/>
+      <c r="I943" s="227"/>
     </row>
     <row r="944" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A944" s="136"/>
       <c r="B944" s="109"/>
       <c r="C944" s="110"/>
       <c r="D944" s="166" t="s">
-        <v>923</v>
-      </c>
-      <c r="E944" s="157" t="s">
-        <v>925</v>
+        <v>847</v>
+      </c>
+      <c r="E944" s="162" t="s">
+        <v>849</v>
       </c>
       <c r="F944" s="150" t="s">
-        <v>232</v>
+        <v>266</v>
       </c>
       <c r="G944" s="178">
-        <v>45009</v>
+        <v>44950</v>
       </c>
       <c r="H944" s="191">
-        <v>45009</v>
+        <v>44893</v>
       </c>
       <c r="I944" s="195" t="s">
         <v>719</v>
@@ -27166,147 +27154,195 @@
       <c r="A945" s="136"/>
       <c r="B945" s="109"/>
       <c r="C945" s="110"/>
-      <c r="D945" s="166" t="s">
-        <v>922</v>
-      </c>
-      <c r="E945" s="157" t="s">
-        <v>924</v>
-      </c>
-      <c r="F945" s="150" t="s">
-        <v>232</v>
-      </c>
-      <c r="G945" s="178">
-        <v>45009</v>
-      </c>
-      <c r="H945" s="191">
-        <v>45009</v>
+      <c r="D945" s="167" t="s">
+        <v>848</v>
+      </c>
+      <c r="E945" s="158" t="s">
+        <v>850</v>
+      </c>
+      <c r="F945" s="151" t="s">
+        <v>266</v>
+      </c>
+      <c r="G945" s="180">
+        <v>44950</v>
+      </c>
+      <c r="H945" s="192">
+        <v>44893</v>
       </c>
       <c r="I945" s="195" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="946" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="946" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A946" s="136"/>
       <c r="B946" s="109"/>
       <c r="C946" s="110"/>
-      <c r="D946" s="166"/>
-      <c r="E946" s="157"/>
-      <c r="F946" s="150"/>
-      <c r="G946" s="178"/>
-      <c r="H946" s="191"/>
-      <c r="I946" s="195"/>
+      <c r="D946" s="166" t="s">
+        <v>851</v>
+      </c>
+      <c r="E946" s="157" t="s">
+        <v>853</v>
+      </c>
+      <c r="F946" s="150" t="s">
+        <v>542</v>
+      </c>
+      <c r="G946" s="178">
+        <v>44970</v>
+      </c>
+      <c r="H946" s="191">
+        <v>44893</v>
+      </c>
+      <c r="I946" s="195" t="s">
+        <v>719</v>
+      </c>
     </row>
     <row r="947" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A947" s="136"/>
       <c r="B947" s="109"/>
       <c r="C947" s="110"/>
       <c r="D947" s="166" t="s">
-        <v>843</v>
-      </c>
-      <c r="E947" s="162" t="s">
-        <v>846</v>
+        <v>852</v>
+      </c>
+      <c r="E947" s="157" t="s">
+        <v>854</v>
       </c>
       <c r="F947" s="150" t="s">
-        <v>266</v>
+        <v>542</v>
       </c>
       <c r="G947" s="178">
-        <v>44986</v>
+        <v>44970</v>
       </c>
       <c r="H947" s="191">
-        <v>44951</v>
+        <v>44893</v>
       </c>
       <c r="I947" s="195" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="948" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="948" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A948" s="136"/>
       <c r="B948" s="109"/>
       <c r="C948" s="110"/>
-      <c r="D948" s="167" t="s">
+      <c r="D948" s="166"/>
+      <c r="E948" s="157"/>
+      <c r="F948" s="150"/>
+      <c r="G948" s="178"/>
+      <c r="H948" s="191"/>
+      <c r="I948" s="195"/>
+    </row>
+    <row r="949" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A949" s="136"/>
+      <c r="B949" s="109"/>
+      <c r="C949" s="110"/>
+      <c r="D949" s="166" t="s">
+        <v>923</v>
+      </c>
+      <c r="E949" s="157" t="s">
+        <v>925</v>
+      </c>
+      <c r="F949" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G949" s="178">
+        <v>45009</v>
+      </c>
+      <c r="H949" s="191">
+        <v>45009</v>
+      </c>
+      <c r="I949" s="195" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="950" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A950" s="136"/>
+      <c r="B950" s="109"/>
+      <c r="C950" s="110"/>
+      <c r="D950" s="166" t="s">
+        <v>922</v>
+      </c>
+      <c r="E950" s="157" t="s">
+        <v>924</v>
+      </c>
+      <c r="F950" s="150" t="s">
+        <v>232</v>
+      </c>
+      <c r="G950" s="178">
+        <v>45009</v>
+      </c>
+      <c r="H950" s="191">
+        <v>45009</v>
+      </c>
+      <c r="I950" s="195" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="951" spans="1:9" s="137" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A951" s="136"/>
+      <c r="B951" s="109"/>
+      <c r="C951" s="110"/>
+      <c r="D951" s="166"/>
+      <c r="E951" s="157"/>
+      <c r="F951" s="150"/>
+      <c r="G951" s="178"/>
+      <c r="H951" s="191"/>
+      <c r="I951" s="195"/>
+    </row>
+    <row r="952" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A952" s="136"/>
+      <c r="B952" s="109"/>
+      <c r="C952" s="110"/>
+      <c r="D952" s="166" t="s">
+        <v>843</v>
+      </c>
+      <c r="E952" s="162" t="s">
+        <v>846</v>
+      </c>
+      <c r="F952" s="150" t="s">
+        <v>266</v>
+      </c>
+      <c r="G952" s="178">
+        <v>44986</v>
+      </c>
+      <c r="H952" s="191">
+        <v>44951</v>
+      </c>
+      <c r="I952" s="195" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="953" spans="1:9" s="137" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A953" s="136"/>
+      <c r="B953" s="109"/>
+      <c r="C953" s="110"/>
+      <c r="D953" s="167" t="s">
         <v>844</v>
       </c>
-      <c r="E948" s="158" t="s">
+      <c r="E953" s="158" t="s">
         <v>845</v>
       </c>
-      <c r="F948" s="151" t="s">
+      <c r="F953" s="151" t="s">
         <v>266</v>
       </c>
-      <c r="G948" s="180">
+      <c r="G953" s="180">
         <v>44986</v>
       </c>
-      <c r="H948" s="192">
+      <c r="H953" s="192">
         <v>44951</v>
       </c>
-      <c r="I948" s="195" t="s">
+      <c r="I953" s="195" t="s">
         <v>719</v>
       </c>
     </row>
-    <row r="949" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A949" s="136"/>
-      <c r="B949" s="111"/>
-      <c r="C949" s="112"/>
-      <c r="D949" s="170"/>
-      <c r="E949" s="163"/>
-      <c r="F949" s="153"/>
-      <c r="G949" s="181"/>
-      <c r="H949" s="194"/>
-      <c r="I949" s="215"/>
-    </row>
-    <row r="950" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A950" s="1"/>
-      <c r="B950" s="1"/>
-      <c r="C950" s="1"/>
-      <c r="D950" s="1"/>
-      <c r="E950" s="146"/>
-      <c r="F950" s="113"/>
-      <c r="G950" s="182"/>
-      <c r="H950" s="182"/>
-      <c r="I950" s="172"/>
-    </row>
-    <row r="951" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A951" s="1"/>
-      <c r="B951" s="1"/>
-      <c r="C951" s="1"/>
-      <c r="D951" s="1"/>
-      <c r="E951" s="146"/>
-      <c r="F951" s="113"/>
-      <c r="G951" s="182"/>
-      <c r="H951" s="182"/>
-      <c r="I951" s="172"/>
-    </row>
-    <row r="952" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A952" s="1"/>
-      <c r="B952" s="1"/>
-      <c r="C952" s="1"/>
-      <c r="D952" s="1"/>
-      <c r="E952" s="146"/>
-      <c r="F952" s="113"/>
-      <c r="G952" s="182"/>
-      <c r="H952" s="182"/>
-      <c r="I952" s="172"/>
-    </row>
-    <row r="953" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A953" s="1"/>
-      <c r="B953" s="1"/>
-      <c r="C953" s="1"/>
-      <c r="D953" s="1"/>
-      <c r="E953" s="146"/>
-      <c r="F953" s="113"/>
-      <c r="G953" s="182"/>
-      <c r="H953" s="182"/>
-      <c r="I953" s="172"/>
-    </row>
-    <row r="954" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A954" s="1"/>
-      <c r="B954" s="1"/>
-      <c r="C954" s="1"/>
-      <c r="D954" s="1"/>
-      <c r="E954" s="146"/>
-      <c r="F954" s="113"/>
-      <c r="G954" s="182"/>
-      <c r="H954" s="182"/>
-      <c r="I954" s="172"/>
+    <row r="954" spans="1:9" s="137" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A954" s="136"/>
+      <c r="B954" s="111"/>
+      <c r="C954" s="112"/>
+      <c r="D954" s="170"/>
+      <c r="E954" s="163"/>
+      <c r="F954" s="153"/>
+      <c r="G954" s="181"/>
+      <c r="H954" s="194"/>
+      <c r="I954" s="215"/>
     </row>
     <row r="955" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A955" s="1"/>
@@ -27429,44 +27465,103 @@
       <c r="H965" s="182"/>
       <c r="I965" s="172"/>
     </row>
-    <row r="966" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E966" s="145"/>
-      <c r="F966" s="95"/>
-      <c r="G966" s="183"/>
-      <c r="H966" s="183"/>
-      <c r="I966" s="173"/>
-    </row>
-    <row r="967" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E967" s="145"/>
-      <c r="F967" s="95"/>
-      <c r="G967" s="183"/>
-      <c r="H967" s="183"/>
-      <c r="I967" s="173"/>
-    </row>
-    <row r="968" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="E968" s="145"/>
-      <c r="F968" s="95"/>
-      <c r="G968" s="183"/>
-      <c r="H968" s="183"/>
-      <c r="I968" s="173"/>
+    <row r="966" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A966" s="1"/>
+      <c r="B966" s="1"/>
+      <c r="C966" s="1"/>
+      <c r="D966" s="1"/>
+      <c r="E966" s="146"/>
+      <c r="F966" s="113"/>
+      <c r="G966" s="182"/>
+      <c r="H966" s="182"/>
+      <c r="I966" s="172"/>
+    </row>
+    <row r="967" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A967" s="1"/>
+      <c r="B967" s="1"/>
+      <c r="C967" s="1"/>
+      <c r="D967" s="1"/>
+      <c r="E967" s="146"/>
+      <c r="F967" s="113"/>
+      <c r="G967" s="182"/>
+      <c r="H967" s="182"/>
+      <c r="I967" s="172"/>
+    </row>
+    <row r="968" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A968" s="1"/>
+      <c r="B968" s="1"/>
+      <c r="C968" s="1"/>
+      <c r="D968" s="1"/>
+      <c r="E968" s="146"/>
+      <c r="F968" s="113"/>
+      <c r="G968" s="182"/>
+      <c r="H968" s="182"/>
+      <c r="I968" s="172"/>
+    </row>
+    <row r="969" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A969" s="1"/>
+      <c r="B969" s="1"/>
+      <c r="C969" s="1"/>
+      <c r="D969" s="1"/>
+      <c r="E969" s="146"/>
+      <c r="F969" s="113"/>
+      <c r="G969" s="182"/>
+      <c r="H969" s="182"/>
+      <c r="I969" s="172"/>
+    </row>
+    <row r="970" spans="1:9" s="78" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A970" s="1"/>
+      <c r="B970" s="1"/>
+      <c r="C970" s="1"/>
+      <c r="D970" s="1"/>
+      <c r="E970" s="146"/>
+      <c r="F970" s="113"/>
+      <c r="G970" s="182"/>
+      <c r="H970" s="182"/>
+      <c r="I970" s="172"/>
+    </row>
+    <row r="971" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E971" s="145"/>
+      <c r="F971" s="95"/>
+      <c r="G971" s="183"/>
+      <c r="H971" s="183"/>
+      <c r="I971" s="173"/>
+    </row>
+    <row r="972" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E972" s="145"/>
+      <c r="F972" s="95"/>
+      <c r="G972" s="183"/>
+      <c r="H972" s="183"/>
+      <c r="I972" s="173"/>
+    </row>
+    <row r="973" spans="1:9" s="78" customFormat="1" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="E973" s="145"/>
+      <c r="F973" s="95"/>
+      <c r="G973" s="183"/>
+      <c r="H973" s="183"/>
+      <c r="I973" s="173"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B770:B771"/>
-    <mergeCell ref="C771:C772"/>
-    <mergeCell ref="C432:C433"/>
-    <mergeCell ref="B766:B767"/>
-    <mergeCell ref="C767:C768"/>
-    <mergeCell ref="C593:C594"/>
-    <mergeCell ref="C760:C761"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B939:B940"/>
+    <mergeCell ref="C940:C941"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="C865:C866"/>
+    <mergeCell ref="C873:C874"/>
+    <mergeCell ref="C888:C889"/>
+    <mergeCell ref="C924:C925"/>
+    <mergeCell ref="C782:C783"/>
+    <mergeCell ref="C791:C792"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C86:C87"/>
+    <mergeCell ref="C112:C113"/>
+    <mergeCell ref="C185:C186"/>
+    <mergeCell ref="C200:C201"/>
     <mergeCell ref="C229:C230"/>
     <mergeCell ref="C341:C342"/>
-    <mergeCell ref="C924:C925"/>
+    <mergeCell ref="C929:C930"/>
     <mergeCell ref="C798:C799"/>
     <mergeCell ref="C805:C806"/>
     <mergeCell ref="C844:C845"/>
@@ -27476,22 +27571,18 @@
     <mergeCell ref="C366:C367"/>
     <mergeCell ref="C406:C407"/>
     <mergeCell ref="C744:C745"/>
-    <mergeCell ref="B934:B935"/>
-    <mergeCell ref="C935:C936"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C865:C866"/>
-    <mergeCell ref="C868:C869"/>
-    <mergeCell ref="C883:C884"/>
-    <mergeCell ref="C919:C920"/>
-    <mergeCell ref="C782:C783"/>
-    <mergeCell ref="C791:C792"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="C185:C186"/>
-    <mergeCell ref="C200:C201"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B770:B771"/>
+    <mergeCell ref="C771:C772"/>
+    <mergeCell ref="C432:C433"/>
+    <mergeCell ref="B766:B767"/>
+    <mergeCell ref="C767:C768"/>
+    <mergeCell ref="C593:C594"/>
+    <mergeCell ref="C760:C761"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -27544,20 +27635,20 @@
   <sheetData>
     <row r="1" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" s="28" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="253" t="s">
+      <c r="B2" s="270" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="254"/>
-      <c r="D2" s="255"/>
-      <c r="E2" s="250" t="s">
+      <c r="C2" s="271"/>
+      <c r="D2" s="272"/>
+      <c r="E2" s="267" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="252"/>
-      <c r="G2" s="250" t="s">
+      <c r="F2" s="269"/>
+      <c r="G2" s="267" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="251"/>
-      <c r="I2" s="252"/>
+      <c r="H2" s="268"/>
+      <c r="I2" s="269"/>
     </row>
     <row r="3" spans="2:11" s="3" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="91" t="s">
@@ -27578,10 +27669,10 @@
       <c r="G3" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="256" t="s">
+      <c r="H3" s="273" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="257"/>
+      <c r="I3" s="274"/>
     </row>
     <row r="4" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="61" t="s">
@@ -27616,8 +27707,8 @@
       <c r="E6" s="25"/>
       <c r="F6" s="22"/>
       <c r="G6" s="25"/>
-      <c r="H6" s="270"/>
-      <c r="I6" s="271"/>
+      <c r="H6" s="248"/>
+      <c r="I6" s="249"/>
     </row>
     <row r="7" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B7" s="61" t="s">
@@ -27659,7 +27750,7 @@
       <c r="F8" s="264" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="267" t="s">
+      <c r="G8" s="255" t="s">
         <v>9</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -27675,11 +27766,11 @@
       <c r="D9" s="262"/>
       <c r="E9" s="35"/>
       <c r="F9" s="265"/>
-      <c r="G9" s="268"/>
-      <c r="H9" s="248" t="s">
+      <c r="G9" s="256"/>
+      <c r="H9" s="250" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="249"/>
+      <c r="I9" s="251"/>
     </row>
     <row r="10" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B10" s="61"/>
@@ -27687,7 +27778,7 @@
       <c r="D10" s="263"/>
       <c r="E10" s="36"/>
       <c r="F10" s="266"/>
-      <c r="G10" s="269"/>
+      <c r="G10" s="257"/>
       <c r="H10" s="8" t="s">
         <v>23</v>
       </c>
@@ -27727,13 +27818,13 @@
       <c r="D12" s="261" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="272" t="s">
+      <c r="E12" s="252" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="264" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="267" t="s">
+      <c r="G12" s="255" t="s">
         <v>22</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -27748,22 +27839,22 @@
       <c r="B13" s="61"/>
       <c r="C13" s="259"/>
       <c r="D13" s="262"/>
-      <c r="E13" s="273"/>
+      <c r="E13" s="253"/>
       <c r="F13" s="265"/>
-      <c r="G13" s="268"/>
-      <c r="H13" s="248" t="s">
+      <c r="G13" s="256"/>
+      <c r="H13" s="250" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="249"/>
+      <c r="I13" s="251"/>
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="2:11" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B14" s="61"/>
       <c r="C14" s="260"/>
       <c r="D14" s="263"/>
-      <c r="E14" s="274"/>
+      <c r="E14" s="254"/>
       <c r="F14" s="266"/>
-      <c r="G14" s="269"/>
+      <c r="G14" s="257"/>
       <c r="H14" s="8" t="s">
         <v>23</v>
       </c>
@@ -27873,7 +27964,7 @@
       <c r="F21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="267" t="s">
+      <c r="G21" s="255" t="s">
         <v>24</v>
       </c>
       <c r="H21" s="6" t="s">
@@ -27893,7 +27984,7 @@
       <c r="F22" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="269"/>
+      <c r="G22" s="257"/>
       <c r="H22" s="8"/>
       <c r="I22" s="17"/>
     </row>
@@ -27976,8 +28067,8 @@
       <c r="E28" s="25"/>
       <c r="F28" s="22"/>
       <c r="G28" s="25"/>
-      <c r="H28" s="270"/>
-      <c r="I28" s="271"/>
+      <c r="H28" s="248"/>
+      <c r="I28" s="249"/>
     </row>
     <row r="29" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="67" t="s">
@@ -28397,13 +28488,13 @@
       <c r="D52" s="261" t="s">
         <v>43</v>
       </c>
-      <c r="E52" s="272" t="s">
+      <c r="E52" s="252" t="s">
         <v>45</v>
       </c>
       <c r="F52" s="264" t="s">
         <v>46</v>
       </c>
-      <c r="G52" s="267" t="s">
+      <c r="G52" s="255" t="s">
         <v>47</v>
       </c>
       <c r="H52" s="6" t="s">
@@ -28417,21 +28508,21 @@
       <c r="B53" s="61"/>
       <c r="C53" s="259"/>
       <c r="D53" s="262"/>
-      <c r="E53" s="273"/>
+      <c r="E53" s="253"/>
       <c r="F53" s="265"/>
-      <c r="G53" s="268"/>
-      <c r="H53" s="248" t="s">
+      <c r="G53" s="256"/>
+      <c r="H53" s="250" t="s">
         <v>32</v>
       </c>
-      <c r="I53" s="249"/>
+      <c r="I53" s="251"/>
     </row>
     <row r="54" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B54" s="61"/>
       <c r="C54" s="260"/>
       <c r="D54" s="263"/>
-      <c r="E54" s="274"/>
+      <c r="E54" s="254"/>
       <c r="F54" s="266"/>
-      <c r="G54" s="269"/>
+      <c r="G54" s="257"/>
       <c r="H54" s="8" t="s">
         <v>23</v>
       </c>
@@ -28471,13 +28562,13 @@
       <c r="D56" s="261" t="s">
         <v>53</v>
       </c>
-      <c r="E56" s="272" t="s">
+      <c r="E56" s="252" t="s">
         <v>55</v>
       </c>
       <c r="F56" s="264" t="s">
         <v>56</v>
       </c>
-      <c r="G56" s="267" t="s">
+      <c r="G56" s="255" t="s">
         <v>9</v>
       </c>
       <c r="H56" s="6" t="s">
@@ -28491,21 +28582,21 @@
       <c r="B57" s="61"/>
       <c r="C57" s="259"/>
       <c r="D57" s="262"/>
-      <c r="E57" s="273"/>
+      <c r="E57" s="253"/>
       <c r="F57" s="265"/>
-      <c r="G57" s="268"/>
-      <c r="H57" s="248" t="s">
+      <c r="G57" s="256"/>
+      <c r="H57" s="250" t="s">
         <v>32</v>
       </c>
-      <c r="I57" s="249"/>
+      <c r="I57" s="251"/>
     </row>
     <row r="58" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B58" s="61"/>
       <c r="C58" s="260"/>
       <c r="D58" s="263"/>
-      <c r="E58" s="274"/>
+      <c r="E58" s="254"/>
       <c r="F58" s="266"/>
-      <c r="G58" s="269"/>
+      <c r="G58" s="257"/>
       <c r="H58" s="8" t="s">
         <v>23</v>
       </c>
@@ -28530,8 +28621,8 @@
       <c r="E60" s="25"/>
       <c r="F60" s="22"/>
       <c r="G60" s="25"/>
-      <c r="H60" s="270"/>
-      <c r="I60" s="271"/>
+      <c r="H60" s="248"/>
+      <c r="I60" s="249"/>
     </row>
     <row r="61" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="61" t="s">
@@ -28594,10 +28685,10 @@
       <c r="E64" s="39"/>
       <c r="F64" s="12"/>
       <c r="G64" s="32"/>
-      <c r="H64" s="248" t="s">
+      <c r="H64" s="250" t="s">
         <v>32</v>
       </c>
-      <c r="I64" s="249"/>
+      <c r="I64" s="251"/>
     </row>
     <row r="65" spans="2:9" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="B65" s="61"/>
@@ -28630,8 +28721,8 @@
       <c r="E67" s="25"/>
       <c r="F67" s="22"/>
       <c r="G67" s="25"/>
-      <c r="H67" s="270"/>
-      <c r="I67" s="271"/>
+      <c r="H67" s="248"/>
+      <c r="I67" s="249"/>
     </row>
     <row r="68" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="64" t="s">
@@ -29044,8 +29135,8 @@
       <c r="E95" s="25"/>
       <c r="F95" s="22"/>
       <c r="G95" s="25"/>
-      <c r="H95" s="270"/>
-      <c r="I95" s="271"/>
+      <c r="H95" s="248"/>
+      <c r="I95" s="249"/>
     </row>
     <row r="96" spans="2:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="61"/>
@@ -29189,22 +29280,16 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="H95:I95"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="G56:G58"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="F56:F58"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="D52:D54"/>
-    <mergeCell ref="E52:E54"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H6:I6"/>
     <mergeCell ref="C21:C22"/>
     <mergeCell ref="D21:D22"/>
     <mergeCell ref="G21:G22"/>
@@ -29217,16 +29302,22 @@
     <mergeCell ref="C12:C14"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="D17:D19"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="H53:I53"/>
+    <mergeCell ref="C52:C54"/>
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="E52:E54"/>
+    <mergeCell ref="F52:F54"/>
+    <mergeCell ref="G52:G54"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H95:I95"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="G56:G58"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H67:I67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -29260,10 +29351,10 @@
         <v>54</v>
       </c>
       <c r="C2" s="276"/>
-      <c r="D2" s="251" t="s">
+      <c r="D2" s="268" t="s">
         <v>174</v>
       </c>
-      <c r="E2" s="252" t="s">
+      <c r="E2" s="269" t="s">
         <v>0</v>
       </c>
     </row>
@@ -29274,8 +29365,8 @@
       <c r="C3" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="256"/>
-      <c r="E3" s="257"/>
+      <c r="D3" s="273"/>
+      <c r="E3" s="274"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="84" t="s">

</xml_diff>